<commit_message>
Added zoning and routing info extraction
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
   <si>
     <t>report_data</t>
   </si>
@@ -71,9 +71,6 @@
     <t>fabricshow</t>
   </si>
   <si>
-    <t>fcrfabricshow</t>
-  </si>
-  <si>
     <t>sfpshow</t>
   </si>
   <si>
@@ -126,6 +123,105 @@
   </si>
   <si>
     <t>portcmd</t>
+  </si>
+  <si>
+    <t>porttrunkarea</t>
+  </si>
+  <si>
+    <t>fdmi</t>
+  </si>
+  <si>
+    <t>nsshow</t>
+  </si>
+  <si>
+    <t>nscamshow</t>
+  </si>
+  <si>
+    <t>islshow</t>
+  </si>
+  <si>
+    <t>ag_principal</t>
+  </si>
+  <si>
+    <t>STEP</t>
+  </si>
+  <si>
+    <t>MODULE NAME</t>
+  </si>
+  <si>
+    <t>access gateway from principal</t>
+  </si>
+  <si>
+    <t>isl</t>
+  </si>
+  <si>
+    <t>trunk</t>
+  </si>
+  <si>
+    <t>trunkshow</t>
+  </si>
+  <si>
+    <t>san_fabrics</t>
+  </si>
+  <si>
+    <t>san_isl</t>
+  </si>
+  <si>
+    <t>san_portinfo</t>
+  </si>
+  <si>
+    <t>san_portcmdshow</t>
+  </si>
+  <si>
+    <t>san_connected_devices</t>
+  </si>
+  <si>
+    <t>san_amsmaps_log</t>
+  </si>
+  <si>
+    <t>san_switch_params</t>
+  </si>
+  <si>
+    <t>san_chassis_params</t>
+  </si>
+  <si>
+    <t>fcrfabric</t>
+  </si>
+  <si>
+    <t>san_fcr</t>
+  </si>
+  <si>
+    <t>fcrproxydev</t>
+  </si>
+  <si>
+    <t>fcrphydev</t>
+  </si>
+  <si>
+    <t>lsan</t>
+  </si>
+  <si>
+    <t>fcredge</t>
+  </si>
+  <si>
+    <t>fcrresource</t>
+  </si>
+  <si>
+    <t>san_zoning</t>
+  </si>
+  <si>
+    <t>cfg</t>
+  </si>
+  <si>
+    <t>zone</t>
+  </si>
+  <si>
+    <t>alias</t>
+  </si>
+  <si>
+    <t>zone_effective</t>
+  </si>
+  <si>
+    <t>cfg_effective</t>
   </si>
 </sst>
 </file>
@@ -486,7 +582,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +608,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -526,7 +622,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -540,7 +636,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -551,189 +647,536 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D28" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ISL and IFL reports added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
   <si>
     <t>report_data</t>
   </si>
@@ -245,13 +245,58 @@
     <t>fabric_statistics</t>
   </si>
   <si>
-    <t>fabric_statistics_summary</t>
-  </si>
-  <si>
     <t>san_fabrics_labels</t>
   </si>
   <si>
     <t>san_fabrics_statistics</t>
+  </si>
+  <si>
+    <t>san_switch_report_tables</t>
+  </si>
+  <si>
+    <t>Коммутаторы</t>
+  </si>
+  <si>
+    <t>Фабрика</t>
+  </si>
+  <si>
+    <t>Глобальные_параметры_фабрики</t>
+  </si>
+  <si>
+    <t>Лицензии</t>
+  </si>
+  <si>
+    <t>Параметры_коммутаторов</t>
+  </si>
+  <si>
+    <t>Статистика</t>
+  </si>
+  <si>
+    <t>Статистика_Итого</t>
+  </si>
+  <si>
+    <t>switch_params_aggregated</t>
+  </si>
+  <si>
+    <t>Межкоммутаторные_соединения</t>
+  </si>
+  <si>
+    <t>Межфабричные_соединения</t>
+  </si>
+  <si>
+    <t>isl_aggregated</t>
+  </si>
+  <si>
+    <t>san_switch_report_isl</t>
+  </si>
+  <si>
+    <t>sbrf</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\SBRF\Nov 2019\switch</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Sberbank\SberbankSAN\SAN Assessment Dec 2019</t>
   </si>
 </sst>
 </file>
@@ -609,27 +654,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="64.7109375" customWidth="1"/>
-    <col min="3" max="3" width="54.5703125" customWidth="1"/>
-    <col min="5" max="5" width="34.140625" customWidth="1"/>
+    <col min="2" max="3" width="64.7109375" customWidth="1"/>
+    <col min="4" max="4" width="54.5703125" customWidth="1"/>
+    <col min="6" max="6" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="1"/>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -637,16 +681,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -654,16 +701,19 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -671,12 +721,15 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>73</v>
       </c>
     </row>
@@ -688,10 +741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38:G39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,13 +1271,13 @@
         <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>69</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1257,13 +1310,13 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>75</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -1271,12 +1324,134 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D36" s="2" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D37" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>17</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
         <v>1</v>
       </c>
-      <c r="F36">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D40" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D42" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D43" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>18</v>
+      </c>
+      <c r="B44" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D45" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D46" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change save excel files names
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6930" activeTab="1"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="101">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -275,9 +275,6 @@
     <t>isl_aggregated</t>
   </si>
   <si>
-    <t>san_switch_report_isl</t>
-  </si>
-  <si>
     <t>sbrf</t>
   </si>
   <si>
@@ -309,6 +306,18 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>san_isl_report_tables</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\SF\packed_sshow</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\SF</t>
+  </si>
+  <si>
+    <t>sf_cust</t>
   </si>
 </sst>
 </file>
@@ -667,10 +676,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,27 +691,26 @@
     <col min="7" max="7" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
@@ -712,19 +721,22 @@
       <c r="G2" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -735,19 +747,22 @@
       <c r="G3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
@@ -757,6 +772,9 @@
       </c>
       <c r="G4" t="s">
         <v>69</v>
+      </c>
+      <c r="H4" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -767,10 +785,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,10 +1111,10 @@
         <v>41</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1112,10 +1131,10 @@
         <v>42</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1333,16 +1352,16 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1350,7 +1369,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D34" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1361,7 +1380,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D35" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -1371,14 +1390,8 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>16</v>
-      </c>
-      <c r="B36" t="s">
-        <v>74</v>
-      </c>
       <c r="D36" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -1389,7 +1402,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D37" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -1400,21 +1413,27 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D38" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>17</v>
+      </c>
+      <c r="B39" t="s">
+        <v>73</v>
+      </c>
       <c r="D39" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1422,7 +1441,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D40" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -1433,7 +1452,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D41" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -1447,16 +1466,16 @@
         <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>83</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1464,10 +1483,10 @@
         <v>84</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1475,7 +1494,7 @@
         <v>85</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44">
         <v>0</v>

</xml_diff>

<commit_message>
Virtual connect parser added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -11,14 +11,14 @@
     <sheet name="service_tables" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$I$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$I$58</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="165">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -494,22 +494,25 @@
     <t>DATA ANALYSIS 2. AGGREGATED SWITCH PARAMETERS</t>
   </si>
   <si>
-    <t>DATA ANALYSIS 3. FABRIC DEVICES IDENTIFICATION</t>
-  </si>
-  <si>
-    <t>DATA ANALYSIS 4. FABRIC STATISTICS</t>
-  </si>
-  <si>
-    <t>DATA ANALYSIS 5. INTERSWITCH AND INTERFABRIC CONNECTIONS</t>
-  </si>
-  <si>
-    <t>PREREQUISITES</t>
-  </si>
-  <si>
     <t>DATA COLLECTION 3. SWITCH PARAMETERS</t>
   </si>
   <si>
     <t>DATA COLLECTION 2. MAPS PARAMETERS</t>
+  </si>
+  <si>
+    <t>PREREQUISITES 1,2,3</t>
+  </si>
+  <si>
+    <t>blade_vc</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 3. INTERSWITCH AND INTERFABRIC CONNECTIONS</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 4. FABRIC DEVICES IDENTIFICATION</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 5. FABRIC STATISTICS</t>
   </si>
 </sst>
 </file>
@@ -893,8 +896,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,7 +915,7 @@
       <c r="A1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1047,10 +1050,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,7 +1119,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1142,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1196,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1223,7 +1226,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1250,7 +1253,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1893,34 +1896,40 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="B32" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
         <v>15</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>142</v>
       </c>
-      <c r="D32" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D33" s="6" t="s">
         <v>99</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1937,7 +1946,7 @@
         <v>99</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -1950,34 +1959,34 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="D35" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>16</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>144</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D36" s="5" t="s">
         <v>100</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -1994,7 +2003,7 @@
         <v>100</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -2011,7 +2020,7 @@
         <v>100</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -2028,7 +2037,7 @@
         <v>100</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -2041,11 +2050,11 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D40" s="6" t="s">
-        <v>99</v>
+      <c r="D40" s="5" t="s">
+        <v>100</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -2058,17 +2067,11 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>20</v>
-      </c>
-      <c r="B41" t="s">
-        <v>136</v>
-      </c>
       <c r="D41" s="6" t="s">
         <v>99</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -2077,41 +2080,41 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>20</v>
+      </c>
       <c r="B42" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F42" s="7" t="s">
-        <v>114</v>
+      <c r="F42" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>124</v>
-      </c>
-      <c r="C43" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>96</v>
+      <c r="F43" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -2120,7 +2123,7 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2134,7 +2137,7 @@
         <v>99</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -2143,18 +2146,21 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>139</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>100</v>
+        <v>124</v>
+      </c>
+      <c r="C45" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -2163,18 +2169,18 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>100</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -2183,15 +2189,18 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>140</v>
+      </c>
       <c r="D47" s="5" t="s">
         <v>100</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -2200,7 +2209,7 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2208,7 +2217,7 @@
         <v>100</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -2217,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2225,7 +2234,7 @@
         <v>100</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -2234,7 +2243,7 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2242,7 +2251,7 @@
         <v>100</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -2251,7 +2260,7 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2259,48 +2268,48 @@
         <v>100</v>
       </c>
       <c r="F51" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D52" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-      <c r="I51" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>17</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>141</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="D53" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52">
-        <v>0</v>
-      </c>
-      <c r="I52" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D53" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="G53">
         <v>0</v>
       </c>
@@ -2308,7 +2317,7 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2316,7 +2325,7 @@
         <v>100</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -2325,21 +2334,15 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>18</v>
-      </c>
-      <c r="B55" t="s">
-        <v>143</v>
-      </c>
       <c r="D55" s="5" t="s">
         <v>100</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -2348,41 +2351,64 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>18</v>
+      </c>
+      <c r="B56" t="s">
+        <v>143</v>
+      </c>
       <c r="D56" s="5" t="s">
         <v>100</v>
       </c>
       <c r="F56" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D57" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D57" s="6" t="s">
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D58" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F57" s="2" t="s">
+      <c r="F58" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="I57" t="s">
-        <v>160</v>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
access gateway switches step1
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6930" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -896,8 +896,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -915,7 +915,7 @@
       <c r="A1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1052,8 +1052,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added isl and switches to portcmd
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,21 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6930" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6930"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
     <sheet name="service_tables" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$I$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$I$62</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="175">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -540,6 +540,9 @@
   </si>
   <si>
     <t>DATA ANALYSIS 2. BLADE CHASSIS</t>
+  </si>
+  <si>
+    <t>report_columns_usage</t>
   </si>
 </sst>
 </file>
@@ -563,7 +566,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -600,6 +603,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -613,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -623,6 +632,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -930,8 +940,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,7 +961,7 @@
       <c r="A1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1098,10 +1108,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29:H42"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2030,7 +2040,7 @@
       <c r="D36" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="9" t="s">
         <v>170</v>
       </c>
       <c r="G36">
@@ -2155,31 +2165,25 @@
       <c r="D43" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="9" t="s">
         <v>69</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>20</v>
-      </c>
-      <c r="B44" t="s">
-        <v>136</v>
-      </c>
       <c r="D44" s="6" t="s">
         <v>99</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>93</v>
+        <v>174</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -2188,24 +2192,27 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>20</v>
+      </c>
       <c r="B45" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F45" s="8" t="s">
-        <v>114</v>
+      <c r="F45" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" t="s">
         <v>162</v>
@@ -2213,16 +2220,13 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>124</v>
-      </c>
-      <c r="C46" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>96</v>
+      <c r="F46" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -2244,8 +2248,8 @@
       <c r="D47" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F47" s="7" t="s">
-        <v>97</v>
+      <c r="F47" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -2258,11 +2262,17 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" t="s">
+        <v>137</v>
+      </c>
       <c r="D48" s="6" t="s">
         <v>99</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>168</v>
+        <v>97</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -2275,14 +2285,11 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>139</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>104</v>
+      <c r="D49" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>168</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -2296,13 +2303,13 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>100</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -2315,11 +2322,14 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>140</v>
+      </c>
       <c r="D51" s="5" t="s">
         <v>100</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -2336,7 +2346,7 @@
         <v>100</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -2353,7 +2363,7 @@
         <v>100</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -2370,7 +2380,7 @@
         <v>100</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -2387,7 +2397,7 @@
         <v>100</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -2400,34 +2410,34 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="D56" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>17</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>141</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D57" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F56" s="2" t="s">
+      <c r="F57" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D57" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -2444,7 +2454,7 @@
         <v>100</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -2457,17 +2467,11 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>18</v>
-      </c>
-      <c r="B59" t="s">
-        <v>143</v>
-      </c>
       <c r="D59" s="5" t="s">
         <v>100</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -2476,15 +2480,21 @@
         <v>0</v>
       </c>
       <c r="I59" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>18</v>
+      </c>
+      <c r="B60" t="s">
+        <v>143</v>
+      </c>
       <c r="D60" s="5" t="s">
         <v>100</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -2497,19 +2507,36 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D61" s="6" t="s">
+      <c r="D61" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D62" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F61" s="2" t="s">
+      <c r="F62" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-      <c r="I61" t="s">
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62" t="s">
         <v>161</v>
       </c>
     </row>

</xml_diff>

<commit_message>
npiv report table added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6930"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="175">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -308,9 +308,6 @@
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\SF\packed_sshow\</t>
   </si>
   <si>
-    <t>nsshow_aggregated</t>
-  </si>
-  <si>
     <t>nsshow_unsplit</t>
   </si>
   <si>
@@ -543,6 +540,9 @@
   </si>
   <si>
     <t>report_columns_usage</t>
+  </si>
+  <si>
+    <t>NPIV</t>
   </si>
 </sst>
 </file>
@@ -940,8 +940,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +961,7 @@
       <c r="A1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>83</v>
       </c>
     </row>
@@ -970,13 +970,13 @@
         <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
         <v>86</v>
@@ -1008,13 +1008,13 @@
         <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F3" t="s">
         <v>88</v>
@@ -1046,13 +1046,13 @@
         <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F4" t="s">
         <v>87</v>
@@ -1084,16 +1084,16 @@
         <v>89</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F5" t="s">
         <v>90</v>
       </c>
       <c r="I5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L5" t="s">
         <v>94</v>
@@ -1110,8 +1110,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,10 +1133,10 @@
         <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
@@ -1151,7 +1151,7 @@
         <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1159,10 +1159,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -1177,7 +1177,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1185,10 +1185,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -1203,7 +1203,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1211,11 +1211,11 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -1230,7 +1230,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1238,11 +1238,11 @@
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -1257,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1265,11 +1265,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1284,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1292,11 +1292,11 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -1311,7 +1311,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1319,13 +1319,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
@@ -1340,7 +1340,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1348,13 +1348,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E9" t="s">
         <v>40</v>
@@ -1369,7 +1369,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1377,13 +1377,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
@@ -1398,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1406,13 +1406,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -1427,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1435,13 +1435,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -1456,7 +1456,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1464,13 +1464,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
@@ -1485,7 +1485,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1493,13 +1493,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E14" t="s">
         <v>34</v>
@@ -1514,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1522,13 +1522,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E15" t="s">
         <v>35</v>
@@ -1543,7 +1543,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1551,13 +1551,13 @@
         <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E16" t="s">
         <v>36</v>
@@ -1572,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1580,13 +1580,13 @@
         <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E17" t="s">
         <v>43</v>
@@ -1601,7 +1601,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1609,13 +1609,13 @@
         <v>11</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -1630,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1638,13 +1638,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E19" t="s">
         <v>17</v>
@@ -1659,7 +1659,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1667,13 +1667,13 @@
         <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>45</v>
@@ -1685,7 +1685,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1693,13 +1693,13 @@
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>46</v>
@@ -1711,7 +1711,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1719,13 +1719,13 @@
         <v>12</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>47</v>
@@ -1737,18 +1737,18 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>48</v>
@@ -1760,18 +1760,18 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>49</v>
@@ -1783,7 +1783,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1791,13 +1791,13 @@
         <v>13</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>50</v>
@@ -1809,18 +1809,18 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>51</v>
@@ -1832,18 +1832,18 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>52</v>
@@ -1855,18 +1855,18 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>54</v>
@@ -1878,18 +1878,18 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>53</v>
@@ -1901,7 +1901,7 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1909,13 +1909,13 @@
         <v>19</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>91</v>
@@ -1927,18 +1927,18 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>92</v>
@@ -1950,21 +1950,21 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -1973,7 +1973,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1981,10 +1981,10 @@
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>55</v>
@@ -1996,12 +1996,12 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D34" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>56</v>
@@ -2013,12 +2013,12 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D35" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>57</v>
@@ -2030,35 +2030,35 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
         <v>172</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D37" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -2067,7 +2067,7 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2075,13 +2075,13 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>144</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>62</v>
+        <v>143</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -2090,15 +2090,15 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D39" s="5" t="s">
-        <v>100</v>
+      <c r="D39" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>63</v>
+        <v>173</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -2107,15 +2107,15 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D40" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -2124,15 +2124,15 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D41" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -2141,50 +2141,50 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D42" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F42" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D43" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D44" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D43" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G43">
-        <v>1</v>
-      </c>
-      <c r="H43">
-        <v>1</v>
-      </c>
-      <c r="I43" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D44" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="G44">
         <v>0</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2200,33 +2200,33 @@
         <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F45" s="9" t="s">
         <v>93</v>
       </c>
       <c r="G45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -2235,61 +2235,58 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D47" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D48" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>138</v>
+      </c>
+      <c r="D49" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-      <c r="I47" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>124</v>
-      </c>
-      <c r="C48" t="s">
-        <v>137</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-      <c r="I48" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D49" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>168</v>
+      <c r="F49" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -2298,7 +2295,7 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2306,10 +2303,10 @@
         <v>139</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -2318,15 +2315,12 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>140</v>
-      </c>
       <c r="D51" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>106</v>
@@ -2338,12 +2332,12 @@
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D52" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>107</v>
@@ -2355,12 +2349,12 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D53" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>108</v>
@@ -2372,12 +2366,12 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D54" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>109</v>
@@ -2389,12 +2383,12 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D55" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>110</v>
@@ -2406,24 +2400,24 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D56" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>111</v>
+        <v>174</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2431,12 +2425,12 @@
         <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F57" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F57" s="9" t="s">
         <v>61</v>
       </c>
       <c r="G57">
@@ -2446,12 +2440,12 @@
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D58" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>67</v>
@@ -2463,12 +2457,12 @@
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D59" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>68</v>
@@ -2480,7 +2474,7 @@
         <v>0</v>
       </c>
       <c r="I59" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2488,13 +2482,13 @@
         <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>143</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>70</v>
+        <v>142</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -2503,33 +2497,33 @@
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D61" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F61" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D62" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-      <c r="I61" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D62" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F62" s="9" t="s">
-        <v>72</v>
-      </c>
       <c r="G62">
         <v>0</v>
       </c>
@@ -2537,7 +2531,7 @@
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sfp check added for non fabric switches
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -11,14 +11,14 @@
     <sheet name="service_tables" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$I$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$I$66</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="185">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -203,9 +203,6 @@
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Uralss</t>
   </si>
   <si>
-    <t>fabric_statistics</t>
-  </si>
-  <si>
     <t>Коммутаторы</t>
   </si>
   <si>
@@ -485,9 +482,6 @@
     <t>step_info</t>
   </si>
   <si>
-    <t>DATA ANALYSIS 2. AGGREGATED SWITCH PARAMETERS</t>
-  </si>
-  <si>
     <t>DATA COLLECTION 3. SWITCH PARAMETERS</t>
   </si>
   <si>
@@ -500,15 +494,6 @@
     <t>blade_vc</t>
   </si>
   <si>
-    <t>DATA ANALYSIS 3. INTERSWITCH AND INTERFABRIC CONNECTIONS</t>
-  </si>
-  <si>
-    <t>DATA ANALYSIS 4. FABRIC DEVICES IDENTIFICATION</t>
-  </si>
-  <si>
-    <t>DATA ANALYSIS 5. FABRIC STATISTICS</t>
-  </si>
-  <si>
     <t>gosznak</t>
   </si>
   <si>
@@ -543,6 +528,51 @@
   </si>
   <si>
     <t>NPIV</t>
+  </si>
+  <si>
+    <t>analysis_err_sfp_cfg</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 5. PORT ERRORS, TRANSCEIVER SUPPORT, PORT CONFIGURATION</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 6. FABRIC STATISTICS</t>
+  </si>
+  <si>
+    <t>port_complete</t>
+  </si>
+  <si>
+    <t>Ошибки</t>
+  </si>
+  <si>
+    <t>Параметры_SFP</t>
+  </si>
+  <si>
+    <t>Параметры_портов</t>
+  </si>
+  <si>
+    <t>statistics</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 3. AGGREGATED SWITCH PARAMETERS</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 4. INTERSWITCH AND INTERFABRIC CONNECTIONS</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 5. FABRIC DEVICES IDENTIFICATION</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 6. PORT ERRORS, TRANSCEIVER SUPPORT, PORT CONFIGURATION</t>
+  </si>
+  <si>
+    <t>switch</t>
+  </si>
+  <si>
+    <t>chassis</t>
+  </si>
+  <si>
+    <t>maps</t>
   </si>
 </sst>
 </file>
@@ -940,8 +970,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,36 +989,36 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>5</v>
@@ -1000,33 +1030,33 @@
         <v>58</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G3" t="s">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J3" t="s">
         <v>4</v>
@@ -1038,33 +1068,33 @@
         <v>60</v>
       </c>
       <c r="M3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J4" t="s">
         <v>3</v>
@@ -1076,27 +1106,27 @@
         <v>59</v>
       </c>
       <c r="M4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" t="s">
         <v>89</v>
       </c>
-      <c r="C5" t="s">
-        <v>166</v>
-      </c>
-      <c r="E5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F5" t="s">
-        <v>90</v>
-      </c>
       <c r="I5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1108,10 +1138,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,10 +1163,10 @@
         <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
@@ -1151,7 +1181,7 @@
         <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1159,10 +1189,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -1177,7 +1207,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1185,10 +1215,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -1203,7 +1233,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1211,11 +1241,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="4"/>
+        <v>118</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>183</v>
+      </c>
       <c r="D4" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -1230,7 +1262,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1238,11 +1270,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="4"/>
+        <v>120</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>182</v>
+      </c>
       <c r="D5" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -1257,7 +1291,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1265,11 +1299,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="4"/>
+        <v>120</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>182</v>
+      </c>
       <c r="D6" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1284,7 +1320,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1292,11 +1328,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" s="4"/>
+        <v>116</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>184</v>
+      </c>
       <c r="D7" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -1311,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1319,13 +1357,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
@@ -1340,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1348,13 +1386,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E9" t="s">
         <v>40</v>
@@ -1369,7 +1407,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1377,13 +1415,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
@@ -1398,7 +1436,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1406,13 +1444,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -1427,7 +1465,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1435,13 +1473,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -1456,7 +1494,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1464,13 +1502,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
@@ -1485,7 +1523,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1493,13 +1531,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E14" t="s">
         <v>34</v>
@@ -1514,7 +1552,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1522,13 +1560,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E15" t="s">
         <v>35</v>
@@ -1543,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1551,13 +1589,13 @@
         <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E16" t="s">
         <v>36</v>
@@ -1572,7 +1610,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1580,13 +1618,13 @@
         <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E17" t="s">
         <v>43</v>
@@ -1601,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1609,13 +1647,13 @@
         <v>11</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -1630,7 +1668,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1638,13 +1676,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E19" t="s">
         <v>17</v>
@@ -1659,7 +1697,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1667,13 +1705,13 @@
         <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>45</v>
@@ -1685,7 +1723,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1693,13 +1731,13 @@
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>46</v>
@@ -1711,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1719,13 +1757,13 @@
         <v>12</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>47</v>
@@ -1737,18 +1775,18 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>48</v>
@@ -1760,18 +1798,18 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>49</v>
@@ -1783,7 +1821,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1791,13 +1829,13 @@
         <v>13</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>50</v>
@@ -1809,18 +1847,18 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>51</v>
@@ -1832,18 +1870,18 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>52</v>
@@ -1855,18 +1893,18 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>54</v>
@@ -1878,18 +1916,18 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>53</v>
@@ -1901,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1909,16 +1947,16 @@
         <v>19</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -1927,21 +1965,21 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1950,21 +1988,21 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -1973,7 +2011,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1981,12 +2019,12 @@
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F33" s="9" t="s">
         <v>55</v>
       </c>
       <c r="G33">
@@ -1996,14 +2034,14 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D34" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F34" s="8" t="s">
         <v>56</v>
       </c>
       <c r="G34">
@@ -2013,14 +2051,14 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D35" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F35" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>57</v>
       </c>
       <c r="G35">
@@ -2030,18 +2068,18 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -2050,15 +2088,15 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D37" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -2067,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2075,13 +2113,13 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -2090,15 +2128,15 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D39" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -2107,15 +2145,15 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D40" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -2124,15 +2162,15 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D41" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -2141,15 +2179,15 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D42" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -2158,15 +2196,15 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D43" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -2175,15 +2213,15 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D44" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -2192,81 +2230,78 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
+        <v>18</v>
+      </c>
+      <c r="B45" t="s">
+        <v>141</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D46" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D47" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>20</v>
       </c>
-      <c r="B45" t="s">
-        <v>135</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>137</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>123</v>
-      </c>
-      <c r="C47" t="s">
-        <v>136</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-      <c r="I47" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>134</v>
+      </c>
       <c r="D48" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>167</v>
+        <v>97</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -2275,18 +2310,18 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>138</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>103</v>
+        <v>136</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>112</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -2295,18 +2330,21 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>139</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>105</v>
+        <v>122</v>
+      </c>
+      <c r="C50" t="s">
+        <v>135</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -2315,15 +2353,15 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D51" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>106</v>
+      <c r="D51" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -2332,15 +2370,18 @@
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>137</v>
+      </c>
       <c r="D52" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -2349,15 +2390,18 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>138</v>
+      </c>
       <c r="D53" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -2366,15 +2410,15 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D54" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -2383,15 +2427,15 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D55" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -2400,15 +2444,15 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D56" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>174</v>
+        <v>107</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -2417,78 +2461,69 @@
         <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>17</v>
-      </c>
-      <c r="B57" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F57" s="9" t="s">
-        <v>61</v>
+      <c r="F57" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="G57">
         <v>0</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D58" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D59" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>68</v>
+        <v>169</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>18</v>
-      </c>
       <c r="B60" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>72</v>
+        <v>173</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -2497,15 +2532,15 @@
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D61" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>70</v>
+        <v>174</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -2514,15 +2549,15 @@
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D62" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>71</v>
+        <v>175</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -2531,7 +2566,81 @@
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>160</v>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D63" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>17</v>
+      </c>
+      <c r="B64" t="s">
+        <v>139</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="65" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D65" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="66" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D66" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comments added to analysis_zoning
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
     <sheet name="service_tables" sheetId="2" r:id="rId2"/>
+    <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$I$70</definedName>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="196">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -591,6 +592,21 @@
   </si>
   <si>
     <t>Псевдонимы</t>
+  </si>
+  <si>
+    <t>analysis_zoning_derived_data</t>
+  </si>
+  <si>
+    <t>analysis_zoning_processed_data</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Faberliс\Jul 2020</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Faberlic</t>
+  </si>
+  <si>
+    <t>Faberlic</t>
   </si>
 </sst>
 </file>
@@ -986,164 +1002,173 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="69" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="5" width="111.5703125" customWidth="1"/>
-    <col min="6" max="6" width="72.5703125" customWidth="1"/>
-    <col min="7" max="9" width="64.7109375" customWidth="1"/>
-    <col min="10" max="10" width="54.5703125" customWidth="1"/>
-    <col min="11" max="11" width="75.42578125" customWidth="1"/>
-    <col min="12" max="12" width="58.140625" customWidth="1"/>
+    <col min="1" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="69" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="111.5703125" customWidth="1"/>
+    <col min="7" max="7" width="72.5703125" customWidth="1"/>
+    <col min="8" max="10" width="64.7109375" customWidth="1"/>
+    <col min="11" max="11" width="54.5703125" customWidth="1"/>
+    <col min="12" max="12" width="75.42578125" customWidth="1"/>
+    <col min="13" max="13" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" t="s">
         <v>158</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>113</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>99</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" t="s">
         <v>160</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>115</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>100</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>87</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>76</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>74</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>4</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>25</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>60</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" t="s">
         <v>159</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>114</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>110</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>86</v>
       </c>
-      <c r="G4" t="s">
-        <v>0</v>
-      </c>
       <c r="H4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
         <v>75</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>73</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>3</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>24</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>59</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>161</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>111</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>89</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>101</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1159,7 +1184,7 @@
   <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2736,4 +2761,118 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fabric statistics module refactoring
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -12,14 +12,14 @@
     <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$I$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$I$68</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="199">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -222,9 +222,6 @@
     <t>Статистика</t>
   </si>
   <si>
-    <t>Статистика_Итого</t>
-  </si>
-  <si>
     <t>switch_params_aggregated</t>
   </si>
   <si>
@@ -537,9 +534,6 @@
     <t>DATA ANALYSIS 5. PORT ERRORS, TRANSCEIVER SUPPORT, PORT CONFIGURATION</t>
   </si>
   <si>
-    <t>DATA ANALYSIS 6. FABRIC STATISTICS</t>
-  </si>
-  <si>
     <t>port_complete</t>
   </si>
   <si>
@@ -607,6 +601,21 @@
   </si>
   <si>
     <t>Faberlic</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Regard\itc48</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Regard</t>
+  </si>
+  <si>
+    <t>Липецк ИТЦ - Регард</t>
+  </si>
+  <si>
+    <t>zonemember_statistics</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 7. FABRIC STATISTICS</t>
   </si>
 </sst>
 </file>
@@ -1002,174 +1011,184 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="69" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" customWidth="1"/>
-    <col min="6" max="6" width="111.5703125" customWidth="1"/>
-    <col min="7" max="7" width="72.5703125" customWidth="1"/>
-    <col min="8" max="10" width="64.7109375" customWidth="1"/>
-    <col min="11" max="11" width="54.5703125" customWidth="1"/>
-    <col min="12" max="12" width="75.42578125" customWidth="1"/>
-    <col min="13" max="13" width="58.140625" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" customWidth="1"/>
+    <col min="5" max="5" width="69" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" customWidth="1"/>
+    <col min="7" max="7" width="111.5703125" customWidth="1"/>
+    <col min="8" max="8" width="72.5703125" customWidth="1"/>
+    <col min="9" max="11" width="64.7109375" customWidth="1"/>
+    <col min="12" max="12" width="54.5703125" customWidth="1"/>
+    <col min="13" max="13" width="75.42578125" customWidth="1"/>
+    <col min="14" max="14" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" t="s">
+        <v>86</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2" t="s">
-        <v>195</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" t="s">
         <v>158</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F4" t="s">
         <v>113</v>
       </c>
-      <c r="F2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="G4" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="I4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" t="s">
         <v>72</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="L4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" t="s">
+        <v>59</v>
+      </c>
+      <c r="O4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" t="s">
         <v>160</v>
       </c>
-      <c r="E3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H5" t="s">
+        <v>88</v>
+      </c>
+      <c r="K5" t="s">
         <v>100</v>
       </c>
-      <c r="G3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J3" t="s">
-        <v>74</v>
-      </c>
-      <c r="K3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" t="s">
-        <v>60</v>
-      </c>
-      <c r="N3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D4" t="s">
-        <v>159</v>
-      </c>
-      <c r="E4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>75</v>
-      </c>
-      <c r="J4" t="s">
-        <v>73</v>
-      </c>
-      <c r="K4" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" t="s">
-        <v>161</v>
-      </c>
-      <c r="F5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G5" t="s">
-        <v>89</v>
-      </c>
-      <c r="J5" t="s">
-        <v>101</v>
-      </c>
-      <c r="M5" t="s">
-        <v>93</v>
+      <c r="N5" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1183,8 +1202,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,10 +1225,10 @@
         <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
@@ -1224,7 +1243,7 @@
         <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1232,10 +1251,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -1250,7 +1269,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1258,10 +1277,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -1276,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1284,13 +1303,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -1305,7 +1324,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1313,13 +1332,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -1334,7 +1353,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1342,13 +1361,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1363,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1371,13 +1390,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -1392,7 +1411,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1400,13 +1419,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
@@ -1421,7 +1440,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1429,13 +1448,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E9" t="s">
         <v>40</v>
@@ -1450,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1458,13 +1477,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
@@ -1479,7 +1498,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1487,13 +1506,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -1508,7 +1527,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1516,13 +1535,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -1537,7 +1556,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1545,13 +1564,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
@@ -1566,7 +1585,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1574,13 +1593,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E14" t="s">
         <v>34</v>
@@ -1595,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1603,13 +1622,13 @@
         <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E15" t="s">
         <v>35</v>
@@ -1624,7 +1643,7 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1632,13 +1651,13 @@
         <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E16" t="s">
         <v>36</v>
@@ -1653,7 +1672,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1661,13 +1680,13 @@
         <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E17" t="s">
         <v>43</v>
@@ -1682,7 +1701,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1690,13 +1709,13 @@
         <v>11</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -1711,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1719,13 +1738,13 @@
         <v>12</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E19" t="s">
         <v>17</v>
@@ -1740,7 +1759,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1748,13 +1767,13 @@
         <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>45</v>
@@ -1766,7 +1785,7 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1774,13 +1793,13 @@
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>46</v>
@@ -1792,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1800,13 +1819,13 @@
         <v>12</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>47</v>
@@ -1818,18 +1837,18 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>48</v>
@@ -1841,18 +1860,18 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>49</v>
@@ -1864,7 +1883,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1872,13 +1891,13 @@
         <v>13</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>50</v>
@@ -1890,18 +1909,18 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>51</v>
@@ -1913,18 +1932,18 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>52</v>
@@ -1936,18 +1955,18 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>54</v>
@@ -1959,18 +1978,18 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>53</v>
@@ -1982,7 +2001,7 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1990,16 +2009,16 @@
         <v>19</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -2008,21 +2027,21 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -2031,21 +2050,21 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -2054,7 +2073,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2062,10 +2081,10 @@
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>55</v>
@@ -2077,12 +2096,12 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D34" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>56</v>
@@ -2094,12 +2113,12 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D35" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>57</v>
@@ -2111,35 +2130,35 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>165</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
         <v>166</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D37" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -2148,7 +2167,7 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2156,13 +2175,13 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -2171,15 +2190,15 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D39" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -2188,12 +2207,12 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D40" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>61</v>
@@ -2205,12 +2224,12 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D41" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>62</v>
@@ -2222,12 +2241,12 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D42" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>63</v>
@@ -2239,12 +2258,12 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D43" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>65</v>
@@ -2256,12 +2275,12 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D44" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>64</v>
@@ -2273,7 +2292,7 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2281,13 +2300,13 @@
         <v>18</v>
       </c>
       <c r="B45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -2296,15 +2315,15 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D46" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -2313,15 +2332,15 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D47" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -2330,7 +2349,7 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2338,426 +2357,427 @@
         <v>20</v>
       </c>
       <c r="B48" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50" t="s">
         <v>134</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D50" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D51" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>136</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F48" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-      <c r="I48" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>136</v>
-      </c>
-      <c r="D49" s="6" t="s">
+      <c r="F52" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>137</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F49" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-      <c r="I49" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>122</v>
-      </c>
-      <c r="C50" t="s">
-        <v>135</v>
-      </c>
-      <c r="D50" s="6" t="s">
+      <c r="F53" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D54" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F50" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-      <c r="I50" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D51" s="6" t="s">
+      <c r="F54" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D55" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F51" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-      <c r="I51" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>137</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52">
-        <v>0</v>
-      </c>
-      <c r="I52" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="F55" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D56" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D57" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D58" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D59" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>169</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D61" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D62" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D63" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>183</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D65" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D66" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F66" t="s">
+        <v>197</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D67" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D68" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>17</v>
+      </c>
+      <c r="B69" t="s">
         <v>138</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="I53" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D54" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-      <c r="H54">
-        <v>0</v>
-      </c>
-      <c r="I54" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D55" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
-      <c r="I55" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D56" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D57" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="I57" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D58" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="G58">
-        <v>0</v>
-      </c>
-      <c r="H58">
-        <v>0</v>
-      </c>
-      <c r="I58" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D59" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>170</v>
-      </c>
-      <c r="D60" s="6" t="s">
+      <c r="D69" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D70" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F60" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="G60">
-        <v>0</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="I60" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D61" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-      <c r="I61" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D62" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G62">
+      <c r="F70" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G70">
         <v>1</v>
       </c>
-      <c r="H62">
-        <v>1</v>
-      </c>
-      <c r="I62" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D63" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="G63">
-        <v>0</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
-      <c r="I63" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>17</v>
-      </c>
-      <c r="B64" t="s">
-        <v>139</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F64" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="G64">
-        <v>0</v>
-      </c>
-      <c r="H64">
-        <v>0</v>
-      </c>
-      <c r="I64" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D65" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G65">
-        <v>0</v>
-      </c>
-      <c r="H65">
-        <v>0</v>
-      </c>
-      <c r="I65" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D66" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G66">
-        <v>0</v>
-      </c>
-      <c r="H66">
-        <v>0</v>
-      </c>
-      <c r="I66" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>185</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="G67">
-        <v>0</v>
-      </c>
-      <c r="H67">
-        <v>0</v>
-      </c>
-      <c r="I67" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D68" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F68" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-      <c r="H68">
-        <v>0</v>
-      </c>
-      <c r="I68" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D69" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-      <c r="H69">
-        <v>0</v>
-      </c>
-      <c r="I69" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D70" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
       <c r="H70">
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I68"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -2765,6 +2785,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2779,15 +2800,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>50</v>
@@ -2795,7 +2816,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>51</v>
@@ -2803,7 +2824,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>52</v>
@@ -2811,7 +2832,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>54</v>
@@ -2819,7 +2840,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2839,7 +2860,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2864,7 +2885,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
compare zone configs report tables added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="200">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -616,6 +616,9 @@
   </si>
   <si>
     <t>DATA ANALYSIS 7. FABRIC STATISTICS</t>
+  </si>
+  <si>
+    <t>Зонирование_A&amp;B</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1017,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1200,10 +1203,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2662,7 +2665,7 @@
         <v>0</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I64" t="s">
         <v>185</v>
@@ -2686,8 +2689,8 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D66" s="5" t="s">
-        <v>97</v>
+      <c r="D66" s="6" t="s">
+        <v>96</v>
       </c>
       <c r="F66" t="s">
         <v>197</v>
@@ -2696,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I66" t="s">
         <v>185</v>
@@ -2710,7 +2713,7 @@
         <v>187</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -2727,7 +2730,7 @@
         <v>188</v>
       </c>
       <c r="G68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -2737,42 +2740,59 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69">
+      <c r="D69" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70">
         <v>17</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>138</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="D70" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F69" s="9" t="s">
+      <c r="F70" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-      <c r="H69">
-        <v>1</v>
-      </c>
-      <c r="I69" t="s">
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D70" s="5" t="s">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D71" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G70">
-        <v>1</v>
-      </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
-      <c r="I70" t="s">
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71" t="s">
         <v>198</v>
       </c>
     </row>

</xml_diff>

<commit_message>
table of contents added. zoning analysis refactoring
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -12,14 +12,14 @@
     <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$I$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$74</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="230">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -219,9 +219,6 @@
     <t>Параметры_коммутаторов</t>
   </si>
   <si>
-    <t>Статистика</t>
-  </si>
-  <si>
     <t>switch_params_aggregated</t>
   </si>
   <si>
@@ -534,9 +531,6 @@
     <t>DATA ANALYSIS 5. PORT ERRORS, TRANSCEIVER SUPPORT, PORT CONFIGURATION</t>
   </si>
   <si>
-    <t>port_complete</t>
-  </si>
-  <si>
     <t>Ошибки</t>
   </si>
   <si>
@@ -546,9 +540,6 @@
     <t>Параметры_портов</t>
   </si>
   <si>
-    <t>statistics</t>
-  </si>
-  <si>
     <t>DATA ANALYSIS 3. AGGREGATED SWITCH PARAMETERS</t>
   </si>
   <si>
@@ -619,6 +610,105 @@
   </si>
   <si>
     <t>Зонирование_A&amp;B</t>
+  </si>
+  <si>
+    <t>Порты_не_в_зонах</t>
+  </si>
+  <si>
+    <t>fabric_statistics</t>
+  </si>
+  <si>
+    <t>Статистика_фабрики</t>
+  </si>
+  <si>
+    <t>Статистика_зон</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Перечень коммутаторов</t>
+  </si>
+  <si>
+    <t>Распределение коммутаторов по фабрикам</t>
+  </si>
+  <si>
+    <t>Лицензированные функции коммутаторов</t>
+  </si>
+  <si>
+    <t>Перечень серверов в сети хранения данных</t>
+  </si>
+  <si>
+    <t>Перечень систем хранения данных</t>
+  </si>
+  <si>
+    <t>Перечень ленточных библиотек</t>
+  </si>
+  <si>
+    <t>Информация о подключении портов NPIV</t>
+  </si>
+  <si>
+    <t>Статистика ошибок на портах коммутаторов</t>
+  </si>
+  <si>
+    <t>Перечень Blade систем</t>
+  </si>
+  <si>
+    <t>Глобальные параметры фабрик</t>
+  </si>
+  <si>
+    <t>Системные параметры коммутаторов</t>
+  </si>
+  <si>
+    <t>Параметры межкоммутаторных соединений</t>
+  </si>
+  <si>
+    <t>Параметры межфабричных соединений</t>
+  </si>
+  <si>
+    <t>Версии микрокодов и драйверов HBA модулей серверов</t>
+  </si>
+  <si>
+    <t>Подключение систем хранения данных к сети</t>
+  </si>
+  <si>
+    <t>Подключение ленточных библиотек к сети</t>
+  </si>
+  <si>
+    <t>Подключение серверов к сети хранения данных</t>
+  </si>
+  <si>
+    <t>Параметры работы трансиверов</t>
+  </si>
+  <si>
+    <t>Настройка портов</t>
+  </si>
+  <si>
+    <t>Конфигурация зон</t>
+  </si>
+  <si>
+    <t>Конфигурация псевдонимов</t>
+  </si>
+  <si>
+    <t>Сравнение активной конфиграции зонирования подсетей А и В</t>
+  </si>
+  <si>
+    <t>Порты устройств, не входящие в конфигурацию зонирования</t>
+  </si>
+  <si>
+    <t>Статистическая информация о портах коммутаторов</t>
+  </si>
+  <si>
+    <t>Статистическая информация о зонах</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>portshow_zoned_aggregated</t>
+  </si>
+  <si>
+    <t>portshow_sfp_aggregated</t>
   </si>
 </sst>
 </file>
@@ -698,7 +788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -709,6 +799,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1016,8 +1107,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1036,42 +1127,42 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>5</v>
@@ -1083,39 +1174,39 @@
         <v>58</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I3" t="s">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L3" t="s">
         <v>4</v>
@@ -1127,39 +1218,39 @@
         <v>60</v>
       </c>
       <c r="O3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I4" t="s">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L4" t="s">
         <v>3</v>
@@ -1171,27 +1262,27 @@
         <v>59</v>
       </c>
       <c r="O4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" t="s">
+        <v>159</v>
+      </c>
+      <c r="G5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" t="s">
         <v>87</v>
       </c>
-      <c r="E5" t="s">
-        <v>160</v>
-      </c>
-      <c r="G5" t="s">
-        <v>110</v>
-      </c>
-      <c r="H5" t="s">
-        <v>88</v>
-      </c>
       <c r="K5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1203,10 +1294,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,10 +1308,11 @@
     <col min="6" max="6" width="45.5703125" customWidth="1"/>
     <col min="7" max="7" width="16.28515625" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="48.5703125" customWidth="1"/>
+    <col min="9" max="9" width="76.28515625" customWidth="1"/>
+    <col min="10" max="10" width="84.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -1228,15 +1320,15 @@
         <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -1246,18 +1338,21 @@
         <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -1272,18 +1367,21 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -1298,21 +1396,24 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -1327,21 +1428,24 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -1356,21 +1460,24 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -1385,21 +1492,24 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -1414,21 +1524,24 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E8" t="s">
         <v>16</v>
@@ -1443,21 +1556,24 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E9" t="s">
         <v>40</v>
@@ -1472,21 +1588,24 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
@@ -1501,21 +1620,24 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -1530,21 +1652,24 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -1559,21 +1684,24 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" t="s">
         <v>33</v>
@@ -1588,21 +1716,24 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E14" t="s">
         <v>34</v>
@@ -1617,21 +1748,24 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E15" t="s">
         <v>35</v>
@@ -1646,21 +1780,24 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E16" t="s">
         <v>36</v>
@@ -1675,21 +1812,24 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E17" t="s">
         <v>43</v>
@@ -1704,21 +1844,24 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E18" t="s">
         <v>32</v>
@@ -1733,21 +1876,24 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E19" t="s">
         <v>17</v>
@@ -1762,21 +1908,24 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>45</v>
@@ -1788,21 +1937,24 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>46</v>
@@ -1814,21 +1966,24 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>47</v>
@@ -1840,18 +1995,21 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>48</v>
@@ -1863,18 +2021,21 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>49</v>
@@ -1886,21 +2047,24 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>13</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>50</v>
@@ -1912,18 +2076,21 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>51</v>
@@ -1935,18 +2102,21 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>52</v>
@@ -1958,18 +2128,21 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>54</v>
@@ -1981,18 +2154,21 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>53</v>
@@ -2004,48 +2180,54 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>19</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F30" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>150</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="G31">
         <v>0</v>
       </c>
@@ -2053,21 +2235,24 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -2076,18 +2261,21 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>55</v>
@@ -2099,12 +2287,15 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D34" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>56</v>
@@ -2116,12 +2307,15 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D35" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>57</v>
@@ -2133,36 +2327,42 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
+        <v>161</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>164</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F36" s="9" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
         <v>165</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="J36" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D37" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F37" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D37" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="G37">
         <v>0</v>
       </c>
@@ -2170,52 +2370,61 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="J37" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D38" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
+        <v>173</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D39" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>173</v>
+      </c>
+      <c r="J39" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D40" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D39" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D40" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>61</v>
@@ -2227,12 +2436,15 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="J40" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D41" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>62</v>
@@ -2244,12 +2456,15 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="J41" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D42" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>63</v>
@@ -2261,12 +2476,15 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="J42" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D43" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>65</v>
@@ -2278,12 +2496,15 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="J43" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D44" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>64</v>
@@ -2295,56 +2516,65 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="J44" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>18</v>
       </c>
       <c r="B45" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D45" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45" t="s">
+        <v>174</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D46" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F45" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D46" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="F46" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
+        <v>174</v>
+      </c>
+      <c r="J46" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D47" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D47" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="G47">
         <v>0</v>
       </c>
@@ -2352,207 +2582,240 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="J47" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>20</v>
       </c>
       <c r="B48" t="s">
+        <v>132</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48" t="s">
+        <v>175</v>
+      </c>
+      <c r="J48" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>134</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49" t="s">
+        <v>175</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>120</v>
+      </c>
+      <c r="C50" t="s">
         <v>133</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D50" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50" t="s">
+        <v>175</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D51" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51" t="s">
+        <v>175</v>
+      </c>
+      <c r="J51" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F48" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-      <c r="I48" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>135</v>
-      </c>
-      <c r="D49" s="6" t="s">
+      <c r="F52" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52" t="s">
+        <v>175</v>
+      </c>
+      <c r="J52" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>136</v>
+      </c>
+      <c r="D53" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F49" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-      <c r="I49" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>121</v>
-      </c>
-      <c r="C50" t="s">
-        <v>134</v>
-      </c>
-      <c r="D50" s="6" t="s">
+      <c r="F53" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53" t="s">
+        <v>175</v>
+      </c>
+      <c r="J53" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D54" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F50" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-      <c r="I50" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D51" s="6" t="s">
+      <c r="F54" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54" t="s">
+        <v>175</v>
+      </c>
+      <c r="J54" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D55" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F51" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-      <c r="I51" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>136</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52">
-        <v>0</v>
-      </c>
-      <c r="I52" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>137</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
-      <c r="I53" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D54" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F54" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-      <c r="H54">
-        <v>0</v>
-      </c>
-      <c r="I54" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D55" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F55" s="2" t="s">
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55" t="s">
+        <v>175</v>
+      </c>
+      <c r="J55" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D56" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
-      <c r="I55" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D56" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F56" s="2" t="s">
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56" t="s">
+        <v>175</v>
+      </c>
+      <c r="J56" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D57" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D57" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F57" s="2" t="s">
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57" t="s">
+        <v>175</v>
+      </c>
+      <c r="J57" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D58" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="I57" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D58" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="G58">
         <v>0</v>
       </c>
@@ -2560,87 +2823,102 @@
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="J58" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D59" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F59" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59" t="s">
+        <v>175</v>
+      </c>
+      <c r="J59" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>168</v>
       </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+      <c r="D60" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60" t="s">
+        <v>176</v>
+      </c>
+      <c r="J60" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D61" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61" t="s">
+        <v>176</v>
+      </c>
+      <c r="J61" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D62" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62" t="s">
         <v>169</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="J62" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D63" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F60" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="G60">
-        <v>0</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="I60" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D61" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F61" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-      <c r="I61" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D62" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G62">
-        <v>0</v>
-      </c>
-      <c r="H62">
-        <v>0</v>
-      </c>
-      <c r="I62" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D63" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>174</v>
-      </c>
       <c r="G63">
         <v>0</v>
       </c>
@@ -2648,69 +2926,81 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="J63" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64">
         <v>1</v>
       </c>
       <c r="I64" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="J64" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D65" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65">
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="J65" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D66" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F66" t="s">
-        <v>197</v>
+        <v>95</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>194</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D67" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
+      </c>
+      <c r="J66" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D67" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>228</v>
       </c>
       <c r="G67">
         <v>1</v>
@@ -2719,15 +3009,18 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="J67" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D68" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G68">
         <v>1</v>
@@ -2736,15 +3029,18 @@
         <v>0</v>
       </c>
       <c r="I68" t="s">
+        <v>182</v>
+      </c>
+      <c r="J68" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D69" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>185</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D69" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>199</v>
       </c>
       <c r="G69">
         <v>1</v>
@@ -2753,51 +3049,119 @@
         <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70">
+        <v>182</v>
+      </c>
+      <c r="J69" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D70" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70" t="s">
+        <v>182</v>
+      </c>
+      <c r="J70" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D71" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71" t="s">
+        <v>182</v>
+      </c>
+      <c r="J71" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D72" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72" t="s">
+        <v>182</v>
+      </c>
+      <c r="J72" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73">
         <v>17</v>
       </c>
-      <c r="B70" t="s">
-        <v>138</v>
-      </c>
-      <c r="D70" s="6" t="s">
+      <c r="B73" t="s">
+        <v>137</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73">
+        <v>1</v>
+      </c>
+      <c r="I73" t="s">
+        <v>195</v>
+      </c>
+      <c r="J73" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D74" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F70" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
-      <c r="I70" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D71" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G71">
-        <v>0</v>
-      </c>
-      <c r="H71">
-        <v>0</v>
-      </c>
-      <c r="I71" t="s">
-        <v>198</v>
+      <c r="F74" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74" t="s">
+        <v>195</v>
+      </c>
+      <c r="J74" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I68"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -2809,7 +3173,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2820,15 +3184,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>50</v>
@@ -2836,7 +3200,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>51</v>
@@ -2844,7 +3208,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>52</v>
@@ -2852,7 +3216,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>54</v>
@@ -2860,7 +3224,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2880,7 +3244,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2905,7 +3269,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AG principal added to NPIV table
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1171,7 +1171,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1196,7 +1196,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1392,8 +1392,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="C55" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2296,10 +2296,10 @@
         <v>249</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" t="s">
         <v>149</v>
@@ -2322,7 +2322,7 @@
         <v>250</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -3011,7 +3011,7 @@
         <v>166</v>
       </c>
       <c r="G62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -3180,7 +3180,7 @@
         <v>0</v>
       </c>
       <c r="H70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I70" t="s">
         <v>181</v>
@@ -3197,7 +3197,7 @@
         <v>183</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -3217,7 +3217,7 @@
         <v>184</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -3237,7 +3237,7 @@
         <v>192</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -3257,7 +3257,7 @@
         <v>193</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -3277,7 +3277,7 @@
         <v>240</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -3297,7 +3297,7 @@
         <v>242</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -3317,7 +3317,7 @@
         <v>196</v>
       </c>
       <c r="G77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -3337,7 +3337,7 @@
         <v>232</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -3403,7 +3403,7 @@
         <v>195</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H81">
         <v>0</v>
@@ -3416,6 +3416,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J81"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fabric labeliling module refactoring
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1171,7 +1171,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,8 +1392,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C55" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2458,7 +2458,7 @@
         <v>0</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" t="s">
         <v>160</v>
@@ -3011,7 +3011,7 @@
         <v>166</v>
       </c>
       <c r="G62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -3180,7 +3180,7 @@
         <v>0</v>
       </c>
       <c r="H70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I70" t="s">
         <v>181</v>
@@ -3197,7 +3197,7 @@
         <v>183</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -3217,7 +3217,7 @@
         <v>184</v>
       </c>
       <c r="G72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -3237,7 +3237,7 @@
         <v>192</v>
       </c>
       <c r="G73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -3257,7 +3257,7 @@
         <v>193</v>
       </c>
       <c r="G74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -3277,7 +3277,7 @@
         <v>240</v>
       </c>
       <c r="G75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -3297,7 +3297,7 @@
         <v>242</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -3317,7 +3317,7 @@
         <v>196</v>
       </c>
       <c r="G77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -3337,7 +3337,7 @@
         <v>232</v>
       </c>
       <c r="G78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -3403,7 +3403,7 @@
         <v>195</v>
       </c>
       <c r="G81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81">
         <v>0</v>
@@ -3416,7 +3416,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J81"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
device manual rename functionality added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -12,14 +12,14 @@
     <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$84</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="256">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -772,6 +772,21 @@
   </si>
   <si>
     <t>peerzone_effective</t>
+  </si>
+  <si>
+    <t>report_columns_usage_upd</t>
+  </si>
+  <si>
+    <t>device_rename</t>
+  </si>
+  <si>
+    <t>Manual device rename</t>
+  </si>
+  <si>
+    <t>manual</t>
+  </si>
+  <si>
+    <t>device_rename_form</t>
   </si>
 </sst>
 </file>
@@ -795,7 +810,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -838,6 +853,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -851,7 +872,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -863,6 +884,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1171,7 +1193,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1390,10 +1412,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="C27" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2458,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="s">
         <v>160</v>
@@ -2779,7 +2801,7 @@
         <v>0</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" t="s">
         <v>174</v>
@@ -2789,14 +2811,11 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>134</v>
-      </c>
       <c r="D52" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F52" s="8" t="s">
-        <v>110</v>
+      <c r="F52" s="2" t="s">
+        <v>251</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -2812,17 +2831,11 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>120</v>
-      </c>
-      <c r="C53" t="s">
-        <v>133</v>
-      </c>
       <c r="D53" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F53" s="7" t="s">
-        <v>93</v>
+      <c r="F53" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -2834,15 +2847,15 @@
         <v>174</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D54" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F54" s="7" t="s">
-        <v>159</v>
+      <c r="D54" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>255</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -2854,18 +2867,18 @@
         <v>174</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>135</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>100</v>
+        <v>134</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -2876,19 +2889,22 @@
       <c r="I55" t="s">
         <v>174</v>
       </c>
-      <c r="J55" t="s">
-        <v>201</v>
+      <c r="J55" s="10" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>136</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>102</v>
+        <v>120</v>
+      </c>
+      <c r="C56" t="s">
+        <v>133</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -2899,16 +2915,16 @@
       <c r="I56" t="s">
         <v>174</v>
       </c>
-      <c r="J56" t="s">
-        <v>202</v>
+      <c r="J56" s="10" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D57" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>103</v>
+      <c r="D57" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -2919,16 +2935,19 @@
       <c r="I57" t="s">
         <v>174</v>
       </c>
-      <c r="J57" t="s">
-        <v>203</v>
+      <c r="J57" s="10" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>135</v>
+      </c>
       <c r="D58" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -2940,15 +2959,18 @@
         <v>174</v>
       </c>
       <c r="J58" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>136</v>
+      </c>
       <c r="D59" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -2960,7 +2982,7 @@
         <v>174</v>
       </c>
       <c r="J59" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -2968,7 +2990,7 @@
         <v>96</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -2980,7 +3002,7 @@
         <v>174</v>
       </c>
       <c r="J60" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -2988,7 +3010,7 @@
         <v>96</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -3000,7 +3022,7 @@
         <v>174</v>
       </c>
       <c r="J61" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -3008,7 +3030,7 @@
         <v>96</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>166</v>
+        <v>105</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -3020,18 +3042,15 @@
         <v>174</v>
       </c>
       <c r="J62" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>167</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F63" s="9" t="s">
-        <v>224</v>
+      <c r="D63" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -3040,10 +3059,10 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>175</v>
-      </c>
-      <c r="J63" s="10" t="s">
-        <v>222</v>
+        <v>174</v>
+      </c>
+      <c r="J63" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -3051,7 +3070,7 @@
         <v>96</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>169</v>
+        <v>107</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -3060,121 +3079,124 @@
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J64" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D65" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F65" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65" t="s">
+        <v>174</v>
+      </c>
+      <c r="J65" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>167</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66" t="s">
+        <v>175</v>
+      </c>
+      <c r="J66" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D67" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67" t="s">
+        <v>175</v>
+      </c>
+      <c r="J67" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D68" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="G65">
-        <v>0</v>
-      </c>
-      <c r="H65">
-        <v>0</v>
-      </c>
-      <c r="I65" t="s">
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68" t="s">
         <v>168</v>
       </c>
-      <c r="J65" t="s">
+      <c r="J68" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D66" s="5" t="s">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D69" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G66">
-        <v>0</v>
-      </c>
-      <c r="H66">
-        <v>0</v>
-      </c>
-      <c r="I66" t="s">
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69" t="s">
         <v>168</v>
       </c>
-      <c r="J66" t="s">
+      <c r="J69" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
         <v>179</v>
       </c>
-      <c r="D67" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="G67">
-        <v>0</v>
-      </c>
-      <c r="H67">
-        <v>0</v>
-      </c>
-      <c r="I67" t="s">
-        <v>181</v>
-      </c>
-      <c r="J67" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D68" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F68" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-      <c r="H68">
-        <v>0</v>
-      </c>
-      <c r="I68" t="s">
-        <v>181</v>
-      </c>
-      <c r="J68" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D69" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F69" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-      <c r="H69">
-        <v>0</v>
-      </c>
-      <c r="I69" t="s">
-        <v>181</v>
-      </c>
-      <c r="J69" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D70" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -3189,12 +3211,12 @@
         <v>222</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D71" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>183</v>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D71" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>182</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -3205,16 +3227,16 @@
       <c r="I71" t="s">
         <v>181</v>
       </c>
-      <c r="J71" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D72" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>184</v>
+      <c r="J71" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D72" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>191</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -3225,16 +3247,16 @@
       <c r="I72" t="s">
         <v>181</v>
       </c>
-      <c r="J72" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D73" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>192</v>
+      <c r="J72" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D73" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -3245,16 +3267,16 @@
       <c r="I73" t="s">
         <v>181</v>
       </c>
-      <c r="J73" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J73" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D74" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -3266,15 +3288,15 @@
         <v>181</v>
       </c>
       <c r="J74" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D75" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>240</v>
+        <v>184</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -3286,15 +3308,15 @@
         <v>181</v>
       </c>
       <c r="J75" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D76" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>242</v>
+        <v>192</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -3306,15 +3328,15 @@
         <v>181</v>
       </c>
       <c r="J76" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D77" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -3326,15 +3348,15 @@
         <v>181</v>
       </c>
       <c r="J77" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D78" s="6" t="s">
-        <v>95</v>
+        <v>219</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D78" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -3343,75 +3365,135 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>245</v>
-      </c>
-      <c r="J78" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+      <c r="J78" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D79" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F79" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79" t="s">
+        <v>181</v>
+      </c>
+      <c r="J79" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D80" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80" t="s">
+        <v>181</v>
+      </c>
+      <c r="J80" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D81" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81" t="s">
+        <v>245</v>
+      </c>
+      <c r="J81" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D82" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="G79">
-        <v>0</v>
-      </c>
-      <c r="H79">
-        <v>0</v>
-      </c>
-      <c r="I79" t="s">
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82" t="s">
         <v>245</v>
       </c>
-      <c r="J79" t="s">
+      <c r="J82" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A80">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83">
         <v>17</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B83" t="s">
         <v>137</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="D83" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F80" s="9" t="s">
+      <c r="F83" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-      <c r="H80">
-        <v>0</v>
-      </c>
-      <c r="I80" t="s">
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83" t="s">
         <v>234</v>
       </c>
-      <c r="J80" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="81" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D81" s="5" t="s">
+      <c r="J83" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D84" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F84" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="G81">
-        <v>0</v>
-      </c>
-      <c r="H81">
-        <v>0</v>
-      </c>
-      <c r="I81" t="s">
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84" t="s">
         <v>234</v>
       </c>
-      <c r="J81" t="s">
+      <c r="J84" t="s">
         <v>220</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fabric statistics. device type in case of ISL absence
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1193,7 +1193,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,8 +1414,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C27" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
+      <selection activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2801,7 +2801,7 @@
         <v>0</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" t="s">
         <v>174</v>
@@ -3468,7 +3468,7 @@
         <v>0</v>
       </c>
       <c r="H83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I83" t="s">
         <v>234</v>
@@ -3485,7 +3485,7 @@
         <v>195</v>
       </c>
       <c r="G84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H84">
         <v>0</v>

</xml_diff>

<commit_message>
zone number count in statitics
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1193,7 +1193,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,7 +1218,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1414,8 +1414,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2801,7 +2801,7 @@
         <v>0</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" t="s">
         <v>174</v>
@@ -2927,7 +2927,7 @@
         <v>159</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -3468,7 +3468,7 @@
         <v>0</v>
       </c>
       <c r="H83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I83" t="s">
         <v>234</v>
@@ -3485,7 +3485,7 @@
         <v>195</v>
       </c>
       <c r="G84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H84">
         <v>0</v>

</xml_diff>

<commit_message>
active configuration statistics added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -12,14 +12,14 @@
     <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$86</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="264">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -787,6 +787,30 @@
   </si>
   <si>
     <t>device_rename_form</t>
+  </si>
+  <si>
+    <t>effective_cfg_statistics</t>
+  </si>
+  <si>
+    <t>Effective zoning configuration statistics</t>
+  </si>
+  <si>
+    <t>Статистика_конфигурации</t>
+  </si>
+  <si>
+    <t>Статистическая информация активной конфигурации зонирования</t>
+  </si>
+  <si>
+    <t>analysis_zoning_cfg_dashboard</t>
+  </si>
+  <si>
+    <t>analysis_zoning_aggregation</t>
+  </si>
+  <si>
+    <t>analysis_zoning_aggregation_aux_fn</t>
+  </si>
+  <si>
+    <t>analysis_zoning_statistics</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1217,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,7 +1242,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1412,10 +1436,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J84"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2801,7 +2825,7 @@
         <v>0</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" t="s">
         <v>174</v>
@@ -2927,7 +2951,7 @@
         <v>159</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -3212,6 +3236,9 @@
       </c>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>261</v>
+      </c>
       <c r="D71" s="6" t="s">
         <v>95</v>
       </c>
@@ -3232,6 +3259,9 @@
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>263</v>
+      </c>
       <c r="D72" s="6" t="s">
         <v>95</v>
       </c>
@@ -3252,6 +3282,9 @@
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>262</v>
+      </c>
       <c r="D73" s="6" t="s">
         <v>95</v>
       </c>
@@ -3272,11 +3305,14 @@
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D74" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>183</v>
+      <c r="B74" t="s">
+        <v>260</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>256</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -3287,8 +3323,8 @@
       <c r="I74" t="s">
         <v>181</v>
       </c>
-      <c r="J74" t="s">
-        <v>217</v>
+      <c r="J74" s="10" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
@@ -3296,7 +3332,7 @@
         <v>96</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -3308,7 +3344,7 @@
         <v>181</v>
       </c>
       <c r="J75" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.25">
@@ -3316,7 +3352,7 @@
         <v>96</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -3328,7 +3364,7 @@
         <v>181</v>
       </c>
       <c r="J76" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
@@ -3336,7 +3372,7 @@
         <v>96</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -3348,7 +3384,7 @@
         <v>181</v>
       </c>
       <c r="J77" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
@@ -3356,7 +3392,7 @@
         <v>96</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>240</v>
+        <v>193</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -3368,7 +3404,7 @@
         <v>181</v>
       </c>
       <c r="J78" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
@@ -3376,7 +3412,7 @@
         <v>96</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -3388,7 +3424,7 @@
         <v>181</v>
       </c>
       <c r="J79" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.25">
@@ -3396,7 +3432,7 @@
         <v>96</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>196</v>
+        <v>242</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -3408,27 +3444,27 @@
         <v>181</v>
       </c>
       <c r="J80" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D81" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81" t="s">
+        <v>181</v>
+      </c>
+      <c r="J81" t="s">
         <v>221</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D81" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="G81">
-        <v>0</v>
-      </c>
-      <c r="H81">
-        <v>0</v>
-      </c>
-      <c r="I81" t="s">
-        <v>245</v>
-      </c>
-      <c r="J81" s="10" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -3436,7 +3472,7 @@
         <v>96</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>233</v>
+        <v>258</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -3445,24 +3481,18 @@
         <v>0</v>
       </c>
       <c r="I82" t="s">
-        <v>245</v>
+        <v>181</v>
       </c>
       <c r="J82" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>17</v>
-      </c>
-      <c r="B83" t="s">
-        <v>137</v>
-      </c>
       <c r="D83" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F83" s="9" t="s">
-        <v>194</v>
+      <c r="F83" s="2" t="s">
+        <v>232</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -3471,7 +3501,7 @@
         <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="J83" s="10" t="s">
         <v>222</v>
@@ -3482,18 +3512,64 @@
         <v>96</v>
       </c>
       <c r="F84" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84" t="s">
+        <v>245</v>
+      </c>
+      <c r="J84" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>17</v>
+      </c>
+      <c r="B85" t="s">
+        <v>137</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85" t="s">
+        <v>234</v>
+      </c>
+      <c r="J85" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D86" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F86" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="G84">
-        <v>0</v>
-      </c>
-      <c r="H84">
-        <v>0</v>
-      </c>
-      <c r="I84" t="s">
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86" t="s">
         <v>234</v>
       </c>
-      <c r="J84" t="s">
+      <c r="J86" t="s">
         <v>220</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fabric label check for errors before saving added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="267">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -811,6 +811,15 @@
   </si>
   <si>
     <t>analysis_zoning_statistics</t>
+  </si>
+  <si>
+    <t>Rencredit</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Rencredit\SAN Assessment OCT2020</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Rencredit\Supportsave</t>
   </si>
 </sst>
 </file>
@@ -1214,31 +1223,32 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="72.28515625" customWidth="1"/>
-    <col min="4" max="4" width="61.7109375" customWidth="1"/>
-    <col min="5" max="5" width="60" customWidth="1"/>
-    <col min="6" max="6" width="38.140625" customWidth="1"/>
-    <col min="7" max="7" width="69" customWidth="1"/>
-    <col min="8" max="8" width="72.42578125" customWidth="1"/>
-    <col min="9" max="9" width="111.5703125" customWidth="1"/>
-    <col min="10" max="10" width="72.5703125" customWidth="1"/>
-    <col min="11" max="11" width="86.85546875" customWidth="1"/>
-    <col min="12" max="13" width="64.7109375" customWidth="1"/>
-    <col min="14" max="14" width="54.5703125" customWidth="1"/>
-    <col min="15" max="15" width="75.42578125" customWidth="1"/>
-    <col min="16" max="16" width="58.140625" customWidth="1"/>
+    <col min="3" max="3" width="76" customWidth="1"/>
+    <col min="4" max="4" width="72.28515625" customWidth="1"/>
+    <col min="5" max="5" width="61.7109375" customWidth="1"/>
+    <col min="6" max="6" width="60" customWidth="1"/>
+    <col min="7" max="7" width="38.140625" customWidth="1"/>
+    <col min="8" max="8" width="69" customWidth="1"/>
+    <col min="9" max="9" width="72.42578125" customWidth="1"/>
+    <col min="10" max="10" width="111.5703125" customWidth="1"/>
+    <col min="11" max="11" width="72.5703125" customWidth="1"/>
+    <col min="12" max="12" width="86.85546875" customWidth="1"/>
+    <col min="13" max="14" width="64.7109375" customWidth="1"/>
+    <col min="15" max="15" width="54.5703125" customWidth="1"/>
+    <col min="16" max="16" width="75.42578125" customWidth="1"/>
+    <col min="17" max="17" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
@@ -1246,184 +1256,193 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D2" t="s">
         <v>246</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>239</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>190</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>189</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>155</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>111</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>97</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>83</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D3" t="s">
         <v>248</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>238</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>227</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>188</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>157</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>113</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>98</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>85</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>74</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>72</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>4</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>25</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>60</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D4" t="s">
         <v>247</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>236</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>226</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>187</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>156</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>112</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>108</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>84</v>
       </c>
-      <c r="K4" t="s">
-        <v>0</v>
-      </c>
       <c r="L4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
         <v>73</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>71</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>3</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>24</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>59</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>237</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>158</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>109</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>87</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>99</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0</v>
       </c>
     </row>
@@ -1438,8 +1457,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2504,7 +2523,7 @@
         <v>0</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" t="s">
         <v>160</v>
@@ -3561,10 +3580,10 @@
         <v>195</v>
       </c>
       <c r="G86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I86" t="s">
         <v>234</v>
@@ -3585,7 +3604,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fabric label module refactoring
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="268">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -820,6 +820,9 @@
   </si>
   <si>
     <t>C:\Users\vlasenko\Documents\06.CONFIGS\Rencredit\Supportsave</t>
+  </si>
+  <si>
+    <t>Chassis parameters</t>
   </si>
 </sst>
 </file>
@@ -1457,8 +1460,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,7 +1595,7 @@
         <v>142</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>222</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
synergy servers and modules added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -12,14 +12,14 @@
     <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$88</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="277">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -823,6 +823,33 @@
   </si>
   <si>
     <t>Chassis parameters</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Rencredit\blades</t>
+  </si>
+  <si>
+    <t>synergy_meddler_folder</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Rencredit\synergy</t>
+  </si>
+  <si>
+    <t>collection_synergy</t>
+  </si>
+  <si>
+    <t>synergy_interconnect</t>
+  </si>
+  <si>
+    <t>synergy_servers</t>
+  </si>
+  <si>
+    <t>Synergy interconnect modules</t>
+  </si>
+  <si>
+    <t>Synergy servers and mezzanine</t>
+  </si>
+  <si>
+    <t>DATA COLLECTION 13. SYNERGY SYSTEMS</t>
   </si>
 </sst>
 </file>
@@ -1226,10 +1253,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,6 +1449,9 @@
       <c r="A5" s="3" t="s">
         <v>86</v>
       </c>
+      <c r="C5" t="s">
+        <v>268</v>
+      </c>
       <c r="E5" t="s">
         <v>237</v>
       </c>
@@ -1443,9 +1473,17 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>0</v>
       </c>
     </row>
@@ -1458,10 +1496,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="E40" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2510,57 +2548,65 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="B36" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
+        <v>276</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
+        <v>276</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>15</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>138</v>
       </c>
-      <c r="D36" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36" t="s">
-        <v>160</v>
-      </c>
-      <c r="J36" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D37" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37" t="s">
-        <v>160</v>
-      </c>
-      <c r="J37" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D38" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F38" s="8" t="s">
-        <v>57</v>
+      <c r="F38" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -2576,14 +2622,11 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>163</v>
-      </c>
       <c r="D39" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F39" s="9" t="s">
-        <v>161</v>
+      <c r="F39" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -2592,18 +2635,18 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="J39" s="10" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D40" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>162</v>
+      <c r="D40" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -2612,64 +2655,67 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>164</v>
-      </c>
-      <c r="J40" t="s">
-        <v>206</v>
+        <v>160</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>16</v>
-      </c>
       <c r="B41" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F41" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41" t="s">
+        <v>164</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D42" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42" t="s">
+        <v>164</v>
+      </c>
+      <c r="J42" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>16</v>
+      </c>
+      <c r="B43" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F43" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41" t="s">
-        <v>172</v>
-      </c>
-      <c r="J41" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D42" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42" t="s">
-        <v>172</v>
-      </c>
-      <c r="J42" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D43" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -2680,16 +2726,16 @@
       <c r="I43" t="s">
         <v>172</v>
       </c>
-      <c r="J43" t="s">
-        <v>198</v>
+      <c r="J43" s="10" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D44" s="5" t="s">
-        <v>96</v>
+      <c r="D44" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>62</v>
+        <v>165</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -2700,8 +2746,8 @@
       <c r="I44" t="s">
         <v>172</v>
       </c>
-      <c r="J44" t="s">
-        <v>199</v>
+      <c r="J44" s="10" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2709,7 +2755,7 @@
         <v>96</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -2721,7 +2767,7 @@
         <v>172</v>
       </c>
       <c r="J45" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -2729,7 +2775,7 @@
         <v>96</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -2741,7 +2787,7 @@
         <v>172</v>
       </c>
       <c r="J46" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2749,7 +2795,7 @@
         <v>96</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -2761,21 +2807,15 @@
         <v>172</v>
       </c>
       <c r="J47" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>18</v>
-      </c>
-      <c r="B48" t="s">
-        <v>139</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>69</v>
+      <c r="D48" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -2784,10 +2824,10 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>173</v>
-      </c>
-      <c r="J48" s="10" t="s">
-        <v>222</v>
+        <v>172</v>
+      </c>
+      <c r="J48" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2795,7 +2835,7 @@
         <v>96</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -2804,18 +2844,24 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J49" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D50" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>68</v>
+      <c r="A50">
+        <v>18</v>
+      </c>
+      <c r="B50" t="s">
+        <v>139</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -2826,82 +2872,82 @@
       <c r="I50" t="s">
         <v>173</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D51" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51" t="s">
+        <v>173</v>
+      </c>
+      <c r="J51" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D52" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52" t="s">
+        <v>173</v>
+      </c>
+      <c r="J52" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>20</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B53" t="s">
         <v>132</v>
       </c>
-      <c r="D51" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-      <c r="I51" t="s">
-        <v>174</v>
-      </c>
-      <c r="J51" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D52" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52">
-        <v>0</v>
-      </c>
-      <c r="I52" t="s">
-        <v>174</v>
-      </c>
-      <c r="J52" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D53" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F53" s="2" t="s">
-        <v>252</v>
+      <c r="F53" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" t="s">
         <v>174</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D54" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="F54" s="11" t="s">
-        <v>255</v>
+      <c r="D54" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>251</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -2913,18 +2959,15 @@
         <v>174</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>134</v>
-      </c>
       <c r="D55" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F55" s="8" t="s">
-        <v>110</v>
+      <c r="F55" s="2" t="s">
+        <v>252</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -2936,21 +2979,15 @@
         <v>174</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>120</v>
-      </c>
-      <c r="C56" t="s">
-        <v>133</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F56" s="7" t="s">
-        <v>93</v>
+      <c r="D56" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>255</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -2962,15 +2999,18 @@
         <v>174</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>222</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>134</v>
+      </c>
       <c r="D57" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F57" s="7" t="s">
-        <v>159</v>
+      <c r="F57" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -2987,13 +3027,16 @@
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>135</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>100</v>
+        <v>120</v>
+      </c>
+      <c r="C58" t="s">
+        <v>133</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -3004,19 +3047,16 @@
       <c r="I58" t="s">
         <v>174</v>
       </c>
-      <c r="J58" t="s">
-        <v>201</v>
+      <c r="J58" s="10" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>136</v>
-      </c>
-      <c r="D59" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>102</v>
+      <c r="D59" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -3027,16 +3067,19 @@
       <c r="I59" t="s">
         <v>174</v>
       </c>
-      <c r="J59" t="s">
-        <v>202</v>
+      <c r="J59" s="10" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>135</v>
+      </c>
       <c r="D60" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -3048,15 +3091,18 @@
         <v>174</v>
       </c>
       <c r="J60" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>136</v>
+      </c>
       <c r="D61" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -3068,7 +3114,7 @@
         <v>174</v>
       </c>
       <c r="J61" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -3076,7 +3122,7 @@
         <v>96</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -3088,7 +3134,7 @@
         <v>174</v>
       </c>
       <c r="J62" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -3096,7 +3142,7 @@
         <v>96</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -3108,7 +3154,7 @@
         <v>174</v>
       </c>
       <c r="J63" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -3116,7 +3162,7 @@
         <v>96</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -3128,7 +3174,7 @@
         <v>174</v>
       </c>
       <c r="J64" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
@@ -3136,7 +3182,7 @@
         <v>96</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>166</v>
+        <v>106</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -3148,18 +3194,15 @@
         <v>174</v>
       </c>
       <c r="J65" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>167</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>224</v>
+      <c r="D66" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -3168,10 +3211,10 @@
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>175</v>
-      </c>
-      <c r="J66" s="10" t="s">
-        <v>222</v>
+        <v>174</v>
+      </c>
+      <c r="J66" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
@@ -3179,39 +3222,42 @@
         <v>96</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67" t="s">
+        <v>174</v>
+      </c>
+      <c r="J67" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>167</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68" t="s">
         <v>175</v>
       </c>
-      <c r="J67" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D68" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-      <c r="H68">
-        <v>0</v>
-      </c>
-      <c r="I68" t="s">
-        <v>168</v>
-      </c>
-      <c r="J68" t="s">
-        <v>215</v>
+      <c r="J68" s="10" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
@@ -3219,76 +3265,70 @@
         <v>96</v>
       </c>
       <c r="F69" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69" t="s">
+        <v>175</v>
+      </c>
+      <c r="J69" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D70" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70" t="s">
+        <v>168</v>
+      </c>
+      <c r="J70" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D71" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F71" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-      <c r="H69">
-        <v>0</v>
-      </c>
-      <c r="I69" t="s">
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71" t="s">
         <v>168</v>
       </c>
-      <c r="J69" t="s">
+      <c r="J71" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>179</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F70" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
-      <c r="I70" t="s">
-        <v>181</v>
-      </c>
-      <c r="J70" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
-        <v>261</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F71" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="G71">
-        <v>0</v>
-      </c>
-      <c r="H71">
-        <v>0</v>
-      </c>
-      <c r="I71" t="s">
-        <v>181</v>
-      </c>
-      <c r="J71" s="10" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>263</v>
+        <v>179</v>
       </c>
       <c r="D72" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -3305,13 +3345,13 @@
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>223</v>
+        <v>182</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -3328,13 +3368,13 @@
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>256</v>
+        <v>191</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -3346,15 +3386,18 @@
         <v>181</v>
       </c>
       <c r="J74" s="10" t="s">
-        <v>257</v>
+        <v>222</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D75" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>183</v>
+      <c r="B75" t="s">
+        <v>262</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -3365,16 +3408,19 @@
       <c r="I75" t="s">
         <v>181</v>
       </c>
-      <c r="J75" t="s">
-        <v>217</v>
+      <c r="J75" s="10" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D76" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>184</v>
+      <c r="B76" t="s">
+        <v>260</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>256</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -3385,8 +3431,8 @@
       <c r="I76" t="s">
         <v>181</v>
       </c>
-      <c r="J76" t="s">
-        <v>218</v>
+      <c r="J76" s="10" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
@@ -3394,7 +3440,7 @@
         <v>96</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -3406,7 +3452,7 @@
         <v>181</v>
       </c>
       <c r="J77" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
@@ -3414,7 +3460,7 @@
         <v>96</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -3426,7 +3472,7 @@
         <v>181</v>
       </c>
       <c r="J78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
@@ -3434,7 +3480,7 @@
         <v>96</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>240</v>
+        <v>192</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -3446,7 +3492,7 @@
         <v>181</v>
       </c>
       <c r="J79" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.25">
@@ -3454,7 +3500,7 @@
         <v>96</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>242</v>
+        <v>193</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -3466,7 +3512,7 @@
         <v>181</v>
       </c>
       <c r="J80" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
@@ -3474,7 +3520,7 @@
         <v>96</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>196</v>
+        <v>240</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -3486,7 +3532,7 @@
         <v>181</v>
       </c>
       <c r="J81" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -3494,7 +3540,7 @@
         <v>96</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -3506,15 +3552,15 @@
         <v>181</v>
       </c>
       <c r="J82" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D83" s="6" t="s">
-        <v>95</v>
+      <c r="D83" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>232</v>
+        <v>196</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -3523,10 +3569,10 @@
         <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>245</v>
-      </c>
-      <c r="J83" s="10" t="s">
-        <v>222</v>
+        <v>181</v>
+      </c>
+      <c r="J83" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
@@ -3534,7 +3580,7 @@
         <v>96</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>233</v>
+        <v>258</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -3543,24 +3589,18 @@
         <v>0</v>
       </c>
       <c r="I84" t="s">
-        <v>245</v>
+        <v>181</v>
       </c>
       <c r="J84" t="s">
-        <v>235</v>
+        <v>259</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>17</v>
-      </c>
-      <c r="B85" t="s">
-        <v>137</v>
-      </c>
       <c r="D85" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F85" s="9" t="s">
-        <v>194</v>
+      <c r="F85" s="2" t="s">
+        <v>232</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -3569,7 +3609,7 @@
         <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="J85" s="10" t="s">
         <v>222</v>
@@ -3580,18 +3620,64 @@
         <v>96</v>
       </c>
       <c r="F86" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86" t="s">
+        <v>245</v>
+      </c>
+      <c r="J86" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>17</v>
+      </c>
+      <c r="B87" t="s">
+        <v>137</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+      <c r="I87" t="s">
+        <v>234</v>
+      </c>
+      <c r="J87" s="10" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D88" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F88" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="G86">
-        <v>0</v>
-      </c>
-      <c r="H86">
-        <v>0</v>
-      </c>
-      <c r="I86" t="s">
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88" t="s">
         <v>234</v>
       </c>
-      <c r="J86" t="s">
+      <c r="J88" t="s">
         <v>220</v>
       </c>
     </row>

</xml_diff>

<commit_message>
target model note correction
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1516,8 +1516,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H76" sqref="H75:H76"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3326,7 +3326,7 @@
         <v>171</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -3581,10 +3581,10 @@
         <v>196</v>
       </c>
       <c r="G83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I83" t="s">
         <v>181</v>
@@ -3601,10 +3601,10 @@
         <v>257</v>
       </c>
       <c r="G84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I84" t="s">
         <v>181</v>

</xml_diff>

<commit_message>
device connection statistics added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1262,7 +1262,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B13" sqref="B13:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,8 +1516,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H87" sqref="H87"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2736,7 +2736,7 @@
         <v>66</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -2948,10 +2948,10 @@
         <v>90</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" t="s">
         <v>174</v>
@@ -3581,10 +3581,10 @@
         <v>196</v>
       </c>
       <c r="G83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I83" t="s">
         <v>181</v>
@@ -3601,10 +3601,10 @@
         <v>257</v>
       </c>
       <c r="G84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I84" t="s">
         <v>181</v>

</xml_diff>

<commit_message>
device connection statistics report table added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -12,14 +12,14 @@
     <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$90</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="283">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -856,6 +856,18 @@
   </si>
   <si>
     <t>C:\Users\vlasenko\Documents\06.CONFIGS\Rencredit\Supportinfo-Thu-10-15-2020-15-00-18</t>
+  </si>
+  <si>
+    <t>device_connection_statistics</t>
+  </si>
+  <si>
+    <t>Device connection statistics</t>
+  </si>
+  <si>
+    <t>Статистическая информация о портах устройств</t>
+  </si>
+  <si>
+    <t>Статистика_устройств</t>
   </si>
 </sst>
 </file>
@@ -1514,10 +1526,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J88"/>
+  <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2736,7 +2748,7 @@
         <v>66</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -2948,10 +2960,10 @@
         <v>90</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" t="s">
         <v>174</v>
@@ -2964,8 +2976,8 @@
       <c r="D54" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F54" s="2" t="s">
-        <v>250</v>
+      <c r="F54" s="9" t="s">
+        <v>279</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -2977,7 +2989,7 @@
         <v>174</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>221</v>
+        <v>280</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -2985,7 +2997,7 @@
         <v>95</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -2997,15 +3009,15 @@
         <v>174</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D56" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="F56" s="11" t="s">
-        <v>254</v>
+      <c r="D56" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>251</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -3021,14 +3033,11 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>134</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>110</v>
+      <c r="D57" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>254</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -3040,21 +3049,18 @@
         <v>174</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>221</v>
+        <v>252</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>120</v>
-      </c>
-      <c r="C58" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F58" s="7" t="s">
-        <v>93</v>
+      <c r="F58" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -3070,11 +3076,17 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" t="s">
+        <v>133</v>
+      </c>
       <c r="D59" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>159</v>
+        <v>93</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -3090,14 +3102,11 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>135</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>100</v>
+      <c r="D60" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -3108,19 +3117,19 @@
       <c r="I60" t="s">
         <v>174</v>
       </c>
-      <c r="J60" t="s">
-        <v>201</v>
+      <c r="J60" s="10" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -3132,15 +3141,18 @@
         <v>174</v>
       </c>
       <c r="J61" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>136</v>
+      </c>
       <c r="D62" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -3152,7 +3164,7 @@
         <v>174</v>
       </c>
       <c r="J62" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -3160,7 +3172,7 @@
         <v>96</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -3172,7 +3184,7 @@
         <v>174</v>
       </c>
       <c r="J63" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -3180,7 +3192,7 @@
         <v>96</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -3192,7 +3204,7 @@
         <v>174</v>
       </c>
       <c r="J64" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
@@ -3200,7 +3212,7 @@
         <v>96</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -3212,7 +3224,7 @@
         <v>174</v>
       </c>
       <c r="J65" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
@@ -3220,7 +3232,7 @@
         <v>96</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -3232,7 +3244,7 @@
         <v>174</v>
       </c>
       <c r="J66" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
@@ -3240,7 +3252,7 @@
         <v>96</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>166</v>
+        <v>107</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -3252,30 +3264,27 @@
         <v>174</v>
       </c>
       <c r="J67" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>167</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F68" s="9" t="s">
-        <v>223</v>
+      <c r="D68" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>282</v>
       </c>
       <c r="G68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I68" t="s">
-        <v>175</v>
-      </c>
-      <c r="J68" s="10" t="s">
-        <v>221</v>
+        <v>174</v>
+      </c>
+      <c r="J68" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
@@ -3283,7 +3292,7 @@
         <v>96</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -3292,30 +3301,33 @@
         <v>0</v>
       </c>
       <c r="I69" t="s">
+        <v>174</v>
+      </c>
+      <c r="J69" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>167</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70" t="s">
         <v>175</v>
       </c>
-      <c r="J69" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D70" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
-      <c r="I70" t="s">
-        <v>168</v>
-      </c>
-      <c r="J70" t="s">
-        <v>215</v>
+      <c r="J70" s="10" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
@@ -3323,76 +3335,70 @@
         <v>96</v>
       </c>
       <c r="F71" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71" t="s">
+        <v>175</v>
+      </c>
+      <c r="J71" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D72" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72" t="s">
+        <v>168</v>
+      </c>
+      <c r="J72" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D73" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="G71">
-        <v>0</v>
-      </c>
-      <c r="H71">
-        <v>0</v>
-      </c>
-      <c r="I71" t="s">
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73" t="s">
         <v>168</v>
       </c>
-      <c r="J71" t="s">
+      <c r="J73" t="s">
         <v>277</v>
-      </c>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>179</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F72" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="G72">
-        <v>0</v>
-      </c>
-      <c r="H72">
-        <v>0</v>
-      </c>
-      <c r="I72" t="s">
-        <v>181</v>
-      </c>
-      <c r="J72" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>260</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F73" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="G73">
-        <v>0</v>
-      </c>
-      <c r="H73">
-        <v>0</v>
-      </c>
-      <c r="I73" t="s">
-        <v>181</v>
-      </c>
-      <c r="J73" s="10" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>262</v>
+        <v>179</v>
       </c>
       <c r="D74" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -3409,13 +3415,13 @@
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>222</v>
+        <v>182</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -3432,13 +3438,13 @@
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>255</v>
+        <v>191</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -3450,15 +3456,18 @@
         <v>181</v>
       </c>
       <c r="J76" s="10" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D77" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>183</v>
+      <c r="B77" t="s">
+        <v>261</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>222</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -3469,16 +3478,19 @@
       <c r="I77" t="s">
         <v>181</v>
       </c>
-      <c r="J77" t="s">
-        <v>216</v>
+      <c r="J77" s="10" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D78" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>184</v>
+      <c r="B78" t="s">
+        <v>259</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F78" s="9" t="s">
+        <v>255</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -3489,8 +3501,8 @@
       <c r="I78" t="s">
         <v>181</v>
       </c>
-      <c r="J78" t="s">
-        <v>217</v>
+      <c r="J78" s="10" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
@@ -3498,7 +3510,7 @@
         <v>96</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -3510,7 +3522,7 @@
         <v>181</v>
       </c>
       <c r="J79" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.25">
@@ -3518,7 +3530,7 @@
         <v>96</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -3530,7 +3542,7 @@
         <v>181</v>
       </c>
       <c r="J80" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
@@ -3538,7 +3550,7 @@
         <v>96</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>239</v>
+        <v>192</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -3550,7 +3562,7 @@
         <v>181</v>
       </c>
       <c r="J81" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -3558,7 +3570,7 @@
         <v>96</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>241</v>
+        <v>193</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -3570,7 +3582,7 @@
         <v>181</v>
       </c>
       <c r="J82" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -3578,7 +3590,7 @@
         <v>96</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>196</v>
+        <v>239</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -3590,7 +3602,7 @@
         <v>181</v>
       </c>
       <c r="J83" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
@@ -3598,7 +3610,7 @@
         <v>96</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -3610,15 +3622,15 @@
         <v>181</v>
       </c>
       <c r="J84" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D85" s="6" t="s">
-        <v>95</v>
+      <c r="D85" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>231</v>
+        <v>196</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -3627,10 +3639,10 @@
         <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>244</v>
-      </c>
-      <c r="J85" s="10" t="s">
-        <v>221</v>
+        <v>181</v>
+      </c>
+      <c r="J85" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
@@ -3638,7 +3650,7 @@
         <v>96</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>232</v>
+        <v>257</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -3647,24 +3659,18 @@
         <v>0</v>
       </c>
       <c r="I86" t="s">
-        <v>244</v>
+        <v>181</v>
       </c>
       <c r="J86" t="s">
-        <v>234</v>
+        <v>258</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>17</v>
-      </c>
-      <c r="B87" t="s">
-        <v>137</v>
-      </c>
       <c r="D87" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F87" s="9" t="s">
-        <v>194</v>
+      <c r="F87" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -3673,7 +3679,7 @@
         <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="J87" s="10" t="s">
         <v>221</v>
@@ -3684,18 +3690,64 @@
         <v>96</v>
       </c>
       <c r="F88" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88" t="s">
+        <v>244</v>
+      </c>
+      <c r="J88" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>17</v>
+      </c>
+      <c r="B89" t="s">
+        <v>137</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89" t="s">
+        <v>233</v>
+      </c>
+      <c r="J89" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D90" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F90" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="G88">
-        <v>0</v>
-      </c>
-      <c r="H88">
-        <v>0</v>
-      </c>
-      <c r="I88" t="s">
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90" t="s">
         <v>233</v>
       </c>
-      <c r="J88" t="s">
+      <c r="J90" t="s">
         <v>219</v>
       </c>
     </row>

</xml_diff>

<commit_message>
zone_statistics report DataFrame drop wwnn_to_wwnp_unpack columns drop
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1528,8 +1528,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3275,10 +3275,10 @@
         <v>282</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68" t="s">
         <v>174</v>
@@ -3633,10 +3633,10 @@
         <v>196</v>
       </c>
       <c r="G85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I85" t="s">
         <v>181</v>

</xml_diff>

<commit_message>
global switch parameters change from drop duplicates to Princiapl switch
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="292">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -868,6 +868,33 @@
   </si>
   <si>
     <t>Статистика_устройств</t>
+  </si>
+  <si>
+    <t>Rossiya</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Rossiya\SANSW</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Rossiya</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\GS_labs\0212\92</t>
+  </si>
+  <si>
+    <t>Gs-labs</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Gs-labs</t>
+  </si>
+  <si>
+    <t>Complight</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Complight\ssave</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Complight\DEC2020</t>
   </si>
 </sst>
 </file>
@@ -1271,248 +1298,277 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:E38"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="4" width="76" customWidth="1"/>
-    <col min="5" max="5" width="72.28515625" customWidth="1"/>
-    <col min="6" max="6" width="61.7109375" customWidth="1"/>
-    <col min="7" max="7" width="60" customWidth="1"/>
-    <col min="8" max="8" width="38.140625" customWidth="1"/>
-    <col min="9" max="9" width="69" customWidth="1"/>
-    <col min="10" max="10" width="72.42578125" customWidth="1"/>
-    <col min="11" max="11" width="111.5703125" customWidth="1"/>
-    <col min="12" max="12" width="72.5703125" customWidth="1"/>
-    <col min="13" max="13" width="86.85546875" customWidth="1"/>
-    <col min="14" max="15" width="64.7109375" customWidth="1"/>
-    <col min="16" max="16" width="54.5703125" customWidth="1"/>
-    <col min="17" max="17" width="75.42578125" customWidth="1"/>
-    <col min="18" max="18" width="58.140625" customWidth="1"/>
+    <col min="1" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="52.140625" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="7" width="76" customWidth="1"/>
+    <col min="8" max="8" width="72.28515625" customWidth="1"/>
+    <col min="9" max="9" width="61.7109375" customWidth="1"/>
+    <col min="10" max="10" width="60" customWidth="1"/>
+    <col min="11" max="11" width="38.140625" customWidth="1"/>
+    <col min="12" max="12" width="69" customWidth="1"/>
+    <col min="13" max="13" width="72.42578125" customWidth="1"/>
+    <col min="14" max="14" width="111.5703125" customWidth="1"/>
+    <col min="15" max="15" width="72.5703125" customWidth="1"/>
+    <col min="16" max="16" width="86.85546875" customWidth="1"/>
+    <col min="17" max="18" width="64.7109375" customWidth="1"/>
+    <col min="19" max="19" width="54.5703125" customWidth="1"/>
+    <col min="20" max="20" width="75.42578125" customWidth="1"/>
+    <col min="21" max="21" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D2" t="s">
+        <v>287</v>
+      </c>
+      <c r="E2" t="s">
+        <v>283</v>
+      </c>
+      <c r="F2" t="s">
         <v>263</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>263</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>245</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>238</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>190</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>189</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>155</v>
       </c>
-      <c r="J2" t="s">
+      <c r="M2" t="s">
         <v>111</v>
       </c>
-      <c r="K2" t="s">
+      <c r="N2" t="s">
         <v>97</v>
       </c>
-      <c r="L2" t="s">
+      <c r="O2" t="s">
         <v>83</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E3" t="s">
+        <v>285</v>
+      </c>
+      <c r="F3" t="s">
         <v>264</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>264</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>247</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>237</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>226</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
         <v>188</v>
       </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
         <v>157</v>
       </c>
-      <c r="J3" t="s">
+      <c r="M3" t="s">
         <v>113</v>
       </c>
-      <c r="K3" t="s">
+      <c r="N3" t="s">
         <v>98</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
         <v>85</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>1</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>74</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>72</v>
       </c>
-      <c r="P3" t="s">
+      <c r="S3" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>25</v>
       </c>
-      <c r="R3" t="s">
+      <c r="U3" t="s">
         <v>60</v>
       </c>
-      <c r="S3" t="s">
+      <c r="V3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D4" t="s">
+        <v>286</v>
+      </c>
+      <c r="E4" t="s">
+        <v>284</v>
+      </c>
+      <c r="F4" t="s">
         <v>278</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>265</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H4" t="s">
         <v>246</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>235</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>225</v>
       </c>
-      <c r="H4" t="s">
+      <c r="K4" t="s">
         <v>187</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
         <v>156</v>
       </c>
-      <c r="J4" t="s">
+      <c r="M4" t="s">
         <v>112</v>
       </c>
-      <c r="K4" t="s">
+      <c r="N4" t="s">
         <v>108</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
         <v>84</v>
       </c>
-      <c r="M4" t="s">
-        <v>0</v>
-      </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
         <v>73</v>
       </c>
-      <c r="O4" t="s">
+      <c r="R4" t="s">
         <v>71</v>
       </c>
-      <c r="P4" t="s">
+      <c r="S4" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="T4" t="s">
         <v>24</v>
       </c>
-      <c r="R4" t="s">
+      <c r="U4" t="s">
         <v>59</v>
       </c>
-      <c r="S4" t="s">
+      <c r="V4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>267</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>267</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>236</v>
       </c>
-      <c r="I5" t="s">
+      <c r="L5" t="s">
         <v>158</v>
       </c>
-      <c r="K5" t="s">
+      <c r="N5" t="s">
         <v>109</v>
       </c>
-      <c r="L5" t="s">
+      <c r="O5" t="s">
         <v>87</v>
       </c>
-      <c r="O5" t="s">
+      <c r="R5" t="s">
         <v>99</v>
       </c>
-      <c r="R5" t="s">
+      <c r="U5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
         <v>269</v>
       </c>
-      <c r="D6" t="s">
+      <c r="G6" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>243</v>
       </c>
@@ -1528,8 +1584,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1910,7 +1966,7 @@
         <v>15</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -2828,10 +2884,10 @@
         <v>63</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47" t="s">
         <v>172</v>
@@ -2894,10 +2950,10 @@
         <v>69</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" t="s">
         <v>173</v>

</xml_diff>

<commit_message>
isl_statistics regex from service file
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1346,12 +1346,13 @@
   <dimension ref="A1:W9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="29.7109375" customWidth="1"/>
+    <col min="1" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="69.85546875" customWidth="1"/>
     <col min="4" max="4" width="52.140625" customWidth="1"/>
     <col min="5" max="5" width="73.140625" customWidth="1"/>
     <col min="6" max="6" width="29.7109375" customWidth="1"/>
@@ -1375,7 +1376,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1673,7 +1674,7 @@
   <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3078,7 +3079,7 @@
         <v>67</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -3118,7 +3119,7 @@
         <v>302</v>
       </c>
       <c r="G54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H54">
         <v>1</v>

</xml_diff>

<commit_message>
list of aliases, wwnp and port quantityt added to manual_device_rename DataFrame
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="324">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -979,6 +979,18 @@
   </si>
   <si>
     <t>DATA ANALYSIS 9. RASLOG</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\OTPBank\SAN Assessment DEC2020</t>
+  </si>
+  <si>
+    <t>OTPBank</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Otpbank</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Otpbank\27-11-2020</t>
   </si>
 </sst>
 </file>
@@ -1391,321 +1403,337 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="69.85546875" customWidth="1"/>
-    <col min="4" max="4" width="52.140625" customWidth="1"/>
-    <col min="5" max="5" width="73.140625" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" customWidth="1"/>
-    <col min="7" max="8" width="76" customWidth="1"/>
-    <col min="9" max="9" width="72.28515625" customWidth="1"/>
-    <col min="10" max="10" width="61.7109375" customWidth="1"/>
-    <col min="11" max="11" width="60" customWidth="1"/>
-    <col min="12" max="12" width="38.140625" customWidth="1"/>
-    <col min="13" max="13" width="69" customWidth="1"/>
-    <col min="14" max="14" width="72.42578125" customWidth="1"/>
-    <col min="15" max="15" width="111.5703125" customWidth="1"/>
-    <col min="16" max="16" width="72.5703125" customWidth="1"/>
-    <col min="17" max="17" width="86.85546875" customWidth="1"/>
-    <col min="18" max="19" width="64.7109375" customWidth="1"/>
-    <col min="20" max="20" width="54.5703125" customWidth="1"/>
-    <col min="21" max="21" width="75.42578125" customWidth="1"/>
-    <col min="22" max="22" width="58.140625" customWidth="1"/>
+    <col min="3" max="3" width="89.5703125" customWidth="1"/>
+    <col min="4" max="4" width="69.85546875" customWidth="1"/>
+    <col min="5" max="5" width="52.140625" customWidth="1"/>
+    <col min="6" max="6" width="73.140625" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="8" max="9" width="76" customWidth="1"/>
+    <col min="10" max="10" width="72.28515625" customWidth="1"/>
+    <col min="11" max="11" width="61.7109375" customWidth="1"/>
+    <col min="12" max="12" width="60" customWidth="1"/>
+    <col min="13" max="13" width="38.140625" customWidth="1"/>
+    <col min="14" max="14" width="69" customWidth="1"/>
+    <col min="15" max="15" width="72.42578125" customWidth="1"/>
+    <col min="16" max="16" width="111.5703125" customWidth="1"/>
+    <col min="17" max="17" width="72.5703125" customWidth="1"/>
+    <col min="18" max="18" width="86.85546875" customWidth="1"/>
+    <col min="19" max="20" width="64.7109375" customWidth="1"/>
+    <col min="21" max="21" width="54.5703125" customWidth="1"/>
+    <col min="22" max="22" width="75.42578125" customWidth="1"/>
+    <col min="23" max="23" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
+        <v>321</v>
+      </c>
+      <c r="D2" t="s">
         <v>289</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>287</v>
-      </c>
-      <c r="E2" t="s">
-        <v>283</v>
       </c>
       <c r="F2" t="s">
         <v>283</v>
       </c>
       <c r="G2" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="H2" t="s">
         <v>263</v>
       </c>
       <c r="I2" t="s">
+        <v>263</v>
+      </c>
+      <c r="J2" t="s">
         <v>245</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>238</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>190</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>189</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>155</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>111</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>97</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="E3" s="12">
+      <c r="C3" s="12">
+        <v>44209</v>
+      </c>
+      <c r="F3" s="12">
         <v>44181</v>
       </c>
-      <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X3" s="1"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>293</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>292</v>
       </c>
-      <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X4" s="1"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
+        <v>320</v>
+      </c>
+      <c r="D5" t="s">
         <v>291</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>288</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>296</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>285</v>
-      </c>
-      <c r="G5" t="s">
-        <v>264</v>
       </c>
       <c r="H5" t="s">
         <v>264</v>
       </c>
       <c r="I5" t="s">
+        <v>264</v>
+      </c>
+      <c r="J5" t="s">
         <v>247</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>237</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>226</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>188</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>157</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>113</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>98</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>85</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>1</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>74</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>72</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>4</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>25</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>60</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C6" t="s">
+        <v>322</v>
+      </c>
+      <c r="D6" t="s">
         <v>290</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>286</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>297</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>284</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>278</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>265</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>246</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>235</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>225</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>187</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>156</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>112</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>108</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>84</v>
       </c>
-      <c r="Q6" t="s">
-        <v>0</v>
-      </c>
       <c r="R6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S6" t="s">
         <v>73</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>71</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>3</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>24</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>59</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G7" t="s">
-        <v>267</v>
+      <c r="C7" t="s">
+        <v>323</v>
       </c>
       <c r="H7" t="s">
         <v>267</v>
       </c>
-      <c r="J7" t="s">
+      <c r="I7" t="s">
+        <v>267</v>
+      </c>
+      <c r="K7" t="s">
         <v>236</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>158</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>109</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>87</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>99</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="G8" t="s">
-        <v>269</v>
-      </c>
       <c r="H8" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>243</v>
       </c>
@@ -1721,8 +1749,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C76" workbookViewId="0">
-      <selection activeCell="G98" sqref="G98"/>
+    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3219,10 +3247,10 @@
         <v>90</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" t="s">
         <v>174</v>
@@ -3348,7 +3376,7 @@
         <v>93</v>
       </c>
       <c r="G62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -4061,10 +4089,10 @@
         <v>311</v>
       </c>
       <c r="G96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96" t="s">
         <v>319</v>

</xml_diff>

<commit_message>
analysis_portcmd warning propose to save dataframe
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -498,9 +498,6 @@
     <t>C:\Users\vlasenko\Documents\06.CONFIGS\Gosznak\Logs</t>
   </si>
   <si>
-    <t>expected_ag_links_df</t>
-  </si>
-  <si>
     <t>DATA ANALYSIS 1. SET FABRIC NAME AND LABEL</t>
   </si>
   <si>
@@ -991,6 +988,9 @@
   </si>
   <si>
     <t>C:\Users\vlasenko\Documents\06.CONFIGS\Otpbank\27-11-2020</t>
+  </si>
+  <si>
+    <t>expected_ag_links</t>
   </si>
 </sst>
 </file>
@@ -1405,8 +1405,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1437,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1446,37 +1446,37 @@
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N2" t="s">
         <v>155</v>
@@ -1514,7 +1514,7 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C3" s="12">
         <v>44209</v>
@@ -1532,13 +1532,13 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -1553,37 +1553,37 @@
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="M5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N5" t="s">
         <v>157</v>
@@ -1624,37 +1624,37 @@
         <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N6" t="s">
         <v>156</v>
@@ -1695,16 +1695,16 @@
         <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N7" t="s">
         <v>158</v>
@@ -1724,18 +1724,18 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="H8" t="s">
         <v>268</v>
       </c>
-      <c r="H8" t="s">
-        <v>269</v>
-      </c>
       <c r="I8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -1746,12 +1746,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" filterMode="1"/>
   <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H65" sqref="H65"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G43" sqref="G43:H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1795,10 +1795,10 @@
         <v>150</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1824,10 +1824,10 @@
         <v>153</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1853,10 +1853,10 @@
         <v>153</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>116</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>94</v>
@@ -1885,10 +1885,10 @@
         <v>142</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>118</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>94</v>
@@ -1917,10 +1917,10 @@
         <v>151</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>118</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>94</v>
@@ -1949,10 +1949,10 @@
         <v>151</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>114</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>94</v>
@@ -1981,10 +1981,10 @@
         <v>152</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2013,10 +2013,10 @@
         <v>148</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2045,10 +2045,10 @@
         <v>148</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2077,10 +2077,10 @@
         <v>146</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2109,10 +2109,10 @@
         <v>147</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2141,10 +2141,10 @@
         <v>147</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2173,10 +2173,10 @@
         <v>144</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -2205,10 +2205,10 @@
         <v>144</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -2237,10 +2237,10 @@
         <v>144</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
       </c>
@@ -2269,10 +2269,10 @@
         <v>145</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -2301,10 +2301,10 @@
         <v>145</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
@@ -2333,10 +2333,10 @@
         <v>145</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
@@ -2365,10 +2365,10 @@
         <v>143</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
@@ -2394,10 +2394,10 @@
         <v>143</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
@@ -2423,10 +2423,10 @@
         <v>143</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12</v>
       </c>
@@ -2452,10 +2452,10 @@
         <v>143</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>124</v>
       </c>
@@ -2478,10 +2478,10 @@
         <v>143</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>124</v>
       </c>
@@ -2504,10 +2504,10 @@
         <v>143</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>13</v>
       </c>
@@ -2533,10 +2533,10 @@
         <v>149</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>127</v>
       </c>
@@ -2559,10 +2559,10 @@
         <v>149</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>127</v>
       </c>
@@ -2585,10 +2585,10 @@
         <v>149</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>127</v>
       </c>
@@ -2611,10 +2611,10 @@
         <v>149</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>127</v>
       </c>
@@ -2637,10 +2637,10 @@
         <v>149</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>127</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>94</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -2663,10 +2663,10 @@
         <v>149</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>127</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>94</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -2689,62 +2689,62 @@
         <v>149</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>227</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>228</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F32" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32" t="s">
         <v>228</v>
       </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32" t="s">
-        <v>229</v>
-      </c>
       <c r="J32" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>307</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>308</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F33" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
         <v>304</v>
       </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="J33" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="J33" s="10" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>19</v>
       </c>
@@ -2767,13 +2767,13 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>115</v>
       </c>
@@ -2793,13 +2793,13 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>115</v>
       </c>
@@ -2819,22 +2819,22 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -2843,22 +2843,22 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -2867,13 +2867,13 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>15</v>
       </c>
@@ -2893,13 +2893,13 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D40" s="6" t="s">
         <v>95</v>
       </c>
@@ -2913,13 +2913,13 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D41" s="6" t="s">
         <v>95</v>
       </c>
@@ -2933,21 +2933,21 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -2956,10 +2956,10 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2967,22 +2967,22 @@
         <v>96</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J43" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>16</v>
       </c>
@@ -3002,18 +3002,18 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D45" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -3022,10 +3022,10 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3036,16 +3036,16 @@
         <v>61</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J46" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -3056,16 +3056,16 @@
         <v>62</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -3076,16 +3076,16 @@
         <v>63</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -3096,16 +3096,16 @@
         <v>65</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J49" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -3116,19 +3116,19 @@
         <v>64</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J50" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>18</v>
       </c>
@@ -3148,30 +3148,30 @@
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D52" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F52" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52" t="s">
+        <v>172</v>
+      </c>
+      <c r="J52" s="10" t="s">
         <v>298</v>
-      </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52">
-        <v>0</v>
-      </c>
-      <c r="I52" t="s">
-        <v>173</v>
-      </c>
-      <c r="J52" s="10" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -3182,16 +3182,16 @@
         <v>67</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J53" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -3202,16 +3202,16 @@
         <v>68</v>
       </c>
       <c r="G54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J54" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3219,22 +3219,22 @@
         <v>96</v>
       </c>
       <c r="F55" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="G55">
+        <v>1</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55" t="s">
+        <v>172</v>
+      </c>
+      <c r="J55" t="s">
         <v>302</v>
       </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
-      <c r="I55" t="s">
-        <v>173</v>
-      </c>
-      <c r="J55" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>20</v>
       </c>
@@ -3248,44 +3248,44 @@
         <v>90</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56">
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D57" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F57" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57" t="s">
+        <v>173</v>
+      </c>
+      <c r="J57" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="I57" t="s">
-        <v>174</v>
-      </c>
-      <c r="J57" s="10" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D58" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -3294,39 +3294,39 @@
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J58" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D59" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F59" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59" t="s">
+        <v>173</v>
+      </c>
+      <c r="J59" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59" t="s">
-        <v>174</v>
-      </c>
-      <c r="J59" s="10" t="s">
+    </row>
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D60" s="11" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D60" s="11" t="s">
+      <c r="F60" s="11" t="s">
         <v>253</v>
       </c>
-      <c r="F60" s="11" t="s">
-        <v>254</v>
-      </c>
       <c r="G60">
         <v>0</v>
       </c>
@@ -3334,13 +3334,13 @@
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>134</v>
       </c>
@@ -3357,13 +3357,13 @@
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>120</v>
       </c>
@@ -3383,18 +3383,18 @@
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D63" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>159</v>
+        <v>323</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -3403,10 +3403,10 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -3420,16 +3420,16 @@
         <v>100</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I64" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J64" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
@@ -3443,16 +3443,16 @@
         <v>102</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I65" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J65" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
@@ -3463,16 +3463,16 @@
         <v>103</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I66" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J66" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
@@ -3483,16 +3483,16 @@
         <v>104</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
@@ -3503,16 +3503,16 @@
         <v>105</v>
       </c>
       <c r="G68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I68" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J68" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
@@ -3523,16 +3523,16 @@
         <v>106</v>
       </c>
       <c r="G69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I69" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J69" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
@@ -3543,16 +3543,16 @@
         <v>107</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I70" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J70" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
@@ -3560,19 +3560,19 @@
         <v>96</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I71" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J71" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
@@ -3580,30 +3580,30 @@
         <v>96</v>
       </c>
       <c r="F72" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="I72" t="s">
+        <v>173</v>
+      </c>
+      <c r="J72" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
         <v>166</v>
-      </c>
-      <c r="G72">
-        <v>0</v>
-      </c>
-      <c r="H72">
-        <v>0</v>
-      </c>
-      <c r="I72" t="s">
-        <v>174</v>
-      </c>
-      <c r="J72" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>167</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -3612,10 +3612,10 @@
         <v>0</v>
       </c>
       <c r="I73" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J73" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
@@ -3623,19 +3623,19 @@
         <v>96</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I74" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J74" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
@@ -3643,19 +3643,19 @@
         <v>96</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I75" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J75" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.25">
@@ -3663,53 +3663,53 @@
         <v>96</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J76" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F77" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77" t="s">
         <v>180</v>
       </c>
-      <c r="G77">
-        <v>0</v>
-      </c>
-      <c r="H77">
-        <v>0</v>
-      </c>
-      <c r="I77" t="s">
-        <v>181</v>
-      </c>
       <c r="J77" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F78" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -3718,21 +3718,21 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J78" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -3741,21 +3741,21 @@
         <v>0</v>
       </c>
       <c r="I79" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J79" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -3764,33 +3764,33 @@
         <v>0</v>
       </c>
       <c r="I80" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J80" s="10" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F81" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81" t="s">
+        <v>180</v>
+      </c>
+      <c r="J81" s="10" t="s">
         <v>255</v>
-      </c>
-      <c r="G81">
-        <v>0</v>
-      </c>
-      <c r="H81">
-        <v>0</v>
-      </c>
-      <c r="I81" t="s">
-        <v>181</v>
-      </c>
-      <c r="J81" s="10" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
@@ -3798,19 +3798,19 @@
         <v>96</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I82" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J82" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -3818,19 +3818,19 @@
         <v>96</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I83" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J83" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
@@ -3838,19 +3838,19 @@
         <v>96</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I84" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J84" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
@@ -3858,19 +3858,19 @@
         <v>96</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I85" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J85" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
@@ -3878,19 +3878,19 @@
         <v>96</v>
       </c>
       <c r="F86" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="I86" t="s">
+        <v>180</v>
+      </c>
+      <c r="J86" t="s">
         <v>239</v>
-      </c>
-      <c r="G86">
-        <v>0</v>
-      </c>
-      <c r="H86">
-        <v>0</v>
-      </c>
-      <c r="I86" t="s">
-        <v>181</v>
-      </c>
-      <c r="J86" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
@@ -3898,19 +3898,19 @@
         <v>96</v>
       </c>
       <c r="F87" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+      <c r="I87" t="s">
+        <v>180</v>
+      </c>
+      <c r="J87" t="s">
         <v>241</v>
-      </c>
-      <c r="G87">
-        <v>0</v>
-      </c>
-      <c r="H87">
-        <v>0</v>
-      </c>
-      <c r="I87" t="s">
-        <v>181</v>
-      </c>
-      <c r="J87" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
@@ -3918,19 +3918,19 @@
         <v>96</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I88" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J88" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
@@ -3938,27 +3938,27 @@
         <v>96</v>
       </c>
       <c r="F89" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89" t="s">
+        <v>180</v>
+      </c>
+      <c r="J89" t="s">
         <v>257</v>
       </c>
-      <c r="G89">
-        <v>0</v>
-      </c>
-      <c r="H89">
-        <v>0</v>
-      </c>
-      <c r="I89" t="s">
-        <v>181</v>
-      </c>
-      <c r="J89" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D90" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -3967,10 +3967,10 @@
         <v>0</v>
       </c>
       <c r="I90" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J90" s="10" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
@@ -3978,22 +3978,22 @@
         <v>96</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I91" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J91" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>17</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>95</v>
       </c>
       <c r="F92" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -4013,10 +4013,10 @@
         <v>0</v>
       </c>
       <c r="I92" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J92" s="10" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
@@ -4024,30 +4024,30 @@
         <v>96</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I93" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J93" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F94" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -4056,30 +4056,30 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J94" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D95" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F95" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95" t="s">
         <v>318</v>
       </c>
-      <c r="G95">
-        <v>0</v>
-      </c>
-      <c r="H95">
-        <v>0</v>
-      </c>
-      <c r="I95" t="s">
-        <v>319</v>
-      </c>
       <c r="J95" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
@@ -4087,22 +4087,29 @@
         <v>96</v>
       </c>
       <c r="F96" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+      <c r="H96">
+        <v>1</v>
+      </c>
+      <c r="I96" t="s">
+        <v>318</v>
+      </c>
+      <c r="J96" t="s">
         <v>311</v>
       </c>
-      <c r="G96">
-        <v>0</v>
-      </c>
-      <c r="H96">
-        <v>0</v>
-      </c>
-      <c r="I96" t="s">
-        <v>319</v>
-      </c>
-      <c r="J96" t="s">
-        <v>312</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J96">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="report"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -4125,15 +4132,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" t="s">
         <v>185</v>
-      </c>
-      <c r="B1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>50</v>
@@ -4141,7 +4148,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>51</v>
@@ -4149,7 +4156,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>52</v>
@@ -4157,7 +4164,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
duplicated zones added to zone statistics
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="328">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -991,6 +991,18 @@
   </si>
   <si>
     <t>expected_ag_links</t>
+  </si>
+  <si>
+    <t>AlfaBank</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\AlfaBank\JAN 2021</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\AlfaBank\JAN 2021\ssave</t>
+  </si>
+  <si>
+    <t>Mechel</t>
   </si>
 </sst>
 </file>
@@ -1403,337 +1415,353 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="89.5703125" customWidth="1"/>
-    <col min="4" max="4" width="69.85546875" customWidth="1"/>
-    <col min="5" max="5" width="52.140625" customWidth="1"/>
-    <col min="6" max="6" width="73.140625" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1"/>
-    <col min="8" max="9" width="76" customWidth="1"/>
-    <col min="10" max="10" width="72.28515625" customWidth="1"/>
-    <col min="11" max="11" width="61.7109375" customWidth="1"/>
-    <col min="12" max="12" width="60" customWidth="1"/>
-    <col min="13" max="13" width="38.140625" customWidth="1"/>
-    <col min="14" max="14" width="69" customWidth="1"/>
-    <col min="15" max="15" width="72.42578125" customWidth="1"/>
-    <col min="16" max="16" width="111.5703125" customWidth="1"/>
-    <col min="17" max="17" width="72.5703125" customWidth="1"/>
-    <col min="18" max="18" width="86.85546875" customWidth="1"/>
-    <col min="19" max="20" width="64.7109375" customWidth="1"/>
-    <col min="21" max="21" width="54.5703125" customWidth="1"/>
-    <col min="22" max="22" width="75.42578125" customWidth="1"/>
-    <col min="23" max="23" width="58.140625" customWidth="1"/>
+    <col min="1" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="62" customWidth="1"/>
+    <col min="5" max="5" width="89.5703125" customWidth="1"/>
+    <col min="6" max="6" width="69.85546875" customWidth="1"/>
+    <col min="7" max="7" width="52.140625" customWidth="1"/>
+    <col min="8" max="8" width="73.140625" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" customWidth="1"/>
+    <col min="10" max="11" width="76" customWidth="1"/>
+    <col min="12" max="12" width="72.28515625" customWidth="1"/>
+    <col min="13" max="13" width="61.7109375" customWidth="1"/>
+    <col min="14" max="14" width="60" customWidth="1"/>
+    <col min="15" max="15" width="38.140625" customWidth="1"/>
+    <col min="16" max="16" width="69" customWidth="1"/>
+    <col min="17" max="17" width="72.42578125" customWidth="1"/>
+    <col min="18" max="18" width="111.5703125" customWidth="1"/>
+    <col min="19" max="19" width="72.5703125" customWidth="1"/>
+    <col min="20" max="20" width="86.85546875" customWidth="1"/>
+    <col min="21" max="22" width="64.7109375" customWidth="1"/>
+    <col min="23" max="23" width="54.5703125" customWidth="1"/>
+    <col min="24" max="24" width="75.42578125" customWidth="1"/>
+    <col min="25" max="25" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E2" t="s">
         <v>320</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>288</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>286</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>282</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>282</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>262</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>262</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>244</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>237</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>189</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>188</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>155</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>111</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>97</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>83</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="C3" s="12">
+      <c r="D3" s="12">
+        <v>44223</v>
+      </c>
+      <c r="E3" s="12">
         <v>44209</v>
       </c>
-      <c r="F3" s="12">
+      <c r="H3" s="12">
         <v>44181</v>
       </c>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>292</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>291</v>
       </c>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>325</v>
+      </c>
+      <c r="E5" t="s">
         <v>319</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>290</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>287</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>295</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>284</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>263</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>263</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>246</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>236</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>225</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>187</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
         <v>157</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
         <v>113</v>
       </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
         <v>98</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>85</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
         <v>1</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
         <v>74</v>
       </c>
-      <c r="T5" t="s">
+      <c r="V5" t="s">
         <v>72</v>
       </c>
-      <c r="U5" t="s">
+      <c r="W5" t="s">
         <v>4</v>
       </c>
-      <c r="V5" t="s">
+      <c r="X5" t="s">
         <v>25</v>
       </c>
-      <c r="W5" t="s">
+      <c r="Y5" t="s">
         <v>60</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Z5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>326</v>
+      </c>
+      <c r="E6" t="s">
         <v>321</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>289</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>285</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>296</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>283</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>277</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>264</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>245</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>234</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>224</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>186</v>
       </c>
-      <c r="N6" t="s">
+      <c r="P6" t="s">
         <v>156</v>
       </c>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
         <v>112</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>108</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="S6" t="s">
         <v>84</v>
       </c>
-      <c r="R6" t="s">
-        <v>0</v>
-      </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" t="s">
         <v>73</v>
       </c>
-      <c r="T6" t="s">
+      <c r="V6" t="s">
         <v>71</v>
       </c>
-      <c r="U6" t="s">
+      <c r="W6" t="s">
         <v>3</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>24</v>
       </c>
-      <c r="W6" t="s">
+      <c r="Y6" t="s">
         <v>59</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Z6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>322</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>266</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>266</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>235</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P7" t="s">
         <v>158</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R7" t="s">
         <v>109</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="S7" t="s">
         <v>87</v>
       </c>
-      <c r="T7" t="s">
+      <c r="V7" t="s">
         <v>99</v>
       </c>
-      <c r="W7" t="s">
+      <c r="Y7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>268</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>242</v>
       </c>
@@ -1750,8 +1778,8 @@
   <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G62" sqref="G62"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3248,10 +3276,10 @@
         <v>90</v>
       </c>
       <c r="G56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" t="s">
         <v>173</v>
@@ -3738,7 +3766,7 @@
         <v>0</v>
       </c>
       <c r="H79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I79" t="s">
         <v>180</v>
@@ -3921,7 +3949,7 @@
         <v>195</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H88">
         <v>0</v>

</xml_diff>

<commit_message>
zone duplicated added to cfg statistics
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1779,7 +1779,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G85" sqref="G85"/>
+      <selection pane="bottomLeft" activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3812,7 +3812,7 @@
         <v>0</v>
       </c>
       <c r="H81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I81" t="s">
         <v>180</v>
@@ -3949,7 +3949,7 @@
         <v>195</v>
       </c>
       <c r="G88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H88">
         <v>0</v>
@@ -3969,7 +3969,7 @@
         <v>256</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H89">
         <v>0</v>

</xml_diff>

<commit_message>
wwnp_duplicated added to zone and effective_cfg statistics
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="331">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -885,15 +885,6 @@
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Gs-labs</t>
   </si>
   <si>
-    <t>Complight</t>
-  </si>
-  <si>
-    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Complight\ssave</t>
-  </si>
-  <si>
-    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Complight\DEC2020</t>
-  </si>
-  <si>
     <t>before install</t>
   </si>
   <si>
@@ -1003,6 +994,24 @@
   </si>
   <si>
     <t>Mechel</t>
+  </si>
+  <si>
+    <t>Lenenergo</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Lenenergo\DEC2020</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Lenenergo\ssave</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Lenenergo\FEB2021</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Lenenergo\FEB2021\ssave</t>
+  </si>
+  <si>
+    <t>SAN Implementation</t>
   </si>
 </sst>
 </file>
@@ -1415,38 +1424,38 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:AA9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="29.7109375" customWidth="1"/>
     <col min="4" max="4" width="62" customWidth="1"/>
-    <col min="5" max="5" width="89.5703125" customWidth="1"/>
-    <col min="6" max="6" width="69.85546875" customWidth="1"/>
-    <col min="7" max="7" width="52.140625" customWidth="1"/>
-    <col min="8" max="8" width="73.140625" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" customWidth="1"/>
-    <col min="10" max="11" width="76" customWidth="1"/>
-    <col min="12" max="12" width="72.28515625" customWidth="1"/>
-    <col min="13" max="13" width="61.7109375" customWidth="1"/>
-    <col min="14" max="14" width="60" customWidth="1"/>
-    <col min="15" max="15" width="38.140625" customWidth="1"/>
-    <col min="16" max="16" width="69" customWidth="1"/>
-    <col min="17" max="17" width="72.42578125" customWidth="1"/>
-    <col min="18" max="18" width="111.5703125" customWidth="1"/>
-    <col min="19" max="19" width="72.5703125" customWidth="1"/>
-    <col min="20" max="20" width="86.85546875" customWidth="1"/>
-    <col min="21" max="22" width="64.7109375" customWidth="1"/>
-    <col min="23" max="23" width="54.5703125" customWidth="1"/>
-    <col min="24" max="24" width="75.42578125" customWidth="1"/>
-    <col min="25" max="25" width="58.140625" customWidth="1"/>
+    <col min="5" max="6" width="89.5703125" customWidth="1"/>
+    <col min="7" max="7" width="69.85546875" customWidth="1"/>
+    <col min="8" max="8" width="52.140625" customWidth="1"/>
+    <col min="9" max="9" width="73.140625" customWidth="1"/>
+    <col min="10" max="10" width="29.7109375" customWidth="1"/>
+    <col min="11" max="12" width="76" customWidth="1"/>
+    <col min="13" max="13" width="72.28515625" customWidth="1"/>
+    <col min="14" max="14" width="61.7109375" customWidth="1"/>
+    <col min="15" max="15" width="60" customWidth="1"/>
+    <col min="16" max="16" width="38.140625" customWidth="1"/>
+    <col min="17" max="17" width="69" customWidth="1"/>
+    <col min="18" max="18" width="72.42578125" customWidth="1"/>
+    <col min="19" max="19" width="111.5703125" customWidth="1"/>
+    <col min="20" max="20" width="72.5703125" customWidth="1"/>
+    <col min="21" max="21" width="86.85546875" customWidth="1"/>
+    <col min="22" max="23" width="64.7109375" customWidth="1"/>
+    <col min="24" max="24" width="54.5703125" customWidth="1"/>
+    <col min="25" max="25" width="75.42578125" customWidth="1"/>
+    <col min="26" max="26" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
@@ -1454,86 +1463,89 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F2" t="s">
-        <v>288</v>
+        <v>325</v>
       </c>
       <c r="G2" t="s">
+        <v>325</v>
+      </c>
+      <c r="H2" t="s">
         <v>286</v>
-      </c>
-      <c r="H2" t="s">
-        <v>282</v>
       </c>
       <c r="I2" t="s">
         <v>282</v>
       </c>
       <c r="J2" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="K2" t="s">
         <v>262</v>
       </c>
       <c r="L2" t="s">
+        <v>262</v>
+      </c>
+      <c r="M2" t="s">
         <v>244</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>237</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>189</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>188</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>155</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>111</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>97</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>83</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D3" s="12">
         <v>44223</v>
@@ -1541,227 +1553,239 @@
       <c r="E3" s="12">
         <v>44209</v>
       </c>
-      <c r="H3" s="12">
+      <c r="F3" s="12">
+        <v>44237</v>
+      </c>
+      <c r="I3" s="12">
         <v>44181</v>
       </c>
-      <c r="T3" s="1"/>
       <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA3" s="1"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>294</v>
-      </c>
-      <c r="H4" t="s">
-        <v>292</v>
+        <v>291</v>
+      </c>
+      <c r="F4" t="s">
+        <v>330</v>
       </c>
       <c r="I4" t="s">
-        <v>291</v>
-      </c>
-      <c r="T4" s="1"/>
+        <v>289</v>
+      </c>
+      <c r="J4" t="s">
+        <v>288</v>
+      </c>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AA4" s="1"/>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F5" t="s">
-        <v>290</v>
+        <v>328</v>
       </c>
       <c r="G5" t="s">
+        <v>326</v>
+      </c>
+      <c r="H5" t="s">
         <v>287</v>
       </c>
-      <c r="H5" t="s">
-        <v>295</v>
-      </c>
       <c r="I5" t="s">
+        <v>292</v>
+      </c>
+      <c r="J5" t="s">
         <v>284</v>
-      </c>
-      <c r="J5" t="s">
-        <v>263</v>
       </c>
       <c r="K5" t="s">
         <v>263</v>
       </c>
       <c r="L5" t="s">
+        <v>263</v>
+      </c>
+      <c r="M5" t="s">
         <v>246</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>236</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>225</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>187</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>157</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>113</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>98</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>85</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>1</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>74</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>72</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>4</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>25</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>60</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E6" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F6" t="s">
-        <v>289</v>
+        <v>329</v>
       </c>
       <c r="G6" t="s">
+        <v>327</v>
+      </c>
+      <c r="H6" t="s">
         <v>285</v>
       </c>
-      <c r="H6" t="s">
-        <v>296</v>
-      </c>
       <c r="I6" t="s">
+        <v>293</v>
+      </c>
+      <c r="J6" t="s">
         <v>283</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>277</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>264</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>245</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>234</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>224</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>186</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>156</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>112</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>108</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>84</v>
       </c>
-      <c r="T6" t="s">
-        <v>0</v>
-      </c>
       <c r="U6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V6" t="s">
         <v>73</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>71</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>3</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>24</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>59</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
       <c r="E7" t="s">
-        <v>322</v>
-      </c>
-      <c r="J7" t="s">
-        <v>266</v>
+        <v>319</v>
       </c>
       <c r="K7" t="s">
         <v>266</v>
       </c>
-      <c r="M7" t="s">
+      <c r="L7" t="s">
+        <v>266</v>
+      </c>
+      <c r="N7" t="s">
         <v>235</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>158</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>109</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>87</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>99</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="J8" t="s">
-        <v>268</v>
-      </c>
       <c r="K8" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>242</v>
       </c>
@@ -1778,8 +1802,8 @@
   <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E90" sqref="E90"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2748,16 +2772,16 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -2766,10 +2790,10 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3033,7 +3057,7 @@
         <v>171</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3179,7 +3203,7 @@
         <v>172</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -3187,7 +3211,7 @@
         <v>95</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -3199,7 +3223,7 @@
         <v>172</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -3247,7 +3271,7 @@
         <v>96</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -3259,7 +3283,7 @@
         <v>172</v>
       </c>
       <c r="J55" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -3422,7 +3446,7 @@
         <v>95</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -3643,7 +3667,7 @@
         <v>174</v>
       </c>
       <c r="J73" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
@@ -3766,7 +3790,7 @@
         <v>0</v>
       </c>
       <c r="H79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I79" t="s">
         <v>180</v>
@@ -3949,7 +3973,7 @@
         <v>195</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H88">
         <v>0</v>
@@ -3998,7 +4022,7 @@
         <v>243</v>
       </c>
       <c r="J90" s="10" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
@@ -4044,7 +4068,7 @@
         <v>232</v>
       </c>
       <c r="J92" s="10" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
@@ -4069,25 +4093,25 @@
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F94" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+      <c r="I94" t="s">
+        <v>315</v>
+      </c>
+      <c r="J94" t="s">
         <v>309</v>
-      </c>
-      <c r="G94">
-        <v>0</v>
-      </c>
-      <c r="H94">
-        <v>0</v>
-      </c>
-      <c r="I94" t="s">
-        <v>318</v>
-      </c>
-      <c r="J94" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
@@ -4095,7 +4119,7 @@
         <v>95</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -4104,10 +4128,10 @@
         <v>0</v>
       </c>
       <c r="I95" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="J95" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
@@ -4115,7 +4139,7 @@
         <v>96</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -4124,10 +4148,10 @@
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="J96" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
port speed and slot speed diversity notes added to the device connection statistics
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1802,8 +1802,8 @@
   <dimension ref="A1:J96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G92" sqref="G92"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G71" sqref="F71:G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3303,7 +3303,7 @@
         <v>0</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" t="s">
         <v>173</v>
@@ -3615,7 +3615,7 @@
         <v>281</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -3836,7 +3836,7 @@
         <v>0</v>
       </c>
       <c r="H81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I81" t="s">
         <v>180</v>
@@ -3973,7 +3973,7 @@
         <v>195</v>
       </c>
       <c r="G88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H88">
         <v>0</v>
@@ -3993,7 +3993,7 @@
         <v>256</v>
       </c>
       <c r="G89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89">
         <v>0</v>

</xml_diff>

<commit_message>
zone statistics and cfg statistics refactored for case if all devices are local
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -12,14 +12,14 @@
     <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$97</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="335">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1012,6 +1012,18 @@
   </si>
   <si>
     <t>SAN Implementation</t>
+  </si>
+  <si>
+    <t>CKR</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\CKR\SAN Impl FEB2021</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\CKR\FEB21</t>
+  </si>
+  <si>
+    <t>zoning_modified</t>
   </si>
 </sst>
 </file>
@@ -1424,368 +1436,383 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AA9"/>
+  <dimension ref="A1:AB9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="62" customWidth="1"/>
-    <col min="5" max="6" width="89.5703125" customWidth="1"/>
-    <col min="7" max="7" width="69.85546875" customWidth="1"/>
-    <col min="8" max="8" width="52.140625" customWidth="1"/>
-    <col min="9" max="9" width="73.140625" customWidth="1"/>
-    <col min="10" max="10" width="29.7109375" customWidth="1"/>
-    <col min="11" max="12" width="76" customWidth="1"/>
-    <col min="13" max="13" width="72.28515625" customWidth="1"/>
-    <col min="14" max="14" width="61.7109375" customWidth="1"/>
-    <col min="15" max="15" width="60" customWidth="1"/>
-    <col min="16" max="16" width="38.140625" customWidth="1"/>
-    <col min="17" max="17" width="69" customWidth="1"/>
-    <col min="18" max="18" width="72.42578125" customWidth="1"/>
-    <col min="19" max="19" width="111.5703125" customWidth="1"/>
-    <col min="20" max="20" width="72.5703125" customWidth="1"/>
-    <col min="21" max="21" width="86.85546875" customWidth="1"/>
-    <col min="22" max="23" width="64.7109375" customWidth="1"/>
-    <col min="24" max="24" width="54.5703125" customWidth="1"/>
-    <col min="25" max="25" width="75.42578125" customWidth="1"/>
-    <col min="26" max="26" width="58.140625" customWidth="1"/>
+    <col min="1" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="62" customWidth="1"/>
+    <col min="6" max="7" width="89.5703125" customWidth="1"/>
+    <col min="8" max="8" width="69.85546875" customWidth="1"/>
+    <col min="9" max="9" width="52.140625" customWidth="1"/>
+    <col min="10" max="10" width="73.140625" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" customWidth="1"/>
+    <col min="12" max="13" width="76" customWidth="1"/>
+    <col min="14" max="14" width="72.28515625" customWidth="1"/>
+    <col min="15" max="15" width="61.7109375" customWidth="1"/>
+    <col min="16" max="16" width="60" customWidth="1"/>
+    <col min="17" max="17" width="38.140625" customWidth="1"/>
+    <col min="18" max="18" width="69" customWidth="1"/>
+    <col min="19" max="19" width="72.42578125" customWidth="1"/>
+    <col min="20" max="20" width="111.5703125" customWidth="1"/>
+    <col min="21" max="21" width="72.5703125" customWidth="1"/>
+    <col min="22" max="22" width="86.85546875" customWidth="1"/>
+    <col min="23" max="24" width="64.7109375" customWidth="1"/>
+    <col min="25" max="25" width="54.5703125" customWidth="1"/>
+    <col min="26" max="26" width="75.42578125" customWidth="1"/>
+    <col min="27" max="27" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D2" t="s">
         <v>324</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>321</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>317</v>
-      </c>
-      <c r="F2" t="s">
-        <v>325</v>
       </c>
       <c r="G2" t="s">
         <v>325</v>
       </c>
       <c r="H2" t="s">
+        <v>325</v>
+      </c>
+      <c r="I2" t="s">
         <v>286</v>
-      </c>
-      <c r="I2" t="s">
-        <v>282</v>
       </c>
       <c r="J2" t="s">
         <v>282</v>
       </c>
       <c r="K2" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="L2" t="s">
         <v>262</v>
       </c>
       <c r="M2" t="s">
+        <v>262</v>
+      </c>
+      <c r="N2" t="s">
         <v>244</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>237</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>189</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>188</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>155</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>111</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>97</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>83</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="D3" s="12">
+      <c r="C3" s="12">
+        <v>44244</v>
+      </c>
+      <c r="E3" s="12">
         <v>44223</v>
       </c>
-      <c r="E3" s="12">
+      <c r="F3" s="12">
         <v>44209</v>
       </c>
-      <c r="F3" s="12">
+      <c r="G3" s="12">
         <v>44237</v>
       </c>
-      <c r="I3" s="12">
+      <c r="J3" s="12">
         <v>44181</v>
       </c>
-      <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB3" s="1"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="F4" t="s">
+      <c r="C4" t="s">
         <v>330</v>
       </c>
-      <c r="I4" t="s">
+      <c r="G4" t="s">
+        <v>330</v>
+      </c>
+      <c r="J4" t="s">
         <v>289</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>288</v>
       </c>
-      <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB4" s="1"/>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D5" t="s">
+      <c r="C5" t="s">
+        <v>332</v>
+      </c>
+      <c r="E5" t="s">
         <v>322</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>316</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>328</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>326</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>287</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>292</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>284</v>
-      </c>
-      <c r="K5" t="s">
-        <v>263</v>
       </c>
       <c r="L5" t="s">
         <v>263</v>
       </c>
       <c r="M5" t="s">
+        <v>263</v>
+      </c>
+      <c r="N5" t="s">
         <v>246</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>236</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>225</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>187</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>157</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>113</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>98</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>85</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>1</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>74</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>72</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>4</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>60</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" t="s">
+        <v>333</v>
+      </c>
+      <c r="E6" t="s">
         <v>323</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>318</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>329</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>327</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>285</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>293</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>283</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>277</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>264</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>245</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>234</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>224</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>186</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>156</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>112</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>108</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>84</v>
       </c>
-      <c r="U6" t="s">
-        <v>0</v>
-      </c>
       <c r="V6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W6" t="s">
         <v>73</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>71</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>3</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>24</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>59</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>319</v>
-      </c>
-      <c r="K7" t="s">
-        <v>266</v>
       </c>
       <c r="L7" t="s">
         <v>266</v>
       </c>
-      <c r="N7" t="s">
+      <c r="M7" t="s">
+        <v>266</v>
+      </c>
+      <c r="O7" t="s">
         <v>235</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>158</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>109</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>87</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>99</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="K8" t="s">
-        <v>268</v>
-      </c>
       <c r="L8" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>242</v>
       </c>
@@ -1799,11 +1826,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J96"/>
+  <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G71" sqref="F71:G72"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3303,7 +3330,7 @@
         <v>0</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" t="s">
         <v>173</v>
@@ -3615,7 +3642,7 @@
         <v>281</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -3853,7 +3880,7 @@
         <v>182</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82">
         <v>0</v>
@@ -3873,7 +3900,7 @@
         <v>183</v>
       </c>
       <c r="G83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H83">
         <v>0</v>
@@ -3893,7 +3920,7 @@
         <v>191</v>
       </c>
       <c r="G84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H84">
         <v>0</v>
@@ -3913,7 +3940,7 @@
         <v>192</v>
       </c>
       <c r="G85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H85">
         <v>0</v>
@@ -3933,7 +3960,7 @@
         <v>238</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H86">
         <v>0</v>
@@ -3953,7 +3980,7 @@
         <v>240</v>
       </c>
       <c r="G87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H87">
         <v>0</v>
@@ -3973,7 +4000,7 @@
         <v>195</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H88">
         <v>0</v>
@@ -3993,7 +4020,7 @@
         <v>256</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H89">
         <v>0</v>
@@ -4033,7 +4060,7 @@
         <v>231</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H91">
         <v>0</v>
@@ -4079,7 +4106,7 @@
         <v>194</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H93">
         <v>0</v>
@@ -4142,7 +4169,7 @@
         <v>307</v>
       </c>
       <c r="G96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H96">
         <v>0</v>
@@ -4152,6 +4179,29 @@
       </c>
       <c r="J96" t="s">
         <v>308</v>
+      </c>
+    </row>
+    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>178</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97" t="s">
+        <v>180</v>
+      </c>
+      <c r="J97" s="10" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
XISL count added to isl statistics
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -12,14 +12,14 @@
     <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$99</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="340">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1024,6 +1024,21 @@
   </si>
   <si>
     <t>zoning_modified</t>
+  </si>
+  <si>
+    <t>SAN Assessment</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Mechel</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Mechel\SAN Assessment FEB21</t>
+  </si>
+  <si>
+    <t>unique_isl_statistics</t>
+  </si>
+  <si>
+    <t>isl_aggregated_modified</t>
   </si>
 </sst>
 </file>
@@ -1439,12 +1454,14 @@
   <dimension ref="A1:AB9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="29.7109375" customWidth="1"/>
+    <col min="1" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="68.5703125" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" customWidth="1"/>
     <col min="5" max="5" width="62" customWidth="1"/>
     <col min="6" max="7" width="89.5703125" customWidth="1"/>
     <col min="8" max="8" width="69.85546875" customWidth="1"/>
@@ -1471,7 +1488,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1564,6 +1581,9 @@
       </c>
       <c r="C3" s="12">
         <v>44244</v>
+      </c>
+      <c r="D3" s="12">
+        <v>44245</v>
       </c>
       <c r="E3" s="12">
         <v>44223</v>
@@ -1592,6 +1612,9 @@
       <c r="C4" t="s">
         <v>330</v>
       </c>
+      <c r="D4" t="s">
+        <v>335</v>
+      </c>
       <c r="G4" t="s">
         <v>330</v>
       </c>
@@ -1616,6 +1639,9 @@
       <c r="C5" t="s">
         <v>332</v>
       </c>
+      <c r="D5" t="s">
+        <v>337</v>
+      </c>
       <c r="E5" t="s">
         <v>322</v>
       </c>
@@ -1695,6 +1721,9 @@
       </c>
       <c r="C6" t="s">
         <v>333</v>
+      </c>
+      <c r="D6" t="s">
+        <v>336</v>
       </c>
       <c r="E6" t="s">
         <v>323</v>
@@ -1826,11 +1855,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G80" sqref="G80"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3049,7 +3078,7 @@
         <v>161</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -3115,7 +3144,7 @@
         <v>61</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -3135,7 +3164,7 @@
         <v>62</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -3155,7 +3184,7 @@
         <v>63</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -3175,7 +3204,7 @@
         <v>65</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -3195,7 +3224,7 @@
         <v>64</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -3244,7 +3273,7 @@
         <v>0</v>
       </c>
       <c r="H52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" t="s">
         <v>172</v>
@@ -3261,7 +3290,7 @@
         <v>67</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -3281,7 +3310,7 @@
         <v>68</v>
       </c>
       <c r="G54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -3301,7 +3330,7 @@
         <v>298</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -3330,7 +3359,7 @@
         <v>0</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" t="s">
         <v>173</v>
@@ -3410,7 +3439,7 @@
         <v>0</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60" t="s">
         <v>173</v>
@@ -3499,7 +3528,7 @@
         <v>100</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -3522,7 +3551,7 @@
         <v>102</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -3542,7 +3571,7 @@
         <v>103</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -3562,7 +3591,7 @@
         <v>104</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -3582,7 +3611,7 @@
         <v>105</v>
       </c>
       <c r="G68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -3602,7 +3631,7 @@
         <v>106</v>
       </c>
       <c r="G69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -3622,7 +3651,7 @@
         <v>107</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -3642,7 +3671,7 @@
         <v>281</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -3662,7 +3691,7 @@
         <v>165</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -3705,7 +3734,7 @@
         <v>168</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -3725,7 +3754,7 @@
         <v>169</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -3745,7 +3774,7 @@
         <v>170</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -3771,7 +3800,7 @@
         <v>0</v>
       </c>
       <c r="H77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I77" t="s">
         <v>180</v>
@@ -4172,7 +4201,7 @@
         <v>1</v>
       </c>
       <c r="H96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I96" t="s">
         <v>315</v>
@@ -4201,6 +4230,46 @@
         <v>180</v>
       </c>
       <c r="J97" s="10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D98" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98" t="s">
+        <v>180</v>
+      </c>
+      <c r="J98" s="10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D99" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99" t="s">
+        <v>180</v>
+      </c>
+      <c r="J99" s="10" t="s">
         <v>220</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fabric labeleing module refactoring. protection from fabric name, fabric label nonuniformity added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="343">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1039,6 +1039,15 @@
   </si>
   <si>
     <t>isl_aggregated_modified</t>
+  </si>
+  <si>
+    <t>Fabric-Device Management Interface (FDMI) information</t>
+  </si>
+  <si>
+    <t>Local NS information</t>
+  </si>
+  <si>
+    <t>Cached NS information</t>
   </si>
 </sst>
 </file>
@@ -1858,8 +1867,8 @@
   <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2281,7 +2290,7 @@
         <v>144</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>220</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2313,7 +2322,7 @@
         <v>144</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>220</v>
+        <v>341</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2345,7 +2354,7 @@
         <v>144</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>220</v>
+        <v>342</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -3078,7 +3087,7 @@
         <v>161</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -3144,7 +3153,7 @@
         <v>61</v>
       </c>
       <c r="G46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -3164,7 +3173,7 @@
         <v>62</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -3184,7 +3193,7 @@
         <v>63</v>
       </c>
       <c r="G48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -3204,7 +3213,7 @@
         <v>65</v>
       </c>
       <c r="G49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -3224,7 +3233,7 @@
         <v>64</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -3273,7 +3282,7 @@
         <v>0</v>
       </c>
       <c r="H52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" t="s">
         <v>172</v>
@@ -3290,7 +3299,7 @@
         <v>67</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -3310,7 +3319,7 @@
         <v>68</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -3330,7 +3339,7 @@
         <v>298</v>
       </c>
       <c r="G55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -3359,7 +3368,7 @@
         <v>0</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" t="s">
         <v>173</v>
@@ -3439,7 +3448,7 @@
         <v>0</v>
       </c>
       <c r="H60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" t="s">
         <v>173</v>
@@ -3528,7 +3537,7 @@
         <v>100</v>
       </c>
       <c r="G64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -3551,7 +3560,7 @@
         <v>102</v>
       </c>
       <c r="G65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -3571,7 +3580,7 @@
         <v>103</v>
       </c>
       <c r="G66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -3591,7 +3600,7 @@
         <v>104</v>
       </c>
       <c r="G67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -3611,7 +3620,7 @@
         <v>105</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -3631,7 +3640,7 @@
         <v>106</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -3651,7 +3660,7 @@
         <v>107</v>
       </c>
       <c r="G70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -3671,7 +3680,7 @@
         <v>281</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -3691,7 +3700,7 @@
         <v>165</v>
       </c>
       <c r="G72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -3734,7 +3743,7 @@
         <v>168</v>
       </c>
       <c r="G74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -3754,7 +3763,7 @@
         <v>169</v>
       </c>
       <c r="G75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -3774,7 +3783,7 @@
         <v>170</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -3800,7 +3809,7 @@
         <v>0</v>
       </c>
       <c r="H77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I77" t="s">
         <v>180</v>
@@ -3909,7 +3918,7 @@
         <v>182</v>
       </c>
       <c r="G82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H82">
         <v>0</v>
@@ -3929,7 +3938,7 @@
         <v>183</v>
       </c>
       <c r="G83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H83">
         <v>0</v>
@@ -3949,7 +3958,7 @@
         <v>191</v>
       </c>
       <c r="G84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H84">
         <v>0</v>
@@ -3969,7 +3978,7 @@
         <v>192</v>
       </c>
       <c r="G85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H85">
         <v>0</v>
@@ -3989,7 +3998,7 @@
         <v>238</v>
       </c>
       <c r="G86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H86">
         <v>0</v>
@@ -4009,7 +4018,7 @@
         <v>240</v>
       </c>
       <c r="G87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H87">
         <v>0</v>
@@ -4029,7 +4038,7 @@
         <v>195</v>
       </c>
       <c r="G88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H88">
         <v>0</v>
@@ -4049,7 +4058,7 @@
         <v>256</v>
       </c>
       <c r="G89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89">
         <v>0</v>
@@ -4089,7 +4098,7 @@
         <v>231</v>
       </c>
       <c r="G91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H91">
         <v>0</v>
@@ -4135,7 +4144,7 @@
         <v>194</v>
       </c>
       <c r="G93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H93">
         <v>0</v>
@@ -4178,7 +4187,7 @@
         <v>314</v>
       </c>
       <c r="G95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H95">
         <v>0</v>

</xml_diff>

<commit_message>
Total unzoned device count added to active cfg statistics module
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="346">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1048,6 +1048,15 @@
   </si>
   <si>
     <t>Cached NS information</t>
+  </si>
+  <si>
+    <t>SAN Implementation. Checking</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Lenenergo\FEB2021_verification</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Lenenergo\FEB2021\ssave_25022021</t>
   </si>
 </sst>
 </file>
@@ -1460,10 +1469,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AB9"/>
+  <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,36 +1481,36 @@
     <col min="3" max="3" width="68.5703125" customWidth="1"/>
     <col min="4" max="4" width="48.7109375" customWidth="1"/>
     <col min="5" max="5" width="62" customWidth="1"/>
-    <col min="6" max="7" width="89.5703125" customWidth="1"/>
-    <col min="8" max="8" width="69.85546875" customWidth="1"/>
-    <col min="9" max="9" width="52.140625" customWidth="1"/>
-    <col min="10" max="10" width="73.140625" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" customWidth="1"/>
-    <col min="12" max="13" width="76" customWidth="1"/>
-    <col min="14" max="14" width="72.28515625" customWidth="1"/>
-    <col min="15" max="15" width="61.7109375" customWidth="1"/>
-    <col min="16" max="16" width="60" customWidth="1"/>
-    <col min="17" max="17" width="38.140625" customWidth="1"/>
-    <col min="18" max="18" width="69" customWidth="1"/>
-    <col min="19" max="19" width="72.42578125" customWidth="1"/>
-    <col min="20" max="20" width="111.5703125" customWidth="1"/>
-    <col min="21" max="21" width="72.5703125" customWidth="1"/>
-    <col min="22" max="22" width="86.85546875" customWidth="1"/>
-    <col min="23" max="24" width="64.7109375" customWidth="1"/>
-    <col min="25" max="25" width="54.5703125" customWidth="1"/>
-    <col min="26" max="26" width="75.42578125" customWidth="1"/>
-    <col min="27" max="27" width="58.140625" customWidth="1"/>
+    <col min="6" max="8" width="89.5703125" customWidth="1"/>
+    <col min="9" max="9" width="69.85546875" customWidth="1"/>
+    <col min="10" max="10" width="52.140625" customWidth="1"/>
+    <col min="11" max="11" width="73.140625" customWidth="1"/>
+    <col min="12" max="12" width="29.7109375" customWidth="1"/>
+    <col min="13" max="14" width="76" customWidth="1"/>
+    <col min="15" max="15" width="72.28515625" customWidth="1"/>
+    <col min="16" max="16" width="61.7109375" customWidth="1"/>
+    <col min="17" max="17" width="60" customWidth="1"/>
+    <col min="18" max="18" width="38.140625" customWidth="1"/>
+    <col min="19" max="19" width="69" customWidth="1"/>
+    <col min="20" max="20" width="72.42578125" customWidth="1"/>
+    <col min="21" max="21" width="111.5703125" customWidth="1"/>
+    <col min="22" max="22" width="72.5703125" customWidth="1"/>
+    <col min="23" max="23" width="86.85546875" customWidth="1"/>
+    <col min="24" max="25" width="64.7109375" customWidth="1"/>
+    <col min="26" max="26" width="54.5703125" customWidth="1"/>
+    <col min="27" max="27" width="75.42578125" customWidth="1"/>
+    <col min="28" max="28" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
@@ -1524,67 +1533,70 @@
         <v>325</v>
       </c>
       <c r="I2" t="s">
+        <v>325</v>
+      </c>
+      <c r="J2" t="s">
         <v>286</v>
-      </c>
-      <c r="J2" t="s">
-        <v>282</v>
       </c>
       <c r="K2" t="s">
         <v>282</v>
       </c>
       <c r="L2" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="M2" t="s">
         <v>262</v>
       </c>
       <c r="N2" t="s">
+        <v>262</v>
+      </c>
+      <c r="O2" t="s">
         <v>244</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>237</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>189</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>188</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>155</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>111</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>97</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>83</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>290</v>
       </c>
@@ -1601,20 +1613,23 @@
         <v>44209</v>
       </c>
       <c r="G3" s="12">
+        <v>44253</v>
+      </c>
+      <c r="H3" s="12">
         <v>44237</v>
       </c>
-      <c r="J3" s="12">
+      <c r="K3" s="12">
         <v>44181</v>
       </c>
-      <c r="V3" s="1"/>
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC3" s="1"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>291</v>
       </c>
@@ -1625,23 +1640,26 @@
         <v>335</v>
       </c>
       <c r="G4" t="s">
+        <v>343</v>
+      </c>
+      <c r="H4" t="s">
         <v>330</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>289</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>288</v>
       </c>
-      <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC4" s="1"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
@@ -1658,73 +1676,76 @@
         <v>316</v>
       </c>
       <c r="G5" t="s">
+        <v>344</v>
+      </c>
+      <c r="H5" t="s">
         <v>328</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>326</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>287</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>292</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>284</v>
-      </c>
-      <c r="L5" t="s">
-        <v>263</v>
       </c>
       <c r="M5" t="s">
         <v>263</v>
       </c>
       <c r="N5" t="s">
+        <v>263</v>
+      </c>
+      <c r="O5" t="s">
         <v>246</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>236</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>225</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>187</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>157</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>113</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>98</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>85</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>1</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>74</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>72</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>4</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>25</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>60</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
@@ -1741,116 +1762,119 @@
         <v>318</v>
       </c>
       <c r="G6" t="s">
+        <v>345</v>
+      </c>
+      <c r="H6" t="s">
         <v>329</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>327</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>285</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>293</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>283</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>277</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>264</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>245</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>234</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>224</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>186</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>156</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>112</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>108</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>84</v>
       </c>
-      <c r="V6" t="s">
-        <v>0</v>
-      </c>
       <c r="W6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X6" t="s">
         <v>73</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>71</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>3</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>24</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>59</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
       <c r="F7" t="s">
         <v>319</v>
       </c>
-      <c r="L7" t="s">
-        <v>266</v>
-      </c>
       <c r="M7" t="s">
         <v>266</v>
       </c>
-      <c r="O7" t="s">
+      <c r="N7" t="s">
+        <v>266</v>
+      </c>
+      <c r="P7" t="s">
         <v>235</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>158</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>109</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>87</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>99</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="L8" t="s">
-        <v>268</v>
-      </c>
       <c r="M8" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>242</v>
       </c>
@@ -1867,8 +1891,8 @@
   <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G98" sqref="G98"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H94" sqref="H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4058,10 +4082,10 @@
         <v>256</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I89" t="s">
         <v>180</v>
@@ -4187,7 +4211,7 @@
         <v>314</v>
       </c>
       <c r="G95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H95">
         <v>0</v>
@@ -4207,10 +4231,10 @@
         <v>307</v>
       </c>
       <c r="G96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96" t="s">
         <v>315</v>

</xml_diff>

<commit_message>
added correct_zone, commented_zone, non-working_zone summary to actice cfg statistics
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1891,8 +1891,8 @@
   <dimension ref="A1:J99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H94" sqref="H94"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3942,7 +3942,7 @@
         <v>182</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82">
         <v>0</v>
@@ -4062,10 +4062,10 @@
         <v>195</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I88" t="s">
         <v>180</v>
@@ -4085,7 +4085,7 @@
         <v>1</v>
       </c>
       <c r="H89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I89" t="s">
         <v>180</v>

</xml_diff>

<commit_message>
unused zone counter added to active cfg statistic
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1471,8 +1471,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AC9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,7 +1506,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1892,7 +1892,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F93" sqref="F93"/>
+      <selection pane="bottomLeft" activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
       <c r="H81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I81" t="s">
         <v>180</v>
@@ -3942,7 +3942,7 @@
         <v>182</v>
       </c>
       <c r="G82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H82">
         <v>0</v>
@@ -4062,10 +4062,10 @@
         <v>195</v>
       </c>
       <c r="G88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I88" t="s">
         <v>180</v>

</xml_diff>

<commit_message>
alias statistics added, cfg statistics refactored
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -12,14 +12,14 @@
     <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$101</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="367">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -675,12 +675,6 @@
     <t>Порты устройств, не входящие в конфигурацию зонирования</t>
   </si>
   <si>
-    <t>Статистическая информация о портах коммутаторов</t>
-  </si>
-  <si>
-    <t>Статистическая информация о зонах</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -816,9 +810,6 @@
     <t>C:\Users\vlasenko\Documents\06.CONFIGS\Rencredit\Supportsave</t>
   </si>
   <si>
-    <t>Chassis parameters</t>
-  </si>
-  <si>
     <t>C:\Users\vlasenko\Documents\06.CONFIGS\Rencredit\blades</t>
   </si>
   <si>
@@ -861,9 +852,6 @@
     <t>Device connection statistics</t>
   </si>
   <si>
-    <t>Статистическая информация о портах устройств</t>
-  </si>
-  <si>
     <t>Статистика_устройств</t>
   </si>
   <si>
@@ -1057,6 +1045,81 @@
   </si>
   <si>
     <t>C:\Users\vlasenko\Documents\06.CONFIGS\Lenenergo\FEB2021\ssave_25022021</t>
+  </si>
+  <si>
+    <t>Unicredit</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Unicredit\SAN Assessment\MAR 2021</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\UniCredit\MAR 2021\blades</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\UniCredit\MAR 2021\synergy</t>
+  </si>
+  <si>
+    <t>NS entries with no regex patterns</t>
+  </si>
+  <si>
+    <t>Flag to force change group name usage mode</t>
+  </si>
+  <si>
+    <t>alias_statistics</t>
+  </si>
+  <si>
+    <t>Alias configuration statistics</t>
+  </si>
+  <si>
+    <t>Zoning configuration</t>
+  </si>
+  <si>
+    <t>Alias configuration</t>
+  </si>
+  <si>
+    <t>Zoning configuration statistics</t>
+  </si>
+  <si>
+    <t>Device connection statistics with zones</t>
+  </si>
+  <si>
+    <t>Статистика_псевдонимов</t>
+  </si>
+  <si>
+    <t>Статистическая информация зон</t>
+  </si>
+  <si>
+    <t>Статистическая информация псевдонимов</t>
+  </si>
+  <si>
+    <t>Expected AG links</t>
+  </si>
+  <si>
+    <t>Chassis parameters collection</t>
+  </si>
+  <si>
+    <t>Switch parameters collection</t>
+  </si>
+  <si>
+    <t>Switch and port status collection</t>
+  </si>
+  <si>
+    <t>MAPS parameters collection</t>
+  </si>
+  <si>
+    <t>Fabricshow collection</t>
+  </si>
+  <si>
+    <t>AG principal collection</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\UniCredit\MAR 2021\supportsave_20210310</t>
+  </si>
+  <si>
+    <t>Статистическая информация портов устройств</t>
+  </si>
+  <si>
+    <t>Статистическая информация портов коммутаторов</t>
   </si>
 </sst>
 </file>
@@ -1469,414 +1532,439 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AC9"/>
+  <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="68.5703125" customWidth="1"/>
-    <col min="4" max="4" width="48.7109375" customWidth="1"/>
-    <col min="5" max="5" width="62" customWidth="1"/>
-    <col min="6" max="8" width="89.5703125" customWidth="1"/>
-    <col min="9" max="9" width="69.85546875" customWidth="1"/>
-    <col min="10" max="10" width="52.140625" customWidth="1"/>
-    <col min="11" max="11" width="73.140625" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" customWidth="1"/>
-    <col min="13" max="14" width="76" customWidth="1"/>
-    <col min="15" max="15" width="72.28515625" customWidth="1"/>
-    <col min="16" max="16" width="61.7109375" customWidth="1"/>
-    <col min="17" max="17" width="60" customWidth="1"/>
-    <col min="18" max="18" width="38.140625" customWidth="1"/>
-    <col min="19" max="19" width="69" customWidth="1"/>
-    <col min="20" max="20" width="72.42578125" customWidth="1"/>
-    <col min="21" max="21" width="111.5703125" customWidth="1"/>
-    <col min="22" max="22" width="72.5703125" customWidth="1"/>
-    <col min="23" max="23" width="86.85546875" customWidth="1"/>
-    <col min="24" max="25" width="64.7109375" customWidth="1"/>
-    <col min="26" max="26" width="54.5703125" customWidth="1"/>
-    <col min="27" max="27" width="75.42578125" customWidth="1"/>
-    <col min="28" max="28" width="58.140625" customWidth="1"/>
+    <col min="3" max="3" width="80.140625" customWidth="1"/>
+    <col min="4" max="4" width="68.5703125" customWidth="1"/>
+    <col min="5" max="5" width="48.7109375" customWidth="1"/>
+    <col min="6" max="6" width="62" customWidth="1"/>
+    <col min="7" max="9" width="89.5703125" customWidth="1"/>
+    <col min="10" max="10" width="69.85546875" customWidth="1"/>
+    <col min="11" max="11" width="52.140625" customWidth="1"/>
+    <col min="12" max="12" width="73.140625" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" customWidth="1"/>
+    <col min="14" max="15" width="76" customWidth="1"/>
+    <col min="16" max="16" width="72.28515625" customWidth="1"/>
+    <col min="17" max="17" width="61.7109375" customWidth="1"/>
+    <col min="18" max="18" width="60" customWidth="1"/>
+    <col min="19" max="19" width="38.140625" customWidth="1"/>
+    <col min="20" max="20" width="69" customWidth="1"/>
+    <col min="21" max="21" width="72.42578125" customWidth="1"/>
+    <col min="22" max="22" width="111.5703125" customWidth="1"/>
+    <col min="23" max="23" width="72.5703125" customWidth="1"/>
+    <col min="24" max="24" width="86.85546875" customWidth="1"/>
+    <col min="25" max="26" width="64.7109375" customWidth="1"/>
+    <col min="27" max="27" width="54.5703125" customWidth="1"/>
+    <col min="28" max="28" width="75.42578125" customWidth="1"/>
+    <col min="29" max="29" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="D2" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="E2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F2" t="s">
         <v>317</v>
       </c>
       <c r="G2" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="H2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="I2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="J2" t="s">
-        <v>286</v>
+        <v>321</v>
       </c>
       <c r="K2" t="s">
         <v>282</v>
       </c>
       <c r="L2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="M2" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="N2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="O2" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="P2" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="Q2" t="s">
+        <v>235</v>
+      </c>
+      <c r="R2" t="s">
         <v>189</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>188</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>155</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>111</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>97</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>83</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C3" s="12">
+        <v>44260</v>
+      </c>
+      <c r="D3" s="12">
         <v>44244</v>
       </c>
-      <c r="D3" s="12">
+      <c r="E3" s="12">
         <v>44245</v>
       </c>
-      <c r="E3" s="12">
+      <c r="F3" s="12">
         <v>44223</v>
       </c>
-      <c r="F3" s="12">
+      <c r="G3" s="12">
         <v>44209</v>
       </c>
-      <c r="G3" s="12">
+      <c r="H3" s="12">
         <v>44253</v>
       </c>
-      <c r="H3" s="12">
+      <c r="I3" s="12">
         <v>44237</v>
       </c>
-      <c r="K3" s="12">
+      <c r="L3" s="12">
         <v>44181</v>
       </c>
-      <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD3" s="1"/>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C4" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D4" t="s">
-        <v>335</v>
+        <v>326</v>
+      </c>
+      <c r="E4" t="s">
+        <v>331</v>
       </c>
       <c r="G4" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="H4" t="s">
-        <v>330</v>
-      </c>
-      <c r="K4" t="s">
-        <v>289</v>
+        <v>339</v>
+      </c>
+      <c r="I4" t="s">
+        <v>326</v>
       </c>
       <c r="L4" t="s">
-        <v>288</v>
-      </c>
-      <c r="W4" s="1"/>
+        <v>285</v>
+      </c>
+      <c r="M4" t="s">
+        <v>284</v>
+      </c>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD4" s="1"/>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="D5" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="E5" t="s">
+        <v>333</v>
+      </c>
+      <c r="F5" t="s">
+        <v>318</v>
+      </c>
+      <c r="G5" t="s">
+        <v>312</v>
+      </c>
+      <c r="H5" t="s">
+        <v>340</v>
+      </c>
+      <c r="I5" t="s">
+        <v>324</v>
+      </c>
+      <c r="J5" t="s">
         <v>322</v>
       </c>
-      <c r="F5" t="s">
-        <v>316</v>
-      </c>
-      <c r="G5" t="s">
-        <v>344</v>
-      </c>
-      <c r="H5" t="s">
-        <v>328</v>
-      </c>
-      <c r="I5" t="s">
-        <v>326</v>
-      </c>
-      <c r="J5" t="s">
-        <v>287</v>
-      </c>
       <c r="K5" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="L5" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="M5" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="N5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="O5" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
       <c r="P5" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="Q5" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="R5" t="s">
+        <v>223</v>
+      </c>
+      <c r="S5" t="s">
         <v>187</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>157</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>113</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>98</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>85</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>1</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>74</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>72</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>4</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>25</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>60</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>333</v>
+        <v>364</v>
       </c>
       <c r="D6" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="E6" t="s">
+        <v>332</v>
+      </c>
+      <c r="F6" t="s">
+        <v>319</v>
+      </c>
+      <c r="G6" t="s">
+        <v>314</v>
+      </c>
+      <c r="H6" t="s">
+        <v>341</v>
+      </c>
+      <c r="I6" t="s">
+        <v>325</v>
+      </c>
+      <c r="J6" t="s">
         <v>323</v>
       </c>
-      <c r="F6" t="s">
-        <v>318</v>
-      </c>
-      <c r="G6" t="s">
-        <v>345</v>
-      </c>
-      <c r="H6" t="s">
-        <v>329</v>
-      </c>
-      <c r="I6" t="s">
-        <v>327</v>
-      </c>
-      <c r="J6" t="s">
-        <v>285</v>
-      </c>
       <c r="K6" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="L6" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="M6" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="N6" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="O6" t="s">
-        <v>245</v>
+        <v>262</v>
       </c>
       <c r="P6" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="Q6" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="R6" t="s">
+        <v>222</v>
+      </c>
+      <c r="S6" t="s">
         <v>186</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>156</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>112</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>108</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>84</v>
       </c>
-      <c r="W6" t="s">
-        <v>0</v>
-      </c>
       <c r="X6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="s">
         <v>73</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>71</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>3</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>24</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>59</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="F7" t="s">
-        <v>319</v>
-      </c>
-      <c r="M7" t="s">
-        <v>266</v>
+      <c r="C7" t="s">
+        <v>344</v>
+      </c>
+      <c r="G7" t="s">
+        <v>315</v>
       </c>
       <c r="N7" t="s">
-        <v>266</v>
-      </c>
-      <c r="P7" t="s">
-        <v>235</v>
-      </c>
-      <c r="S7" t="s">
+        <v>263</v>
+      </c>
+      <c r="O7" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>233</v>
+      </c>
+      <c r="T7" t="s">
         <v>158</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>109</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>87</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>99</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="M8" t="s">
-        <v>268</v>
+        <v>264</v>
+      </c>
+      <c r="C8" t="s">
+        <v>345</v>
       </c>
       <c r="N8" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+      <c r="O8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -1888,11 +1976,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J99"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G94" sqref="G94"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O110" sqref="O109:O110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1965,7 +2053,7 @@
         <v>153</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1994,7 +2082,7 @@
         <v>153</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2026,7 +2114,7 @@
         <v>142</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>265</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2058,7 +2146,7 @@
         <v>151</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>220</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2090,7 +2178,7 @@
         <v>151</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>220</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2122,7 +2210,7 @@
         <v>152</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>220</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2154,7 +2242,7 @@
         <v>148</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>220</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2186,7 +2274,7 @@
         <v>148</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>220</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2218,7 +2306,7 @@
         <v>146</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2250,7 +2338,7 @@
         <v>147</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2282,7 +2370,7 @@
         <v>147</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2314,7 +2402,7 @@
         <v>144</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2346,7 +2434,7 @@
         <v>144</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2378,7 +2466,7 @@
         <v>144</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2410,7 +2498,7 @@
         <v>145</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2442,7 +2530,7 @@
         <v>145</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2474,7 +2562,7 @@
         <v>145</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2506,7 +2594,7 @@
         <v>143</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2535,7 +2623,7 @@
         <v>143</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2564,7 +2652,7 @@
         <v>143</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2593,7 +2681,7 @@
         <v>143</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -2619,7 +2707,7 @@
         <v>143</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2645,7 +2733,7 @@
         <v>143</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -2674,7 +2762,7 @@
         <v>149</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -2700,7 +2788,7 @@
         <v>149</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2726,7 +2814,7 @@
         <v>149</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2752,7 +2840,7 @@
         <v>149</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2778,7 +2866,7 @@
         <v>149</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2792,7 +2880,7 @@
         <v>94</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -2804,7 +2892,7 @@
         <v>149</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2818,7 +2906,7 @@
         <v>94</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -2830,21 +2918,21 @@
         <v>149</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -2853,24 +2941,24 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -2879,10 +2967,10 @@
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -2908,10 +2996,10 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -2934,10 +3022,10 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2960,22 +3048,22 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -2984,34 +3072,34 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F38" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
         <v>271</v>
       </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38" t="s">
-        <v>274</v>
-      </c>
       <c r="J38" s="10" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -3037,7 +3125,7 @@
         <v>159</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -3057,7 +3145,7 @@
         <v>159</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -3077,7 +3165,7 @@
         <v>159</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -3100,7 +3188,7 @@
         <v>163</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -3146,7 +3234,7 @@
         <v>171</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3166,7 +3254,7 @@
         <v>171</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3292,7 +3380,7 @@
         <v>172</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -3300,7 +3388,7 @@
         <v>95</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -3312,7 +3400,7 @@
         <v>172</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -3360,7 +3448,7 @@
         <v>96</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -3372,7 +3460,7 @@
         <v>172</v>
       </c>
       <c r="J55" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -3398,7 +3486,7 @@
         <v>173</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -3406,7 +3494,7 @@
         <v>95</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -3418,7 +3506,7 @@
         <v>173</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -3426,7 +3514,7 @@
         <v>95</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -3438,7 +3526,7 @@
         <v>173</v>
       </c>
       <c r="J58" s="10" t="s">
-        <v>220</v>
+        <v>347</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -3446,7 +3534,7 @@
         <v>95</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -3458,15 +3546,15 @@
         <v>173</v>
       </c>
       <c r="J59" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D60" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -3478,7 +3566,7 @@
         <v>173</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -3501,7 +3589,7 @@
         <v>173</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -3527,7 +3615,7 @@
         <v>173</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>220</v>
+        <v>346</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -3535,7 +3623,7 @@
         <v>95</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -3547,7 +3635,7 @@
         <v>173</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>220</v>
+        <v>357</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -3701,7 +3789,7 @@
         <v>96</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -3713,7 +3801,7 @@
         <v>173</v>
       </c>
       <c r="J71" t="s">
-        <v>280</v>
+        <v>365</v>
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
@@ -3744,7 +3832,7 @@
         <v>95</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -3756,7 +3844,7 @@
         <v>174</v>
       </c>
       <c r="J73" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
@@ -3816,7 +3904,7 @@
         <v>167</v>
       </c>
       <c r="J76" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
@@ -3839,12 +3927,12 @@
         <v>180</v>
       </c>
       <c r="J77" s="10" t="s">
-        <v>220</v>
+        <v>350</v>
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>95</v>
@@ -3862,12 +3950,12 @@
         <v>180</v>
       </c>
       <c r="J78" s="10" t="s">
-        <v>220</v>
+        <v>351</v>
       </c>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>95</v>
@@ -3885,18 +3973,18 @@
         <v>180</v>
       </c>
       <c r="J79" s="10" t="s">
-        <v>220</v>
+        <v>352</v>
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -3908,38 +3996,38 @@
         <v>180</v>
       </c>
       <c r="J80" s="10" t="s">
-        <v>220</v>
+        <v>353</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>258</v>
-      </c>
       <c r="D81" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>254</v>
+        <v>348</v>
       </c>
       <c r="G81">
         <v>0</v>
       </c>
       <c r="H81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I81" t="s">
         <v>180</v>
       </c>
       <c r="J81" s="10" t="s">
-        <v>255</v>
+        <v>349</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D82" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>182</v>
+      <c r="B82" t="s">
+        <v>256</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>252</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -3950,8 +4038,8 @@
       <c r="I82" t="s">
         <v>180</v>
       </c>
-      <c r="J82" t="s">
-        <v>215</v>
+      <c r="J82" s="10" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -3959,7 +4047,7 @@
         <v>96</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -3971,7 +4059,7 @@
         <v>180</v>
       </c>
       <c r="J83" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
@@ -3979,7 +4067,7 @@
         <v>96</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -3991,7 +4079,7 @@
         <v>180</v>
       </c>
       <c r="J84" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
@@ -3999,7 +4087,7 @@
         <v>96</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -4011,7 +4099,7 @@
         <v>180</v>
       </c>
       <c r="J85" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
@@ -4019,7 +4107,7 @@
         <v>96</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>238</v>
+        <v>192</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -4031,7 +4119,7 @@
         <v>180</v>
       </c>
       <c r="J86" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
@@ -4039,7 +4127,7 @@
         <v>96</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -4051,7 +4139,7 @@
         <v>180</v>
       </c>
       <c r="J87" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
@@ -4059,7 +4147,7 @@
         <v>96</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>195</v>
+        <v>238</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -4071,7 +4159,7 @@
         <v>180</v>
       </c>
       <c r="J88" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
@@ -4079,10 +4167,10 @@
         <v>96</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>256</v>
+        <v>195</v>
       </c>
       <c r="G89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89">
         <v>0</v>
@@ -4091,27 +4179,27 @@
         <v>180</v>
       </c>
       <c r="J89" t="s">
-        <v>257</v>
+        <v>355</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D90" s="6" t="s">
-        <v>95</v>
+      <c r="D90" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>230</v>
+        <v>354</v>
       </c>
       <c r="G90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I90" t="s">
-        <v>243</v>
-      </c>
-      <c r="J90" s="10" t="s">
-        <v>312</v>
+        <v>180</v>
+      </c>
+      <c r="J90" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
@@ -4119,33 +4207,27 @@
         <v>96</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H91">
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>243</v>
+        <v>180</v>
       </c>
       <c r="J91" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>17</v>
-      </c>
-      <c r="B92" t="s">
-        <v>137</v>
-      </c>
       <c r="D92" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F92" s="9" t="s">
-        <v>193</v>
+      <c r="F92" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -4154,10 +4236,10 @@
         <v>0</v>
       </c>
       <c r="I92" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="J92" s="10" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
@@ -4165,7 +4247,7 @@
         <v>96</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>194</v>
+        <v>229</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -4174,21 +4256,24 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="J93" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>17</v>
+      </c>
       <c r="B94" t="s">
-        <v>305</v>
+        <v>137</v>
       </c>
       <c r="D94" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F94" s="9" t="s">
-        <v>306</v>
+        <v>193</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -4197,38 +4282,41 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>315</v>
-      </c>
-      <c r="J94" t="s">
+        <v>230</v>
+      </c>
+      <c r="J94" s="10" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D95" s="6" t="s">
+      <c r="D95" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95" t="s">
+        <v>230</v>
+      </c>
+      <c r="J95" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>301</v>
+      </c>
+      <c r="D96" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F95" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="G95">
-        <v>0</v>
-      </c>
-      <c r="H95">
-        <v>0</v>
-      </c>
-      <c r="I95" t="s">
-        <v>315</v>
-      </c>
-      <c r="J95" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D96" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>307</v>
+      <c r="F96" s="9" t="s">
+        <v>302</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -4237,21 +4325,18 @@
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="J96" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>178</v>
-      </c>
       <c r="D97" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F97" s="9" t="s">
-        <v>334</v>
+      <c r="F97" s="2" t="s">
+        <v>310</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -4260,18 +4345,18 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>180</v>
-      </c>
-      <c r="J97" s="10" t="s">
-        <v>220</v>
+        <v>311</v>
+      </c>
+      <c r="J97" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D98" s="6" t="s">
-        <v>95</v>
+      <c r="D98" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>338</v>
+        <v>303</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -4280,18 +4365,21 @@
         <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>180</v>
-      </c>
-      <c r="J98" s="10" t="s">
-        <v>220</v>
+        <v>311</v>
+      </c>
+      <c r="J98" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>178</v>
+      </c>
       <c r="D99" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F99" s="2" t="s">
-        <v>339</v>
+      <c r="F99" s="9" t="s">
+        <v>330</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -4303,7 +4391,47 @@
         <v>180</v>
       </c>
       <c r="J99" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D100" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100" t="s">
+        <v>180</v>
+      </c>
+      <c r="J100" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D101" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101" t="s">
+        <v>180</v>
+      </c>
+      <c r="J101" s="10" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3PAR hosts analysis added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -12,14 +12,14 @@
     <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$109</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="398">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -711,9 +711,6 @@
     <t>Датчики</t>
   </si>
   <si>
-    <t>DATA ANALYSIS 8. FABRIC STATISTICS</t>
-  </si>
-  <si>
     <t>Показания датчиков коммутаторов</t>
   </si>
   <si>
@@ -744,9 +741,6 @@
     <t>sfp_write</t>
   </si>
   <si>
-    <t>DATA ANALYSIS 7. SENSOR READINGS</t>
-  </si>
-  <si>
     <t>IBS</t>
   </si>
   <si>
@@ -954,9 +948,6 @@
     <t>raslog_counter</t>
   </si>
   <si>
-    <t>DATA ANALYSIS 9. RASLOG</t>
-  </si>
-  <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\OTPBank\SAN Assessment DEC2020</t>
   </si>
   <si>
@@ -1032,12 +1023,6 @@
     <t>Fabric-Device Management Interface (FDMI) information</t>
   </si>
   <si>
-    <t>Local NS information</t>
-  </si>
-  <si>
-    <t>Cached NS information</t>
-  </si>
-  <si>
     <t>SAN Implementation. Checking</t>
   </si>
   <si>
@@ -1147,6 +1132,87 @@
   </si>
   <si>
     <t xml:space="preserve">3PAR system information </t>
+  </si>
+  <si>
+    <t>nsh-spb</t>
+  </si>
+  <si>
+    <t>SAN checking</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\NCH-SPB\SAN Assessment\MAR21</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\ZSD\MAR21\ZES_supportsave</t>
+  </si>
+  <si>
+    <t>alias_wwnp</t>
+  </si>
+  <si>
+    <t>апмама</t>
+  </si>
+  <si>
+    <t>Sensors collection</t>
+  </si>
+  <si>
+    <t>Zoning configuration. Configurations collection</t>
+  </si>
+  <si>
+    <t>Zoning configuration. Zones collection</t>
+  </si>
+  <si>
+    <t>Zoning configuration. Aliases collection</t>
+  </si>
+  <si>
+    <t>Zoning configuration. Effective configuration collection</t>
+  </si>
+  <si>
+    <t>Zoning configuration. Effective zones collection</t>
+  </si>
+  <si>
+    <t>Zoning configuration. Peerzones collection</t>
+  </si>
+  <si>
+    <t>Zoning configuration. Peerzones effective collection</t>
+  </si>
+  <si>
+    <t>Local Name Server collection</t>
+  </si>
+  <si>
+    <t>Cached Name Server collection</t>
+  </si>
+  <si>
+    <t>Alias Wwnn</t>
+  </si>
+  <si>
+    <t>Презентация</t>
+  </si>
+  <si>
+    <t>Презентация_A&amp;B</t>
+  </si>
+  <si>
+    <t>storage_host_aggregated</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 7. STORAGE HOST PRESENTATION</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 8. SENSOR READINGS</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 9. FABRIC STATISTICS</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 10. RASLOG</t>
+  </si>
+  <si>
+    <t>Storage Host presentation</t>
+  </si>
+  <si>
+    <t>Презентация массивов</t>
+  </si>
+  <si>
+    <t>Сравнение презентаций массивов</t>
   </si>
 </sst>
 </file>
@@ -1559,41 +1625,41 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AD10"/>
+  <dimension ref="A1:AE10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="80.140625" customWidth="1"/>
-    <col min="4" max="4" width="68.5703125" customWidth="1"/>
-    <col min="5" max="5" width="48.7109375" customWidth="1"/>
-    <col min="6" max="6" width="62" customWidth="1"/>
-    <col min="7" max="9" width="89.5703125" customWidth="1"/>
-    <col min="10" max="10" width="69.85546875" customWidth="1"/>
-    <col min="11" max="11" width="52.140625" customWidth="1"/>
-    <col min="12" max="12" width="73.140625" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" customWidth="1"/>
-    <col min="14" max="15" width="76" customWidth="1"/>
-    <col min="16" max="16" width="72.28515625" customWidth="1"/>
-    <col min="17" max="17" width="61.7109375" customWidth="1"/>
-    <col min="18" max="18" width="60" customWidth="1"/>
-    <col min="19" max="19" width="38.140625" customWidth="1"/>
-    <col min="20" max="20" width="69" customWidth="1"/>
-    <col min="21" max="21" width="72.42578125" customWidth="1"/>
-    <col min="22" max="22" width="111.5703125" customWidth="1"/>
-    <col min="23" max="23" width="72.5703125" customWidth="1"/>
-    <col min="24" max="24" width="86.85546875" customWidth="1"/>
-    <col min="25" max="26" width="64.7109375" customWidth="1"/>
-    <col min="27" max="27" width="54.5703125" customWidth="1"/>
-    <col min="28" max="28" width="75.42578125" customWidth="1"/>
-    <col min="29" max="29" width="58.140625" customWidth="1"/>
+    <col min="1" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="80.140625" customWidth="1"/>
+    <col min="5" max="5" width="68.5703125" customWidth="1"/>
+    <col min="6" max="6" width="48.7109375" customWidth="1"/>
+    <col min="7" max="7" width="62" customWidth="1"/>
+    <col min="8" max="10" width="89.5703125" customWidth="1"/>
+    <col min="11" max="11" width="69.85546875" customWidth="1"/>
+    <col min="12" max="12" width="52.140625" customWidth="1"/>
+    <col min="13" max="13" width="73.140625" customWidth="1"/>
+    <col min="14" max="14" width="29.7109375" customWidth="1"/>
+    <col min="15" max="16" width="76" customWidth="1"/>
+    <col min="17" max="17" width="72.28515625" customWidth="1"/>
+    <col min="18" max="18" width="61.7109375" customWidth="1"/>
+    <col min="19" max="19" width="60" customWidth="1"/>
+    <col min="20" max="20" width="38.140625" customWidth="1"/>
+    <col min="21" max="21" width="69" customWidth="1"/>
+    <col min="22" max="22" width="72.42578125" customWidth="1"/>
+    <col min="23" max="23" width="111.5703125" customWidth="1"/>
+    <col min="24" max="24" width="72.5703125" customWidth="1"/>
+    <col min="25" max="25" width="86.85546875" customWidth="1"/>
+    <col min="26" max="27" width="64.7109375" customWidth="1"/>
+    <col min="28" max="28" width="54.5703125" customWidth="1"/>
+    <col min="29" max="29" width="75.42578125" customWidth="1"/>
+    <col min="30" max="30" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
@@ -1601,402 +1667,417 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>342</v>
+        <v>371</v>
       </c>
       <c r="D2" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="E2" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="F2" t="s">
         <v>317</v>
       </c>
       <c r="G2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="H2" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="I2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="J2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="K2" t="s">
-        <v>282</v>
+        <v>318</v>
       </c>
       <c r="L2" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="M2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="N2" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="O2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="P2" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="Q2" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="R2" t="s">
+        <v>234</v>
+      </c>
+      <c r="S2" t="s">
         <v>189</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>188</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>155</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>111</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>97</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>83</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C3" s="12">
+        <v>44286</v>
+      </c>
+      <c r="D3" s="12">
         <v>44260</v>
       </c>
-      <c r="D3" s="12">
+      <c r="E3" s="12">
         <v>44244</v>
       </c>
-      <c r="E3" s="12">
+      <c r="F3" s="12">
         <v>44245</v>
       </c>
-      <c r="F3" s="12">
+      <c r="G3" s="12">
         <v>44223</v>
       </c>
-      <c r="G3" s="12">
+      <c r="H3" s="12">
         <v>44209</v>
       </c>
-      <c r="H3" s="12">
+      <c r="I3" s="12">
         <v>44253</v>
       </c>
-      <c r="I3" s="12">
+      <c r="J3" s="12">
         <v>44237</v>
       </c>
-      <c r="L3" s="12">
+      <c r="M3" s="12">
         <v>44181</v>
       </c>
-      <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE3" s="1"/>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C4" t="s">
-        <v>331</v>
+        <v>372</v>
       </c>
       <c r="D4" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="E4" t="s">
-        <v>331</v>
-      </c>
-      <c r="G4" t="s">
-        <v>331</v>
+        <v>323</v>
+      </c>
+      <c r="F4" t="s">
+        <v>328</v>
       </c>
       <c r="H4" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="I4" t="s">
-        <v>326</v>
-      </c>
-      <c r="L4" t="s">
-        <v>285</v>
+        <v>334</v>
+      </c>
+      <c r="J4" t="s">
+        <v>323</v>
       </c>
       <c r="M4" t="s">
-        <v>284</v>
-      </c>
-      <c r="X4" s="1"/>
+        <v>283</v>
+      </c>
+      <c r="N4" t="s">
+        <v>282</v>
+      </c>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AE4" s="1"/>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>343</v>
+        <v>373</v>
       </c>
       <c r="D5" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="E5" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="F5" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="G5" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="H5" t="s">
-        <v>340</v>
+        <v>309</v>
       </c>
       <c r="I5" t="s">
-        <v>324</v>
+        <v>335</v>
       </c>
       <c r="J5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K5" t="s">
-        <v>283</v>
+        <v>319</v>
       </c>
       <c r="L5" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="M5" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="N5" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="O5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="P5" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="Q5" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="R5" t="s">
+        <v>233</v>
+      </c>
+      <c r="S5" t="s">
         <v>223</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>187</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>157</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>113</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>98</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>85</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>1</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>74</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>72</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>4</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>25</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>60</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="D6" t="s">
+        <v>359</v>
+      </c>
+      <c r="E6" t="s">
+        <v>326</v>
+      </c>
+      <c r="F6" t="s">
         <v>329</v>
       </c>
-      <c r="E6" t="s">
-        <v>332</v>
-      </c>
-      <c r="F6" t="s">
-        <v>319</v>
-      </c>
       <c r="G6" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="H6" t="s">
-        <v>341</v>
+        <v>311</v>
       </c>
       <c r="I6" t="s">
-        <v>325</v>
+        <v>336</v>
       </c>
       <c r="J6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K6" t="s">
-        <v>281</v>
+        <v>320</v>
       </c>
       <c r="L6" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="M6" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="N6" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="O6" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
       <c r="P6" t="s">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="Q6" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="R6" t="s">
+        <v>231</v>
+      </c>
+      <c r="S6" t="s">
         <v>222</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>186</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>156</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>112</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>108</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>84</v>
       </c>
-      <c r="X6" t="s">
-        <v>0</v>
-      </c>
       <c r="Y6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="s">
         <v>73</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>71</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>3</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>24</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>59</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C7" t="s">
-        <v>344</v>
-      </c>
-      <c r="G7" t="s">
-        <v>315</v>
-      </c>
-      <c r="N7" t="s">
+      <c r="D7" t="s">
+        <v>339</v>
+      </c>
+      <c r="H7" t="s">
+        <v>312</v>
+      </c>
+      <c r="O7" t="s">
+        <v>261</v>
+      </c>
+      <c r="P7" t="s">
+        <v>261</v>
+      </c>
+      <c r="R7" t="s">
+        <v>232</v>
+      </c>
+      <c r="U7" t="s">
+        <v>158</v>
+      </c>
+      <c r="W7" t="s">
+        <v>109</v>
+      </c>
+      <c r="X7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="D8" t="s">
+        <v>340</v>
+      </c>
+      <c r="O8" t="s">
         <v>263</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P8" t="s">
         <v>263</v>
       </c>
-      <c r="Q7" t="s">
-        <v>233</v>
-      </c>
-      <c r="T7" t="s">
-        <v>158</v>
-      </c>
-      <c r="V7" t="s">
-        <v>109</v>
-      </c>
-      <c r="W7" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>99</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="C8" t="s">
-        <v>345</v>
-      </c>
-      <c r="N8" t="s">
-        <v>265</v>
-      </c>
-      <c r="O8" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2008,11 +2089,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J104"/>
+  <dimension ref="A1:J109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2146,7 +2227,7 @@
         <v>142</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2178,7 +2259,7 @@
         <v>151</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2210,7 +2291,7 @@
         <v>151</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2242,7 +2323,7 @@
         <v>152</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2274,7 +2355,7 @@
         <v>148</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2306,7 +2387,7 @@
         <v>148</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2434,7 +2515,7 @@
         <v>144</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2466,7 +2547,7 @@
         <v>144</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>337</v>
+        <v>385</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2498,7 +2579,7 @@
         <v>144</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>338</v>
+        <v>386</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2794,7 +2875,7 @@
         <v>149</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>218</v>
+        <v>378</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -2820,7 +2901,7 @@
         <v>149</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>218</v>
+        <v>379</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -2846,7 +2927,7 @@
         <v>149</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>218</v>
+        <v>380</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -2872,7 +2953,7 @@
         <v>149</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>218</v>
+        <v>381</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2898,7 +2979,7 @@
         <v>149</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>218</v>
+        <v>382</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2912,7 +2993,7 @@
         <v>94</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -2924,7 +3005,7 @@
         <v>149</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>218</v>
+        <v>383</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -2938,7 +3019,7 @@
         <v>94</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -2950,7 +3031,7 @@
         <v>149</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>218</v>
+        <v>384</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2976,33 +3057,33 @@
         <v>226</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>218</v>
+        <v>377</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F33" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>295</v>
+      </c>
+      <c r="J33" s="10" t="s">
         <v>296</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33" t="s">
-        <v>297</v>
-      </c>
-      <c r="J33" s="10" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3088,122 +3169,122 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F37" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37" t="s">
+        <v>269</v>
+      </c>
+      <c r="J37" s="10" t="s">
         <v>267</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37" t="s">
-        <v>271</v>
-      </c>
-      <c r="J37" s="10" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F38" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
+        <v>269</v>
+      </c>
+      <c r="J38" s="10" t="s">
         <v>268</v>
-      </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38" t="s">
-        <v>271</v>
-      </c>
-      <c r="J38" s="10" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" t="s">
+        <v>365</v>
+      </c>
+      <c r="J39" s="10" t="s">
         <v>370</v>
-      </c>
-      <c r="J39" s="10" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="G40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40">
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41">
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -3249,7 +3330,7 @@
         <v>159</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>218</v>
+        <v>307</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -3338,7 +3419,7 @@
         <v>171</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -3369,7 +3450,7 @@
         <v>61</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -3389,7 +3470,7 @@
         <v>62</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -3409,7 +3490,7 @@
         <v>63</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -3429,7 +3510,7 @@
         <v>65</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -3449,7 +3530,7 @@
         <v>64</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -3484,7 +3565,7 @@
         <v>172</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -3492,7 +3573,7 @@
         <v>95</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -3504,7 +3585,7 @@
         <v>172</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -3515,7 +3596,7 @@
         <v>67</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -3535,7 +3616,7 @@
         <v>68</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -3552,19 +3633,19 @@
         <v>96</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58" t="s">
         <v>172</v>
       </c>
       <c r="J58" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -3584,13 +3665,13 @@
         <v>0</v>
       </c>
       <c r="H59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59" t="s">
         <v>173</v>
       </c>
       <c r="J59" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -3598,7 +3679,7 @@
         <v>95</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -3610,7 +3691,7 @@
         <v>173</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -3618,7 +3699,7 @@
         <v>95</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -3630,7 +3711,7 @@
         <v>173</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -3638,7 +3719,7 @@
         <v>95</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -3650,15 +3731,15 @@
         <v>173</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D63" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -3670,7 +3751,7 @@
         <v>173</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -3693,7 +3774,7 @@
         <v>173</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>218</v>
+        <v>387</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
@@ -3719,7 +3800,7 @@
         <v>173</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
@@ -3727,7 +3808,7 @@
         <v>95</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -3739,7 +3820,7 @@
         <v>173</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
@@ -3753,7 +3834,7 @@
         <v>100</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -3776,7 +3857,7 @@
         <v>102</v>
       </c>
       <c r="G68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -3796,7 +3877,7 @@
         <v>103</v>
       </c>
       <c r="G69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -3836,7 +3917,7 @@
         <v>105</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -3856,7 +3937,7 @@
         <v>106</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -3876,7 +3957,7 @@
         <v>107</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -3893,19 +3974,19 @@
         <v>96</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I74" t="s">
         <v>173</v>
       </c>
       <c r="J74" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
@@ -3916,7 +3997,7 @@
         <v>165</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -3948,7 +4029,7 @@
         <v>174</v>
       </c>
       <c r="J76" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
@@ -3959,7 +4040,7 @@
         <v>168</v>
       </c>
       <c r="G77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -3979,7 +4060,7 @@
         <v>169</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -3999,7 +4080,7 @@
         <v>170</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -4008,7 +4089,7 @@
         <v>167</v>
       </c>
       <c r="J79" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.25">
@@ -4031,12 +4112,12 @@
         <v>180</v>
       </c>
       <c r="J80" s="10" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>95</v>
@@ -4054,12 +4135,12 @@
         <v>180</v>
       </c>
       <c r="J81" s="10" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>95</v>
@@ -4077,12 +4158,12 @@
         <v>180</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>95</v>
@@ -4100,7 +4181,7 @@
         <v>180</v>
       </c>
       <c r="J83" s="10" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.25">
@@ -4108,7 +4189,7 @@
         <v>95</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -4120,18 +4201,18 @@
         <v>180</v>
       </c>
       <c r="J84" s="10" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -4143,7 +4224,7 @@
         <v>180</v>
       </c>
       <c r="J85" s="10" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.25">
@@ -4231,7 +4312,7 @@
         <v>96</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -4243,7 +4324,7 @@
         <v>180</v>
       </c>
       <c r="J90" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.25">
@@ -4251,7 +4332,7 @@
         <v>96</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -4263,7 +4344,7 @@
         <v>180</v>
       </c>
       <c r="J91" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
@@ -4274,16 +4355,16 @@
         <v>195</v>
       </c>
       <c r="G92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I92" t="s">
         <v>180</v>
       </c>
       <c r="J92" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.25">
@@ -4291,19 +4372,19 @@
         <v>96</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I93" t="s">
         <v>180</v>
       </c>
       <c r="J93" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.25">
@@ -4311,19 +4392,19 @@
         <v>96</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I94" t="s">
         <v>180</v>
       </c>
       <c r="J94" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.25">
@@ -4331,7 +4412,7 @@
         <v>95</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>228</v>
+        <v>390</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -4340,10 +4421,10 @@
         <v>0</v>
       </c>
       <c r="I95" t="s">
-        <v>241</v>
-      </c>
-      <c r="J95" s="10" t="s">
-        <v>308</v>
+        <v>391</v>
+      </c>
+      <c r="J95" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.25">
@@ -4351,96 +4432,93 @@
         <v>96</v>
       </c>
       <c r="F96" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96" t="s">
+        <v>391</v>
+      </c>
+      <c r="J96" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D97" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97" t="s">
+        <v>391</v>
+      </c>
+      <c r="J97" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D98" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98" t="s">
+        <v>392</v>
+      </c>
+      <c r="J98" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D99" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F99" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="G96">
-        <v>0</v>
-      </c>
-      <c r="H96">
-        <v>0</v>
-      </c>
-      <c r="I96" t="s">
-        <v>241</v>
-      </c>
-      <c r="J96" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A97">
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99" t="s">
+        <v>392</v>
+      </c>
+      <c r="J99" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100">
         <v>17</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B100" t="s">
         <v>137</v>
       </c>
-      <c r="D97" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F97" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="G97">
-        <v>0</v>
-      </c>
-      <c r="H97">
-        <v>0</v>
-      </c>
-      <c r="I97" t="s">
-        <v>230</v>
-      </c>
-      <c r="J97" s="10" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D98" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="G98">
-        <v>0</v>
-      </c>
-      <c r="H98">
-        <v>0</v>
-      </c>
-      <c r="I98" t="s">
-        <v>230</v>
-      </c>
-      <c r="J98" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>301</v>
-      </c>
-      <c r="D99" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F99" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="G99">
-        <v>0</v>
-      </c>
-      <c r="H99">
-        <v>0</v>
-      </c>
-      <c r="I99" t="s">
-        <v>311</v>
-      </c>
-      <c r="J99" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D100" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F100" s="2" t="s">
-        <v>310</v>
+      <c r="F100" s="9" t="s">
+        <v>193</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -4449,10 +4527,10 @@
         <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>311</v>
-      </c>
-      <c r="J100" t="s">
-        <v>306</v>
+        <v>393</v>
+      </c>
+      <c r="J100" s="10" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
@@ -4460,30 +4538,30 @@
         <v>96</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>303</v>
+        <v>194</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I101" t="s">
-        <v>311</v>
+        <v>393</v>
       </c>
       <c r="J101" t="s">
-        <v>304</v>
+        <v>361</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>178</v>
+        <v>299</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F102" s="9" t="s">
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -4492,10 +4570,10 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>180</v>
-      </c>
-      <c r="J102" s="10" t="s">
-        <v>218</v>
+        <v>394</v>
+      </c>
+      <c r="J102" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
@@ -4503,7 +4581,7 @@
         <v>95</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>334</v>
+        <v>308</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -4512,30 +4590,133 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
+        <v>394</v>
+      </c>
+      <c r="J103" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D104" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="G104">
+        <v>1</v>
+      </c>
+      <c r="H104">
+        <v>1</v>
+      </c>
+      <c r="I104" t="s">
+        <v>394</v>
+      </c>
+      <c r="J104" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>178</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="I105" t="s">
         <v>180</v>
       </c>
-      <c r="J103" s="10" t="s">
+      <c r="J105" s="10" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D104" s="6" t="s">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D106" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F104" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="G104">
-        <v>0</v>
-      </c>
-      <c r="H104">
-        <v>0</v>
-      </c>
-      <c r="I104" t="s">
+      <c r="F106" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+      <c r="H106">
+        <v>0</v>
+      </c>
+      <c r="I106" t="s">
         <v>180</v>
       </c>
-      <c r="J104" s="10" t="s">
+      <c r="J106" s="10" t="s">
         <v>218</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D107" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+      <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="I107" t="s">
+        <v>180</v>
+      </c>
+      <c r="J107" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D108" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+      <c r="H108">
+        <v>0</v>
+      </c>
+      <c r="I108" t="s">
+        <v>180</v>
+      </c>
+      <c r="J108" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D109" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
+      <c r="I109" t="s">
+        <v>376</v>
+      </c>
+      <c r="J109" s="2" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3par downlaod summary added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$109</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$J$110</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="411">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1213,6 +1213,45 @@
   </si>
   <si>
     <t>Сравнение презентаций массивов</t>
+  </si>
+  <si>
+    <t>TransneftUral</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Transneft - Ural\SAN Assessment\APR21</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\TansneftUral\APR21\sshow</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\TansneftUral\APR21\blade</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\TansneftUral\APR21\3par</t>
+  </si>
+  <si>
+    <t>Blade Virtual connect collection</t>
+  </si>
+  <si>
+    <t>Blade servers collection</t>
+  </si>
+  <si>
+    <t>Blade Interconnect modules collection</t>
+  </si>
+  <si>
+    <t>MegafonMSK</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\MegafonMSK\APR21\ssave</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\MegafonMSK\SAN Assessment\APR21</t>
+  </si>
+  <si>
+    <t>ns_3par</t>
+  </si>
+  <si>
+    <t>3PAR configs download status</t>
   </si>
 </sst>
 </file>
@@ -1304,7 +1343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1320,6 +1359,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1625,41 +1665,44 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AE10"/>
+  <dimension ref="A1:AG10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="80.140625" customWidth="1"/>
-    <col min="5" max="5" width="68.5703125" customWidth="1"/>
-    <col min="6" max="6" width="48.7109375" customWidth="1"/>
-    <col min="7" max="7" width="62" customWidth="1"/>
-    <col min="8" max="10" width="89.5703125" customWidth="1"/>
-    <col min="11" max="11" width="69.85546875" customWidth="1"/>
-    <col min="12" max="12" width="52.140625" customWidth="1"/>
-    <col min="13" max="13" width="73.140625" customWidth="1"/>
-    <col min="14" max="14" width="29.7109375" customWidth="1"/>
-    <col min="15" max="16" width="76" customWidth="1"/>
-    <col min="17" max="17" width="72.28515625" customWidth="1"/>
-    <col min="18" max="18" width="61.7109375" customWidth="1"/>
-    <col min="19" max="19" width="60" customWidth="1"/>
-    <col min="20" max="20" width="38.140625" customWidth="1"/>
-    <col min="21" max="21" width="69" customWidth="1"/>
-    <col min="22" max="22" width="72.42578125" customWidth="1"/>
-    <col min="23" max="23" width="111.5703125" customWidth="1"/>
-    <col min="24" max="24" width="72.5703125" customWidth="1"/>
-    <col min="25" max="25" width="86.85546875" customWidth="1"/>
-    <col min="26" max="27" width="64.7109375" customWidth="1"/>
-    <col min="28" max="28" width="54.5703125" customWidth="1"/>
-    <col min="29" max="29" width="75.42578125" customWidth="1"/>
-    <col min="30" max="30" width="58.140625" customWidth="1"/>
+    <col min="1" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="122.7109375" customWidth="1"/>
+    <col min="4" max="4" width="48.42578125" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="80.140625" customWidth="1"/>
+    <col min="7" max="7" width="68.5703125" customWidth="1"/>
+    <col min="8" max="8" width="48.7109375" customWidth="1"/>
+    <col min="9" max="9" width="62" customWidth="1"/>
+    <col min="10" max="12" width="89.5703125" customWidth="1"/>
+    <col min="13" max="13" width="69.85546875" customWidth="1"/>
+    <col min="14" max="14" width="52.140625" customWidth="1"/>
+    <col min="15" max="15" width="73.140625" customWidth="1"/>
+    <col min="16" max="16" width="29.7109375" customWidth="1"/>
+    <col min="17" max="18" width="76" customWidth="1"/>
+    <col min="19" max="19" width="72.28515625" customWidth="1"/>
+    <col min="20" max="20" width="61.7109375" customWidth="1"/>
+    <col min="21" max="21" width="60" customWidth="1"/>
+    <col min="22" max="22" width="38.140625" customWidth="1"/>
+    <col min="23" max="23" width="69" customWidth="1"/>
+    <col min="24" max="24" width="72.42578125" customWidth="1"/>
+    <col min="25" max="25" width="111.5703125" customWidth="1"/>
+    <col min="26" max="26" width="72.5703125" customWidth="1"/>
+    <col min="27" max="27" width="86.85546875" customWidth="1"/>
+    <col min="28" max="29" width="64.7109375" customWidth="1"/>
+    <col min="30" max="30" width="54.5703125" customWidth="1"/>
+    <col min="31" max="31" width="75.42578125" customWidth="1"/>
+    <col min="32" max="32" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
@@ -1667,416 +1710,452 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
+        <v>406</v>
+      </c>
+      <c r="D2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E2" t="s">
         <v>371</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>337</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>324</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>317</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>314</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>310</v>
-      </c>
-      <c r="I2" t="s">
-        <v>318</v>
-      </c>
-      <c r="J2" t="s">
-        <v>318</v>
       </c>
       <c r="K2" t="s">
         <v>318</v>
       </c>
       <c r="L2" t="s">
+        <v>318</v>
+      </c>
+      <c r="M2" t="s">
+        <v>318</v>
+      </c>
+      <c r="N2" t="s">
         <v>280</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>276</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>276</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>258</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>258</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>240</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>234</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>189</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>188</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>155</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>111</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Y2" t="s">
         <v>97</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>83</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>284</v>
       </c>
       <c r="C3" s="12">
+        <v>44292</v>
+      </c>
+      <c r="D3" s="12">
+        <v>29681</v>
+      </c>
+      <c r="E3" s="12">
         <v>44286</v>
       </c>
-      <c r="D3" s="12">
+      <c r="F3" s="12">
         <v>44260</v>
       </c>
-      <c r="E3" s="12">
+      <c r="G3" s="12">
         <v>44244</v>
       </c>
-      <c r="F3" s="12">
+      <c r="H3" s="12">
         <v>44245</v>
       </c>
-      <c r="G3" s="12">
+      <c r="I3" s="12">
         <v>44223</v>
       </c>
-      <c r="H3" s="12">
+      <c r="J3" s="12">
         <v>44209</v>
       </c>
-      <c r="I3" s="12">
+      <c r="K3" s="12">
         <v>44253</v>
       </c>
-      <c r="J3" s="12">
+      <c r="L3" s="12">
         <v>44237</v>
       </c>
-      <c r="M3" s="12">
+      <c r="O3" s="12">
         <v>44181</v>
       </c>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>285</v>
       </c>
       <c r="C4" t="s">
-        <v>372</v>
+        <v>328</v>
       </c>
       <c r="D4" t="s">
         <v>328</v>
       </c>
       <c r="E4" t="s">
-        <v>323</v>
+        <v>372</v>
       </c>
       <c r="F4" t="s">
         <v>328</v>
       </c>
+      <c r="G4" t="s">
+        <v>323</v>
+      </c>
       <c r="H4" t="s">
         <v>328</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
+        <v>328</v>
+      </c>
+      <c r="K4" t="s">
         <v>334</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>323</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>283</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>282</v>
       </c>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
+        <v>408</v>
+      </c>
+      <c r="D5" t="s">
+        <v>399</v>
+      </c>
+      <c r="E5" t="s">
         <v>373</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>338</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>325</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>330</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>315</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>309</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>335</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>321</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>319</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>281</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>286</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
         <v>278</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
         <v>259</v>
       </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
         <v>259</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>242</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
         <v>233</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
         <v>223</v>
       </c>
-      <c r="T5" t="s">
+      <c r="V5" t="s">
         <v>187</v>
       </c>
-      <c r="U5" t="s">
+      <c r="W5" t="s">
         <v>157</v>
       </c>
-      <c r="V5" t="s">
+      <c r="X5" t="s">
         <v>113</v>
       </c>
-      <c r="W5" t="s">
+      <c r="Y5" t="s">
         <v>98</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Z5" t="s">
         <v>85</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="AA5" t="s">
         <v>1</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AB5" t="s">
         <v>74</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AC5" t="s">
         <v>72</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AD5" t="s">
         <v>4</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AE5" t="s">
         <v>25</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AF5" t="s">
         <v>60</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AG5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C6" t="s">
+        <v>407</v>
+      </c>
+      <c r="D6" t="s">
+        <v>400</v>
+      </c>
+      <c r="E6" t="s">
         <v>374</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>359</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>326</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>329</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>316</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>311</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>336</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>322</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>320</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>279</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>287</v>
       </c>
-      <c r="N6" t="s">
+      <c r="P6" t="s">
         <v>277</v>
       </c>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
         <v>272</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>260</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="S6" t="s">
         <v>241</v>
       </c>
-      <c r="R6" t="s">
+      <c r="T6" t="s">
         <v>231</v>
       </c>
-      <c r="S6" t="s">
+      <c r="U6" t="s">
         <v>222</v>
       </c>
-      <c r="T6" t="s">
+      <c r="V6" t="s">
         <v>186</v>
       </c>
-      <c r="U6" t="s">
+      <c r="W6" t="s">
         <v>156</v>
       </c>
-      <c r="V6" t="s">
+      <c r="X6" t="s">
         <v>112</v>
       </c>
-      <c r="W6" t="s">
+      <c r="Y6" t="s">
         <v>108</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Z6" t="s">
         <v>84</v>
       </c>
-      <c r="Y6" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB6" t="s">
         <v>73</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AC6" t="s">
         <v>71</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AD6" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AE6" t="s">
         <v>24</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AF6" t="s">
         <v>59</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AG6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
       <c r="D7" t="s">
+        <v>401</v>
+      </c>
+      <c r="F7" t="s">
         <v>339</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>312</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
         <v>261</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R7" t="s">
         <v>261</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>232</v>
       </c>
-      <c r="U7" t="s">
+      <c r="W7" t="s">
         <v>158</v>
       </c>
-      <c r="W7" t="s">
+      <c r="Y7" t="s">
         <v>109</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Z7" t="s">
         <v>87</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AC7" t="s">
         <v>99</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AF7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>340</v>
       </c>
-      <c r="O8" t="s">
+      <c r="Q8" t="s">
         <v>263</v>
       </c>
-      <c r="P8" t="s">
+      <c r="R8" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="D9" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>239</v>
       </c>
     </row>
@@ -2089,11 +2168,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:J109"/>
+  <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G98" sqref="G98"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3112,7 +3191,7 @@
         <v>227</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>218</v>
+        <v>405</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3138,7 +3217,7 @@
         <v>227</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>218</v>
+        <v>404</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -3164,7 +3243,7 @@
         <v>227</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>218</v>
+        <v>403</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -3230,7 +3309,7 @@
         <v>0</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" t="s">
         <v>365</v>
@@ -3288,37 +3367,41 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="B42" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42" t="s">
+        <v>365</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>15</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>138</v>
       </c>
-      <c r="D42" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42" t="s">
-        <v>159</v>
-      </c>
-      <c r="J42" s="10" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D43" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F43" s="8" t="s">
-        <v>56</v>
+      <c r="F43" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -3330,7 +3413,7 @@
         <v>159</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>307</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -3338,7 +3421,7 @@
         <v>95</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -3350,18 +3433,15 @@
         <v>159</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>218</v>
+        <v>307</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>162</v>
-      </c>
       <c r="D45" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F45" s="9" t="s">
-        <v>160</v>
+      <c r="F45" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -3370,18 +3450,21 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="J45" s="10" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D46" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>161</v>
+      <c r="B46" t="s">
+        <v>162</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>160</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -3392,42 +3475,42 @@
       <c r="I46" t="s">
         <v>163</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J46" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D47" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47" t="s">
+        <v>163</v>
+      </c>
+      <c r="J47" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>16</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>140</v>
       </c>
-      <c r="D47" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-      <c r="I47" t="s">
-        <v>171</v>
-      </c>
-      <c r="J47" s="10" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D48" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>164</v>
+      <c r="F48" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -3439,15 +3522,15 @@
         <v>171</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>218</v>
+        <v>291</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D49" s="5" t="s">
-        <v>96</v>
+      <c r="D49" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>61</v>
+        <v>164</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -3458,8 +3541,8 @@
       <c r="I49" t="s">
         <v>171</v>
       </c>
-      <c r="J49" t="s">
-        <v>197</v>
+      <c r="J49" s="10" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -3467,7 +3550,7 @@
         <v>96</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -3479,7 +3562,7 @@
         <v>171</v>
       </c>
       <c r="J50" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -3487,7 +3570,7 @@
         <v>96</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -3499,7 +3582,7 @@
         <v>171</v>
       </c>
       <c r="J51" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -3507,7 +3590,7 @@
         <v>96</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -3519,7 +3602,7 @@
         <v>171</v>
       </c>
       <c r="J52" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -3527,7 +3610,7 @@
         <v>96</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -3539,41 +3622,41 @@
         <v>171</v>
       </c>
       <c r="J53" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D54" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54" t="s">
+        <v>171</v>
+      </c>
+      <c r="J54" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55">
         <v>18</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>139</v>
       </c>
-      <c r="D54" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-      <c r="H54">
-        <v>0</v>
-      </c>
-      <c r="I54" t="s">
-        <v>172</v>
-      </c>
-      <c r="J54" s="10" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D55" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>288</v>
+        <v>69</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -3585,15 +3668,15 @@
         <v>172</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D56" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>67</v>
+      <c r="D56" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>288</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -3604,8 +3687,8 @@
       <c r="I56" t="s">
         <v>172</v>
       </c>
-      <c r="J56" t="s">
-        <v>208</v>
+      <c r="J56" s="10" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
@@ -3613,7 +3696,7 @@
         <v>96</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -3625,7 +3708,7 @@
         <v>172</v>
       </c>
       <c r="J57" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -3633,7 +3716,7 @@
         <v>96</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>292</v>
+        <v>68</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -3645,41 +3728,41 @@
         <v>172</v>
       </c>
       <c r="J58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D59" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59" t="s">
+        <v>172</v>
+      </c>
+      <c r="J59" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>20</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>132</v>
       </c>
-      <c r="D59" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59" t="s">
-        <v>173</v>
-      </c>
-      <c r="J59" s="10" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D60" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>273</v>
+        <v>90</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -3691,15 +3774,15 @@
         <v>173</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D61" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F61" s="2" t="s">
-        <v>245</v>
+      <c r="F61" s="9" t="s">
+        <v>273</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -3711,7 +3794,7 @@
         <v>173</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>342</v>
+        <v>274</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -3719,7 +3802,7 @@
         <v>95</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -3731,15 +3814,15 @@
         <v>173</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>247</v>
+        <v>342</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D63" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="F63" s="11" t="s">
-        <v>249</v>
+      <c r="D63" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -3755,14 +3838,11 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>134</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F64" s="8" t="s">
-        <v>110</v>
+      <c r="D64" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>249</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -3774,21 +3854,18 @@
         <v>173</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>387</v>
+        <v>247</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>120</v>
-      </c>
-      <c r="C65" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F65" s="7" t="s">
-        <v>93</v>
+      <c r="F65" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -3800,15 +3877,21 @@
         <v>173</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>341</v>
+        <v>387</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>120</v>
+      </c>
+      <c r="C66" t="s">
+        <v>133</v>
+      </c>
       <c r="D66" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>313</v>
+        <v>93</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -3820,18 +3903,15 @@
         <v>173</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>135</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>100</v>
+      <c r="D67" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>313</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -3842,19 +3922,19 @@
       <c r="I67" t="s">
         <v>173</v>
       </c>
-      <c r="J67" t="s">
-        <v>200</v>
+      <c r="J67" s="10" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -3866,15 +3946,18 @@
         <v>173</v>
       </c>
       <c r="J68" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>136</v>
+      </c>
       <c r="D69" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -3886,7 +3969,7 @@
         <v>173</v>
       </c>
       <c r="J69" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
@@ -3894,7 +3977,7 @@
         <v>96</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -3906,7 +3989,7 @@
         <v>173</v>
       </c>
       <c r="J70" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
@@ -3914,7 +3997,7 @@
         <v>96</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -3926,7 +4009,7 @@
         <v>173</v>
       </c>
       <c r="J71" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
@@ -3934,7 +4017,7 @@
         <v>96</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -3946,7 +4029,7 @@
         <v>173</v>
       </c>
       <c r="J72" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
@@ -3954,7 +4037,7 @@
         <v>96</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -3966,7 +4049,7 @@
         <v>173</v>
       </c>
       <c r="J73" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
@@ -3974,7 +4057,7 @@
         <v>96</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>275</v>
+        <v>107</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -3986,7 +4069,7 @@
         <v>173</v>
       </c>
       <c r="J74" t="s">
-        <v>360</v>
+        <v>213</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
@@ -3994,7 +4077,7 @@
         <v>96</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>165</v>
+        <v>275</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -4006,38 +4089,38 @@
         <v>173</v>
       </c>
       <c r="J75" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D76" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76" t="s">
+        <v>173</v>
+      </c>
+      <c r="J76" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>166</v>
       </c>
-      <c r="D76" s="6" t="s">
+      <c r="D77" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F76" s="9" t="s">
+      <c r="F77" s="9" t="s">
         <v>220</v>
-      </c>
-      <c r="G76">
-        <v>0</v>
-      </c>
-      <c r="H76">
-        <v>0</v>
-      </c>
-      <c r="I76" t="s">
-        <v>174</v>
-      </c>
-      <c r="J76" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D77" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -4049,7 +4132,7 @@
         <v>174</v>
       </c>
       <c r="J77" t="s">
-        <v>204</v>
+        <v>305</v>
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
@@ -4057,7 +4140,7 @@
         <v>96</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -4066,10 +4149,10 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="J78" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
@@ -4077,7 +4160,7 @@
         <v>96</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -4089,41 +4172,38 @@
         <v>167</v>
       </c>
       <c r="J79" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D80" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80" t="s">
+        <v>167</v>
+      </c>
+      <c r="J80" t="s">
         <v>271</v>
-      </c>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>178</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-      <c r="H80">
-        <v>0</v>
-      </c>
-      <c r="I80" t="s">
-        <v>180</v>
-      </c>
-      <c r="J80" s="10" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>255</v>
+        <v>178</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -4135,18 +4215,18 @@
         <v>180</v>
       </c>
       <c r="J81" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -4158,18 +4238,18 @@
         <v>180</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>219</v>
+        <v>190</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -4181,15 +4261,18 @@
         <v>180</v>
       </c>
       <c r="J83" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>256</v>
+      </c>
       <c r="D84" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>343</v>
+        <v>219</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -4201,18 +4284,15 @@
         <v>180</v>
       </c>
       <c r="J84" s="10" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>254</v>
-      </c>
       <c r="D85" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>250</v>
+        <v>343</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -4224,15 +4304,18 @@
         <v>180</v>
       </c>
       <c r="J85" s="10" t="s">
-        <v>251</v>
+        <v>344</v>
       </c>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D86" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>182</v>
+      <c r="B86" t="s">
+        <v>254</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>250</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -4243,8 +4326,8 @@
       <c r="I86" t="s">
         <v>180</v>
       </c>
-      <c r="J86" t="s">
-        <v>215</v>
+      <c r="J86" s="10" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.25">
@@ -4252,7 +4335,7 @@
         <v>96</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -4264,7 +4347,7 @@
         <v>180</v>
       </c>
       <c r="J87" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.25">
@@ -4272,7 +4355,7 @@
         <v>96</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -4284,7 +4367,7 @@
         <v>180</v>
       </c>
       <c r="J88" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.25">
@@ -4292,7 +4375,7 @@
         <v>96</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -4304,7 +4387,7 @@
         <v>180</v>
       </c>
       <c r="J89" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.25">
@@ -4312,7 +4395,7 @@
         <v>96</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>235</v>
+        <v>192</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -4324,7 +4407,7 @@
         <v>180</v>
       </c>
       <c r="J90" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.25">
@@ -4332,7 +4415,7 @@
         <v>96</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -4344,7 +4427,7 @@
         <v>180</v>
       </c>
       <c r="J91" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
@@ -4352,7 +4435,7 @@
         <v>96</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>195</v>
+        <v>237</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -4364,7 +4447,7 @@
         <v>180</v>
       </c>
       <c r="J92" t="s">
-        <v>350</v>
+        <v>238</v>
       </c>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.25">
@@ -4372,7 +4455,7 @@
         <v>96</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>349</v>
+        <v>195</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -4384,7 +4467,7 @@
         <v>180</v>
       </c>
       <c r="J93" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.25">
@@ -4392,7 +4475,7 @@
         <v>96</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>252</v>
+        <v>349</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -4404,47 +4487,47 @@
         <v>180</v>
       </c>
       <c r="J94" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D95" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95" t="s">
+        <v>180</v>
+      </c>
+      <c r="J95" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="95" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D95" s="6" t="s">
+    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D96" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F95" s="2" t="s">
+      <c r="F96" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="G95">
-        <v>0</v>
-      </c>
-      <c r="H95">
-        <v>0</v>
-      </c>
-      <c r="I95" t="s">
-        <v>391</v>
-      </c>
-      <c r="J95" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="96" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D96" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>388</v>
-      </c>
       <c r="G96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96" t="s">
         <v>391</v>
       </c>
       <c r="J96" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
@@ -4452,7 +4535,7 @@
         <v>96</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -4464,35 +4547,35 @@
         <v>391</v>
       </c>
       <c r="J97" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D98" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+      <c r="I98" t="s">
+        <v>391</v>
+      </c>
+      <c r="J98" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D98" s="6" t="s">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D99" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F98" s="2" t="s">
+      <c r="F99" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="G98">
-        <v>0</v>
-      </c>
-      <c r="H98">
-        <v>0</v>
-      </c>
-      <c r="I98" t="s">
-        <v>392</v>
-      </c>
-      <c r="J98" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D99" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -4504,41 +4587,41 @@
         <v>392</v>
       </c>
       <c r="J99" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D100" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100" t="s">
+        <v>392</v>
+      </c>
+      <c r="J100" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A100">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101">
         <v>17</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
         <v>137</v>
       </c>
-      <c r="D100" s="6" t="s">
+      <c r="D101" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F100" s="9" t="s">
+      <c r="F101" s="9" t="s">
         <v>193</v>
-      </c>
-      <c r="G100">
-        <v>0</v>
-      </c>
-      <c r="H100">
-        <v>0</v>
-      </c>
-      <c r="I100" t="s">
-        <v>393</v>
-      </c>
-      <c r="J100" s="10" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D101" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>194</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -4549,39 +4632,39 @@
       <c r="I101" t="s">
         <v>393</v>
       </c>
-      <c r="J101" t="s">
+      <c r="J101" s="10" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D102" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="I102" t="s">
+        <v>393</v>
+      </c>
+      <c r="J102" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
         <v>299</v>
       </c>
-      <c r="D102" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F102" s="9" t="s">
-        <v>300</v>
-      </c>
-      <c r="G102">
-        <v>0</v>
-      </c>
-      <c r="H102">
-        <v>0</v>
-      </c>
-      <c r="I102" t="s">
-        <v>394</v>
-      </c>
-      <c r="J102" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D103" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F103" s="2" t="s">
-        <v>308</v>
+      <c r="F103" s="9" t="s">
+        <v>300</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -4593,15 +4676,15 @@
         <v>394</v>
       </c>
       <c r="J103" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D104" s="5" t="s">
-        <v>96</v>
+      <c r="D104" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -4613,38 +4696,38 @@
         <v>394</v>
       </c>
       <c r="J104" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D105" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="I105" t="s">
+        <v>394</v>
+      </c>
+      <c r="J105" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
         <v>178</v>
       </c>
-      <c r="D105" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F105" s="9" t="s">
-        <v>327</v>
-      </c>
-      <c r="G105">
-        <v>0</v>
-      </c>
-      <c r="H105">
-        <v>0</v>
-      </c>
-      <c r="I105" t="s">
-        <v>180</v>
-      </c>
-      <c r="J105" s="10" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D106" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F106" s="2" t="s">
-        <v>331</v>
+      <c r="F106" s="9" t="s">
+        <v>327</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -4664,7 +4747,7 @@
         <v>95</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -4704,18 +4787,38 @@
         <v>95</v>
       </c>
       <c r="F109" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
+      <c r="I109" t="s">
+        <v>180</v>
+      </c>
+      <c r="J109" s="10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D110" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F110" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="G109">
-        <v>0</v>
-      </c>
-      <c r="H109">
-        <v>0</v>
-      </c>
-      <c r="I109" t="s">
+      <c r="G110">
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="I110" t="s">
         <v>376</v>
       </c>
-      <c r="J109" s="2" t="s">
+      <c r="J110" s="2" t="s">
         <v>375</v>
       </c>
     </row>

</xml_diff>

<commit_message>
storage host presentation refactoring
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="424">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1267,6 +1267,30 @@
   </si>
   <si>
     <t>C:\Users\vlasenko\Documents\06.CONFIGS\Gazprom\APR21</t>
+  </si>
+  <si>
+    <t>Blade chassis modules</t>
+  </si>
+  <si>
+    <t>Port connected Wwns, frames and errors counters collection</t>
+  </si>
+  <si>
+    <t>SFP collection</t>
+  </si>
+  <si>
+    <t>Portcfg collection</t>
+  </si>
+  <si>
+    <t>ISL collection</t>
+  </si>
+  <si>
+    <t>Trunk collection</t>
+  </si>
+  <si>
+    <t>Porttrunkarea collection</t>
+  </si>
+  <si>
+    <t>fcrfabric collection</t>
   </si>
 </sst>
 </file>
@@ -2205,8 +2229,8 @@
   <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H64" sqref="H64"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2535,7 +2559,7 @@
         <v>146</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>218</v>
+        <v>417</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2567,7 +2591,7 @@
         <v>147</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>218</v>
+        <v>418</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2599,7 +2623,7 @@
         <v>147</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>218</v>
+        <v>419</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2727,7 +2751,7 @@
         <v>145</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>218</v>
+        <v>420</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2759,7 +2783,7 @@
         <v>145</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>218</v>
+        <v>421</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2791,7 +2815,7 @@
         <v>145</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>218</v>
+        <v>422</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2823,7 +2847,7 @@
         <v>143</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>218</v>
+        <v>423</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -3513,7 +3537,7 @@
         <v>163</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>218</v>
+        <v>416</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
storage host presentation final refactoring
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="13935"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -1706,8 +1706,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1746,7 +1746,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>80</v>
       </c>
       <c r="K1" s="3" t="s">
@@ -2228,9 +2228,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F97" sqref="F97:H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3548,10 +3548,10 @@
         <v>161</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47" t="s">
         <v>163</v>
@@ -3614,10 +3614,10 @@
         <v>61</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" t="s">
         <v>171</v>
@@ -3634,10 +3634,10 @@
         <v>62</v>
       </c>
       <c r="G51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" t="s">
         <v>171</v>
@@ -3654,10 +3654,10 @@
         <v>63</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" t="s">
         <v>171</v>
@@ -3674,10 +3674,10 @@
         <v>65</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" t="s">
         <v>171</v>
@@ -3694,10 +3694,10 @@
         <v>64</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" t="s">
         <v>171</v>
@@ -3743,7 +3743,7 @@
         <v>0</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" t="s">
         <v>172</v>
@@ -3763,10 +3763,10 @@
         <v>67</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="s">
         <v>172</v>
@@ -3783,10 +3783,10 @@
         <v>68</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58" t="s">
         <v>172</v>
@@ -3803,10 +3803,10 @@
         <v>292</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59" t="s">
         <v>172</v>
@@ -3835,7 +3835,7 @@
         <v>0</v>
       </c>
       <c r="H60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" t="s">
         <v>173</v>
@@ -3855,7 +3855,7 @@
         <v>0</v>
       </c>
       <c r="H61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" t="s">
         <v>173</v>
@@ -4007,10 +4007,10 @@
         <v>100</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68" t="s">
         <v>173</v>
@@ -4030,10 +4030,10 @@
         <v>102</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69" t="s">
         <v>173</v>
@@ -4050,10 +4050,10 @@
         <v>103</v>
       </c>
       <c r="G70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I70" t="s">
         <v>173</v>
@@ -4070,10 +4070,10 @@
         <v>104</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I71" t="s">
         <v>173</v>
@@ -4090,10 +4090,10 @@
         <v>105</v>
       </c>
       <c r="G72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I72" t="s">
         <v>173</v>
@@ -4110,10 +4110,10 @@
         <v>106</v>
       </c>
       <c r="G73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I73" t="s">
         <v>173</v>
@@ -4130,10 +4130,10 @@
         <v>107</v>
       </c>
       <c r="G74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I74" t="s">
         <v>173</v>
@@ -4150,10 +4150,10 @@
         <v>275</v>
       </c>
       <c r="G75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I75" t="s">
         <v>173</v>
@@ -4173,10 +4173,10 @@
         <v>165</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I76" t="s">
         <v>173</v>
@@ -4216,10 +4216,10 @@
         <v>168</v>
       </c>
       <c r="G78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I78" t="s">
         <v>174</v>
@@ -4236,10 +4236,10 @@
         <v>169</v>
       </c>
       <c r="G79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I79" t="s">
         <v>167</v>
@@ -4256,10 +4256,10 @@
         <v>170</v>
       </c>
       <c r="G80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I80" t="s">
         <v>167</v>
@@ -4328,7 +4328,7 @@
         <v>0</v>
       </c>
       <c r="H83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I83" t="s">
         <v>180</v>
@@ -4354,7 +4354,7 @@
         <v>0</v>
       </c>
       <c r="H84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I84" t="s">
         <v>180</v>
@@ -4377,7 +4377,7 @@
         <v>0</v>
       </c>
       <c r="H85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I85" t="s">
         <v>180</v>
@@ -4403,7 +4403,7 @@
         <v>0</v>
       </c>
       <c r="H86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I86" t="s">
         <v>180</v>
@@ -4423,10 +4423,10 @@
         <v>182</v>
       </c>
       <c r="G87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I87" t="s">
         <v>180</v>
@@ -4443,10 +4443,10 @@
         <v>183</v>
       </c>
       <c r="G88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I88" t="s">
         <v>180</v>
@@ -4463,10 +4463,10 @@
         <v>191</v>
       </c>
       <c r="G89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I89" t="s">
         <v>180</v>
@@ -4483,10 +4483,10 @@
         <v>192</v>
       </c>
       <c r="G90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I90" t="s">
         <v>180</v>
@@ -4503,10 +4503,10 @@
         <v>235</v>
       </c>
       <c r="G91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I91" t="s">
         <v>180</v>
@@ -4523,10 +4523,10 @@
         <v>237</v>
       </c>
       <c r="G92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I92" t="s">
         <v>180</v>
@@ -4546,10 +4546,10 @@
         <v>195</v>
       </c>
       <c r="G93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I93" t="s">
         <v>180</v>
@@ -4569,10 +4569,10 @@
         <v>349</v>
       </c>
       <c r="G94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I94" t="s">
         <v>180</v>
@@ -4592,10 +4592,10 @@
         <v>252</v>
       </c>
       <c r="G95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I95" t="s">
         <v>180</v>
@@ -4695,10 +4695,10 @@
         <v>229</v>
       </c>
       <c r="G100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I100" t="s">
         <v>392</v>
@@ -4724,7 +4724,7 @@
         <v>0</v>
       </c>
       <c r="H101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I101" t="s">
         <v>393</v>
@@ -4744,10 +4744,10 @@
         <v>194</v>
       </c>
       <c r="G102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I102" t="s">
         <v>393</v>
@@ -4793,7 +4793,7 @@
         <v>0</v>
       </c>
       <c r="H104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I104" t="s">
         <v>394</v>
@@ -4813,10 +4813,10 @@
         <v>301</v>
       </c>
       <c r="G105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I105" t="s">
         <v>394</v>

</xml_diff>

<commit_message>
local 3par configs added only if config was not downloaded from stats
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="424">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1101,9 +1101,6 @@
     <t>C:\Users\vlasenko\Documents\06.CONFIGS\UniCredit\MAR 2021\supportsave_20210310</t>
   </si>
   <si>
-    <t>Статистическая информация портов устройств</t>
-  </si>
-  <si>
     <t>Статистическая информация портов коммутаторов</t>
   </si>
   <si>
@@ -1291,6 +1288,9 @@
   </si>
   <si>
     <t>fcrfabric collection</t>
+  </si>
+  <si>
+    <t>Статистическая информация подключения портов устройств</t>
   </si>
 </sst>
 </file>
@@ -1707,7 +1707,7 @@
   <dimension ref="A1:AH10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1749,25 +1749,22 @@
       <c r="E1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G2" t="s">
         <v>337</v>
@@ -1907,7 +1904,7 @@
         <v>285</v>
       </c>
       <c r="C4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D4" t="s">
         <v>328</v>
@@ -1916,7 +1913,7 @@
         <v>328</v>
       </c>
       <c r="F4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G4" t="s">
         <v>328</v>
@@ -1955,16 +1952,16 @@
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G5" t="s">
         <v>338</v>
@@ -2056,16 +2053,16 @@
         <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G6" t="s">
         <v>359</v>
@@ -2157,7 +2154,7 @@
         <v>86</v>
       </c>
       <c r="E7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G7" t="s">
         <v>339</v>
@@ -2206,10 +2203,10 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
@@ -2229,8 +2226,8 @@
   <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F97" sqref="F97:H98"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H39" sqref="F37:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,7 +2274,7 @@
         <v>196</v>
       </c>
       <c r="K1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2559,7 +2556,7 @@
         <v>146</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2591,7 +2588,7 @@
         <v>147</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2623,7 +2620,7 @@
         <v>147</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2687,7 +2684,7 @@
         <v>144</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2719,7 +2716,7 @@
         <v>144</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2751,7 +2748,7 @@
         <v>145</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2783,7 +2780,7 @@
         <v>145</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2815,7 +2812,7 @@
         <v>145</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2847,7 +2844,7 @@
         <v>143</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -3015,7 +3012,7 @@
         <v>149</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -3041,7 +3038,7 @@
         <v>149</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -3067,7 +3064,7 @@
         <v>149</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -3093,7 +3090,7 @@
         <v>149</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -3119,7 +3116,7 @@
         <v>149</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -3145,7 +3142,7 @@
         <v>149</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -3171,7 +3168,7 @@
         <v>149</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -3197,7 +3194,7 @@
         <v>226</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -3252,7 +3249,7 @@
         <v>227</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3278,7 +3275,7 @@
         <v>227</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -3304,7 +3301,7 @@
         <v>227</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -3357,38 +3354,38 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F39" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39" t="s">
+        <v>364</v>
+      </c>
+      <c r="J39" s="10" t="s">
         <v>369</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39" t="s">
-        <v>365</v>
-      </c>
-      <c r="J39" s="10" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -3397,46 +3394,46 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F41" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41" t="s">
         <v>364</v>
       </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41" t="s">
-        <v>365</v>
-      </c>
       <c r="J41" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -3445,10 +3442,10 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -3537,7 +3534,7 @@
         <v>163</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -3752,7 +3749,7 @@
         <v>289</v>
       </c>
       <c r="K56" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -3815,7 +3812,7 @@
         <v>293</v>
       </c>
       <c r="K59" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -3864,7 +3861,7 @@
         <v>274</v>
       </c>
       <c r="K61" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -3947,7 +3944,7 @@
         <v>173</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.25">
@@ -4159,10 +4156,10 @@
         <v>173</v>
       </c>
       <c r="J75" t="s">
-        <v>360</v>
+        <v>423</v>
       </c>
       <c r="K75" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
@@ -4337,7 +4334,7 @@
         <v>347</v>
       </c>
       <c r="K83" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.25">
@@ -4363,7 +4360,7 @@
         <v>348</v>
       </c>
       <c r="K84" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
@@ -4386,7 +4383,7 @@
         <v>344</v>
       </c>
       <c r="K85" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.25">
@@ -4412,7 +4409,7 @@
         <v>251</v>
       </c>
       <c r="K86" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.25">
@@ -4535,7 +4532,7 @@
         <v>238</v>
       </c>
       <c r="K92" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.25">
@@ -4558,7 +4555,7 @@
         <v>350</v>
       </c>
       <c r="K93" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.25">
@@ -4581,7 +4578,7 @@
         <v>351</v>
       </c>
       <c r="K94" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.25">
@@ -4604,7 +4601,7 @@
         <v>253</v>
       </c>
       <c r="K95" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.25">
@@ -4612,19 +4609,19 @@
         <v>95</v>
       </c>
       <c r="F96" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96" t="s">
         <v>390</v>
       </c>
-      <c r="G96">
-        <v>0</v>
-      </c>
-      <c r="H96">
-        <v>0</v>
-      </c>
-      <c r="I96" t="s">
-        <v>391</v>
-      </c>
       <c r="J96" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -4632,19 +4629,19 @@
         <v>96</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J97" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -4652,19 +4649,19 @@
         <v>96</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J98" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -4681,7 +4678,7 @@
         <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J99" t="s">
         <v>306</v>
@@ -4701,7 +4698,7 @@
         <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J100" t="s">
         <v>230</v>
@@ -4727,13 +4724,13 @@
         <v>0</v>
       </c>
       <c r="I101" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J101" s="10" t="s">
         <v>307</v>
       </c>
       <c r="K101" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -4750,13 +4747,13 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K102" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
@@ -4776,7 +4773,7 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J103" t="s">
         <v>303</v>
@@ -4796,13 +4793,13 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J104" t="s">
         <v>304</v>
       </c>
       <c r="K104" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
@@ -4819,13 +4816,13 @@
         <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J105" t="s">
         <v>302</v>
       </c>
       <c r="K105" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
@@ -4916,19 +4913,19 @@
         <v>95</v>
       </c>
       <c r="F110" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="I110" t="s">
         <v>375</v>
       </c>
-      <c r="G110">
-        <v>0</v>
-      </c>
-      <c r="H110">
-        <v>0</v>
-      </c>
-      <c r="I110" t="s">
-        <v>376</v>
-      </c>
       <c r="J110" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lsan detection added to strorage host presentation module
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="13935"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="13935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="428">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1291,6 +1291,18 @@
   </si>
   <si>
     <t>Статистическая информация подключения портов устройств</t>
+  </si>
+  <si>
+    <t>Synergy review</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\IBS\SAN APR21</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\IBS\APR21\ssave</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\IBS\APR21\synergy</t>
   </si>
 </sst>
 </file>
@@ -1704,85 +1716,86 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AH10"/>
+  <dimension ref="A1:AI10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" customWidth="1"/>
-    <col min="4" max="4" width="122.7109375" customWidth="1"/>
-    <col min="5" max="5" width="48.42578125" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" customWidth="1"/>
-    <col min="7" max="7" width="80.140625" customWidth="1"/>
-    <col min="8" max="8" width="68.5703125" customWidth="1"/>
-    <col min="9" max="9" width="48.7109375" customWidth="1"/>
-    <col min="10" max="10" width="62" customWidth="1"/>
-    <col min="11" max="13" width="89.5703125" customWidth="1"/>
-    <col min="14" max="14" width="69.85546875" customWidth="1"/>
-    <col min="15" max="15" width="52.140625" customWidth="1"/>
-    <col min="16" max="16" width="73.140625" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" customWidth="1"/>
-    <col min="18" max="19" width="76" customWidth="1"/>
-    <col min="20" max="20" width="72.28515625" customWidth="1"/>
-    <col min="21" max="21" width="61.7109375" customWidth="1"/>
-    <col min="22" max="22" width="60" customWidth="1"/>
-    <col min="23" max="23" width="38.140625" customWidth="1"/>
-    <col min="24" max="24" width="69" customWidth="1"/>
-    <col min="25" max="25" width="72.42578125" customWidth="1"/>
-    <col min="26" max="26" width="111.5703125" customWidth="1"/>
-    <col min="27" max="27" width="72.5703125" customWidth="1"/>
-    <col min="28" max="28" width="86.85546875" customWidth="1"/>
-    <col min="29" max="30" width="64.7109375" customWidth="1"/>
-    <col min="31" max="31" width="54.5703125" customWidth="1"/>
-    <col min="32" max="32" width="75.42578125" customWidth="1"/>
-    <col min="33" max="33" width="58.140625" customWidth="1"/>
+    <col min="3" max="3" width="80.140625" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
+    <col min="5" max="5" width="122.7109375" customWidth="1"/>
+    <col min="6" max="6" width="48.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="8" max="8" width="80.140625" customWidth="1"/>
+    <col min="9" max="9" width="68.5703125" customWidth="1"/>
+    <col min="10" max="10" width="48.7109375" customWidth="1"/>
+    <col min="11" max="11" width="62" customWidth="1"/>
+    <col min="12" max="14" width="89.5703125" customWidth="1"/>
+    <col min="15" max="15" width="69.85546875" customWidth="1"/>
+    <col min="16" max="16" width="52.140625" customWidth="1"/>
+    <col min="17" max="17" width="73.140625" customWidth="1"/>
+    <col min="18" max="18" width="29.7109375" customWidth="1"/>
+    <col min="19" max="20" width="76" customWidth="1"/>
+    <col min="21" max="21" width="72.28515625" customWidth="1"/>
+    <col min="22" max="22" width="61.7109375" customWidth="1"/>
+    <col min="23" max="23" width="60" customWidth="1"/>
+    <col min="24" max="24" width="38.140625" customWidth="1"/>
+    <col min="25" max="25" width="69" customWidth="1"/>
+    <col min="26" max="26" width="72.42578125" customWidth="1"/>
+    <col min="27" max="27" width="111.5703125" customWidth="1"/>
+    <col min="28" max="28" width="72.5703125" customWidth="1"/>
+    <col min="29" max="29" width="86.85546875" customWidth="1"/>
+    <col min="30" max="31" width="64.7109375" customWidth="1"/>
+    <col min="32" max="32" width="54.5703125" customWidth="1"/>
+    <col min="33" max="33" width="75.42578125" customWidth="1"/>
+    <col min="34" max="34" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2" t="s">
         <v>411</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>405</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>397</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>370</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>337</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>324</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>317</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>314</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>310</v>
-      </c>
-      <c r="L2" t="s">
-        <v>318</v>
       </c>
       <c r="M2" t="s">
         <v>318</v>
@@ -1791,425 +1804,443 @@
         <v>318</v>
       </c>
       <c r="O2" t="s">
+        <v>318</v>
+      </c>
+      <c r="P2" t="s">
         <v>280</v>
-      </c>
-      <c r="P2" t="s">
-        <v>276</v>
       </c>
       <c r="Q2" t="s">
         <v>276</v>
       </c>
       <c r="R2" t="s">
-        <v>258</v>
+        <v>276</v>
       </c>
       <c r="S2" t="s">
         <v>258</v>
       </c>
       <c r="T2" t="s">
+        <v>258</v>
+      </c>
+      <c r="U2" t="s">
         <v>240</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>234</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>189</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>188</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>155</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>111</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>97</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>83</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>284</v>
       </c>
       <c r="C3" s="12">
+        <v>44307</v>
+      </c>
+      <c r="D3" s="12">
         <v>44294</v>
       </c>
-      <c r="D3" s="12">
+      <c r="E3" s="12">
         <v>44292</v>
       </c>
-      <c r="E3" s="12">
+      <c r="F3" s="12">
         <v>29681</v>
       </c>
-      <c r="F3" s="12">
+      <c r="G3" s="12">
         <v>44286</v>
       </c>
-      <c r="G3" s="12">
+      <c r="H3" s="12">
         <v>44260</v>
       </c>
-      <c r="H3" s="12">
+      <c r="I3" s="12">
         <v>44244</v>
       </c>
-      <c r="I3" s="12">
+      <c r="J3" s="12">
         <v>44245</v>
       </c>
-      <c r="J3" s="12">
+      <c r="K3" s="12">
         <v>44223</v>
       </c>
-      <c r="K3" s="12">
+      <c r="L3" s="12">
         <v>44209</v>
       </c>
-      <c r="L3" s="12">
+      <c r="M3" s="12">
         <v>44253</v>
       </c>
-      <c r="M3" s="12">
+      <c r="N3" s="12">
         <v>44237</v>
       </c>
-      <c r="P3" s="12">
+      <c r="Q3" s="12">
         <v>44181</v>
       </c>
-      <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI3" s="1"/>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>285</v>
       </c>
       <c r="C4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D4" t="s">
         <v>412</v>
-      </c>
-      <c r="D4" t="s">
-        <v>328</v>
       </c>
       <c r="E4" t="s">
         <v>328</v>
       </c>
       <c r="F4" t="s">
+        <v>328</v>
+      </c>
+      <c r="G4" t="s">
         <v>371</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>328</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>323</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>328</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>328</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>334</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>323</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>283</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>282</v>
       </c>
-      <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AI4" s="1"/>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
+        <v>425</v>
+      </c>
+      <c r="D5" t="s">
         <v>413</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>407</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>398</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>372</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>338</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>325</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>330</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>315</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>309</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>335</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>321</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>319</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>281</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>286</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>278</v>
-      </c>
-      <c r="R5" t="s">
-        <v>259</v>
       </c>
       <c r="S5" t="s">
         <v>259</v>
       </c>
       <c r="T5" t="s">
+        <v>259</v>
+      </c>
+      <c r="U5" t="s">
         <v>242</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>233</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>223</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>187</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>157</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>113</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>98</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>85</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>1</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>74</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>72</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>4</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>25</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>60</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C6" t="s">
+        <v>426</v>
+      </c>
+      <c r="D6" t="s">
         <v>414</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>406</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>399</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>373</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>359</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>326</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>329</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>316</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>311</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>336</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>322</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>320</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>279</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>287</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>277</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>272</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>260</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>241</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>231</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>222</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>186</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>156</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>112</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>108</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>84</v>
       </c>
-      <c r="AB6" t="s">
-        <v>0</v>
-      </c>
       <c r="AC6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD6" t="s">
         <v>73</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>71</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>3</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>24</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>59</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>400</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>339</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>312</v>
-      </c>
-      <c r="R7" t="s">
-        <v>261</v>
       </c>
       <c r="S7" t="s">
         <v>261</v>
       </c>
-      <c r="U7" t="s">
+      <c r="T7" t="s">
+        <v>261</v>
+      </c>
+      <c r="V7" t="s">
         <v>232</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>158</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>109</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>87</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>99</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="G8" t="s">
+      <c r="C8" t="s">
+        <v>427</v>
+      </c>
+      <c r="H8" t="s">
         <v>340</v>
-      </c>
-      <c r="R8" t="s">
-        <v>263</v>
       </c>
       <c r="S8" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="T8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>361</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>239</v>
       </c>
@@ -2225,9 +2256,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K110"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H39" sqref="F37:H39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G100" sqref="G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3367,7 +3398,7 @@
         <v>0</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" t="s">
         <v>364</v>
@@ -4632,10 +4663,10 @@
         <v>387</v>
       </c>
       <c r="G97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I97" t="s">
         <v>390</v>
@@ -4652,7 +4683,7 @@
         <v>388</v>
       </c>
       <c r="G98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H98">
         <v>0</v>

</xml_diff>

<commit_message>
storage port partner conncetion added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="13935" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27960" windowHeight="8925" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -321,9 +321,6 @@
     <t>C:\Users\vlasenko\Documents\06.CONFIGS\SBRF\Nov 2019\blade\SZB_Chassis</t>
   </si>
   <si>
-    <t>Сервера</t>
-  </si>
-  <si>
     <t>report_type</t>
   </si>
   <si>
@@ -1303,6 +1300,9 @@
   </si>
   <si>
     <t>C:\Users\vlasenko\Documents\06.CONFIGS\IBS\APR21\synergy</t>
+  </si>
+  <si>
+    <t>Серверы</t>
   </si>
 </sst>
 </file>
@@ -1719,7 +1719,7 @@
   <dimension ref="A1:AI10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1768,76 +1768,76 @@
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F2" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J2" t="s">
+        <v>316</v>
+      </c>
+      <c r="K2" t="s">
+        <v>313</v>
+      </c>
+      <c r="L2" t="s">
+        <v>309</v>
+      </c>
+      <c r="M2" t="s">
         <v>317</v>
       </c>
-      <c r="K2" t="s">
-        <v>314</v>
-      </c>
-      <c r="L2" t="s">
-        <v>310</v>
-      </c>
-      <c r="M2" t="s">
-        <v>318</v>
-      </c>
       <c r="N2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="O2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Q2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="R2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="S2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="T2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="U2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="V2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="W2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="X2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Y2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Z2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AA2" t="s">
         <v>97</v>
@@ -1869,7 +1869,7 @@
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C3" s="12">
         <v>44307</v>
@@ -1920,46 +1920,46 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="M4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="Q4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="R4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
@@ -1974,76 +1974,76 @@
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="N5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="O5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="P5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="R5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="S5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="T5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="U5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="V5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="W5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Y5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Z5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AA5" t="s">
         <v>98</v>
@@ -2078,79 +2078,79 @@
         <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="J6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Q6" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="R6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="S6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="T6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="U6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="V6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="W6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="X6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Y6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Z6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AA6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AB6" t="s">
         <v>84</v>
@@ -2182,28 +2182,28 @@
         <v>86</v>
       </c>
       <c r="F7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="L7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="S7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="T7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="V7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Y7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="AA7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AB7" t="s">
         <v>87</v>
@@ -2217,32 +2217,32 @@
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="C8" t="s">
+        <v>426</v>
+      </c>
+      <c r="H8" t="s">
+        <v>339</v>
+      </c>
+      <c r="S8" t="s">
         <v>262</v>
       </c>
-      <c r="C8" t="s">
-        <v>427</v>
-      </c>
-      <c r="H8" t="s">
-        <v>340</v>
-      </c>
-      <c r="S8" t="s">
-        <v>263</v>
-      </c>
       <c r="T8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2257,8 +2257,8 @@
   <dimension ref="A1:K110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G100" sqref="G100"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2281,10 +2281,10 @@
         <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E1" t="s">
         <v>11</v>
@@ -2299,13 +2299,13 @@
         <v>23</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2313,7 +2313,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>94</v>
@@ -2331,10 +2331,10 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2342,7 +2342,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>94</v>
@@ -2360,10 +2360,10 @@
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2371,10 +2371,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>94</v>
@@ -2392,10 +2392,10 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2403,10 +2403,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>94</v>
@@ -2424,10 +2424,10 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2435,10 +2435,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>94</v>
@@ -2456,10 +2456,10 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2467,10 +2467,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>94</v>
@@ -2488,10 +2488,10 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2499,7 +2499,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>13</v>
@@ -2520,10 +2520,10 @@
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2531,7 +2531,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>13</v>
@@ -2552,10 +2552,10 @@
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2563,7 +2563,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>31</v>
@@ -2584,10 +2584,10 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2595,10 +2595,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>94</v>
@@ -2616,10 +2616,10 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2627,10 +2627,10 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>94</v>
@@ -2648,10 +2648,10 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2659,10 +2659,10 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>94</v>
@@ -2680,10 +2680,10 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2691,10 +2691,10 @@
         <v>10</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>94</v>
@@ -2712,10 +2712,10 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2723,10 +2723,10 @@
         <v>10</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>94</v>
@@ -2744,10 +2744,10 @@
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2755,7 +2755,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>41</v>
@@ -2776,10 +2776,10 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2787,7 +2787,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>41</v>
@@ -2808,10 +2808,10 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2819,7 +2819,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>41</v>
@@ -2840,10 +2840,10 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2851,10 +2851,10 @@
         <v>12</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>94</v>
@@ -2872,10 +2872,10 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2883,10 +2883,10 @@
         <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>94</v>
@@ -2901,10 +2901,10 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2912,10 +2912,10 @@
         <v>12</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>94</v>
@@ -2930,10 +2930,10 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2941,10 +2941,10 @@
         <v>12</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>94</v>
@@ -2959,18 +2959,18 @@
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>94</v>
@@ -2985,18 +2985,18 @@
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>94</v>
@@ -3011,10 +3011,10 @@
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -3022,10 +3022,10 @@
         <v>13</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>94</v>
@@ -3040,18 +3040,18 @@
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>94</v>
@@ -3066,18 +3066,18 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>94</v>
@@ -3092,18 +3092,18 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>94</v>
@@ -3118,18 +3118,18 @@
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>94</v>
@@ -3144,24 +3144,24 @@
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -3170,24 +3170,24 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -3196,62 +3196,62 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>225</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F32" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32" t="s">
         <v>225</v>
       </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32" t="s">
-        <v>226</v>
-      </c>
       <c r="J32" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>297</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>298</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F33" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
         <v>294</v>
       </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="J33" s="10" t="s">
         <v>295</v>
-      </c>
-      <c r="J33" s="10" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3259,10 +3259,10 @@
         <v>19</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>94</v>
@@ -3277,18 +3277,18 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>94</v>
@@ -3303,24 +3303,24 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -3329,22 +3329,22 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -3353,22 +3353,22 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -3377,46 +3377,46 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F39" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>363</v>
+      </c>
+      <c r="J39" s="10" t="s">
         <v>368</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39" t="s">
-        <v>364</v>
-      </c>
-      <c r="J39" s="10" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -3425,46 +3425,46 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F41" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41" t="s">
         <v>363</v>
       </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41" t="s">
-        <v>364</v>
-      </c>
       <c r="J41" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -3473,10 +3473,10 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -3484,7 +3484,7 @@
         <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>95</v>
@@ -3499,10 +3499,10 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -3519,10 +3519,10 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3539,21 +3539,21 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -3562,10 +3562,10 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -3573,7 +3573,7 @@
         <v>96</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -3582,10 +3582,10 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J47" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -3593,7 +3593,7 @@
         <v>16</v>
       </c>
       <c r="B48" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>95</v>
@@ -3608,10 +3608,10 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -3619,7 +3619,7 @@
         <v>95</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -3628,10 +3628,10 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -3648,10 +3648,10 @@
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J50" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -3668,10 +3668,10 @@
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J51" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -3688,10 +3688,10 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J52" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -3708,10 +3708,10 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J53" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -3728,10 +3728,10 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -3739,7 +3739,7 @@
         <v>18</v>
       </c>
       <c r="B55" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>95</v>
@@ -3754,10 +3754,10 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -3765,22 +3765,22 @@
         <v>95</v>
       </c>
       <c r="F56" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56" t="s">
+        <v>171</v>
+      </c>
+      <c r="J56" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56" t="s">
-        <v>172</v>
-      </c>
-      <c r="J56" s="10" t="s">
-        <v>289</v>
-      </c>
       <c r="K56" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -3797,10 +3797,10 @@
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J57" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -3817,10 +3817,10 @@
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J58" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -3828,22 +3828,22 @@
         <v>96</v>
       </c>
       <c r="F59" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59" t="s">
+        <v>171</v>
+      </c>
+      <c r="J59" t="s">
         <v>292</v>
       </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59" t="s">
-        <v>172</v>
-      </c>
-      <c r="J59" t="s">
-        <v>293</v>
-      </c>
       <c r="K59" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -3851,7 +3851,7 @@
         <v>20</v>
       </c>
       <c r="B60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>95</v>
@@ -3866,10 +3866,10 @@
         <v>0</v>
       </c>
       <c r="I60" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -3877,22 +3877,22 @@
         <v>95</v>
       </c>
       <c r="F61" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61" t="s">
+        <v>172</v>
+      </c>
+      <c r="J61" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-      <c r="I61" t="s">
-        <v>173</v>
-      </c>
-      <c r="J61" s="10" t="s">
-        <v>274</v>
-      </c>
       <c r="K61" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -3900,7 +3900,7 @@
         <v>95</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -3909,10 +3909,10 @@
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -3920,28 +3920,28 @@
         <v>95</v>
       </c>
       <c r="F63" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63" t="s">
+        <v>172</v>
+      </c>
+      <c r="J63" s="10" t="s">
         <v>246</v>
-      </c>
-      <c r="G63">
-        <v>0</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
-      <c r="I63" t="s">
-        <v>173</v>
-      </c>
-      <c r="J63" s="10" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D64" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F64" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="F64" s="11" t="s">
-        <v>249</v>
-      </c>
       <c r="G64">
         <v>0</v>
       </c>
@@ -3949,21 +3949,21 @@
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -3972,18 +3972,18 @@
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C66" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>95</v>
@@ -3998,10 +3998,10 @@
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.25">
@@ -4009,7 +4009,7 @@
         <v>95</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -4018,44 +4018,44 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>100</v>
+        <v>427</v>
       </c>
       <c r="G68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I68" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J68" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -4064,10 +4064,10 @@
         <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J69" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.25">
@@ -4075,7 +4075,7 @@
         <v>96</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -4084,10 +4084,10 @@
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J70" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.25">
@@ -4095,7 +4095,7 @@
         <v>96</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -4104,10 +4104,10 @@
         <v>0</v>
       </c>
       <c r="I71" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J71" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.25">
@@ -4115,7 +4115,7 @@
         <v>96</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -4124,10 +4124,10 @@
         <v>0</v>
       </c>
       <c r="I72" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J72" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.25">
@@ -4135,7 +4135,7 @@
         <v>96</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -4144,10 +4144,10 @@
         <v>0</v>
       </c>
       <c r="I73" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J73" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.25">
@@ -4155,7 +4155,7 @@
         <v>96</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -4164,10 +4164,10 @@
         <v>0</v>
       </c>
       <c r="I74" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J74" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.25">
@@ -4175,7 +4175,7 @@
         <v>96</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -4184,13 +4184,13 @@
         <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J75" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="K75" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
@@ -4198,7 +4198,7 @@
         <v>96</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -4207,21 +4207,21 @@
         <v>0</v>
       </c>
       <c r="I76" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J76" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D77" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -4230,10 +4230,10 @@
         <v>0</v>
       </c>
       <c r="I77" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J77" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.25">
@@ -4241,7 +4241,7 @@
         <v>96</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -4250,10 +4250,10 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J78" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.25">
@@ -4261,7 +4261,7 @@
         <v>96</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -4270,10 +4270,10 @@
         <v>0</v>
       </c>
       <c r="I79" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J79" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.25">
@@ -4281,7 +4281,7 @@
         <v>96</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -4290,44 +4290,44 @@
         <v>0</v>
       </c>
       <c r="I80" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J80" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F81" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81" t="s">
         <v>179</v>
       </c>
-      <c r="G81">
-        <v>0</v>
-      </c>
-      <c r="H81">
-        <v>0</v>
-      </c>
-      <c r="I81" t="s">
-        <v>180</v>
-      </c>
       <c r="J81" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -4336,21 +4336,21 @@
         <v>0</v>
       </c>
       <c r="I82" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -4359,24 +4359,24 @@
         <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J83" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K83" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -4385,13 +4385,13 @@
         <v>0</v>
       </c>
       <c r="I84" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J84" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K84" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
@@ -4399,48 +4399,48 @@
         <v>95</v>
       </c>
       <c r="F85" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85" t="s">
+        <v>179</v>
+      </c>
+      <c r="J85" s="10" t="s">
         <v>343</v>
       </c>
-      <c r="G85">
-        <v>0</v>
-      </c>
-      <c r="H85">
-        <v>0</v>
-      </c>
-      <c r="I85" t="s">
-        <v>180</v>
-      </c>
-      <c r="J85" s="10" t="s">
-        <v>344</v>
-      </c>
       <c r="K85" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F86" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86" t="s">
+        <v>179</v>
+      </c>
+      <c r="J86" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="G86">
-        <v>0</v>
-      </c>
-      <c r="H86">
-        <v>0</v>
-      </c>
-      <c r="I86" t="s">
-        <v>180</v>
-      </c>
-      <c r="J86" s="10" t="s">
-        <v>251</v>
-      </c>
       <c r="K86" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.25">
@@ -4448,7 +4448,7 @@
         <v>96</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -4457,10 +4457,10 @@
         <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J87" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.25">
@@ -4468,7 +4468,7 @@
         <v>96</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -4477,10 +4477,10 @@
         <v>0</v>
       </c>
       <c r="I88" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J88" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.25">
@@ -4488,7 +4488,7 @@
         <v>96</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -4497,10 +4497,10 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J89" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.25">
@@ -4508,7 +4508,7 @@
         <v>96</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -4517,10 +4517,10 @@
         <v>0</v>
       </c>
       <c r="I90" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J90" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.25">
@@ -4528,19 +4528,19 @@
         <v>96</v>
       </c>
       <c r="F91" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91" t="s">
+        <v>179</v>
+      </c>
+      <c r="J91" t="s">
         <v>235</v>
-      </c>
-      <c r="G91">
-        <v>0</v>
-      </c>
-      <c r="H91">
-        <v>0</v>
-      </c>
-      <c r="I91" t="s">
-        <v>180</v>
-      </c>
-      <c r="J91" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.25">
@@ -4548,22 +4548,22 @@
         <v>96</v>
       </c>
       <c r="F92" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92" t="s">
+        <v>179</v>
+      </c>
+      <c r="J92" t="s">
         <v>237</v>
       </c>
-      <c r="G92">
-        <v>0</v>
-      </c>
-      <c r="H92">
-        <v>0</v>
-      </c>
-      <c r="I92" t="s">
-        <v>180</v>
-      </c>
-      <c r="J92" t="s">
-        <v>238</v>
-      </c>
       <c r="K92" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.25">
@@ -4571,7 +4571,7 @@
         <v>96</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -4580,13 +4580,13 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J93" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K93" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.25">
@@ -4594,7 +4594,7 @@
         <v>96</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -4603,13 +4603,13 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J94" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K94" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.25">
@@ -4617,22 +4617,22 @@
         <v>96</v>
       </c>
       <c r="F95" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95" t="s">
+        <v>179</v>
+      </c>
+      <c r="J95" t="s">
         <v>252</v>
       </c>
-      <c r="G95">
-        <v>0</v>
-      </c>
-      <c r="H95">
-        <v>0</v>
-      </c>
-      <c r="I95" t="s">
-        <v>180</v>
-      </c>
-      <c r="J95" t="s">
-        <v>253</v>
-      </c>
       <c r="K95" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.25">
@@ -4640,19 +4640,19 @@
         <v>95</v>
       </c>
       <c r="F96" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+      <c r="I96" t="s">
         <v>389</v>
       </c>
-      <c r="G96">
-        <v>0</v>
-      </c>
-      <c r="H96">
-        <v>0</v>
-      </c>
-      <c r="I96" t="s">
-        <v>390</v>
-      </c>
       <c r="J96" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -4660,19 +4660,19 @@
         <v>96</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J97" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -4680,19 +4680,19 @@
         <v>96</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H98">
         <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J98" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -4700,7 +4700,7 @@
         <v>95</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -4709,10 +4709,10 @@
         <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J99" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -4720,19 +4720,19 @@
         <v>96</v>
       </c>
       <c r="F100" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100" t="s">
+        <v>390</v>
+      </c>
+      <c r="J100" t="s">
         <v>229</v>
-      </c>
-      <c r="G100">
-        <v>0</v>
-      </c>
-      <c r="H100">
-        <v>0</v>
-      </c>
-      <c r="I100" t="s">
-        <v>391</v>
-      </c>
-      <c r="J100" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
@@ -4740,13 +4740,13 @@
         <v>17</v>
       </c>
       <c r="B101" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F101" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -4755,13 +4755,13 @@
         <v>0</v>
       </c>
       <c r="I101" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J101" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K101" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -4769,7 +4769,7 @@
         <v>96</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -4778,24 +4778,24 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J102" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K102" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -4804,10 +4804,10 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J103" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -4815,7 +4815,7 @@
         <v>95</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -4824,13 +4824,13 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J104" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K104" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
@@ -4838,33 +4838,33 @@
         <v>96</v>
       </c>
       <c r="F105" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+      <c r="I105" t="s">
+        <v>392</v>
+      </c>
+      <c r="J105" t="s">
         <v>301</v>
       </c>
-      <c r="G105">
-        <v>0</v>
-      </c>
-      <c r="H105">
-        <v>0</v>
-      </c>
-      <c r="I105" t="s">
-        <v>393</v>
-      </c>
-      <c r="J105" t="s">
-        <v>302</v>
-      </c>
       <c r="K105" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F106" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -4873,10 +4873,10 @@
         <v>0</v>
       </c>
       <c r="I106" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J106" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
@@ -4884,7 +4884,7 @@
         <v>95</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -4893,10 +4893,10 @@
         <v>0</v>
       </c>
       <c r="I107" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J107" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
@@ -4904,7 +4904,7 @@
         <v>95</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -4913,10 +4913,10 @@
         <v>0</v>
       </c>
       <c r="I108" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J108" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
@@ -4924,7 +4924,7 @@
         <v>95</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -4933,10 +4933,10 @@
         <v>0</v>
       </c>
       <c r="I109" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J109" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
@@ -4944,19 +4944,19 @@
         <v>95</v>
       </c>
       <c r="F110" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="I110" t="s">
         <v>374</v>
       </c>
-      <c r="G110">
-        <v>0</v>
-      </c>
-      <c r="H110">
-        <v>0</v>
-      </c>
-      <c r="I110" t="s">
-        <v>375</v>
-      </c>
       <c r="J110" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -4982,15 +4982,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" t="s">
         <v>184</v>
-      </c>
-      <c r="B1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>50</v>
@@ -4998,7 +4998,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>51</v>
@@ -5006,7 +5006,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>52</v>
@@ -5014,7 +5014,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
storage connection statistics added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -12,14 +12,14 @@
     <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$K$110</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$K$112</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="432">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1303,6 +1303,18 @@
   </si>
   <si>
     <t>Серверы</t>
+  </si>
+  <si>
+    <t>Storage connection statistics</t>
+  </si>
+  <si>
+    <t>Статистическая информация подключения портов массивов</t>
+  </si>
+  <si>
+    <t>Статистика_массивов</t>
+  </si>
+  <si>
+    <t>storage_connection_statistics</t>
   </si>
 </sst>
 </file>
@@ -1718,8 +1730,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AI10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2254,11 +2266,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K110"/>
+  <dimension ref="A1:K112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H73" sqref="H73"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3863,7 +3875,7 @@
         <v>0</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60" t="s">
         <v>172</v>
@@ -3877,7 +3889,7 @@
         <v>95</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>272</v>
+        <v>431</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -3889,7 +3901,7 @@
         <v>172</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>273</v>
+        <v>428</v>
       </c>
       <c r="K61" t="s">
         <v>409</v>
@@ -3899,8 +3911,8 @@
       <c r="D62" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F62" s="2" t="s">
-        <v>244</v>
+      <c r="F62" s="9" t="s">
+        <v>272</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -3912,7 +3924,10 @@
         <v>172</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>341</v>
+        <v>273</v>
+      </c>
+      <c r="K62" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -3920,7 +3935,7 @@
         <v>95</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -3932,15 +3947,15 @@
         <v>172</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>246</v>
+        <v>341</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D64" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="F64" s="11" t="s">
-        <v>248</v>
+      <c r="D64" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -3956,14 +3971,11 @@
       </c>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>133</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F65" s="8" t="s">
-        <v>109</v>
+      <c r="D65" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>248</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -3975,21 +3987,18 @@
         <v>172</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>385</v>
+        <v>246</v>
       </c>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>119</v>
-      </c>
-      <c r="C66" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F66" s="7" t="s">
-        <v>93</v>
+      <c r="F66" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -4001,15 +4010,21 @@
         <v>172</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>340</v>
+        <v>385</v>
       </c>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67" t="s">
+        <v>132</v>
+      </c>
       <c r="D67" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>312</v>
+        <v>93</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -4021,41 +4036,38 @@
         <v>172</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>134</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>427</v>
+      <c r="D68" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>312</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68" t="s">
         <v>172</v>
       </c>
-      <c r="J68" t="s">
-        <v>199</v>
+      <c r="J68" s="10" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>101</v>
+        <v>427</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -4067,15 +4079,18 @@
         <v>172</v>
       </c>
       <c r="J69" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>135</v>
+      </c>
       <c r="D70" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -4087,7 +4102,7 @@
         <v>172</v>
       </c>
       <c r="J70" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.25">
@@ -4095,7 +4110,7 @@
         <v>96</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -4107,7 +4122,7 @@
         <v>172</v>
       </c>
       <c r="J71" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.25">
@@ -4115,7 +4130,7 @@
         <v>96</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -4127,7 +4142,7 @@
         <v>172</v>
       </c>
       <c r="J72" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.25">
@@ -4135,7 +4150,7 @@
         <v>96</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -4147,7 +4162,7 @@
         <v>172</v>
       </c>
       <c r="J73" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.25">
@@ -4155,7 +4170,7 @@
         <v>96</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -4167,7 +4182,7 @@
         <v>172</v>
       </c>
       <c r="J74" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.25">
@@ -4175,7 +4190,7 @@
         <v>96</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>274</v>
+        <v>106</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -4187,10 +4202,7 @@
         <v>172</v>
       </c>
       <c r="J75" t="s">
-        <v>422</v>
-      </c>
-      <c r="K75" t="s">
-        <v>409</v>
+        <v>212</v>
       </c>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
@@ -4198,10 +4210,10 @@
         <v>96</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>164</v>
+        <v>430</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -4210,18 +4222,18 @@
         <v>172</v>
       </c>
       <c r="J76" t="s">
-        <v>202</v>
+        <v>429</v>
+      </c>
+      <c r="K76" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>165</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F77" s="9" t="s">
-        <v>219</v>
+      <c r="D77" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>274</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -4230,10 +4242,13 @@
         <v>0</v>
       </c>
       <c r="I77" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J77" t="s">
-        <v>304</v>
+        <v>422</v>
+      </c>
+      <c r="K77" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.25">
@@ -4241,7 +4256,7 @@
         <v>96</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -4250,30 +4265,33 @@
         <v>0</v>
       </c>
       <c r="I78" t="s">
+        <v>172</v>
+      </c>
+      <c r="J78" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>165</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79" t="s">
         <v>173</v>
       </c>
-      <c r="J78" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D79" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="G79">
-        <v>0</v>
-      </c>
-      <c r="H79">
-        <v>0</v>
-      </c>
-      <c r="I79" t="s">
-        <v>166</v>
-      </c>
       <c r="J79" t="s">
-        <v>213</v>
+        <v>304</v>
       </c>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.25">
@@ -4281,76 +4299,70 @@
         <v>96</v>
       </c>
       <c r="F80" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80" t="s">
+        <v>173</v>
+      </c>
+      <c r="J80" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D81" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81" t="s">
+        <v>166</v>
+      </c>
+      <c r="J81" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D82" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F82" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-      <c r="H80">
-        <v>0</v>
-      </c>
-      <c r="I80" t="s">
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82" t="s">
         <v>166</v>
       </c>
-      <c r="J80" t="s">
+      <c r="J82" t="s">
         <v>270</v>
-      </c>
-    </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>177</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F81" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="G81">
-        <v>0</v>
-      </c>
-      <c r="H81">
-        <v>0</v>
-      </c>
-      <c r="I81" t="s">
-        <v>179</v>
-      </c>
-      <c r="J81" s="10" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
-        <v>254</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F82" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="G82">
-        <v>0</v>
-      </c>
-      <c r="H82">
-        <v>0</v>
-      </c>
-      <c r="I82" t="s">
-        <v>179</v>
-      </c>
-      <c r="J82" s="10" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>256</v>
+        <v>177</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -4362,21 +4374,18 @@
         <v>179</v>
       </c>
       <c r="J83" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="K83" t="s">
-        <v>409</v>
+        <v>344</v>
       </c>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>218</v>
+        <v>180</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -4388,18 +4397,18 @@
         <v>179</v>
       </c>
       <c r="J84" s="10" t="s">
-        <v>347</v>
-      </c>
-      <c r="K84" t="s">
-        <v>409</v>
+        <v>345</v>
       </c>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>256</v>
+      </c>
       <c r="D85" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>342</v>
+        <v>189</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -4411,7 +4420,7 @@
         <v>179</v>
       </c>
       <c r="J85" s="10" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="K85" t="s">
         <v>409</v>
@@ -4419,13 +4428,13 @@
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>249</v>
+        <v>218</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -4437,18 +4446,18 @@
         <v>179</v>
       </c>
       <c r="J86" s="10" t="s">
-        <v>250</v>
+        <v>347</v>
       </c>
       <c r="K86" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D87" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>181</v>
+      <c r="D87" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>342</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -4459,16 +4468,22 @@
       <c r="I87" t="s">
         <v>179</v>
       </c>
-      <c r="J87" t="s">
-        <v>214</v>
+      <c r="J87" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="K87" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D88" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>182</v>
+      <c r="B88" t="s">
+        <v>253</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>249</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -4479,8 +4494,11 @@
       <c r="I88" t="s">
         <v>179</v>
       </c>
-      <c r="J88" t="s">
-        <v>215</v>
+      <c r="J88" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="K88" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.25">
@@ -4488,7 +4506,7 @@
         <v>96</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -4500,7 +4518,7 @@
         <v>179</v>
       </c>
       <c r="J89" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.25">
@@ -4508,7 +4526,7 @@
         <v>96</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -4520,7 +4538,7 @@
         <v>179</v>
       </c>
       <c r="J90" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.25">
@@ -4528,7 +4546,7 @@
         <v>96</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>234</v>
+        <v>190</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -4540,7 +4558,7 @@
         <v>179</v>
       </c>
       <c r="J91" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.25">
@@ -4548,7 +4566,7 @@
         <v>96</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>236</v>
+        <v>191</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -4560,10 +4578,7 @@
         <v>179</v>
       </c>
       <c r="J92" t="s">
-        <v>237</v>
-      </c>
-      <c r="K92" t="s">
-        <v>409</v>
+        <v>216</v>
       </c>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.25">
@@ -4571,7 +4586,7 @@
         <v>96</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>194</v>
+        <v>234</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -4583,10 +4598,7 @@
         <v>179</v>
       </c>
       <c r="J93" t="s">
-        <v>349</v>
-      </c>
-      <c r="K93" t="s">
-        <v>409</v>
+        <v>235</v>
       </c>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.25">
@@ -4594,7 +4606,7 @@
         <v>96</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>348</v>
+        <v>236</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -4606,7 +4618,7 @@
         <v>179</v>
       </c>
       <c r="J94" t="s">
-        <v>350</v>
+        <v>237</v>
       </c>
       <c r="K94" t="s">
         <v>409</v>
@@ -4617,7 +4629,7 @@
         <v>96</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>251</v>
+        <v>194</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -4629,18 +4641,18 @@
         <v>179</v>
       </c>
       <c r="J95" t="s">
-        <v>252</v>
+        <v>349</v>
       </c>
       <c r="K95" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D96" s="6" t="s">
-        <v>95</v>
+      <c r="D96" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>388</v>
+        <v>348</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -4649,10 +4661,13 @@
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>389</v>
+        <v>179</v>
       </c>
       <c r="J96" t="s">
-        <v>393</v>
+        <v>350</v>
+      </c>
+      <c r="K96" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -4660,7 +4675,7 @@
         <v>96</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>386</v>
+        <v>251</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -4669,18 +4684,21 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>389</v>
+        <v>179</v>
       </c>
       <c r="J97" t="s">
-        <v>394</v>
+        <v>252</v>
+      </c>
+      <c r="K97" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D98" s="5" t="s">
-        <v>96</v>
+      <c r="D98" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -4692,15 +4710,15 @@
         <v>389</v>
       </c>
       <c r="J98" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D99" s="6" t="s">
-        <v>95</v>
+      <c r="D99" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>227</v>
+        <v>386</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -4709,10 +4727,10 @@
         <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J99" t="s">
-        <v>305</v>
+        <v>394</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -4720,7 +4738,7 @@
         <v>96</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>228</v>
+        <v>387</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -4729,24 +4747,18 @@
         <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J100" t="s">
-        <v>229</v>
+        <v>395</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A101">
-        <v>17</v>
-      </c>
-      <c r="B101" t="s">
-        <v>136</v>
-      </c>
       <c r="D101" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F101" s="9" t="s">
-        <v>192</v>
+      <c r="F101" s="2" t="s">
+        <v>227</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -4755,13 +4767,10 @@
         <v>0</v>
       </c>
       <c r="I101" t="s">
-        <v>391</v>
-      </c>
-      <c r="J101" s="10" t="s">
-        <v>306</v>
-      </c>
-      <c r="K101" t="s">
-        <v>409</v>
+        <v>390</v>
+      </c>
+      <c r="J101" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -4769,7 +4778,7 @@
         <v>96</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>193</v>
+        <v>228</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -4778,24 +4787,24 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J102" t="s">
-        <v>359</v>
-      </c>
-      <c r="K102" t="s">
-        <v>409</v>
+        <v>229</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>17</v>
+      </c>
       <c r="B103" t="s">
-        <v>298</v>
+        <v>136</v>
       </c>
       <c r="D103" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>299</v>
+        <v>192</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -4804,18 +4813,21 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>392</v>
-      </c>
-      <c r="J103" t="s">
-        <v>302</v>
+        <v>391</v>
+      </c>
+      <c r="J103" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="K103" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D104" s="6" t="s">
-        <v>95</v>
+      <c r="D104" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>307</v>
+        <v>193</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -4824,21 +4836,24 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J104" t="s">
-        <v>303</v>
+        <v>359</v>
       </c>
       <c r="K104" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D105" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>300</v>
+      <c r="B105" t="s">
+        <v>298</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>299</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -4850,21 +4865,15 @@
         <v>392</v>
       </c>
       <c r="J105" t="s">
-        <v>301</v>
-      </c>
-      <c r="K105" t="s">
-        <v>409</v>
+        <v>302</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
-        <v>177</v>
-      </c>
       <c r="D106" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F106" s="9" t="s">
-        <v>326</v>
+      <c r="F106" s="2" t="s">
+        <v>307</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -4873,18 +4882,21 @@
         <v>0</v>
       </c>
       <c r="I106" t="s">
-        <v>179</v>
-      </c>
-      <c r="J106" s="10" t="s">
-        <v>217</v>
+        <v>392</v>
+      </c>
+      <c r="J106" t="s">
+        <v>303</v>
+      </c>
+      <c r="K106" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D107" s="6" t="s">
-        <v>95</v>
+      <c r="D107" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>330</v>
+        <v>300</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -4893,18 +4905,24 @@
         <v>0</v>
       </c>
       <c r="I107" t="s">
-        <v>179</v>
-      </c>
-      <c r="J107" s="10" t="s">
-        <v>217</v>
+        <v>392</v>
+      </c>
+      <c r="J107" t="s">
+        <v>301</v>
+      </c>
+      <c r="K107" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>177</v>
+      </c>
       <c r="D108" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F108" s="2" t="s">
-        <v>331</v>
+      <c r="F108" s="9" t="s">
+        <v>326</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -4924,7 +4942,7 @@
         <v>95</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -4944,18 +4962,58 @@
         <v>95</v>
       </c>
       <c r="F110" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="I110" t="s">
+        <v>179</v>
+      </c>
+      <c r="J110" s="10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D111" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <v>0</v>
+      </c>
+      <c r="I111" t="s">
+        <v>179</v>
+      </c>
+      <c r="J111" s="10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D112" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F112" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="G110">
-        <v>0</v>
-      </c>
-      <c r="H110">
-        <v>0</v>
-      </c>
-      <c r="I110" t="s">
+      <c r="G112">
+        <v>0</v>
+      </c>
+      <c r="H112">
+        <v>0</v>
+      </c>
+      <c r="I112" t="s">
         <v>374</v>
       </c>
-      <c r="J110" s="2" t="s">
+      <c r="J112" s="2" t="s">
         <v>373</v>
       </c>
     </row>

</xml_diff>

<commit_message>
pair zone verification added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -2269,8 +2269,8 @@
   <dimension ref="A1:K112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G64" sqref="G64"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3875,7 +3875,7 @@
         <v>0</v>
       </c>
       <c r="H60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" t="s">
         <v>172</v>
@@ -4213,7 +4213,7 @@
         <v>430</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -4368,7 +4368,7 @@
         <v>0</v>
       </c>
       <c r="H83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I83" t="s">
         <v>179</v>
@@ -4632,10 +4632,10 @@
         <v>194</v>
       </c>
       <c r="G95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I95" t="s">
         <v>179</v>

</xml_diff>

<commit_message>
list of unequal port configuration parameters values added to isl module
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27960" windowHeight="8925" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27960" windowHeight="8925"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -1742,8 +1742,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,7 +1783,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2298,9 +2298,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F89" sqref="F89"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3793,7 +3793,7 @@
         <v>0</v>
       </c>
       <c r="H55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I55" t="s">
         <v>171</v>
@@ -3833,7 +3833,7 @@
         <v>67</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -4398,7 +4398,7 @@
         <v>0</v>
       </c>
       <c r="H83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I83" t="s">
         <v>179</v>
@@ -4539,7 +4539,7 @@
         <v>181</v>
       </c>
       <c r="G89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89">
         <v>0</v>
@@ -4662,7 +4662,7 @@
         <v>194</v>
       </c>
       <c r="G95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H95">
         <v>0</v>

</xml_diff>

<commit_message>
Device_type take into account for zone verification
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27960" windowHeight="8925"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27960" windowHeight="8925" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -1742,8 +1742,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2298,9 +2298,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K112"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H56" sqref="H56:H107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3618,10 +3618,10 @@
         <v>160</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47" t="s">
         <v>162</v>
@@ -3684,10 +3684,10 @@
         <v>61</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" t="s">
         <v>170</v>
@@ -3704,10 +3704,10 @@
         <v>62</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" t="s">
         <v>170</v>
@@ -3724,10 +3724,10 @@
         <v>63</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52" t="s">
         <v>170</v>
@@ -3744,10 +3744,10 @@
         <v>65</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" t="s">
         <v>170</v>
@@ -3764,10 +3764,10 @@
         <v>64</v>
       </c>
       <c r="G54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I54" t="s">
         <v>170</v>
@@ -3793,7 +3793,7 @@
         <v>0</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" t="s">
         <v>171</v>
@@ -3813,7 +3813,7 @@
         <v>0</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" t="s">
         <v>171</v>
@@ -3836,7 +3836,7 @@
         <v>1</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57" t="s">
         <v>171</v>
@@ -3853,10 +3853,10 @@
         <v>68</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I58" t="s">
         <v>171</v>
@@ -3873,10 +3873,10 @@
         <v>291</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59" t="s">
         <v>171</v>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" t="s">
         <v>172</v>
@@ -3948,7 +3948,7 @@
         <v>0</v>
       </c>
       <c r="H62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62" t="s">
         <v>172</v>
@@ -4100,10 +4100,10 @@
         <v>427</v>
       </c>
       <c r="G69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I69" t="s">
         <v>172</v>
@@ -4123,10 +4123,10 @@
         <v>101</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I70" t="s">
         <v>172</v>
@@ -4143,10 +4143,10 @@
         <v>102</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I71" t="s">
         <v>172</v>
@@ -4163,10 +4163,10 @@
         <v>103</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I72" t="s">
         <v>172</v>
@@ -4183,10 +4183,10 @@
         <v>104</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I73" t="s">
         <v>172</v>
@@ -4203,10 +4203,10 @@
         <v>105</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I74" t="s">
         <v>172</v>
@@ -4223,10 +4223,10 @@
         <v>106</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I75" t="s">
         <v>172</v>
@@ -4243,10 +4243,10 @@
         <v>430</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I76" t="s">
         <v>172</v>
@@ -4266,10 +4266,10 @@
         <v>274</v>
       </c>
       <c r="G77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I77" t="s">
         <v>172</v>
@@ -4289,10 +4289,10 @@
         <v>164</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I78" t="s">
         <v>172</v>
@@ -4332,10 +4332,10 @@
         <v>167</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I80" t="s">
         <v>173</v>
@@ -4352,10 +4352,10 @@
         <v>168</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I81" t="s">
         <v>166</v>
@@ -4372,10 +4372,10 @@
         <v>169</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I82" t="s">
         <v>166</v>
@@ -4398,7 +4398,7 @@
         <v>0</v>
       </c>
       <c r="H83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I83" t="s">
         <v>179</v>
@@ -4441,10 +4441,10 @@
         <v>189</v>
       </c>
       <c r="G85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I85" t="s">
         <v>179</v>
@@ -4470,7 +4470,7 @@
         <v>0</v>
       </c>
       <c r="H86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I86" t="s">
         <v>179</v>
@@ -4493,7 +4493,7 @@
         <v>0</v>
       </c>
       <c r="H87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I87" t="s">
         <v>179</v>
@@ -4519,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="H88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I88" t="s">
         <v>179</v>
@@ -4539,10 +4539,10 @@
         <v>181</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I89" t="s">
         <v>179</v>
@@ -4559,10 +4559,10 @@
         <v>182</v>
       </c>
       <c r="G90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I90" t="s">
         <v>179</v>
@@ -4579,10 +4579,10 @@
         <v>190</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I91" t="s">
         <v>179</v>
@@ -4599,10 +4599,10 @@
         <v>191</v>
       </c>
       <c r="G92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I92" t="s">
         <v>179</v>
@@ -4619,10 +4619,10 @@
         <v>234</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I93" t="s">
         <v>179</v>
@@ -4639,10 +4639,10 @@
         <v>236</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I94" t="s">
         <v>179</v>
@@ -4662,10 +4662,10 @@
         <v>194</v>
       </c>
       <c r="G95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I95" t="s">
         <v>179</v>
@@ -4685,10 +4685,10 @@
         <v>348</v>
       </c>
       <c r="G96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I96" t="s">
         <v>179</v>
@@ -4708,10 +4708,10 @@
         <v>251</v>
       </c>
       <c r="G97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I97" t="s">
         <v>179</v>
@@ -4751,10 +4751,10 @@
         <v>386</v>
       </c>
       <c r="G99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I99" t="s">
         <v>389</v>
@@ -4771,10 +4771,10 @@
         <v>387</v>
       </c>
       <c r="G100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I100" t="s">
         <v>389</v>
@@ -4811,10 +4811,10 @@
         <v>228</v>
       </c>
       <c r="G102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I102" t="s">
         <v>390</v>
@@ -4840,7 +4840,7 @@
         <v>0</v>
       </c>
       <c r="H103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I103" t="s">
         <v>391</v>
@@ -4860,10 +4860,10 @@
         <v>193</v>
       </c>
       <c r="G104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I104" t="s">
         <v>391</v>
@@ -4909,7 +4909,7 @@
         <v>0</v>
       </c>
       <c r="H106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I106" t="s">
         <v>392</v>
@@ -4929,10 +4929,10 @@
         <v>300</v>
       </c>
       <c r="G107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I107" t="s">
         <v>392</v>

</xml_diff>

<commit_message>
sensor aggregation. switches from one chassis are groped together to avoid duplication
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1742,8 +1742,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,7 +1783,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2298,9 +2298,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H56" sqref="H56:H107"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3618,10 +3618,10 @@
         <v>160</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47" t="s">
         <v>162</v>
@@ -3684,10 +3684,10 @@
         <v>61</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" t="s">
         <v>170</v>
@@ -3704,10 +3704,10 @@
         <v>62</v>
       </c>
       <c r="G51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" t="s">
         <v>170</v>
@@ -3724,10 +3724,10 @@
         <v>63</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" t="s">
         <v>170</v>
@@ -3744,10 +3744,10 @@
         <v>65</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" t="s">
         <v>170</v>
@@ -3764,10 +3764,10 @@
         <v>64</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" t="s">
         <v>170</v>
@@ -3813,7 +3813,7 @@
         <v>0</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" t="s">
         <v>171</v>
@@ -3833,10 +3833,10 @@
         <v>67</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="s">
         <v>171</v>
@@ -3853,10 +3853,10 @@
         <v>68</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58" t="s">
         <v>171</v>
@@ -3873,10 +3873,10 @@
         <v>291</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59" t="s">
         <v>171</v>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
       <c r="H61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" t="s">
         <v>172</v>
@@ -3948,7 +3948,7 @@
         <v>0</v>
       </c>
       <c r="H62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I62" t="s">
         <v>172</v>
@@ -4100,10 +4100,10 @@
         <v>427</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69" t="s">
         <v>172</v>
@@ -4123,10 +4123,10 @@
         <v>101</v>
       </c>
       <c r="G70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I70" t="s">
         <v>172</v>
@@ -4143,10 +4143,10 @@
         <v>102</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I71" t="s">
         <v>172</v>
@@ -4163,10 +4163,10 @@
         <v>103</v>
       </c>
       <c r="G72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I72" t="s">
         <v>172</v>
@@ -4183,10 +4183,10 @@
         <v>104</v>
       </c>
       <c r="G73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I73" t="s">
         <v>172</v>
@@ -4203,10 +4203,10 @@
         <v>105</v>
       </c>
       <c r="G74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I74" t="s">
         <v>172</v>
@@ -4223,10 +4223,10 @@
         <v>106</v>
       </c>
       <c r="G75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I75" t="s">
         <v>172</v>
@@ -4243,10 +4243,10 @@
         <v>430</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I76" t="s">
         <v>172</v>
@@ -4266,10 +4266,10 @@
         <v>274</v>
       </c>
       <c r="G77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I77" t="s">
         <v>172</v>
@@ -4289,10 +4289,10 @@
         <v>164</v>
       </c>
       <c r="G78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I78" t="s">
         <v>172</v>
@@ -4332,10 +4332,10 @@
         <v>167</v>
       </c>
       <c r="G80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I80" t="s">
         <v>173</v>
@@ -4352,10 +4352,10 @@
         <v>168</v>
       </c>
       <c r="G81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I81" t="s">
         <v>166</v>
@@ -4372,10 +4372,10 @@
         <v>169</v>
       </c>
       <c r="G82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I82" t="s">
         <v>166</v>
@@ -4398,7 +4398,7 @@
         <v>0</v>
       </c>
       <c r="H83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I83" t="s">
         <v>179</v>
@@ -4441,10 +4441,10 @@
         <v>189</v>
       </c>
       <c r="G85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I85" t="s">
         <v>179</v>
@@ -4470,7 +4470,7 @@
         <v>0</v>
       </c>
       <c r="H86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I86" t="s">
         <v>179</v>
@@ -4493,7 +4493,7 @@
         <v>0</v>
       </c>
       <c r="H87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I87" t="s">
         <v>179</v>
@@ -4519,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="H88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I88" t="s">
         <v>179</v>
@@ -4539,10 +4539,10 @@
         <v>181</v>
       </c>
       <c r="G89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I89" t="s">
         <v>179</v>
@@ -4559,10 +4559,10 @@
         <v>182</v>
       </c>
       <c r="G90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I90" t="s">
         <v>179</v>
@@ -4579,10 +4579,10 @@
         <v>190</v>
       </c>
       <c r="G91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I91" t="s">
         <v>179</v>
@@ -4599,10 +4599,10 @@
         <v>191</v>
       </c>
       <c r="G92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I92" t="s">
         <v>179</v>
@@ -4619,10 +4619,10 @@
         <v>234</v>
       </c>
       <c r="G93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I93" t="s">
         <v>179</v>
@@ -4639,10 +4639,10 @@
         <v>236</v>
       </c>
       <c r="G94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I94" t="s">
         <v>179</v>
@@ -4662,10 +4662,10 @@
         <v>194</v>
       </c>
       <c r="G95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I95" t="s">
         <v>179</v>
@@ -4685,10 +4685,10 @@
         <v>348</v>
       </c>
       <c r="G96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96" t="s">
         <v>179</v>
@@ -4708,10 +4708,10 @@
         <v>251</v>
       </c>
       <c r="G97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I97" t="s">
         <v>179</v>
@@ -4751,10 +4751,10 @@
         <v>386</v>
       </c>
       <c r="G99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I99" t="s">
         <v>389</v>
@@ -4771,10 +4771,10 @@
         <v>387</v>
       </c>
       <c r="G100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I100" t="s">
         <v>389</v>
@@ -4794,7 +4794,7 @@
         <v>0</v>
       </c>
       <c r="H101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I101" t="s">
         <v>390</v>
@@ -4814,7 +4814,7 @@
         <v>1</v>
       </c>
       <c r="H102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I102" t="s">
         <v>390</v>
@@ -4840,7 +4840,7 @@
         <v>0</v>
       </c>
       <c r="H103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I103" t="s">
         <v>391</v>
@@ -4860,10 +4860,10 @@
         <v>193</v>
       </c>
       <c r="G104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I104" t="s">
         <v>391</v>
@@ -4909,7 +4909,7 @@
         <v>0</v>
       </c>
       <c r="H106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I106" t="s">
         <v>392</v>
@@ -4929,10 +4929,10 @@
         <v>300</v>
       </c>
       <c r="G107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I107" t="s">
         <v>392</v>

</xml_diff>

<commit_message>
trunk area slave links device information added, npiv link nymbering added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="440">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1327,6 +1327,18 @@
   </si>
   <si>
     <t>C:\Users\vlasenko\Documents\06.CONFIGS\Sibintek\MAY21\blade</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\MegafonMSK\SAN Assessment\MAY21</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\MegafonMSK\APR21\ssave\supportsave-20-05-2021</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\MegafonMSK\APR21\showall-all-encl</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\MegafonMSK\APR21\3PAR</t>
   </si>
 </sst>
 </file>
@@ -1740,10 +1752,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AJ10"/>
+  <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,43 +1763,43 @@
     <col min="1" max="3" width="29.7109375" customWidth="1"/>
     <col min="4" max="4" width="80.140625" customWidth="1"/>
     <col min="5" max="5" width="35.7109375" customWidth="1"/>
-    <col min="6" max="6" width="122.7109375" customWidth="1"/>
-    <col min="7" max="7" width="48.42578125" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" customWidth="1"/>
-    <col min="9" max="9" width="80.140625" customWidth="1"/>
-    <col min="10" max="10" width="68.5703125" customWidth="1"/>
-    <col min="11" max="11" width="48.7109375" customWidth="1"/>
-    <col min="12" max="12" width="62" customWidth="1"/>
-    <col min="13" max="15" width="89.5703125" customWidth="1"/>
-    <col min="16" max="16" width="69.85546875" customWidth="1"/>
-    <col min="17" max="17" width="52.140625" customWidth="1"/>
-    <col min="18" max="18" width="73.140625" customWidth="1"/>
-    <col min="19" max="19" width="29.7109375" customWidth="1"/>
-    <col min="20" max="21" width="76" customWidth="1"/>
-    <col min="22" max="22" width="72.28515625" customWidth="1"/>
-    <col min="23" max="23" width="61.7109375" customWidth="1"/>
-    <col min="24" max="24" width="60" customWidth="1"/>
-    <col min="25" max="25" width="38.140625" customWidth="1"/>
-    <col min="26" max="26" width="69" customWidth="1"/>
-    <col min="27" max="27" width="72.42578125" customWidth="1"/>
-    <col min="28" max="28" width="111.5703125" customWidth="1"/>
-    <col min="29" max="29" width="72.5703125" customWidth="1"/>
-    <col min="30" max="30" width="86.85546875" customWidth="1"/>
-    <col min="31" max="32" width="64.7109375" customWidth="1"/>
-    <col min="33" max="33" width="54.5703125" customWidth="1"/>
-    <col min="34" max="34" width="75.42578125" customWidth="1"/>
-    <col min="35" max="35" width="58.140625" customWidth="1"/>
+    <col min="6" max="7" width="122.7109375" customWidth="1"/>
+    <col min="8" max="8" width="48.42578125" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" customWidth="1"/>
+    <col min="10" max="10" width="80.140625" customWidth="1"/>
+    <col min="11" max="11" width="68.5703125" customWidth="1"/>
+    <col min="12" max="12" width="48.7109375" customWidth="1"/>
+    <col min="13" max="13" width="62" customWidth="1"/>
+    <col min="14" max="16" width="89.5703125" customWidth="1"/>
+    <col min="17" max="17" width="69.85546875" customWidth="1"/>
+    <col min="18" max="18" width="52.140625" customWidth="1"/>
+    <col min="19" max="19" width="73.140625" customWidth="1"/>
+    <col min="20" max="20" width="29.7109375" customWidth="1"/>
+    <col min="21" max="22" width="76" customWidth="1"/>
+    <col min="23" max="23" width="72.28515625" customWidth="1"/>
+    <col min="24" max="24" width="61.7109375" customWidth="1"/>
+    <col min="25" max="25" width="60" customWidth="1"/>
+    <col min="26" max="26" width="38.140625" customWidth="1"/>
+    <col min="27" max="27" width="69" customWidth="1"/>
+    <col min="28" max="28" width="72.42578125" customWidth="1"/>
+    <col min="29" max="29" width="111.5703125" customWidth="1"/>
+    <col min="30" max="30" width="72.5703125" customWidth="1"/>
+    <col min="31" max="31" width="86.85546875" customWidth="1"/>
+    <col min="32" max="33" width="64.7109375" customWidth="1"/>
+    <col min="34" max="34" width="54.5703125" customWidth="1"/>
+    <col min="35" max="35" width="75.42578125" customWidth="1"/>
+    <col min="36" max="36" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
@@ -1804,28 +1816,28 @@
         <v>404</v>
       </c>
       <c r="G2" t="s">
+        <v>404</v>
+      </c>
+      <c r="H2" t="s">
         <v>396</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>369</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>336</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>323</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>316</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>313</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>309</v>
-      </c>
-      <c r="N2" t="s">
-        <v>317</v>
       </c>
       <c r="O2" t="s">
         <v>317</v>
@@ -1834,67 +1846,70 @@
         <v>317</v>
       </c>
       <c r="Q2" t="s">
+        <v>317</v>
+      </c>
+      <c r="R2" t="s">
         <v>279</v>
-      </c>
-      <c r="R2" t="s">
-        <v>275</v>
       </c>
       <c r="S2" t="s">
         <v>275</v>
       </c>
       <c r="T2" t="s">
-        <v>257</v>
+        <v>275</v>
       </c>
       <c r="U2" t="s">
         <v>257</v>
       </c>
       <c r="V2" t="s">
+        <v>257</v>
+      </c>
+      <c r="W2" t="s">
         <v>239</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>233</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>188</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>187</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>154</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>110</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>97</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>83</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>283</v>
       </c>
@@ -1908,47 +1923,50 @@
         <v>44294</v>
       </c>
       <c r="F3" s="12">
+        <v>44343</v>
+      </c>
+      <c r="G3" s="12">
         <v>44292</v>
       </c>
-      <c r="G3" s="12">
+      <c r="H3" s="12">
         <v>29681</v>
       </c>
-      <c r="H3" s="12">
+      <c r="I3" s="12">
         <v>44286</v>
       </c>
-      <c r="I3" s="12">
+      <c r="J3" s="12">
         <v>44260</v>
       </c>
-      <c r="J3" s="12">
+      <c r="K3" s="12">
         <v>44244</v>
       </c>
-      <c r="K3" s="12">
+      <c r="L3" s="12">
         <v>44245</v>
       </c>
-      <c r="L3" s="12">
+      <c r="M3" s="12">
         <v>44223</v>
       </c>
-      <c r="M3" s="12">
+      <c r="N3" s="12">
         <v>44209</v>
       </c>
-      <c r="N3" s="12">
+      <c r="O3" s="12">
         <v>44253</v>
       </c>
-      <c r="O3" s="12">
+      <c r="P3" s="12">
         <v>44237</v>
       </c>
-      <c r="R3" s="12">
+      <c r="S3" s="12">
         <v>44181</v>
       </c>
-      <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK3" s="1"/>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>284</v>
       </c>
@@ -1968,41 +1986,44 @@
         <v>327</v>
       </c>
       <c r="H4" t="s">
+        <v>327</v>
+      </c>
+      <c r="I4" t="s">
         <v>370</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>327</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>322</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>327</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>327</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>333</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>322</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>282</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>281</v>
       </c>
-      <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK4" s="1"/>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
@@ -2016,100 +2037,103 @@
         <v>412</v>
       </c>
       <c r="F5" t="s">
+        <v>436</v>
+      </c>
+      <c r="G5" t="s">
         <v>406</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>397</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>371</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>337</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>324</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>329</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>314</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>308</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>334</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>320</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>318</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>280</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>285</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>277</v>
-      </c>
-      <c r="T5" t="s">
-        <v>258</v>
       </c>
       <c r="U5" t="s">
         <v>258</v>
       </c>
       <c r="V5" t="s">
+        <v>258</v>
+      </c>
+      <c r="W5" t="s">
         <v>241</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>232</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>222</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>186</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>156</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>112</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>98</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>85</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>1</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>74</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>72</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>4</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>25</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>60</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
@@ -2123,166 +2147,175 @@
         <v>413</v>
       </c>
       <c r="F6" t="s">
+        <v>437</v>
+      </c>
+      <c r="G6" t="s">
         <v>405</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>398</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>372</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>358</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>325</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>328</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>315</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>310</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>335</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>321</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>319</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>278</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>286</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>276</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>271</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>259</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>240</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>230</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>221</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>185</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>155</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>111</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>107</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>84</v>
       </c>
-      <c r="AD6" t="s">
-        <v>0</v>
-      </c>
       <c r="AE6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="s">
         <v>73</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>71</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>3</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>24</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>59</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
       <c r="C7" t="s">
         <v>435</v>
       </c>
-      <c r="G7" t="s">
+      <c r="F7" t="s">
+        <v>438</v>
+      </c>
+      <c r="H7" t="s">
         <v>399</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>338</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>311</v>
-      </c>
-      <c r="T7" t="s">
-        <v>260</v>
       </c>
       <c r="U7" t="s">
         <v>260</v>
       </c>
-      <c r="W7" t="s">
+      <c r="V7" t="s">
+        <v>260</v>
+      </c>
+      <c r="X7" t="s">
         <v>231</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>157</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>108</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>87</v>
       </c>
-      <c r="AF7" t="s">
+      <c r="AG7" t="s">
         <v>99</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>261</v>
       </c>
       <c r="D8" t="s">
         <v>426</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>339</v>
-      </c>
-      <c r="T8" t="s">
-        <v>262</v>
       </c>
       <c r="U8" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="V8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>360</v>
       </c>
-      <c r="G9" t="s">
+      <c r="F9" t="s">
+        <v>439</v>
+      </c>
+      <c r="H9" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>238</v>
       </c>
@@ -2299,8 +2332,8 @@
   <dimension ref="A1:K112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3684,7 +3717,7 @@
         <v>61</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -3704,7 +3737,7 @@
         <v>62</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -4794,7 +4827,7 @@
         <v>0</v>
       </c>
       <c r="H101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I101" t="s">
         <v>390</v>
@@ -4811,7 +4844,7 @@
         <v>228</v>
       </c>
       <c r="G102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H102">
         <v>0</v>

</xml_diff>

<commit_message>
NPIV devices and statistics
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27960" windowHeight="8925" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27960" windowHeight="10560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$K$112</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$K$117</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="449">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -519,9 +519,6 @@
     <t>analysis_err_sfp_cfg</t>
   </si>
   <si>
-    <t>DATA ANALYSIS 5. PORT ERRORS, TRANSCEIVER SUPPORT, PORT CONFIGURATION</t>
-  </si>
-  <si>
     <t>Ошибки</t>
   </si>
   <si>
@@ -1188,18 +1185,6 @@
     <t>storage_host_aggregated</t>
   </si>
   <si>
-    <t>DATA ANALYSIS 7. STORAGE HOST PRESENTATION</t>
-  </si>
-  <si>
-    <t>DATA ANALYSIS 8. SENSOR READINGS</t>
-  </si>
-  <si>
-    <t>DATA ANALYSIS 9. FABRIC STATISTICS</t>
-  </si>
-  <si>
-    <t>DATA ANALYSIS 10. RASLOG</t>
-  </si>
-  <si>
     <t>Storage Host presentation</t>
   </si>
   <si>
@@ -1339,6 +1324,48 @@
   </si>
   <si>
     <t>C:\Users\vlasenko\Documents\06.CONFIGS\MegafonMSK\APR21\3PAR</t>
+  </si>
+  <si>
+    <t>NPIV_statistics</t>
+  </si>
+  <si>
+    <t>Статистика_NPIV</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 7. ZONING CONFIGURATION</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 8. STORAGE HOST PRESENTATION</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 9. SENSOR READINGS</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 10. FABRIC STATISTICS</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 11. RASLOG</t>
+  </si>
+  <si>
+    <t>Статистическая информация о портах NPIV</t>
+  </si>
+  <si>
+    <t>NPIV_порты</t>
+  </si>
+  <si>
+    <t>NPIV statistics</t>
+  </si>
+  <si>
+    <t>NPIV ports</t>
+  </si>
+  <si>
+    <t>MAPS</t>
+  </si>
+  <si>
+    <t>Настройки и сообщения службы MAPS</t>
+  </si>
+  <si>
+    <t>NPIV_</t>
   </si>
 </sst>
 </file>
@@ -1754,8 +1781,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1795,7 +1822,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1804,76 +1831,76 @@
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E2" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="F2" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="G2" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="H2" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="I2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L2" t="s">
+        <v>315</v>
+      </c>
+      <c r="M2" t="s">
+        <v>312</v>
+      </c>
+      <c r="N2" t="s">
+        <v>308</v>
+      </c>
+      <c r="O2" t="s">
         <v>316</v>
       </c>
-      <c r="M2" t="s">
-        <v>313</v>
-      </c>
-      <c r="N2" t="s">
-        <v>309</v>
-      </c>
-      <c r="O2" t="s">
-        <v>317</v>
-      </c>
       <c r="P2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="R2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="S2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="T2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="U2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="V2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="W2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="X2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Y2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="Z2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AA2" t="s">
         <v>154</v>
@@ -1911,7 +1938,7 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C3" s="12">
         <v>44330</v>
@@ -1968,52 +1995,52 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D4" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="E4" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="F4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="N4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="P4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="S4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="T4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
@@ -2028,76 +2055,76 @@
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="D5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="E5" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="F5" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G5" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="H5" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="M5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="N5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="P5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="R5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="S5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="U5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="V5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="W5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="X5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Y5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="Z5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AA5" t="s">
         <v>156</v>
@@ -2138,76 +2165,76 @@
         <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="D6" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="E6" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="F6" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="G6" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="H6" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="I6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="M6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="N6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="O6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="R6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="S6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="T6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="U6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="V6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="W6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="X6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Y6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="Z6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AA6" t="s">
         <v>155</v>
@@ -2248,28 +2275,28 @@
         <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="F7" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="H7" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="J7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="N7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="V7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="X7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AA7" t="s">
         <v>157</v>
@@ -2289,35 +2316,35 @@
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="D8" t="s">
+        <v>421</v>
+      </c>
+      <c r="J8" t="s">
+        <v>338</v>
+      </c>
+      <c r="U8" t="s">
         <v>261</v>
       </c>
-      <c r="D8" t="s">
-        <v>426</v>
-      </c>
-      <c r="J8" t="s">
-        <v>339</v>
-      </c>
-      <c r="U8" t="s">
-        <v>262</v>
-      </c>
       <c r="V8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F9" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="H9" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2329,11 +2356,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K112"/>
+  <dimension ref="A1:K117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2377,10 +2404,10 @@
         <v>149</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K1" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2409,7 +2436,7 @@
         <v>152</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2438,7 +2465,7 @@
         <v>152</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2449,7 +2476,7 @@
         <v>115</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>94</v>
@@ -2470,7 +2497,7 @@
         <v>141</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2481,7 +2508,7 @@
         <v>117</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>94</v>
@@ -2502,7 +2529,7 @@
         <v>150</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2513,7 +2540,7 @@
         <v>117</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>94</v>
@@ -2534,7 +2561,7 @@
         <v>150</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2545,7 +2572,7 @@
         <v>113</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>94</v>
@@ -2566,7 +2593,7 @@
         <v>151</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2598,7 +2625,7 @@
         <v>147</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2630,7 +2657,7 @@
         <v>147</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2662,7 +2689,7 @@
         <v>145</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2694,7 +2721,7 @@
         <v>146</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2726,7 +2753,7 @@
         <v>146</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2758,7 +2785,7 @@
         <v>143</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2790,7 +2817,7 @@
         <v>143</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2822,7 +2849,7 @@
         <v>143</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2854,7 +2881,7 @@
         <v>144</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2886,7 +2913,7 @@
         <v>144</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -2918,7 +2945,7 @@
         <v>144</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2950,7 +2977,7 @@
         <v>142</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2979,7 +3006,7 @@
         <v>142</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -3008,7 +3035,7 @@
         <v>142</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -3037,7 +3064,7 @@
         <v>142</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -3063,7 +3090,7 @@
         <v>142</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -3089,7 +3116,7 @@
         <v>142</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -3118,7 +3145,7 @@
         <v>148</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -3144,7 +3171,7 @@
         <v>148</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -3170,7 +3197,7 @@
         <v>148</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -3196,7 +3223,7 @@
         <v>148</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -3222,7 +3249,7 @@
         <v>148</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -3236,7 +3263,7 @@
         <v>94</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -3248,7 +3275,7 @@
         <v>148</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -3262,7 +3289,7 @@
         <v>94</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -3274,59 +3301,59 @@
         <v>148</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>223</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>224</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F32" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32" t="s">
         <v>224</v>
       </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32" t="s">
-        <v>225</v>
-      </c>
       <c r="J32" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>296</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>297</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F33" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33" t="s">
         <v>293</v>
       </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="J33" s="10" t="s">
         <v>294</v>
-      </c>
-      <c r="J33" s="10" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -3352,10 +3379,10 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3378,10 +3405,10 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -3404,22 +3431,22 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -3428,22 +3455,22 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -3452,46 +3479,46 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F39" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>362</v>
+      </c>
+      <c r="J39" s="10" t="s">
         <v>367</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39" t="s">
-        <v>363</v>
-      </c>
-      <c r="J39" s="10" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -3500,46 +3527,46 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F41" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41" t="s">
         <v>362</v>
       </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41" t="s">
-        <v>363</v>
-      </c>
       <c r="J41" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -3548,10 +3575,10 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -3577,7 +3604,7 @@
         <v>158</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -3597,7 +3624,7 @@
         <v>158</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3617,7 +3644,7 @@
         <v>158</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -3640,7 +3667,7 @@
         <v>162</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -3660,7 +3687,7 @@
         <v>162</v>
       </c>
       <c r="J47" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -3683,10 +3710,10 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -3703,10 +3730,10 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -3717,16 +3744,16 @@
         <v>61</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H50">
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J50" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -3737,16 +3764,16 @@
         <v>62</v>
       </c>
       <c r="G51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H51">
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J51" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -3763,10 +3790,10 @@
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J52" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -3783,10 +3810,10 @@
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J53" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -3803,44 +3830,44 @@
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J54" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="D55" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55" t="s">
+        <v>169</v>
+      </c>
+      <c r="J55" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56">
         <v>18</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>138</v>
       </c>
-      <c r="D55" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
-      <c r="I55" t="s">
-        <v>171</v>
-      </c>
-      <c r="J55" s="10" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D56" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>287</v>
+        <v>69</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -3849,21 +3876,18 @@
         <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J56" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="K56" t="s">
-        <v>409</v>
-      </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D57" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>67</v>
+      <c r="D57" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>286</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -3872,10 +3896,13 @@
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>171</v>
-      </c>
-      <c r="J57" t="s">
-        <v>207</v>
+        <v>170</v>
+      </c>
+      <c r="J57" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="K57" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -3883,7 +3910,7 @@
         <v>96</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -3892,10 +3919,10 @@
         <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J58" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -3903,56 +3930,56 @@
         <v>96</v>
       </c>
       <c r="F59" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59" t="s">
+        <v>170</v>
+      </c>
+      <c r="J59" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D60" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60" t="s">
+        <v>170</v>
+      </c>
+      <c r="J60" t="s">
         <v>291</v>
       </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59" t="s">
-        <v>171</v>
-      </c>
-      <c r="J59" t="s">
-        <v>292</v>
-      </c>
-      <c r="K59" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60">
+      <c r="K60" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>20</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>131</v>
       </c>
-      <c r="D60" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G60">
-        <v>0</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-      <c r="I60" t="s">
-        <v>172</v>
-      </c>
-      <c r="J60" s="10" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D61" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>431</v>
+        <v>90</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -3961,13 +3988,10 @@
         <v>0</v>
       </c>
       <c r="I61" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>428</v>
-      </c>
-      <c r="K61" t="s">
-        <v>409</v>
+        <v>268</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -3975,7 +3999,7 @@
         <v>95</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>272</v>
+        <v>426</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -3984,21 +4008,21 @@
         <v>0</v>
       </c>
       <c r="I62" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>273</v>
+        <v>423</v>
       </c>
       <c r="K62" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D63" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F63" s="2" t="s">
-        <v>244</v>
+      <c r="F63" s="9" t="s">
+        <v>271</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -4007,10 +4031,13 @@
         <v>0</v>
       </c>
       <c r="I63" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>341</v>
+        <v>272</v>
+      </c>
+      <c r="K63" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -4018,51 +4045,48 @@
         <v>95</v>
       </c>
       <c r="F64" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64" t="s">
+        <v>171</v>
+      </c>
+      <c r="J64" s="10" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D65" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65" t="s">
+        <v>171</v>
+      </c>
+      <c r="J65" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="G64">
-        <v>0</v>
-      </c>
-      <c r="H64">
-        <v>0</v>
-      </c>
-      <c r="I64" t="s">
-        <v>172</v>
-      </c>
-      <c r="J64" s="10" t="s">
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D66" s="11" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D65" s="11" t="s">
+      <c r="F66" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="F65" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="G65">
-        <v>0</v>
-      </c>
-      <c r="H65">
-        <v>0</v>
-      </c>
-      <c r="I65" t="s">
-        <v>172</v>
-      </c>
-      <c r="J65" s="10" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>133</v>
-      </c>
-      <c r="D66" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F66" s="8" t="s">
-        <v>109</v>
-      </c>
       <c r="G66">
         <v>0</v>
       </c>
@@ -4070,24 +4094,21 @@
         <v>0</v>
       </c>
       <c r="I66" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>385</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>119</v>
-      </c>
-      <c r="C67" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F67" s="7" t="s">
-        <v>93</v>
+      <c r="F67" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -4096,18 +4117,24 @@
         <v>0</v>
       </c>
       <c r="I67" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>340</v>
+        <v>384</v>
       </c>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68" t="s">
+        <v>132</v>
+      </c>
       <c r="D68" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>312</v>
+        <v>93</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -4116,21 +4143,18 @@
         <v>0</v>
       </c>
       <c r="I68" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>134</v>
-      </c>
-      <c r="D69" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>427</v>
+      <c r="D69" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>311</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -4139,21 +4163,21 @@
         <v>0</v>
       </c>
       <c r="I69" t="s">
-        <v>172</v>
-      </c>
-      <c r="J69" t="s">
-        <v>199</v>
+        <v>171</v>
+      </c>
+      <c r="J69" s="10" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>101</v>
+        <v>422</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -4162,18 +4186,21 @@
         <v>0</v>
       </c>
       <c r="I70" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J70" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>135</v>
+      </c>
       <c r="D71" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -4182,10 +4209,10 @@
         <v>0</v>
       </c>
       <c r="I71" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J71" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.25">
@@ -4193,7 +4220,7 @@
         <v>96</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -4202,10 +4229,10 @@
         <v>0</v>
       </c>
       <c r="I72" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J72" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.25">
@@ -4213,7 +4240,7 @@
         <v>96</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -4222,10 +4249,10 @@
         <v>0</v>
       </c>
       <c r="I73" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J73" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.25">
@@ -4233,7 +4260,7 @@
         <v>96</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -4242,10 +4269,10 @@
         <v>0</v>
       </c>
       <c r="I74" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J74" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.25">
@@ -4253,7 +4280,7 @@
         <v>96</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -4262,10 +4289,10 @@
         <v>0</v>
       </c>
       <c r="I75" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J75" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
@@ -4273,7 +4300,7 @@
         <v>96</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>430</v>
+        <v>106</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -4282,13 +4309,10 @@
         <v>0</v>
       </c>
       <c r="I76" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J76" t="s">
-        <v>429</v>
-      </c>
-      <c r="K76" t="s">
-        <v>409</v>
+        <v>211</v>
       </c>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.25">
@@ -4296,7 +4320,7 @@
         <v>96</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>274</v>
+        <v>425</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -4305,13 +4329,13 @@
         <v>0</v>
       </c>
       <c r="I77" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J77" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="K77" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.25">
@@ -4319,349 +4343,358 @@
         <v>96</v>
       </c>
       <c r="F78" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78" t="s">
+        <v>171</v>
+      </c>
+      <c r="J78" t="s">
+        <v>417</v>
+      </c>
+      <c r="K78" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D79" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F79" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="G78">
-        <v>0</v>
-      </c>
-      <c r="H78">
-        <v>0</v>
-      </c>
-      <c r="I78" t="s">
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79" t="s">
+        <v>171</v>
+      </c>
+      <c r="J79" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>165</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80" t="s">
         <v>172</v>
       </c>
-      <c r="J78" t="s">
+      <c r="J80" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D81" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81" t="s">
+        <v>172</v>
+      </c>
+      <c r="J81" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D82" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82" t="s">
+        <v>172</v>
+      </c>
+      <c r="J82" t="s">
+        <v>444</v>
+      </c>
+      <c r="K82" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D83" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83" t="s">
+        <v>172</v>
+      </c>
+      <c r="J83" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>165</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F79" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="G79">
-        <v>0</v>
-      </c>
-      <c r="H79">
-        <v>0</v>
-      </c>
-      <c r="I79" t="s">
-        <v>173</v>
-      </c>
-      <c r="J79" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D80" s="5" t="s">
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D84" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="F84" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-      <c r="H80">
-        <v>0</v>
-      </c>
-      <c r="I80" t="s">
-        <v>173</v>
-      </c>
-      <c r="J80" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D81" s="5" t="s">
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84" t="s">
+        <v>172</v>
+      </c>
+      <c r="J84" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D85" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F85" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="G81">
-        <v>0</v>
-      </c>
-      <c r="H81">
-        <v>0</v>
-      </c>
-      <c r="I81" t="s">
-        <v>166</v>
-      </c>
-      <c r="J81" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D82" s="5" t="s">
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85" t="s">
+        <v>172</v>
+      </c>
+      <c r="J85" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D86" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F82" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="G82">
-        <v>0</v>
-      </c>
-      <c r="H82">
-        <v>0</v>
-      </c>
-      <c r="I82" t="s">
-        <v>166</v>
-      </c>
-      <c r="J82" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
-        <v>177</v>
-      </c>
-      <c r="D83" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="G83">
-        <v>0</v>
-      </c>
-      <c r="H83">
-        <v>0</v>
-      </c>
-      <c r="I83" t="s">
-        <v>179</v>
-      </c>
-      <c r="J83" s="10" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>254</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="G84">
-        <v>0</v>
-      </c>
-      <c r="H84">
-        <v>0</v>
-      </c>
-      <c r="I84" t="s">
-        <v>179</v>
-      </c>
-      <c r="J84" s="10" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
-        <v>256</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F85" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="G85">
-        <v>0</v>
-      </c>
-      <c r="H85">
-        <v>0</v>
-      </c>
-      <c r="I85" t="s">
-        <v>179</v>
-      </c>
-      <c r="J85" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="K85" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>255</v>
-      </c>
-      <c r="D86" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F86" s="9" t="s">
-        <v>218</v>
+      <c r="F86" s="2" t="s">
+        <v>443</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I86" t="s">
-        <v>179</v>
-      </c>
-      <c r="J86" s="10" t="s">
-        <v>347</v>
-      </c>
-      <c r="K86" t="s">
-        <v>409</v>
+        <v>172</v>
+      </c>
+      <c r="J86" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D87" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F87" s="9" t="s">
-        <v>342</v>
+      <c r="D87" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>436</v>
       </c>
       <c r="G87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H87">
         <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>179</v>
-      </c>
-      <c r="J87" s="10" t="s">
-        <v>343</v>
+        <v>172</v>
+      </c>
+      <c r="J87" t="s">
+        <v>442</v>
       </c>
       <c r="K87" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>253</v>
+        <v>176</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F88" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88" t="s">
+        <v>437</v>
+      </c>
+      <c r="J88" s="10" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>253</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89" t="s">
+        <v>437</v>
+      </c>
+      <c r="J89" s="10" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>255</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90" t="s">
+        <v>437</v>
+      </c>
+      <c r="J90" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="K90" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>254</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91" t="s">
+        <v>437</v>
+      </c>
+      <c r="J91" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="K91" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D92" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92" t="s">
+        <v>437</v>
+      </c>
+      <c r="J92" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="K92" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>252</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93" t="s">
+        <v>437</v>
+      </c>
+      <c r="J93" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="G88">
-        <v>0</v>
-      </c>
-      <c r="H88">
-        <v>0</v>
-      </c>
-      <c r="I88" t="s">
-        <v>179</v>
-      </c>
-      <c r="J88" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="K88" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D89" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G89">
-        <v>0</v>
-      </c>
-      <c r="H89">
-        <v>0</v>
-      </c>
-      <c r="I89" t="s">
-        <v>179</v>
-      </c>
-      <c r="J89" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D90" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G90">
-        <v>0</v>
-      </c>
-      <c r="H90">
-        <v>0</v>
-      </c>
-      <c r="I90" t="s">
-        <v>179</v>
-      </c>
-      <c r="J90" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D91" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="G91">
-        <v>0</v>
-      </c>
-      <c r="H91">
-        <v>0</v>
-      </c>
-      <c r="I91" t="s">
-        <v>179</v>
-      </c>
-      <c r="J91" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D92" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G92">
-        <v>0</v>
-      </c>
-      <c r="H92">
-        <v>0</v>
-      </c>
-      <c r="I92" t="s">
-        <v>179</v>
-      </c>
-      <c r="J92" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D93" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="G93">
-        <v>0</v>
-      </c>
-      <c r="H93">
-        <v>0</v>
-      </c>
-      <c r="I93" t="s">
-        <v>179</v>
-      </c>
-      <c r="J93" t="s">
-        <v>235</v>
+      <c r="K93" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.25">
@@ -4669,7 +4702,7 @@
         <v>96</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>236</v>
+        <v>180</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -4678,13 +4711,10 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>179</v>
+        <v>437</v>
       </c>
       <c r="J94" t="s">
-        <v>237</v>
-      </c>
-      <c r="K94" t="s">
-        <v>409</v>
+        <v>213</v>
       </c>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.25">
@@ -4692,7 +4722,7 @@
         <v>96</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -4701,13 +4731,10 @@
         <v>0</v>
       </c>
       <c r="I95" t="s">
-        <v>179</v>
+        <v>437</v>
       </c>
       <c r="J95" t="s">
-        <v>349</v>
-      </c>
-      <c r="K95" t="s">
-        <v>409</v>
+        <v>214</v>
       </c>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.25">
@@ -4715,7 +4742,7 @@
         <v>96</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>348</v>
+        <v>189</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -4724,13 +4751,10 @@
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>179</v>
+        <v>437</v>
       </c>
       <c r="J96" t="s">
-        <v>350</v>
-      </c>
-      <c r="K96" t="s">
-        <v>409</v>
+        <v>219</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -4738,7 +4762,7 @@
         <v>96</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>251</v>
+        <v>190</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -4747,21 +4771,18 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>179</v>
+        <v>437</v>
       </c>
       <c r="J97" t="s">
-        <v>252</v>
-      </c>
-      <c r="K97" t="s">
-        <v>409</v>
+        <v>215</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D98" s="6" t="s">
-        <v>95</v>
+      <c r="D98" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>388</v>
+        <v>233</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -4770,10 +4791,10 @@
         <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>389</v>
+        <v>437</v>
       </c>
       <c r="J98" t="s">
-        <v>393</v>
+        <v>234</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -4781,7 +4802,7 @@
         <v>96</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>386</v>
+        <v>235</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -4790,10 +4811,13 @@
         <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>389</v>
+        <v>437</v>
       </c>
       <c r="J99" t="s">
-        <v>394</v>
+        <v>236</v>
+      </c>
+      <c r="K99" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -4801,7 +4825,7 @@
         <v>96</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>387</v>
+        <v>193</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -4810,18 +4834,21 @@
         <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>389</v>
+        <v>437</v>
       </c>
       <c r="J100" t="s">
-        <v>395</v>
+        <v>348</v>
+      </c>
+      <c r="K100" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D101" s="6" t="s">
-        <v>95</v>
+      <c r="D101" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>227</v>
+        <v>347</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -4830,10 +4857,13 @@
         <v>0</v>
       </c>
       <c r="I101" t="s">
-        <v>390</v>
+        <v>437</v>
       </c>
       <c r="J101" t="s">
-        <v>305</v>
+        <v>349</v>
+      </c>
+      <c r="K101" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -4841,7 +4871,7 @@
         <v>96</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -4850,24 +4880,21 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>390</v>
+        <v>437</v>
       </c>
       <c r="J102" t="s">
-        <v>229</v>
+        <v>251</v>
+      </c>
+      <c r="K102" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <v>17</v>
-      </c>
-      <c r="B103" t="s">
-        <v>136</v>
-      </c>
       <c r="D103" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F103" s="9" t="s">
-        <v>192</v>
+      <c r="F103" s="2" t="s">
+        <v>387</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -4876,13 +4903,10 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>391</v>
-      </c>
-      <c r="J103" s="10" t="s">
-        <v>306</v>
-      </c>
-      <c r="K103" t="s">
-        <v>409</v>
+        <v>438</v>
+      </c>
+      <c r="J103" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -4890,7 +4914,7 @@
         <v>96</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>193</v>
+        <v>385</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -4899,24 +4923,18 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>391</v>
+        <v>438</v>
       </c>
       <c r="J104" t="s">
-        <v>359</v>
-      </c>
-      <c r="K104" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>298</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F105" s="9" t="s">
-        <v>299</v>
+      <c r="D105" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>386</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -4925,10 +4943,10 @@
         <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>392</v>
+        <v>438</v>
       </c>
       <c r="J105" t="s">
-        <v>302</v>
+        <v>390</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
@@ -4936,7 +4954,7 @@
         <v>95</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>307</v>
+        <v>226</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -4945,13 +4963,10 @@
         <v>0</v>
       </c>
       <c r="I106" t="s">
-        <v>392</v>
+        <v>439</v>
       </c>
       <c r="J106" t="s">
-        <v>303</v>
-      </c>
-      <c r="K106" t="s">
-        <v>409</v>
+        <v>304</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
@@ -4959,7 +4974,7 @@
         <v>96</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>300</v>
+        <v>227</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -4968,24 +4983,24 @@
         <v>0</v>
       </c>
       <c r="I107" t="s">
-        <v>392</v>
+        <v>439</v>
       </c>
       <c r="J107" t="s">
-        <v>301</v>
-      </c>
-      <c r="K107" t="s">
-        <v>409</v>
+        <v>228</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>17</v>
+      </c>
       <c r="B108" t="s">
-        <v>177</v>
+        <v>136</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>326</v>
+        <v>191</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -4994,18 +5009,21 @@
         <v>0</v>
       </c>
       <c r="I108" t="s">
-        <v>179</v>
+        <v>440</v>
       </c>
       <c r="J108" s="10" t="s">
-        <v>217</v>
+        <v>305</v>
+      </c>
+      <c r="K108" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D109" s="6" t="s">
-        <v>95</v>
+      <c r="D109" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>330</v>
+        <v>192</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -5014,18 +5032,24 @@
         <v>0</v>
       </c>
       <c r="I109" t="s">
-        <v>179</v>
-      </c>
-      <c r="J109" s="10" t="s">
-        <v>217</v>
+        <v>440</v>
+      </c>
+      <c r="J109" t="s">
+        <v>358</v>
+      </c>
+      <c r="K109" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>297</v>
+      </c>
       <c r="D110" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F110" s="2" t="s">
-        <v>331</v>
+      <c r="F110" s="9" t="s">
+        <v>298</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -5034,10 +5058,10 @@
         <v>0</v>
       </c>
       <c r="I110" t="s">
-        <v>179</v>
-      </c>
-      <c r="J110" s="10" t="s">
-        <v>217</v>
+        <v>441</v>
+      </c>
+      <c r="J110" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
@@ -5045,7 +5069,7 @@
         <v>95</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>331</v>
+        <v>306</v>
       </c>
       <c r="G111">
         <v>0</v>
@@ -5054,30 +5078,139 @@
         <v>0</v>
       </c>
       <c r="I111" t="s">
-        <v>179</v>
-      </c>
-      <c r="J111" s="10" t="s">
-        <v>217</v>
+        <v>441</v>
+      </c>
+      <c r="J111" t="s">
+        <v>302</v>
+      </c>
+      <c r="K111" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D112" s="6" t="s">
+      <c r="D112" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="G112">
+        <v>0</v>
+      </c>
+      <c r="H112">
+        <v>0</v>
+      </c>
+      <c r="I112" t="s">
+        <v>441</v>
+      </c>
+      <c r="J112" t="s">
+        <v>300</v>
+      </c>
+      <c r="K112" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="113" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>176</v>
+      </c>
+      <c r="D113" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F112" s="2" t="s">
+      <c r="F113" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+      <c r="H113">
+        <v>0</v>
+      </c>
+      <c r="I113" t="s">
+        <v>178</v>
+      </c>
+      <c r="J113" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="114" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D114" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+      <c r="H114">
+        <v>0</v>
+      </c>
+      <c r="I114" t="s">
+        <v>178</v>
+      </c>
+      <c r="J114" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="115" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D115" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>0</v>
+      </c>
+      <c r="I115" t="s">
+        <v>178</v>
+      </c>
+      <c r="J115" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="116" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D116" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="G116">
+        <v>0</v>
+      </c>
+      <c r="H116">
+        <v>0</v>
+      </c>
+      <c r="I116" t="s">
+        <v>178</v>
+      </c>
+      <c r="J116" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="117" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D117" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="G117">
+        <v>0</v>
+      </c>
+      <c r="H117">
+        <v>0</v>
+      </c>
+      <c r="I117" t="s">
         <v>373</v>
       </c>
-      <c r="G112">
-        <v>0</v>
-      </c>
-      <c r="H112">
-        <v>0</v>
-      </c>
-      <c r="I112" t="s">
-        <v>374</v>
-      </c>
-      <c r="J112" s="2" t="s">
-        <v>373</v>
+      <c r="J117" s="2" t="s">
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -5103,15 +5236,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
         <v>183</v>
-      </c>
-      <c r="B1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>50</v>
@@ -5119,7 +5252,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>51</v>
@@ -5127,7 +5260,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>52</v>
@@ -5135,7 +5268,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
MAPS Dashboard ports verification
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -12,14 +12,14 @@
     <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$K$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$K$120</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="454">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1366,6 +1366,21 @@
   </si>
   <si>
     <t>NPIV_</t>
+  </si>
+  <si>
+    <t>fabric_labels_summary</t>
+  </si>
+  <si>
+    <t>MAPS_ports</t>
+  </si>
+  <si>
+    <t>MAPS_порты</t>
+  </si>
+  <si>
+    <t>MAPS Dashboard ports</t>
+  </si>
+  <si>
+    <t>MAPS Dashboard порты</t>
   </si>
 </sst>
 </file>
@@ -1781,8 +1796,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1822,7 +1837,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2356,11 +2371,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K117"/>
+  <dimension ref="A1:K120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5:H9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3611,8 +3626,8 @@
       <c r="D44" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F44" s="8" t="s">
-        <v>56</v>
+      <c r="F44" s="9" t="s">
+        <v>449</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -3624,7 +3639,7 @@
         <v>158</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>305</v>
+        <v>216</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -3632,7 +3647,7 @@
         <v>95</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -3644,38 +3659,38 @@
         <v>158</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>216</v>
+        <v>305</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>161</v>
-      </c>
       <c r="D46" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="F46" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46" t="s">
+        <v>158</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>161</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F47" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46" t="s">
-        <v>162</v>
-      </c>
-      <c r="J46" s="10" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D47" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -3686,42 +3701,42 @@
       <c r="I47" t="s">
         <v>162</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J47" s="10" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D48" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48" t="s">
+        <v>162</v>
+      </c>
+      <c r="J48" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>16</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>139</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-      <c r="I48" t="s">
-        <v>169</v>
-      </c>
-      <c r="J48" s="10" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D49" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>163</v>
+      <c r="F49" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -3733,15 +3748,15 @@
         <v>169</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>216</v>
+        <v>289</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D50" s="5" t="s">
-        <v>96</v>
+      <c r="D50" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>61</v>
+        <v>163</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -3752,8 +3767,8 @@
       <c r="I50" t="s">
         <v>169</v>
       </c>
-      <c r="J50" t="s">
-        <v>195</v>
+      <c r="J50" s="10" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -3761,7 +3776,7 @@
         <v>96</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -3773,7 +3788,7 @@
         <v>169</v>
       </c>
       <c r="J51" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -3781,7 +3796,7 @@
         <v>96</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -3793,7 +3808,7 @@
         <v>169</v>
       </c>
       <c r="J52" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -3801,7 +3816,7 @@
         <v>96</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -3813,7 +3828,7 @@
         <v>169</v>
       </c>
       <c r="J53" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -3821,7 +3836,7 @@
         <v>96</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -3833,7 +3848,7 @@
         <v>169</v>
       </c>
       <c r="J54" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -3841,7 +3856,7 @@
         <v>96</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>446</v>
+        <v>64</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -3853,41 +3868,41 @@
         <v>169</v>
       </c>
       <c r="J55" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D56" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56" t="s">
+        <v>169</v>
+      </c>
+      <c r="J56" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>18</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>138</v>
       </c>
-      <c r="D56" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="I56" t="s">
-        <v>170</v>
-      </c>
-      <c r="J56" s="10" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D57" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>286</v>
+        <v>69</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -3899,18 +3914,15 @@
         <v>170</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="K57" t="s">
-        <v>404</v>
+        <v>288</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D58" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>67</v>
+      <c r="D58" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>286</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -3921,8 +3933,11 @@
       <c r="I58" t="s">
         <v>170</v>
       </c>
-      <c r="J58" t="s">
-        <v>206</v>
+      <c r="J58" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="K58" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -3930,7 +3945,7 @@
         <v>96</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -3942,7 +3957,7 @@
         <v>170</v>
       </c>
       <c r="J59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -3950,7 +3965,7 @@
         <v>96</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>290</v>
+        <v>68</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -3962,44 +3977,44 @@
         <v>170</v>
       </c>
       <c r="J60" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D61" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61" t="s">
+        <v>170</v>
+      </c>
+      <c r="J61" t="s">
         <v>291</v>
       </c>
-      <c r="K60" t="s">
+      <c r="K61" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>20</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>131</v>
       </c>
-      <c r="D61" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-      <c r="I61" t="s">
-        <v>171</v>
-      </c>
-      <c r="J61" s="10" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D62" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>426</v>
+        <v>90</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -4011,10 +4026,7 @@
         <v>171</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>423</v>
-      </c>
-      <c r="K62" t="s">
-        <v>404</v>
+        <v>268</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -4022,7 +4034,7 @@
         <v>95</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>271</v>
+        <v>426</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -4034,7 +4046,7 @@
         <v>171</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>272</v>
+        <v>423</v>
       </c>
       <c r="K63" t="s">
         <v>404</v>
@@ -4044,8 +4056,8 @@
       <c r="D64" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F64" s="2" t="s">
-        <v>243</v>
+      <c r="F64" s="9" t="s">
+        <v>271</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -4057,7 +4069,10 @@
         <v>171</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>340</v>
+        <v>272</v>
+      </c>
+      <c r="K64" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.25">
@@ -4065,7 +4080,7 @@
         <v>95</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -4077,15 +4092,15 @@
         <v>171</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>245</v>
+        <v>340</v>
       </c>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D66" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="F66" s="11" t="s">
-        <v>247</v>
+      <c r="D66" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -4101,14 +4116,11 @@
       </c>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>133</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F67" s="8" t="s">
-        <v>109</v>
+      <c r="D67" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="F67" s="11" t="s">
+        <v>247</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -4120,21 +4132,18 @@
         <v>171</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>384</v>
+        <v>245</v>
       </c>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>119</v>
-      </c>
-      <c r="C68" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F68" s="7" t="s">
-        <v>93</v>
+      <c r="F68" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -4146,15 +4155,21 @@
         <v>171</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>339</v>
+        <v>384</v>
       </c>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>119</v>
+      </c>
+      <c r="C69" t="s">
+        <v>132</v>
+      </c>
       <c r="D69" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>311</v>
+        <v>93</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -4166,18 +4181,15 @@
         <v>171</v>
       </c>
       <c r="J69" s="10" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>134</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>422</v>
+      <c r="D70" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>311</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -4188,19 +4200,19 @@
       <c r="I70" t="s">
         <v>171</v>
       </c>
-      <c r="J70" t="s">
-        <v>198</v>
+      <c r="J70" s="10" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>101</v>
+        <v>422</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -4212,15 +4224,18 @@
         <v>171</v>
       </c>
       <c r="J71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>135</v>
+      </c>
       <c r="D72" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -4232,7 +4247,7 @@
         <v>171</v>
       </c>
       <c r="J72" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.25">
@@ -4240,7 +4255,7 @@
         <v>96</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -4252,7 +4267,7 @@
         <v>171</v>
       </c>
       <c r="J73" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.25">
@@ -4260,7 +4275,7 @@
         <v>96</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -4272,7 +4287,7 @@
         <v>171</v>
       </c>
       <c r="J74" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.25">
@@ -4280,7 +4295,7 @@
         <v>96</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -4292,7 +4307,7 @@
         <v>171</v>
       </c>
       <c r="J75" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
@@ -4300,7 +4315,7 @@
         <v>96</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -4312,7 +4327,7 @@
         <v>171</v>
       </c>
       <c r="J76" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.25">
@@ -4320,7 +4335,7 @@
         <v>96</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>425</v>
+        <v>106</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -4332,10 +4347,7 @@
         <v>171</v>
       </c>
       <c r="J77" t="s">
-        <v>424</v>
-      </c>
-      <c r="K77" t="s">
-        <v>404</v>
+        <v>211</v>
       </c>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.25">
@@ -4343,7 +4355,7 @@
         <v>96</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>273</v>
+        <v>425</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -4355,7 +4367,7 @@
         <v>171</v>
       </c>
       <c r="J78" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="K78" t="s">
         <v>404</v>
@@ -4366,7 +4378,7 @@
         <v>96</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>164</v>
+        <v>273</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -4378,38 +4390,41 @@
         <v>171</v>
       </c>
       <c r="J79" t="s">
+        <v>417</v>
+      </c>
+      <c r="K79" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D80" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F80" s="2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80" t="s">
+        <v>171</v>
+      </c>
+      <c r="J80" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
         <v>165</v>
       </c>
-      <c r="D80" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-      <c r="H80">
-        <v>0</v>
-      </c>
-      <c r="I80" t="s">
-        <v>172</v>
-      </c>
-      <c r="J80" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D81" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F81" s="2" t="s">
-        <v>448</v>
+      <c r="F81" s="9" t="s">
+        <v>218</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -4421,7 +4436,7 @@
         <v>172</v>
       </c>
       <c r="J81" t="s">
-        <v>445</v>
+        <v>303</v>
       </c>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.25">
@@ -4429,7 +4444,7 @@
         <v>95</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>435</v>
+        <v>450</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -4441,18 +4456,15 @@
         <v>172</v>
       </c>
       <c r="J82" t="s">
-        <v>444</v>
-      </c>
-      <c r="K82" t="s">
-        <v>404</v>
+        <v>452</v>
       </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D83" s="5" t="s">
-        <v>96</v>
+      <c r="D83" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>166</v>
+        <v>448</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -4464,15 +4476,15 @@
         <v>172</v>
       </c>
       <c r="J83" t="s">
-        <v>202</v>
+        <v>445</v>
       </c>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D84" s="5" t="s">
-        <v>96</v>
+      <c r="D84" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>167</v>
+        <v>435</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -4484,7 +4496,10 @@
         <v>172</v>
       </c>
       <c r="J84" t="s">
-        <v>212</v>
+        <v>444</v>
+      </c>
+      <c r="K84" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
@@ -4492,7 +4507,7 @@
         <v>96</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -4504,7 +4519,7 @@
         <v>172</v>
       </c>
       <c r="J85" t="s">
-        <v>269</v>
+        <v>202</v>
       </c>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.25">
@@ -4512,19 +4527,19 @@
         <v>96</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>443</v>
+        <v>167</v>
       </c>
       <c r="G86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I86" t="s">
         <v>172</v>
       </c>
       <c r="J86" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.25">
@@ -4532,10 +4547,10 @@
         <v>96</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>436</v>
+        <v>168</v>
       </c>
       <c r="G87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H87">
         <v>0</v>
@@ -4544,79 +4559,67 @@
         <v>172</v>
       </c>
       <c r="J87" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D88" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88" t="s">
+        <v>172</v>
+      </c>
+      <c r="J88" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D89" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89" t="s">
+        <v>172</v>
+      </c>
+      <c r="J89" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D90" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90" t="s">
+        <v>172</v>
+      </c>
+      <c r="J90" t="s">
         <v>442</v>
-      </c>
-      <c r="K87" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>176</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F88" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="G88">
-        <v>0</v>
-      </c>
-      <c r="H88">
-        <v>0</v>
-      </c>
-      <c r="I88" t="s">
-        <v>437</v>
-      </c>
-      <c r="J88" s="10" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>253</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F89" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="G89">
-        <v>0</v>
-      </c>
-      <c r="H89">
-        <v>0</v>
-      </c>
-      <c r="I89" t="s">
-        <v>437</v>
-      </c>
-      <c r="J89" s="10" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
-        <v>255</v>
-      </c>
-      <c r="D90" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F90" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="G90">
-        <v>0</v>
-      </c>
-      <c r="H90">
-        <v>0</v>
-      </c>
-      <c r="I90" t="s">
-        <v>437</v>
-      </c>
-      <c r="J90" s="10" t="s">
-        <v>345</v>
       </c>
       <c r="K90" t="s">
         <v>404</v>
@@ -4624,13 +4627,13 @@
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>254</v>
+        <v>176</v>
       </c>
       <c r="D91" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F91" s="9" t="s">
-        <v>217</v>
+        <v>177</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -4642,18 +4645,18 @@
         <v>437</v>
       </c>
       <c r="J91" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="K91" t="s">
-        <v>404</v>
+        <v>343</v>
       </c>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>253</v>
+      </c>
       <c r="D92" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F92" s="9" t="s">
-        <v>341</v>
+        <v>179</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -4665,21 +4668,18 @@
         <v>437</v>
       </c>
       <c r="J92" s="10" t="s">
-        <v>342</v>
-      </c>
-      <c r="K92" t="s">
-        <v>404</v>
+        <v>344</v>
       </c>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>248</v>
+        <v>188</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -4691,18 +4691,21 @@
         <v>437</v>
       </c>
       <c r="J93" s="10" t="s">
-        <v>249</v>
+        <v>345</v>
       </c>
       <c r="K93" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D94" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>180</v>
+      <c r="B94" t="s">
+        <v>254</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>217</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -4713,16 +4716,19 @@
       <c r="I94" t="s">
         <v>437</v>
       </c>
-      <c r="J94" t="s">
-        <v>213</v>
+      <c r="J94" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="K94" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D95" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>181</v>
+      <c r="D95" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>341</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -4733,16 +4739,22 @@
       <c r="I95" t="s">
         <v>437</v>
       </c>
-      <c r="J95" t="s">
-        <v>214</v>
+      <c r="J95" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="K95" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D96" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>189</v>
+      <c r="B96" t="s">
+        <v>252</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>248</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -4753,8 +4765,11 @@
       <c r="I96" t="s">
         <v>437</v>
       </c>
-      <c r="J96" t="s">
-        <v>219</v>
+      <c r="J96" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="K96" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -4762,7 +4777,7 @@
         <v>96</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -4774,7 +4789,7 @@
         <v>437</v>
       </c>
       <c r="J97" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -4782,7 +4797,7 @@
         <v>96</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>233</v>
+        <v>181</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -4794,7 +4809,7 @@
         <v>437</v>
       </c>
       <c r="J98" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -4802,7 +4817,7 @@
         <v>96</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>235</v>
+        <v>189</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -4814,10 +4829,7 @@
         <v>437</v>
       </c>
       <c r="J99" t="s">
-        <v>236</v>
-      </c>
-      <c r="K99" t="s">
-        <v>404</v>
+        <v>219</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
@@ -4825,7 +4837,7 @@
         <v>96</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -4837,10 +4849,7 @@
         <v>437</v>
       </c>
       <c r="J100" t="s">
-        <v>348</v>
-      </c>
-      <c r="K100" t="s">
-        <v>404</v>
+        <v>215</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
@@ -4848,7 +4857,7 @@
         <v>96</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>347</v>
+        <v>233</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -4860,10 +4869,7 @@
         <v>437</v>
       </c>
       <c r="J101" t="s">
-        <v>349</v>
-      </c>
-      <c r="K101" t="s">
-        <v>404</v>
+        <v>234</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -4871,7 +4877,7 @@
         <v>96</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -4883,18 +4889,18 @@
         <v>437</v>
       </c>
       <c r="J102" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="K102" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D103" s="6" t="s">
-        <v>95</v>
+      <c r="D103" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>387</v>
+        <v>193</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -4903,10 +4909,13 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J103" t="s">
-        <v>388</v>
+        <v>348</v>
+      </c>
+      <c r="K103" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -4914,7 +4923,7 @@
         <v>96</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>385</v>
+        <v>347</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -4923,10 +4932,13 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J104" t="s">
-        <v>389</v>
+        <v>349</v>
+      </c>
+      <c r="K104" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
@@ -4934,7 +4946,7 @@
         <v>96</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>386</v>
+        <v>250</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -4943,10 +4955,13 @@
         <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J105" t="s">
-        <v>390</v>
+        <v>251</v>
+      </c>
+      <c r="K105" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
@@ -4954,7 +4969,7 @@
         <v>95</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>226</v>
+        <v>387</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -4963,10 +4978,10 @@
         <v>0</v>
       </c>
       <c r="I106" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="J106" t="s">
-        <v>304</v>
+        <v>388</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
@@ -4974,102 +4989,93 @@
         <v>96</v>
       </c>
       <c r="F107" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+      <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="I107" t="s">
+        <v>438</v>
+      </c>
+      <c r="J107" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D108" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+      <c r="H108">
+        <v>0</v>
+      </c>
+      <c r="I108" t="s">
+        <v>438</v>
+      </c>
+      <c r="J108" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D109" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
+      <c r="I109" t="s">
+        <v>439</v>
+      </c>
+      <c r="J109" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D110" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F110" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="G107">
-        <v>0</v>
-      </c>
-      <c r="H107">
-        <v>0</v>
-      </c>
-      <c r="I107" t="s">
+      <c r="G110">
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="I110" t="s">
         <v>439</v>
       </c>
-      <c r="J107" t="s">
+      <c r="J110" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A108">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111">
         <v>17</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B111" t="s">
         <v>136</v>
       </c>
-      <c r="D108" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F108" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="G108">
-        <v>0</v>
-      </c>
-      <c r="H108">
-        <v>0</v>
-      </c>
-      <c r="I108" t="s">
-        <v>440</v>
-      </c>
-      <c r="J108" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="K108" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D109" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="G109">
-        <v>0</v>
-      </c>
-      <c r="H109">
-        <v>0</v>
-      </c>
-      <c r="I109" t="s">
-        <v>440</v>
-      </c>
-      <c r="J109" t="s">
-        <v>358</v>
-      </c>
-      <c r="K109" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>297</v>
-      </c>
-      <c r="D110" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F110" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="G110">
-        <v>0</v>
-      </c>
-      <c r="H110">
-        <v>0</v>
-      </c>
-      <c r="I110" t="s">
-        <v>441</v>
-      </c>
-      <c r="J110" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D111" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F111" s="2" t="s">
-        <v>306</v>
+      <c r="F111" s="9" t="s">
+        <v>191</v>
       </c>
       <c r="G111">
         <v>0</v>
@@ -5078,10 +5084,10 @@
         <v>0</v>
       </c>
       <c r="I111" t="s">
-        <v>441</v>
-      </c>
-      <c r="J111" t="s">
-        <v>302</v>
+        <v>440</v>
+      </c>
+      <c r="J111" s="10" t="s">
+        <v>305</v>
       </c>
       <c r="K111" t="s">
         <v>404</v>
@@ -5092,7 +5098,7 @@
         <v>96</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>299</v>
+        <v>192</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -5101,24 +5107,24 @@
         <v>0</v>
       </c>
       <c r="I112" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="J112" t="s">
-        <v>300</v>
+        <v>358</v>
       </c>
       <c r="K112" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="113" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>176</v>
+        <v>297</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F113" s="9" t="s">
-        <v>325</v>
+        <v>298</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -5127,18 +5133,18 @@
         <v>0</v>
       </c>
       <c r="I113" t="s">
-        <v>178</v>
-      </c>
-      <c r="J113" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="114" spans="2:10" x14ac:dyDescent="0.25">
+        <v>441</v>
+      </c>
+      <c r="J113" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D114" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>329</v>
+        <v>306</v>
       </c>
       <c r="G114">
         <v>0</v>
@@ -5147,18 +5153,21 @@
         <v>0</v>
       </c>
       <c r="I114" t="s">
-        <v>178</v>
-      </c>
-      <c r="J114" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="115" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D115" s="6" t="s">
-        <v>95</v>
+        <v>441</v>
+      </c>
+      <c r="J114" t="s">
+        <v>302</v>
+      </c>
+      <c r="K114" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="115" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D115" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>330</v>
+        <v>299</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -5167,18 +5176,24 @@
         <v>0</v>
       </c>
       <c r="I115" t="s">
-        <v>178</v>
-      </c>
-      <c r="J115" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="116" spans="2:10" x14ac:dyDescent="0.25">
+        <v>441</v>
+      </c>
+      <c r="J115" t="s">
+        <v>300</v>
+      </c>
+      <c r="K115" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="116" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>176</v>
+      </c>
       <c r="D116" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F116" s="2" t="s">
-        <v>330</v>
+      <c r="F116" s="9" t="s">
+        <v>325</v>
       </c>
       <c r="G116">
         <v>0</v>
@@ -5193,23 +5208,83 @@
         <v>216</v>
       </c>
     </row>
-    <row r="117" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D117" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F117" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="G117">
+        <v>0</v>
+      </c>
+      <c r="H117">
+        <v>0</v>
+      </c>
+      <c r="I117" t="s">
+        <v>178</v>
+      </c>
+      <c r="J117" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="118" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D118" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="G118">
+        <v>0</v>
+      </c>
+      <c r="H118">
+        <v>0</v>
+      </c>
+      <c r="I118" t="s">
+        <v>178</v>
+      </c>
+      <c r="J118" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="119" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D119" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+      <c r="H119">
+        <v>0</v>
+      </c>
+      <c r="I119" t="s">
+        <v>178</v>
+      </c>
+      <c r="J119" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D120" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F120" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="G117">
-        <v>0</v>
-      </c>
-      <c r="H117">
-        <v>0</v>
-      </c>
-      <c r="I117" t="s">
+      <c r="G120">
+        <v>0</v>
+      </c>
+      <c r="H120">
+        <v>0</v>
+      </c>
+      <c r="I120" t="s">
         <v>373</v>
       </c>
-      <c r="J117" s="2" t="s">
+      <c r="J120" s="2" t="s">
         <v>372</v>
       </c>
     </row>

</xml_diff>

<commit_message>
switch params aggregation refactoring
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -2370,12 +2370,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" filterMode="1"/>
   <dimension ref="A1:K120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H91" sqref="H91"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G124" sqref="G124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2425,7 +2425,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>10</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>11</v>
       </c>
@@ -2899,7 +2899,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>12</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>123</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>123</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>13</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>126</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>126</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>126</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>126</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>126</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>126</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>222</v>
       </c>
@@ -3345,7 +3345,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>295</v>
       </c>
@@ -3371,7 +3371,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>19</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>114</v>
       </c>
@@ -3426,7 +3426,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>114</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>262</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
         <v>262</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
         <v>363</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
         <v>363</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
         <v>363</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
         <v>363</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>15</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D44" s="6" t="s">
         <v>95</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D45" s="6" t="s">
         <v>95</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="D46" s="6" t="s">
         <v>95</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>161</v>
       </c>
@@ -3725,7 +3725,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>16</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D50" s="6" t="s">
         <v>95</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>18</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D58" s="6" t="s">
         <v>95</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>20</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D63" s="6" t="s">
         <v>95</v>
       </c>
@@ -4052,7 +4052,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D64" s="6" t="s">
         <v>95</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D65" s="6" t="s">
         <v>95</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D66" s="6" t="s">
         <v>95</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D67" s="11" t="s">
         <v>246</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>133</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>119</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D70" s="6" t="s">
         <v>95</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>165</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D82" s="6" t="s">
         <v>95</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D83" s="6" t="s">
         <v>95</v>
       </c>
@@ -4479,7 +4479,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D84" s="6" t="s">
         <v>95</v>
       </c>
@@ -4570,10 +4570,10 @@
         <v>451</v>
       </c>
       <c r="G88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I88" t="s">
         <v>172</v>
@@ -4625,7 +4625,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>176</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>0</v>
       </c>
       <c r="H91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I91" t="s">
         <v>437</v>
@@ -4648,7 +4648,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>253</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>0</v>
       </c>
       <c r="H92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I92" t="s">
         <v>437</v>
@@ -4671,7 +4671,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>255</v>
       </c>
@@ -4685,7 +4685,7 @@
         <v>0</v>
       </c>
       <c r="H93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I93" t="s">
         <v>437</v>
@@ -4697,7 +4697,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>254</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>0</v>
       </c>
       <c r="H94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I94" t="s">
         <v>437</v>
@@ -4723,7 +4723,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D95" s="6" t="s">
         <v>95</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>0</v>
       </c>
       <c r="H95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I95" t="s">
         <v>437</v>
@@ -4746,7 +4746,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>252</v>
       </c>
@@ -4760,7 +4760,7 @@
         <v>0</v>
       </c>
       <c r="H96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I96" t="s">
         <v>437</v>
@@ -4780,10 +4780,10 @@
         <v>180</v>
       </c>
       <c r="G97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I97" t="s">
         <v>437</v>
@@ -4800,10 +4800,10 @@
         <v>181</v>
       </c>
       <c r="G98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I98" t="s">
         <v>437</v>
@@ -4820,10 +4820,10 @@
         <v>189</v>
       </c>
       <c r="G99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I99" t="s">
         <v>437</v>
@@ -4840,10 +4840,10 @@
         <v>190</v>
       </c>
       <c r="G100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I100" t="s">
         <v>437</v>
@@ -4860,10 +4860,10 @@
         <v>233</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I101" t="s">
         <v>437</v>
@@ -4880,10 +4880,10 @@
         <v>235</v>
       </c>
       <c r="G102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I102" t="s">
         <v>437</v>
@@ -4903,10 +4903,10 @@
         <v>193</v>
       </c>
       <c r="G103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I103" t="s">
         <v>437</v>
@@ -4926,10 +4926,10 @@
         <v>347</v>
       </c>
       <c r="G104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I104" t="s">
         <v>437</v>
@@ -4949,10 +4949,10 @@
         <v>250</v>
       </c>
       <c r="G105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I105" t="s">
         <v>437</v>
@@ -4964,7 +4964,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D106" s="6" t="s">
         <v>95</v>
       </c>
@@ -4975,7 +4975,7 @@
         <v>0</v>
       </c>
       <c r="H106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I106" t="s">
         <v>438</v>
@@ -4992,10 +4992,10 @@
         <v>385</v>
       </c>
       <c r="G107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I107" t="s">
         <v>438</v>
@@ -5012,10 +5012,10 @@
         <v>386</v>
       </c>
       <c r="G108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I108" t="s">
         <v>438</v>
@@ -5024,7 +5024,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D109" s="6" t="s">
         <v>95</v>
       </c>
@@ -5035,7 +5035,7 @@
         <v>0</v>
       </c>
       <c r="H109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I109" t="s">
         <v>439</v>
@@ -5052,10 +5052,10 @@
         <v>227</v>
       </c>
       <c r="G110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I110" t="s">
         <v>439</v>
@@ -5064,7 +5064,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>17</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>0</v>
       </c>
       <c r="H111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I111" t="s">
         <v>440</v>
@@ -5101,10 +5101,10 @@
         <v>192</v>
       </c>
       <c r="G112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I112" t="s">
         <v>440</v>
@@ -5116,7 +5116,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>297</v>
       </c>
@@ -5130,7 +5130,7 @@
         <v>0</v>
       </c>
       <c r="H113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I113" t="s">
         <v>441</v>
@@ -5139,7 +5139,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D114" s="6" t="s">
         <v>95</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>0</v>
       </c>
       <c r="H114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I114" t="s">
         <v>441</v>
@@ -5170,10 +5170,10 @@
         <v>299</v>
       </c>
       <c r="G115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I115" t="s">
         <v>441</v>
@@ -5185,7 +5185,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="116" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>176</v>
       </c>
@@ -5199,7 +5199,7 @@
         <v>0</v>
       </c>
       <c r="H116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I116" t="s">
         <v>178</v>
@@ -5208,7 +5208,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="117" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D117" s="6" t="s">
         <v>95</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>0</v>
       </c>
       <c r="H117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I117" t="s">
         <v>178</v>
@@ -5228,7 +5228,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="118" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D118" s="6" t="s">
         <v>95</v>
       </c>
@@ -5239,7 +5239,7 @@
         <v>0</v>
       </c>
       <c r="H118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I118" t="s">
         <v>178</v>
@@ -5248,7 +5248,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="119" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D119" s="6" t="s">
         <v>95</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>0</v>
       </c>
       <c r="H119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I119" t="s">
         <v>178</v>
@@ -5268,7 +5268,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="120" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D120" s="6" t="s">
         <v>95</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>0</v>
       </c>
       <c r="H120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I120" t="s">
         <v>373</v>
@@ -5289,6 +5289,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K120">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="report"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
zone and device name ratio corrected for peer zones
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1817,8 +1817,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2395,8 +2395,8 @@
   <dimension ref="A1:K122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H56" sqref="H56"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3784,7 +3784,7 @@
         <v>0</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" t="s">
         <v>169</v>
@@ -4704,10 +4704,10 @@
         <v>177</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I93" t="s">
         <v>437</v>
@@ -4750,7 +4750,7 @@
         <v>188</v>
       </c>
       <c r="G95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H95">
         <v>0</v>
@@ -4825,7 +4825,7 @@
         <v>248</v>
       </c>
       <c r="G98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H98">
         <v>0</v>

</xml_diff>

<commit_message>
zone name and device names ratio refactoring
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -2394,9 +2394,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G104" sqref="G104"/>
+      <selection pane="bottomLeft" activeCell="H99" sqref="H99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4088,7 +4088,7 @@
         <v>0</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I64" t="s">
         <v>171</v>
@@ -4704,7 +4704,7 @@
         <v>177</v>
       </c>
       <c r="G93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H93">
         <v>1</v>
@@ -4750,7 +4750,7 @@
         <v>188</v>
       </c>
       <c r="G95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H95">
         <v>0</v>
@@ -4825,7 +4825,7 @@
         <v>248</v>
       </c>
       <c r="G98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H98">
         <v>0</v>
@@ -4848,10 +4848,10 @@
         <v>180</v>
       </c>
       <c r="G99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I99" t="s">
         <v>437</v>
@@ -4868,10 +4868,10 @@
         <v>181</v>
       </c>
       <c r="G100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I100" t="s">
         <v>437</v>
@@ -4888,10 +4888,10 @@
         <v>189</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I101" t="s">
         <v>437</v>
@@ -4908,10 +4908,10 @@
         <v>190</v>
       </c>
       <c r="G102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I102" t="s">
         <v>437</v>
@@ -4928,10 +4928,10 @@
         <v>233</v>
       </c>
       <c r="G103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I103" t="s">
         <v>437</v>
@@ -4948,10 +4948,10 @@
         <v>235</v>
       </c>
       <c r="G104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I104" t="s">
         <v>437</v>
@@ -4971,10 +4971,10 @@
         <v>193</v>
       </c>
       <c r="G105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I105" t="s">
         <v>437</v>
@@ -4994,10 +4994,10 @@
         <v>347</v>
       </c>
       <c r="G106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I106" t="s">
         <v>437</v>
@@ -5017,10 +5017,10 @@
         <v>250</v>
       </c>
       <c r="G107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I107" t="s">
         <v>437</v>
@@ -5060,10 +5060,10 @@
         <v>385</v>
       </c>
       <c r="G109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I109" t="s">
         <v>438</v>
@@ -5080,10 +5080,10 @@
         <v>386</v>
       </c>
       <c r="G110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I110" t="s">
         <v>438</v>
@@ -5120,10 +5120,10 @@
         <v>227</v>
       </c>
       <c r="G112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I112" t="s">
         <v>439</v>
@@ -5169,10 +5169,10 @@
         <v>192</v>
       </c>
       <c r="G114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I114" t="s">
         <v>440</v>
@@ -5238,10 +5238,10 @@
         <v>299</v>
       </c>
       <c r="G117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I117" t="s">
         <v>441</v>

</xml_diff>

<commit_message>
npiv statistics note. single link trunk note added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -2395,8 +2395,8 @@
   <dimension ref="A1:K122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G108" sqref="G108"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G96" sqref="G96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4558,7 +4558,7 @@
         <v>0</v>
       </c>
       <c r="H86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I86" t="s">
         <v>172</v>
@@ -4678,7 +4678,7 @@
         <v>436</v>
       </c>
       <c r="G92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H92">
         <v>0</v>
@@ -4707,7 +4707,7 @@
         <v>0</v>
       </c>
       <c r="H93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I93" t="s">
         <v>437</v>
@@ -5017,7 +5017,7 @@
         <v>250</v>
       </c>
       <c r="G107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H107">
         <v>0</v>

</xml_diff>

<commit_message>
storage connection stat single fabric connection note added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1817,8 +1817,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2394,9 +2394,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G96" sqref="G96"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H95" sqref="H95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4558,7 +4558,7 @@
         <v>0</v>
       </c>
       <c r="H86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I86" t="s">
         <v>172</v>
@@ -4658,10 +4658,10 @@
         <v>443</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I91" t="s">
         <v>172</v>
@@ -4678,7 +4678,7 @@
         <v>436</v>
       </c>
       <c r="G92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H92">
         <v>0</v>

</xml_diff>

<commit_message>
switch quantity and switch connection quantity in isl_statistics
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1855,7 +1855,7 @@
   <dimension ref="A1:AL10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1898,7 +1898,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2453,8 +2453,8 @@
   <dimension ref="A1:K123"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3062,10 +3062,10 @@
         <v>468</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" t="s">
         <v>144</v>
@@ -4086,7 +4086,7 @@
         <v>0</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61" t="s">
         <v>170</v>
@@ -4146,7 +4146,7 @@
         <v>290</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -5305,7 +5305,7 @@
         <v>306</v>
       </c>
       <c r="G117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H117">
         <v>0</v>

</xml_diff>

<commit_message>
isl and ifl numbering correction
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27960" windowHeight="10560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19155" windowHeight="6840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -1855,7 +1855,7 @@
   <dimension ref="A1:AL10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2452,9 +2452,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4066,7 +4066,7 @@
         <v>0</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60" t="s">
         <v>170</v>
@@ -4086,7 +4086,7 @@
         <v>0</v>
       </c>
       <c r="H61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" t="s">
         <v>170</v>
@@ -5569,6 +5569,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
save_xlsx fn refactored to dataframe_to_report fn
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -1855,7 +1855,7 @@
   <dimension ref="A1:AL10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1898,7 +1898,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2453,8 +2453,8 @@
   <dimension ref="A1:K123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G68" sqref="G68"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4066,7 +4066,7 @@
         <v>0</v>
       </c>
       <c r="H60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" t="s">
         <v>170</v>
@@ -4106,7 +4106,7 @@
         <v>67</v>
       </c>
       <c r="G62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -4146,7 +4146,7 @@
         <v>290</v>
       </c>
       <c r="G64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64">
         <v>0</v>

</xml_diff>

<commit_message>
dataframe to report protocol changed to avoid excessive excel file access
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="474">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1430,6 +1430,18 @@
   </si>
   <si>
     <t>Fabric Shortest Path First (FSPF) link state database</t>
+  </si>
+  <si>
+    <t>LSAN zones collection</t>
+  </si>
+  <si>
+    <t>Novatek</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Novatek\SAN Assessment\SEP2021</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Novatek\SEP21\Supportinfo-Fri-2021-09-10-01-36-25-650</t>
   </si>
 </sst>
 </file>
@@ -1852,49 +1864,49 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AL10"/>
+  <dimension ref="A1:AM10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="70" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="5" width="80.140625" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" customWidth="1"/>
-    <col min="7" max="8" width="122.7109375" customWidth="1"/>
-    <col min="9" max="9" width="48.42578125" customWidth="1"/>
-    <col min="10" max="10" width="29.7109375" customWidth="1"/>
-    <col min="11" max="11" width="80.140625" customWidth="1"/>
-    <col min="12" max="12" width="68.5703125" customWidth="1"/>
-    <col min="13" max="13" width="48.7109375" customWidth="1"/>
-    <col min="14" max="14" width="62" customWidth="1"/>
-    <col min="15" max="17" width="89.5703125" customWidth="1"/>
-    <col min="18" max="18" width="69.85546875" customWidth="1"/>
-    <col min="19" max="19" width="52.140625" customWidth="1"/>
-    <col min="20" max="20" width="73.140625" customWidth="1"/>
-    <col min="21" max="21" width="29.7109375" customWidth="1"/>
-    <col min="22" max="23" width="76" customWidth="1"/>
-    <col min="24" max="24" width="72.28515625" customWidth="1"/>
-    <col min="25" max="25" width="61.7109375" customWidth="1"/>
-    <col min="26" max="26" width="60" customWidth="1"/>
-    <col min="27" max="27" width="38.140625" customWidth="1"/>
-    <col min="28" max="28" width="69" customWidth="1"/>
-    <col min="29" max="29" width="72.42578125" customWidth="1"/>
-    <col min="30" max="30" width="111.5703125" customWidth="1"/>
-    <col min="31" max="31" width="72.5703125" customWidth="1"/>
-    <col min="32" max="32" width="86.85546875" customWidth="1"/>
-    <col min="33" max="34" width="64.7109375" customWidth="1"/>
-    <col min="35" max="35" width="54.5703125" customWidth="1"/>
-    <col min="36" max="36" width="75.42578125" customWidth="1"/>
-    <col min="37" max="37" width="58.140625" customWidth="1"/>
+    <col min="2" max="3" width="70" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="80.140625" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" customWidth="1"/>
+    <col min="8" max="9" width="122.7109375" customWidth="1"/>
+    <col min="10" max="10" width="48.42578125" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" customWidth="1"/>
+    <col min="12" max="12" width="80.140625" customWidth="1"/>
+    <col min="13" max="13" width="68.5703125" customWidth="1"/>
+    <col min="14" max="14" width="48.7109375" customWidth="1"/>
+    <col min="15" max="15" width="62" customWidth="1"/>
+    <col min="16" max="18" width="89.5703125" customWidth="1"/>
+    <col min="19" max="19" width="69.85546875" customWidth="1"/>
+    <col min="20" max="20" width="52.140625" customWidth="1"/>
+    <col min="21" max="21" width="73.140625" customWidth="1"/>
+    <col min="22" max="22" width="29.7109375" customWidth="1"/>
+    <col min="23" max="24" width="76" customWidth="1"/>
+    <col min="25" max="25" width="72.28515625" customWidth="1"/>
+    <col min="26" max="26" width="61.7109375" customWidth="1"/>
+    <col min="27" max="27" width="60" customWidth="1"/>
+    <col min="28" max="28" width="38.140625" customWidth="1"/>
+    <col min="29" max="29" width="69" customWidth="1"/>
+    <col min="30" max="30" width="72.42578125" customWidth="1"/>
+    <col min="31" max="31" width="111.5703125" customWidth="1"/>
+    <col min="32" max="32" width="72.5703125" customWidth="1"/>
+    <col min="33" max="33" width="86.85546875" customWidth="1"/>
+    <col min="34" max="35" width="64.7109375" customWidth="1"/>
+    <col min="36" max="36" width="54.5703125" customWidth="1"/>
+    <col min="37" max="37" width="75.42578125" customWidth="1"/>
+    <col min="38" max="38" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
@@ -1902,51 +1914,51 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
+        <v>471</v>
+      </c>
+      <c r="D2" t="s">
         <v>458</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>427</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>238</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>405</v>
-      </c>
-      <c r="G2" t="s">
-        <v>399</v>
       </c>
       <c r="H2" t="s">
         <v>399</v>
       </c>
       <c r="I2" t="s">
+        <v>399</v>
+      </c>
+      <c r="J2" t="s">
         <v>391</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>368</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>335</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>322</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>315</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>312</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>308</v>
-      </c>
-      <c r="P2" t="s">
-        <v>316</v>
       </c>
       <c r="Q2" t="s">
         <v>316</v>
@@ -1955,144 +1967,147 @@
         <v>316</v>
       </c>
       <c r="S2" t="s">
+        <v>316</v>
+      </c>
+      <c r="T2" t="s">
         <v>278</v>
-      </c>
-      <c r="T2" t="s">
-        <v>274</v>
       </c>
       <c r="U2" t="s">
         <v>274</v>
       </c>
       <c r="V2" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="W2" t="s">
         <v>256</v>
       </c>
       <c r="X2" t="s">
+        <v>256</v>
+      </c>
+      <c r="Y2" t="s">
         <v>238</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>232</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>187</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>186</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>154</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>110</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>97</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>83</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>282</v>
       </c>
       <c r="C3" s="12">
+        <v>44453</v>
+      </c>
+      <c r="D3" s="12">
         <v>44426</v>
       </c>
-      <c r="D3" s="12">
+      <c r="E3" s="12">
         <v>44330</v>
       </c>
-      <c r="E3" s="12">
+      <c r="F3" s="12">
         <v>44307</v>
       </c>
-      <c r="F3" s="12">
+      <c r="G3" s="12">
         <v>44294</v>
       </c>
-      <c r="G3" s="12">
+      <c r="H3" s="12">
         <v>44343</v>
       </c>
-      <c r="H3" s="12">
+      <c r="I3" s="12">
         <v>44292</v>
       </c>
-      <c r="I3" s="12">
+      <c r="J3" s="12">
         <v>29681</v>
       </c>
-      <c r="J3" s="12">
+      <c r="K3" s="12">
         <v>44286</v>
       </c>
-      <c r="K3" s="12">
+      <c r="L3" s="12">
         <v>44260</v>
       </c>
-      <c r="L3" s="12">
+      <c r="M3" s="12">
         <v>44244</v>
       </c>
-      <c r="M3" s="12">
+      <c r="N3" s="12">
         <v>44245</v>
       </c>
-      <c r="N3" s="12">
+      <c r="O3" s="12">
         <v>44223</v>
       </c>
-      <c r="O3" s="12">
+      <c r="P3" s="12">
         <v>44209</v>
       </c>
-      <c r="P3" s="12">
+      <c r="Q3" s="12">
         <v>44253</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="R3" s="12">
         <v>44237</v>
       </c>
-      <c r="T3" s="12">
+      <c r="U3" s="12">
         <v>44181</v>
       </c>
-      <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM3" s="1"/>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="C4" t="s">
-        <v>326</v>
-      </c>
       <c r="D4" t="s">
         <v>326</v>
       </c>
       <c r="E4" t="s">
+        <v>326</v>
+      </c>
+      <c r="F4" t="s">
         <v>418</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>406</v>
-      </c>
-      <c r="G4" t="s">
-        <v>326</v>
       </c>
       <c r="H4" t="s">
         <v>326</v>
@@ -2101,342 +2116,351 @@
         <v>326</v>
       </c>
       <c r="J4" t="s">
+        <v>326</v>
+      </c>
+      <c r="K4" t="s">
         <v>369</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>326</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>321</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>326</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>326</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>332</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>321</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>281</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>280</v>
       </c>
-      <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM4" s="1"/>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
+        <v>472</v>
+      </c>
+      <c r="D5" t="s">
         <v>459</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>428</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>419</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>407</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>431</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>401</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>392</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>370</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>336</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>323</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>328</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>313</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>307</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>333</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>319</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>317</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>279</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>284</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>276</v>
-      </c>
-      <c r="V5" t="s">
-        <v>257</v>
       </c>
       <c r="W5" t="s">
         <v>257</v>
       </c>
       <c r="X5" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y5" t="s">
         <v>240</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>231</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>221</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>185</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>156</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>112</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>98</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>85</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>1</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>74</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>72</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>4</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>25</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AL5" t="s">
         <v>60</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AM5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C6" t="s">
+        <v>473</v>
+      </c>
+      <c r="D6" t="s">
         <v>460</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>429</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>420</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>408</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>432</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>400</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>393</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>371</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>357</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>324</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>327</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>314</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>309</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>334</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>320</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>318</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>277</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>285</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>275</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>270</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>258</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>239</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>229</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>220</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>184</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>155</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>111</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>107</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>84</v>
       </c>
-      <c r="AF6" t="s">
-        <v>0</v>
-      </c>
       <c r="AG6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH6" t="s">
         <v>73</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>71</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>3</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>24</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" t="s">
         <v>59</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AM6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>461</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>430</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>433</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>394</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>337</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>310</v>
-      </c>
-      <c r="V7" t="s">
-        <v>259</v>
       </c>
       <c r="W7" t="s">
         <v>259</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="X7" t="s">
+        <v>259</v>
+      </c>
+      <c r="Z7" t="s">
         <v>230</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>157</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>108</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>87</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AI7" t="s">
         <v>99</v>
       </c>
-      <c r="AK7" t="s">
+      <c r="AL7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>421</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>338</v>
-      </c>
-      <c r="V8" t="s">
-        <v>261</v>
       </c>
       <c r="W8" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="X8" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>359</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>434</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>237</v>
       </c>
@@ -2453,8 +2477,8 @@
   <dimension ref="A1:K123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3190,7 +3214,7 @@
         <v>142</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>216</v>
+        <v>470</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -4106,7 +4130,7 @@
         <v>67</v>
       </c>
       <c r="G62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -5210,10 +5234,10 @@
         <v>227</v>
       </c>
       <c r="G113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I113" t="s">
         <v>439</v>

</xml_diff>

<commit_message>
change fn for report generation
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -2477,8 +2477,8 @@
   <dimension ref="A1:K123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H59" sqref="H59"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3958,10 +3958,10 @@
         <v>62</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" t="s">
         <v>169</v>
@@ -4962,10 +4962,10 @@
         <v>180</v>
       </c>
       <c r="G100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I100" t="s">
         <v>437</v>

</xml_diff>

<commit_message>
switch connection statistics added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19155" windowHeight="6840" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19155" windowHeight="6840"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,14 @@
     <sheet name="software" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$K$123</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$K$124</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="482">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -697,9 +697,6 @@
     <t>DATA COLLECTION 11. SENSOR READINGS</t>
   </si>
   <si>
-    <t>DATA COLLECTION 12. BLADE SYSTEMS</t>
-  </si>
-  <si>
     <t>sensor_aggregated</t>
   </si>
   <si>
@@ -823,9 +820,6 @@
     <t>Synergy servers and mezzanine</t>
   </si>
   <si>
-    <t>DATA COLLECTION 13. SYNERGY SYSTEMS</t>
-  </si>
-  <si>
     <t>Port statistics</t>
   </si>
   <si>
@@ -1108,9 +1102,6 @@
     <t>host_3par</t>
   </si>
   <si>
-    <t>DATA COLLECTION 14. 3PAR STORAGES</t>
-  </si>
-  <si>
     <t>collection_3par</t>
   </si>
   <si>
@@ -1333,21 +1324,6 @@
     <t>Статистика_NPIV</t>
   </si>
   <si>
-    <t>DATA ANALYSIS 7. ZONING CONFIGURATION</t>
-  </si>
-  <si>
-    <t>DATA ANALYSIS 8. STORAGE HOST PRESENTATION</t>
-  </si>
-  <si>
-    <t>DATA ANALYSIS 9. SENSOR READINGS</t>
-  </si>
-  <si>
-    <t>DATA ANALYSIS 10. FABRIC STATISTICS</t>
-  </si>
-  <si>
-    <t>DATA ANALYSIS 11. RASLOG</t>
-  </si>
-  <si>
     <t>Статистическая информация о портах NPIV</t>
   </si>
   <si>
@@ -1366,9 +1342,6 @@
     <t>Настройки и сообщения службы MAPS</t>
   </si>
   <si>
-    <t>NPIV_</t>
-  </si>
-  <si>
     <t>fabric_labels_summary</t>
   </si>
   <si>
@@ -1441,7 +1414,58 @@
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Novatek\SAN Assessment\SEP2021</t>
   </si>
   <si>
-    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Novatek\SEP21\Supportinfo-Fri-2021-09-10-01-36-25-650</t>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Novatek\SEP21\ssave</t>
+  </si>
+  <si>
+    <t>fcrproxydev  collection</t>
+  </si>
+  <si>
+    <t>fcrphydev collection</t>
+  </si>
+  <si>
+    <t>Edge fabrics collection</t>
+  </si>
+  <si>
+    <t>DATA COLLECTION 13. BLADE SYSTEMS</t>
+  </si>
+  <si>
+    <t>DATA COLLECTION 14. SYNERGY SYSTEMS</t>
+  </si>
+  <si>
+    <t>DATA COLLECTION 15. 3PAR STORAGES</t>
+  </si>
+  <si>
+    <t>Статистика_соединений</t>
+  </si>
+  <si>
+    <t>Статистическая информация о  соединении коммутаторов</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 7. MAPS PORTS, NPIV PORTS, NPIV AND SWITCH CONNECTION STATISTICS</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 8. ZONING CONFIGURATION</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 9. STORAGE HOST PRESENTATION</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 10. SENSOR READINGS</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 11. FABRIC STATISTICS</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 12. RASLOG</t>
+  </si>
+  <si>
+    <t>analysis_maps_npiv_ports</t>
+  </si>
+  <si>
+    <t>Connection_statistics</t>
+  </si>
+  <si>
+    <t>Switch connection statistics</t>
   </si>
 </sst>
 </file>
@@ -1866,8 +1890,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AM10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1910,7 +1934,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1919,76 +1943,76 @@
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="D2" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="E2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="F2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G2" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="H2" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="I2" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="J2" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="K2" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="L2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="M2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="N2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="P2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="Q2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="R2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="S2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="T2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="U2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="V2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="W2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="X2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Y2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Z2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AA2" t="s">
         <v>187</v>
@@ -2032,7 +2056,7 @@
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C3" s="12">
         <v>44453</v>
@@ -2095,55 +2119,55 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F4" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="G4" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="H4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="I4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="J4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K4" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="L4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="M4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="N4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="P4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="Q4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="R4" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="U4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="V4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
@@ -2158,76 +2182,76 @@
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="D5" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="E5" t="s">
+        <v>425</v>
+      </c>
+      <c r="F5" t="s">
+        <v>416</v>
+      </c>
+      <c r="G5" t="s">
+        <v>404</v>
+      </c>
+      <c r="H5" t="s">
         <v>428</v>
       </c>
-      <c r="F5" t="s">
-        <v>419</v>
-      </c>
-      <c r="G5" t="s">
-        <v>407</v>
-      </c>
-      <c r="H5" t="s">
-        <v>431</v>
-      </c>
       <c r="I5" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="J5" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="K5" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="L5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="M5" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="N5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="O5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="P5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="Q5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="R5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="S5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="T5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="U5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="V5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="W5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="X5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Y5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Z5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AA5" t="s">
         <v>221</v>
@@ -2274,76 +2298,76 @@
         <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="D6" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="E6" t="s">
+        <v>426</v>
+      </c>
+      <c r="F6" t="s">
+        <v>417</v>
+      </c>
+      <c r="G6" t="s">
+        <v>405</v>
+      </c>
+      <c r="H6" t="s">
         <v>429</v>
       </c>
-      <c r="F6" t="s">
-        <v>420</v>
-      </c>
-      <c r="G6" t="s">
-        <v>408</v>
-      </c>
-      <c r="H6" t="s">
-        <v>432</v>
-      </c>
       <c r="I6" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="J6" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="K6" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="L6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="M6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="N6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="O6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="P6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="Q6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="R6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="S6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="T6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="U6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="V6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="W6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="X6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Y6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Z6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AA6" t="s">
         <v>220</v>
@@ -2390,31 +2414,31 @@
         <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="E7" t="s">
+        <v>427</v>
+      </c>
+      <c r="H7" t="s">
         <v>430</v>
       </c>
-      <c r="H7" t="s">
-        <v>433</v>
-      </c>
       <c r="J7" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="L7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="P7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="W7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="X7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Z7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AC7" t="s">
         <v>157</v>
@@ -2434,35 +2458,35 @@
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="F8" t="s">
+        <v>418</v>
+      </c>
+      <c r="L8" t="s">
+        <v>336</v>
+      </c>
+      <c r="W8" t="s">
         <v>260</v>
       </c>
-      <c r="F8" t="s">
-        <v>421</v>
-      </c>
-      <c r="L8" t="s">
-        <v>338</v>
-      </c>
-      <c r="W8" t="s">
-        <v>261</v>
-      </c>
       <c r="X8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="H9" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="J9" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2474,11 +2498,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K123"/>
+  <dimension ref="A1:K124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H56" sqref="H56"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2525,7 +2549,7 @@
         <v>194</v>
       </c>
       <c r="K1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2615,7 +2639,7 @@
         <v>141</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2647,7 +2671,7 @@
         <v>150</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2679,7 +2703,7 @@
         <v>150</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2711,7 +2735,7 @@
         <v>151</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2743,7 +2767,7 @@
         <v>147</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2775,7 +2799,7 @@
         <v>147</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2807,7 +2831,7 @@
         <v>145</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2839,7 +2863,7 @@
         <v>146</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2871,7 +2895,7 @@
         <v>146</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2903,7 +2927,7 @@
         <v>143</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2935,7 +2959,7 @@
         <v>143</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2967,7 +2991,7 @@
         <v>143</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2999,7 +3023,7 @@
         <v>144</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -3031,7 +3055,7 @@
         <v>144</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -3063,7 +3087,7 @@
         <v>144</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -3080,10 +3104,10 @@
         <v>94</v>
       </c>
       <c r="E19" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -3095,7 +3119,7 @@
         <v>144</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -3127,7 +3151,7 @@
         <v>142</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -3156,7 +3180,7 @@
         <v>142</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>216</v>
+        <v>465</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -3185,7 +3209,7 @@
         <v>142</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>216</v>
+        <v>466</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -3214,7 +3238,7 @@
         <v>142</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -3240,7 +3264,7 @@
         <v>142</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>216</v>
+        <v>467</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -3295,7 +3319,7 @@
         <v>148</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -3321,7 +3345,7 @@
         <v>148</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -3347,7 +3371,7 @@
         <v>148</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -3373,7 +3397,7 @@
         <v>148</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -3399,7 +3423,7 @@
         <v>148</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -3413,7 +3437,7 @@
         <v>94</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -3425,7 +3449,7 @@
         <v>148</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -3439,7 +3463,7 @@
         <v>94</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -3451,7 +3475,7 @@
         <v>148</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -3477,33 +3501,33 @@
         <v>224</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F34" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
+        <v>291</v>
+      </c>
+      <c r="J34" s="10" t="s">
         <v>292</v>
-      </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34" t="s">
-        <v>293</v>
-      </c>
-      <c r="J34" s="10" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -3529,10 +3553,10 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>225</v>
+        <v>468</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -3555,10 +3579,10 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>225</v>
+        <v>468</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -3581,22 +3605,22 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>225</v>
+        <v>468</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -3605,22 +3629,22 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>267</v>
+        <v>469</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -3629,22 +3653,22 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>267</v>
+        <v>469</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -3653,22 +3677,22 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>362</v>
+        <v>470</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -3677,22 +3701,22 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>362</v>
+        <v>470</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -3701,22 +3725,22 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
+        <v>470</v>
+      </c>
+      <c r="J42" s="10" t="s">
         <v>362</v>
-      </c>
-      <c r="J42" s="10" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -3725,10 +3749,10 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>362</v>
+        <v>470</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -3762,7 +3786,7 @@
         <v>95</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="G45">
         <v>0</v>
@@ -3794,7 +3818,7 @@
         <v>158</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -3837,7 +3861,7 @@
         <v>162</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -3883,7 +3907,7 @@
         <v>169</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -3892,7 +3916,7 @@
       </c>
       <c r="E51" s="16"/>
       <c r="F51" s="2" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -3904,10 +3928,10 @@
         <v>169</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="K51" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -3938,10 +3962,10 @@
         <v>61</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" t="s">
         <v>169</v>
@@ -4035,7 +4059,7 @@
         <v>96</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -4047,7 +4071,7 @@
         <v>169</v>
       </c>
       <c r="J58" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -4055,7 +4079,7 @@
         <v>96</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -4067,10 +4091,10 @@
         <v>169</v>
       </c>
       <c r="J59" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="K59" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -4096,7 +4120,7 @@
         <v>170</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -4104,7 +4128,7 @@
         <v>95</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -4116,10 +4140,10 @@
         <v>170</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="K61" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -4167,7 +4191,7 @@
         <v>96</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -4179,10 +4203,10 @@
         <v>170</v>
       </c>
       <c r="J64" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="K64" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -4208,7 +4232,7 @@
         <v>171</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -4216,7 +4240,7 @@
         <v>95</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -4228,10 +4252,10 @@
         <v>171</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="K66" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -4239,7 +4263,7 @@
         <v>95</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -4251,10 +4275,10 @@
         <v>171</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="K67" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -4262,7 +4286,7 @@
         <v>95</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -4274,7 +4298,7 @@
         <v>171</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -4282,7 +4306,7 @@
         <v>95</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -4294,15 +4318,15 @@
         <v>171</v>
       </c>
       <c r="J69" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D70" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="F70" s="11" t="s">
         <v>246</v>
-      </c>
-      <c r="F70" s="11" t="s">
-        <v>247</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -4314,7 +4338,7 @@
         <v>171</v>
       </c>
       <c r="J70" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -4337,7 +4361,7 @@
         <v>171</v>
       </c>
       <c r="J71" s="10" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -4363,7 +4387,7 @@
         <v>171</v>
       </c>
       <c r="J72" s="10" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -4371,7 +4395,7 @@
         <v>95</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -4383,7 +4407,7 @@
         <v>171</v>
       </c>
       <c r="J73" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -4394,7 +4418,7 @@
         <v>96</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -4537,7 +4561,7 @@
         <v>96</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -4549,10 +4573,10 @@
         <v>171</v>
       </c>
       <c r="J81" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="K81" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.25">
@@ -4560,7 +4584,7 @@
         <v>96</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -4572,41 +4596,41 @@
         <v>171</v>
       </c>
       <c r="J82" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="K82" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D83" s="5" t="s">
+      <c r="B83" t="s">
+        <v>165</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83" t="s">
+        <v>172</v>
+      </c>
+      <c r="J83" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D84" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F83" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="G83">
-        <v>0</v>
-      </c>
-      <c r="H83">
-        <v>0</v>
-      </c>
-      <c r="I83" t="s">
-        <v>171</v>
-      </c>
-      <c r="J83" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>165</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>218</v>
+      <c r="F84" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -4618,15 +4642,15 @@
         <v>172</v>
       </c>
       <c r="J84" t="s">
-        <v>303</v>
+        <v>202</v>
       </c>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D85" s="6" t="s">
-        <v>95</v>
+      <c r="D85" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>450</v>
+        <v>167</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -4638,15 +4662,15 @@
         <v>172</v>
       </c>
       <c r="J85" t="s">
-        <v>452</v>
+        <v>212</v>
       </c>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D86" s="6" t="s">
-        <v>95</v>
+      <c r="D86" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>448</v>
+        <v>168</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -4658,15 +4682,18 @@
         <v>172</v>
       </c>
       <c r="J86" t="s">
-        <v>445</v>
+        <v>267</v>
       </c>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>479</v>
+      </c>
       <c r="D87" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -4675,21 +4702,18 @@
         <v>0</v>
       </c>
       <c r="I87" t="s">
-        <v>172</v>
+        <v>473</v>
       </c>
       <c r="J87" t="s">
-        <v>444</v>
-      </c>
-      <c r="K87" t="s">
-        <v>404</v>
+        <v>443</v>
       </c>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D88" s="5" t="s">
-        <v>96</v>
+      <c r="D88" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -4698,18 +4722,18 @@
         <v>0</v>
       </c>
       <c r="I88" t="s">
-        <v>172</v>
+        <v>473</v>
       </c>
       <c r="J88" t="s">
-        <v>202</v>
+        <v>437</v>
       </c>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D89" s="5" t="s">
-        <v>96</v>
+      <c r="D89" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>167</v>
+        <v>432</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -4718,18 +4742,21 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>172</v>
+        <v>473</v>
       </c>
       <c r="J89" t="s">
-        <v>212</v>
+        <v>436</v>
+      </c>
+      <c r="K89" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D90" s="5" t="s">
-        <v>96</v>
+      <c r="D90" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>168</v>
+        <v>480</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -4738,10 +4765,13 @@
         <v>0</v>
       </c>
       <c r="I90" t="s">
-        <v>172</v>
+        <v>473</v>
       </c>
       <c r="J90" t="s">
-        <v>269</v>
+        <v>481</v>
+      </c>
+      <c r="K90" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.25">
@@ -4749,7 +4779,7 @@
         <v>96</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -4758,10 +4788,10 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>172</v>
+        <v>473</v>
       </c>
       <c r="J91" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.25">
@@ -4769,7 +4799,7 @@
         <v>96</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -4778,7 +4808,7 @@
         <v>0</v>
       </c>
       <c r="I92" t="s">
-        <v>172</v>
+        <v>473</v>
       </c>
       <c r="J92" t="s">
         <v>201</v>
@@ -4789,7 +4819,7 @@
         <v>96</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -4798,47 +4828,47 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>172</v>
+        <v>473</v>
       </c>
       <c r="J93" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="K93" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
-        <v>176</v>
-      </c>
-      <c r="D94" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F94" s="9" t="s">
-        <v>177</v>
+      <c r="D94" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>471</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I94" t="s">
-        <v>437</v>
-      </c>
-      <c r="J94" s="10" t="s">
-        <v>343</v>
+        <v>473</v>
+      </c>
+      <c r="J94" t="s">
+        <v>472</v>
+      </c>
+      <c r="K94" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>253</v>
+        <v>176</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F95" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -4847,21 +4877,21 @@
         <v>0</v>
       </c>
       <c r="I95" t="s">
-        <v>437</v>
+        <v>474</v>
       </c>
       <c r="J95" s="10" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D96" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F96" s="9" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -4870,13 +4900,10 @@
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>437</v>
+        <v>474</v>
       </c>
       <c r="J96" s="10" t="s">
-        <v>345</v>
-      </c>
-      <c r="K96" t="s">
-        <v>404</v>
+        <v>342</v>
       </c>
     </row>
     <row r="97" spans="2:11" x14ac:dyDescent="0.25">
@@ -4887,7 +4914,7 @@
         <v>95</v>
       </c>
       <c r="F97" s="9" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -4896,21 +4923,24 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>437</v>
+        <v>474</v>
       </c>
       <c r="J97" s="10" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="K97" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="98" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>253</v>
+      </c>
       <c r="D98" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="9" t="s">
-        <v>341</v>
+        <v>217</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -4919,59 +4949,62 @@
         <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>437</v>
+        <v>474</v>
       </c>
       <c r="J98" s="10" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="K98" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="99" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>252</v>
-      </c>
       <c r="D99" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F99" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99" t="s">
+        <v>474</v>
+      </c>
+      <c r="J99" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K99" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>251</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100" t="s">
+        <v>474</v>
+      </c>
+      <c r="J100" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="G99">
-        <v>0</v>
-      </c>
-      <c r="H99">
-        <v>0</v>
-      </c>
-      <c r="I99" t="s">
-        <v>437</v>
-      </c>
-      <c r="J99" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="K99" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D100" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="G100">
-        <v>1</v>
-      </c>
-      <c r="H100">
-        <v>1</v>
-      </c>
-      <c r="I100" t="s">
-        <v>437</v>
-      </c>
-      <c r="J100" t="s">
-        <v>213</v>
+      <c r="K100" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="101" spans="2:11" x14ac:dyDescent="0.25">
@@ -4979,7 +5012,7 @@
         <v>96</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -4988,10 +5021,10 @@
         <v>0</v>
       </c>
       <c r="I101" t="s">
-        <v>437</v>
+        <v>474</v>
       </c>
       <c r="J101" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="102" spans="2:11" x14ac:dyDescent="0.25">
@@ -4999,7 +5032,7 @@
         <v>96</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -5008,10 +5041,10 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>437</v>
+        <v>474</v>
       </c>
       <c r="J102" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="103" spans="2:11" x14ac:dyDescent="0.25">
@@ -5019,7 +5052,7 @@
         <v>96</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -5028,10 +5061,10 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>437</v>
+        <v>474</v>
       </c>
       <c r="J103" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="104" spans="2:11" x14ac:dyDescent="0.25">
@@ -5039,7 +5072,7 @@
         <v>96</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>233</v>
+        <v>190</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -5048,10 +5081,10 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>437</v>
+        <v>474</v>
       </c>
       <c r="J104" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
     </row>
     <row r="105" spans="2:11" x14ac:dyDescent="0.25">
@@ -5059,7 +5092,7 @@
         <v>96</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -5068,13 +5101,10 @@
         <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>437</v>
+        <v>474</v>
       </c>
       <c r="J105" t="s">
-        <v>236</v>
-      </c>
-      <c r="K105" t="s">
-        <v>404</v>
+        <v>233</v>
       </c>
     </row>
     <row r="106" spans="2:11" x14ac:dyDescent="0.25">
@@ -5082,7 +5112,7 @@
         <v>96</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>193</v>
+        <v>234</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -5091,13 +5121,13 @@
         <v>0</v>
       </c>
       <c r="I106" t="s">
-        <v>437</v>
+        <v>474</v>
       </c>
       <c r="J106" t="s">
-        <v>348</v>
+        <v>235</v>
       </c>
       <c r="K106" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="107" spans="2:11" x14ac:dyDescent="0.25">
@@ -5105,7 +5135,7 @@
         <v>96</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>347</v>
+        <v>193</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -5114,13 +5144,13 @@
         <v>0</v>
       </c>
       <c r="I107" t="s">
-        <v>437</v>
+        <v>474</v>
       </c>
       <c r="J107" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="K107" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="108" spans="2:11" x14ac:dyDescent="0.25">
@@ -5128,62 +5158,65 @@
         <v>96</v>
       </c>
       <c r="F108" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+      <c r="H108">
+        <v>0</v>
+      </c>
+      <c r="I108" t="s">
+        <v>474</v>
+      </c>
+      <c r="J108" t="s">
+        <v>347</v>
+      </c>
+      <c r="K108" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D109" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
+      <c r="I109" t="s">
+        <v>474</v>
+      </c>
+      <c r="J109" t="s">
         <v>250</v>
       </c>
-      <c r="G108">
-        <v>0</v>
-      </c>
-      <c r="H108">
-        <v>0</v>
-      </c>
-      <c r="I108" t="s">
-        <v>437</v>
-      </c>
-      <c r="J108" t="s">
-        <v>251</v>
-      </c>
-      <c r="K108" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D109" s="6" t="s">
+      <c r="K109" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D110" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F109" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="G109">
-        <v>0</v>
-      </c>
-      <c r="H109">
-        <v>0</v>
-      </c>
-      <c r="I109" t="s">
-        <v>438</v>
-      </c>
-      <c r="J109" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D110" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="F110" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="I110" t="s">
+        <v>475</v>
+      </c>
+      <c r="J110" t="s">
         <v>385</v>
-      </c>
-      <c r="G110">
-        <v>0</v>
-      </c>
-      <c r="H110">
-        <v>0</v>
-      </c>
-      <c r="I110" t="s">
-        <v>438</v>
-      </c>
-      <c r="J110" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="111" spans="2:11" x14ac:dyDescent="0.25">
@@ -5191,123 +5224,117 @@
         <v>96</v>
       </c>
       <c r="F111" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+      <c r="H111">
+        <v>0</v>
+      </c>
+      <c r="I111" t="s">
+        <v>475</v>
+      </c>
+      <c r="J111" t="s">
         <v>386</v>
       </c>
-      <c r="G111">
-        <v>0</v>
-      </c>
-      <c r="H111">
-        <v>0</v>
-      </c>
-      <c r="I111" t="s">
-        <v>438</v>
-      </c>
-      <c r="J111" t="s">
-        <v>390</v>
-      </c>
     </row>
     <row r="112" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D112" s="6" t="s">
+      <c r="D112" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="G112">
+        <v>0</v>
+      </c>
+      <c r="H112">
+        <v>0</v>
+      </c>
+      <c r="I112" t="s">
+        <v>475</v>
+      </c>
+      <c r="J112" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D113" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F112" s="2" t="s">
+      <c r="F113" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+      <c r="H113">
+        <v>0</v>
+      </c>
+      <c r="I113" t="s">
+        <v>476</v>
+      </c>
+      <c r="J113" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D114" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F114" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="G112">
-        <v>0</v>
-      </c>
-      <c r="H112">
-        <v>0</v>
-      </c>
-      <c r="I112" t="s">
-        <v>439</v>
-      </c>
-      <c r="J112" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D113" s="5" t="s">
+      <c r="G114">
+        <v>0</v>
+      </c>
+      <c r="H114">
+        <v>0</v>
+      </c>
+      <c r="I114" t="s">
+        <v>476</v>
+      </c>
+      <c r="J114" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>17</v>
+      </c>
+      <c r="B115" t="s">
+        <v>136</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F115" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>0</v>
+      </c>
+      <c r="I115" t="s">
+        <v>477</v>
+      </c>
+      <c r="J115" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="K115" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D116" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F113" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="G113">
-        <v>1</v>
-      </c>
-      <c r="H113">
-        <v>1</v>
-      </c>
-      <c r="I113" t="s">
-        <v>439</v>
-      </c>
-      <c r="J113" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A114">
-        <v>17</v>
-      </c>
-      <c r="B114" t="s">
-        <v>136</v>
-      </c>
-      <c r="D114" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F114" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="G114">
-        <v>0</v>
-      </c>
-      <c r="H114">
-        <v>0</v>
-      </c>
-      <c r="I114" t="s">
-        <v>440</v>
-      </c>
-      <c r="J114" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="K114" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D115" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F115" s="2" t="s">
+      <c r="F116" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G115">
-        <v>0</v>
-      </c>
-      <c r="H115">
-        <v>0</v>
-      </c>
-      <c r="I115" t="s">
-        <v>440</v>
-      </c>
-      <c r="J115" t="s">
-        <v>358</v>
-      </c>
-      <c r="K115" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B116" t="s">
-        <v>297</v>
-      </c>
-      <c r="D116" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F116" s="9" t="s">
-        <v>298</v>
-      </c>
       <c r="G116">
         <v>0</v>
       </c>
@@ -5315,18 +5342,24 @@
         <v>0</v>
       </c>
       <c r="I116" t="s">
-        <v>441</v>
+        <v>477</v>
       </c>
       <c r="J116" t="s">
-        <v>301</v>
+        <v>356</v>
+      </c>
+      <c r="K116" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>295</v>
+      </c>
       <c r="D117" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F117" s="2" t="s">
-        <v>306</v>
+      <c r="F117" s="9" t="s">
+        <v>296</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -5335,21 +5368,18 @@
         <v>0</v>
       </c>
       <c r="I117" t="s">
-        <v>441</v>
+        <v>478</v>
       </c>
       <c r="J117" t="s">
-        <v>302</v>
-      </c>
-      <c r="K117" t="s">
-        <v>404</v>
+        <v>299</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D118" s="5" t="s">
-        <v>96</v>
+      <c r="D118" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -5358,44 +5388,47 @@
         <v>0</v>
       </c>
       <c r="I118" t="s">
-        <v>441</v>
+        <v>478</v>
       </c>
       <c r="J118" t="s">
         <v>300</v>
       </c>
       <c r="K118" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B119" t="s">
+      <c r="D119" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+      <c r="H119">
+        <v>0</v>
+      </c>
+      <c r="I119" t="s">
+        <v>478</v>
+      </c>
+      <c r="J119" t="s">
+        <v>298</v>
+      </c>
+      <c r="K119" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
         <v>176</v>
       </c>
-      <c r="D119" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F119" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="G119">
-        <v>0</v>
-      </c>
-      <c r="H119">
-        <v>0</v>
-      </c>
-      <c r="I119" t="s">
-        <v>178</v>
-      </c>
-      <c r="J119" s="10" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D120" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F120" s="2" t="s">
-        <v>329</v>
+      <c r="F120" s="9" t="s">
+        <v>323</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -5415,7 +5448,7 @@
         <v>95</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -5435,7 +5468,7 @@
         <v>95</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -5455,7 +5488,7 @@
         <v>95</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>372</v>
+        <v>328</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -5464,10 +5497,30 @@
         <v>0</v>
       </c>
       <c r="I123" t="s">
-        <v>373</v>
-      </c>
-      <c r="J123" s="2" t="s">
-        <v>372</v>
+        <v>178</v>
+      </c>
+      <c r="J123" s="10" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D124" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="G124">
+        <v>0</v>
+      </c>
+      <c r="H124">
+        <v>0</v>
+      </c>
+      <c r="I124" t="s">
+        <v>370</v>
+      </c>
+      <c r="J124" s="2" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -5482,7 +5535,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5609,10 +5662,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>79</v>
@@ -5620,18 +5673,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="B3" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="C3" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
switch connection and switch models aymmetry notes added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="483">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1466,6 +1466,9 @@
   </si>
   <si>
     <t>Switch connection statistics</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Novatek\SEP21\synergy</t>
   </si>
 </sst>
 </file>
@@ -1890,8 +1893,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AM10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1937,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2459,6 +2462,9 @@
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>259</v>
+      </c>
+      <c r="C8" t="s">
+        <v>482</v>
       </c>
       <c r="F8" t="s">
         <v>418</v>
@@ -2501,8 +2507,8 @@
   <dimension ref="A1:K124"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F83" sqref="F83"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3626,7 +3632,7 @@
         <v>0</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" t="s">
         <v>469</v>
@@ -3650,7 +3656,7 @@
         <v>0</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" t="s">
         <v>469</v>
@@ -3872,10 +3878,10 @@
         <v>160</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49" t="s">
         <v>162</v>
@@ -4421,10 +4427,10 @@
         <v>419</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I74" t="s">
         <v>171</v>
@@ -4845,10 +4851,10 @@
         <v>471</v>
       </c>
       <c r="G94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I94" t="s">
         <v>473</v>

</xml_diff>

<commit_message>
transition to sql database
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -2496,8 +2496,8 @@
   <dimension ref="A1:L120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G64" sqref="G64"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4276,7 +4276,7 @@
         <v>442</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -4660,7 +4660,7 @@
         <v>413</v>
       </c>
       <c r="G75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -4686,7 +4686,7 @@
         <v>101</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -4709,7 +4709,7 @@
         <v>102</v>
       </c>
       <c r="G77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H77">
         <v>0</v>

</xml_diff>

<commit_message>
transition to sql database completed
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -587,9 +587,6 @@
     <t>zonemember_statistics</t>
   </si>
   <si>
-    <t>Зонирование_A&amp;B</t>
-  </si>
-  <si>
     <t>Порты_не_в_зонах</t>
   </si>
   <si>
@@ -1154,9 +1151,6 @@
     <t>Презентация</t>
   </si>
   <si>
-    <t>Презентация_A&amp;B</t>
-  </si>
-  <si>
     <t>storage_host_aggregated</t>
   </si>
   <si>
@@ -1458,6 +1452,12 @@
   </si>
   <si>
     <t>Содержание</t>
+  </si>
+  <si>
+    <t>Зонирование_AB</t>
+  </si>
+  <si>
+    <t>Презентация_AB</t>
   </si>
 </sst>
 </file>
@@ -1935,76 +1935,76 @@
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="F2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="J2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="K2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="M2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="N2" t="s">
+        <v>311</v>
+      </c>
+      <c r="O2" t="s">
+        <v>308</v>
+      </c>
+      <c r="P2" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q2" t="s">
         <v>312</v>
       </c>
-      <c r="O2" t="s">
-        <v>309</v>
-      </c>
-      <c r="P2" t="s">
-        <v>305</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>313</v>
-      </c>
       <c r="R2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="S2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="T2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="U2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="V2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="W2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="X2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Y2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Z2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AA2" t="s">
         <v>186</v>
@@ -2048,7 +2048,7 @@
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C3" s="12">
         <v>44453</v>
@@ -2111,55 +2111,55 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G4" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="P4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="Q4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="R4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="U4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="V4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
@@ -2174,79 +2174,79 @@
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D5" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="F5" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="I5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="J5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="M5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="N5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="O5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Q5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="T5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="U5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="V5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="W5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="X5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Y5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Z5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AA5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AB5" t="s">
         <v>184</v>
@@ -2290,79 +2290,79 @@
         <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D6" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="G6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="I6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="J6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="N6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="O6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q6" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="R6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="S6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="T6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="U6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="V6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="W6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="X6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Y6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Z6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AA6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AB6" t="s">
         <v>183</v>
@@ -2406,31 +2406,31 @@
         <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E7" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H7" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="J7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="W7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="X7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Z7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AC7" t="s">
         <v>157</v>
@@ -2450,38 +2450,38 @@
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C8" t="s">
+        <v>474</v>
+      </c>
+      <c r="F8" t="s">
+        <v>410</v>
+      </c>
+      <c r="L8" t="s">
+        <v>331</v>
+      </c>
+      <c r="W8" t="s">
         <v>258</v>
       </c>
-      <c r="C8" t="s">
-        <v>476</v>
-      </c>
-      <c r="F8" t="s">
-        <v>412</v>
-      </c>
-      <c r="L8" t="s">
-        <v>332</v>
-      </c>
-      <c r="W8" t="s">
-        <v>259</v>
-      </c>
       <c r="X8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H9" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="J9" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -2496,8 +2496,8 @@
   <dimension ref="A1:L120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H84" sqref="H84"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2543,13 +2543,13 @@
         <v>149</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="L1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2557,7 +2557,7 @@
         <v>94</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -2566,10 +2566,10 @@
         <v>0</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2601,7 +2601,7 @@
         <v>152</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K3" s="10">
         <v>1</v>
@@ -2633,7 +2633,7 @@
         <v>152</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K4" s="10">
         <v>1</v>
@@ -2668,7 +2668,7 @@
         <v>141</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K5" s="10">
         <v>1</v>
@@ -2703,7 +2703,7 @@
         <v>150</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K6" s="10">
         <v>1</v>
@@ -2738,7 +2738,7 @@
         <v>150</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K7" s="10">
         <v>1</v>
@@ -2767,13 +2767,13 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="s">
         <v>151</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K8" s="10">
         <v>1</v>
@@ -2808,7 +2808,7 @@
         <v>147</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K9" s="10">
         <v>1</v>
@@ -2843,7 +2843,7 @@
         <v>147</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K10" s="10">
         <v>1</v>
@@ -2878,7 +2878,7 @@
         <v>145</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="K11" s="10">
         <v>1</v>
@@ -2913,7 +2913,7 @@
         <v>146</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="K12" s="10">
         <v>1</v>
@@ -2948,7 +2948,7 @@
         <v>146</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="K13" s="10">
         <v>1</v>
@@ -2983,7 +2983,7 @@
         <v>143</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K14" s="10">
         <v>1</v>
@@ -3018,7 +3018,7 @@
         <v>143</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="K15" s="10">
         <v>1</v>
@@ -3053,7 +3053,7 @@
         <v>143</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K16" s="10">
         <v>1</v>
@@ -3088,7 +3088,7 @@
         <v>144</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="K17" s="10">
         <v>1</v>
@@ -3123,7 +3123,7 @@
         <v>144</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="K18" s="10">
         <v>1</v>
@@ -3158,7 +3158,7 @@
         <v>144</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="K19" s="10">
         <v>1</v>
@@ -3178,10 +3178,10 @@
         <v>94</v>
       </c>
       <c r="E20" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -3193,7 +3193,7 @@
         <v>144</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="K20" s="10">
         <v>1</v>
@@ -3228,7 +3228,7 @@
         <v>142</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="K21" s="10">
         <v>1</v>
@@ -3260,7 +3260,7 @@
         <v>142</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="K22" s="10">
         <v>1</v>
@@ -3292,7 +3292,7 @@
         <v>142</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="K23" s="10">
         <v>1</v>
@@ -3324,7 +3324,7 @@
         <v>142</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="K24" s="10">
         <v>1</v>
@@ -3353,7 +3353,7 @@
         <v>142</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="K25" s="10">
         <v>1</v>
@@ -3382,7 +3382,7 @@
         <v>142</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K26" s="10">
         <v>1</v>
@@ -3414,7 +3414,7 @@
         <v>148</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K27" s="10">
         <v>1</v>
@@ -3443,7 +3443,7 @@
         <v>148</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K28" s="10">
         <v>1</v>
@@ -3472,7 +3472,7 @@
         <v>148</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K29" s="10">
         <v>1</v>
@@ -3501,7 +3501,7 @@
         <v>148</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K30" s="10">
         <v>1</v>
@@ -3530,7 +3530,7 @@
         <v>148</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K31" s="10">
         <v>1</v>
@@ -3547,7 +3547,7 @@
         <v>94</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -3559,7 +3559,7 @@
         <v>148</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="K32" s="10">
         <v>1</v>
@@ -3576,7 +3576,7 @@
         <v>94</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -3588,7 +3588,7 @@
         <v>148</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K33" s="10">
         <v>1</v>
@@ -3596,28 +3596,28 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>221</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>222</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F34" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
         <v>222</v>
       </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-      <c r="I34" t="s">
-        <v>223</v>
-      </c>
       <c r="J34" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K34" s="10">
         <v>1</v>
@@ -3625,28 +3625,28 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>292</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>293</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F35" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
         <v>289</v>
       </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="J35" s="10" t="s">
         <v>290</v>
-      </c>
-      <c r="J35" s="10" t="s">
-        <v>291</v>
       </c>
       <c r="K35" s="10">
         <v>1</v>
@@ -3675,10 +3675,10 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="K36" s="10">
         <v>1</v>
@@ -3704,10 +3704,10 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="K37" s="10">
         <v>1</v>
@@ -3733,10 +3733,10 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="K38" s="10">
         <v>1</v>
@@ -3744,14 +3744,14 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -3760,10 +3760,10 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K39" s="10">
         <v>1</v>
@@ -3771,14 +3771,14 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -3787,10 +3787,10 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K40" s="10">
         <v>1</v>
@@ -3798,26 +3798,26 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F41" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41" t="s">
+        <v>462</v>
+      </c>
+      <c r="J41" s="10" t="s">
         <v>359</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41" t="s">
-        <v>464</v>
-      </c>
-      <c r="J41" s="10" t="s">
-        <v>360</v>
       </c>
       <c r="K41" s="10">
         <v>1</v>
@@ -3825,14 +3825,14 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -3841,10 +3841,10 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K42" s="10">
         <v>1</v>
@@ -3852,14 +3852,14 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -3868,10 +3868,10 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K43" s="10">
         <v>1</v>
@@ -3879,14 +3879,14 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -3895,10 +3895,10 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K44" s="10">
         <v>1</v>
@@ -3927,7 +3927,7 @@
         <v>158</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K45" s="10">
         <v>1</v>
@@ -3938,7 +3938,7 @@
         <v>95</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -3950,7 +3950,7 @@
         <v>158</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K46" s="10">
         <v>1</v>
@@ -3973,7 +3973,7 @@
         <v>158</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K47" s="10">
         <v>1</v>
@@ -3996,7 +3996,7 @@
         <v>158</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K48" s="10">
         <v>1</v>
@@ -4022,7 +4022,7 @@
         <v>162</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="K49" s="10">
         <v>1</v>
@@ -4045,7 +4045,7 @@
         <v>162</v>
       </c>
       <c r="J50" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K50">
         <v>14</v>
@@ -4074,7 +4074,7 @@
         <v>169</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K51" s="10">
         <v>1</v>
@@ -4086,7 +4086,7 @@
       </c>
       <c r="E52" s="16"/>
       <c r="F52" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -4098,13 +4098,13 @@
         <v>169</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="K52" s="10">
         <v>1</v>
       </c>
       <c r="L52" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -4124,7 +4124,7 @@
         <v>169</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K53" s="10">
         <v>1</v>
@@ -4147,7 +4147,7 @@
         <v>169</v>
       </c>
       <c r="J54" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K54">
         <v>12</v>
@@ -4170,7 +4170,7 @@
         <v>169</v>
       </c>
       <c r="J55" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K55">
         <v>13</v>
@@ -4193,7 +4193,7 @@
         <v>169</v>
       </c>
       <c r="J56" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K56">
         <v>21</v>
@@ -4216,7 +4216,7 @@
         <v>169</v>
       </c>
       <c r="J57" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K57">
         <v>22</v>
@@ -4239,7 +4239,7 @@
         <v>169</v>
       </c>
       <c r="J58" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K58">
         <v>24</v>
@@ -4250,7 +4250,7 @@
         <v>96</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -4262,7 +4262,7 @@
         <v>169</v>
       </c>
       <c r="J59" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="K59">
         <v>23</v>
@@ -4273,7 +4273,7 @@
         <v>96</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -4285,13 +4285,13 @@
         <v>169</v>
       </c>
       <c r="J60" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="K60">
         <v>11</v>
       </c>
       <c r="L60" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -4317,7 +4317,7 @@
         <v>170</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K61" s="10">
         <v>1</v>
@@ -4328,7 +4328,7 @@
         <v>95</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -4340,13 +4340,13 @@
         <v>170</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K62" s="10">
         <v>1</v>
       </c>
       <c r="L62" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -4366,7 +4366,7 @@
         <v>170</v>
       </c>
       <c r="J63" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K63">
         <v>35</v>
@@ -4389,7 +4389,7 @@
         <v>170</v>
       </c>
       <c r="J64" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K64">
         <v>34</v>
@@ -4400,7 +4400,7 @@
         <v>96</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -4412,13 +4412,13 @@
         <v>170</v>
       </c>
       <c r="J65" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K65">
         <v>32</v>
       </c>
       <c r="L65" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -4444,7 +4444,7 @@
         <v>171</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K66" s="10">
         <v>1</v>
@@ -4455,7 +4455,7 @@
         <v>95</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -4467,13 +4467,13 @@
         <v>171</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="K67" s="10">
         <v>1</v>
       </c>
       <c r="L67" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -4481,7 +4481,7 @@
         <v>95</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -4493,13 +4493,13 @@
         <v>171</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K68" s="10">
         <v>1</v>
       </c>
       <c r="L68" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -4507,7 +4507,7 @@
         <v>95</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -4519,7 +4519,7 @@
         <v>171</v>
       </c>
       <c r="J69" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K69" s="10">
         <v>1</v>
@@ -4530,7 +4530,7 @@
         <v>95</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -4542,7 +4542,7 @@
         <v>171</v>
       </c>
       <c r="J70" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K70" s="10">
         <v>1</v>
@@ -4550,10 +4550,10 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D71" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="F71" s="11" t="s">
         <v>244</v>
-      </c>
-      <c r="F71" s="11" t="s">
-        <v>245</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -4565,7 +4565,7 @@
         <v>171</v>
       </c>
       <c r="J71" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K71" s="10">
         <v>1</v>
@@ -4591,7 +4591,7 @@
         <v>171</v>
       </c>
       <c r="J72" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K72" s="10">
         <v>1</v>
@@ -4620,7 +4620,7 @@
         <v>171</v>
       </c>
       <c r="J73" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K73" s="10">
         <v>1</v>
@@ -4631,7 +4631,7 @@
         <v>95</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -4643,7 +4643,7 @@
         <v>171</v>
       </c>
       <c r="J74" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K74" s="10">
         <v>1</v>
@@ -4657,7 +4657,7 @@
         <v>96</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -4669,7 +4669,7 @@
         <v>171</v>
       </c>
       <c r="J75" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K75">
         <v>17</v>
@@ -4695,7 +4695,7 @@
         <v>171</v>
       </c>
       <c r="J76" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="K76">
         <v>15</v>
@@ -4718,7 +4718,7 @@
         <v>171</v>
       </c>
       <c r="J77" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K77">
         <v>16</v>
@@ -4741,7 +4741,7 @@
         <v>171</v>
       </c>
       <c r="J78" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K78">
         <v>57</v>
@@ -4764,7 +4764,7 @@
         <v>171</v>
       </c>
       <c r="J79" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K79">
         <v>54</v>
@@ -4787,7 +4787,7 @@
         <v>171</v>
       </c>
       <c r="J80" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K80">
         <v>55</v>
@@ -4810,7 +4810,7 @@
         <v>171</v>
       </c>
       <c r="J81" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K81">
         <v>56</v>
@@ -4821,7 +4821,7 @@
         <v>96</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -4833,13 +4833,13 @@
         <v>171</v>
       </c>
       <c r="J82" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="K82">
         <v>53</v>
       </c>
       <c r="L82" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
@@ -4847,7 +4847,7 @@
         <v>96</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -4859,13 +4859,13 @@
         <v>171</v>
       </c>
       <c r="J83" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="K83">
         <v>52</v>
       </c>
       <c r="L83" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.25">
@@ -4876,7 +4876,7 @@
         <v>95</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -4888,7 +4888,7 @@
         <v>172</v>
       </c>
       <c r="J84" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K84" s="10">
         <v>1</v>
@@ -4911,7 +4911,7 @@
         <v>172</v>
       </c>
       <c r="J85" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K85">
         <v>41</v>
@@ -4934,7 +4934,7 @@
         <v>172</v>
       </c>
       <c r="J86" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K86">
         <v>43</v>
@@ -4957,7 +4957,7 @@
         <v>172</v>
       </c>
       <c r="J87" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K87">
         <v>42</v>
@@ -4965,25 +4965,25 @@
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F88" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88" t="s">
+        <v>465</v>
+      </c>
+      <c r="J88" t="s">
         <v>435</v>
-      </c>
-      <c r="G88">
-        <v>0</v>
-      </c>
-      <c r="H88">
-        <v>0</v>
-      </c>
-      <c r="I88" t="s">
-        <v>467</v>
-      </c>
-      <c r="J88" t="s">
-        <v>437</v>
       </c>
       <c r="K88" s="10">
         <v>1</v>
@@ -5003,10 +5003,10 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J89" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K89" s="10">
         <v>1</v>
@@ -5017,7 +5017,7 @@
         <v>95</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -5026,16 +5026,16 @@
         <v>0</v>
       </c>
       <c r="I90" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J90" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K90" s="10">
         <v>1</v>
       </c>
       <c r="L90" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.25">
@@ -5043,7 +5043,7 @@
         <v>95</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -5052,16 +5052,16 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J91" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="K91" s="10">
         <v>1</v>
       </c>
       <c r="L91" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="92" spans="2:12" x14ac:dyDescent="0.25">
@@ -5069,19 +5069,19 @@
         <v>96</v>
       </c>
       <c r="F92" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92" t="s">
+        <v>465</v>
+      </c>
+      <c r="J92" t="s">
         <v>436</v>
-      </c>
-      <c r="G92">
-        <v>0</v>
-      </c>
-      <c r="H92">
-        <v>0</v>
-      </c>
-      <c r="I92" t="s">
-        <v>467</v>
-      </c>
-      <c r="J92" t="s">
-        <v>438</v>
       </c>
       <c r="K92">
         <v>44</v>
@@ -5092,7 +5092,7 @@
         <v>96</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -5101,10 +5101,10 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J93" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K93">
         <v>36</v>
@@ -5115,7 +5115,7 @@
         <v>96</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -5124,16 +5124,16 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J94" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="K94">
         <v>33</v>
       </c>
       <c r="L94" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.25">
@@ -5141,25 +5141,25 @@
         <v>96</v>
       </c>
       <c r="F95" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95" t="s">
         <v>465</v>
       </c>
-      <c r="G95">
-        <v>0</v>
-      </c>
-      <c r="H95">
-        <v>0</v>
-      </c>
-      <c r="I95" t="s">
-        <v>467</v>
-      </c>
       <c r="J95" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="K95">
         <v>31</v>
       </c>
       <c r="L95" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.25">
@@ -5179,10 +5179,10 @@
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J96" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K96" s="10">
         <v>1</v>
@@ -5190,7 +5190,7 @@
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>95</v>
@@ -5205,10 +5205,10 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J97" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K97" s="10">
         <v>1</v>
@@ -5216,7 +5216,7 @@
     </row>
     <row r="98" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>95</v>
@@ -5231,27 +5231,27 @@
         <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J98" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="K98" s="10">
         <v>1</v>
       </c>
       <c r="L98" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="99" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F99" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -5260,16 +5260,16 @@
         <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J99" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K99" s="10">
         <v>1</v>
       </c>
       <c r="L99" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="100" spans="2:12" x14ac:dyDescent="0.25">
@@ -5277,54 +5277,54 @@
         <v>95</v>
       </c>
       <c r="F100" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100" t="s">
+        <v>466</v>
+      </c>
+      <c r="J100" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="G100">
-        <v>0</v>
-      </c>
-      <c r="H100">
-        <v>0</v>
-      </c>
-      <c r="I100" t="s">
-        <v>468</v>
-      </c>
-      <c r="J100" s="10" t="s">
-        <v>336</v>
-      </c>
       <c r="K100" s="10">
         <v>1</v>
       </c>
       <c r="L100" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="101" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F101" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101" t="s">
+        <v>466</v>
+      </c>
+      <c r="J101" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="G101">
-        <v>0</v>
-      </c>
-      <c r="H101">
-        <v>0</v>
-      </c>
-      <c r="I101" t="s">
-        <v>468</v>
-      </c>
-      <c r="J101" s="10" t="s">
-        <v>247</v>
-      </c>
       <c r="K101" s="10">
         <v>1</v>
       </c>
       <c r="L101" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="102" spans="2:12" x14ac:dyDescent="0.25">
@@ -5341,10 +5341,10 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J102" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K102">
         <v>64</v>
@@ -5364,10 +5364,10 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J103" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K103">
         <v>65</v>
@@ -5378,7 +5378,7 @@
         <v>96</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>188</v>
+        <v>477</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -5387,10 +5387,10 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="K104">
         <v>66</v>
@@ -5401,7 +5401,7 @@
         <v>96</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -5410,10 +5410,10 @@
         <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J105" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K105">
         <v>68</v>
@@ -5424,19 +5424,19 @@
         <v>96</v>
       </c>
       <c r="F106" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+      <c r="H106">
+        <v>0</v>
+      </c>
+      <c r="I106" t="s">
+        <v>466</v>
+      </c>
+      <c r="J106" t="s">
         <v>231</v>
-      </c>
-      <c r="G106">
-        <v>0</v>
-      </c>
-      <c r="H106">
-        <v>0</v>
-      </c>
-      <c r="I106" t="s">
-        <v>468</v>
-      </c>
-      <c r="J106" t="s">
-        <v>232</v>
       </c>
       <c r="K106">
         <v>67</v>
@@ -5447,25 +5447,25 @@
         <v>96</v>
       </c>
       <c r="F107" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+      <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="I107" t="s">
+        <v>466</v>
+      </c>
+      <c r="J107" t="s">
         <v>233</v>
-      </c>
-      <c r="G107">
-        <v>0</v>
-      </c>
-      <c r="H107">
-        <v>0</v>
-      </c>
-      <c r="I107" t="s">
-        <v>468</v>
-      </c>
-      <c r="J107" t="s">
-        <v>234</v>
       </c>
       <c r="K107">
         <v>69</v>
       </c>
       <c r="L107" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="108" spans="2:12" x14ac:dyDescent="0.25">
@@ -5473,7 +5473,7 @@
         <v>96</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -5482,16 +5482,16 @@
         <v>0</v>
       </c>
       <c r="I108" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J108" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K108">
         <v>63</v>
       </c>
       <c r="L108" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="109" spans="2:12" x14ac:dyDescent="0.25">
@@ -5499,7 +5499,7 @@
         <v>96</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -5508,16 +5508,16 @@
         <v>0</v>
       </c>
       <c r="I109" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J109" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K109">
         <v>62</v>
       </c>
       <c r="L109" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="110" spans="2:12" x14ac:dyDescent="0.25">
@@ -5525,25 +5525,25 @@
         <v>96</v>
       </c>
       <c r="F110" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="I110" t="s">
+        <v>466</v>
+      </c>
+      <c r="J110" t="s">
         <v>248</v>
-      </c>
-      <c r="G110">
-        <v>0</v>
-      </c>
-      <c r="H110">
-        <v>0</v>
-      </c>
-      <c r="I110" t="s">
-        <v>468</v>
-      </c>
-      <c r="J110" t="s">
-        <v>249</v>
       </c>
       <c r="K110">
         <v>61</v>
       </c>
       <c r="L110" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="111" spans="2:12" x14ac:dyDescent="0.25">
@@ -5551,7 +5551,7 @@
         <v>95</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G111">
         <v>0</v>
@@ -5560,10 +5560,10 @@
         <v>0</v>
       </c>
       <c r="I111" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J111" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="K111" s="10">
         <v>1</v>
@@ -5574,7 +5574,7 @@
         <v>96</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -5583,10 +5583,10 @@
         <v>0</v>
       </c>
       <c r="I112" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J112" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="K112">
         <v>71</v>
@@ -5597,7 +5597,7 @@
         <v>96</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>377</v>
+        <v>478</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -5606,10 +5606,10 @@
         <v>0</v>
       </c>
       <c r="I113" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J113" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="K113">
         <v>72</v>
@@ -5620,7 +5620,7 @@
         <v>95</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G114">
         <v>0</v>
@@ -5629,10 +5629,10 @@
         <v>0</v>
       </c>
       <c r="I114" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="J114" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K114" s="10">
         <v>1</v>
@@ -5643,19 +5643,19 @@
         <v>96</v>
       </c>
       <c r="F115" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>0</v>
+      </c>
+      <c r="I115" t="s">
+        <v>468</v>
+      </c>
+      <c r="J115" t="s">
         <v>225</v>
-      </c>
-      <c r="G115">
-        <v>0</v>
-      </c>
-      <c r="H115">
-        <v>0</v>
-      </c>
-      <c r="I115" t="s">
-        <v>470</v>
-      </c>
-      <c r="J115" t="s">
-        <v>226</v>
       </c>
       <c r="K115">
         <v>45</v>
@@ -5672,7 +5672,7 @@
         <v>95</v>
       </c>
       <c r="F116" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G116">
         <v>0</v>
@@ -5681,16 +5681,16 @@
         <v>0</v>
       </c>
       <c r="I116" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="J116" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K116" s="10">
         <v>1</v>
       </c>
       <c r="L116" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
@@ -5698,7 +5698,7 @@
         <v>96</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -5707,27 +5707,27 @@
         <v>0</v>
       </c>
       <c r="I117" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="J117" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K117">
         <v>51</v>
       </c>
       <c r="L117" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F118" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -5736,10 +5736,10 @@
         <v>0</v>
       </c>
       <c r="I118" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="J118" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K118" s="10">
         <v>1</v>
@@ -5750,7 +5750,7 @@
         <v>95</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -5759,16 +5759,16 @@
         <v>0</v>
       </c>
       <c r="I119" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="J119" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K119" s="10">
         <v>1</v>
       </c>
       <c r="L119" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
@@ -5776,25 +5776,25 @@
         <v>96</v>
       </c>
       <c r="F120" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+      <c r="H120">
+        <v>0</v>
+      </c>
+      <c r="I120" t="s">
+        <v>470</v>
+      </c>
+      <c r="J120" t="s">
         <v>296</v>
-      </c>
-      <c r="G120">
-        <v>0</v>
-      </c>
-      <c r="H120">
-        <v>0</v>
-      </c>
-      <c r="I120" t="s">
-        <v>472</v>
-      </c>
-      <c r="J120" t="s">
-        <v>297</v>
       </c>
       <c r="K120">
         <v>46</v>
       </c>
       <c r="L120" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -6156,10 +6156,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>79</v>
@@ -6167,18 +6167,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B3" t="s">
+        <v>448</v>
+      </c>
+      <c r="C3" t="s">
         <v>450</v>
-      </c>
-      <c r="C3" t="s">
-        <v>452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
verification if blade systems io bay parity group connected to single fabric_label
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -9,9 +9,8 @@
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
     <sheet name="service_tables" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
-    <sheet name="data_dependency" sheetId="3" r:id="rId4"/>
-    <sheet name="software" sheetId="4" r:id="rId5"/>
+    <sheet name="data_dependency" sheetId="3" r:id="rId3"/>
+    <sheet name="software" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$L$120</definedName>
@@ -1919,7 +1918,7 @@
   <dimension ref="A1:AO14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,10 +1963,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2171,6 +2167,9 @@
       </c>
       <c r="D4" t="s">
         <v>478</v>
+      </c>
+      <c r="E4" t="s">
+        <v>320</v>
       </c>
       <c r="F4" t="s">
         <v>320</v>
@@ -2590,8 +2589,8 @@
   <dimension ref="A1:L120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G57" sqref="G57"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4162,7 +4161,7 @@
         <v>0</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" t="s">
         <v>169</v>
@@ -4232,7 +4231,7 @@
         <v>61</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -4255,7 +4254,7 @@
         <v>62</v>
       </c>
       <c r="G55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -5429,7 +5428,7 @@
         <v>179</v>
       </c>
       <c r="G102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H102">
         <v>0</v>
@@ -5570,7 +5569,7 @@
         <v>191</v>
       </c>
       <c r="G108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H108">
         <v>0</v>
@@ -5898,226 +5897,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S36" sqref="S36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B16"/>
@@ -6232,7 +6011,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C3"/>

</xml_diff>

<commit_message>
device names per port added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="492">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -589,12 +589,6 @@
     <t>Порты_не_в_зонах</t>
   </si>
   <si>
-    <t>fabric_statistics</t>
-  </si>
-  <si>
-    <t>Статистика_фабрики</t>
-  </si>
-  <si>
     <t>Статистика_зон</t>
   </si>
   <si>
@@ -1426,9 +1420,6 @@
     <t>DATA ANALYSIS 10. SENSOR READINGS</t>
   </si>
   <si>
-    <t>DATA ANALYSIS 11. FABRIC STATISTICS</t>
-  </si>
-  <si>
     <t>DATA ANALYSIS 12. RASLOG</t>
   </si>
   <si>
@@ -1493,6 +1484,18 @@
   </si>
   <si>
     <t>C:\Users\vlasenko\Documents\06.CONFIGS\Sibintek\OCT21\2021-10-04</t>
+  </si>
+  <si>
+    <t>Статистика_портов</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 11. FABRIC PORTS STATISTICS</t>
+  </si>
+  <si>
+    <t>Fabric ports statistics</t>
+  </si>
+  <si>
+    <t>fabric_ports_statistics</t>
   </si>
 </sst>
 </file>
@@ -1918,7 +1921,7 @@
   <dimension ref="A1:AO14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1963,7 +1966,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1972,82 +1975,82 @@
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F2" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="G2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="J2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="K2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="M2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="N2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="O2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="P2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="Q2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="R2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="S2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="T2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="U2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="V2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="W2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="X2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Y2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Z2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="AA2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="AB2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="AC2" t="s">
         <v>186</v>
@@ -2091,7 +2094,7 @@
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C3" s="12">
         <v>44473</v>
@@ -2160,64 +2163,64 @@
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C4" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D4" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="E4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="H4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="I4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="K4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="L4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="M4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="N4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="O4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="P4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="R4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="S4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="T4" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="W4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="X4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
@@ -2232,85 +2235,85 @@
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D5" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G5" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="I5" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="J5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="K5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="M5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="N5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="O5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="P5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="Q5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="R5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="S5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="T5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="U5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="V5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="W5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="X5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="Y5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="Z5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="AA5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AB5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="AC5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AD5" t="s">
         <v>184</v>
@@ -2354,85 +2357,85 @@
         <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D6" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="E6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="G6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="I6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="K6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="L6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="M6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="N6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="O6" t="s">
+        <v>317</v>
+      </c>
+      <c r="P6" t="s">
         <v>319</v>
       </c>
-      <c r="P6" t="s">
-        <v>321</v>
-      </c>
       <c r="Q6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="R6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="S6" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="T6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="U6" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="V6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="W6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="X6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="Y6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="Z6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="AA6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="AB6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AC6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AD6" t="s">
         <v>183</v>
@@ -2476,34 +2479,34 @@
         <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="F7" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="G7" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="J7" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="L7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="N7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="R7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="Y7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="Z7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AB7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AE7" t="s">
         <v>157</v>
@@ -2523,58 +2526,58 @@
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E8" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="H8" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="N8" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="Y8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="Z8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="J9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="L9" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -2589,8 +2592,8 @@
   <dimension ref="A1:L120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G112" sqref="G112"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2636,13 +2639,13 @@
         <v>149</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="L1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2650,7 +2653,7 @@
         <v>94</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -2659,10 +2662,10 @@
         <v>0</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2694,7 +2697,7 @@
         <v>152</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K3" s="10">
         <v>1</v>
@@ -2726,7 +2729,7 @@
         <v>152</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K4" s="10">
         <v>1</v>
@@ -2761,7 +2764,7 @@
         <v>141</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K5" s="10">
         <v>1</v>
@@ -2796,7 +2799,7 @@
         <v>150</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="K6" s="10">
         <v>1</v>
@@ -2831,7 +2834,7 @@
         <v>150</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="K7" s="10">
         <v>1</v>
@@ -2866,7 +2869,7 @@
         <v>151</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K8" s="10">
         <v>1</v>
@@ -2901,7 +2904,7 @@
         <v>147</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="K9" s="10">
         <v>1</v>
@@ -2936,7 +2939,7 @@
         <v>147</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="K10" s="10">
         <v>1</v>
@@ -2971,7 +2974,7 @@
         <v>145</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="K11" s="10">
         <v>1</v>
@@ -3006,7 +3009,7 @@
         <v>146</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="K12" s="10">
         <v>1</v>
@@ -3041,7 +3044,7 @@
         <v>146</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="K13" s="10">
         <v>1</v>
@@ -3076,7 +3079,7 @@
         <v>143</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="K14" s="10">
         <v>1</v>
@@ -3111,7 +3114,7 @@
         <v>143</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="K15" s="10">
         <v>1</v>
@@ -3146,7 +3149,7 @@
         <v>143</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K16" s="10">
         <v>1</v>
@@ -3181,7 +3184,7 @@
         <v>144</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="K17" s="10">
         <v>1</v>
@@ -3216,7 +3219,7 @@
         <v>144</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="K18" s="10">
         <v>1</v>
@@ -3251,7 +3254,7 @@
         <v>144</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="K19" s="10">
         <v>1</v>
@@ -3271,10 +3274,10 @@
         <v>94</v>
       </c>
       <c r="E20" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -3286,7 +3289,7 @@
         <v>144</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="K20" s="10">
         <v>1</v>
@@ -3321,7 +3324,7 @@
         <v>142</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="K21" s="10">
         <v>1</v>
@@ -3353,7 +3356,7 @@
         <v>142</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K22" s="10">
         <v>1</v>
@@ -3385,7 +3388,7 @@
         <v>142</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="K23" s="10">
         <v>1</v>
@@ -3417,7 +3420,7 @@
         <v>142</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="K24" s="10">
         <v>1</v>
@@ -3446,7 +3449,7 @@
         <v>142</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="K25" s="10">
         <v>1</v>
@@ -3475,7 +3478,7 @@
         <v>142</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K26" s="10">
         <v>1</v>
@@ -3507,7 +3510,7 @@
         <v>148</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="K27" s="10">
         <v>1</v>
@@ -3536,7 +3539,7 @@
         <v>148</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="K28" s="10">
         <v>1</v>
@@ -3565,7 +3568,7 @@
         <v>148</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="K29" s="10">
         <v>1</v>
@@ -3594,7 +3597,7 @@
         <v>148</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="K30" s="10">
         <v>1</v>
@@ -3623,7 +3626,7 @@
         <v>148</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="K31" s="10">
         <v>1</v>
@@ -3640,7 +3643,7 @@
         <v>94</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -3652,7 +3655,7 @@
         <v>148</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="K32" s="10">
         <v>1</v>
@@ -3669,7 +3672,7 @@
         <v>94</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -3681,7 +3684,7 @@
         <v>148</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="K33" s="10">
         <v>1</v>
@@ -3689,16 +3692,16 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -3707,10 +3710,10 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="K34" s="10">
         <v>1</v>
@@ -3718,28 +3721,28 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F35" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
+        <v>286</v>
+      </c>
+      <c r="J35" s="10" t="s">
         <v>287</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35" t="s">
-        <v>288</v>
-      </c>
-      <c r="J35" s="10" t="s">
-        <v>289</v>
       </c>
       <c r="K35" s="10">
         <v>1</v>
@@ -3768,10 +3771,10 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K36" s="10">
         <v>1</v>
@@ -3797,10 +3800,10 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K37" s="10">
         <v>1</v>
@@ -3826,10 +3829,10 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K38" s="10">
         <v>1</v>
@@ -3837,26 +3840,26 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F39" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39" t="s">
+        <v>458</v>
+      </c>
+      <c r="J39" s="10" t="s">
         <v>260</v>
-      </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39" t="s">
-        <v>460</v>
-      </c>
-      <c r="J39" s="10" t="s">
-        <v>262</v>
       </c>
       <c r="K39" s="10">
         <v>1</v>
@@ -3864,26 +3867,26 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F40" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40" t="s">
+        <v>458</v>
+      </c>
+      <c r="J40" s="10" t="s">
         <v>261</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40" t="s">
-        <v>460</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>263</v>
       </c>
       <c r="K40" s="10">
         <v>1</v>
@@ -3891,14 +3894,14 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -3907,10 +3910,10 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="K41" s="10">
         <v>1</v>
@@ -3918,14 +3921,14 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -3934,10 +3937,10 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="K42" s="10">
         <v>1</v>
@@ -3945,14 +3948,14 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -3961,10 +3964,10 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="K43" s="10">
         <v>1</v>
@@ -3972,14 +3975,14 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -3988,10 +3991,10 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="K44" s="10">
         <v>1</v>
@@ -4020,7 +4023,7 @@
         <v>158</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K45" s="10">
         <v>1</v>
@@ -4031,7 +4034,7 @@
         <v>95</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -4043,7 +4046,7 @@
         <v>158</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K46" s="10">
         <v>1</v>
@@ -4066,7 +4069,7 @@
         <v>158</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="K47" s="10">
         <v>1</v>
@@ -4089,7 +4092,7 @@
         <v>158</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K48" s="10">
         <v>1</v>
@@ -4115,7 +4118,7 @@
         <v>162</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K49" s="10">
         <v>1</v>
@@ -4138,7 +4141,7 @@
         <v>162</v>
       </c>
       <c r="J50" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="K50">
         <v>14</v>
@@ -4167,7 +4170,7 @@
         <v>169</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K51" s="10">
         <v>1</v>
@@ -4179,7 +4182,7 @@
       </c>
       <c r="E52" s="16"/>
       <c r="F52" s="2" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -4191,13 +4194,13 @@
         <v>169</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="K52" s="10">
         <v>1</v>
       </c>
       <c r="L52" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -4217,7 +4220,7 @@
         <v>169</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K53" s="10">
         <v>1</v>
@@ -4240,7 +4243,7 @@
         <v>169</v>
       </c>
       <c r="J54" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K54">
         <v>12</v>
@@ -4263,7 +4266,7 @@
         <v>169</v>
       </c>
       <c r="J55" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K55">
         <v>13</v>
@@ -4286,7 +4289,7 @@
         <v>169</v>
       </c>
       <c r="J56" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K56">
         <v>21</v>
@@ -4309,7 +4312,7 @@
         <v>169</v>
       </c>
       <c r="J57" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K57">
         <v>22</v>
@@ -4332,7 +4335,7 @@
         <v>169</v>
       </c>
       <c r="J58" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K58">
         <v>24</v>
@@ -4343,7 +4346,7 @@
         <v>96</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -4355,7 +4358,7 @@
         <v>169</v>
       </c>
       <c r="J59" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="K59">
         <v>23</v>
@@ -4366,7 +4369,7 @@
         <v>96</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -4378,13 +4381,13 @@
         <v>169</v>
       </c>
       <c r="J60" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="K60">
         <v>11</v>
       </c>
       <c r="L60" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -4410,7 +4413,7 @@
         <v>170</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K61" s="10">
         <v>1</v>
@@ -4421,7 +4424,7 @@
         <v>95</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -4433,13 +4436,13 @@
         <v>170</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="K62" s="10">
         <v>1</v>
       </c>
       <c r="L62" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -4459,7 +4462,7 @@
         <v>170</v>
       </c>
       <c r="J63" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K63">
         <v>35</v>
@@ -4482,7 +4485,7 @@
         <v>170</v>
       </c>
       <c r="J64" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K64">
         <v>34</v>
@@ -4493,7 +4496,7 @@
         <v>96</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -4505,13 +4508,13 @@
         <v>170</v>
       </c>
       <c r="J65" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="K65">
         <v>32</v>
       </c>
       <c r="L65" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -4531,13 +4534,13 @@
         <v>0</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I66" t="s">
         <v>171</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="K66" s="10">
         <v>1</v>
@@ -4548,7 +4551,7 @@
         <v>95</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -4560,13 +4563,13 @@
         <v>171</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="K67" s="10">
         <v>1</v>
       </c>
       <c r="L67" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -4574,7 +4577,7 @@
         <v>95</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -4586,13 +4589,13 @@
         <v>171</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="K68" s="10">
         <v>1</v>
       </c>
       <c r="L68" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -4600,7 +4603,7 @@
         <v>95</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -4612,7 +4615,7 @@
         <v>171</v>
       </c>
       <c r="J69" s="10" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="K69" s="10">
         <v>1</v>
@@ -4623,7 +4626,7 @@
         <v>95</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -4635,7 +4638,7 @@
         <v>171</v>
       </c>
       <c r="J70" s="10" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K70" s="10">
         <v>1</v>
@@ -4643,10 +4646,10 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D71" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -4658,7 +4661,7 @@
         <v>171</v>
       </c>
       <c r="J71" s="10" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K71" s="10">
         <v>1</v>
@@ -4684,7 +4687,7 @@
         <v>171</v>
       </c>
       <c r="J72" s="10" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="K72" s="10">
         <v>1</v>
@@ -4713,7 +4716,7 @@
         <v>171</v>
       </c>
       <c r="J73" s="10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="K73" s="10">
         <v>1</v>
@@ -4724,7 +4727,7 @@
         <v>95</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -4736,7 +4739,7 @@
         <v>171</v>
       </c>
       <c r="J74" s="10" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="K74" s="10">
         <v>1</v>
@@ -4750,7 +4753,7 @@
         <v>96</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -4762,7 +4765,7 @@
         <v>171</v>
       </c>
       <c r="J75" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K75">
         <v>17</v>
@@ -4788,7 +4791,7 @@
         <v>171</v>
       </c>
       <c r="J76" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K76">
         <v>15</v>
@@ -4811,7 +4814,7 @@
         <v>171</v>
       </c>
       <c r="J77" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K77">
         <v>16</v>
@@ -4834,7 +4837,7 @@
         <v>171</v>
       </c>
       <c r="J78" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K78">
         <v>57</v>
@@ -4857,7 +4860,7 @@
         <v>171</v>
       </c>
       <c r="J79" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K79">
         <v>54</v>
@@ -4880,7 +4883,7 @@
         <v>171</v>
       </c>
       <c r="J80" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K80">
         <v>55</v>
@@ -4903,7 +4906,7 @@
         <v>171</v>
       </c>
       <c r="J81" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K81">
         <v>56</v>
@@ -4914,7 +4917,7 @@
         <v>96</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -4926,13 +4929,13 @@
         <v>171</v>
       </c>
       <c r="J82" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="K82">
         <v>53</v>
       </c>
       <c r="L82" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
@@ -4940,7 +4943,7 @@
         <v>96</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -4952,13 +4955,13 @@
         <v>171</v>
       </c>
       <c r="J83" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="K83">
         <v>52</v>
       </c>
       <c r="L83" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.25">
@@ -4969,7 +4972,7 @@
         <v>95</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -4981,7 +4984,7 @@
         <v>172</v>
       </c>
       <c r="J84" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="K84" s="10">
         <v>1</v>
@@ -5004,7 +5007,7 @@
         <v>172</v>
       </c>
       <c r="J85" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K85">
         <v>41</v>
@@ -5027,7 +5030,7 @@
         <v>172</v>
       </c>
       <c r="J86" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K86">
         <v>43</v>
@@ -5050,7 +5053,7 @@
         <v>172</v>
       </c>
       <c r="J87" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="K87">
         <v>42</v>
@@ -5058,25 +5061,25 @@
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F88" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88" t="s">
+        <v>462</v>
+      </c>
+      <c r="J88" t="s">
         <v>432</v>
-      </c>
-      <c r="G88">
-        <v>0</v>
-      </c>
-      <c r="H88">
-        <v>0</v>
-      </c>
-      <c r="I88" t="s">
-        <v>464</v>
-      </c>
-      <c r="J88" t="s">
-        <v>434</v>
       </c>
       <c r="K88" s="10">
         <v>1</v>
@@ -5096,10 +5099,10 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J89" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="K89" s="10">
         <v>1</v>
@@ -5110,7 +5113,7 @@
         <v>95</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -5119,16 +5122,16 @@
         <v>0</v>
       </c>
       <c r="I90" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J90" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="K90" s="10">
         <v>1</v>
       </c>
       <c r="L90" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.25">
@@ -5136,7 +5139,7 @@
         <v>95</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -5145,16 +5148,16 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J91" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="K91" s="10">
         <v>1</v>
       </c>
       <c r="L91" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="92" spans="2:12" x14ac:dyDescent="0.25">
@@ -5162,19 +5165,19 @@
         <v>96</v>
       </c>
       <c r="F92" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+      <c r="I92" t="s">
+        <v>462</v>
+      </c>
+      <c r="J92" t="s">
         <v>433</v>
-      </c>
-      <c r="G92">
-        <v>0</v>
-      </c>
-      <c r="H92">
-        <v>0</v>
-      </c>
-      <c r="I92" t="s">
-        <v>464</v>
-      </c>
-      <c r="J92" t="s">
-        <v>435</v>
       </c>
       <c r="K92">
         <v>44</v>
@@ -5185,7 +5188,7 @@
         <v>96</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -5194,10 +5197,10 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J93" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K93">
         <v>36</v>
@@ -5208,7 +5211,7 @@
         <v>96</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -5217,16 +5220,16 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J94" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="K94">
         <v>33</v>
       </c>
       <c r="L94" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.25">
@@ -5234,25 +5237,25 @@
         <v>96</v>
       </c>
       <c r="F95" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95" t="s">
         <v>462</v>
       </c>
-      <c r="G95">
-        <v>0</v>
-      </c>
-      <c r="H95">
-        <v>0</v>
-      </c>
-      <c r="I95" t="s">
-        <v>464</v>
-      </c>
       <c r="J95" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K95">
         <v>31</v>
       </c>
       <c r="L95" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.25">
@@ -5272,10 +5275,10 @@
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J96" s="10" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="K96" s="10">
         <v>1</v>
@@ -5283,7 +5286,7 @@
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>95</v>
@@ -5298,10 +5301,10 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J97" s="10" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="K97" s="10">
         <v>1</v>
@@ -5309,7 +5312,7 @@
     </row>
     <row r="98" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D98" s="6" t="s">
         <v>95</v>
@@ -5324,27 +5327,27 @@
         <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J98" s="10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="K98" s="10">
         <v>1</v>
       </c>
       <c r="L98" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="99" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F99" s="9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -5353,16 +5356,16 @@
         <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J99" s="10" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K99" s="10">
         <v>1</v>
       </c>
       <c r="L99" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="100" spans="2:12" x14ac:dyDescent="0.25">
@@ -5370,7 +5373,7 @@
         <v>95</v>
       </c>
       <c r="F100" s="9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -5379,27 +5382,27 @@
         <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J100" s="10" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="K100" s="10">
         <v>1</v>
       </c>
       <c r="L100" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="101" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D101" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F101" s="9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -5408,16 +5411,16 @@
         <v>0</v>
       </c>
       <c r="I101" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J101" s="10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="K101" s="10">
         <v>1</v>
       </c>
       <c r="L101" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="102" spans="2:12" x14ac:dyDescent="0.25">
@@ -5428,16 +5431,16 @@
         <v>179</v>
       </c>
       <c r="G102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H102">
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J102" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K102">
         <v>64</v>
@@ -5457,10 +5460,10 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J103" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K103">
         <v>65</v>
@@ -5471,7 +5474,7 @@
         <v>96</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -5480,10 +5483,10 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J104" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K104">
         <v>66</v>
@@ -5503,10 +5506,10 @@
         <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J105" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K105">
         <v>68</v>
@@ -5517,7 +5520,7 @@
         <v>96</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -5526,10 +5529,10 @@
         <v>0</v>
       </c>
       <c r="I106" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J106" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K106">
         <v>67</v>
@@ -5540,7 +5543,7 @@
         <v>96</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -5549,16 +5552,16 @@
         <v>0</v>
       </c>
       <c r="I107" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J107" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K107">
         <v>69</v>
       </c>
       <c r="L107" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="108" spans="2:12" x14ac:dyDescent="0.25">
@@ -5566,25 +5569,25 @@
         <v>96</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H108">
         <v>0</v>
       </c>
       <c r="I108" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J108" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="K108">
         <v>63</v>
       </c>
       <c r="L108" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="109" spans="2:12" x14ac:dyDescent="0.25">
@@ -5592,25 +5595,25 @@
         <v>96</v>
       </c>
       <c r="F109" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
+      <c r="I109" t="s">
+        <v>463</v>
+      </c>
+      <c r="J109" t="s">
         <v>339</v>
-      </c>
-      <c r="G109">
-        <v>0</v>
-      </c>
-      <c r="H109">
-        <v>0</v>
-      </c>
-      <c r="I109" t="s">
-        <v>465</v>
-      </c>
-      <c r="J109" t="s">
-        <v>341</v>
       </c>
       <c r="K109">
         <v>62</v>
       </c>
       <c r="L109" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="110" spans="2:12" x14ac:dyDescent="0.25">
@@ -5618,7 +5621,7 @@
         <v>96</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -5627,16 +5630,16 @@
         <v>0</v>
       </c>
       <c r="I110" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J110" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="K110">
         <v>61</v>
       </c>
       <c r="L110" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="111" spans="2:12" x14ac:dyDescent="0.25">
@@ -5644,7 +5647,7 @@
         <v>95</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="G111">
         <v>0</v>
@@ -5653,10 +5656,10 @@
         <v>0</v>
       </c>
       <c r="I111" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="J111" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="K111" s="10">
         <v>1</v>
@@ -5667,7 +5670,7 @@
         <v>96</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -5676,10 +5679,10 @@
         <v>0</v>
       </c>
       <c r="I112" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="J112" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="K112">
         <v>71</v>
@@ -5690,7 +5693,7 @@
         <v>96</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -5699,10 +5702,10 @@
         <v>0</v>
       </c>
       <c r="I113" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="J113" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="K113">
         <v>72</v>
@@ -5713,7 +5716,7 @@
         <v>95</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G114">
         <v>0</v>
@@ -5722,10 +5725,10 @@
         <v>0</v>
       </c>
       <c r="I114" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J114" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K114" s="10">
         <v>1</v>
@@ -5736,7 +5739,7 @@
         <v>96</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -5745,10 +5748,10 @@
         <v>0</v>
       </c>
       <c r="I115" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J115" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="K115">
         <v>45</v>
@@ -5765,7 +5768,7 @@
         <v>95</v>
       </c>
       <c r="F116" s="9" t="s">
-        <v>189</v>
+        <v>491</v>
       </c>
       <c r="G116">
         <v>0</v>
@@ -5774,16 +5777,16 @@
         <v>0</v>
       </c>
       <c r="I116" t="s">
-        <v>468</v>
+        <v>489</v>
       </c>
       <c r="J116" s="10" t="s">
-        <v>300</v>
+        <v>490</v>
       </c>
       <c r="K116" s="10">
         <v>1</v>
       </c>
       <c r="L116" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
@@ -5791,7 +5794,7 @@
         <v>96</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>190</v>
+        <v>488</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -5800,27 +5803,27 @@
         <v>0</v>
       </c>
       <c r="I117" t="s">
-        <v>468</v>
+        <v>489</v>
       </c>
       <c r="J117" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="K117">
         <v>51</v>
       </c>
       <c r="L117" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F118" s="9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -5829,10 +5832,10 @@
         <v>0</v>
       </c>
       <c r="I118" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="J118" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="K118" s="10">
         <v>1</v>
@@ -5843,7 +5846,7 @@
         <v>95</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -5852,16 +5855,16 @@
         <v>0</v>
       </c>
       <c r="I119" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="J119" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K119" s="10">
         <v>1</v>
       </c>
       <c r="L119" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
@@ -5869,7 +5872,7 @@
         <v>96</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -5878,16 +5881,16 @@
         <v>0</v>
       </c>
       <c r="I120" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="J120" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K120">
         <v>46</v>
       </c>
       <c r="L120" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -6029,10 +6032,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>79</v>
@@ -6040,24 +6043,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B2" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="C2" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B3" t="s">
+        <v>445</v>
+      </c>
+      <c r="C3" t="s">
         <v>447</v>
-      </c>
-      <c r="C3" t="s">
-        <v>449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
filtered error reports added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -13,14 +13,14 @@
     <sheet name="software" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$L$120</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$L$129</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="513">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1496,6 +1496,69 @@
   </si>
   <si>
     <t>fabric_ports_statistics</t>
+  </si>
+  <si>
+    <t>link_reset</t>
+  </si>
+  <si>
+    <t>crc_good_eof</t>
+  </si>
+  <si>
+    <t>fec</t>
+  </si>
+  <si>
+    <t>pcs_blk</t>
+  </si>
+  <si>
+    <t>link_failure</t>
+  </si>
+  <si>
+    <t>discard</t>
+  </si>
+  <si>
+    <t>enc</t>
+  </si>
+  <si>
+    <t>crc</t>
+  </si>
+  <si>
+    <t>bad_eof</t>
+  </si>
+  <si>
+    <t>bad_os</t>
+  </si>
+  <si>
+    <t>ошибки</t>
+  </si>
+  <si>
+    <t>porterr_link_reset</t>
+  </si>
+  <si>
+    <t>porterr_crc_good_eof</t>
+  </si>
+  <si>
+    <t>porterr_fec</t>
+  </si>
+  <si>
+    <t>porterr_pcs_blk</t>
+  </si>
+  <si>
+    <t>porterr_link_failure</t>
+  </si>
+  <si>
+    <t>porterr_discard</t>
+  </si>
+  <si>
+    <t>porterr_bad_eof</t>
+  </si>
+  <si>
+    <t>porterr_bad_os</t>
+  </si>
+  <si>
+    <t>porterr_enc_crc</t>
+  </si>
+  <si>
+    <t>enc_crc</t>
   </si>
 </sst>
 </file>
@@ -2589,11 +2652,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:L120"/>
+  <dimension ref="A1:L150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I87" sqref="I87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4534,7 +4597,7 @@
         <v>0</v>
       </c>
       <c r="H66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I66" t="s">
         <v>171</v>
@@ -4978,7 +5041,7 @@
         <v>0</v>
       </c>
       <c r="H84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I84" t="s">
         <v>172</v>
@@ -5060,14 +5123,11 @@
       </c>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
-        <v>467</v>
-      </c>
       <c r="D88" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>430</v>
+        <v>503</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -5076,13 +5136,16 @@
         <v>0</v>
       </c>
       <c r="I88" t="s">
-        <v>462</v>
+        <v>172</v>
       </c>
       <c r="J88" t="s">
-        <v>432</v>
-      </c>
-      <c r="K88" s="10">
-        <v>1</v>
+        <v>492</v>
+      </c>
+      <c r="K88">
+        <v>1</v>
+      </c>
+      <c r="L88" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.25">
@@ -5090,7 +5153,7 @@
         <v>95</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>164</v>
+        <v>504</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -5099,13 +5162,16 @@
         <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>462</v>
+        <v>172</v>
       </c>
       <c r="J89" t="s">
-        <v>426</v>
-      </c>
-      <c r="K89" s="10">
-        <v>1</v>
+        <v>493</v>
+      </c>
+      <c r="K89">
+        <v>1</v>
+      </c>
+      <c r="L89" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="90" spans="2:12" x14ac:dyDescent="0.25">
@@ -5113,7 +5179,7 @@
         <v>95</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>421</v>
+        <v>505</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -5122,16 +5188,16 @@
         <v>0</v>
       </c>
       <c r="I90" t="s">
-        <v>462</v>
+        <v>172</v>
       </c>
       <c r="J90" t="s">
-        <v>425</v>
-      </c>
-      <c r="K90" s="10">
+        <v>494</v>
+      </c>
+      <c r="K90">
         <v>1</v>
       </c>
       <c r="L90" t="s">
-        <v>390</v>
+        <v>502</v>
       </c>
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.25">
@@ -5139,7 +5205,7 @@
         <v>95</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>468</v>
+        <v>506</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -5148,24 +5214,24 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>462</v>
+        <v>172</v>
       </c>
       <c r="J91" t="s">
-        <v>469</v>
-      </c>
-      <c r="K91" s="10">
+        <v>495</v>
+      </c>
+      <c r="K91">
         <v>1</v>
       </c>
       <c r="L91" t="s">
-        <v>390</v>
+        <v>502</v>
       </c>
     </row>
     <row r="92" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D92" s="5" t="s">
-        <v>96</v>
+      <c r="D92" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>431</v>
+        <v>507</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -5174,21 +5240,24 @@
         <v>0</v>
       </c>
       <c r="I92" t="s">
-        <v>462</v>
+        <v>172</v>
       </c>
       <c r="J92" t="s">
-        <v>433</v>
+        <v>496</v>
       </c>
       <c r="K92">
-        <v>44</v>
+        <v>1</v>
+      </c>
+      <c r="L92" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D93" s="5" t="s">
-        <v>96</v>
+      <c r="D93" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>424</v>
+        <v>508</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -5197,21 +5266,24 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>462</v>
+        <v>172</v>
       </c>
       <c r="J93" t="s">
-        <v>197</v>
+        <v>497</v>
       </c>
       <c r="K93">
-        <v>36</v>
+        <v>1</v>
+      </c>
+      <c r="L93" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D94" s="5" t="s">
-        <v>96</v>
+      <c r="D94" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>422</v>
+        <v>511</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -5220,24 +5292,24 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>462</v>
+        <v>172</v>
       </c>
       <c r="J94" t="s">
-        <v>423</v>
+        <v>512</v>
       </c>
       <c r="K94">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="L94" t="s">
-        <v>390</v>
+        <v>502</v>
       </c>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D95" s="5" t="s">
-        <v>96</v>
+      <c r="D95" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>460</v>
+        <v>509</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -5246,27 +5318,24 @@
         <v>0</v>
       </c>
       <c r="I95" t="s">
-        <v>462</v>
+        <v>172</v>
       </c>
       <c r="J95" t="s">
-        <v>461</v>
+        <v>500</v>
       </c>
       <c r="K95">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="L95" t="s">
-        <v>390</v>
+        <v>502</v>
       </c>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>176</v>
-      </c>
       <c r="D96" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F96" s="9" t="s">
-        <v>177</v>
+      <c r="F96" s="2" t="s">
+        <v>510</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -5275,24 +5344,27 @@
         <v>0</v>
       </c>
       <c r="I96" t="s">
-        <v>463</v>
-      </c>
-      <c r="J96" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="K96" s="10">
-        <v>1</v>
+        <v>172</v>
+      </c>
+      <c r="J96" t="s">
+        <v>501</v>
+      </c>
+      <c r="K96">
+        <v>1</v>
+      </c>
+      <c r="L96" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>248</v>
+        <v>467</v>
       </c>
       <c r="D97" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F97" s="9" t="s">
-        <v>178</v>
+      <c r="F97" s="2" t="s">
+        <v>430</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -5301,24 +5373,21 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>463</v>
-      </c>
-      <c r="J97" s="10" t="s">
-        <v>334</v>
+        <v>462</v>
+      </c>
+      <c r="J97" t="s">
+        <v>432</v>
       </c>
       <c r="K97" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="98" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B98" t="s">
-        <v>250</v>
-      </c>
       <c r="D98" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F98" s="9" t="s">
-        <v>187</v>
+      <c r="F98" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -5327,27 +5396,21 @@
         <v>0</v>
       </c>
       <c r="I98" t="s">
-        <v>463</v>
-      </c>
-      <c r="J98" s="10" t="s">
-        <v>335</v>
+        <v>462</v>
+      </c>
+      <c r="J98" t="s">
+        <v>426</v>
       </c>
       <c r="K98" s="10">
         <v>1</v>
       </c>
-      <c r="L98" t="s">
-        <v>390</v>
-      </c>
     </row>
     <row r="99" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>249</v>
-      </c>
       <c r="D99" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F99" s="9" t="s">
-        <v>213</v>
+      <c r="F99" s="2" t="s">
+        <v>421</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -5356,10 +5419,10 @@
         <v>0</v>
       </c>
       <c r="I99" t="s">
-        <v>463</v>
-      </c>
-      <c r="J99" s="10" t="s">
-        <v>336</v>
+        <v>462</v>
+      </c>
+      <c r="J99" t="s">
+        <v>425</v>
       </c>
       <c r="K99" s="10">
         <v>1</v>
@@ -5372,8 +5435,8 @@
       <c r="D100" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F100" s="9" t="s">
-        <v>331</v>
+      <c r="F100" s="2" t="s">
+        <v>468</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -5382,10 +5445,10 @@
         <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>463</v>
-      </c>
-      <c r="J100" s="10" t="s">
-        <v>332</v>
+        <v>462</v>
+      </c>
+      <c r="J100" t="s">
+        <v>469</v>
       </c>
       <c r="K100" s="10">
         <v>1</v>
@@ -5395,14 +5458,11 @@
       </c>
     </row>
     <row r="101" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>247</v>
-      </c>
-      <c r="D101" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F101" s="9" t="s">
-        <v>243</v>
+      <c r="D101" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>431</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -5411,16 +5471,13 @@
         <v>0</v>
       </c>
       <c r="I101" t="s">
-        <v>463</v>
-      </c>
-      <c r="J101" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="K101" s="10">
-        <v>1</v>
-      </c>
-      <c r="L101" t="s">
-        <v>390</v>
+        <v>462</v>
+      </c>
+      <c r="J101" t="s">
+        <v>433</v>
+      </c>
+      <c r="K101">
+        <v>44</v>
       </c>
     </row>
     <row r="102" spans="2:12" x14ac:dyDescent="0.25">
@@ -5428,7 +5485,7 @@
         <v>96</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>179</v>
+        <v>424</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -5437,13 +5494,13 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J102" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="K102">
-        <v>64</v>
+        <v>36</v>
       </c>
     </row>
     <row r="103" spans="2:12" x14ac:dyDescent="0.25">
@@ -5451,7 +5508,7 @@
         <v>96</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>180</v>
+        <v>422</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -5460,13 +5517,16 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J103" t="s">
-        <v>210</v>
+        <v>423</v>
       </c>
       <c r="K103">
-        <v>65</v>
+        <v>33</v>
+      </c>
+      <c r="L103" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="104" spans="2:12" x14ac:dyDescent="0.25">
@@ -5474,7 +5534,7 @@
         <v>96</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -5483,21 +5543,27 @@
         <v>0</v>
       </c>
       <c r="I104" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="J104" t="s">
-        <v>215</v>
+        <v>461</v>
       </c>
       <c r="K104">
-        <v>66</v>
+        <v>31</v>
+      </c>
+      <c r="L104" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="105" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D105" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>188</v>
+      <c r="B105" t="s">
+        <v>176</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -5508,19 +5574,22 @@
       <c r="I105" t="s">
         <v>463</v>
       </c>
-      <c r="J105" t="s">
-        <v>211</v>
-      </c>
-      <c r="K105">
-        <v>68</v>
+      <c r="J105" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="K105" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D106" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F106" s="2" t="s">
-        <v>228</v>
+      <c r="B106" t="s">
+        <v>248</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F106" s="9" t="s">
+        <v>178</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -5531,19 +5600,22 @@
       <c r="I106" t="s">
         <v>463</v>
       </c>
-      <c r="J106" t="s">
-        <v>229</v>
-      </c>
-      <c r="K106">
-        <v>67</v>
+      <c r="J106" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="K106" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D107" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>230</v>
+      <c r="B107" t="s">
+        <v>250</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F107" s="9" t="s">
+        <v>187</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -5554,22 +5626,25 @@
       <c r="I107" t="s">
         <v>463</v>
       </c>
-      <c r="J107" t="s">
-        <v>231</v>
-      </c>
-      <c r="K107">
-        <v>69</v>
+      <c r="J107" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="K107" s="10">
+        <v>1</v>
       </c>
       <c r="L107" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="108" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D108" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F108" s="2" t="s">
-        <v>189</v>
+      <c r="B108" t="s">
+        <v>249</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F108" s="9" t="s">
+        <v>213</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -5580,22 +5655,22 @@
       <c r="I108" t="s">
         <v>463</v>
       </c>
-      <c r="J108" t="s">
-        <v>338</v>
-      </c>
-      <c r="K108">
-        <v>63</v>
+      <c r="J108" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="K108" s="10">
+        <v>1</v>
       </c>
       <c r="L108" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="109" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D109" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>337</v>
+      <c r="D109" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F109" s="9" t="s">
+        <v>331</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -5606,22 +5681,25 @@
       <c r="I109" t="s">
         <v>463</v>
       </c>
-      <c r="J109" t="s">
-        <v>339</v>
-      </c>
-      <c r="K109">
-        <v>62</v>
+      <c r="J109" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="K109" s="10">
+        <v>1</v>
       </c>
       <c r="L109" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="110" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D110" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>245</v>
+      <c r="B110" t="s">
+        <v>247</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F110" s="9" t="s">
+        <v>243</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -5632,22 +5710,22 @@
       <c r="I110" t="s">
         <v>463</v>
       </c>
-      <c r="J110" t="s">
-        <v>246</v>
-      </c>
-      <c r="K110">
-        <v>61</v>
+      <c r="J110" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="K110" s="10">
+        <v>1</v>
       </c>
       <c r="L110" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="111" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D111" s="6" t="s">
-        <v>95</v>
+      <c r="D111" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>373</v>
+        <v>179</v>
       </c>
       <c r="G111">
         <v>0</v>
@@ -5656,13 +5734,13 @@
         <v>0</v>
       </c>
       <c r="I111" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J111" t="s">
-        <v>374</v>
-      </c>
-      <c r="K111" s="10">
-        <v>1</v>
+        <v>209</v>
+      </c>
+      <c r="K111">
+        <v>64</v>
       </c>
     </row>
     <row r="112" spans="2:12" x14ac:dyDescent="0.25">
@@ -5670,7 +5748,7 @@
         <v>96</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>372</v>
+        <v>180</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -5679,13 +5757,13 @@
         <v>0</v>
       </c>
       <c r="I112" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J112" t="s">
-        <v>375</v>
+        <v>210</v>
       </c>
       <c r="K112">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
@@ -5693,7 +5771,7 @@
         <v>96</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -5702,21 +5780,21 @@
         <v>0</v>
       </c>
       <c r="I113" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="J113" t="s">
-        <v>376</v>
+        <v>215</v>
       </c>
       <c r="K113">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D114" s="6" t="s">
-        <v>95</v>
+      <c r="D114" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>221</v>
+        <v>188</v>
       </c>
       <c r="G114">
         <v>0</v>
@@ -5725,13 +5803,13 @@
         <v>0</v>
       </c>
       <c r="I114" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J114" t="s">
-        <v>297</v>
-      </c>
-      <c r="K114" s="10">
-        <v>1</v>
+        <v>211</v>
+      </c>
+      <c r="K114">
+        <v>68</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
@@ -5739,7 +5817,7 @@
         <v>96</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -5748,27 +5826,21 @@
         <v>0</v>
       </c>
       <c r="I115" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J115" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="K115">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A116">
-        <v>17</v>
-      </c>
-      <c r="B116" t="s">
-        <v>136</v>
-      </c>
-      <c r="D116" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F116" s="9" t="s">
-        <v>491</v>
+      <c r="D116" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="G116">
         <v>0</v>
@@ -5777,13 +5849,13 @@
         <v>0</v>
       </c>
       <c r="I116" t="s">
-        <v>489</v>
-      </c>
-      <c r="J116" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="K116" s="10">
-        <v>1</v>
+        <v>463</v>
+      </c>
+      <c r="J116" t="s">
+        <v>231</v>
+      </c>
+      <c r="K116">
+        <v>69</v>
       </c>
       <c r="L116" t="s">
         <v>390</v>
@@ -5794,7 +5866,7 @@
         <v>96</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>488</v>
+        <v>189</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -5803,27 +5875,24 @@
         <v>0</v>
       </c>
       <c r="I117" t="s">
-        <v>489</v>
+        <v>463</v>
       </c>
       <c r="J117" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="K117">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="L117" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B118" t="s">
-        <v>290</v>
-      </c>
-      <c r="D118" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F118" s="9" t="s">
-        <v>291</v>
+      <c r="D118" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>337</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -5832,21 +5901,24 @@
         <v>0</v>
       </c>
       <c r="I118" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="J118" t="s">
-        <v>294</v>
-      </c>
-      <c r="K118" s="10">
-        <v>1</v>
+        <v>339</v>
+      </c>
+      <c r="K118">
+        <v>62</v>
+      </c>
+      <c r="L118" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D119" s="6" t="s">
-        <v>95</v>
+      <c r="D119" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>299</v>
+        <v>245</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -5855,42 +5927,317 @@
         <v>0</v>
       </c>
       <c r="I119" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="J119" t="s">
-        <v>295</v>
-      </c>
-      <c r="K119" s="10">
-        <v>1</v>
+        <v>246</v>
+      </c>
+      <c r="K119">
+        <v>61</v>
       </c>
       <c r="L119" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D120" s="5" t="s">
+      <c r="D120" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+      <c r="H120">
+        <v>0</v>
+      </c>
+      <c r="I120" t="s">
+        <v>464</v>
+      </c>
+      <c r="J120" t="s">
+        <v>374</v>
+      </c>
+      <c r="K120" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D121" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F120" s="2" t="s">
+      <c r="F121" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="G121">
+        <v>0</v>
+      </c>
+      <c r="H121">
+        <v>0</v>
+      </c>
+      <c r="I121" t="s">
+        <v>464</v>
+      </c>
+      <c r="J121" t="s">
+        <v>375</v>
+      </c>
+      <c r="K121">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D122" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="G122">
+        <v>0</v>
+      </c>
+      <c r="H122">
+        <v>0</v>
+      </c>
+      <c r="I122" t="s">
+        <v>464</v>
+      </c>
+      <c r="J122" t="s">
+        <v>376</v>
+      </c>
+      <c r="K122">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D123" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="G123">
+        <v>0</v>
+      </c>
+      <c r="H123">
+        <v>0</v>
+      </c>
+      <c r="I123" t="s">
+        <v>465</v>
+      </c>
+      <c r="J123" t="s">
+        <v>297</v>
+      </c>
+      <c r="K123" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D124" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G124">
+        <v>0</v>
+      </c>
+      <c r="H124">
+        <v>0</v>
+      </c>
+      <c r="I124" t="s">
+        <v>465</v>
+      </c>
+      <c r="J124" t="s">
+        <v>223</v>
+      </c>
+      <c r="K124">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>17</v>
+      </c>
+      <c r="B125" t="s">
+        <v>136</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F125" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="G125">
+        <v>0</v>
+      </c>
+      <c r="H125">
+        <v>0</v>
+      </c>
+      <c r="I125" t="s">
+        <v>489</v>
+      </c>
+      <c r="J125" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="K125" s="10">
+        <v>1</v>
+      </c>
+      <c r="L125" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D126" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="G126">
+        <v>0</v>
+      </c>
+      <c r="H126">
+        <v>0</v>
+      </c>
+      <c r="I126" t="s">
+        <v>489</v>
+      </c>
+      <c r="J126" t="s">
+        <v>348</v>
+      </c>
+      <c r="K126">
+        <v>51</v>
+      </c>
+      <c r="L126" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>290</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F127" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G127">
+        <v>0</v>
+      </c>
+      <c r="H127">
+        <v>0</v>
+      </c>
+      <c r="I127" t="s">
+        <v>466</v>
+      </c>
+      <c r="J127" t="s">
+        <v>294</v>
+      </c>
+      <c r="K127" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D128" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
+      <c r="H128">
+        <v>0</v>
+      </c>
+      <c r="I128" t="s">
+        <v>466</v>
+      </c>
+      <c r="J128" t="s">
+        <v>295</v>
+      </c>
+      <c r="K128" s="10">
+        <v>1</v>
+      </c>
+      <c r="L128" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="129" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D129" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F129" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="G120">
-        <v>0</v>
-      </c>
-      <c r="H120">
-        <v>0</v>
-      </c>
-      <c r="I120" t="s">
+      <c r="G129">
+        <v>0</v>
+      </c>
+      <c r="H129">
+        <v>0</v>
+      </c>
+      <c r="I129" t="s">
         <v>466</v>
       </c>
-      <c r="J120" t="s">
+      <c r="J129" t="s">
         <v>293</v>
       </c>
-      <c r="K120">
+      <c r="K129">
         <v>46</v>
       </c>
-      <c r="L120" t="s">
+      <c r="L129" t="s">
         <v>390</v>
+      </c>
+    </row>
+    <row r="141" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E141" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="142" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E142" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="143" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E143" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="144" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E144" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E145" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E146" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E147" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E148" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E149" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E150" t="s">
+        <v>501</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multiple enclosures in the same vc config collection
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="518">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1555,10 +1555,25 @@
     <t>porterr_bad_os</t>
   </si>
   <si>
-    <t>porterr_enc_crc</t>
-  </si>
-  <si>
     <t>enc_crc</t>
+  </si>
+  <si>
+    <t>porterr_enc_crc_bad_os</t>
+  </si>
+  <si>
+    <t>Uralsibins</t>
+  </si>
+  <si>
+    <t>SAN_Assessment</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Uralsib\OCT21\FCSWITCH</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Uralsib\OCT21\blade</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Uralsibins\SAN Assessment\OCT2021</t>
   </si>
 </sst>
 </file>
@@ -1981,112 +1996,112 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AO14"/>
+  <dimension ref="A1:AP14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="3" width="70" customWidth="1"/>
-    <col min="4" max="4" width="124.42578125" customWidth="1"/>
-    <col min="5" max="5" width="70" customWidth="1"/>
-    <col min="6" max="6" width="48.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1"/>
-    <col min="8" max="8" width="80.140625" customWidth="1"/>
-    <col min="9" max="9" width="35.7109375" customWidth="1"/>
-    <col min="10" max="11" width="122.7109375" customWidth="1"/>
-    <col min="12" max="12" width="48.42578125" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" customWidth="1"/>
-    <col min="14" max="14" width="80.140625" customWidth="1"/>
-    <col min="15" max="15" width="68.5703125" customWidth="1"/>
-    <col min="16" max="16" width="48.7109375" customWidth="1"/>
-    <col min="17" max="17" width="62" customWidth="1"/>
-    <col min="18" max="20" width="89.5703125" customWidth="1"/>
-    <col min="21" max="21" width="69.85546875" customWidth="1"/>
-    <col min="22" max="22" width="52.140625" customWidth="1"/>
-    <col min="23" max="23" width="73.140625" customWidth="1"/>
-    <col min="24" max="24" width="29.7109375" customWidth="1"/>
-    <col min="25" max="26" width="76" customWidth="1"/>
-    <col min="27" max="27" width="72.28515625" customWidth="1"/>
-    <col min="28" max="28" width="61.7109375" customWidth="1"/>
-    <col min="29" max="29" width="60" customWidth="1"/>
-    <col min="30" max="30" width="38.140625" customWidth="1"/>
-    <col min="31" max="31" width="69" customWidth="1"/>
-    <col min="32" max="32" width="72.42578125" customWidth="1"/>
-    <col min="33" max="33" width="111.5703125" customWidth="1"/>
-    <col min="34" max="34" width="72.5703125" customWidth="1"/>
-    <col min="35" max="35" width="86.85546875" customWidth="1"/>
-    <col min="36" max="37" width="64.7109375" customWidth="1"/>
-    <col min="38" max="38" width="54.5703125" customWidth="1"/>
-    <col min="39" max="39" width="75.42578125" customWidth="1"/>
-    <col min="40" max="40" width="58.140625" customWidth="1"/>
+    <col min="2" max="4" width="70" customWidth="1"/>
+    <col min="5" max="5" width="124.42578125" customWidth="1"/>
+    <col min="6" max="6" width="70" customWidth="1"/>
+    <col min="7" max="7" width="48.85546875" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" customWidth="1"/>
+    <col min="9" max="9" width="80.140625" customWidth="1"/>
+    <col min="10" max="10" width="35.7109375" customWidth="1"/>
+    <col min="11" max="12" width="122.7109375" customWidth="1"/>
+    <col min="13" max="13" width="48.42578125" customWidth="1"/>
+    <col min="14" max="14" width="29.7109375" customWidth="1"/>
+    <col min="15" max="15" width="80.140625" customWidth="1"/>
+    <col min="16" max="16" width="68.5703125" customWidth="1"/>
+    <col min="17" max="17" width="48.7109375" customWidth="1"/>
+    <col min="18" max="18" width="62" customWidth="1"/>
+    <col min="19" max="21" width="89.5703125" customWidth="1"/>
+    <col min="22" max="22" width="69.85546875" customWidth="1"/>
+    <col min="23" max="23" width="52.140625" customWidth="1"/>
+    <col min="24" max="24" width="73.140625" customWidth="1"/>
+    <col min="25" max="25" width="29.7109375" customWidth="1"/>
+    <col min="26" max="27" width="76" customWidth="1"/>
+    <col min="28" max="28" width="72.28515625" customWidth="1"/>
+    <col min="29" max="29" width="61.7109375" customWidth="1"/>
+    <col min="30" max="30" width="60" customWidth="1"/>
+    <col min="31" max="31" width="38.140625" customWidth="1"/>
+    <col min="32" max="32" width="69" customWidth="1"/>
+    <col min="33" max="33" width="72.42578125" customWidth="1"/>
+    <col min="34" max="34" width="111.5703125" customWidth="1"/>
+    <col min="35" max="35" width="72.5703125" customWidth="1"/>
+    <col min="36" max="36" width="86.85546875" customWidth="1"/>
+    <col min="37" max="38" width="64.7109375" customWidth="1"/>
+    <col min="39" max="39" width="54.5703125" customWidth="1"/>
+    <col min="40" max="40" width="75.42578125" customWidth="1"/>
+    <col min="41" max="41" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>413</v>
+        <v>513</v>
       </c>
       <c r="D2" t="s">
         <v>413</v>
       </c>
       <c r="E2" t="s">
+        <v>413</v>
+      </c>
+      <c r="F2" t="s">
         <v>451</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>438</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>413</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>233</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>391</v>
-      </c>
-      <c r="J2" t="s">
-        <v>385</v>
       </c>
       <c r="K2" t="s">
         <v>385</v>
       </c>
       <c r="L2" t="s">
+        <v>385</v>
+      </c>
+      <c r="M2" t="s">
         <v>377</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>357</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>325</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>315</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>308</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>305</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>301</v>
-      </c>
-      <c r="S2" t="s">
-        <v>309</v>
       </c>
       <c r="T2" t="s">
         <v>309</v>
@@ -2095,147 +2110,153 @@
         <v>309</v>
       </c>
       <c r="V2" t="s">
+        <v>309</v>
+      </c>
+      <c r="W2" t="s">
         <v>272</v>
-      </c>
-      <c r="W2" t="s">
-        <v>268</v>
       </c>
       <c r="X2" t="s">
         <v>268</v>
       </c>
       <c r="Y2" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="Z2" t="s">
         <v>251</v>
       </c>
       <c r="AA2" t="s">
+        <v>251</v>
+      </c>
+      <c r="AB2" t="s">
         <v>233</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>227</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>186</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>185</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>154</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>110</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>97</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>83</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>276</v>
       </c>
       <c r="C3" s="12">
+        <v>44484</v>
+      </c>
+      <c r="D3" s="12">
         <v>44473</v>
       </c>
-      <c r="D3" s="12">
+      <c r="E3" s="12">
         <v>44469</v>
       </c>
-      <c r="E3" s="12">
+      <c r="F3" s="12">
         <v>44453</v>
       </c>
-      <c r="F3" s="12">
+      <c r="G3" s="12">
         <v>44426</v>
       </c>
-      <c r="G3" s="12">
+      <c r="H3" s="12">
         <v>44330</v>
       </c>
-      <c r="H3" s="12">
+      <c r="I3" s="12">
         <v>44307</v>
       </c>
-      <c r="I3" s="12">
+      <c r="J3" s="12">
         <v>44294</v>
       </c>
-      <c r="J3" s="12">
+      <c r="K3" s="12">
         <v>44343</v>
       </c>
-      <c r="K3" s="12">
+      <c r="L3" s="12">
         <v>44292</v>
       </c>
-      <c r="L3" s="12">
+      <c r="M3" s="12">
         <v>29681</v>
       </c>
-      <c r="M3" s="12">
+      <c r="N3" s="12">
         <v>44286</v>
       </c>
-      <c r="N3" s="12">
+      <c r="O3" s="12">
         <v>44260</v>
       </c>
-      <c r="O3" s="12">
+      <c r="P3" s="12">
         <v>44244</v>
       </c>
-      <c r="P3" s="12">
+      <c r="Q3" s="12">
         <v>44245</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="R3" s="12">
         <v>44223</v>
       </c>
-      <c r="R3" s="12">
+      <c r="S3" s="12">
         <v>44209</v>
       </c>
-      <c r="S3" s="12">
+      <c r="T3" s="12">
         <v>44253</v>
       </c>
-      <c r="T3" s="12">
+      <c r="U3" s="12">
         <v>44237</v>
       </c>
-      <c r="W3" s="12">
+      <c r="X3" s="12">
         <v>44181</v>
       </c>
-      <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP3" s="1"/>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>481</v>
       </c>
       <c r="C4" t="s">
-        <v>475</v>
+        <v>514</v>
       </c>
       <c r="D4" t="s">
         <v>475</v>
       </c>
       <c r="E4" t="s">
-        <v>318</v>
+        <v>475</v>
       </c>
       <c r="F4" t="s">
         <v>318</v>
@@ -2244,13 +2265,13 @@
         <v>318</v>
       </c>
       <c r="H4" t="s">
+        <v>318</v>
+      </c>
+      <c r="I4" t="s">
         <v>404</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>392</v>
-      </c>
-      <c r="J4" t="s">
-        <v>318</v>
       </c>
       <c r="K4" t="s">
         <v>318</v>
@@ -2259,386 +2280,398 @@
         <v>318</v>
       </c>
       <c r="M4" t="s">
+        <v>318</v>
+      </c>
+      <c r="N4" t="s">
         <v>358</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>318</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>314</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>318</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>318</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>322</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>314</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>275</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>274</v>
       </c>
-      <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP4" s="1"/>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
+        <v>517</v>
+      </c>
+      <c r="D5" t="s">
         <v>486</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>476</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>452</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>439</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>414</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>405</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>393</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>417</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>387</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>378</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>359</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>326</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>316</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>320</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>306</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>300</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>323</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>312</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>310</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>273</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>277</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>270</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>252</v>
       </c>
       <c r="Z5" t="s">
         <v>252</v>
       </c>
       <c r="AA5" t="s">
+        <v>252</v>
+      </c>
+      <c r="AB5" t="s">
         <v>235</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>226</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>217</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>184</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>156</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>112</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>98</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>85</v>
       </c>
-      <c r="AI5" t="s">
-        <v>1</v>
-      </c>
       <c r="AJ5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK5" t="s">
         <v>74</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AL5" t="s">
         <v>72</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AM5" t="s">
         <v>4</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AN5" t="s">
         <v>25</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>60</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AP5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C6" t="s">
+        <v>515</v>
+      </c>
+      <c r="D6" t="s">
         <v>487</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>477</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>453</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>440</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>415</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>406</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>394</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>418</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>386</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>379</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>360</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>347</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>317</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>319</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>307</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>302</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>324</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>313</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>311</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>271</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>278</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>269</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>264</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>253</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>234</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>224</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>216</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>183</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>155</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>111</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>107</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>84</v>
       </c>
-      <c r="AI6" t="s">
-        <v>0</v>
-      </c>
       <c r="AJ6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="s">
         <v>73</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" t="s">
         <v>71</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AM6" t="s">
         <v>3</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>24</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>59</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AP6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" t="s">
+        <v>516</v>
+      </c>
+      <c r="E7" t="s">
         <v>478</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>441</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>416</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>419</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>380</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>327</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>303</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>254</v>
       </c>
       <c r="Z7" t="s">
         <v>254</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AA7" t="s">
+        <v>254</v>
+      </c>
+      <c r="AC7" t="s">
         <v>225</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>157</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>108</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AI7" t="s">
         <v>87</v>
       </c>
-      <c r="AK7" t="s">
+      <c r="AL7" t="s">
         <v>99</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AO7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>470</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>407</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>328</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>256</v>
       </c>
       <c r="Z8" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AA8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>420</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>485</v>
       </c>
@@ -2655,8 +2688,8 @@
   <dimension ref="A1:L150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I87" sqref="I87"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H81" sqref="H80:H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5041,7 +5074,7 @@
         <v>0</v>
       </c>
       <c r="H84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I84" t="s">
         <v>172</v>
@@ -5283,7 +5316,7 @@
         <v>95</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -5295,7 +5328,7 @@
         <v>172</v>
       </c>
       <c r="J94" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="K94">
         <v>1</v>
@@ -6172,10 +6205,10 @@
         <v>292</v>
       </c>
       <c r="G129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I129" t="s">
         <v>466</v>

</xml_diff>

<commit_message>
parse dediacted nsshow files
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -13,14 +13,14 @@
     <sheet name="software" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$L$129</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$L$130</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="522">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1574,6 +1574,18 @@
   </si>
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Uralsibins\SAN Assessment\OCT2021</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Uralsib\OCT21\nsshow</t>
+  </si>
+  <si>
+    <t>nsshow_dedicated_folder</t>
+  </si>
+  <si>
+    <t>nsshow_dedicated</t>
+  </si>
+  <si>
+    <t>Dedicated files Name Serevr collection</t>
   </si>
 </sst>
 </file>
@@ -1996,10 +2008,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AP14"/>
+  <dimension ref="A1:AP15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2652,27 +2664,35 @@
       </c>
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
+        <v>519</v>
+      </c>
+      <c r="C10" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>232</v>
-      </c>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>485</v>
       </c>
     </row>
@@ -2685,11 +2705,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:L150"/>
+  <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H81" sqref="H80:H81"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3253,22 +3273,19 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E17" t="s">
-        <v>36</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>41</v>
+        <v>520</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -3277,14 +3294,12 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>399</v>
-      </c>
-      <c r="K17" s="10">
-        <v>1</v>
-      </c>
+        <v>521</v>
+      </c>
+      <c r="K17" s="10"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -3300,10 +3315,10 @@
         <v>94</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -3315,7 +3330,7 @@
         <v>144</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K18" s="10">
         <v>1</v>
@@ -3335,10 +3350,10 @@
         <v>94</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -3350,7 +3365,7 @@
         <v>144</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="K19" s="10">
         <v>1</v>
@@ -3370,10 +3385,10 @@
         <v>94</v>
       </c>
       <c r="E20" t="s">
-        <v>448</v>
+        <v>32</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>448</v>
+        <v>32</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -3385,7 +3400,7 @@
         <v>144</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>449</v>
+        <v>401</v>
       </c>
       <c r="K20" s="10">
         <v>1</v>
@@ -3393,22 +3408,22 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>122</v>
+        <v>41</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>94</v>
       </c>
       <c r="E21" t="s">
-        <v>17</v>
+        <v>448</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>44</v>
+        <v>448</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -3417,10 +3432,10 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>402</v>
+        <v>449</v>
       </c>
       <c r="K21" s="10">
         <v>1</v>
@@ -3439,8 +3454,11 @@
       <c r="D22" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
       <c r="F22" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -3452,7 +3470,7 @@
         <v>142</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>454</v>
+        <v>402</v>
       </c>
       <c r="K22" s="10">
         <v>1</v>
@@ -3472,7 +3490,7 @@
         <v>94</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -3484,7 +3502,7 @@
         <v>142</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="K23" s="10">
         <v>1</v>
@@ -3504,7 +3522,7 @@
         <v>94</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -3516,13 +3534,16 @@
         <v>142</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="K24" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>12</v>
+      </c>
       <c r="B25" s="4" t="s">
         <v>123</v>
       </c>
@@ -3533,7 +3554,7 @@
         <v>94</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -3545,7 +3566,7 @@
         <v>142</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="K25" s="10">
         <v>1</v>
@@ -3562,7 +3583,7 @@
         <v>94</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -3574,27 +3595,24 @@
         <v>142</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>212</v>
+        <v>456</v>
       </c>
       <c r="K26" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>13</v>
-      </c>
       <c r="B27" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -3603,16 +3621,19 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>362</v>
+        <v>212</v>
       </c>
       <c r="K27" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>13</v>
+      </c>
       <c r="B28" s="4" t="s">
         <v>126</v>
       </c>
@@ -3623,7 +3644,7 @@
         <v>94</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -3635,7 +3656,7 @@
         <v>148</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K28" s="10">
         <v>1</v>
@@ -3652,7 +3673,7 @@
         <v>94</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -3664,7 +3685,7 @@
         <v>148</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K29" s="10">
         <v>1</v>
@@ -3681,7 +3702,7 @@
         <v>94</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -3693,7 +3714,7 @@
         <v>148</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K30" s="10">
         <v>1</v>
@@ -3710,7 +3731,7 @@
         <v>94</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -3722,7 +3743,7 @@
         <v>148</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K31" s="10">
         <v>1</v>
@@ -3739,7 +3760,7 @@
         <v>94</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>236</v>
+        <v>53</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -3751,7 +3772,7 @@
         <v>148</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K32" s="10">
         <v>1</v>
@@ -3768,7 +3789,7 @@
         <v>94</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -3780,7 +3801,7 @@
         <v>148</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K33" s="10">
         <v>1</v>
@@ -3788,16 +3809,16 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>218</v>
+        <v>126</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>219</v>
+        <v>125</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>219</v>
+        <v>237</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -3806,10 +3827,10 @@
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>220</v>
+        <v>148</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="K34" s="10">
         <v>1</v>
@@ -3817,16 +3838,16 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>288</v>
+        <v>218</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>289</v>
+        <v>219</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>285</v>
+        <v>219</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -3835,30 +3856,27 @@
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>286</v>
+        <v>220</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>287</v>
+        <v>361</v>
       </c>
       <c r="K35" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>19</v>
-      </c>
       <c r="B36" s="4" t="s">
-        <v>114</v>
+        <v>288</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>130</v>
+        <v>289</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>88</v>
+        <v>285</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -3867,16 +3885,19 @@
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>457</v>
+        <v>286</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>384</v>
+        <v>287</v>
       </c>
       <c r="K36" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>19</v>
+      </c>
       <c r="B37" s="4" t="s">
         <v>114</v>
       </c>
@@ -3887,7 +3908,7 @@
         <v>94</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G37">
         <v>0</v>
@@ -3899,7 +3920,7 @@
         <v>457</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K37" s="10">
         <v>1</v>
@@ -3916,7 +3937,7 @@
         <v>94</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -3928,7 +3949,7 @@
         <v>457</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="K38" s="10">
         <v>1</v>
@@ -3936,14 +3957,16 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="C39" s="4"/>
+        <v>114</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="D39" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>258</v>
+        <v>153</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -3952,10 +3975,10 @@
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>260</v>
+        <v>382</v>
       </c>
       <c r="K39" s="10">
         <v>1</v>
@@ -3970,7 +3993,7 @@
         <v>94</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -3982,7 +4005,7 @@
         <v>458</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K40" s="10">
         <v>1</v>
@@ -3990,14 +4013,14 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>352</v>
+        <v>257</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>355</v>
+        <v>259</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -4006,10 +4029,10 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>356</v>
+        <v>261</v>
       </c>
       <c r="K41" s="10">
         <v>1</v>
@@ -4024,7 +4047,7 @@
         <v>94</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -4036,7 +4059,7 @@
         <v>459</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="K42" s="10">
         <v>1</v>
@@ -4051,7 +4074,7 @@
         <v>94</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -4063,7 +4086,7 @@
         <v>459</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K43" s="10">
         <v>1</v>
@@ -4078,7 +4101,7 @@
         <v>94</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>389</v>
+        <v>351</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -4090,47 +4113,51 @@
         <v>459</v>
       </c>
       <c r="J44" s="10" t="s">
+        <v>354</v>
+      </c>
+      <c r="K44" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45" t="s">
+        <v>459</v>
+      </c>
+      <c r="J45" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="K44" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="K45" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>15</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>137</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45" t="s">
-        <v>158</v>
-      </c>
-      <c r="J45" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="K45" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D46" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>429</v>
+        <v>55</v>
       </c>
       <c r="G46">
         <v>0</v>
@@ -4152,8 +4179,8 @@
       <c r="D47" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F47" s="8" t="s">
-        <v>56</v>
+      <c r="F47" s="9" t="s">
+        <v>429</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -4165,7 +4192,7 @@
         <v>158</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>298</v>
+        <v>212</v>
       </c>
       <c r="K47" s="10">
         <v>1</v>
@@ -4176,7 +4203,7 @@
         <v>95</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -4188,44 +4215,44 @@
         <v>158</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>212</v>
+        <v>298</v>
       </c>
       <c r="K48" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>161</v>
-      </c>
       <c r="D49" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49" t="s">
+        <v>158</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="K49" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>161</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F50" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-      <c r="I49" t="s">
-        <v>162</v>
-      </c>
-      <c r="J49" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="K49" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D50" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -4236,49 +4263,48 @@
       <c r="I50" t="s">
         <v>162</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="K50" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D51" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51" t="s">
+        <v>162</v>
+      </c>
+      <c r="J51" t="s">
         <v>199</v>
       </c>
-      <c r="K50">
+      <c r="K51">
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52">
         <v>16</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>139</v>
       </c>
-      <c r="D51" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
-      <c r="I51" t="s">
-        <v>169</v>
-      </c>
-      <c r="J51" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="K51" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D52" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E52" s="16"/>
-      <c r="F52" s="2" t="s">
-        <v>434</v>
+      <c r="F52" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -4290,21 +4316,19 @@
         <v>169</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>435</v>
+        <v>282</v>
       </c>
       <c r="K52" s="10">
         <v>1</v>
-      </c>
-      <c r="L52" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D53" s="6" t="s">
         <v>95</v>
       </c>
+      <c r="E53" s="16"/>
       <c r="F53" s="2" t="s">
-        <v>163</v>
+        <v>434</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -4316,18 +4340,21 @@
         <v>169</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>212</v>
+        <v>435</v>
       </c>
       <c r="K53" s="10">
         <v>1</v>
       </c>
+      <c r="L53" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D54" s="5" t="s">
-        <v>96</v>
+      <c r="D54" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>61</v>
+        <v>163</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -4338,11 +4365,11 @@
       <c r="I54" t="s">
         <v>169</v>
       </c>
-      <c r="J54" t="s">
-        <v>191</v>
-      </c>
-      <c r="K54">
-        <v>12</v>
+      <c r="J54" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="K54" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -4350,7 +4377,7 @@
         <v>96</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -4362,10 +4389,10 @@
         <v>169</v>
       </c>
       <c r="J55" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K55">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -4373,7 +4400,7 @@
         <v>96</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -4385,10 +4412,10 @@
         <v>169</v>
       </c>
       <c r="J56" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="K56">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -4396,7 +4423,7 @@
         <v>96</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -4408,10 +4435,10 @@
         <v>169</v>
       </c>
       <c r="J57" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K57">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -4419,7 +4446,7 @@
         <v>96</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -4431,10 +4458,10 @@
         <v>169</v>
       </c>
       <c r="J58" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="K58">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -4442,7 +4469,7 @@
         <v>96</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>427</v>
+        <v>64</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -4454,10 +4481,10 @@
         <v>169</v>
       </c>
       <c r="J59" t="s">
-        <v>428</v>
+        <v>193</v>
       </c>
       <c r="K59">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -4465,7 +4492,7 @@
         <v>96</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>437</v>
+        <v>427</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -4477,50 +4504,50 @@
         <v>169</v>
       </c>
       <c r="J60" t="s">
+        <v>428</v>
+      </c>
+      <c r="K60">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D61" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61" t="s">
+        <v>169</v>
+      </c>
+      <c r="J61" t="s">
         <v>436</v>
       </c>
-      <c r="K60">
+      <c r="K61">
         <v>11</v>
       </c>
-      <c r="L60" t="s">
+      <c r="L61" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>18</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>138</v>
       </c>
-      <c r="D61" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-      <c r="I61" t="s">
-        <v>170</v>
-      </c>
-      <c r="J61" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="K61" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D62" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>279</v>
+        <v>69</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -4532,21 +4559,18 @@
         <v>170</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="K62" s="10">
         <v>1</v>
       </c>
-      <c r="L62" t="s">
-        <v>390</v>
-      </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D63" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>67</v>
+      <c r="D63" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>279</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -4557,11 +4581,14 @@
       <c r="I63" t="s">
         <v>170</v>
       </c>
-      <c r="J63" t="s">
-        <v>202</v>
-      </c>
-      <c r="K63">
-        <v>35</v>
+      <c r="J63" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="K63" s="10">
+        <v>1</v>
+      </c>
+      <c r="L63" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
@@ -4569,7 +4596,7 @@
         <v>96</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -4581,10 +4608,10 @@
         <v>170</v>
       </c>
       <c r="J64" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K64">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -4592,7 +4619,7 @@
         <v>96</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>283</v>
+        <v>68</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -4604,68 +4631,65 @@
         <v>170</v>
       </c>
       <c r="J65" t="s">
+        <v>203</v>
+      </c>
+      <c r="K65">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D66" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66" t="s">
+        <v>170</v>
+      </c>
+      <c r="J66" t="s">
         <v>284</v>
       </c>
-      <c r="K65">
+      <c r="K66">
         <v>32</v>
       </c>
-      <c r="L65" t="s">
+      <c r="L66" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67">
         <v>20</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>131</v>
       </c>
-      <c r="D66" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G66">
-        <v>0</v>
-      </c>
-      <c r="H66">
-        <v>0</v>
-      </c>
-      <c r="I66" t="s">
-        <v>171</v>
-      </c>
-      <c r="J66" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="K66" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D67" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>412</v>
+        <v>90</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67" t="s">
         <v>171</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>409</v>
+        <v>262</v>
       </c>
       <c r="K67" s="10">
         <v>1</v>
-      </c>
-      <c r="L67" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -4673,7 +4697,7 @@
         <v>95</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>265</v>
+        <v>412</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -4685,7 +4709,7 @@
         <v>171</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>266</v>
+        <v>409</v>
       </c>
       <c r="K68" s="10">
         <v>1</v>
@@ -4698,8 +4722,8 @@
       <c r="D69" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F69" s="2" t="s">
-        <v>238</v>
+      <c r="F69" s="9" t="s">
+        <v>265</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -4711,10 +4735,13 @@
         <v>171</v>
       </c>
       <c r="J69" s="10" t="s">
-        <v>330</v>
+        <v>266</v>
       </c>
       <c r="K69" s="10">
         <v>1</v>
+      </c>
+      <c r="L69" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -4722,7 +4749,7 @@
         <v>95</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -4734,18 +4761,18 @@
         <v>171</v>
       </c>
       <c r="J70" s="10" t="s">
-        <v>240</v>
+        <v>330</v>
       </c>
       <c r="K70" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D71" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="F71" s="11" t="s">
-        <v>242</v>
+      <c r="D71" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -4764,14 +4791,11 @@
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
-        <v>133</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F72" s="8" t="s">
-        <v>109</v>
+      <c r="D72" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="F72" s="11" t="s">
+        <v>242</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -4783,7 +4807,7 @@
         <v>171</v>
       </c>
       <c r="J72" s="10" t="s">
-        <v>371</v>
+        <v>240</v>
       </c>
       <c r="K72" s="10">
         <v>1</v>
@@ -4791,16 +4815,13 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>119</v>
-      </c>
-      <c r="C73" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F73" s="7" t="s">
-        <v>93</v>
+      <c r="F73" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -4812,18 +4833,24 @@
         <v>171</v>
       </c>
       <c r="J73" s="10" t="s">
-        <v>329</v>
+        <v>371</v>
       </c>
       <c r="K73" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C74" t="s">
+        <v>132</v>
+      </c>
       <c r="D74" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>304</v>
+        <v>93</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -4835,21 +4862,18 @@
         <v>171</v>
       </c>
       <c r="J74" s="10" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="K74" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
-        <v>134</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>408</v>
+      <c r="D75" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>304</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -4860,22 +4884,22 @@
       <c r="I75" t="s">
         <v>171</v>
       </c>
-      <c r="J75" t="s">
-        <v>194</v>
-      </c>
-      <c r="K75">
-        <v>17</v>
+      <c r="J75" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="K75" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>101</v>
+        <v>408</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -4887,18 +4911,21 @@
         <v>171</v>
       </c>
       <c r="J76" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K76">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>135</v>
+      </c>
       <c r="D77" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -4910,10 +4937,10 @@
         <v>171</v>
       </c>
       <c r="J77" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K77">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -4921,7 +4948,7 @@
         <v>96</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -4933,10 +4960,10 @@
         <v>171</v>
       </c>
       <c r="J78" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="K78">
-        <v>57</v>
+        <v>16</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -4944,7 +4971,7 @@
         <v>96</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -4956,10 +4983,10 @@
         <v>171</v>
       </c>
       <c r="J79" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K79">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
@@ -4967,7 +4994,7 @@
         <v>96</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -4979,10 +5006,10 @@
         <v>171</v>
       </c>
       <c r="J80" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K80">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.25">
@@ -4990,7 +5017,7 @@
         <v>96</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -5002,10 +5029,10 @@
         <v>171</v>
       </c>
       <c r="J81" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K81">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.25">
@@ -5013,7 +5040,7 @@
         <v>96</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>411</v>
+        <v>106</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -5025,13 +5052,10 @@
         <v>171</v>
       </c>
       <c r="J82" t="s">
-        <v>410</v>
+        <v>207</v>
       </c>
       <c r="K82">
-        <v>53</v>
-      </c>
-      <c r="L82" t="s">
-        <v>390</v>
+        <v>56</v>
       </c>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
@@ -5039,7 +5063,7 @@
         <v>96</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>267</v>
+        <v>411</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -5051,47 +5075,50 @@
         <v>171</v>
       </c>
       <c r="J83" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="K83">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L83" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
+      <c r="D84" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84" t="s">
+        <v>171</v>
+      </c>
+      <c r="J84" t="s">
+        <v>403</v>
+      </c>
+      <c r="K84">
+        <v>52</v>
+      </c>
+      <c r="L84" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
         <v>165</v>
       </c>
-      <c r="D84" s="6" t="s">
+      <c r="D85" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F84" s="9" t="s">
+      <c r="F85" s="9" t="s">
         <v>214</v>
-      </c>
-      <c r="G84">
-        <v>0</v>
-      </c>
-      <c r="H84">
-        <v>0</v>
-      </c>
-      <c r="I84" t="s">
-        <v>172</v>
-      </c>
-      <c r="J84" t="s">
-        <v>296</v>
-      </c>
-      <c r="K84" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D85" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -5103,10 +5130,10 @@
         <v>172</v>
       </c>
       <c r="J85" t="s">
-        <v>198</v>
-      </c>
-      <c r="K85">
-        <v>41</v>
+        <v>296</v>
+      </c>
+      <c r="K85" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.25">
@@ -5114,7 +5141,7 @@
         <v>96</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -5126,10 +5153,10 @@
         <v>172</v>
       </c>
       <c r="J86" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="K86">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.25">
@@ -5137,7 +5164,7 @@
         <v>96</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -5149,18 +5176,18 @@
         <v>172</v>
       </c>
       <c r="J87" t="s">
-        <v>263</v>
+        <v>208</v>
       </c>
       <c r="K87">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D88" s="6" t="s">
-        <v>95</v>
+      <c r="D88" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>503</v>
+        <v>168</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -5172,13 +5199,10 @@
         <v>172</v>
       </c>
       <c r="J88" t="s">
-        <v>492</v>
+        <v>263</v>
       </c>
       <c r="K88">
-        <v>1</v>
-      </c>
-      <c r="L88" t="s">
-        <v>502</v>
+        <v>42</v>
       </c>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.25">
@@ -5186,7 +5210,7 @@
         <v>95</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -5198,7 +5222,7 @@
         <v>172</v>
       </c>
       <c r="J89" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="K89">
         <v>1</v>
@@ -5212,7 +5236,7 @@
         <v>95</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -5224,7 +5248,7 @@
         <v>172</v>
       </c>
       <c r="J90" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="K90">
         <v>1</v>
@@ -5238,7 +5262,7 @@
         <v>95</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -5250,7 +5274,7 @@
         <v>172</v>
       </c>
       <c r="J91" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="K91">
         <v>1</v>
@@ -5264,7 +5288,7 @@
         <v>95</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -5276,7 +5300,7 @@
         <v>172</v>
       </c>
       <c r="J92" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K92">
         <v>1</v>
@@ -5290,7 +5314,7 @@
         <v>95</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -5302,7 +5326,7 @@
         <v>172</v>
       </c>
       <c r="J93" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="K93">
         <v>1</v>
@@ -5316,7 +5340,7 @@
         <v>95</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -5328,7 +5352,7 @@
         <v>172</v>
       </c>
       <c r="J94" t="s">
-        <v>511</v>
+        <v>497</v>
       </c>
       <c r="K94">
         <v>1</v>
@@ -5342,7 +5366,7 @@
         <v>95</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -5354,7 +5378,7 @@
         <v>172</v>
       </c>
       <c r="J95" t="s">
-        <v>500</v>
+        <v>511</v>
       </c>
       <c r="K95">
         <v>1</v>
@@ -5368,7 +5392,7 @@
         <v>95</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -5380,7 +5404,7 @@
         <v>172</v>
       </c>
       <c r="J96" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="K96">
         <v>1</v>
@@ -5390,14 +5414,11 @@
       </c>
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>467</v>
-      </c>
       <c r="D97" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>430</v>
+        <v>510</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -5406,21 +5427,27 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>462</v>
+        <v>172</v>
       </c>
       <c r="J97" t="s">
-        <v>432</v>
-      </c>
-      <c r="K97" s="10">
-        <v>1</v>
+        <v>501</v>
+      </c>
+      <c r="K97">
+        <v>1</v>
+      </c>
+      <c r="L97" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="98" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>467</v>
+      </c>
       <c r="D98" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>164</v>
+        <v>430</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -5432,7 +5459,7 @@
         <v>462</v>
       </c>
       <c r="J98" t="s">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="K98" s="10">
         <v>1</v>
@@ -5443,7 +5470,7 @@
         <v>95</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>421</v>
+        <v>164</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -5455,13 +5482,10 @@
         <v>462</v>
       </c>
       <c r="J99" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="K99" s="10">
         <v>1</v>
-      </c>
-      <c r="L99" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="100" spans="2:12" x14ac:dyDescent="0.25">
@@ -5469,7 +5493,7 @@
         <v>95</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>468</v>
+        <v>421</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -5481,7 +5505,7 @@
         <v>462</v>
       </c>
       <c r="J100" t="s">
-        <v>469</v>
+        <v>425</v>
       </c>
       <c r="K100" s="10">
         <v>1</v>
@@ -5491,11 +5515,11 @@
       </c>
     </row>
     <row r="101" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D101" s="5" t="s">
-        <v>96</v>
+      <c r="D101" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>431</v>
+        <v>468</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -5507,10 +5531,13 @@
         <v>462</v>
       </c>
       <c r="J101" t="s">
-        <v>433</v>
-      </c>
-      <c r="K101">
-        <v>44</v>
+        <v>469</v>
+      </c>
+      <c r="K101" s="10">
+        <v>1</v>
+      </c>
+      <c r="L101" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="102" spans="2:12" x14ac:dyDescent="0.25">
@@ -5518,7 +5545,7 @@
         <v>96</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -5530,10 +5557,10 @@
         <v>462</v>
       </c>
       <c r="J102" t="s">
-        <v>197</v>
+        <v>433</v>
       </c>
       <c r="K102">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="103" spans="2:12" x14ac:dyDescent="0.25">
@@ -5541,7 +5568,7 @@
         <v>96</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -5553,13 +5580,10 @@
         <v>462</v>
       </c>
       <c r="J103" t="s">
-        <v>423</v>
+        <v>197</v>
       </c>
       <c r="K103">
-        <v>33</v>
-      </c>
-      <c r="L103" t="s">
-        <v>390</v>
+        <v>36</v>
       </c>
     </row>
     <row r="104" spans="2:12" x14ac:dyDescent="0.25">
@@ -5567,7 +5591,7 @@
         <v>96</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>460</v>
+        <v>422</v>
       </c>
       <c r="G104">
         <v>0</v>
@@ -5579,24 +5603,21 @@
         <v>462</v>
       </c>
       <c r="J104" t="s">
-        <v>461</v>
+        <v>423</v>
       </c>
       <c r="K104">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L104" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="105" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>176</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F105" s="9" t="s">
-        <v>177</v>
+      <c r="D105" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>460</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -5605,24 +5626,27 @@
         <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>463</v>
-      </c>
-      <c r="J105" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="K105" s="10">
-        <v>1</v>
+        <v>462</v>
+      </c>
+      <c r="J105" t="s">
+        <v>461</v>
+      </c>
+      <c r="K105">
+        <v>31</v>
+      </c>
+      <c r="L105" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="106" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>248</v>
+        <v>176</v>
       </c>
       <c r="D106" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F106" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -5634,7 +5658,7 @@
         <v>463</v>
       </c>
       <c r="J106" s="10" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K106" s="10">
         <v>1</v>
@@ -5642,13 +5666,13 @@
     </row>
     <row r="107" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -5660,24 +5684,21 @@
         <v>463</v>
       </c>
       <c r="J107" s="10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K107" s="10">
         <v>1</v>
-      </c>
-      <c r="L107" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="108" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D108" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>213</v>
+        <v>187</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -5689,7 +5710,7 @@
         <v>463</v>
       </c>
       <c r="J108" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K108" s="10">
         <v>1</v>
@@ -5699,11 +5720,14 @@
       </c>
     </row>
     <row r="109" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>249</v>
+      </c>
       <c r="D109" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F109" s="9" t="s">
-        <v>331</v>
+        <v>213</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -5715,7 +5739,7 @@
         <v>463</v>
       </c>
       <c r="J109" s="10" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="K109" s="10">
         <v>1</v>
@@ -5725,14 +5749,11 @@
       </c>
     </row>
     <row r="110" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>247</v>
-      </c>
       <c r="D110" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F110" s="9" t="s">
-        <v>243</v>
+        <v>331</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -5744,7 +5765,7 @@
         <v>463</v>
       </c>
       <c r="J110" s="10" t="s">
-        <v>244</v>
+        <v>332</v>
       </c>
       <c r="K110" s="10">
         <v>1</v>
@@ -5754,11 +5775,14 @@
       </c>
     </row>
     <row r="111" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D111" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>179</v>
+      <c r="B111" t="s">
+        <v>247</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F111" s="9" t="s">
+        <v>243</v>
       </c>
       <c r="G111">
         <v>0</v>
@@ -5769,11 +5793,14 @@
       <c r="I111" t="s">
         <v>463</v>
       </c>
-      <c r="J111" t="s">
-        <v>209</v>
-      </c>
-      <c r="K111">
-        <v>64</v>
+      <c r="J111" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="K111" s="10">
+        <v>1</v>
+      </c>
+      <c r="L111" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="112" spans="2:12" x14ac:dyDescent="0.25">
@@ -5781,7 +5808,7 @@
         <v>96</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -5793,10 +5820,10 @@
         <v>463</v>
       </c>
       <c r="J112" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K112">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
@@ -5804,7 +5831,7 @@
         <v>96</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>473</v>
+        <v>180</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -5816,10 +5843,10 @@
         <v>463</v>
       </c>
       <c r="J113" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="K113">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
@@ -5827,7 +5854,7 @@
         <v>96</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>188</v>
+        <v>473</v>
       </c>
       <c r="G114">
         <v>0</v>
@@ -5839,10 +5866,10 @@
         <v>463</v>
       </c>
       <c r="J114" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="K114">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
@@ -5850,7 +5877,7 @@
         <v>96</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>228</v>
+        <v>188</v>
       </c>
       <c r="G115">
         <v>0</v>
@@ -5862,10 +5889,10 @@
         <v>463</v>
       </c>
       <c r="J115" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="K115">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
@@ -5873,7 +5900,7 @@
         <v>96</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G116">
         <v>0</v>
@@ -5885,13 +5912,10 @@
         <v>463</v>
       </c>
       <c r="J116" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K116">
-        <v>69</v>
-      </c>
-      <c r="L116" t="s">
-        <v>390</v>
+        <v>67</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
@@ -5899,7 +5923,7 @@
         <v>96</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>189</v>
+        <v>230</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -5911,10 +5935,10 @@
         <v>463</v>
       </c>
       <c r="J117" t="s">
-        <v>338</v>
+        <v>231</v>
       </c>
       <c r="K117">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="L117" t="s">
         <v>390</v>
@@ -5925,7 +5949,7 @@
         <v>96</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>337</v>
+        <v>189</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -5937,10 +5961,10 @@
         <v>463</v>
       </c>
       <c r="J118" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="K118">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L118" t="s">
         <v>390</v>
@@ -5951,7 +5975,7 @@
         <v>96</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>245</v>
+        <v>337</v>
       </c>
       <c r="G119">
         <v>0</v>
@@ -5963,44 +5987,47 @@
         <v>463</v>
       </c>
       <c r="J119" t="s">
-        <v>246</v>
+        <v>339</v>
       </c>
       <c r="K119">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L119" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D120" s="6" t="s">
+      <c r="D120" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+      <c r="H120">
+        <v>0</v>
+      </c>
+      <c r="I120" t="s">
+        <v>463</v>
+      </c>
+      <c r="J120" t="s">
+        <v>246</v>
+      </c>
+      <c r="K120">
+        <v>61</v>
+      </c>
+      <c r="L120" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D121" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F120" s="2" t="s">
+      <c r="F121" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="G120">
-        <v>0</v>
-      </c>
-      <c r="H120">
-        <v>0</v>
-      </c>
-      <c r="I120" t="s">
-        <v>464</v>
-      </c>
-      <c r="J120" t="s">
-        <v>374</v>
-      </c>
-      <c r="K120" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D121" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>372</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -6012,10 +6039,10 @@
         <v>464</v>
       </c>
       <c r="J121" t="s">
-        <v>375</v>
-      </c>
-      <c r="K121">
-        <v>71</v>
+        <v>374</v>
+      </c>
+      <c r="K121" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
@@ -6023,7 +6050,7 @@
         <v>96</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>474</v>
+        <v>372</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -6035,41 +6062,41 @@
         <v>464</v>
       </c>
       <c r="J122" t="s">
+        <v>375</v>
+      </c>
+      <c r="K122">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D123" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="G123">
+        <v>0</v>
+      </c>
+      <c r="H123">
+        <v>0</v>
+      </c>
+      <c r="I123" t="s">
+        <v>464</v>
+      </c>
+      <c r="J123" t="s">
         <v>376</v>
       </c>
-      <c r="K122">
+      <c r="K123">
         <v>72</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D123" s="6" t="s">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D124" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F123" s="2" t="s">
+      <c r="F124" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="G123">
-        <v>0</v>
-      </c>
-      <c r="H123">
-        <v>0</v>
-      </c>
-      <c r="I123" t="s">
-        <v>465</v>
-      </c>
-      <c r="J123" t="s">
-        <v>297</v>
-      </c>
-      <c r="K123" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D124" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="G124">
         <v>0</v>
@@ -6081,50 +6108,47 @@
         <v>465</v>
       </c>
       <c r="J124" t="s">
+        <v>297</v>
+      </c>
+      <c r="K124" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D125" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G125">
+        <v>0</v>
+      </c>
+      <c r="H125">
+        <v>0</v>
+      </c>
+      <c r="I125" t="s">
+        <v>465</v>
+      </c>
+      <c r="J125" t="s">
         <v>223</v>
       </c>
-      <c r="K124">
+      <c r="K125">
         <v>45</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A125">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A126">
         <v>17</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B126" t="s">
         <v>136</v>
       </c>
-      <c r="D125" s="6" t="s">
+      <c r="D126" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F125" s="9" t="s">
+      <c r="F126" s="9" t="s">
         <v>491</v>
-      </c>
-      <c r="G125">
-        <v>0</v>
-      </c>
-      <c r="H125">
-        <v>0</v>
-      </c>
-      <c r="I125" t="s">
-        <v>489</v>
-      </c>
-      <c r="J125" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="K125" s="10">
-        <v>1</v>
-      </c>
-      <c r="L125" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D126" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F126" s="2" t="s">
-        <v>488</v>
       </c>
       <c r="G126">
         <v>0</v>
@@ -6135,48 +6159,51 @@
       <c r="I126" t="s">
         <v>489</v>
       </c>
-      <c r="J126" t="s">
-        <v>348</v>
-      </c>
-      <c r="K126">
-        <v>51</v>
+      <c r="J126" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="K126" s="10">
+        <v>1</v>
       </c>
       <c r="L126" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B127" t="s">
+      <c r="D127" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="G127">
+        <v>0</v>
+      </c>
+      <c r="H127">
+        <v>0</v>
+      </c>
+      <c r="I127" t="s">
+        <v>489</v>
+      </c>
+      <c r="J127" t="s">
+        <v>348</v>
+      </c>
+      <c r="K127">
+        <v>51</v>
+      </c>
+      <c r="L127" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
         <v>290</v>
       </c>
-      <c r="D127" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F127" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="G127">
-        <v>0</v>
-      </c>
-      <c r="H127">
-        <v>0</v>
-      </c>
-      <c r="I127" t="s">
-        <v>466</v>
-      </c>
-      <c r="J127" t="s">
-        <v>294</v>
-      </c>
-      <c r="K127" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D128" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F128" s="2" t="s">
-        <v>299</v>
+      <c r="F128" s="9" t="s">
+        <v>291</v>
       </c>
       <c r="G128">
         <v>0</v>
@@ -6188,88 +6215,111 @@
         <v>466</v>
       </c>
       <c r="J128" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K128" s="10">
         <v>1</v>
       </c>
-      <c r="L128" t="s">
-        <v>390</v>
-      </c>
     </row>
     <row r="129" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D129" s="5" t="s">
-        <v>96</v>
+      <c r="D129" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="G129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I129" t="s">
         <v>466</v>
       </c>
       <c r="J129" t="s">
-        <v>293</v>
-      </c>
-      <c r="K129">
-        <v>46</v>
+        <v>295</v>
+      </c>
+      <c r="K129" s="10">
+        <v>1</v>
       </c>
       <c r="L129" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="141" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="E141" t="s">
-        <v>492</v>
+    <row r="130" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D130" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G130">
+        <v>0</v>
+      </c>
+      <c r="H130">
+        <v>0</v>
+      </c>
+      <c r="I130" t="s">
+        <v>466</v>
+      </c>
+      <c r="J130" t="s">
+        <v>293</v>
+      </c>
+      <c r="K130">
+        <v>46</v>
+      </c>
+      <c r="L130" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="142" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E142" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="143" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E143" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="144" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E144" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="145" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E145" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="146" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E146" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="147" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E147" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="148" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E148" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="149" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E149" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="150" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E150" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E151" t="s">
         <v>501</v>
       </c>
     </row>

</xml_diff>

<commit_message>
duplicates from Device-Host_Name_Port_group removal
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -13,7 +13,7 @@
     <sheet name="software" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$L$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$L$151</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -1555,9 +1555,6 @@
     <t>porterr_bad_os</t>
   </si>
   <si>
-    <t>enc_crc</t>
-  </si>
-  <si>
     <t>porterr_enc_crc_bad_os</t>
   </si>
   <si>
@@ -1586,6 +1583,9 @@
   </si>
   <si>
     <t>Dedicated files Name Serevr collection</t>
+  </si>
+  <si>
+    <t>enc_crc, bad_os</t>
   </si>
 </sst>
 </file>
@@ -2065,7 +2065,7 @@
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D2" t="s">
         <v>413</v>
@@ -2262,7 +2262,7 @@
         <v>481</v>
       </c>
       <c r="C4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D4" t="s">
         <v>475</v>
@@ -2334,7 +2334,7 @@
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D5" t="s">
         <v>486</v>
@@ -2459,7 +2459,7 @@
         <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D6" t="s">
         <v>487</v>
@@ -2584,7 +2584,7 @@
         <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E7" t="s">
         <v>478</v>
@@ -2665,10 +2665,10 @@
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C10" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
@@ -2707,9 +2707,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3285,7 +3285,7 @@
         <v>94</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -3297,9 +3297,11 @@
         <v>143</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>521</v>
-      </c>
-      <c r="K17" s="10"/>
+        <v>520</v>
+      </c>
+      <c r="K17" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -4677,10 +4679,10 @@
         <v>90</v>
       </c>
       <c r="G67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67" t="s">
         <v>171</v>
@@ -5291,7 +5293,7 @@
         <v>506</v>
       </c>
       <c r="G92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H92">
         <v>0</v>
@@ -5366,10 +5368,10 @@
         <v>95</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H95">
         <v>0</v>
@@ -5378,7 +5380,7 @@
         <v>172</v>
       </c>
       <c r="J95" t="s">
-        <v>511</v>
+        <v>521</v>
       </c>
       <c r="K95">
         <v>1</v>

</xml_diff>

<commit_message>
report_column_usage_sr correction when force flag for device raname ii off
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -2741,8 +2741,8 @@
   <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E132" sqref="E132"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
3par config download procedure changed
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="529">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1598,6 +1598,15 @@
   </si>
   <si>
     <t>port_statistics</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\01.CUSTOMERS\Megafon\MegafonMSK\SAN Assessment\OCT21</t>
+  </si>
+  <si>
+    <t>Performance issue</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MegafonMSK\OCT21\ssave</t>
   </si>
 </sst>
 </file>
@@ -2020,51 +2029,53 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AQ15"/>
+  <dimension ref="A1:AR15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D27:D29"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="5" width="70" customWidth="1"/>
-    <col min="6" max="6" width="124.42578125" customWidth="1"/>
-    <col min="7" max="7" width="70" customWidth="1"/>
-    <col min="8" max="8" width="48.85546875" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" customWidth="1"/>
-    <col min="10" max="10" width="80.140625" customWidth="1"/>
-    <col min="11" max="11" width="35.7109375" customWidth="1"/>
-    <col min="12" max="13" width="122.7109375" customWidth="1"/>
-    <col min="14" max="14" width="48.42578125" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" customWidth="1"/>
-    <col min="16" max="16" width="80.140625" customWidth="1"/>
-    <col min="17" max="17" width="68.5703125" customWidth="1"/>
-    <col min="18" max="18" width="48.7109375" customWidth="1"/>
-    <col min="19" max="19" width="62" customWidth="1"/>
-    <col min="20" max="22" width="89.5703125" customWidth="1"/>
-    <col min="23" max="23" width="69.85546875" customWidth="1"/>
-    <col min="24" max="24" width="52.140625" customWidth="1"/>
-    <col min="25" max="25" width="73.140625" customWidth="1"/>
-    <col min="26" max="26" width="29.7109375" customWidth="1"/>
-    <col min="27" max="28" width="76" customWidth="1"/>
-    <col min="29" max="29" width="72.28515625" customWidth="1"/>
-    <col min="30" max="30" width="61.7109375" customWidth="1"/>
-    <col min="31" max="31" width="60" customWidth="1"/>
-    <col min="32" max="32" width="38.140625" customWidth="1"/>
-    <col min="33" max="33" width="69" customWidth="1"/>
-    <col min="34" max="34" width="72.42578125" customWidth="1"/>
-    <col min="35" max="35" width="111.5703125" customWidth="1"/>
-    <col min="36" max="36" width="72.5703125" customWidth="1"/>
-    <col min="37" max="37" width="86.85546875" customWidth="1"/>
-    <col min="38" max="39" width="64.7109375" customWidth="1"/>
-    <col min="40" max="40" width="54.5703125" customWidth="1"/>
-    <col min="41" max="41" width="75.42578125" customWidth="1"/>
-    <col min="42" max="42" width="58.140625" customWidth="1"/>
+    <col min="2" max="2" width="70" customWidth="1"/>
+    <col min="3" max="3" width="158.5703125" customWidth="1"/>
+    <col min="4" max="6" width="70" customWidth="1"/>
+    <col min="7" max="7" width="124.42578125" customWidth="1"/>
+    <col min="8" max="8" width="70" customWidth="1"/>
+    <col min="9" max="9" width="48.85546875" customWidth="1"/>
+    <col min="10" max="10" width="29.7109375" customWidth="1"/>
+    <col min="11" max="11" width="80.140625" customWidth="1"/>
+    <col min="12" max="12" width="35.7109375" customWidth="1"/>
+    <col min="13" max="14" width="122.7109375" customWidth="1"/>
+    <col min="15" max="15" width="48.42578125" customWidth="1"/>
+    <col min="16" max="16" width="29.7109375" customWidth="1"/>
+    <col min="17" max="17" width="80.140625" customWidth="1"/>
+    <col min="18" max="18" width="68.5703125" customWidth="1"/>
+    <col min="19" max="19" width="48.7109375" customWidth="1"/>
+    <col min="20" max="20" width="62" customWidth="1"/>
+    <col min="21" max="23" width="89.5703125" customWidth="1"/>
+    <col min="24" max="24" width="69.85546875" customWidth="1"/>
+    <col min="25" max="25" width="52.140625" customWidth="1"/>
+    <col min="26" max="26" width="73.140625" customWidth="1"/>
+    <col min="27" max="27" width="29.7109375" customWidth="1"/>
+    <col min="28" max="29" width="76" customWidth="1"/>
+    <col min="30" max="30" width="72.28515625" customWidth="1"/>
+    <col min="31" max="31" width="61.7109375" customWidth="1"/>
+    <col min="32" max="32" width="60" customWidth="1"/>
+    <col min="33" max="33" width="38.140625" customWidth="1"/>
+    <col min="34" max="34" width="69" customWidth="1"/>
+    <col min="35" max="35" width="72.42578125" customWidth="1"/>
+    <col min="36" max="36" width="111.5703125" customWidth="1"/>
+    <col min="37" max="37" width="72.5703125" customWidth="1"/>
+    <col min="38" max="38" width="86.85546875" customWidth="1"/>
+    <col min="39" max="40" width="64.7109375" customWidth="1"/>
+    <col min="41" max="41" width="54.5703125" customWidth="1"/>
+    <col min="42" max="42" width="75.42578125" customWidth="1"/>
+    <col min="43" max="43" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
@@ -2072,66 +2083,66 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>511</v>
+        <v>385</v>
       </c>
       <c r="D2" t="s">
         <v>511</v>
       </c>
       <c r="E2" t="s">
-        <v>413</v>
+        <v>511</v>
       </c>
       <c r="F2" t="s">
         <v>413</v>
       </c>
       <c r="G2" t="s">
+        <v>413</v>
+      </c>
+      <c r="H2" t="s">
         <v>451</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>438</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>413</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>233</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>391</v>
-      </c>
-      <c r="L2" t="s">
-        <v>385</v>
       </c>
       <c r="M2" t="s">
         <v>385</v>
       </c>
       <c r="N2" t="s">
+        <v>385</v>
+      </c>
+      <c r="O2" t="s">
         <v>377</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>357</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>325</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>315</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>308</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>305</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>301</v>
-      </c>
-      <c r="U2" t="s">
-        <v>309</v>
       </c>
       <c r="V2" t="s">
         <v>309</v>
@@ -2140,159 +2151,165 @@
         <v>309</v>
       </c>
       <c r="X2" t="s">
+        <v>309</v>
+      </c>
+      <c r="Y2" t="s">
         <v>272</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>268</v>
       </c>
       <c r="Z2" t="s">
         <v>268</v>
       </c>
       <c r="AA2" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="AB2" t="s">
         <v>251</v>
       </c>
       <c r="AC2" t="s">
+        <v>251</v>
+      </c>
+      <c r="AD2" t="s">
         <v>233</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>227</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>186</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>185</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>154</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>110</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>97</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>83</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>276</v>
       </c>
       <c r="C3" s="12">
-        <v>44484</v>
+        <v>44343</v>
       </c>
       <c r="D3" s="12">
         <v>44484</v>
       </c>
       <c r="E3" s="12">
+        <v>44484</v>
+      </c>
+      <c r="F3" s="12">
         <v>44473</v>
       </c>
-      <c r="F3" s="12">
+      <c r="G3" s="12">
         <v>44469</v>
       </c>
-      <c r="G3" s="12">
+      <c r="H3" s="12">
         <v>44453</v>
       </c>
-      <c r="H3" s="12">
+      <c r="I3" s="12">
         <v>44426</v>
       </c>
-      <c r="I3" s="12">
+      <c r="J3" s="12">
         <v>44330</v>
       </c>
-      <c r="J3" s="12">
+      <c r="K3" s="12">
         <v>44307</v>
       </c>
-      <c r="K3" s="12">
+      <c r="L3" s="12">
         <v>44294</v>
       </c>
-      <c r="L3" s="12">
+      <c r="M3" s="12">
         <v>44343</v>
       </c>
-      <c r="M3" s="12">
+      <c r="N3" s="12">
         <v>44292</v>
       </c>
-      <c r="N3" s="12">
+      <c r="O3" s="12">
         <v>29681</v>
       </c>
-      <c r="O3" s="12">
+      <c r="P3" s="12">
         <v>44286</v>
       </c>
-      <c r="P3" s="12">
+      <c r="Q3" s="12">
         <v>44260</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="R3" s="12">
         <v>44244</v>
       </c>
-      <c r="R3" s="12">
+      <c r="S3" s="12">
         <v>44245</v>
       </c>
-      <c r="S3" s="12">
+      <c r="T3" s="12">
         <v>44223</v>
       </c>
-      <c r="T3" s="12">
+      <c r="U3" s="12">
         <v>44209</v>
       </c>
-      <c r="U3" s="12">
+      <c r="V3" s="12">
         <v>44253</v>
       </c>
-      <c r="V3" s="12">
+      <c r="W3" s="12">
         <v>44237</v>
       </c>
-      <c r="Y3" s="12">
+      <c r="Z3" s="12">
         <v>44181</v>
       </c>
-      <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
       <c r="AQ3" s="1"/>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR3" s="1"/>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>481</v>
       </c>
       <c r="C4" t="s">
-        <v>512</v>
+        <v>527</v>
       </c>
       <c r="D4" t="s">
         <v>512</v>
       </c>
       <c r="E4" t="s">
-        <v>475</v>
+        <v>512</v>
       </c>
       <c r="F4" t="s">
         <v>475</v>
       </c>
       <c r="G4" t="s">
-        <v>318</v>
+        <v>475</v>
       </c>
       <c r="H4" t="s">
         <v>318</v>
@@ -2301,13 +2318,13 @@
         <v>318</v>
       </c>
       <c r="J4" t="s">
+        <v>318</v>
+      </c>
+      <c r="K4" t="s">
         <v>404</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>392</v>
-      </c>
-      <c r="L4" t="s">
-        <v>318</v>
       </c>
       <c r="M4" t="s">
         <v>318</v>
@@ -2316,415 +2333,424 @@
         <v>318</v>
       </c>
       <c r="O4" t="s">
+        <v>318</v>
+      </c>
+      <c r="P4" t="s">
         <v>358</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>318</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>314</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>318</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>318</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>322</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>314</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>275</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>274</v>
       </c>
-      <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
       <c r="AQ4" s="1"/>
-    </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AR4" s="1"/>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
+        <v>526</v>
+      </c>
+      <c r="D5" t="s">
         <v>521</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>515</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>486</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>476</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>452</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>439</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>414</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>405</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>393</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>417</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>387</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>378</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>359</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>326</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>316</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>320</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>306</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>300</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>323</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>312</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>310</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>273</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>277</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>270</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>252</v>
       </c>
       <c r="AB5" t="s">
         <v>252</v>
       </c>
       <c r="AC5" t="s">
+        <v>252</v>
+      </c>
+      <c r="AD5" t="s">
         <v>235</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>226</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>217</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>184</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>156</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>112</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>98</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>85</v>
       </c>
-      <c r="AK5" t="s">
-        <v>1</v>
-      </c>
       <c r="AL5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM5" t="s">
         <v>74</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AN5" t="s">
         <v>72</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>4</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AP5" t="s">
         <v>25</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AQ5" t="s">
         <v>60</v>
       </c>
-      <c r="AQ5" t="s">
+      <c r="AR5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C6" t="s">
+        <v>528</v>
+      </c>
+      <c r="D6" t="s">
         <v>522</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>513</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>487</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>477</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>453</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>440</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>415</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>406</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>394</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>418</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>386</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>379</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>360</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>347</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>317</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>319</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>307</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>302</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>324</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>313</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>311</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>271</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>278</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>269</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>264</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>253</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>234</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>224</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>216</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>183</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>155</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>111</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>107</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>84</v>
       </c>
-      <c r="AK6" t="s">
-        <v>0</v>
-      </c>
       <c r="AL6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM6" t="s">
         <v>73</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>71</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>3</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AP6" t="s">
         <v>24</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AQ6" t="s">
         <v>59</v>
       </c>
-      <c r="AQ6" t="s">
+      <c r="AR6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>523</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>514</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>478</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>441</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>416</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>419</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>380</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>327</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>303</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>254</v>
       </c>
       <c r="AB7" t="s">
         <v>254</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AC7" t="s">
+        <v>254</v>
+      </c>
+      <c r="AE7" t="s">
         <v>225</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>157</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>108</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AK7" t="s">
         <v>87</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AN7" t="s">
         <v>99</v>
       </c>
-      <c r="AP7" t="s">
+      <c r="AQ7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>470</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>407</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>328</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>256</v>
       </c>
       <c r="AB8" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="AC8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>420</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>517</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>524</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>485</v>
       </c>
@@ -2741,8 +2767,8 @@
   <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H69" sqref="H69"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4142,7 +4168,7 @@
         <v>0</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" t="s">
         <v>459</v>
@@ -6215,7 +6241,7 @@
         <v>0</v>
       </c>
       <c r="H127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I127" t="s">
         <v>489</v>

</xml_diff>

<commit_message>
dataframe operations moved to module
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -16,6 +16,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$L$151</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -2767,8 +2768,8 @@
   <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H142" sqref="H142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2965,10 +2966,10 @@
         <v>27</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" t="s">
         <v>150</v>
@@ -4168,7 +4169,7 @@
         <v>0</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" t="s">
         <v>459</v>

</xml_diff>

<commit_message>
san_parse common_operations replaced by utilities module
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -2033,7 +2033,7 @@
   <dimension ref="A1:AR15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2764,12 +2764,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" filterMode="1"/>
   <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H142" sqref="H142"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F43" sqref="F43:G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2966,10 +2966,10 @@
         <v>27</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" t="s">
         <v>150</v>
@@ -4115,7 +4115,7 @@
         <v>0</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" t="s">
         <v>459</v>
@@ -4142,7 +4142,7 @@
         <v>0</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43" t="s">
         <v>459</v>
@@ -4169,7 +4169,7 @@
         <v>0</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" t="s">
         <v>459</v>
@@ -4196,7 +4196,7 @@
         <v>0</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" t="s">
         <v>459</v>
@@ -4208,7 +4208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>15</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D47" s="6" t="s">
         <v>95</v>
       </c>
@@ -4260,7 +4260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="D48" s="6" t="s">
         <v>95</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D49" s="6" t="s">
         <v>95</v>
       </c>
@@ -4306,7 +4306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>161</v>
       </c>
@@ -4332,7 +4332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D51" s="5" t="s">
         <v>96</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>16</v>
       </c>
@@ -4384,7 +4384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D53" s="6" t="s">
         <v>95</v>
       </c>
@@ -4411,7 +4411,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D54" s="6" t="s">
         <v>95</v>
       </c>
@@ -4434,7 +4434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D55" s="5" t="s">
         <v>96</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D56" s="5" t="s">
         <v>96</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D57" s="5" t="s">
         <v>96</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D58" s="5" t="s">
         <v>96</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D59" s="5" t="s">
         <v>96</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D60" s="5" t="s">
         <v>96</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D61" s="5" t="s">
         <v>96</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>18</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D63" s="6" t="s">
         <v>95</v>
       </c>
@@ -4653,7 +4653,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D64" s="5" t="s">
         <v>96</v>
       </c>
@@ -4676,7 +4676,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D65" s="5" t="s">
         <v>96</v>
       </c>
@@ -4699,7 +4699,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D66" s="5" t="s">
         <v>96</v>
       </c>
@@ -4725,7 +4725,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>20</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D68" s="6" t="s">
         <v>95</v>
       </c>
@@ -4780,7 +4780,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D69" s="6" t="s">
         <v>95</v>
       </c>
@@ -4806,7 +4806,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D70" s="6" t="s">
         <v>95</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D71" s="6" t="s">
         <v>95</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D72" s="11" t="s">
         <v>241</v>
       </c>
@@ -4875,7 +4875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>133</v>
       </c>
@@ -4901,7 +4901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>119</v>
       </c>
@@ -4930,7 +4930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D75" s="6" t="s">
         <v>95</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>134</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>135</v>
       </c>
@@ -5005,7 +5005,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D78" s="5" t="s">
         <v>96</v>
       </c>
@@ -5028,7 +5028,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D79" s="5" t="s">
         <v>96</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D80" s="5" t="s">
         <v>96</v>
       </c>
@@ -5074,7 +5074,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D81" s="5" t="s">
         <v>96</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D82" s="5" t="s">
         <v>96</v>
       </c>
@@ -5120,7 +5120,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D83" s="5" t="s">
         <v>96</v>
       </c>
@@ -5146,7 +5146,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D84" s="5" t="s">
         <v>96</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>165</v>
       </c>
@@ -5198,7 +5198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D86" s="5" t="s">
         <v>96</v>
       </c>
@@ -5221,7 +5221,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D87" s="5" t="s">
         <v>96</v>
       </c>
@@ -5244,7 +5244,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D88" s="5" t="s">
         <v>96</v>
       </c>
@@ -5267,7 +5267,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D89" s="6" t="s">
         <v>95</v>
       </c>
@@ -5293,7 +5293,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D90" s="6" t="s">
         <v>95</v>
       </c>
@@ -5319,7 +5319,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D91" s="6" t="s">
         <v>95</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D92" s="6" t="s">
         <v>95</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D93" s="6" t="s">
         <v>95</v>
       </c>
@@ -5397,7 +5397,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D94" s="6" t="s">
         <v>95</v>
       </c>
@@ -5423,7 +5423,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D95" s="6" t="s">
         <v>95</v>
       </c>
@@ -5449,7 +5449,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D96" s="6" t="s">
         <v>95</v>
       </c>
@@ -5475,7 +5475,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D97" s="6" t="s">
         <v>95</v>
       </c>
@@ -5501,7 +5501,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>467</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D99" s="6" t="s">
         <v>95</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D100" s="6" t="s">
         <v>95</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D101" s="6" t="s">
         <v>95</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D102" s="5" t="s">
         <v>96</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D103" s="5" t="s">
         <v>96</v>
       </c>
@@ -5648,7 +5648,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D104" s="5" t="s">
         <v>96</v>
       </c>
@@ -5674,7 +5674,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D105" s="5" t="s">
         <v>96</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="106" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>176</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>248</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>250</v>
       </c>
@@ -5781,7 +5781,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="109" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>249</v>
       </c>
@@ -5810,7 +5810,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D110" s="6" t="s">
         <v>95</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>247</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D112" s="5" t="s">
         <v>96</v>
       </c>
@@ -5888,7 +5888,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D113" s="5" t="s">
         <v>96</v>
       </c>
@@ -5911,7 +5911,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D114" s="5" t="s">
         <v>96</v>
       </c>
@@ -5934,7 +5934,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D115" s="5" t="s">
         <v>96</v>
       </c>
@@ -5957,7 +5957,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D116" s="5" t="s">
         <v>96</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D117" s="5" t="s">
         <v>96</v>
       </c>
@@ -6006,7 +6006,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D118" s="5" t="s">
         <v>96</v>
       </c>
@@ -6032,7 +6032,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D119" s="5" t="s">
         <v>96</v>
       </c>
@@ -6058,7 +6058,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D120" s="5" t="s">
         <v>96</v>
       </c>
@@ -6084,7 +6084,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D121" s="6" t="s">
         <v>95</v>
       </c>
@@ -6107,7 +6107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D122" s="5" t="s">
         <v>96</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D123" s="5" t="s">
         <v>96</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D124" s="6" t="s">
         <v>95</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D125" s="5" t="s">
         <v>96</v>
       </c>
@@ -6199,7 +6199,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>17</v>
       </c>
@@ -6231,7 +6231,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D127" s="5" t="s">
         <v>96</v>
       </c>
@@ -6257,7 +6257,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>290</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="4:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D129" s="6" t="s">
         <v>95</v>
       </c>
@@ -6309,7 +6309,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="130" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="4:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="D130" s="5" t="s">
         <v>96</v>
       </c>
@@ -6335,57 +6335,75 @@
         <v>390</v>
       </c>
     </row>
-    <row r="142" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="4:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="4:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="133" spans="4:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="4:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="4:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="4:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="4:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="4:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="4:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="4:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="141" spans="4:12" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="4:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E142" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="143" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="4:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E143" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="144" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="4:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="E144" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="E145" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="5:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="E146" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="5:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="E147" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="5:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="E148" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="5:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="E149" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="5:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="E150" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="5:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="E151" t="s">
         <v>500</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L151">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="collection"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
domain_index alias added to portshow_aggregated
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -2798,8 +2798,8 @@
   <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H115" sqref="H115"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H104" sqref="H104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5568,7 +5568,7 @@
         <v>0</v>
       </c>
       <c r="H99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I99" t="s">
         <v>461</v>

</xml_diff>

<commit_message>
uptime limit note added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="550">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1655,6 +1655,21 @@
   </si>
   <si>
     <t>Участники конфигурации зонирования, отсутствующие в сети</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\NOV21\blade_sib</t>
+  </si>
+  <si>
+    <t>MTS_south</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\01.CUSTOMERS\MTS\SAN Assessment\NOV2021\mts_south</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\NOV21\blade_south</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\NOV21\ssave_south</t>
   </si>
 </sst>
 </file>
@@ -2077,57 +2092,60 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AW15"/>
+  <dimension ref="A1:AX15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="4" width="70" customWidth="1"/>
-    <col min="5" max="5" width="151.28515625" customWidth="1"/>
-    <col min="6" max="6" width="120.42578125" customWidth="1"/>
-    <col min="7" max="7" width="70" customWidth="1"/>
-    <col min="8" max="8" width="158.5703125" customWidth="1"/>
-    <col min="9" max="9" width="83.28515625" customWidth="1"/>
-    <col min="10" max="11" width="70" customWidth="1"/>
-    <col min="12" max="12" width="124.42578125" customWidth="1"/>
-    <col min="13" max="13" width="70" customWidth="1"/>
-    <col min="14" max="14" width="48.85546875" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" customWidth="1"/>
-    <col min="16" max="16" width="80.140625" customWidth="1"/>
-    <col min="17" max="17" width="35.7109375" customWidth="1"/>
-    <col min="18" max="19" width="122.7109375" customWidth="1"/>
-    <col min="20" max="20" width="48.42578125" customWidth="1"/>
-    <col min="21" max="21" width="29.7109375" customWidth="1"/>
-    <col min="22" max="22" width="80.140625" customWidth="1"/>
-    <col min="23" max="23" width="68.5703125" customWidth="1"/>
-    <col min="24" max="24" width="48.7109375" customWidth="1"/>
-    <col min="25" max="25" width="62" customWidth="1"/>
-    <col min="26" max="28" width="89.5703125" customWidth="1"/>
-    <col min="29" max="29" width="69.85546875" customWidth="1"/>
-    <col min="30" max="30" width="52.140625" customWidth="1"/>
-    <col min="31" max="31" width="73.140625" customWidth="1"/>
-    <col min="32" max="32" width="29.7109375" customWidth="1"/>
-    <col min="33" max="34" width="76" customWidth="1"/>
-    <col min="35" max="35" width="72.28515625" customWidth="1"/>
-    <col min="36" max="36" width="61.7109375" customWidth="1"/>
-    <col min="37" max="37" width="60" customWidth="1"/>
-    <col min="38" max="38" width="38.140625" customWidth="1"/>
-    <col min="39" max="39" width="69" customWidth="1"/>
-    <col min="40" max="40" width="72.42578125" customWidth="1"/>
-    <col min="41" max="41" width="111.5703125" customWidth="1"/>
-    <col min="42" max="42" width="72.5703125" customWidth="1"/>
-    <col min="43" max="43" width="86.85546875" customWidth="1"/>
-    <col min="44" max="45" width="64.7109375" customWidth="1"/>
-    <col min="46" max="46" width="54.5703125" customWidth="1"/>
-    <col min="47" max="47" width="75.42578125" customWidth="1"/>
-    <col min="48" max="48" width="58.140625" customWidth="1"/>
+    <col min="2" max="2" width="70" customWidth="1"/>
+    <col min="3" max="3" width="128.5703125" customWidth="1"/>
+    <col min="4" max="4" width="99.85546875" customWidth="1"/>
+    <col min="5" max="5" width="126.5703125" customWidth="1"/>
+    <col min="6" max="6" width="151.28515625" customWidth="1"/>
+    <col min="7" max="7" width="120.42578125" customWidth="1"/>
+    <col min="8" max="8" width="70" customWidth="1"/>
+    <col min="9" max="9" width="158.5703125" customWidth="1"/>
+    <col min="10" max="10" width="83.28515625" customWidth="1"/>
+    <col min="11" max="12" width="70" customWidth="1"/>
+    <col min="13" max="13" width="124.42578125" customWidth="1"/>
+    <col min="14" max="14" width="70" customWidth="1"/>
+    <col min="15" max="15" width="48.85546875" customWidth="1"/>
+    <col min="16" max="16" width="29.7109375" customWidth="1"/>
+    <col min="17" max="17" width="80.140625" customWidth="1"/>
+    <col min="18" max="18" width="35.7109375" customWidth="1"/>
+    <col min="19" max="20" width="122.7109375" customWidth="1"/>
+    <col min="21" max="21" width="48.42578125" customWidth="1"/>
+    <col min="22" max="22" width="29.7109375" customWidth="1"/>
+    <col min="23" max="23" width="80.140625" customWidth="1"/>
+    <col min="24" max="24" width="68.5703125" customWidth="1"/>
+    <col min="25" max="25" width="48.7109375" customWidth="1"/>
+    <col min="26" max="26" width="62" customWidth="1"/>
+    <col min="27" max="29" width="89.5703125" customWidth="1"/>
+    <col min="30" max="30" width="69.85546875" customWidth="1"/>
+    <col min="31" max="31" width="52.140625" customWidth="1"/>
+    <col min="32" max="32" width="73.140625" customWidth="1"/>
+    <col min="33" max="33" width="29.7109375" customWidth="1"/>
+    <col min="34" max="35" width="76" customWidth="1"/>
+    <col min="36" max="36" width="72.28515625" customWidth="1"/>
+    <col min="37" max="37" width="61.7109375" customWidth="1"/>
+    <col min="38" max="38" width="60" customWidth="1"/>
+    <col min="39" max="39" width="38.140625" customWidth="1"/>
+    <col min="40" max="40" width="69" customWidth="1"/>
+    <col min="41" max="41" width="72.42578125" customWidth="1"/>
+    <col min="42" max="42" width="111.5703125" customWidth="1"/>
+    <col min="43" max="43" width="72.5703125" customWidth="1"/>
+    <col min="44" max="44" width="86.85546875" customWidth="1"/>
+    <col min="45" max="46" width="64.7109375" customWidth="1"/>
+    <col min="47" max="47" width="54.5703125" customWidth="1"/>
+    <col min="48" max="48" width="75.42578125" customWidth="1"/>
+    <col min="49" max="49" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
@@ -2135,84 +2153,84 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
+        <v>546</v>
+      </c>
+      <c r="D2" t="s">
         <v>541</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>538</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>536</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>529</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>525</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>383</v>
-      </c>
-      <c r="I2" t="s">
-        <v>507</v>
       </c>
       <c r="J2" t="s">
         <v>507</v>
       </c>
       <c r="K2" t="s">
-        <v>411</v>
+        <v>507</v>
       </c>
       <c r="L2" t="s">
         <v>411</v>
       </c>
       <c r="M2" t="s">
+        <v>411</v>
+      </c>
+      <c r="N2" t="s">
         <v>449</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>436</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>411</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>231</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>389</v>
-      </c>
-      <c r="R2" t="s">
-        <v>383</v>
       </c>
       <c r="S2" t="s">
         <v>383</v>
       </c>
       <c r="T2" t="s">
+        <v>383</v>
+      </c>
+      <c r="U2" t="s">
         <v>375</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>355</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>323</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>313</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>306</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>303</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>299</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>307</v>
       </c>
       <c r="AB2" t="s">
         <v>307</v>
@@ -2221,160 +2239,166 @@
         <v>307</v>
       </c>
       <c r="AD2" t="s">
+        <v>307</v>
+      </c>
+      <c r="AE2" t="s">
         <v>270</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>266</v>
       </c>
       <c r="AF2" t="s">
         <v>266</v>
       </c>
       <c r="AG2" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="AH2" t="s">
         <v>249</v>
       </c>
       <c r="AI2" t="s">
+        <v>249</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>231</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>226</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>185</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>184</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>154</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>110</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>97</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>83</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>274</v>
       </c>
       <c r="C3" s="12">
+        <v>44537</v>
+      </c>
+      <c r="D3" s="12">
         <v>44531</v>
       </c>
-      <c r="D3" s="12">
+      <c r="E3" s="12">
         <v>44530</v>
       </c>
-      <c r="E3" s="12">
+      <c r="F3" s="12">
         <v>44529</v>
       </c>
-      <c r="F3" s="12">
+      <c r="G3" s="12">
         <v>44524</v>
       </c>
-      <c r="G3" s="12">
+      <c r="H3" s="12">
         <v>44503</v>
       </c>
-      <c r="H3" s="12">
+      <c r="I3" s="12">
         <v>44343</v>
-      </c>
-      <c r="I3" s="12">
-        <v>44484</v>
       </c>
       <c r="J3" s="12">
         <v>44484</v>
       </c>
       <c r="K3" s="12">
+        <v>44484</v>
+      </c>
+      <c r="L3" s="12">
         <v>44473</v>
       </c>
-      <c r="L3" s="12">
+      <c r="M3" s="12">
         <v>44469</v>
       </c>
-      <c r="M3" s="12">
+      <c r="N3" s="12">
         <v>44453</v>
       </c>
-      <c r="N3" s="12">
+      <c r="O3" s="12">
         <v>44426</v>
       </c>
-      <c r="O3" s="12">
+      <c r="P3" s="12">
         <v>44330</v>
       </c>
-      <c r="P3" s="12">
+      <c r="Q3" s="12">
         <v>44307</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="R3" s="12">
         <v>44294</v>
       </c>
-      <c r="R3" s="12">
+      <c r="S3" s="12">
         <v>44343</v>
       </c>
-      <c r="S3" s="12">
+      <c r="T3" s="12">
         <v>44292</v>
       </c>
-      <c r="T3" s="12">
+      <c r="U3" s="12">
         <v>29681</v>
       </c>
-      <c r="U3" s="12">
+      <c r="V3" s="12">
         <v>44286</v>
       </c>
-      <c r="V3" s="12">
+      <c r="W3" s="12">
         <v>44260</v>
       </c>
-      <c r="W3" s="12">
+      <c r="X3" s="12">
         <v>44244</v>
       </c>
-      <c r="X3" s="12">
+      <c r="Y3" s="12">
         <v>44245</v>
       </c>
-      <c r="Y3" s="12">
+      <c r="Z3" s="12">
         <v>44223</v>
       </c>
-      <c r="Z3" s="12">
+      <c r="AA3" s="12">
         <v>44209</v>
       </c>
-      <c r="AA3" s="12">
+      <c r="AB3" s="12">
         <v>44253</v>
       </c>
-      <c r="AB3" s="12">
+      <c r="AC3" s="12">
         <v>44237</v>
       </c>
-      <c r="AE3" s="12">
+      <c r="AF3" s="12">
         <v>44181</v>
       </c>
-      <c r="AQ3" s="1"/>
       <c r="AR3" s="1"/>
       <c r="AS3" s="1"/>
       <c r="AT3" s="1"/>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
-    </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX3" s="1"/>
+    </row>
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>479</v>
       </c>
@@ -2394,22 +2418,22 @@
         <v>316</v>
       </c>
       <c r="H4" t="s">
+        <v>316</v>
+      </c>
+      <c r="I4" t="s">
         <v>522</v>
-      </c>
-      <c r="I4" t="s">
-        <v>508</v>
       </c>
       <c r="J4" t="s">
         <v>508</v>
       </c>
       <c r="K4" t="s">
-        <v>473</v>
+        <v>508</v>
       </c>
       <c r="L4" t="s">
         <v>473</v>
       </c>
       <c r="M4" t="s">
-        <v>316</v>
+        <v>473</v>
       </c>
       <c r="N4" t="s">
         <v>316</v>
@@ -2418,13 +2442,13 @@
         <v>316</v>
       </c>
       <c r="P4" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q4" t="s">
         <v>402</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>390</v>
-      </c>
-      <c r="R4" t="s">
-        <v>316</v>
       </c>
       <c r="S4" t="s">
         <v>316</v>
@@ -2433,457 +2457,472 @@
         <v>316</v>
       </c>
       <c r="U4" t="s">
+        <v>316</v>
+      </c>
+      <c r="V4" t="s">
         <v>356</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>316</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>312</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>316</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>316</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>320</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>312</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>273</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>272</v>
       </c>
-      <c r="AQ4" s="1"/>
       <c r="AR4" s="1"/>
       <c r="AS4" s="1"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
-    </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX4" s="1"/>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
+        <v>547</v>
+      </c>
+      <c r="D5" t="s">
         <v>542</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>539</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>535</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>530</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>526</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>521</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>516</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>511</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>484</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>474</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>450</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>437</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>412</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>403</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>391</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>415</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>385</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>376</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>357</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>324</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>314</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>318</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>304</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>298</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>321</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>310</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>308</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>271</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>275</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>268</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>250</v>
       </c>
       <c r="AH5" t="s">
         <v>250</v>
       </c>
       <c r="AI5" t="s">
+        <v>250</v>
+      </c>
+      <c r="AJ5" t="s">
         <v>233</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>225</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AL5" t="s">
         <v>216</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AM5" t="s">
         <v>183</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AN5" t="s">
         <v>156</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>112</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AP5" t="s">
         <v>98</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AQ5" t="s">
         <v>85</v>
       </c>
-      <c r="AQ5" t="s">
-        <v>1</v>
-      </c>
       <c r="AR5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS5" t="s">
         <v>74</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AT5" t="s">
         <v>72</v>
       </c>
-      <c r="AT5" t="s">
+      <c r="AU5" t="s">
         <v>4</v>
       </c>
-      <c r="AU5" t="s">
+      <c r="AV5" t="s">
         <v>25</v>
       </c>
-      <c r="AV5" t="s">
+      <c r="AW5" t="s">
         <v>60</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AX5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C6" t="s">
+        <v>549</v>
+      </c>
+      <c r="D6" t="s">
         <v>543</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>540</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>537</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>531</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>528</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>523</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>517</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>509</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>485</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>475</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>451</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>438</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>413</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>404</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>392</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>416</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>384</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>377</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>358</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>345</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>315</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>317</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>305</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>300</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>322</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>311</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>309</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>269</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>276</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>267</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>262</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>251</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>232</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>223</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" t="s">
         <v>215</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AM6" t="s">
         <v>182</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>155</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>111</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AP6" t="s">
         <v>107</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AQ6" t="s">
         <v>84</v>
       </c>
-      <c r="AQ6" t="s">
-        <v>0</v>
-      </c>
       <c r="AR6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS6" t="s">
         <v>73</v>
       </c>
-      <c r="AS6" t="s">
+      <c r="AT6" t="s">
         <v>71</v>
       </c>
-      <c r="AT6" t="s">
+      <c r="AU6" t="s">
         <v>3</v>
       </c>
-      <c r="AU6" t="s">
+      <c r="AV6" t="s">
         <v>24</v>
       </c>
-      <c r="AV6" t="s">
+      <c r="AW6" t="s">
         <v>59</v>
       </c>
-      <c r="AW6" t="s">
+      <c r="AX6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="F7" t="s">
-        <v>527</v>
+      <c r="C7" t="s">
+        <v>548</v>
+      </c>
+      <c r="D7" t="s">
+        <v>545</v>
       </c>
       <c r="G7" t="s">
         <v>527</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7" t="s">
+        <v>527</v>
+      </c>
+      <c r="J7" t="s">
         <v>518</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>510</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>476</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>439</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>414</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>417</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>378</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>325</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>301</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>252</v>
       </c>
       <c r="AH7" t="s">
         <v>252</v>
       </c>
-      <c r="AJ7" t="s">
+      <c r="AI7" t="s">
+        <v>252</v>
+      </c>
+      <c r="AK7" t="s">
         <v>224</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AN7" t="s">
         <v>157</v>
       </c>
-      <c r="AO7" t="s">
+      <c r="AP7" t="s">
         <v>108</v>
       </c>
-      <c r="AP7" t="s">
+      <c r="AQ7" t="s">
         <v>87</v>
       </c>
-      <c r="AS7" t="s">
+      <c r="AT7" t="s">
         <v>99</v>
       </c>
-      <c r="AV7" t="s">
+      <c r="AW7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>468</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>405</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>326</v>
-      </c>
-      <c r="AG8" t="s">
-        <v>254</v>
       </c>
       <c r="AH8" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AI8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>418</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>513</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>519</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>512</v>
       </c>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>483</v>
       </c>
@@ -2900,8 +2939,8 @@
   <dimension ref="A1:L134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J110" sqref="J110"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3010,7 +3049,7 @@
         <v>96</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -4698,10 +4737,10 @@
         <v>62</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60" t="s">
         <v>168</v>

</xml_diff>

<commit_message>
Code refactoring. Pattern dictionary import fn replaced
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12270" windowHeight="975" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="551">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1264,18 +1264,6 @@
     <t>C:\Users\vlasenko\Documents\06.CONFIGS\Sibintek\MAY21\blade</t>
   </si>
   <si>
-    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\MegafonMSK\SAN Assessment\MAY21</t>
-  </si>
-  <si>
-    <t>C:\Users\vlasenko\Documents\06.CONFIGS\MegafonMSK\APR21\ssave\supportsave-20-05-2021</t>
-  </si>
-  <si>
-    <t>C:\Users\vlasenko\Documents\06.CONFIGS\MegafonMSK\APR21\showall-all-encl</t>
-  </si>
-  <si>
-    <t>C:\Users\vlasenko\Documents\06.CONFIGS\MegafonMSK\APR21\3PAR</t>
-  </si>
-  <si>
     <t>NPIV_statistics</t>
   </si>
   <si>
@@ -1639,9 +1627,6 @@
     <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\01.CUSTOMERS\MTS\SAN Assessment\NOV2021\mts_spb</t>
   </si>
   <si>
-    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\NOV21\ssave_spb</t>
-  </si>
-  <si>
     <t>MTS_sib</t>
   </si>
   <si>
@@ -1670,6 +1655,24 @@
   </si>
   <si>
     <t>Отсутствуют_в_сети</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\01.CUSTOMERS\Megafon\MegafonMSK\SAN Assessment\MAY21</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MegafonMSK\APR21\ssave\supportsave-20-05-2021</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MegafonMSK\APR21\showall-all-encl</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MegafonMSK\APR21\3PAR</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\NOV21\ssave_spb\29_11_2021</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\NOV21\blade_spb</t>
   </si>
 </sst>
 </file>
@@ -2095,7 +2098,7 @@
   <dimension ref="A1:AX15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,12 +2110,12 @@
     <col min="5" max="5" width="126.5703125" customWidth="1"/>
     <col min="6" max="6" width="151.28515625" customWidth="1"/>
     <col min="7" max="7" width="120.42578125" customWidth="1"/>
-    <col min="8" max="8" width="70" customWidth="1"/>
+    <col min="8" max="8" width="112.42578125" customWidth="1"/>
     <col min="9" max="9" width="158.5703125" customWidth="1"/>
     <col min="10" max="10" width="83.28515625" customWidth="1"/>
     <col min="11" max="12" width="70" customWidth="1"/>
     <col min="13" max="13" width="124.42578125" customWidth="1"/>
-    <col min="14" max="14" width="70" customWidth="1"/>
+    <col min="14" max="14" width="103.85546875" customWidth="1"/>
     <col min="15" max="15" width="48.85546875" customWidth="1"/>
     <col min="16" max="16" width="29.7109375" customWidth="1"/>
     <col min="17" max="17" width="80.140625" customWidth="1"/>
@@ -2149,7 +2152,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2158,31 +2161,31 @@
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="D2" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="E2" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="F2" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="G2" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="H2" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="I2" t="s">
         <v>382</v>
       </c>
       <c r="J2" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="K2" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="L2" t="s">
         <v>410</v>
@@ -2191,10 +2194,10 @@
         <v>410</v>
       </c>
       <c r="N2" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="O2" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="P2" t="s">
         <v>410</v>
@@ -2400,7 +2403,7 @@
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C4" t="s">
         <v>315</v>
@@ -2421,19 +2424,19 @@
         <v>315</v>
       </c>
       <c r="I4" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="J4" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="K4" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="L4" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="M4" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="N4" t="s">
         <v>315</v>
@@ -2499,43 +2502,43 @@
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="D5" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="E5" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="F5" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="G5" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="H5" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="I5" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="J5" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="K5" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="L5" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="M5" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="N5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="O5" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="P5" t="s">
         <v>411</v>
@@ -2547,7 +2550,7 @@
         <v>390</v>
       </c>
       <c r="S5" t="s">
-        <v>414</v>
+        <v>545</v>
       </c>
       <c r="T5" t="s">
         <v>384</v>
@@ -2648,43 +2651,43 @@
         <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="D6" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="E6" t="s">
-        <v>539</v>
+        <v>549</v>
       </c>
       <c r="F6" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="G6" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="H6" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="I6" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="J6" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="K6" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="L6" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="M6" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="N6" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="O6" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="P6" t="s">
         <v>412</v>
@@ -2696,7 +2699,7 @@
         <v>391</v>
       </c>
       <c r="S6" t="s">
-        <v>415</v>
+        <v>546</v>
       </c>
       <c r="T6" t="s">
         <v>383</v>
@@ -2797,34 +2800,37 @@
         <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="D7" t="s">
-        <v>544</v>
+        <v>539</v>
+      </c>
+      <c r="E7" t="s">
+        <v>550</v>
       </c>
       <c r="G7" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="H7" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="J7" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="K7" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="M7" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="O7" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="P7" t="s">
         <v>413</v>
       </c>
       <c r="S7" t="s">
-        <v>416</v>
+        <v>547</v>
       </c>
       <c r="U7" t="s">
         <v>377</v>
@@ -2865,7 +2871,7 @@
         <v>252</v>
       </c>
       <c r="N8" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="Q8" t="s">
         <v>404</v>
@@ -2885,7 +2891,7 @@
         <v>346</v>
       </c>
       <c r="S9" t="s">
-        <v>417</v>
+        <v>548</v>
       </c>
       <c r="U9" t="s">
         <v>378</v>
@@ -2893,13 +2899,13 @@
     </row>
     <row r="10" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="J10" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="K10" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="11" spans="1:50" x14ac:dyDescent="0.25">
@@ -2909,22 +2915,22 @@
     </row>
     <row r="12" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="13" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="15" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -2939,8 +2945,8 @@
   <dimension ref="A1:L134"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H115" sqref="H115"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2989,7 +2995,7 @@
         <v>189</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="L1" t="s">
         <v>387</v>
@@ -3049,7 +3055,7 @@
         <v>96</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -3069,7 +3075,7 @@
         <v>94</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -3585,7 +3591,7 @@
         <v>94</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -3597,7 +3603,7 @@
         <v>143</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="K20" s="10">
         <v>1</v>
@@ -3617,7 +3623,7 @@
         <v>94</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -3629,7 +3635,7 @@
         <v>143</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="K21" s="10">
         <v>1</v>
@@ -3754,10 +3760,10 @@
         <v>94</v>
       </c>
       <c r="E25" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -3769,7 +3775,7 @@
         <v>144</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="K25" s="10">
         <v>1</v>
@@ -3836,7 +3842,7 @@
         <v>142</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="K27" s="10">
         <v>1</v>
@@ -3868,7 +3874,7 @@
         <v>142</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="K28" s="10">
         <v>1</v>
@@ -3900,7 +3906,7 @@
         <v>142</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="K29" s="10">
         <v>1</v>
@@ -3929,7 +3935,7 @@
         <v>142</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="K30" s="10">
         <v>1</v>
@@ -4251,7 +4257,7 @@
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="J41" s="10" t="s">
         <v>381</v>
@@ -4280,7 +4286,7 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="J42" s="10" t="s">
         <v>380</v>
@@ -4309,7 +4315,7 @@
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="J43" s="10" t="s">
         <v>379</v>
@@ -4336,7 +4342,7 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J44" s="10" t="s">
         <v>257</v>
@@ -4363,7 +4369,7 @@
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="J45" s="10" t="s">
         <v>258</v>
@@ -4390,7 +4396,7 @@
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J46" s="10" t="s">
         <v>353</v>
@@ -4417,7 +4423,7 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J47" s="10" t="s">
         <v>350</v>
@@ -4444,7 +4450,7 @@
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J48" s="10" t="s">
         <v>351</v>
@@ -4471,7 +4477,7 @@
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="J49" s="10" t="s">
         <v>385</v>
@@ -4514,7 +4520,7 @@
         <v>95</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -4662,7 +4668,7 @@
       </c>
       <c r="E57" s="16"/>
       <c r="F57" s="2" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -4674,7 +4680,7 @@
         <v>168</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="K57" s="10">
         <v>1</v>
@@ -4826,7 +4832,7 @@
         <v>96</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -4838,7 +4844,7 @@
         <v>168</v>
       </c>
       <c r="J64" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="K64">
         <v>23</v>
@@ -4849,7 +4855,7 @@
         <v>96</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -4861,7 +4867,7 @@
         <v>168</v>
       </c>
       <c r="J65" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="K65">
         <v>11</v>
@@ -5544,7 +5550,7 @@
         <v>95</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -5556,13 +5562,13 @@
         <v>171</v>
       </c>
       <c r="J93" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="K93">
         <v>1</v>
       </c>
       <c r="L93" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.25">
@@ -5570,7 +5576,7 @@
         <v>95</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -5582,13 +5588,13 @@
         <v>171</v>
       </c>
       <c r="J94" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="K94">
         <v>1</v>
       </c>
       <c r="L94" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.25">
@@ -5596,7 +5602,7 @@
         <v>95</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -5608,13 +5614,13 @@
         <v>171</v>
       </c>
       <c r="J95" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="K95">
         <v>1</v>
       </c>
       <c r="L95" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.25">
@@ -5622,7 +5628,7 @@
         <v>95</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -5634,13 +5640,13 @@
         <v>171</v>
       </c>
       <c r="J96" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="K96">
         <v>1</v>
       </c>
       <c r="L96" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.25">
@@ -5648,7 +5654,7 @@
         <v>95</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -5660,13 +5666,13 @@
         <v>171</v>
       </c>
       <c r="J97" t="s">
+        <v>488</v>
+      </c>
+      <c r="K97">
+        <v>1</v>
+      </c>
+      <c r="L97" t="s">
         <v>492</v>
-      </c>
-      <c r="K97">
-        <v>1</v>
-      </c>
-      <c r="L97" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="98" spans="2:12" x14ac:dyDescent="0.25">
@@ -5674,7 +5680,7 @@
         <v>95</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -5686,13 +5692,13 @@
         <v>171</v>
       </c>
       <c r="J98" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="K98">
         <v>1</v>
       </c>
       <c r="L98" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="99" spans="2:12" x14ac:dyDescent="0.25">
@@ -5700,7 +5706,7 @@
         <v>95</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -5712,13 +5718,13 @@
         <v>171</v>
       </c>
       <c r="J99" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="K99">
         <v>1</v>
       </c>
       <c r="L99" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="100" spans="2:12" x14ac:dyDescent="0.25">
@@ -5726,7 +5732,7 @@
         <v>95</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -5738,13 +5744,13 @@
         <v>171</v>
       </c>
       <c r="J100" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="K100">
         <v>1</v>
       </c>
       <c r="L100" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="101" spans="2:12" x14ac:dyDescent="0.25">
@@ -5752,7 +5758,7 @@
         <v>95</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -5764,24 +5770,24 @@
         <v>171</v>
       </c>
       <c r="J101" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="K101">
         <v>1</v>
       </c>
       <c r="L101" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="102" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="G102">
         <v>0</v>
@@ -5790,10 +5796,10 @@
         <v>0</v>
       </c>
       <c r="I102" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="J102" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="K102" s="10">
         <v>1</v>
@@ -5804,7 +5810,7 @@
         <v>95</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G103">
         <v>0</v>
@@ -5813,10 +5819,10 @@
         <v>0</v>
       </c>
       <c r="I103" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="J103" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="K103" s="10">
         <v>1</v>
@@ -5827,19 +5833,19 @@
         <v>95</v>
       </c>
       <c r="F104" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
+      <c r="I104" t="s">
+        <v>455</v>
+      </c>
+      <c r="J104" t="s">
         <v>418</v>
-      </c>
-      <c r="G104">
-        <v>0</v>
-      </c>
-      <c r="H104">
-        <v>0</v>
-      </c>
-      <c r="I104" t="s">
-        <v>459</v>
-      </c>
-      <c r="J104" t="s">
-        <v>422</v>
       </c>
       <c r="K104" s="10">
         <v>1</v>
@@ -5853,7 +5859,7 @@
         <v>95</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="G105">
         <v>0</v>
@@ -5862,10 +5868,10 @@
         <v>0</v>
       </c>
       <c r="I105" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="J105" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="K105" s="10">
         <v>1</v>
@@ -5879,7 +5885,7 @@
         <v>96</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G106">
         <v>0</v>
@@ -5888,10 +5894,10 @@
         <v>0</v>
       </c>
       <c r="I106" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="J106" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="K106">
         <v>44</v>
@@ -5902,7 +5908,7 @@
         <v>96</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -5911,7 +5917,7 @@
         <v>0</v>
       </c>
       <c r="I107" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="J107" t="s">
         <v>196</v>
@@ -5925,7 +5931,7 @@
         <v>96</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G108">
         <v>0</v>
@@ -5934,10 +5940,10 @@
         <v>0</v>
       </c>
       <c r="I108" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="J108" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="K108">
         <v>33</v>
@@ -5951,7 +5957,7 @@
         <v>96</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -5960,10 +5966,10 @@
         <v>0</v>
       </c>
       <c r="I109" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="J109" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="K109">
         <v>31</v>
@@ -5986,10 +5992,10 @@
         <v>0</v>
       </c>
       <c r="H110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I110" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J110" s="10" t="s">
         <v>330</v>
@@ -6015,7 +6021,7 @@
         <v>0</v>
       </c>
       <c r="I111" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J111" s="10" t="s">
         <v>331</v>
@@ -6041,7 +6047,7 @@
         <v>0</v>
       </c>
       <c r="I112" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J112" s="10" t="s">
         <v>332</v>
@@ -6070,7 +6076,7 @@
         <v>0</v>
       </c>
       <c r="I113" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J113" s="10" t="s">
         <v>333</v>
@@ -6096,7 +6102,7 @@
         <v>0</v>
       </c>
       <c r="I114" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J114" s="10" t="s">
         <v>329</v>
@@ -6125,7 +6131,7 @@
         <v>0</v>
       </c>
       <c r="I115" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J115" s="10" t="s">
         <v>241</v>
@@ -6151,7 +6157,7 @@
         <v>0</v>
       </c>
       <c r="I116" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J116" t="s">
         <v>208</v>
@@ -6174,7 +6180,7 @@
         <v>0</v>
       </c>
       <c r="I117" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J117" t="s">
         <v>209</v>
@@ -6188,7 +6194,7 @@
         <v>96</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="G118">
         <v>0</v>
@@ -6197,7 +6203,7 @@
         <v>0</v>
       </c>
       <c r="I118" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J118" t="s">
         <v>214</v>
@@ -6220,7 +6226,7 @@
         <v>0</v>
       </c>
       <c r="I119" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J119" t="s">
         <v>210</v>
@@ -6243,7 +6249,7 @@
         <v>0</v>
       </c>
       <c r="I120" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J120" t="s">
         <v>228</v>
@@ -6257,7 +6263,7 @@
         <v>96</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="G121">
         <v>0</v>
@@ -6266,10 +6272,10 @@
         <v>0</v>
       </c>
       <c r="I121" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J121" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="K121">
         <v>69</v>
@@ -6292,7 +6298,7 @@
         <v>0</v>
       </c>
       <c r="I122" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J122" t="s">
         <v>335</v>
@@ -6318,7 +6324,7 @@
         <v>0</v>
       </c>
       <c r="I123" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J123" t="s">
         <v>336</v>
@@ -6344,7 +6350,7 @@
         <v>0</v>
       </c>
       <c r="I124" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="J124" t="s">
         <v>243</v>
@@ -6370,7 +6376,7 @@
         <v>0</v>
       </c>
       <c r="I125" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="J125" t="s">
         <v>371</v>
@@ -6393,7 +6399,7 @@
         <v>0</v>
       </c>
       <c r="I126" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="J126" t="s">
         <v>372</v>
@@ -6407,7 +6413,7 @@
         <v>96</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="G127">
         <v>0</v>
@@ -6416,7 +6422,7 @@
         <v>0</v>
       </c>
       <c r="I127" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="J127" t="s">
         <v>373</v>
@@ -6439,7 +6445,7 @@
         <v>0</v>
       </c>
       <c r="I128" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="J128" t="s">
         <v>294</v>
@@ -6462,7 +6468,7 @@
         <v>0</v>
       </c>
       <c r="I129" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="J129" t="s">
         <v>222</v>
@@ -6482,7 +6488,7 @@
         <v>95</v>
       </c>
       <c r="F130" s="9" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="G130">
         <v>0</v>
@@ -6491,10 +6497,10 @@
         <v>0</v>
       </c>
       <c r="I130" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="J130" s="10" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="K130" s="10">
         <v>1</v>
@@ -6508,7 +6514,7 @@
         <v>96</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="G131">
         <v>0</v>
@@ -6517,7 +6523,7 @@
         <v>0</v>
       </c>
       <c r="I131" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="J131" t="s">
         <v>345</v>
@@ -6546,7 +6552,7 @@
         <v>0</v>
       </c>
       <c r="I132" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="J132" t="s">
         <v>291</v>
@@ -6569,7 +6575,7 @@
         <v>0</v>
       </c>
       <c r="I133" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="J133" t="s">
         <v>292</v>
@@ -6595,7 +6601,7 @@
         <v>0</v>
       </c>
       <c r="I134" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="J134" t="s">
         <v>290</v>
@@ -6746,10 +6752,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>79</v>
@@ -6757,24 +6763,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B2" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C2" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="B3" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C3" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
device type identification correction
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13665" windowHeight="11520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="553">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1673,6 +1673,12 @@
   </si>
   <si>
     <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\NOV21\blade_spb</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\01.CUSTOMERS\MTS\SAN Assessment\JAN2022\mts_msc</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\JAN22\mts_msc\ssave</t>
   </si>
 </sst>
 </file>
@@ -2095,148 +2101,148 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AX15"/>
+  <dimension ref="A1:AY15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="70" customWidth="1"/>
-    <col min="3" max="3" width="128.5703125" customWidth="1"/>
-    <col min="4" max="4" width="99.85546875" customWidth="1"/>
-    <col min="5" max="5" width="126.5703125" customWidth="1"/>
-    <col min="6" max="6" width="151.28515625" customWidth="1"/>
-    <col min="7" max="7" width="120.42578125" customWidth="1"/>
-    <col min="8" max="8" width="112.42578125" customWidth="1"/>
-    <col min="9" max="9" width="158.5703125" customWidth="1"/>
-    <col min="10" max="10" width="83.28515625" customWidth="1"/>
-    <col min="11" max="12" width="70" customWidth="1"/>
-    <col min="13" max="13" width="124.42578125" customWidth="1"/>
-    <col min="14" max="14" width="103.85546875" customWidth="1"/>
-    <col min="15" max="15" width="48.85546875" customWidth="1"/>
-    <col min="16" max="16" width="29.7109375" customWidth="1"/>
-    <col min="17" max="17" width="80.140625" customWidth="1"/>
-    <col min="18" max="18" width="35.7109375" customWidth="1"/>
-    <col min="19" max="20" width="122.7109375" customWidth="1"/>
-    <col min="21" max="21" width="48.42578125" customWidth="1"/>
-    <col min="22" max="22" width="29.7109375" customWidth="1"/>
-    <col min="23" max="23" width="80.140625" customWidth="1"/>
-    <col min="24" max="24" width="68.5703125" customWidth="1"/>
-    <col min="25" max="25" width="48.7109375" customWidth="1"/>
-    <col min="26" max="26" width="62" customWidth="1"/>
-    <col min="27" max="29" width="89.5703125" customWidth="1"/>
-    <col min="30" max="30" width="69.85546875" customWidth="1"/>
-    <col min="31" max="31" width="52.140625" customWidth="1"/>
-    <col min="32" max="32" width="73.140625" customWidth="1"/>
-    <col min="33" max="33" width="29.7109375" customWidth="1"/>
-    <col min="34" max="35" width="76" customWidth="1"/>
-    <col min="36" max="36" width="72.28515625" customWidth="1"/>
-    <col min="37" max="37" width="61.7109375" customWidth="1"/>
-    <col min="38" max="38" width="60" customWidth="1"/>
-    <col min="39" max="39" width="38.140625" customWidth="1"/>
-    <col min="40" max="40" width="69" customWidth="1"/>
-    <col min="41" max="41" width="72.42578125" customWidth="1"/>
-    <col min="42" max="42" width="111.5703125" customWidth="1"/>
-    <col min="43" max="43" width="72.5703125" customWidth="1"/>
-    <col min="44" max="44" width="86.85546875" customWidth="1"/>
-    <col min="45" max="46" width="64.7109375" customWidth="1"/>
-    <col min="47" max="47" width="54.5703125" customWidth="1"/>
-    <col min="48" max="48" width="75.42578125" customWidth="1"/>
-    <col min="49" max="49" width="58.140625" customWidth="1"/>
+    <col min="2" max="3" width="70" customWidth="1"/>
+    <col min="4" max="4" width="128.5703125" customWidth="1"/>
+    <col min="5" max="5" width="99.85546875" customWidth="1"/>
+    <col min="6" max="6" width="126.5703125" customWidth="1"/>
+    <col min="7" max="7" width="151.28515625" customWidth="1"/>
+    <col min="8" max="8" width="120.42578125" customWidth="1"/>
+    <col min="9" max="9" width="112.42578125" customWidth="1"/>
+    <col min="10" max="10" width="158.5703125" customWidth="1"/>
+    <col min="11" max="11" width="83.28515625" customWidth="1"/>
+    <col min="12" max="13" width="70" customWidth="1"/>
+    <col min="14" max="14" width="124.42578125" customWidth="1"/>
+    <col min="15" max="15" width="103.85546875" customWidth="1"/>
+    <col min="16" max="16" width="48.85546875" customWidth="1"/>
+    <col min="17" max="17" width="29.7109375" customWidth="1"/>
+    <col min="18" max="18" width="80.140625" customWidth="1"/>
+    <col min="19" max="19" width="35.7109375" customWidth="1"/>
+    <col min="20" max="21" width="122.7109375" customWidth="1"/>
+    <col min="22" max="22" width="48.42578125" customWidth="1"/>
+    <col min="23" max="23" width="29.7109375" customWidth="1"/>
+    <col min="24" max="24" width="80.140625" customWidth="1"/>
+    <col min="25" max="25" width="68.5703125" customWidth="1"/>
+    <col min="26" max="26" width="48.7109375" customWidth="1"/>
+    <col min="27" max="27" width="62" customWidth="1"/>
+    <col min="28" max="30" width="89.5703125" customWidth="1"/>
+    <col min="31" max="31" width="69.85546875" customWidth="1"/>
+    <col min="32" max="32" width="52.140625" customWidth="1"/>
+    <col min="33" max="33" width="73.140625" customWidth="1"/>
+    <col min="34" max="34" width="29.7109375" customWidth="1"/>
+    <col min="35" max="36" width="76" customWidth="1"/>
+    <col min="37" max="37" width="72.28515625" customWidth="1"/>
+    <col min="38" max="38" width="61.7109375" customWidth="1"/>
+    <col min="39" max="39" width="60" customWidth="1"/>
+    <col min="40" max="40" width="38.140625" customWidth="1"/>
+    <col min="41" max="41" width="69" customWidth="1"/>
+    <col min="42" max="42" width="72.42578125" customWidth="1"/>
+    <col min="43" max="43" width="111.5703125" customWidth="1"/>
+    <col min="44" max="44" width="72.5703125" customWidth="1"/>
+    <col min="45" max="45" width="86.85546875" customWidth="1"/>
+    <col min="46" max="47" width="64.7109375" customWidth="1"/>
+    <col min="48" max="48" width="54.5703125" customWidth="1"/>
+    <col min="49" max="49" width="75.42578125" customWidth="1"/>
+    <col min="50" max="50" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
+        <v>531</v>
+      </c>
+      <c r="D2" t="s">
         <v>540</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>535</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>533</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>531</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>524</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>520</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>382</v>
-      </c>
-      <c r="J2" t="s">
-        <v>502</v>
       </c>
       <c r="K2" t="s">
         <v>502</v>
       </c>
       <c r="L2" t="s">
-        <v>410</v>
+        <v>502</v>
       </c>
       <c r="M2" t="s">
         <v>410</v>
       </c>
       <c r="N2" t="s">
+        <v>410</v>
+      </c>
+      <c r="O2" t="s">
         <v>444</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>431</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>410</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>230</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>388</v>
-      </c>
-      <c r="S2" t="s">
-        <v>382</v>
       </c>
       <c r="T2" t="s">
         <v>382</v>
       </c>
       <c r="U2" t="s">
+        <v>382</v>
+      </c>
+      <c r="V2" t="s">
         <v>374</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>354</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>322</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>312</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>305</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>302</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>298</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>306</v>
       </c>
       <c r="AC2" t="s">
         <v>306</v>
@@ -2245,163 +2251,169 @@
         <v>306</v>
       </c>
       <c r="AE2" t="s">
+        <v>306</v>
+      </c>
+      <c r="AF2" t="s">
         <v>269</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>265</v>
       </c>
       <c r="AG2" t="s">
         <v>265</v>
       </c>
       <c r="AH2" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="AI2" t="s">
         <v>248</v>
       </c>
       <c r="AJ2" t="s">
+        <v>248</v>
+      </c>
+      <c r="AK2" t="s">
         <v>230</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>226</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>185</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>184</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>154</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>110</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>97</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>83</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>273</v>
       </c>
       <c r="C3" s="12">
+        <v>44575</v>
+      </c>
+      <c r="D3" s="12">
         <v>44537</v>
       </c>
-      <c r="D3" s="12">
+      <c r="E3" s="12">
         <v>44531</v>
       </c>
-      <c r="E3" s="12">
+      <c r="F3" s="12">
         <v>44530</v>
       </c>
-      <c r="F3" s="12">
+      <c r="G3" s="12">
         <v>44529</v>
       </c>
-      <c r="G3" s="12">
+      <c r="H3" s="12">
         <v>44524</v>
       </c>
-      <c r="H3" s="12">
+      <c r="I3" s="12">
         <v>44503</v>
       </c>
-      <c r="I3" s="12">
+      <c r="J3" s="12">
         <v>44343</v>
-      </c>
-      <c r="J3" s="12">
-        <v>44484</v>
       </c>
       <c r="K3" s="12">
         <v>44484</v>
       </c>
       <c r="L3" s="12">
+        <v>44484</v>
+      </c>
+      <c r="M3" s="12">
         <v>44473</v>
       </c>
-      <c r="M3" s="12">
+      <c r="N3" s="12">
         <v>44469</v>
       </c>
-      <c r="N3" s="12">
+      <c r="O3" s="12">
         <v>44453</v>
       </c>
-      <c r="O3" s="12">
+      <c r="P3" s="12">
         <v>44426</v>
       </c>
-      <c r="P3" s="12">
+      <c r="Q3" s="12">
         <v>44330</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="R3" s="12">
         <v>44307</v>
       </c>
-      <c r="R3" s="12">
+      <c r="S3" s="12">
         <v>44294</v>
       </c>
-      <c r="S3" s="12">
+      <c r="T3" s="12">
         <v>44343</v>
       </c>
-      <c r="T3" s="12">
+      <c r="U3" s="12">
         <v>44292</v>
       </c>
-      <c r="U3" s="12">
+      <c r="V3" s="12">
         <v>29681</v>
       </c>
-      <c r="V3" s="12">
+      <c r="W3" s="12">
         <v>44286</v>
       </c>
-      <c r="W3" s="12">
+      <c r="X3" s="12">
         <v>44260</v>
       </c>
-      <c r="X3" s="12">
+      <c r="Y3" s="12">
         <v>44244</v>
       </c>
-      <c r="Y3" s="12">
+      <c r="Z3" s="12">
         <v>44245</v>
       </c>
-      <c r="Z3" s="12">
+      <c r="AA3" s="12">
         <v>44223</v>
       </c>
-      <c r="AA3" s="12">
+      <c r="AB3" s="12">
         <v>44209</v>
       </c>
-      <c r="AB3" s="12">
+      <c r="AC3" s="12">
         <v>44253</v>
       </c>
-      <c r="AC3" s="12">
+      <c r="AD3" s="12">
         <v>44237</v>
       </c>
-      <c r="AF3" s="12">
+      <c r="AG3" s="12">
         <v>44181</v>
       </c>
-      <c r="AR3" s="1"/>
       <c r="AS3" s="1"/>
       <c r="AT3" s="1"/>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
-    </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY3" s="1"/>
+    </row>
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>474</v>
       </c>
@@ -2424,22 +2436,22 @@
         <v>315</v>
       </c>
       <c r="I4" t="s">
+        <v>315</v>
+      </c>
+      <c r="J4" t="s">
         <v>517</v>
-      </c>
-      <c r="J4" t="s">
-        <v>503</v>
       </c>
       <c r="K4" t="s">
         <v>503</v>
       </c>
       <c r="L4" t="s">
-        <v>468</v>
+        <v>503</v>
       </c>
       <c r="M4" t="s">
         <v>468</v>
       </c>
       <c r="N4" t="s">
-        <v>315</v>
+        <v>468</v>
       </c>
       <c r="O4" t="s">
         <v>315</v>
@@ -2448,13 +2460,13 @@
         <v>315</v>
       </c>
       <c r="Q4" t="s">
+        <v>315</v>
+      </c>
+      <c r="R4" t="s">
         <v>401</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>389</v>
-      </c>
-      <c r="S4" t="s">
-        <v>315</v>
       </c>
       <c r="T4" t="s">
         <v>315</v>
@@ -2463,472 +2475,481 @@
         <v>315</v>
       </c>
       <c r="V4" t="s">
+        <v>315</v>
+      </c>
+      <c r="W4" t="s">
         <v>355</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>315</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>311</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>315</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>315</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>319</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>311</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>272</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>271</v>
       </c>
-      <c r="AR4" s="1"/>
       <c r="AS4" s="1"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AY4" s="1"/>
+    </row>
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
+        <v>551</v>
+      </c>
+      <c r="D5" t="s">
         <v>541</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>536</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>534</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>530</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>525</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>521</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>516</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>511</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>506</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>479</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>469</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>445</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>432</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>411</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>402</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>390</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>545</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>384</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>375</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>356</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>323</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>313</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>317</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>303</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>297</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>320</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>309</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>307</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>270</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>274</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>267</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>249</v>
       </c>
       <c r="AI5" t="s">
         <v>249</v>
       </c>
       <c r="AJ5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AK5" t="s">
         <v>232</v>
       </c>
-      <c r="AK5" t="s">
+      <c r="AL5" t="s">
         <v>225</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AM5" t="s">
         <v>216</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AN5" t="s">
         <v>183</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>156</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AP5" t="s">
         <v>112</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AQ5" t="s">
         <v>98</v>
       </c>
-      <c r="AQ5" t="s">
+      <c r="AR5" t="s">
         <v>85</v>
       </c>
-      <c r="AR5" t="s">
-        <v>1</v>
-      </c>
       <c r="AS5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT5" t="s">
         <v>74</v>
       </c>
-      <c r="AT5" t="s">
+      <c r="AU5" t="s">
         <v>72</v>
       </c>
-      <c r="AU5" t="s">
+      <c r="AV5" t="s">
         <v>4</v>
       </c>
-      <c r="AV5" t="s">
+      <c r="AW5" t="s">
         <v>25</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AX5" t="s">
         <v>60</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="AY5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C6" t="s">
+        <v>552</v>
+      </c>
+      <c r="D6" t="s">
         <v>543</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>537</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>549</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>532</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>526</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>523</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>518</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>512</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>504</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>480</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>470</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>446</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>433</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>412</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>403</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>391</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>546</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>383</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>376</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>357</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>344</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>314</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>316</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>304</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>299</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>321</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>310</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>308</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>268</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>275</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>266</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>261</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>250</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>231</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" t="s">
         <v>223</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AM6" t="s">
         <v>215</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>182</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>155</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AP6" t="s">
         <v>111</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AQ6" t="s">
         <v>107</v>
       </c>
-      <c r="AQ6" t="s">
+      <c r="AR6" t="s">
         <v>84</v>
       </c>
-      <c r="AR6" t="s">
-        <v>0</v>
-      </c>
       <c r="AS6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT6" t="s">
         <v>73</v>
       </c>
-      <c r="AT6" t="s">
+      <c r="AU6" t="s">
         <v>71</v>
       </c>
-      <c r="AU6" t="s">
+      <c r="AV6" t="s">
         <v>3</v>
       </c>
-      <c r="AV6" t="s">
+      <c r="AW6" t="s">
         <v>24</v>
       </c>
-      <c r="AW6" t="s">
+      <c r="AX6" t="s">
         <v>59</v>
       </c>
-      <c r="AX6" t="s">
+      <c r="AY6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>542</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>539</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>550</v>
-      </c>
-      <c r="G7" t="s">
-        <v>522</v>
       </c>
       <c r="H7" t="s">
         <v>522</v>
       </c>
-      <c r="J7" t="s">
+      <c r="I7" t="s">
+        <v>522</v>
+      </c>
+      <c r="K7" t="s">
         <v>513</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>505</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>471</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>434</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>413</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>547</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>377</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>324</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>300</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>251</v>
       </c>
       <c r="AI7" t="s">
         <v>251</v>
       </c>
-      <c r="AK7" t="s">
+      <c r="AJ7" t="s">
+        <v>251</v>
+      </c>
+      <c r="AL7" t="s">
         <v>224</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AO7" t="s">
         <v>157</v>
       </c>
-      <c r="AP7" t="s">
+      <c r="AQ7" t="s">
         <v>108</v>
       </c>
-      <c r="AQ7" t="s">
+      <c r="AR7" t="s">
         <v>87</v>
       </c>
-      <c r="AT7" t="s">
+      <c r="AU7" t="s">
         <v>99</v>
       </c>
-      <c r="AW7" t="s">
+      <c r="AX7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>463</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>404</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>325</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>253</v>
       </c>
       <c r="AI8" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AJ8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>548</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>508</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>514</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>478</v>
       </c>
@@ -2944,9 +2965,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6625,7 +6646,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
storage connection stats counting when slots are missing is fixed
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="557">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1669,9 +1669,6 @@
     <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MegafonMSK\APR21\3PAR</t>
   </si>
   <si>
-    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\NOV21\ssave_spb\29_11_2021</t>
-  </si>
-  <si>
     <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\NOV21\blade_spb</t>
   </si>
   <si>
@@ -1679,6 +1676,21 @@
   </si>
   <si>
     <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\JAN22\mts_msc\ssave</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\NOV21\ssave_spb\10_12_2021</t>
+  </si>
+  <si>
+    <t>rnc.rosneft</t>
+  </si>
+  <si>
+    <t>SAN check</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\Rosneft\JAN2022</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\01.CUSTOMERS\Rosneft\JAN2022</t>
   </si>
 </sst>
 </file>
@@ -2101,151 +2113,153 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AY15"/>
+  <dimension ref="A1:AZ15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="3" width="70" customWidth="1"/>
-    <col min="4" max="4" width="128.5703125" customWidth="1"/>
-    <col min="5" max="5" width="99.85546875" customWidth="1"/>
-    <col min="6" max="6" width="126.5703125" customWidth="1"/>
-    <col min="7" max="7" width="151.28515625" customWidth="1"/>
-    <col min="8" max="8" width="120.42578125" customWidth="1"/>
-    <col min="9" max="9" width="112.42578125" customWidth="1"/>
-    <col min="10" max="10" width="158.5703125" customWidth="1"/>
-    <col min="11" max="11" width="83.28515625" customWidth="1"/>
-    <col min="12" max="13" width="70" customWidth="1"/>
-    <col min="14" max="14" width="124.42578125" customWidth="1"/>
-    <col min="15" max="15" width="103.85546875" customWidth="1"/>
-    <col min="16" max="16" width="48.85546875" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" customWidth="1"/>
-    <col min="18" max="18" width="80.140625" customWidth="1"/>
-    <col min="19" max="19" width="35.7109375" customWidth="1"/>
-    <col min="20" max="21" width="122.7109375" customWidth="1"/>
-    <col min="22" max="22" width="48.42578125" customWidth="1"/>
-    <col min="23" max="23" width="29.7109375" customWidth="1"/>
-    <col min="24" max="24" width="80.140625" customWidth="1"/>
-    <col min="25" max="25" width="68.5703125" customWidth="1"/>
-    <col min="26" max="26" width="48.7109375" customWidth="1"/>
-    <col min="27" max="27" width="62" customWidth="1"/>
-    <col min="28" max="30" width="89.5703125" customWidth="1"/>
-    <col min="31" max="31" width="69.85546875" customWidth="1"/>
-    <col min="32" max="32" width="52.140625" customWidth="1"/>
-    <col min="33" max="33" width="73.140625" customWidth="1"/>
-    <col min="34" max="34" width="29.7109375" customWidth="1"/>
-    <col min="35" max="36" width="76" customWidth="1"/>
-    <col min="37" max="37" width="72.28515625" customWidth="1"/>
-    <col min="38" max="38" width="61.7109375" customWidth="1"/>
-    <col min="39" max="39" width="60" customWidth="1"/>
-    <col min="40" max="40" width="38.140625" customWidth="1"/>
-    <col min="41" max="41" width="69" customWidth="1"/>
-    <col min="42" max="42" width="72.42578125" customWidth="1"/>
-    <col min="43" max="43" width="111.5703125" customWidth="1"/>
-    <col min="44" max="44" width="72.5703125" customWidth="1"/>
-    <col min="45" max="45" width="86.85546875" customWidth="1"/>
-    <col min="46" max="47" width="64.7109375" customWidth="1"/>
-    <col min="48" max="48" width="54.5703125" customWidth="1"/>
-    <col min="49" max="49" width="75.42578125" customWidth="1"/>
-    <col min="50" max="50" width="58.140625" customWidth="1"/>
+    <col min="2" max="2" width="70" customWidth="1"/>
+    <col min="3" max="3" width="109.42578125" customWidth="1"/>
+    <col min="4" max="4" width="70" customWidth="1"/>
+    <col min="5" max="5" width="128.5703125" customWidth="1"/>
+    <col min="6" max="6" width="99.85546875" customWidth="1"/>
+    <col min="7" max="7" width="126.5703125" customWidth="1"/>
+    <col min="8" max="8" width="151.28515625" customWidth="1"/>
+    <col min="9" max="9" width="120.42578125" customWidth="1"/>
+    <col min="10" max="10" width="112.42578125" customWidth="1"/>
+    <col min="11" max="11" width="158.5703125" customWidth="1"/>
+    <col min="12" max="12" width="83.28515625" customWidth="1"/>
+    <col min="13" max="14" width="70" customWidth="1"/>
+    <col min="15" max="15" width="124.42578125" customWidth="1"/>
+    <col min="16" max="16" width="103.85546875" customWidth="1"/>
+    <col min="17" max="17" width="48.85546875" customWidth="1"/>
+    <col min="18" max="18" width="29.7109375" customWidth="1"/>
+    <col min="19" max="19" width="80.140625" customWidth="1"/>
+    <col min="20" max="20" width="35.7109375" customWidth="1"/>
+    <col min="21" max="22" width="122.7109375" customWidth="1"/>
+    <col min="23" max="23" width="48.42578125" customWidth="1"/>
+    <col min="24" max="24" width="29.7109375" customWidth="1"/>
+    <col min="25" max="25" width="80.140625" customWidth="1"/>
+    <col min="26" max="26" width="68.5703125" customWidth="1"/>
+    <col min="27" max="27" width="48.7109375" customWidth="1"/>
+    <col min="28" max="28" width="62" customWidth="1"/>
+    <col min="29" max="31" width="89.5703125" customWidth="1"/>
+    <col min="32" max="32" width="69.85546875" customWidth="1"/>
+    <col min="33" max="33" width="52.140625" customWidth="1"/>
+    <col min="34" max="34" width="73.140625" customWidth="1"/>
+    <col min="35" max="35" width="29.7109375" customWidth="1"/>
+    <col min="36" max="37" width="76" customWidth="1"/>
+    <col min="38" max="38" width="72.28515625" customWidth="1"/>
+    <col min="39" max="39" width="61.7109375" customWidth="1"/>
+    <col min="40" max="40" width="60" customWidth="1"/>
+    <col min="41" max="41" width="38.140625" customWidth="1"/>
+    <col min="42" max="42" width="69" customWidth="1"/>
+    <col min="43" max="43" width="72.42578125" customWidth="1"/>
+    <col min="44" max="44" width="111.5703125" customWidth="1"/>
+    <col min="45" max="45" width="72.5703125" customWidth="1"/>
+    <col min="46" max="46" width="86.85546875" customWidth="1"/>
+    <col min="47" max="48" width="64.7109375" customWidth="1"/>
+    <col min="49" max="49" width="54.5703125" customWidth="1"/>
+    <col min="50" max="50" width="75.42578125" customWidth="1"/>
+    <col min="51" max="51" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
+        <v>553</v>
+      </c>
+      <c r="D2" t="s">
         <v>531</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>540</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>535</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>533</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>531</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>524</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>520</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>382</v>
-      </c>
-      <c r="K2" t="s">
-        <v>502</v>
       </c>
       <c r="L2" t="s">
         <v>502</v>
       </c>
       <c r="M2" t="s">
-        <v>410</v>
+        <v>502</v>
       </c>
       <c r="N2" t="s">
         <v>410</v>
       </c>
       <c r="O2" t="s">
+        <v>410</v>
+      </c>
+      <c r="P2" t="s">
         <v>444</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>431</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>410</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>230</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>388</v>
-      </c>
-      <c r="T2" t="s">
-        <v>382</v>
       </c>
       <c r="U2" t="s">
         <v>382</v>
       </c>
       <c r="V2" t="s">
+        <v>382</v>
+      </c>
+      <c r="W2" t="s">
         <v>374</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>354</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>322</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>312</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>305</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>302</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>298</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>306</v>
       </c>
       <c r="AD2" t="s">
         <v>306</v>
@@ -2254,171 +2268,177 @@
         <v>306</v>
       </c>
       <c r="AF2" t="s">
+        <v>306</v>
+      </c>
+      <c r="AG2" t="s">
         <v>269</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>265</v>
       </c>
       <c r="AH2" t="s">
         <v>265</v>
       </c>
       <c r="AI2" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="AJ2" t="s">
         <v>248</v>
       </c>
       <c r="AK2" t="s">
+        <v>248</v>
+      </c>
+      <c r="AL2" t="s">
         <v>230</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>226</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>185</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>184</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>154</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>110</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>97</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>83</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>273</v>
       </c>
       <c r="C3" s="12">
+        <v>44592</v>
+      </c>
+      <c r="D3" s="12">
         <v>44575</v>
       </c>
-      <c r="D3" s="12">
+      <c r="E3" s="12">
         <v>44537</v>
       </c>
-      <c r="E3" s="12">
+      <c r="F3" s="12">
         <v>44531</v>
       </c>
-      <c r="F3" s="12">
+      <c r="G3" s="12">
         <v>44530</v>
       </c>
-      <c r="G3" s="12">
+      <c r="H3" s="12">
         <v>44529</v>
       </c>
-      <c r="H3" s="12">
+      <c r="I3" s="12">
         <v>44524</v>
       </c>
-      <c r="I3" s="12">
+      <c r="J3" s="12">
         <v>44503</v>
       </c>
-      <c r="J3" s="12">
+      <c r="K3" s="12">
         <v>44343</v>
-      </c>
-      <c r="K3" s="12">
-        <v>44484</v>
       </c>
       <c r="L3" s="12">
         <v>44484</v>
       </c>
       <c r="M3" s="12">
+        <v>44484</v>
+      </c>
+      <c r="N3" s="12">
         <v>44473</v>
       </c>
-      <c r="N3" s="12">
+      <c r="O3" s="12">
         <v>44469</v>
       </c>
-      <c r="O3" s="12">
+      <c r="P3" s="12">
         <v>44453</v>
       </c>
-      <c r="P3" s="12">
+      <c r="Q3" s="12">
         <v>44426</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="R3" s="12">
         <v>44330</v>
       </c>
-      <c r="R3" s="12">
+      <c r="S3" s="12">
         <v>44307</v>
       </c>
-      <c r="S3" s="12">
+      <c r="T3" s="12">
         <v>44294</v>
       </c>
-      <c r="T3" s="12">
+      <c r="U3" s="12">
         <v>44343</v>
       </c>
-      <c r="U3" s="12">
+      <c r="V3" s="12">
         <v>44292</v>
       </c>
-      <c r="V3" s="12">
+      <c r="W3" s="12">
         <v>29681</v>
       </c>
-      <c r="W3" s="12">
+      <c r="X3" s="12">
         <v>44286</v>
       </c>
-      <c r="X3" s="12">
+      <c r="Y3" s="12">
         <v>44260</v>
       </c>
-      <c r="Y3" s="12">
+      <c r="Z3" s="12">
         <v>44244</v>
       </c>
-      <c r="Z3" s="12">
+      <c r="AA3" s="12">
         <v>44245</v>
       </c>
-      <c r="AA3" s="12">
+      <c r="AB3" s="12">
         <v>44223</v>
       </c>
-      <c r="AB3" s="12">
+      <c r="AC3" s="12">
         <v>44209</v>
       </c>
-      <c r="AC3" s="12">
+      <c r="AD3" s="12">
         <v>44253</v>
       </c>
-      <c r="AD3" s="12">
+      <c r="AE3" s="12">
         <v>44237</v>
       </c>
-      <c r="AG3" s="12">
+      <c r="AH3" s="12">
         <v>44181</v>
       </c>
-      <c r="AS3" s="1"/>
       <c r="AT3" s="1"/>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
       <c r="AY3" s="1"/>
-    </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ3" s="1"/>
+    </row>
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>474</v>
       </c>
       <c r="C4" t="s">
-        <v>315</v>
+        <v>554</v>
       </c>
       <c r="D4" t="s">
         <v>315</v>
@@ -2439,22 +2459,22 @@
         <v>315</v>
       </c>
       <c r="J4" t="s">
+        <v>315</v>
+      </c>
+      <c r="K4" t="s">
         <v>517</v>
-      </c>
-      <c r="K4" t="s">
-        <v>503</v>
       </c>
       <c r="L4" t="s">
         <v>503</v>
       </c>
       <c r="M4" t="s">
-        <v>468</v>
+        <v>503</v>
       </c>
       <c r="N4" t="s">
         <v>468</v>
       </c>
       <c r="O4" t="s">
-        <v>315</v>
+        <v>468</v>
       </c>
       <c r="P4" t="s">
         <v>315</v>
@@ -2463,13 +2483,13 @@
         <v>315</v>
       </c>
       <c r="R4" t="s">
+        <v>315</v>
+      </c>
+      <c r="S4" t="s">
         <v>401</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>389</v>
-      </c>
-      <c r="T4" t="s">
-        <v>315</v>
       </c>
       <c r="U4" t="s">
         <v>315</v>
@@ -2478,478 +2498,487 @@
         <v>315</v>
       </c>
       <c r="W4" t="s">
+        <v>315</v>
+      </c>
+      <c r="X4" t="s">
         <v>355</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>315</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>311</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>315</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>315</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>319</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>311</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>272</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>271</v>
       </c>
-      <c r="AS4" s="1"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
       <c r="AY4" s="1"/>
-    </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ4" s="1"/>
+    </row>
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="D5" t="s">
+        <v>550</v>
+      </c>
+      <c r="E5" t="s">
         <v>541</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>536</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>534</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>530</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>525</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>521</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>516</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>511</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>506</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>479</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>469</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>445</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>432</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>411</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>402</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>390</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>545</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>384</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>375</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>356</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>323</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>313</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>317</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>303</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>297</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>320</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>309</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>307</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>270</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>274</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>267</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>249</v>
       </c>
       <c r="AJ5" t="s">
         <v>249</v>
       </c>
       <c r="AK5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AL5" t="s">
         <v>232</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="AM5" t="s">
         <v>225</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AN5" t="s">
         <v>216</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>183</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AP5" t="s">
         <v>156</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AQ5" t="s">
         <v>112</v>
       </c>
-      <c r="AQ5" t="s">
+      <c r="AR5" t="s">
         <v>98</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="AS5" t="s">
         <v>85</v>
       </c>
-      <c r="AS5" t="s">
-        <v>1</v>
-      </c>
       <c r="AT5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU5" t="s">
         <v>74</v>
       </c>
-      <c r="AU5" t="s">
+      <c r="AV5" t="s">
         <v>72</v>
       </c>
-      <c r="AV5" t="s">
+      <c r="AW5" t="s">
         <v>4</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AX5" t="s">
         <v>25</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="AY5" t="s">
         <v>60</v>
       </c>
-      <c r="AY5" t="s">
+      <c r="AZ5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C6" t="s">
+        <v>555</v>
+      </c>
+      <c r="D6" t="s">
+        <v>551</v>
+      </c>
+      <c r="E6" t="s">
+        <v>543</v>
+      </c>
+      <c r="F6" t="s">
+        <v>537</v>
+      </c>
+      <c r="G6" t="s">
         <v>552</v>
       </c>
-      <c r="D6" t="s">
-        <v>543</v>
-      </c>
-      <c r="E6" t="s">
-        <v>537</v>
-      </c>
-      <c r="F6" t="s">
-        <v>549</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>532</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>526</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>523</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>518</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>512</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>504</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>480</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>470</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>446</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>433</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>412</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>403</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>391</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>546</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>383</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>376</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>357</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>344</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>314</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>316</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>304</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>299</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>321</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>310</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>308</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>268</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>275</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>266</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>261</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>250</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" t="s">
         <v>231</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AM6" t="s">
         <v>223</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>215</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>182</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AP6" t="s">
         <v>155</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AQ6" t="s">
         <v>111</v>
       </c>
-      <c r="AQ6" t="s">
+      <c r="AR6" t="s">
         <v>107</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AS6" t="s">
         <v>84</v>
       </c>
-      <c r="AS6" t="s">
+      <c r="AT6" t="s">
         <v>0</v>
       </c>
-      <c r="AT6" t="s">
+      <c r="AU6" t="s">
         <v>73</v>
       </c>
-      <c r="AU6" t="s">
+      <c r="AV6" t="s">
         <v>71</v>
       </c>
-      <c r="AV6" t="s">
+      <c r="AW6" t="s">
         <v>3</v>
       </c>
-      <c r="AW6" t="s">
+      <c r="AX6" t="s">
         <v>24</v>
       </c>
-      <c r="AX6" t="s">
+      <c r="AY6" t="s">
         <v>59</v>
       </c>
-      <c r="AY6" t="s">
+      <c r="AZ6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>542</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>539</v>
       </c>
-      <c r="F7" t="s">
-        <v>550</v>
-      </c>
-      <c r="H7" t="s">
-        <v>522</v>
+      <c r="G7" t="s">
+        <v>549</v>
       </c>
       <c r="I7" t="s">
         <v>522</v>
       </c>
-      <c r="K7" t="s">
+      <c r="J7" t="s">
+        <v>522</v>
+      </c>
+      <c r="L7" t="s">
         <v>513</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>505</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>471</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>434</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>413</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>547</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>377</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>324</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>300</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>251</v>
       </c>
       <c r="AJ7" t="s">
         <v>251</v>
       </c>
-      <c r="AL7" t="s">
+      <c r="AK7" t="s">
+        <v>251</v>
+      </c>
+      <c r="AM7" t="s">
         <v>224</v>
       </c>
-      <c r="AO7" t="s">
+      <c r="AP7" t="s">
         <v>157</v>
       </c>
-      <c r="AQ7" t="s">
+      <c r="AR7" t="s">
         <v>108</v>
       </c>
-      <c r="AR7" t="s">
+      <c r="AS7" t="s">
         <v>87</v>
       </c>
-      <c r="AU7" t="s">
+      <c r="AV7" t="s">
         <v>99</v>
       </c>
-      <c r="AX7" t="s">
+      <c r="AY7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>463</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>404</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>325</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>253</v>
       </c>
       <c r="AJ8" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AK8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>548</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>508</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>514</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>478</v>
       </c>
@@ -2965,9 +2994,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3029,12 +3058,6 @@
       <c r="F2" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
       <c r="I2" t="s">
         <v>211</v>
       </c>
@@ -3052,12 +3075,6 @@
       <c r="F3" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
       <c r="I3" t="s">
         <v>211</v>
       </c>
@@ -3075,12 +3092,6 @@
       <c r="F4" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
       <c r="I4" t="s">
         <v>211</v>
       </c>
@@ -3098,12 +3109,6 @@
       <c r="F5" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
       <c r="I5" s="10" t="s">
         <v>211</v>
       </c>
@@ -3130,12 +3135,6 @@
       <c r="F6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
       <c r="I6" t="s">
         <v>152</v>
       </c>
@@ -3162,12 +3161,6 @@
       <c r="F7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
       <c r="I7" t="s">
         <v>152</v>
       </c>
@@ -3197,12 +3190,6 @@
       <c r="F8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
       <c r="I8" t="s">
         <v>141</v>
       </c>
@@ -3232,12 +3219,6 @@
       <c r="F9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
       <c r="I9" t="s">
         <v>150</v>
       </c>
@@ -3267,12 +3248,6 @@
       <c r="F10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
       <c r="I10" t="s">
         <v>150</v>
       </c>
@@ -3302,12 +3277,6 @@
       <c r="F11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
       <c r="I11" t="s">
         <v>151</v>
       </c>
@@ -3337,12 +3306,6 @@
       <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
       <c r="I12" t="s">
         <v>147</v>
       </c>
@@ -3372,12 +3335,6 @@
       <c r="F13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
       <c r="I13" t="s">
         <v>147</v>
       </c>
@@ -3407,12 +3364,6 @@
       <c r="F14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
       <c r="I14" t="s">
         <v>145</v>
       </c>
@@ -3442,12 +3393,6 @@
       <c r="F15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
       <c r="I15" t="s">
         <v>146</v>
       </c>
@@ -3477,12 +3422,6 @@
       <c r="F16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
       <c r="I16" t="s">
         <v>146</v>
       </c>
@@ -3512,12 +3451,6 @@
       <c r="F17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
       <c r="I17" t="s">
         <v>143</v>
       </c>
@@ -3547,12 +3480,6 @@
       <c r="F18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
       <c r="I18" t="s">
         <v>143</v>
       </c>
@@ -3582,12 +3509,6 @@
       <c r="F19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
       <c r="I19" t="s">
         <v>143</v>
       </c>
@@ -3614,12 +3535,6 @@
       <c r="F20" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
       <c r="I20" t="s">
         <v>143</v>
       </c>
@@ -3646,12 +3561,6 @@
       <c r="F21" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
       <c r="I21" t="s">
         <v>143</v>
       </c>
@@ -3681,12 +3590,6 @@
       <c r="F22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
       <c r="I22" t="s">
         <v>144</v>
       </c>
@@ -3716,12 +3619,6 @@
       <c r="F23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
       <c r="I23" t="s">
         <v>144</v>
       </c>
@@ -3751,12 +3648,6 @@
       <c r="F24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
       <c r="I24" t="s">
         <v>144</v>
       </c>
@@ -3786,12 +3677,6 @@
       <c r="F25" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
       <c r="I25" t="s">
         <v>144</v>
       </c>
@@ -3821,12 +3706,6 @@
       <c r="F26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
       <c r="I26" t="s">
         <v>142</v>
       </c>
@@ -3853,12 +3732,6 @@
       <c r="F27" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
       <c r="I27" t="s">
         <v>142</v>
       </c>
@@ -3885,12 +3758,6 @@
       <c r="F28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
       <c r="I28" t="s">
         <v>142</v>
       </c>
@@ -3917,12 +3784,6 @@
       <c r="F29" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
       <c r="I29" t="s">
         <v>142</v>
       </c>
@@ -3946,12 +3807,6 @@
       <c r="F30" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
       <c r="I30" t="s">
         <v>142</v>
       </c>
@@ -3975,12 +3830,6 @@
       <c r="F31" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
       <c r="I31" t="s">
         <v>142</v>
       </c>
@@ -4007,12 +3856,6 @@
       <c r="F32" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
       <c r="I32" t="s">
         <v>148</v>
       </c>
@@ -4036,12 +3879,6 @@
       <c r="F33" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
       <c r="I33" t="s">
         <v>148</v>
       </c>
@@ -4065,12 +3902,6 @@
       <c r="F34" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
       <c r="I34" t="s">
         <v>148</v>
       </c>
@@ -4094,12 +3925,6 @@
       <c r="F35" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
       <c r="I35" t="s">
         <v>148</v>
       </c>
@@ -4123,12 +3948,6 @@
       <c r="F36" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
       <c r="I36" t="s">
         <v>148</v>
       </c>
@@ -4152,12 +3971,6 @@
       <c r="F37" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
       <c r="I37" t="s">
         <v>148</v>
       </c>
@@ -4181,12 +3994,6 @@
       <c r="F38" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
       <c r="I38" t="s">
         <v>148</v>
       </c>
@@ -4210,12 +4017,6 @@
       <c r="F39" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="G39">
-        <v>0</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
       <c r="I39" t="s">
         <v>219</v>
       </c>
@@ -4239,12 +4040,6 @@
       <c r="F40" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
       <c r="I40" t="s">
         <v>283</v>
       </c>
@@ -4271,12 +4066,6 @@
       <c r="F41" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
       <c r="I41" t="s">
         <v>450</v>
       </c>
@@ -4300,12 +4089,6 @@
       <c r="F42" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
       <c r="I42" t="s">
         <v>450</v>
       </c>
@@ -4329,12 +4112,6 @@
       <c r="F43" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
       <c r="I43" t="s">
         <v>450</v>
       </c>
@@ -4356,12 +4133,6 @@
       <c r="F44" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
       <c r="I44" t="s">
         <v>451</v>
       </c>
@@ -4383,12 +4154,6 @@
       <c r="F45" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
       <c r="I45" t="s">
         <v>451</v>
       </c>
@@ -4410,12 +4175,6 @@
       <c r="F46" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
       <c r="I46" t="s">
         <v>452</v>
       </c>
@@ -4437,12 +4196,6 @@
       <c r="F47" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
       <c r="I47" t="s">
         <v>452</v>
       </c>
@@ -4464,12 +4217,6 @@
       <c r="F48" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
       <c r="I48" t="s">
         <v>452</v>
       </c>
@@ -4491,12 +4238,6 @@
       <c r="F49" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
       <c r="I49" t="s">
         <v>452</v>
       </c>
@@ -4520,12 +4261,6 @@
       <c r="F50" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
       <c r="I50" t="s">
         <v>158</v>
       </c>
@@ -4543,12 +4278,6 @@
       <c r="F51" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="G51">
-        <v>0</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
-      </c>
       <c r="I51" t="s">
         <v>158</v>
       </c>
@@ -4566,12 +4295,6 @@
       <c r="F52" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G52">
-        <v>0</v>
-      </c>
-      <c r="H52">
-        <v>0</v>
-      </c>
       <c r="I52" t="s">
         <v>158</v>
       </c>
@@ -4589,12 +4312,6 @@
       <c r="F53" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G53">
-        <v>0</v>
-      </c>
-      <c r="H53">
-        <v>0</v>
-      </c>
       <c r="I53" t="s">
         <v>158</v>
       </c>
@@ -4615,12 +4332,6 @@
       <c r="F54" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="G54">
-        <v>0</v>
-      </c>
-      <c r="H54">
-        <v>0</v>
-      </c>
       <c r="I54" t="s">
         <v>162</v>
       </c>
@@ -4638,12 +4349,6 @@
       <c r="F55" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G55">
-        <v>0</v>
-      </c>
-      <c r="H55">
-        <v>0</v>
-      </c>
       <c r="I55" t="s">
         <v>162</v>
       </c>
@@ -4667,12 +4372,6 @@
       <c r="F56" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="G56">
-        <v>0</v>
-      </c>
-      <c r="H56">
-        <v>0</v>
-      </c>
       <c r="I56" t="s">
         <v>168</v>
       </c>
@@ -4691,12 +4390,6 @@
       <c r="F57" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
       <c r="I57" t="s">
         <v>168</v>
       </c>
@@ -4717,12 +4410,6 @@
       <c r="F58" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="G58">
-        <v>0</v>
-      </c>
-      <c r="H58">
-        <v>0</v>
-      </c>
       <c r="I58" t="s">
         <v>168</v>
       </c>
@@ -4741,10 +4428,7 @@
         <v>61</v>
       </c>
       <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59" t="s">
         <v>168</v>
@@ -4764,10 +4448,7 @@
         <v>62</v>
       </c>
       <c r="G60">
-        <v>0</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I60" t="s">
         <v>168</v>
@@ -4786,12 +4467,6 @@
       <c r="F61" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G61">
-        <v>0</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
       <c r="I61" t="s">
         <v>168</v>
       </c>
@@ -4809,12 +4484,6 @@
       <c r="F62" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G62">
-        <v>0</v>
-      </c>
-      <c r="H62">
-        <v>0</v>
-      </c>
       <c r="I62" t="s">
         <v>168</v>
       </c>
@@ -4832,12 +4501,6 @@
       <c r="F63" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G63">
-        <v>0</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
       <c r="I63" t="s">
         <v>168</v>
       </c>
@@ -4855,12 +4518,6 @@
       <c r="F64" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="G64">
-        <v>0</v>
-      </c>
-      <c r="H64">
-        <v>0</v>
-      </c>
       <c r="I64" t="s">
         <v>168</v>
       </c>
@@ -4878,12 +4535,6 @@
       <c r="F65" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="G65">
-        <v>0</v>
-      </c>
-      <c r="H65">
-        <v>0</v>
-      </c>
       <c r="I65" t="s">
         <v>168</v>
       </c>
@@ -4910,12 +4561,6 @@
       <c r="F66" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G66">
-        <v>0</v>
-      </c>
-      <c r="H66">
-        <v>0</v>
-      </c>
       <c r="I66" t="s">
         <v>169</v>
       </c>
@@ -4933,12 +4578,6 @@
       <c r="F67" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="G67">
-        <v>0</v>
-      </c>
-      <c r="H67">
-        <v>0</v>
-      </c>
       <c r="I67" t="s">
         <v>169</v>
       </c>
@@ -4959,12 +4598,6 @@
       <c r="F68" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-      <c r="H68">
-        <v>0</v>
-      </c>
       <c r="I68" t="s">
         <v>169</v>
       </c>
@@ -4982,12 +4615,6 @@
       <c r="F69" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-      <c r="H69">
-        <v>0</v>
-      </c>
       <c r="I69" t="s">
         <v>169</v>
       </c>
@@ -5005,12 +4632,6 @@
       <c r="F70" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
       <c r="I70" t="s">
         <v>169</v>
       </c>
@@ -5037,12 +4658,6 @@
       <c r="F71" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="G71">
-        <v>0</v>
-      </c>
-      <c r="H71">
-        <v>0</v>
-      </c>
       <c r="I71" t="s">
         <v>170</v>
       </c>
@@ -5060,12 +4675,6 @@
       <c r="F72" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="G72">
-        <v>0</v>
-      </c>
-      <c r="H72">
-        <v>0</v>
-      </c>
       <c r="I72" t="s">
         <v>170</v>
       </c>
@@ -5086,12 +4695,6 @@
       <c r="F73" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="G73">
-        <v>0</v>
-      </c>
-      <c r="H73">
-        <v>0</v>
-      </c>
       <c r="I73" t="s">
         <v>170</v>
       </c>
@@ -5112,12 +4715,6 @@
       <c r="F74" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="G74">
-        <v>0</v>
-      </c>
-      <c r="H74">
-        <v>0</v>
-      </c>
       <c r="I74" t="s">
         <v>170</v>
       </c>
@@ -5135,12 +4732,6 @@
       <c r="F75" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="G75">
-        <v>0</v>
-      </c>
-      <c r="H75">
-        <v>0</v>
-      </c>
       <c r="I75" t="s">
         <v>170</v>
       </c>
@@ -5158,12 +4749,6 @@
       <c r="F76" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="G76">
-        <v>0</v>
-      </c>
-      <c r="H76">
-        <v>0</v>
-      </c>
       <c r="I76" t="s">
         <v>170</v>
       </c>
@@ -5184,12 +4769,6 @@
       <c r="F77" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="G77">
-        <v>0</v>
-      </c>
-      <c r="H77">
-        <v>0</v>
-      </c>
       <c r="I77" t="s">
         <v>170</v>
       </c>
@@ -5213,12 +4792,6 @@
       <c r="F78" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="G78">
-        <v>0</v>
-      </c>
-      <c r="H78">
-        <v>0</v>
-      </c>
       <c r="I78" t="s">
         <v>170</v>
       </c>
@@ -5236,12 +4809,6 @@
       <c r="F79" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="G79">
-        <v>0</v>
-      </c>
-      <c r="H79">
-        <v>0</v>
-      </c>
       <c r="I79" t="s">
         <v>170</v>
       </c>
@@ -5262,12 +4829,6 @@
       <c r="F80" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="G80">
-        <v>0</v>
-      </c>
-      <c r="H80">
-        <v>0</v>
-      </c>
       <c r="I80" t="s">
         <v>170</v>
       </c>
@@ -5288,12 +4849,6 @@
       <c r="F81" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G81">
-        <v>0</v>
-      </c>
-      <c r="H81">
-        <v>0</v>
-      </c>
       <c r="I81" t="s">
         <v>170</v>
       </c>
@@ -5311,12 +4866,6 @@
       <c r="F82" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="G82">
-        <v>0</v>
-      </c>
-      <c r="H82">
-        <v>0</v>
-      </c>
       <c r="I82" t="s">
         <v>170</v>
       </c>
@@ -5334,12 +4883,6 @@
       <c r="F83" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G83">
-        <v>0</v>
-      </c>
-      <c r="H83">
-        <v>0</v>
-      </c>
       <c r="I83" t="s">
         <v>170</v>
       </c>
@@ -5357,12 +4900,6 @@
       <c r="F84" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="G84">
-        <v>0</v>
-      </c>
-      <c r="H84">
-        <v>0</v>
-      </c>
       <c r="I84" t="s">
         <v>170</v>
       </c>
@@ -5380,12 +4917,6 @@
       <c r="F85" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="G85">
-        <v>0</v>
-      </c>
-      <c r="H85">
-        <v>0</v>
-      </c>
       <c r="I85" t="s">
         <v>170</v>
       </c>
@@ -5403,12 +4934,6 @@
       <c r="F86" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G86">
-        <v>0</v>
-      </c>
-      <c r="H86">
-        <v>0</v>
-      </c>
       <c r="I86" t="s">
         <v>170</v>
       </c>
@@ -5426,12 +4951,6 @@
       <c r="F87" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G87">
-        <v>0</v>
-      </c>
-      <c r="H87">
-        <v>0</v>
-      </c>
       <c r="I87" t="s">
         <v>170</v>
       </c>
@@ -5452,12 +4971,6 @@
       <c r="F88" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="G88">
-        <v>0</v>
-      </c>
-      <c r="H88">
-        <v>0</v>
-      </c>
       <c r="I88" t="s">
         <v>170</v>
       </c>
@@ -5481,12 +4994,6 @@
       <c r="F89" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="G89">
-        <v>0</v>
-      </c>
-      <c r="H89">
-        <v>0</v>
-      </c>
       <c r="I89" t="s">
         <v>171</v>
       </c>
@@ -5504,12 +5011,6 @@
       <c r="F90" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G90">
-        <v>0</v>
-      </c>
-      <c r="H90">
-        <v>0</v>
-      </c>
       <c r="I90" t="s">
         <v>171</v>
       </c>
@@ -5527,12 +5028,6 @@
       <c r="F91" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="G91">
-        <v>0</v>
-      </c>
-      <c r="H91">
-        <v>0</v>
-      </c>
       <c r="I91" t="s">
         <v>171</v>
       </c>
@@ -5550,12 +5045,6 @@
       <c r="F92" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="G92">
-        <v>0</v>
-      </c>
-      <c r="H92">
-        <v>0</v>
-      </c>
       <c r="I92" t="s">
         <v>171</v>
       </c>
@@ -5573,12 +5062,6 @@
       <c r="F93" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="G93">
-        <v>0</v>
-      </c>
-      <c r="H93">
-        <v>0</v>
-      </c>
       <c r="I93" t="s">
         <v>171</v>
       </c>
@@ -5599,12 +5082,6 @@
       <c r="F94" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="G94">
-        <v>0</v>
-      </c>
-      <c r="H94">
-        <v>0</v>
-      </c>
       <c r="I94" t="s">
         <v>171</v>
       </c>
@@ -5625,12 +5102,6 @@
       <c r="F95" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="G95">
-        <v>0</v>
-      </c>
-      <c r="H95">
-        <v>0</v>
-      </c>
       <c r="I95" t="s">
         <v>171</v>
       </c>
@@ -5651,12 +5122,6 @@
       <c r="F96" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="G96">
-        <v>0</v>
-      </c>
-      <c r="H96">
-        <v>0</v>
-      </c>
       <c r="I96" t="s">
         <v>171</v>
       </c>
@@ -5677,12 +5142,6 @@
       <c r="F97" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="G97">
-        <v>0</v>
-      </c>
-      <c r="H97">
-        <v>0</v>
-      </c>
       <c r="I97" t="s">
         <v>171</v>
       </c>
@@ -5703,12 +5162,6 @@
       <c r="F98" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="G98">
-        <v>0</v>
-      </c>
-      <c r="H98">
-        <v>0</v>
-      </c>
       <c r="I98" t="s">
         <v>171</v>
       </c>
@@ -5729,12 +5182,6 @@
       <c r="F99" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="G99">
-        <v>0</v>
-      </c>
-      <c r="H99">
-        <v>0</v>
-      </c>
       <c r="I99" t="s">
         <v>171</v>
       </c>
@@ -5755,12 +5202,6 @@
       <c r="F100" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="G100">
-        <v>0</v>
-      </c>
-      <c r="H100">
-        <v>0</v>
-      </c>
       <c r="I100" t="s">
         <v>171</v>
       </c>
@@ -5781,12 +5222,6 @@
       <c r="F101" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="G101">
-        <v>0</v>
-      </c>
-      <c r="H101">
-        <v>0</v>
-      </c>
       <c r="I101" t="s">
         <v>171</v>
       </c>
@@ -5810,12 +5245,6 @@
       <c r="F102" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="G102">
-        <v>0</v>
-      </c>
-      <c r="H102">
-        <v>0</v>
-      </c>
       <c r="I102" t="s">
         <v>455</v>
       </c>
@@ -5833,12 +5262,6 @@
       <c r="F103" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="G103">
-        <v>0</v>
-      </c>
-      <c r="H103">
-        <v>0</v>
-      </c>
       <c r="I103" t="s">
         <v>455</v>
       </c>
@@ -5856,12 +5279,6 @@
       <c r="F104" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="G104">
-        <v>0</v>
-      </c>
-      <c r="H104">
-        <v>0</v>
-      </c>
       <c r="I104" t="s">
         <v>455</v>
       </c>
@@ -5882,12 +5299,6 @@
       <c r="F105" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="G105">
-        <v>0</v>
-      </c>
-      <c r="H105">
-        <v>0</v>
-      </c>
       <c r="I105" t="s">
         <v>455</v>
       </c>
@@ -5908,12 +5319,6 @@
       <c r="F106" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="G106">
-        <v>0</v>
-      </c>
-      <c r="H106">
-        <v>0</v>
-      </c>
       <c r="I106" t="s">
         <v>455</v>
       </c>
@@ -5931,12 +5336,6 @@
       <c r="F107" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="G107">
-        <v>0</v>
-      </c>
-      <c r="H107">
-        <v>0</v>
-      </c>
       <c r="I107" t="s">
         <v>455</v>
       </c>
@@ -5954,12 +5353,6 @@
       <c r="F108" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="G108">
-        <v>0</v>
-      </c>
-      <c r="H108">
-        <v>0</v>
-      </c>
       <c r="I108" t="s">
         <v>455</v>
       </c>
@@ -5980,12 +5373,6 @@
       <c r="F109" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="G109">
-        <v>0</v>
-      </c>
-      <c r="H109">
-        <v>0</v>
-      </c>
       <c r="I109" t="s">
         <v>455</v>
       </c>
@@ -6009,12 +5396,6 @@
       <c r="F110" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="G110">
-        <v>0</v>
-      </c>
-      <c r="H110">
-        <v>0</v>
-      </c>
       <c r="I110" t="s">
         <v>456</v>
       </c>
@@ -6035,12 +5416,6 @@
       <c r="F111" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="G111">
-        <v>0</v>
-      </c>
-      <c r="H111">
-        <v>0</v>
-      </c>
       <c r="I111" t="s">
         <v>456</v>
       </c>
@@ -6061,12 +5436,6 @@
       <c r="F112" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G112">
-        <v>0</v>
-      </c>
-      <c r="H112">
-        <v>0</v>
-      </c>
       <c r="I112" t="s">
         <v>456</v>
       </c>
@@ -6090,12 +5459,6 @@
       <c r="F113" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="G113">
-        <v>0</v>
-      </c>
-      <c r="H113">
-        <v>0</v>
-      </c>
       <c r="I113" t="s">
         <v>456</v>
       </c>
@@ -6116,12 +5479,6 @@
       <c r="F114" s="9" t="s">
         <v>328</v>
       </c>
-      <c r="G114">
-        <v>0</v>
-      </c>
-      <c r="H114">
-        <v>0</v>
-      </c>
       <c r="I114" t="s">
         <v>456</v>
       </c>
@@ -6145,12 +5502,6 @@
       <c r="F115" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="G115">
-        <v>0</v>
-      </c>
-      <c r="H115">
-        <v>0</v>
-      </c>
       <c r="I115" t="s">
         <v>456</v>
       </c>
@@ -6171,12 +5522,6 @@
       <c r="F116" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="G116">
-        <v>0</v>
-      </c>
-      <c r="H116">
-        <v>0</v>
-      </c>
       <c r="I116" t="s">
         <v>456</v>
       </c>
@@ -6194,12 +5539,6 @@
       <c r="F117" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="G117">
-        <v>0</v>
-      </c>
-      <c r="H117">
-        <v>0</v>
-      </c>
       <c r="I117" t="s">
         <v>456</v>
       </c>
@@ -6217,12 +5556,6 @@
       <c r="F118" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="G118">
-        <v>0</v>
-      </c>
-      <c r="H118">
-        <v>0</v>
-      </c>
       <c r="I118" t="s">
         <v>456</v>
       </c>
@@ -6240,12 +5573,6 @@
       <c r="F119" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="G119">
-        <v>0</v>
-      </c>
-      <c r="H119">
-        <v>0</v>
-      </c>
       <c r="I119" t="s">
         <v>456</v>
       </c>
@@ -6263,12 +5590,6 @@
       <c r="F120" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="G120">
-        <v>0</v>
-      </c>
-      <c r="H120">
-        <v>0</v>
-      </c>
       <c r="I120" t="s">
         <v>456</v>
       </c>
@@ -6286,12 +5607,6 @@
       <c r="F121" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="G121">
-        <v>0</v>
-      </c>
-      <c r="H121">
-        <v>0</v>
-      </c>
       <c r="I121" t="s">
         <v>456</v>
       </c>
@@ -6312,12 +5627,6 @@
       <c r="F122" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="G122">
-        <v>0</v>
-      </c>
-      <c r="H122">
-        <v>0</v>
-      </c>
       <c r="I122" t="s">
         <v>456</v>
       </c>
@@ -6338,12 +5647,6 @@
       <c r="F123" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="G123">
-        <v>0</v>
-      </c>
-      <c r="H123">
-        <v>0</v>
-      </c>
       <c r="I123" t="s">
         <v>456</v>
       </c>
@@ -6364,12 +5667,6 @@
       <c r="F124" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="G124">
-        <v>0</v>
-      </c>
-      <c r="H124">
-        <v>0</v>
-      </c>
       <c r="I124" t="s">
         <v>456</v>
       </c>
@@ -6390,12 +5687,6 @@
       <c r="F125" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="G125">
-        <v>0</v>
-      </c>
-      <c r="H125">
-        <v>0</v>
-      </c>
       <c r="I125" t="s">
         <v>457</v>
       </c>
@@ -6413,12 +5704,6 @@
       <c r="F126" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="G126">
-        <v>0</v>
-      </c>
-      <c r="H126">
-        <v>0</v>
-      </c>
       <c r="I126" t="s">
         <v>457</v>
       </c>
@@ -6436,12 +5721,6 @@
       <c r="F127" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="G127">
-        <v>0</v>
-      </c>
-      <c r="H127">
-        <v>0</v>
-      </c>
       <c r="I127" t="s">
         <v>457</v>
       </c>
@@ -6459,12 +5738,6 @@
       <c r="F128" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="G128">
-        <v>0</v>
-      </c>
-      <c r="H128">
-        <v>0</v>
-      </c>
       <c r="I128" t="s">
         <v>458</v>
       </c>
@@ -6482,12 +5755,6 @@
       <c r="F129" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="G129">
-        <v>0</v>
-      </c>
-      <c r="H129">
-        <v>0</v>
-      </c>
       <c r="I129" t="s">
         <v>458</v>
       </c>
@@ -6511,12 +5778,6 @@
       <c r="F130" s="9" t="s">
         <v>515</v>
       </c>
-      <c r="G130">
-        <v>0</v>
-      </c>
-      <c r="H130">
-        <v>0</v>
-      </c>
       <c r="I130" t="s">
         <v>482</v>
       </c>
@@ -6537,12 +5798,6 @@
       <c r="F131" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="G131">
-        <v>0</v>
-      </c>
-      <c r="H131">
-        <v>0</v>
-      </c>
       <c r="I131" t="s">
         <v>482</v>
       </c>
@@ -6566,12 +5821,6 @@
       <c r="F132" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="G132">
-        <v>0</v>
-      </c>
-      <c r="H132">
-        <v>0</v>
-      </c>
       <c r="I132" t="s">
         <v>459</v>
       </c>
@@ -6589,12 +5838,6 @@
       <c r="F133" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="G133">
-        <v>0</v>
-      </c>
-      <c r="H133">
-        <v>0</v>
-      </c>
       <c r="I133" t="s">
         <v>459</v>
       </c>
@@ -6614,12 +5857,6 @@
       </c>
       <c r="F134" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="G134">
-        <v>0</v>
-      </c>
-      <c r="H134">
-        <v>0</v>
       </c>
       <c r="I134" t="s">
         <v>459</v>
@@ -6761,7 +5998,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Swith pairs identification mudule added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13665" windowHeight="11520" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,14 @@
     <sheet name="software" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$L$134</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$L$137</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="565">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1691,6 +1691,30 @@
   </si>
   <si>
     <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\01.CUSTOMERS\Rosneft\JAN2022</t>
+  </si>
+  <si>
+    <t>switch_pair</t>
+  </si>
+  <si>
+    <t>sw_wwn_occurrence_stats</t>
+  </si>
+  <si>
+    <t>analysis_switch_pair</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS 6. SWITCH PAIRS IDENTIFICATION</t>
+  </si>
+  <si>
+    <t>Switch pairs</t>
+  </si>
+  <si>
+    <t>Switch pairs statistics</t>
+  </si>
+  <si>
+    <t>switch_pair_manual</t>
+  </si>
+  <si>
+    <t>Switch pairs correction</t>
   </si>
 </sst>
 </file>
@@ -2115,8 +2139,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AZ15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2172,7 +2196,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2992,11 +3016,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:L134"/>
+  <dimension ref="A1:L137"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G66" sqref="G66"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I85" sqref="I85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4427,9 +4451,6 @@
       <c r="F59" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G59">
-        <v>1</v>
-      </c>
       <c r="I59" t="s">
         <v>168</v>
       </c>
@@ -4447,9 +4468,6 @@
       <c r="F60" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G60">
-        <v>1</v>
-      </c>
       <c r="I60" t="s">
         <v>168</v>
       </c>
@@ -4986,133 +5004,130 @@
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>164</v>
+        <v>559</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F89" s="9" t="s">
+        <v>557</v>
+      </c>
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89" t="s">
+        <v>560</v>
+      </c>
+      <c r="J89" t="s">
+        <v>561</v>
+      </c>
+      <c r="K89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D90" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="I90" t="s">
+        <v>560</v>
+      </c>
+      <c r="J90" t="s">
+        <v>562</v>
+      </c>
+      <c r="K90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D91" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="F91" s="11" t="s">
+        <v>563</v>
+      </c>
+      <c r="I91" t="s">
+        <v>560</v>
+      </c>
+      <c r="J91" t="s">
+        <v>564</v>
+      </c>
+      <c r="K91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>164</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F92" s="9" t="s">
         <v>213</v>
-      </c>
-      <c r="I89" t="s">
-        <v>171</v>
-      </c>
-      <c r="J89" t="s">
-        <v>293</v>
-      </c>
-      <c r="K89" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D90" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I90" t="s">
-        <v>171</v>
-      </c>
-      <c r="J90" t="s">
-        <v>197</v>
-      </c>
-      <c r="K90">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D91" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="I91" t="s">
-        <v>171</v>
-      </c>
-      <c r="J91" t="s">
-        <v>207</v>
-      </c>
-      <c r="K91">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D92" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="I92" t="s">
         <v>171</v>
       </c>
       <c r="J92" t="s">
-        <v>260</v>
-      </c>
-      <c r="K92">
-        <v>42</v>
+        <v>293</v>
+      </c>
+      <c r="K92" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D93" s="6" t="s">
-        <v>95</v>
+      <c r="D93" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>493</v>
+        <v>165</v>
       </c>
       <c r="I93" t="s">
         <v>171</v>
       </c>
       <c r="J93" t="s">
-        <v>484</v>
+        <v>197</v>
       </c>
       <c r="K93">
-        <v>1</v>
-      </c>
-      <c r="L93" t="s">
-        <v>492</v>
+        <v>41</v>
       </c>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D94" s="6" t="s">
-        <v>95</v>
+      <c r="D94" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>494</v>
+        <v>166</v>
       </c>
       <c r="I94" t="s">
         <v>171</v>
       </c>
       <c r="J94" t="s">
-        <v>485</v>
+        <v>207</v>
       </c>
       <c r="K94">
-        <v>1</v>
-      </c>
-      <c r="L94" t="s">
-        <v>492</v>
+        <v>43</v>
       </c>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D95" s="6" t="s">
-        <v>95</v>
+      <c r="D95" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>495</v>
+        <v>167</v>
       </c>
       <c r="I95" t="s">
         <v>171</v>
       </c>
       <c r="J95" t="s">
-        <v>486</v>
+        <v>260</v>
       </c>
       <c r="K95">
-        <v>1</v>
-      </c>
-      <c r="L95" t="s">
-        <v>492</v>
+        <v>42</v>
       </c>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.25">
@@ -5120,13 +5135,13 @@
         <v>95</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="I96" t="s">
         <v>171</v>
       </c>
       <c r="J96" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="K96">
         <v>1</v>
@@ -5140,13 +5155,13 @@
         <v>95</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="I97" t="s">
         <v>171</v>
       </c>
       <c r="J97" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="K97">
         <v>1</v>
@@ -5160,13 +5175,13 @@
         <v>95</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="I98" t="s">
         <v>171</v>
       </c>
       <c r="J98" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="K98">
         <v>1</v>
@@ -5180,13 +5195,13 @@
         <v>95</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="I99" t="s">
         <v>171</v>
       </c>
       <c r="J99" t="s">
-        <v>510</v>
+        <v>487</v>
       </c>
       <c r="K99">
         <v>1</v>
@@ -5200,13 +5215,13 @@
         <v>95</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="I100" t="s">
         <v>171</v>
       </c>
       <c r="J100" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="K100">
         <v>1</v>
@@ -5220,13 +5235,13 @@
         <v>95</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="I101" t="s">
         <v>171</v>
       </c>
       <c r="J101" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="K101">
         <v>1</v>
@@ -5236,23 +5251,23 @@
       </c>
     </row>
     <row r="102" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>460</v>
-      </c>
       <c r="D102" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>423</v>
+        <v>501</v>
       </c>
       <c r="I102" t="s">
-        <v>455</v>
+        <v>171</v>
       </c>
       <c r="J102" t="s">
-        <v>425</v>
-      </c>
-      <c r="K102" s="10">
-        <v>1</v>
+        <v>510</v>
+      </c>
+      <c r="K102">
+        <v>1</v>
+      </c>
+      <c r="L102" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="103" spans="2:12" x14ac:dyDescent="0.25">
@@ -5260,16 +5275,19 @@
         <v>95</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>519</v>
+        <v>499</v>
       </c>
       <c r="I103" t="s">
-        <v>455</v>
+        <v>171</v>
       </c>
       <c r="J103" t="s">
-        <v>419</v>
-      </c>
-      <c r="K103" s="10">
-        <v>1</v>
+        <v>490</v>
+      </c>
+      <c r="K103">
+        <v>1</v>
+      </c>
+      <c r="L103" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="104" spans="2:12" x14ac:dyDescent="0.25">
@@ -5277,90 +5295,93 @@
         <v>95</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>414</v>
+        <v>500</v>
       </c>
       <c r="I104" t="s">
-        <v>455</v>
+        <v>171</v>
       </c>
       <c r="J104" t="s">
-        <v>418</v>
-      </c>
-      <c r="K104" s="10">
+        <v>491</v>
+      </c>
+      <c r="K104">
         <v>1</v>
       </c>
       <c r="L104" t="s">
-        <v>387</v>
+        <v>492</v>
       </c>
     </row>
     <row r="105" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>460</v>
+      </c>
       <c r="D105" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>461</v>
+        <v>423</v>
       </c>
       <c r="I105" t="s">
         <v>455</v>
       </c>
       <c r="J105" t="s">
-        <v>462</v>
+        <v>425</v>
       </c>
       <c r="K105" s="10">
         <v>1</v>
       </c>
-      <c r="L105" t="s">
-        <v>387</v>
-      </c>
     </row>
     <row r="106" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D106" s="5" t="s">
-        <v>96</v>
+      <c r="D106" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>424</v>
+        <v>519</v>
       </c>
       <c r="I106" t="s">
         <v>455</v>
       </c>
       <c r="J106" t="s">
-        <v>426</v>
-      </c>
-      <c r="K106">
-        <v>44</v>
+        <v>419</v>
+      </c>
+      <c r="K106" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D107" s="5" t="s">
-        <v>96</v>
+      <c r="D107" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="I107" t="s">
         <v>455</v>
       </c>
       <c r="J107" t="s">
-        <v>196</v>
-      </c>
-      <c r="K107">
-        <v>36</v>
+        <v>418</v>
+      </c>
+      <c r="K107" s="10">
+        <v>1</v>
+      </c>
+      <c r="L107" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="108" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D108" s="5" t="s">
-        <v>96</v>
+      <c r="D108" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>415</v>
+        <v>461</v>
       </c>
       <c r="I108" t="s">
         <v>455</v>
       </c>
       <c r="J108" t="s">
-        <v>416</v>
-      </c>
-      <c r="K108">
-        <v>33</v>
+        <v>462</v>
+      </c>
+      <c r="K108" s="10">
+        <v>1</v>
       </c>
       <c r="L108" t="s">
         <v>387</v>
@@ -5371,79 +5392,70 @@
         <v>96</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>453</v>
+        <v>424</v>
       </c>
       <c r="I109" t="s">
         <v>455</v>
       </c>
       <c r="J109" t="s">
+        <v>426</v>
+      </c>
+      <c r="K109">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D110" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="I110" t="s">
+        <v>455</v>
+      </c>
+      <c r="J110" t="s">
+        <v>196</v>
+      </c>
+      <c r="K110">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D111" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="I111" t="s">
+        <v>455</v>
+      </c>
+      <c r="J111" t="s">
+        <v>416</v>
+      </c>
+      <c r="K111">
+        <v>33</v>
+      </c>
+      <c r="L111" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D112" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="I112" t="s">
+        <v>455</v>
+      </c>
+      <c r="J112" t="s">
         <v>454</v>
       </c>
-      <c r="K109">
+      <c r="K112">
         <v>31</v>
-      </c>
-      <c r="L109" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>175</v>
-      </c>
-      <c r="D110" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F110" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="I110" t="s">
-        <v>456</v>
-      </c>
-      <c r="J110" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="K110" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
-        <v>245</v>
-      </c>
-      <c r="D111" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F111" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="I111" t="s">
-        <v>456</v>
-      </c>
-      <c r="J111" s="10" t="s">
-        <v>331</v>
-      </c>
-      <c r="K111" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B112" t="s">
-        <v>247</v>
-      </c>
-      <c r="D112" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F112" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="I112" t="s">
-        <v>456</v>
-      </c>
-      <c r="J112" s="10" t="s">
-        <v>332</v>
-      </c>
-      <c r="K112" s="10">
-        <v>1</v>
       </c>
       <c r="L112" t="s">
         <v>387</v>
@@ -5451,62 +5463,59 @@
     </row>
     <row r="113" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>246</v>
+        <v>175</v>
       </c>
       <c r="D113" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F113" s="9" t="s">
-        <v>212</v>
+        <v>176</v>
       </c>
       <c r="I113" t="s">
         <v>456</v>
       </c>
       <c r="J113" s="10" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="K113" s="10">
         <v>1</v>
       </c>
-      <c r="L113" t="s">
-        <v>387</v>
-      </c>
     </row>
     <row r="114" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>245</v>
+      </c>
       <c r="D114" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F114" s="9" t="s">
-        <v>328</v>
+        <v>177</v>
       </c>
       <c r="I114" t="s">
         <v>456</v>
       </c>
       <c r="J114" s="10" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K114" s="10">
         <v>1</v>
-      </c>
-      <c r="L114" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="115" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F115" s="9" t="s">
-        <v>240</v>
+        <v>186</v>
       </c>
       <c r="I115" t="s">
         <v>456</v>
       </c>
       <c r="J115" s="10" t="s">
-        <v>241</v>
+        <v>332</v>
       </c>
       <c r="K115" s="10">
         <v>1</v>
@@ -5516,54 +5525,69 @@
       </c>
     </row>
     <row r="116" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D116" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>178</v>
+      <c r="B116" t="s">
+        <v>246</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F116" s="9" t="s">
+        <v>212</v>
       </c>
       <c r="I116" t="s">
         <v>456</v>
       </c>
-      <c r="J116" t="s">
-        <v>208</v>
-      </c>
-      <c r="K116">
-        <v>64</v>
+      <c r="J116" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="K116" s="10">
+        <v>1</v>
+      </c>
+      <c r="L116" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="117" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D117" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>179</v>
+      <c r="D117" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F117" s="9" t="s">
+        <v>328</v>
       </c>
       <c r="I117" t="s">
         <v>456</v>
       </c>
-      <c r="J117" t="s">
-        <v>209</v>
-      </c>
-      <c r="K117">
-        <v>65</v>
+      <c r="J117" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="K117" s="10">
+        <v>1</v>
+      </c>
+      <c r="L117" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="118" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D118" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>466</v>
+      <c r="B118" t="s">
+        <v>244</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F118" s="9" t="s">
+        <v>240</v>
       </c>
       <c r="I118" t="s">
         <v>456</v>
       </c>
-      <c r="J118" t="s">
-        <v>214</v>
-      </c>
-      <c r="K118">
-        <v>66</v>
+      <c r="J118" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="K118" s="10">
+        <v>1</v>
+      </c>
+      <c r="L118" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="119" spans="2:12" x14ac:dyDescent="0.25">
@@ -5571,16 +5595,16 @@
         <v>96</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="I119" t="s">
         <v>456</v>
       </c>
       <c r="J119" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K119">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="120" spans="2:12" x14ac:dyDescent="0.25">
@@ -5588,16 +5612,16 @@
         <v>96</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>227</v>
+        <v>179</v>
       </c>
       <c r="I120" t="s">
         <v>456</v>
       </c>
       <c r="J120" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="K120">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="121" spans="2:12" x14ac:dyDescent="0.25">
@@ -5605,19 +5629,16 @@
         <v>96</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>544</v>
+        <v>466</v>
       </c>
       <c r="I121" t="s">
         <v>456</v>
       </c>
       <c r="J121" t="s">
-        <v>538</v>
+        <v>214</v>
       </c>
       <c r="K121">
-        <v>69</v>
-      </c>
-      <c r="L121" t="s">
-        <v>387</v>
+        <v>66</v>
       </c>
     </row>
     <row r="122" spans="2:12" x14ac:dyDescent="0.25">
@@ -5625,19 +5646,16 @@
         <v>96</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I122" t="s">
         <v>456</v>
       </c>
       <c r="J122" t="s">
-        <v>335</v>
+        <v>210</v>
       </c>
       <c r="K122">
-        <v>63</v>
-      </c>
-      <c r="L122" t="s">
-        <v>387</v>
+        <v>68</v>
       </c>
     </row>
     <row r="123" spans="2:12" x14ac:dyDescent="0.25">
@@ -5645,19 +5663,16 @@
         <v>96</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>334</v>
+        <v>227</v>
       </c>
       <c r="I123" t="s">
         <v>456</v>
       </c>
       <c r="J123" t="s">
-        <v>336</v>
+        <v>228</v>
       </c>
       <c r="K123">
-        <v>62</v>
-      </c>
-      <c r="L123" t="s">
-        <v>387</v>
+        <v>67</v>
       </c>
     </row>
     <row r="124" spans="2:12" x14ac:dyDescent="0.25">
@@ -5665,36 +5680,39 @@
         <v>96</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>242</v>
+        <v>544</v>
       </c>
       <c r="I124" t="s">
         <v>456</v>
       </c>
       <c r="J124" t="s">
-        <v>243</v>
+        <v>538</v>
       </c>
       <c r="K124">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="L124" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="125" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D125" s="6" t="s">
-        <v>95</v>
+      <c r="D125" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>370</v>
+        <v>188</v>
       </c>
       <c r="I125" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J125" t="s">
-        <v>371</v>
-      </c>
-      <c r="K125" s="10">
-        <v>1</v>
+        <v>335</v>
+      </c>
+      <c r="K125">
+        <v>63</v>
+      </c>
+      <c r="L125" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="126" spans="2:12" x14ac:dyDescent="0.25">
@@ -5702,16 +5720,19 @@
         <v>96</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>369</v>
+        <v>334</v>
       </c>
       <c r="I126" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J126" t="s">
-        <v>372</v>
+        <v>336</v>
       </c>
       <c r="K126">
-        <v>71</v>
+        <v>62</v>
+      </c>
+      <c r="L126" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="127" spans="2:12" x14ac:dyDescent="0.25">
@@ -5719,16 +5740,19 @@
         <v>96</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>467</v>
+        <v>242</v>
       </c>
       <c r="I127" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J127" t="s">
-        <v>373</v>
+        <v>243</v>
       </c>
       <c r="K127">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="L127" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="128" spans="2:12" x14ac:dyDescent="0.25">
@@ -5736,13 +5760,13 @@
         <v>95</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>220</v>
+        <v>370</v>
       </c>
       <c r="I128" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J128" t="s">
-        <v>294</v>
+        <v>371</v>
       </c>
       <c r="K128" s="10">
         <v>1</v>
@@ -5753,96 +5777,87 @@
         <v>96</v>
       </c>
       <c r="F129" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="I129" t="s">
+        <v>457</v>
+      </c>
+      <c r="J129" t="s">
+        <v>372</v>
+      </c>
+      <c r="K129">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D130" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="I130" t="s">
+        <v>457</v>
+      </c>
+      <c r="J130" t="s">
+        <v>373</v>
+      </c>
+      <c r="K130">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D131" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="I131" t="s">
+        <v>458</v>
+      </c>
+      <c r="J131" t="s">
+        <v>294</v>
+      </c>
+      <c r="K131" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D132" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F132" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="I129" t="s">
+      <c r="I132" t="s">
         <v>458</v>
       </c>
-      <c r="J129" t="s">
+      <c r="J132" t="s">
         <v>222</v>
       </c>
-      <c r="K129">
+      <c r="K132">
         <v>45</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A130">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A133">
         <v>17</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B133" t="s">
         <v>136</v>
       </c>
-      <c r="D130" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F130" s="9" t="s">
-        <v>515</v>
-      </c>
-      <c r="I130" t="s">
-        <v>482</v>
-      </c>
-      <c r="J130" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="K130" s="10">
-        <v>1</v>
-      </c>
-      <c r="L130" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D131" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F131" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="I131" t="s">
-        <v>482</v>
-      </c>
-      <c r="J131" t="s">
-        <v>345</v>
-      </c>
-      <c r="K131">
-        <v>51</v>
-      </c>
-      <c r="L131" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B132" t="s">
-        <v>287</v>
-      </c>
-      <c r="D132" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F132" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="I132" t="s">
-        <v>459</v>
-      </c>
-      <c r="J132" t="s">
-        <v>291</v>
-      </c>
-      <c r="K132" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D133" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F133" s="2" t="s">
-        <v>296</v>
+      <c r="F133" s="9" t="s">
+        <v>515</v>
       </c>
       <c r="I133" t="s">
-        <v>459</v>
-      </c>
-      <c r="J133" t="s">
-        <v>292</v>
+        <v>482</v>
+      </c>
+      <c r="J133" s="10" t="s">
+        <v>483</v>
       </c>
       <c r="K133" s="10">
         <v>1</v>
@@ -5856,18 +5871,78 @@
         <v>96</v>
       </c>
       <c r="F134" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="I134" t="s">
+        <v>482</v>
+      </c>
+      <c r="J134" t="s">
+        <v>345</v>
+      </c>
+      <c r="K134">
+        <v>51</v>
+      </c>
+      <c r="L134" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>287</v>
+      </c>
+      <c r="D135" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F135" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="I135" t="s">
+        <v>459</v>
+      </c>
+      <c r="J135" t="s">
+        <v>291</v>
+      </c>
+      <c r="K135" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D136" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="I136" t="s">
+        <v>459</v>
+      </c>
+      <c r="J136" t="s">
+        <v>292</v>
+      </c>
+      <c r="K136" s="10">
+        <v>1</v>
+      </c>
+      <c r="L136" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D137" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F137" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="I134" t="s">
+      <c r="I137" t="s">
         <v>459</v>
       </c>
-      <c r="J134" t="s">
+      <c r="J137" t="s">
         <v>290</v>
       </c>
-      <c r="K134">
+      <c r="K137">
         <v>46</v>
       </c>
-      <c r="L134" t="s">
+      <c r="L137" t="s">
         <v>387</v>
       </c>
     </row>

</xml_diff>

<commit_message>
switchPair_id integrated to connection statistics
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,14 @@
     <sheet name="software" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$L$137</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$L$141</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="572">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1715,6 +1715,27 @@
   </si>
   <si>
     <t>Switch pairs correction</t>
+  </si>
+  <si>
+    <t>switch_params_aggregated_upd</t>
+  </si>
+  <si>
+    <t>Switch parameters updated with switch pairs id</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS X. AGGREGATED SWITCH PARAMETERS AND SWITCH PAIRS</t>
+  </si>
+  <si>
+    <t>isl_aggregated_upd</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS X. INTERSWITCH, INTERFABRIC CONNECTIONS AND SWITCH PAIRS</t>
+  </si>
+  <si>
+    <t>ISL with switch pairs ID</t>
+  </si>
+  <si>
+    <t>fcredge_upd</t>
   </si>
 </sst>
 </file>
@@ -2139,8 +2160,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AZ15"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2156,8 +2177,9 @@
     <col min="9" max="9" width="120.42578125" customWidth="1"/>
     <col min="10" max="10" width="112.42578125" customWidth="1"/>
     <col min="11" max="11" width="158.5703125" customWidth="1"/>
-    <col min="12" max="12" width="83.28515625" customWidth="1"/>
-    <col min="13" max="14" width="70" customWidth="1"/>
+    <col min="12" max="12" width="103.7109375" customWidth="1"/>
+    <col min="13" max="13" width="91.85546875" customWidth="1"/>
+    <col min="14" max="14" width="70" customWidth="1"/>
     <col min="15" max="15" width="124.42578125" customWidth="1"/>
     <col min="16" max="16" width="103.85546875" customWidth="1"/>
     <col min="17" max="17" width="48.85546875" customWidth="1"/>
@@ -2196,7 +2218,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3016,11 +3038,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:L137"/>
+  <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I85" sqref="I85"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4410,55 +4432,55 @@
       <c r="D57" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E57" s="16"/>
-      <c r="F57" s="2" t="s">
-        <v>427</v>
+      <c r="F57" s="9" t="s">
+        <v>565</v>
       </c>
       <c r="I57" t="s">
-        <v>168</v>
+        <v>567</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>428</v>
+        <v>566</v>
       </c>
       <c r="K57" s="10">
         <v>1</v>
-      </c>
-      <c r="L57" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D58" s="6" t="s">
         <v>95</v>
       </c>
+      <c r="E58" s="16"/>
       <c r="F58" s="2" t="s">
-        <v>163</v>
+        <v>427</v>
       </c>
       <c r="I58" t="s">
         <v>168</v>
       </c>
       <c r="J58" s="10" t="s">
-        <v>211</v>
+        <v>428</v>
       </c>
       <c r="K58" s="10">
         <v>1</v>
       </c>
+      <c r="L58" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D59" s="5" t="s">
-        <v>96</v>
+      <c r="D59" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>61</v>
+        <v>163</v>
       </c>
       <c r="I59" t="s">
         <v>168</v>
       </c>
-      <c r="J59" t="s">
-        <v>190</v>
-      </c>
-      <c r="K59">
-        <v>12</v>
+      <c r="J59" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="K59" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -4466,16 +4488,16 @@
         <v>96</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I60" t="s">
         <v>168</v>
       </c>
       <c r="J60" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K60">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -4483,16 +4505,16 @@
         <v>96</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I61" t="s">
         <v>168</v>
       </c>
       <c r="J61" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="K61">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -4500,16 +4522,16 @@
         <v>96</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I62" t="s">
         <v>168</v>
       </c>
       <c r="J62" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K62">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -4517,16 +4539,16 @@
         <v>96</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I63" t="s">
         <v>168</v>
       </c>
       <c r="J63" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="K63">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
@@ -4534,16 +4556,16 @@
         <v>96</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>420</v>
+        <v>64</v>
       </c>
       <c r="I64" t="s">
         <v>168</v>
       </c>
       <c r="J64" t="s">
-        <v>421</v>
+        <v>192</v>
       </c>
       <c r="K64">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -4551,270 +4573,264 @@
         <v>96</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="I65" t="s">
         <v>168</v>
       </c>
       <c r="J65" t="s">
+        <v>421</v>
+      </c>
+      <c r="K65">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D66" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="I66" t="s">
+        <v>168</v>
+      </c>
+      <c r="J66" t="s">
         <v>429</v>
       </c>
-      <c r="K65">
+      <c r="K66">
         <v>11</v>
       </c>
-      <c r="L65" t="s">
+      <c r="L66" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67">
         <v>18</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B67" t="s">
         <v>138</v>
       </c>
-      <c r="D66" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I66" t="s">
-        <v>169</v>
-      </c>
-      <c r="J66" s="10" t="s">
-        <v>278</v>
-      </c>
-      <c r="K66" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D67" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>276</v>
+        <v>69</v>
       </c>
       <c r="I67" t="s">
         <v>169</v>
       </c>
-      <c r="J67" s="10" t="s">
-        <v>277</v>
+      <c r="J67" t="s">
+        <v>278</v>
       </c>
       <c r="K67" s="10">
         <v>1</v>
       </c>
-      <c r="L67" t="s">
-        <v>387</v>
-      </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D68" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I68" t="s">
-        <v>169</v>
+      <c r="D68" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I68" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="J68" t="s">
-        <v>201</v>
-      </c>
-      <c r="K68">
-        <v>35</v>
+        <v>48</v>
+      </c>
+      <c r="K68" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D69" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>68</v>
+      <c r="D69" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>568</v>
       </c>
       <c r="I69" t="s">
-        <v>169</v>
+        <v>569</v>
       </c>
       <c r="J69" t="s">
-        <v>202</v>
-      </c>
-      <c r="K69">
-        <v>34</v>
+        <v>570</v>
+      </c>
+      <c r="K69" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D70" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="I70" t="s">
-        <v>169</v>
+      <c r="D70" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>571</v>
+      </c>
+      <c r="I70" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="J70" t="s">
-        <v>281</v>
-      </c>
-      <c r="K70">
-        <v>32</v>
-      </c>
-      <c r="L70" t="s">
-        <v>387</v>
+        <v>48</v>
+      </c>
+      <c r="K70" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>20</v>
-      </c>
-      <c r="B71" t="s">
-        <v>131</v>
-      </c>
       <c r="D71" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>90</v>
+        <v>276</v>
       </c>
       <c r="I71" t="s">
-        <v>170</v>
-      </c>
-      <c r="J71" s="10" t="s">
-        <v>259</v>
+        <v>169</v>
+      </c>
+      <c r="J71" t="s">
+        <v>277</v>
       </c>
       <c r="K71" s="10">
         <v>1</v>
       </c>
+      <c r="L71" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D72" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F72" s="9" t="s">
-        <v>409</v>
+      <c r="D72" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="I72" t="s">
-        <v>170</v>
-      </c>
-      <c r="J72" s="10" t="s">
-        <v>406</v>
-      </c>
-      <c r="K72" s="10">
-        <v>1</v>
-      </c>
-      <c r="L72" t="s">
+        <v>169</v>
+      </c>
+      <c r="J72" t="s">
+        <v>201</v>
+      </c>
+      <c r="K72">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D73" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I73" t="s">
+        <v>169</v>
+      </c>
+      <c r="J73" t="s">
+        <v>202</v>
+      </c>
+      <c r="K73">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D74" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74" t="s">
+        <v>169</v>
+      </c>
+      <c r="J74" t="s">
+        <v>281</v>
+      </c>
+      <c r="K74">
+        <v>32</v>
+      </c>
+      <c r="L74" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D73" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F73" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="I73" t="s">
-        <v>170</v>
-      </c>
-      <c r="J73" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="K73" s="10">
-        <v>1</v>
-      </c>
-      <c r="L73" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D74" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="I74" t="s">
-        <v>170</v>
-      </c>
-      <c r="J74" s="10" t="s">
-        <v>327</v>
-      </c>
-      <c r="K74" s="10">
-        <v>1</v>
-      </c>
-    </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>20</v>
+      </c>
+      <c r="B75" t="s">
+        <v>131</v>
+      </c>
       <c r="D75" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F75" s="2" t="s">
-        <v>236</v>
+      <c r="F75" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="I75" t="s">
         <v>170</v>
       </c>
       <c r="J75" s="10" t="s">
-        <v>237</v>
+        <v>259</v>
       </c>
       <c r="K75" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D76" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="F76" s="11" t="s">
-        <v>239</v>
+      <c r="D76" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>409</v>
       </c>
       <c r="I76" t="s">
         <v>170</v>
       </c>
       <c r="J76" s="10" t="s">
-        <v>237</v>
+        <v>406</v>
       </c>
       <c r="K76" s="10">
         <v>1</v>
       </c>
+      <c r="L76" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>133</v>
-      </c>
       <c r="D77" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F77" s="8" t="s">
-        <v>109</v>
+      <c r="F77" s="9" t="s">
+        <v>262</v>
       </c>
       <c r="I77" t="s">
         <v>170</v>
       </c>
       <c r="J77" s="10" t="s">
-        <v>368</v>
+        <v>263</v>
       </c>
       <c r="K77" s="10">
         <v>1</v>
       </c>
+      <c r="L77" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>119</v>
-      </c>
-      <c r="C78" t="s">
-        <v>132</v>
-      </c>
       <c r="D78" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F78" s="7" t="s">
-        <v>93</v>
+      <c r="F78" s="2" t="s">
+        <v>235</v>
       </c>
       <c r="I78" t="s">
         <v>170</v>
       </c>
       <c r="J78" s="10" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="K78" s="10">
         <v>1</v>
@@ -4824,125 +4840,134 @@
       <c r="D79" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F79" s="7" t="s">
-        <v>301</v>
+      <c r="F79" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="I79" t="s">
         <v>170</v>
       </c>
       <c r="J79" s="10" t="s">
-        <v>337</v>
+        <v>237</v>
       </c>
       <c r="K79" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>134</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>405</v>
+      <c r="D80" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="F80" s="11" t="s">
+        <v>239</v>
       </c>
       <c r="I80" t="s">
         <v>170</v>
       </c>
-      <c r="J80" t="s">
-        <v>193</v>
-      </c>
-      <c r="K80">
-        <v>17</v>
+      <c r="J80" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="K80" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>135</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>101</v>
+        <v>133</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="I81" t="s">
         <v>170</v>
       </c>
-      <c r="J81" t="s">
-        <v>194</v>
-      </c>
-      <c r="K81">
-        <v>15</v>
+      <c r="J81" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="K81" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D82" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>102</v>
+      <c r="B82" t="s">
+        <v>119</v>
+      </c>
+      <c r="C82" t="s">
+        <v>132</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F82" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="I82" t="s">
         <v>170</v>
       </c>
-      <c r="J82" t="s">
-        <v>195</v>
-      </c>
-      <c r="K82">
-        <v>16</v>
+      <c r="J82" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="K82" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D83" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>103</v>
+      <c r="D83" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F83" s="7" t="s">
+        <v>301</v>
       </c>
       <c r="I83" t="s">
         <v>170</v>
       </c>
-      <c r="J83" t="s">
-        <v>203</v>
-      </c>
-      <c r="K83">
-        <v>57</v>
+      <c r="J83" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="K83" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>134</v>
+      </c>
       <c r="D84" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>104</v>
+        <v>405</v>
       </c>
       <c r="I84" t="s">
         <v>170</v>
       </c>
       <c r="J84" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="K84">
-        <v>54</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>135</v>
+      </c>
       <c r="D85" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I85" t="s">
         <v>170</v>
       </c>
       <c r="J85" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="K85">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.25">
@@ -4950,16 +4975,16 @@
         <v>96</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I86" t="s">
         <v>170</v>
       </c>
       <c r="J86" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="K86">
-        <v>56</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.25">
@@ -4967,19 +4992,16 @@
         <v>96</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>408</v>
+        <v>103</v>
       </c>
       <c r="I87" t="s">
         <v>170</v>
       </c>
       <c r="J87" t="s">
-        <v>407</v>
+        <v>203</v>
       </c>
       <c r="K87">
-        <v>53</v>
-      </c>
-      <c r="L87" t="s">
-        <v>387</v>
+        <v>57</v>
       </c>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.25">
@@ -4987,227 +5009,215 @@
         <v>96</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>264</v>
+        <v>104</v>
       </c>
       <c r="I88" t="s">
         <v>170</v>
       </c>
       <c r="J88" t="s">
+        <v>204</v>
+      </c>
+      <c r="K88">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D89" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I89" t="s">
+        <v>170</v>
+      </c>
+      <c r="J89" t="s">
+        <v>205</v>
+      </c>
+      <c r="K89">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D90" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I90" t="s">
+        <v>170</v>
+      </c>
+      <c r="J90" t="s">
+        <v>206</v>
+      </c>
+      <c r="K90">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D91" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="I91" t="s">
+        <v>170</v>
+      </c>
+      <c r="J91" t="s">
+        <v>407</v>
+      </c>
+      <c r="K91">
+        <v>53</v>
+      </c>
+      <c r="L91" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D92" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="I92" t="s">
+        <v>170</v>
+      </c>
+      <c r="J92" t="s">
         <v>400</v>
       </c>
-      <c r="K88">
+      <c r="K92">
         <v>52</v>
       </c>
-      <c r="L88" t="s">
+      <c r="L92" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
         <v>559</v>
       </c>
-      <c r="D89" s="6" t="s">
+      <c r="D93" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F89" s="9" t="s">
+      <c r="F93" s="9" t="s">
         <v>557</v>
       </c>
-      <c r="H89">
-        <v>1</v>
-      </c>
-      <c r="I89" t="s">
+      <c r="I93" t="s">
         <v>560</v>
       </c>
-      <c r="J89" t="s">
+      <c r="J93" t="s">
         <v>561</v>
       </c>
-      <c r="K89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D90" s="6" t="s">
+      <c r="K93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D94" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F90" s="9" t="s">
+      <c r="F94" s="9" t="s">
         <v>558</v>
       </c>
-      <c r="I90" t="s">
+      <c r="I94" t="s">
         <v>560</v>
       </c>
-      <c r="J90" t="s">
+      <c r="J94" t="s">
         <v>562</v>
       </c>
-      <c r="K90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D91" s="11" t="s">
+      <c r="K94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D95" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="F91" s="11" t="s">
+      <c r="F95" s="11" t="s">
         <v>563</v>
       </c>
-      <c r="I91" t="s">
+      <c r="I95" t="s">
         <v>560</v>
       </c>
-      <c r="J91" t="s">
+      <c r="J95" t="s">
         <v>564</v>
       </c>
-      <c r="K91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
+      <c r="K95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
         <v>164</v>
       </c>
-      <c r="D92" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F92" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="I92" t="s">
-        <v>171</v>
-      </c>
-      <c r="J92" t="s">
-        <v>293</v>
-      </c>
-      <c r="K92" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D93" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I93" t="s">
-        <v>171</v>
-      </c>
-      <c r="J93" t="s">
-        <v>197</v>
-      </c>
-      <c r="K93">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D94" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="I94" t="s">
-        <v>171</v>
-      </c>
-      <c r="J94" t="s">
-        <v>207</v>
-      </c>
-      <c r="K94">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D95" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="I95" t="s">
-        <v>171</v>
-      </c>
-      <c r="J95" t="s">
-        <v>260</v>
-      </c>
-      <c r="K95">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D96" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F96" s="2" t="s">
-        <v>493</v>
+      <c r="F96" s="9" t="s">
+        <v>213</v>
       </c>
       <c r="I96" t="s">
         <v>171</v>
       </c>
       <c r="J96" t="s">
-        <v>484</v>
-      </c>
-      <c r="K96">
-        <v>1</v>
-      </c>
-      <c r="L96" t="s">
-        <v>492</v>
+        <v>293</v>
+      </c>
+      <c r="K96" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D97" s="6" t="s">
-        <v>95</v>
+      <c r="D97" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>494</v>
+        <v>165</v>
       </c>
       <c r="I97" t="s">
         <v>171</v>
       </c>
       <c r="J97" t="s">
-        <v>485</v>
+        <v>197</v>
       </c>
       <c r="K97">
-        <v>1</v>
-      </c>
-      <c r="L97" t="s">
-        <v>492</v>
+        <v>41</v>
       </c>
     </row>
     <row r="98" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D98" s="6" t="s">
-        <v>95</v>
+      <c r="D98" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>495</v>
+        <v>166</v>
       </c>
       <c r="I98" t="s">
         <v>171</v>
       </c>
       <c r="J98" t="s">
-        <v>486</v>
+        <v>207</v>
       </c>
       <c r="K98">
-        <v>1</v>
-      </c>
-      <c r="L98" t="s">
-        <v>492</v>
+        <v>43</v>
       </c>
     </row>
     <row r="99" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D99" s="6" t="s">
-        <v>95</v>
+      <c r="D99" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>496</v>
+        <v>167</v>
       </c>
       <c r="I99" t="s">
         <v>171</v>
       </c>
       <c r="J99" t="s">
-        <v>487</v>
+        <v>260</v>
       </c>
       <c r="K99">
-        <v>1</v>
-      </c>
-      <c r="L99" t="s">
-        <v>492</v>
+        <v>42</v>
       </c>
     </row>
     <row r="100" spans="2:12" x14ac:dyDescent="0.25">
@@ -5215,13 +5225,13 @@
         <v>95</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="I100" t="s">
         <v>171</v>
       </c>
       <c r="J100" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="K100">
         <v>1</v>
@@ -5235,13 +5245,13 @@
         <v>95</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="I101" t="s">
         <v>171</v>
       </c>
       <c r="J101" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="K101">
         <v>1</v>
@@ -5255,13 +5265,13 @@
         <v>95</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="I102" t="s">
         <v>171</v>
       </c>
       <c r="J102" t="s">
-        <v>510</v>
+        <v>486</v>
       </c>
       <c r="K102">
         <v>1</v>
@@ -5275,13 +5285,13 @@
         <v>95</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="I103" t="s">
         <v>171</v>
       </c>
       <c r="J103" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="K103">
         <v>1</v>
@@ -5295,13 +5305,13 @@
         <v>95</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="I104" t="s">
         <v>171</v>
       </c>
       <c r="J104" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="K104">
         <v>1</v>
@@ -5311,23 +5321,23 @@
       </c>
     </row>
     <row r="105" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>460</v>
-      </c>
       <c r="D105" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>423</v>
+        <v>498</v>
       </c>
       <c r="I105" t="s">
-        <v>455</v>
+        <v>171</v>
       </c>
       <c r="J105" t="s">
-        <v>425</v>
-      </c>
-      <c r="K105" s="10">
-        <v>1</v>
+        <v>489</v>
+      </c>
+      <c r="K105">
+        <v>1</v>
+      </c>
+      <c r="L105" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="106" spans="2:12" x14ac:dyDescent="0.25">
@@ -5335,16 +5345,19 @@
         <v>95</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>519</v>
+        <v>501</v>
       </c>
       <c r="I106" t="s">
-        <v>455</v>
+        <v>171</v>
       </c>
       <c r="J106" t="s">
-        <v>419</v>
-      </c>
-      <c r="K106" s="10">
-        <v>1</v>
+        <v>510</v>
+      </c>
+      <c r="K106">
+        <v>1</v>
+      </c>
+      <c r="L106" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="107" spans="2:12" x14ac:dyDescent="0.25">
@@ -5352,19 +5365,19 @@
         <v>95</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>414</v>
+        <v>499</v>
       </c>
       <c r="I107" t="s">
-        <v>455</v>
+        <v>171</v>
       </c>
       <c r="J107" t="s">
-        <v>418</v>
-      </c>
-      <c r="K107" s="10">
+        <v>490</v>
+      </c>
+      <c r="K107">
         <v>1</v>
       </c>
       <c r="L107" t="s">
-        <v>387</v>
+        <v>492</v>
       </c>
     </row>
     <row r="108" spans="2:12" x14ac:dyDescent="0.25">
@@ -5372,290 +5385,305 @@
         <v>95</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>461</v>
+        <v>500</v>
       </c>
       <c r="I108" t="s">
-        <v>455</v>
+        <v>171</v>
       </c>
       <c r="J108" t="s">
-        <v>462</v>
-      </c>
-      <c r="K108" s="10">
+        <v>491</v>
+      </c>
+      <c r="K108">
         <v>1</v>
       </c>
       <c r="L108" t="s">
-        <v>387</v>
+        <v>492</v>
       </c>
     </row>
     <row r="109" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D109" s="5" t="s">
-        <v>96</v>
+      <c r="B109" t="s">
+        <v>460</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="I109" t="s">
         <v>455</v>
       </c>
       <c r="J109" t="s">
-        <v>426</v>
-      </c>
-      <c r="K109">
-        <v>44</v>
+        <v>425</v>
+      </c>
+      <c r="K109" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D110" s="5" t="s">
-        <v>96</v>
+      <c r="D110" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>417</v>
+        <v>519</v>
+      </c>
+      <c r="H110">
+        <v>1</v>
       </c>
       <c r="I110" t="s">
         <v>455</v>
       </c>
       <c r="J110" t="s">
-        <v>196</v>
-      </c>
-      <c r="K110">
-        <v>36</v>
+        <v>419</v>
+      </c>
+      <c r="K110" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D111" s="5" t="s">
-        <v>96</v>
+      <c r="D111" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I111" t="s">
         <v>455</v>
       </c>
       <c r="J111" t="s">
-        <v>416</v>
-      </c>
-      <c r="K111">
-        <v>33</v>
+        <v>418</v>
+      </c>
+      <c r="K111" s="10">
+        <v>1</v>
       </c>
       <c r="L111" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="112" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D112" s="5" t="s">
-        <v>96</v>
+      <c r="D112" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>453</v>
+        <v>461</v>
       </c>
       <c r="I112" t="s">
         <v>455</v>
       </c>
       <c r="J112" t="s">
-        <v>454</v>
-      </c>
-      <c r="K112">
-        <v>31</v>
+        <v>462</v>
+      </c>
+      <c r="K112" s="10">
+        <v>1</v>
       </c>
       <c r="L112" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="113" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
-        <v>175</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F113" s="9" t="s">
-        <v>176</v>
+      <c r="D113" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>424</v>
       </c>
       <c r="I113" t="s">
-        <v>456</v>
-      </c>
-      <c r="J113" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="K113" s="10">
-        <v>1</v>
+        <v>455</v>
+      </c>
+      <c r="J113" t="s">
+        <v>426</v>
+      </c>
+      <c r="K113">
+        <v>44</v>
       </c>
     </row>
     <row r="114" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
-        <v>245</v>
-      </c>
-      <c r="D114" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F114" s="9" t="s">
-        <v>177</v>
+      <c r="D114" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>417</v>
       </c>
       <c r="I114" t="s">
-        <v>456</v>
-      </c>
-      <c r="J114" s="10" t="s">
-        <v>331</v>
-      </c>
-      <c r="K114" s="10">
-        <v>1</v>
+        <v>455</v>
+      </c>
+      <c r="J114" t="s">
+        <v>196</v>
+      </c>
+      <c r="K114">
+        <v>36</v>
       </c>
     </row>
     <row r="115" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
-        <v>247</v>
-      </c>
-      <c r="D115" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F115" s="9" t="s">
-        <v>186</v>
+      <c r="D115" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>415</v>
       </c>
       <c r="I115" t="s">
-        <v>456</v>
-      </c>
-      <c r="J115" s="10" t="s">
-        <v>332</v>
-      </c>
-      <c r="K115" s="10">
-        <v>1</v>
+        <v>455</v>
+      </c>
+      <c r="J115" t="s">
+        <v>416</v>
+      </c>
+      <c r="K115">
+        <v>33</v>
       </c>
       <c r="L115" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="116" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B116" t="s">
-        <v>246</v>
-      </c>
-      <c r="D116" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F116" s="9" t="s">
-        <v>212</v>
+      <c r="D116" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="H116">
+        <v>1</v>
       </c>
       <c r="I116" t="s">
-        <v>456</v>
-      </c>
-      <c r="J116" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="K116" s="10">
-        <v>1</v>
+        <v>455</v>
+      </c>
+      <c r="J116" t="s">
+        <v>454</v>
+      </c>
+      <c r="K116">
+        <v>31</v>
       </c>
       <c r="L116" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="117" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>175</v>
+      </c>
       <c r="D117" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F117" s="9" t="s">
-        <v>328</v>
+        <v>176</v>
       </c>
       <c r="I117" t="s">
         <v>456</v>
       </c>
       <c r="J117" s="10" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="K117" s="10">
         <v>1</v>
-      </c>
-      <c r="L117" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="118" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D118" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F118" s="9" t="s">
-        <v>240</v>
+        <v>177</v>
       </c>
       <c r="I118" t="s">
         <v>456</v>
       </c>
       <c r="J118" s="10" t="s">
-        <v>241</v>
+        <v>331</v>
       </c>
       <c r="K118" s="10">
         <v>1</v>
       </c>
-      <c r="L118" t="s">
-        <v>387</v>
-      </c>
     </row>
     <row r="119" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D119" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F119" s="2" t="s">
-        <v>178</v>
+      <c r="B119" t="s">
+        <v>247</v>
+      </c>
+      <c r="D119" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F119" s="9" t="s">
+        <v>186</v>
       </c>
       <c r="I119" t="s">
         <v>456</v>
       </c>
-      <c r="J119" t="s">
-        <v>208</v>
-      </c>
-      <c r="K119">
-        <v>64</v>
+      <c r="J119" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="K119" s="10">
+        <v>1</v>
+      </c>
+      <c r="L119" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="120" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D120" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>179</v>
+      <c r="B120" t="s">
+        <v>246</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F120" s="9" t="s">
+        <v>212</v>
       </c>
       <c r="I120" t="s">
         <v>456</v>
       </c>
-      <c r="J120" t="s">
-        <v>209</v>
-      </c>
-      <c r="K120">
-        <v>65</v>
+      <c r="J120" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="K120" s="10">
+        <v>1</v>
+      </c>
+      <c r="L120" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="121" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D121" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>466</v>
+      <c r="D121" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F121" s="9" t="s">
+        <v>328</v>
       </c>
       <c r="I121" t="s">
         <v>456</v>
       </c>
-      <c r="J121" t="s">
-        <v>214</v>
-      </c>
-      <c r="K121">
-        <v>66</v>
+      <c r="J121" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="K121" s="10">
+        <v>1</v>
+      </c>
+      <c r="L121" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="122" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D122" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F122" s="2" t="s">
-        <v>187</v>
+      <c r="B122" t="s">
+        <v>244</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F122" s="9" t="s">
+        <v>240</v>
       </c>
       <c r="I122" t="s">
         <v>456</v>
       </c>
-      <c r="J122" t="s">
-        <v>210</v>
-      </c>
-      <c r="K122">
-        <v>68</v>
+      <c r="J122" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="K122" s="10">
+        <v>1</v>
+      </c>
+      <c r="L122" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="123" spans="2:12" x14ac:dyDescent="0.25">
@@ -5663,16 +5691,16 @@
         <v>96</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>227</v>
+        <v>178</v>
       </c>
       <c r="I123" t="s">
         <v>456</v>
       </c>
       <c r="J123" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="K123">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="124" spans="2:12" x14ac:dyDescent="0.25">
@@ -5680,19 +5708,16 @@
         <v>96</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>544</v>
+        <v>179</v>
       </c>
       <c r="I124" t="s">
         <v>456</v>
       </c>
       <c r="J124" t="s">
-        <v>538</v>
+        <v>209</v>
       </c>
       <c r="K124">
-        <v>69</v>
-      </c>
-      <c r="L124" t="s">
-        <v>387</v>
+        <v>65</v>
       </c>
     </row>
     <row r="125" spans="2:12" x14ac:dyDescent="0.25">
@@ -5700,19 +5725,16 @@
         <v>96</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>188</v>
+        <v>466</v>
       </c>
       <c r="I125" t="s">
         <v>456</v>
       </c>
       <c r="J125" t="s">
-        <v>335</v>
+        <v>214</v>
       </c>
       <c r="K125">
-        <v>63</v>
-      </c>
-      <c r="L125" t="s">
-        <v>387</v>
+        <v>66</v>
       </c>
     </row>
     <row r="126" spans="2:12" x14ac:dyDescent="0.25">
@@ -5720,19 +5742,16 @@
         <v>96</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>334</v>
+        <v>187</v>
       </c>
       <c r="I126" t="s">
         <v>456</v>
       </c>
       <c r="J126" t="s">
-        <v>336</v>
+        <v>210</v>
       </c>
       <c r="K126">
-        <v>62</v>
-      </c>
-      <c r="L126" t="s">
-        <v>387</v>
+        <v>68</v>
       </c>
     </row>
     <row r="127" spans="2:12" x14ac:dyDescent="0.25">
@@ -5740,36 +5759,36 @@
         <v>96</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="I127" t="s">
         <v>456</v>
       </c>
       <c r="J127" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="K127">
-        <v>61</v>
-      </c>
-      <c r="L127" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="128" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D128" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="I128" t="s">
+        <v>456</v>
+      </c>
+      <c r="J128" t="s">
+        <v>538</v>
+      </c>
+      <c r="K128">
+        <v>69</v>
+      </c>
+      <c r="L128" t="s">
         <v>387</v>
-      </c>
-    </row>
-    <row r="128" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D128" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="I128" t="s">
-        <v>457</v>
-      </c>
-      <c r="J128" t="s">
-        <v>371</v>
-      </c>
-      <c r="K128" s="10">
-        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
@@ -5777,16 +5796,19 @@
         <v>96</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>369</v>
+        <v>188</v>
       </c>
       <c r="I129" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J129" t="s">
-        <v>372</v>
+        <v>335</v>
       </c>
       <c r="K129">
-        <v>71</v>
+        <v>63</v>
+      </c>
+      <c r="L129" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
@@ -5794,76 +5816,73 @@
         <v>96</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>467</v>
+        <v>334</v>
       </c>
       <c r="I130" t="s">
+        <v>456</v>
+      </c>
+      <c r="J130" t="s">
+        <v>336</v>
+      </c>
+      <c r="K130">
+        <v>62</v>
+      </c>
+      <c r="L130" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D131" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="I131" t="s">
+        <v>456</v>
+      </c>
+      <c r="J131" t="s">
+        <v>243</v>
+      </c>
+      <c r="K131">
+        <v>61</v>
+      </c>
+      <c r="L131" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D132" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="I132" t="s">
         <v>457</v>
       </c>
-      <c r="J130" t="s">
-        <v>373</v>
-      </c>
-      <c r="K130">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D131" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F131" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="I131" t="s">
-        <v>458</v>
-      </c>
-      <c r="J131" t="s">
-        <v>294</v>
-      </c>
-      <c r="K131" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D132" s="5" t="s">
+      <c r="J132" t="s">
+        <v>371</v>
+      </c>
+      <c r="K132" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D133" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F132" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="I132" t="s">
-        <v>458</v>
-      </c>
-      <c r="J132" t="s">
-        <v>222</v>
-      </c>
-      <c r="K132">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A133">
-        <v>17</v>
-      </c>
-      <c r="B133" t="s">
-        <v>136</v>
-      </c>
-      <c r="D133" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F133" s="9" t="s">
-        <v>515</v>
+      <c r="F133" s="2" t="s">
+        <v>369</v>
       </c>
       <c r="I133" t="s">
-        <v>482</v>
-      </c>
-      <c r="J133" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="K133" s="10">
-        <v>1</v>
-      </c>
-      <c r="L133" t="s">
-        <v>387</v>
+        <v>457</v>
+      </c>
+      <c r="J133" t="s">
+        <v>372</v>
+      </c>
+      <c r="K133">
+        <v>71</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.25">
@@ -5871,78 +5890,155 @@
         <v>96</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>481</v>
+        <v>467</v>
       </c>
       <c r="I134" t="s">
-        <v>482</v>
+        <v>457</v>
       </c>
       <c r="J134" t="s">
-        <v>345</v>
+        <v>373</v>
       </c>
       <c r="K134">
-        <v>51</v>
-      </c>
-      <c r="L134" t="s">
-        <v>387</v>
+        <v>72</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B135" t="s">
-        <v>287</v>
-      </c>
       <c r="D135" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F135" s="9" t="s">
+      <c r="F135" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="I135" t="s">
+        <v>458</v>
+      </c>
+      <c r="J135" t="s">
+        <v>294</v>
+      </c>
+      <c r="K135" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D136" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="I136" t="s">
+        <v>458</v>
+      </c>
+      <c r="J136" t="s">
+        <v>222</v>
+      </c>
+      <c r="K136">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>17</v>
+      </c>
+      <c r="B137" t="s">
+        <v>136</v>
+      </c>
+      <c r="D137" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F137" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="I137" t="s">
+        <v>482</v>
+      </c>
+      <c r="J137" s="10" t="s">
+        <v>483</v>
+      </c>
+      <c r="K137" s="10">
+        <v>1</v>
+      </c>
+      <c r="L137" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D138" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="I138" t="s">
+        <v>482</v>
+      </c>
+      <c r="J138" t="s">
+        <v>345</v>
+      </c>
+      <c r="K138">
+        <v>51</v>
+      </c>
+      <c r="L138" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>287</v>
+      </c>
+      <c r="D139" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F139" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="I135" t="s">
+      <c r="I139" t="s">
         <v>459</v>
       </c>
-      <c r="J135" t="s">
+      <c r="J139" t="s">
         <v>291</v>
       </c>
-      <c r="K135" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D136" s="6" t="s">
+      <c r="K139" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D140" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F136" s="2" t="s">
+      <c r="F140" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="I136" t="s">
+      <c r="I140" t="s">
         <v>459</v>
       </c>
-      <c r="J136" t="s">
+      <c r="J140" t="s">
         <v>292</v>
       </c>
-      <c r="K136" s="10">
-        <v>1</v>
-      </c>
-      <c r="L136" t="s">
+      <c r="K140" s="10">
+        <v>1</v>
+      </c>
+      <c r="L140" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D137" s="5" t="s">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D141" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F137" s="2" t="s">
+      <c r="F141" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="I137" t="s">
+      <c r="I141" t="s">
         <v>459</v>
       </c>
-      <c r="J137" t="s">
+      <c r="J141" t="s">
         <v>290</v>
       </c>
-      <c r="K137">
+      <c r="K141">
         <v>46</v>
       </c>
-      <c r="L137" t="s">
+      <c r="L141" t="s">
         <v>387</v>
       </c>
     </row>

</xml_diff>

<commit_message>
switch_pairs npiv devices connected approach changed
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="47925" windowHeight="17235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="572">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1618,9 +1618,6 @@
     <t>MTS_msk</t>
   </si>
   <si>
-    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\NOV21\ssave_msk</t>
-  </si>
-  <si>
     <t>MTS_spb</t>
   </si>
   <si>
@@ -1675,9 +1672,6 @@
     <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\01.CUSTOMERS\MTS\SAN Assessment\JAN2022\mts_msc</t>
   </si>
   <si>
-    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\JAN22\mts_msc\ssave</t>
-  </si>
-  <si>
     <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\NOV21\ssave_spb\10_12_2021</t>
   </si>
   <si>
@@ -1736,6 +1730,12 @@
   </si>
   <si>
     <t>fcredge_upd</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\JAN22\mts_msc\ssave_2</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\JAN22\mts_msc\blades</t>
   </si>
 </sst>
 </file>
@@ -2160,8 +2160,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AZ15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2169,7 +2169,7 @@
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="70" customWidth="1"/>
     <col min="3" max="3" width="109.42578125" customWidth="1"/>
-    <col min="4" max="4" width="70" customWidth="1"/>
+    <col min="4" max="4" width="116.7109375" customWidth="1"/>
     <col min="5" max="5" width="128.5703125" customWidth="1"/>
     <col min="6" max="6" width="99.85546875" customWidth="1"/>
     <col min="7" max="7" width="126.5703125" customWidth="1"/>
@@ -2218,7 +2218,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2227,19 +2227,19 @@
         <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D2" t="s">
         <v>531</v>
       </c>
       <c r="E2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="G2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="H2" t="s">
         <v>531</v>
@@ -2484,7 +2484,7 @@
         <v>474</v>
       </c>
       <c r="C4" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D4" t="s">
         <v>315</v>
@@ -2586,19 +2586,19 @@
         <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D5" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F5" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="H5" t="s">
         <v>530</v>
@@ -2640,7 +2640,7 @@
         <v>390</v>
       </c>
       <c r="U5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="V5" t="s">
         <v>384</v>
@@ -2741,22 +2741,22 @@
         <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D6" t="s">
-        <v>551</v>
+        <v>570</v>
       </c>
       <c r="E6" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F6" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G6" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="H6" t="s">
-        <v>532</v>
+        <v>570</v>
       </c>
       <c r="I6" t="s">
         <v>526</v>
@@ -2795,7 +2795,7 @@
         <v>391</v>
       </c>
       <c r="U6" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="V6" t="s">
         <v>383</v>
@@ -2895,14 +2895,20 @@
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
+      <c r="D7" t="s">
+        <v>571</v>
+      </c>
       <c r="E7" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G7" t="s">
-        <v>549</v>
+        <v>548</v>
+      </c>
+      <c r="H7" t="s">
+        <v>571</v>
       </c>
       <c r="I7" t="s">
         <v>522</v>
@@ -2926,7 +2932,7 @@
         <v>413</v>
       </c>
       <c r="U7" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="W7" t="s">
         <v>377</v>
@@ -2987,7 +2993,7 @@
         <v>346</v>
       </c>
       <c r="U9" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="W9" t="s">
         <v>378</v>
@@ -3040,9 +3046,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4433,13 +4439,13 @@
         <v>95</v>
       </c>
       <c r="F57" s="9" t="s">
+        <v>563</v>
+      </c>
+      <c r="I57" t="s">
         <v>565</v>
       </c>
-      <c r="I57" t="s">
-        <v>567</v>
-      </c>
       <c r="J57" s="10" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="K57" s="10">
         <v>1</v>
@@ -4650,13 +4656,13 @@
         <v>95</v>
       </c>
       <c r="F69" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="I69" t="s">
+        <v>567</v>
+      </c>
+      <c r="J69" t="s">
         <v>568</v>
-      </c>
-      <c r="I69" t="s">
-        <v>569</v>
-      </c>
-      <c r="J69" t="s">
-        <v>570</v>
       </c>
       <c r="K69" s="10">
         <v>1</v>
@@ -4667,7 +4673,7 @@
         <v>95</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="I70" s="10" t="s">
         <v>211</v>
@@ -4740,9 +4746,6 @@
       <c r="F74" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="H74">
-        <v>1</v>
-      </c>
       <c r="I74" t="s">
         <v>169</v>
       </c>
@@ -5097,19 +5100,22 @@
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D93" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>557</v>
+        <v>555</v>
+      </c>
+      <c r="H93">
+        <v>1</v>
       </c>
       <c r="I93" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="J93" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="K93">
         <v>1</v>
@@ -5120,13 +5126,13 @@
         <v>95</v>
       </c>
       <c r="F94" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="I94" t="s">
         <v>558</v>
       </c>
-      <c r="I94" t="s">
+      <c r="J94" t="s">
         <v>560</v>
-      </c>
-      <c r="J94" t="s">
-        <v>562</v>
       </c>
       <c r="K94">
         <v>1</v>
@@ -5137,13 +5143,13 @@
         <v>238</v>
       </c>
       <c r="F95" s="11" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="I95" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="J95" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="K95">
         <v>1</v>
@@ -5427,9 +5433,6 @@
       <c r="F110" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="H110">
-        <v>1</v>
-      </c>
       <c r="I110" t="s">
         <v>455</v>
       </c>
@@ -5541,9 +5544,6 @@
       <c r="F116" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="H116">
-        <v>1</v>
-      </c>
       <c r="I116" t="s">
         <v>455</v>
       </c>
@@ -5776,13 +5776,13 @@
         <v>96</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I128" t="s">
         <v>456</v>
       </c>
       <c r="J128" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="K128">
         <v>69</v>

</xml_diff>

<commit_message>
fcr collection regex patterns change
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="575">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1729,13 +1729,22 @@
     <t>ISL with switch pairs ID</t>
   </si>
   <si>
-    <t>fcredge_upd</t>
-  </si>
-  <si>
     <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\JAN22\mts_msc\ssave_2</t>
   </si>
   <si>
     <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\MTS\JAN22\mts_msc\blades</t>
+  </si>
+  <si>
+    <t>fcredge_aggregated</t>
+  </si>
+  <si>
+    <t>fcredge_aggregated_upd</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\01.CUSTOMERS\IBS\SAN FEB22</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\IBS\FEB22\ssave</t>
   </si>
 </sst>
 </file>
@@ -2158,157 +2167,157 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AZ15"/>
+  <dimension ref="A1:BA15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="70" customWidth="1"/>
-    <col min="3" max="3" width="109.42578125" customWidth="1"/>
-    <col min="4" max="4" width="116.7109375" customWidth="1"/>
-    <col min="5" max="5" width="128.5703125" customWidth="1"/>
-    <col min="6" max="6" width="99.85546875" customWidth="1"/>
-    <col min="7" max="7" width="126.5703125" customWidth="1"/>
-    <col min="8" max="8" width="151.28515625" customWidth="1"/>
-    <col min="9" max="9" width="120.42578125" customWidth="1"/>
-    <col min="10" max="10" width="112.42578125" customWidth="1"/>
-    <col min="11" max="11" width="158.5703125" customWidth="1"/>
-    <col min="12" max="12" width="103.7109375" customWidth="1"/>
-    <col min="13" max="13" width="91.85546875" customWidth="1"/>
-    <col min="14" max="14" width="70" customWidth="1"/>
-    <col min="15" max="15" width="124.42578125" customWidth="1"/>
-    <col min="16" max="16" width="103.85546875" customWidth="1"/>
-    <col min="17" max="17" width="48.85546875" customWidth="1"/>
-    <col min="18" max="18" width="29.7109375" customWidth="1"/>
-    <col min="19" max="19" width="80.140625" customWidth="1"/>
-    <col min="20" max="20" width="35.7109375" customWidth="1"/>
-    <col min="21" max="22" width="122.7109375" customWidth="1"/>
-    <col min="23" max="23" width="48.42578125" customWidth="1"/>
-    <col min="24" max="24" width="29.7109375" customWidth="1"/>
-    <col min="25" max="25" width="80.140625" customWidth="1"/>
-    <col min="26" max="26" width="68.5703125" customWidth="1"/>
-    <col min="27" max="27" width="48.7109375" customWidth="1"/>
-    <col min="28" max="28" width="62" customWidth="1"/>
-    <col min="29" max="31" width="89.5703125" customWidth="1"/>
-    <col min="32" max="32" width="69.85546875" customWidth="1"/>
-    <col min="33" max="33" width="52.140625" customWidth="1"/>
-    <col min="34" max="34" width="73.140625" customWidth="1"/>
-    <col min="35" max="35" width="29.7109375" customWidth="1"/>
-    <col min="36" max="37" width="76" customWidth="1"/>
-    <col min="38" max="38" width="72.28515625" customWidth="1"/>
-    <col min="39" max="39" width="61.7109375" customWidth="1"/>
-    <col min="40" max="40" width="60" customWidth="1"/>
-    <col min="41" max="41" width="38.140625" customWidth="1"/>
-    <col min="42" max="42" width="69" customWidth="1"/>
-    <col min="43" max="43" width="72.42578125" customWidth="1"/>
-    <col min="44" max="44" width="111.5703125" customWidth="1"/>
-    <col min="45" max="45" width="72.5703125" customWidth="1"/>
-    <col min="46" max="46" width="86.85546875" customWidth="1"/>
-    <col min="47" max="48" width="64.7109375" customWidth="1"/>
-    <col min="49" max="49" width="54.5703125" customWidth="1"/>
-    <col min="50" max="50" width="75.42578125" customWidth="1"/>
-    <col min="51" max="51" width="58.140625" customWidth="1"/>
+    <col min="2" max="3" width="70" customWidth="1"/>
+    <col min="4" max="4" width="109.42578125" customWidth="1"/>
+    <col min="5" max="5" width="116.7109375" customWidth="1"/>
+    <col min="6" max="6" width="128.5703125" customWidth="1"/>
+    <col min="7" max="7" width="99.85546875" customWidth="1"/>
+    <col min="8" max="8" width="126.5703125" customWidth="1"/>
+    <col min="9" max="9" width="151.28515625" customWidth="1"/>
+    <col min="10" max="10" width="120.42578125" customWidth="1"/>
+    <col min="11" max="11" width="112.42578125" customWidth="1"/>
+    <col min="12" max="12" width="158.5703125" customWidth="1"/>
+    <col min="13" max="13" width="103.7109375" customWidth="1"/>
+    <col min="14" max="14" width="91.85546875" customWidth="1"/>
+    <col min="15" max="15" width="70" customWidth="1"/>
+    <col min="16" max="16" width="124.42578125" customWidth="1"/>
+    <col min="17" max="17" width="103.85546875" customWidth="1"/>
+    <col min="18" max="18" width="48.85546875" customWidth="1"/>
+    <col min="19" max="19" width="29.7109375" customWidth="1"/>
+    <col min="20" max="20" width="80.140625" customWidth="1"/>
+    <col min="21" max="21" width="35.7109375" customWidth="1"/>
+    <col min="22" max="23" width="122.7109375" customWidth="1"/>
+    <col min="24" max="24" width="48.42578125" customWidth="1"/>
+    <col min="25" max="25" width="29.7109375" customWidth="1"/>
+    <col min="26" max="26" width="80.140625" customWidth="1"/>
+    <col min="27" max="27" width="68.5703125" customWidth="1"/>
+    <col min="28" max="28" width="48.7109375" customWidth="1"/>
+    <col min="29" max="29" width="62" customWidth="1"/>
+    <col min="30" max="32" width="89.5703125" customWidth="1"/>
+    <col min="33" max="33" width="69.85546875" customWidth="1"/>
+    <col min="34" max="34" width="52.140625" customWidth="1"/>
+    <col min="35" max="35" width="73.140625" customWidth="1"/>
+    <col min="36" max="36" width="29.7109375" customWidth="1"/>
+    <col min="37" max="38" width="76" customWidth="1"/>
+    <col min="39" max="39" width="72.28515625" customWidth="1"/>
+    <col min="40" max="40" width="61.7109375" customWidth="1"/>
+    <col min="41" max="41" width="60" customWidth="1"/>
+    <col min="42" max="42" width="38.140625" customWidth="1"/>
+    <col min="43" max="43" width="69" customWidth="1"/>
+    <col min="44" max="44" width="72.42578125" customWidth="1"/>
+    <col min="45" max="45" width="111.5703125" customWidth="1"/>
+    <col min="46" max="46" width="72.5703125" customWidth="1"/>
+    <col min="47" max="47" width="86.85546875" customWidth="1"/>
+    <col min="48" max="49" width="64.7109375" customWidth="1"/>
+    <col min="50" max="50" width="54.5703125" customWidth="1"/>
+    <col min="51" max="51" width="75.42578125" customWidth="1"/>
+    <col min="52" max="52" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D2" t="s">
         <v>551</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>531</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>539</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>534</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>532</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>531</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>524</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>520</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>382</v>
-      </c>
-      <c r="L2" t="s">
-        <v>502</v>
       </c>
       <c r="M2" t="s">
         <v>502</v>
       </c>
       <c r="N2" t="s">
-        <v>410</v>
+        <v>502</v>
       </c>
       <c r="O2" t="s">
         <v>410</v>
       </c>
       <c r="P2" t="s">
+        <v>410</v>
+      </c>
+      <c r="Q2" t="s">
         <v>444</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>431</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>410</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>230</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>388</v>
-      </c>
-      <c r="U2" t="s">
-        <v>382</v>
       </c>
       <c r="V2" t="s">
         <v>382</v>
       </c>
       <c r="W2" t="s">
+        <v>382</v>
+      </c>
+      <c r="X2" t="s">
         <v>374</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>354</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>322</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>312</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>305</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>302</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>298</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>306</v>
       </c>
       <c r="AE2" t="s">
         <v>306</v>
@@ -2317,169 +2326,175 @@
         <v>306</v>
       </c>
       <c r="AG2" t="s">
+        <v>306</v>
+      </c>
+      <c r="AH2" t="s">
         <v>269</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>265</v>
       </c>
       <c r="AI2" t="s">
         <v>265</v>
       </c>
       <c r="AJ2" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="AK2" t="s">
         <v>248</v>
       </c>
       <c r="AL2" t="s">
+        <v>248</v>
+      </c>
+      <c r="AM2" t="s">
         <v>230</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>226</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>185</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>184</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>154</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>110</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>97</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>83</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>273</v>
       </c>
       <c r="C3" s="12">
+        <v>44608</v>
+      </c>
+      <c r="D3" s="12">
         <v>44592</v>
       </c>
-      <c r="D3" s="12">
+      <c r="E3" s="12">
         <v>44575</v>
       </c>
-      <c r="E3" s="12">
+      <c r="F3" s="12">
         <v>44537</v>
       </c>
-      <c r="F3" s="12">
+      <c r="G3" s="12">
         <v>44531</v>
       </c>
-      <c r="G3" s="12">
+      <c r="H3" s="12">
         <v>44530</v>
       </c>
-      <c r="H3" s="12">
+      <c r="I3" s="12">
         <v>44529</v>
       </c>
-      <c r="I3" s="12">
+      <c r="J3" s="12">
         <v>44524</v>
       </c>
-      <c r="J3" s="12">
+      <c r="K3" s="12">
         <v>44503</v>
       </c>
-      <c r="K3" s="12">
+      <c r="L3" s="12">
         <v>44343</v>
-      </c>
-      <c r="L3" s="12">
-        <v>44484</v>
       </c>
       <c r="M3" s="12">
         <v>44484</v>
       </c>
       <c r="N3" s="12">
+        <v>44484</v>
+      </c>
+      <c r="O3" s="12">
         <v>44473</v>
       </c>
-      <c r="O3" s="12">
+      <c r="P3" s="12">
         <v>44469</v>
       </c>
-      <c r="P3" s="12">
+      <c r="Q3" s="12">
         <v>44453</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="R3" s="12">
         <v>44426</v>
       </c>
-      <c r="R3" s="12">
+      <c r="S3" s="12">
         <v>44330</v>
       </c>
-      <c r="S3" s="12">
+      <c r="T3" s="12">
         <v>44307</v>
       </c>
-      <c r="T3" s="12">
+      <c r="U3" s="12">
         <v>44294</v>
       </c>
-      <c r="U3" s="12">
+      <c r="V3" s="12">
         <v>44343</v>
       </c>
-      <c r="V3" s="12">
+      <c r="W3" s="12">
         <v>44292</v>
       </c>
-      <c r="W3" s="12">
+      <c r="X3" s="12">
         <v>29681</v>
       </c>
-      <c r="X3" s="12">
+      <c r="Y3" s="12">
         <v>44286</v>
       </c>
-      <c r="Y3" s="12">
+      <c r="Z3" s="12">
         <v>44260</v>
       </c>
-      <c r="Z3" s="12">
+      <c r="AA3" s="12">
         <v>44244</v>
       </c>
-      <c r="AA3" s="12">
+      <c r="AB3" s="12">
         <v>44245</v>
       </c>
-      <c r="AB3" s="12">
+      <c r="AC3" s="12">
         <v>44223</v>
       </c>
-      <c r="AC3" s="12">
+      <c r="AD3" s="12">
         <v>44209</v>
       </c>
-      <c r="AD3" s="12">
+      <c r="AE3" s="12">
         <v>44253</v>
       </c>
-      <c r="AE3" s="12">
+      <c r="AF3" s="12">
         <v>44237</v>
       </c>
-      <c r="AH3" s="12">
+      <c r="AI3" s="12">
         <v>44181</v>
       </c>
-      <c r="AT3" s="1"/>
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
       <c r="AY3" s="1"/>
       <c r="AZ3" s="1"/>
-    </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="BA3" s="1"/>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>474</v>
       </c>
@@ -2487,7 +2502,7 @@
         <v>552</v>
       </c>
       <c r="D4" t="s">
-        <v>315</v>
+        <v>552</v>
       </c>
       <c r="E4" t="s">
         <v>315</v>
@@ -2508,22 +2523,22 @@
         <v>315</v>
       </c>
       <c r="K4" t="s">
+        <v>315</v>
+      </c>
+      <c r="L4" t="s">
         <v>517</v>
-      </c>
-      <c r="L4" t="s">
-        <v>503</v>
       </c>
       <c r="M4" t="s">
         <v>503</v>
       </c>
       <c r="N4" t="s">
-        <v>468</v>
+        <v>503</v>
       </c>
       <c r="O4" t="s">
         <v>468</v>
       </c>
       <c r="P4" t="s">
-        <v>315</v>
+        <v>468</v>
       </c>
       <c r="Q4" t="s">
         <v>315</v>
@@ -2532,13 +2547,13 @@
         <v>315</v>
       </c>
       <c r="S4" t="s">
+        <v>315</v>
+      </c>
+      <c r="T4" t="s">
         <v>401</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>389</v>
-      </c>
-      <c r="U4" t="s">
-        <v>315</v>
       </c>
       <c r="V4" t="s">
         <v>315</v>
@@ -2547,490 +2562,499 @@
         <v>315</v>
       </c>
       <c r="X4" t="s">
+        <v>315</v>
+      </c>
+      <c r="Y4" t="s">
         <v>355</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>315</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>311</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>315</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>315</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>319</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>311</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>272</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>271</v>
       </c>
-      <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
       <c r="AY4" s="1"/>
       <c r="AZ4" s="1"/>
-    </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="BA4" s="1"/>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
+        <v>573</v>
+      </c>
+      <c r="D5" t="s">
         <v>554</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>549</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>540</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>535</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>533</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>530</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>525</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>521</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>516</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>511</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>506</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>479</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>469</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>445</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>432</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>411</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>402</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>390</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>544</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>384</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>375</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>356</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>323</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>313</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>317</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>303</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>297</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>320</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>309</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>307</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>270</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>274</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>267</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>249</v>
       </c>
       <c r="AK5" t="s">
         <v>249</v>
       </c>
       <c r="AL5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AM5" t="s">
         <v>232</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AN5" t="s">
         <v>225</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>216</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AP5" t="s">
         <v>183</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AQ5" t="s">
         <v>156</v>
       </c>
-      <c r="AQ5" t="s">
+      <c r="AR5" t="s">
         <v>112</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="AS5" t="s">
         <v>98</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AT5" t="s">
         <v>85</v>
       </c>
-      <c r="AT5" t="s">
-        <v>1</v>
-      </c>
       <c r="AU5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV5" t="s">
         <v>74</v>
       </c>
-      <c r="AV5" t="s">
+      <c r="AW5" t="s">
         <v>72</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AX5" t="s">
         <v>4</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="AY5" t="s">
         <v>25</v>
       </c>
-      <c r="AY5" t="s">
+      <c r="AZ5" t="s">
         <v>60</v>
       </c>
-      <c r="AZ5" t="s">
+      <c r="BA5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C6" t="s">
+        <v>574</v>
+      </c>
+      <c r="D6" t="s">
         <v>553</v>
       </c>
-      <c r="D6" t="s">
-        <v>570</v>
-      </c>
       <c r="E6" t="s">
+        <v>569</v>
+      </c>
+      <c r="F6" t="s">
         <v>542</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>536</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>550</v>
       </c>
-      <c r="H6" t="s">
-        <v>570</v>
-      </c>
       <c r="I6" t="s">
+        <v>569</v>
+      </c>
+      <c r="J6" t="s">
         <v>526</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>523</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>518</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>512</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>504</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>480</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>470</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>446</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>433</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>412</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>403</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>391</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>545</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>383</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>376</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>357</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>344</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>314</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>316</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>304</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>299</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>321</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>310</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>308</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>268</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>275</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>266</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>261</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" t="s">
         <v>250</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AM6" t="s">
         <v>231</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>223</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>215</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AP6" t="s">
         <v>182</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AQ6" t="s">
         <v>155</v>
       </c>
-      <c r="AQ6" t="s">
+      <c r="AR6" t="s">
         <v>111</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AS6" t="s">
         <v>107</v>
       </c>
-      <c r="AS6" t="s">
+      <c r="AT6" t="s">
         <v>84</v>
       </c>
-      <c r="AT6" t="s">
+      <c r="AU6" t="s">
         <v>0</v>
       </c>
-      <c r="AU6" t="s">
+      <c r="AV6" t="s">
         <v>73</v>
       </c>
-      <c r="AV6" t="s">
+      <c r="AW6" t="s">
         <v>71</v>
       </c>
-      <c r="AW6" t="s">
+      <c r="AX6" t="s">
         <v>3</v>
       </c>
-      <c r="AX6" t="s">
+      <c r="AY6" t="s">
         <v>24</v>
       </c>
-      <c r="AY6" t="s">
+      <c r="AZ6" t="s">
         <v>59</v>
       </c>
-      <c r="AZ6" t="s">
+      <c r="BA6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D7" t="s">
-        <v>571</v>
-      </c>
       <c r="E7" t="s">
+        <v>570</v>
+      </c>
+      <c r="F7" t="s">
         <v>541</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>538</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>548</v>
       </c>
-      <c r="H7" t="s">
-        <v>571</v>
-      </c>
       <c r="I7" t="s">
-        <v>522</v>
+        <v>570</v>
       </c>
       <c r="J7" t="s">
         <v>522</v>
       </c>
-      <c r="L7" t="s">
+      <c r="K7" t="s">
+        <v>522</v>
+      </c>
+      <c r="M7" t="s">
         <v>513</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>505</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>471</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>434</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>413</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>546</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>377</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>324</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>300</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>251</v>
       </c>
       <c r="AK7" t="s">
         <v>251</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AL7" t="s">
+        <v>251</v>
+      </c>
+      <c r="AN7" t="s">
         <v>224</v>
       </c>
-      <c r="AP7" t="s">
+      <c r="AQ7" t="s">
         <v>157</v>
       </c>
-      <c r="AR7" t="s">
+      <c r="AS7" t="s">
         <v>108</v>
       </c>
-      <c r="AS7" t="s">
+      <c r="AT7" t="s">
         <v>87</v>
       </c>
-      <c r="AV7" t="s">
+      <c r="AW7" t="s">
         <v>99</v>
       </c>
-      <c r="AY7" t="s">
+      <c r="AZ7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>463</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>404</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>325</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>253</v>
       </c>
       <c r="AK8" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
+      <c r="AL8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>547</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>508</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>514</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>478</v>
       </c>
@@ -3047,8 +3071,8 @@
   <dimension ref="A1:L141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G116" sqref="G116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4639,7 +4663,7 @@
         <v>95</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>48</v>
+        <v>571</v>
       </c>
       <c r="I68" s="10" t="s">
         <v>211</v>
@@ -4673,7 +4697,7 @@
         <v>95</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="I70" s="10" t="s">
         <v>211</v>
@@ -5108,9 +5132,6 @@
       <c r="F93" s="9" t="s">
         <v>555</v>
       </c>
-      <c r="H93">
-        <v>1</v>
-      </c>
       <c r="I93" t="s">
         <v>558</v>
       </c>
@@ -5506,6 +5527,9 @@
       </c>
       <c r="F114" s="2" t="s">
         <v>417</v>
+      </c>
+      <c r="G114">
+        <v>1</v>
       </c>
       <c r="I114" t="s">
         <v>455</v>

</xml_diff>

<commit_message>
port stats counting correction
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="47925" windowHeight="17235" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -2169,8 +2169,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BA15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2227,7 +2227,7 @@
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3070,9 +3070,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G116" sqref="G116"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,6 +3782,9 @@
       <c r="F26" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
       <c r="I26" t="s">
         <v>142</v>
       </c>
@@ -5527,9 +5530,6 @@
       </c>
       <c r="F114" s="2" t="s">
         <v>417</v>
-      </c>
-      <c r="G114">
-        <v>1</v>
       </c>
       <c r="I114" t="s">
         <v>455</v>
@@ -6078,7 +6078,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="A2" sqref="A2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
bladesystem collection file refactoring
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -2170,7 +2170,7 @@
   <dimension ref="A1:BA15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3071,8 +3071,8 @@
   <dimension ref="A1:L141"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,9 +3782,6 @@
       <c r="F26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H26">
-        <v>1</v>
-      </c>
       <c r="I26" t="s">
         <v>142</v>
       </c>
@@ -4167,6 +4164,9 @@
       </c>
       <c r="F42" s="2" t="s">
         <v>89</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
       </c>
       <c r="I42" t="s">
         <v>450</v>

</xml_diff>

<commit_message>
security violations are added to raslog frequent messages table
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
@@ -2169,8 +2169,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BA15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3070,9 +3070,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L141"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H151" sqref="H151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4165,9 +4165,6 @@
       <c r="F42" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H42">
-        <v>1</v>
-      </c>
       <c r="I42" t="s">
         <v>450</v>
       </c>
@@ -6052,6 +6049,9 @@
       </c>
       <c r="F141" s="2" t="s">
         <v>289</v>
+      </c>
+      <c r="G141">
+        <v>1</v>
       </c>
       <c r="I141" t="s">
         <v>459</v>

</xml_diff>

<commit_message>
front and translate domain pairs
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -13,14 +13,14 @@
     <sheet name="software" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$L$141</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">service_tables!$A$1:$L$143</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="580">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1745,6 +1745,21 @@
   </si>
   <si>
     <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\IBS\FEB22\ssave</t>
+  </si>
+  <si>
+    <t>fcrxlateconfig</t>
+  </si>
+  <si>
+    <t>Translate (xlate) domain ID</t>
+  </si>
+  <si>
+    <t>fcr_xd_proxydev</t>
+  </si>
+  <si>
+    <t>Translate domain proxy devices</t>
+  </si>
+  <si>
+    <t>DATA ANALYSIS X. TRANSLATE DOMAIN (XD) PROXY DEVICES</t>
   </si>
 </sst>
 </file>
@@ -2170,7 +2185,7 @@
   <dimension ref="A1:BA15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3068,11 +3083,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:L141"/>
+  <dimension ref="A1:L143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H151" sqref="H151"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3917,32 +3932,32 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>13</v>
-      </c>
       <c r="B32" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>50</v>
+        <v>575</v>
       </c>
       <c r="I32" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>359</v>
+        <v>576</v>
       </c>
       <c r="K32" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>13</v>
+      </c>
       <c r="B33" s="4" t="s">
         <v>126</v>
       </c>
@@ -3953,13 +3968,13 @@
         <v>94</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I33" t="s">
         <v>148</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K33" s="10">
         <v>1</v>
@@ -3976,13 +3991,13 @@
         <v>94</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I34" t="s">
         <v>148</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K34" s="10">
         <v>1</v>
@@ -3999,13 +4014,13 @@
         <v>94</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I35" t="s">
         <v>148</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K35" s="10">
         <v>1</v>
@@ -4022,13 +4037,13 @@
         <v>94</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I36" t="s">
         <v>148</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K36" s="10">
         <v>1</v>
@@ -4045,13 +4060,13 @@
         <v>94</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>233</v>
+        <v>53</v>
       </c>
       <c r="I37" t="s">
         <v>148</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K37" s="10">
         <v>1</v>
@@ -4068,13 +4083,13 @@
         <v>94</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I38" t="s">
         <v>148</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K38" s="10">
         <v>1</v>
@@ -4082,22 +4097,22 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>217</v>
+        <v>126</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>218</v>
+        <v>125</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="I39" t="s">
-        <v>219</v>
+        <v>148</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="K39" s="10">
         <v>1</v>
@@ -4105,54 +4120,54 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>285</v>
+        <v>217</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>286</v>
+        <v>218</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>282</v>
+        <v>218</v>
       </c>
       <c r="I40" t="s">
-        <v>283</v>
+        <v>219</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>284</v>
+        <v>358</v>
       </c>
       <c r="K40" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>19</v>
-      </c>
       <c r="B41" s="4" t="s">
-        <v>114</v>
+        <v>285</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>130</v>
+        <v>286</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>88</v>
+        <v>282</v>
       </c>
       <c r="I41" t="s">
-        <v>450</v>
+        <v>283</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>381</v>
+        <v>284</v>
       </c>
       <c r="K41" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>19</v>
+      </c>
       <c r="B42" s="4" t="s">
         <v>114</v>
       </c>
@@ -4163,13 +4178,13 @@
         <v>94</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I42" t="s">
         <v>450</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="K42" s="10">
         <v>1</v>
@@ -4186,13 +4201,13 @@
         <v>94</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>153</v>
+        <v>89</v>
       </c>
       <c r="I43" t="s">
         <v>450</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="K43" s="10">
         <v>1</v>
@@ -4200,20 +4215,22 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="C44" s="4"/>
+        <v>114</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="D44" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>255</v>
+        <v>153</v>
       </c>
       <c r="I44" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>257</v>
+        <v>379</v>
       </c>
       <c r="K44" s="10">
         <v>1</v>
@@ -4228,13 +4245,13 @@
         <v>94</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I45" t="s">
         <v>451</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K45" s="10">
         <v>1</v>
@@ -4242,20 +4259,20 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
-        <v>349</v>
+        <v>254</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4" t="s">
         <v>94</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>352</v>
+        <v>256</v>
       </c>
       <c r="I46" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>353</v>
+        <v>258</v>
       </c>
       <c r="K46" s="10">
         <v>1</v>
@@ -4270,13 +4287,13 @@
         <v>94</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="I47" t="s">
         <v>452</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="K47" s="10">
         <v>1</v>
@@ -4291,13 +4308,13 @@
         <v>94</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I48" t="s">
         <v>452</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K48" s="10">
         <v>1</v>
@@ -4312,47 +4329,51 @@
         <v>94</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>386</v>
+        <v>348</v>
       </c>
       <c r="I49" t="s">
         <v>452</v>
       </c>
       <c r="J49" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="K49" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="I50" t="s">
+        <v>452</v>
+      </c>
+      <c r="J50" s="10" t="s">
         <v>385</v>
       </c>
-      <c r="K49" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="K50" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>15</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>137</v>
       </c>
-      <c r="D50" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I50" t="s">
-        <v>158</v>
-      </c>
-      <c r="J50" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="K50" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D51" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>422</v>
+        <v>55</v>
       </c>
       <c r="I51" t="s">
         <v>158</v>
@@ -4368,14 +4389,14 @@
       <c r="D52" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F52" s="8" t="s">
-        <v>56</v>
+      <c r="F52" s="9" t="s">
+        <v>422</v>
       </c>
       <c r="I52" t="s">
         <v>158</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>295</v>
+        <v>211</v>
       </c>
       <c r="K52" s="10">
         <v>1</v>
@@ -4386,90 +4407,90 @@
         <v>95</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I53" t="s">
         <v>158</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>211</v>
+        <v>295</v>
       </c>
       <c r="K53" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>161</v>
-      </c>
       <c r="D54" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F54" s="9" t="s">
+      <c r="F54" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I54" t="s">
+        <v>158</v>
+      </c>
+      <c r="J54" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="K54" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>161</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F55" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="I54" t="s">
-        <v>162</v>
-      </c>
-      <c r="J54" s="10" t="s">
-        <v>392</v>
-      </c>
-      <c r="K54" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D55" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="I55" t="s">
         <v>162</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J55" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="K55" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D56" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I56" t="s">
+        <v>162</v>
+      </c>
+      <c r="J56" t="s">
         <v>198</v>
       </c>
-      <c r="K55">
+      <c r="K56">
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>16</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>139</v>
       </c>
-      <c r="D56" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="I56" t="s">
-        <v>168</v>
-      </c>
-      <c r="J56" s="10" t="s">
-        <v>279</v>
-      </c>
-      <c r="K56" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D57" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>563</v>
+        <v>66</v>
       </c>
       <c r="I57" t="s">
-        <v>565</v>
+        <v>168</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>564</v>
+        <v>279</v>
       </c>
       <c r="K57" s="10">
         <v>1</v>
@@ -4479,55 +4500,55 @@
       <c r="D58" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E58" s="16"/>
-      <c r="F58" s="2" t="s">
-        <v>427</v>
+      <c r="F58" s="9" t="s">
+        <v>563</v>
       </c>
       <c r="I58" t="s">
-        <v>168</v>
+        <v>565</v>
       </c>
       <c r="J58" s="10" t="s">
-        <v>428</v>
+        <v>564</v>
       </c>
       <c r="K58" s="10">
         <v>1</v>
-      </c>
-      <c r="L58" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D59" s="6" t="s">
         <v>95</v>
       </c>
+      <c r="E59" s="16"/>
       <c r="F59" s="2" t="s">
-        <v>163</v>
+        <v>427</v>
       </c>
       <c r="I59" t="s">
         <v>168</v>
       </c>
       <c r="J59" s="10" t="s">
-        <v>211</v>
+        <v>428</v>
       </c>
       <c r="K59" s="10">
         <v>1</v>
       </c>
+      <c r="L59" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D60" s="5" t="s">
-        <v>96</v>
+      <c r="D60" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>61</v>
+        <v>163</v>
       </c>
       <c r="I60" t="s">
         <v>168</v>
       </c>
-      <c r="J60" t="s">
-        <v>190</v>
-      </c>
-      <c r="K60">
-        <v>12</v>
+      <c r="J60" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="K60" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -4535,16 +4556,16 @@
         <v>96</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I61" t="s">
         <v>168</v>
       </c>
       <c r="J61" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K61">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -4552,16 +4573,16 @@
         <v>96</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I62" t="s">
         <v>168</v>
       </c>
       <c r="J62" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="K62">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -4569,16 +4590,16 @@
         <v>96</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I63" t="s">
         <v>168</v>
       </c>
       <c r="J63" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K63">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
@@ -4586,16 +4607,16 @@
         <v>96</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I64" t="s">
         <v>168</v>
       </c>
       <c r="J64" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="K64">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -4603,16 +4624,16 @@
         <v>96</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>420</v>
+        <v>64</v>
       </c>
       <c r="I65" t="s">
         <v>168</v>
       </c>
       <c r="J65" t="s">
-        <v>421</v>
+        <v>192</v>
       </c>
       <c r="K65">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -4620,56 +4641,56 @@
         <v>96</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="I66" t="s">
         <v>168</v>
       </c>
       <c r="J66" t="s">
+        <v>421</v>
+      </c>
+      <c r="K66">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D67" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="I67" t="s">
+        <v>168</v>
+      </c>
+      <c r="J67" t="s">
         <v>429</v>
       </c>
-      <c r="K66">
+      <c r="K67">
         <v>11</v>
       </c>
-      <c r="L66" t="s">
+      <c r="L67" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68">
         <v>18</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>138</v>
       </c>
-      <c r="D67" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I67" t="s">
-        <v>169</v>
-      </c>
-      <c r="J67" t="s">
-        <v>278</v>
-      </c>
-      <c r="K67" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D68" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>571</v>
-      </c>
-      <c r="I68" s="10" t="s">
-        <v>211</v>
+        <v>69</v>
+      </c>
+      <c r="I68" t="s">
+        <v>169</v>
       </c>
       <c r="J68" t="s">
-        <v>48</v>
+        <v>278</v>
       </c>
       <c r="K68" s="10">
         <v>1</v>
@@ -4680,13 +4701,13 @@
         <v>95</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="I69" t="s">
-        <v>567</v>
+        <v>571</v>
+      </c>
+      <c r="I69" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="J69" t="s">
-        <v>568</v>
+        <v>48</v>
       </c>
       <c r="K69" s="10">
         <v>1</v>
@@ -4697,13 +4718,13 @@
         <v>95</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>572</v>
-      </c>
-      <c r="I70" s="10" t="s">
-        <v>211</v>
+        <v>566</v>
+      </c>
+      <c r="I70" t="s">
+        <v>567</v>
       </c>
       <c r="J70" t="s">
-        <v>48</v>
+        <v>568</v>
       </c>
       <c r="K70" s="10">
         <v>1</v>
@@ -4714,36 +4735,36 @@
         <v>95</v>
       </c>
       <c r="F71" s="9" t="s">
+        <v>572</v>
+      </c>
+      <c r="I71" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="J71" t="s">
+        <v>48</v>
+      </c>
+      <c r="K71" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D72" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F72" s="9" t="s">
         <v>276</v>
-      </c>
-      <c r="I71" t="s">
-        <v>169</v>
-      </c>
-      <c r="J71" t="s">
-        <v>277</v>
-      </c>
-      <c r="K71" s="10">
-        <v>1</v>
-      </c>
-      <c r="L71" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D72" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="I72" t="s">
         <v>169</v>
       </c>
       <c r="J72" t="s">
-        <v>201</v>
-      </c>
-      <c r="K72">
-        <v>35</v>
+        <v>277</v>
+      </c>
+      <c r="K72" s="10">
+        <v>1</v>
+      </c>
+      <c r="L72" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -4751,16 +4772,16 @@
         <v>96</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I73" t="s">
         <v>169</v>
       </c>
       <c r="J73" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K73">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -4768,62 +4789,59 @@
         <v>96</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>280</v>
+        <v>68</v>
       </c>
       <c r="I74" t="s">
         <v>169</v>
       </c>
       <c r="J74" t="s">
+        <v>202</v>
+      </c>
+      <c r="K74">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D75" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="I75" t="s">
+        <v>169</v>
+      </c>
+      <c r="J75" t="s">
         <v>281</v>
       </c>
-      <c r="K74">
+      <c r="K75">
         <v>32</v>
       </c>
-      <c r="L74" t="s">
+      <c r="L75" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A75">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76">
         <v>20</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>131</v>
       </c>
-      <c r="D75" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F75" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="I75" t="s">
-        <v>170</v>
-      </c>
-      <c r="J75" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="K75" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D76" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>409</v>
+        <v>90</v>
       </c>
       <c r="I76" t="s">
         <v>170</v>
       </c>
       <c r="J76" s="10" t="s">
-        <v>406</v>
+        <v>259</v>
       </c>
       <c r="K76" s="10">
         <v>1</v>
-      </c>
-      <c r="L76" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -4831,13 +4849,13 @@
         <v>95</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>262</v>
+        <v>409</v>
       </c>
       <c r="I77" t="s">
         <v>170</v>
       </c>
       <c r="J77" s="10" t="s">
-        <v>263</v>
+        <v>406</v>
       </c>
       <c r="K77" s="10">
         <v>1</v>
@@ -4850,17 +4868,20 @@
       <c r="D78" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F78" s="2" t="s">
-        <v>235</v>
+      <c r="F78" s="9" t="s">
+        <v>262</v>
       </c>
       <c r="I78" t="s">
         <v>170</v>
       </c>
       <c r="J78" s="10" t="s">
-        <v>327</v>
+        <v>263</v>
       </c>
       <c r="K78" s="10">
         <v>1</v>
+      </c>
+      <c r="L78" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -4868,24 +4889,24 @@
         <v>95</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I79" t="s">
         <v>170</v>
       </c>
       <c r="J79" s="10" t="s">
-        <v>237</v>
+        <v>327</v>
       </c>
       <c r="K79" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D80" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="F80" s="11" t="s">
-        <v>239</v>
+      <c r="D80" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="I80" t="s">
         <v>170</v>
@@ -4898,20 +4919,17 @@
       </c>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>133</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F81" s="8" t="s">
-        <v>109</v>
+      <c r="D81" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="F81" s="11" t="s">
+        <v>239</v>
       </c>
       <c r="I81" t="s">
         <v>170</v>
       </c>
       <c r="J81" s="10" t="s">
-        <v>368</v>
+        <v>237</v>
       </c>
       <c r="K81" s="10">
         <v>1</v>
@@ -4919,99 +4937,102 @@
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>119</v>
-      </c>
-      <c r="C82" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F82" s="7" t="s">
-        <v>93</v>
+      <c r="F82" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="I82" t="s">
         <v>170</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>326</v>
+        <v>368</v>
       </c>
       <c r="K82" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>119</v>
+      </c>
+      <c r="C83" t="s">
+        <v>132</v>
+      </c>
       <c r="D83" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>301</v>
+        <v>93</v>
       </c>
       <c r="I83" t="s">
         <v>170</v>
       </c>
       <c r="J83" s="10" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="K83" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>134</v>
-      </c>
-      <c r="D84" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>405</v>
+      <c r="D84" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>301</v>
       </c>
       <c r="I84" t="s">
         <v>170</v>
       </c>
-      <c r="J84" t="s">
-        <v>193</v>
-      </c>
-      <c r="K84">
-        <v>17</v>
+      <c r="J84" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="K84" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>101</v>
+        <v>405</v>
       </c>
       <c r="I85" t="s">
         <v>170</v>
       </c>
       <c r="J85" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K85">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>135</v>
+      </c>
       <c r="D86" s="5" t="s">
         <v>96</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I86" t="s">
         <v>170</v>
       </c>
       <c r="J86" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K86">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.25">
@@ -5019,16 +5040,16 @@
         <v>96</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I87" t="s">
         <v>170</v>
       </c>
       <c r="J87" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="K87">
-        <v>57</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.25">
@@ -5036,16 +5057,16 @@
         <v>96</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I88" t="s">
         <v>170</v>
       </c>
       <c r="J88" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K88">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.25">
@@ -5053,16 +5074,16 @@
         <v>96</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I89" t="s">
         <v>170</v>
       </c>
       <c r="J89" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K89">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="90" spans="2:12" x14ac:dyDescent="0.25">
@@ -5070,16 +5091,16 @@
         <v>96</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I90" t="s">
         <v>170</v>
       </c>
       <c r="J90" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K90">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.25">
@@ -5087,19 +5108,16 @@
         <v>96</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>408</v>
+        <v>106</v>
       </c>
       <c r="I91" t="s">
         <v>170</v>
       </c>
       <c r="J91" t="s">
-        <v>407</v>
+        <v>206</v>
       </c>
       <c r="K91">
-        <v>53</v>
-      </c>
-      <c r="L91" t="s">
-        <v>387</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" spans="2:12" x14ac:dyDescent="0.25">
@@ -5107,127 +5125,133 @@
         <v>96</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>264</v>
+        <v>408</v>
       </c>
       <c r="I92" t="s">
         <v>170</v>
       </c>
       <c r="J92" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="K92">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L92" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>557</v>
-      </c>
-      <c r="D93" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F93" s="9" t="s">
-        <v>555</v>
+      <c r="D93" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>264</v>
       </c>
       <c r="I93" t="s">
-        <v>558</v>
+        <v>170</v>
       </c>
       <c r="J93" t="s">
-        <v>559</v>
+        <v>400</v>
       </c>
       <c r="K93">
-        <v>1</v>
+        <v>52</v>
+      </c>
+      <c r="L93" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D94" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F94" s="9" t="s">
-        <v>556</v>
+      <c r="F94" s="2" t="s">
+        <v>577</v>
       </c>
       <c r="I94" t="s">
-        <v>558</v>
+        <v>579</v>
       </c>
       <c r="J94" t="s">
-        <v>560</v>
+        <v>578</v>
       </c>
       <c r="K94">
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D95" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="F95" s="11" t="s">
-        <v>561</v>
+      <c r="B95" t="s">
+        <v>557</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="H95">
+        <v>1</v>
       </c>
       <c r="I95" t="s">
         <v>558</v>
       </c>
       <c r="J95" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="K95">
         <v>1</v>
       </c>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B96" t="s">
-        <v>164</v>
-      </c>
       <c r="D96" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F96" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="I96" t="s">
+        <v>558</v>
+      </c>
+      <c r="J96" t="s">
+        <v>560</v>
+      </c>
+      <c r="K96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D97" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="F97" s="11" t="s">
+        <v>561</v>
+      </c>
+      <c r="I97" t="s">
+        <v>558</v>
+      </c>
+      <c r="J97" t="s">
+        <v>562</v>
+      </c>
+      <c r="K97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>164</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F98" s="9" t="s">
         <v>213</v>
-      </c>
-      <c r="I96" t="s">
-        <v>171</v>
-      </c>
-      <c r="J96" t="s">
-        <v>293</v>
-      </c>
-      <c r="K96" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D97" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="I97" t="s">
-        <v>171</v>
-      </c>
-      <c r="J97" t="s">
-        <v>197</v>
-      </c>
-      <c r="K97">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D98" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>166</v>
       </c>
       <c r="I98" t="s">
         <v>171</v>
       </c>
       <c r="J98" t="s">
-        <v>207</v>
-      </c>
-      <c r="K98">
-        <v>43</v>
+        <v>293</v>
+      </c>
+      <c r="K98" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="2:12" x14ac:dyDescent="0.25">
@@ -5235,56 +5259,50 @@
         <v>96</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I99" t="s">
         <v>171</v>
       </c>
       <c r="J99" t="s">
-        <v>260</v>
+        <v>197</v>
       </c>
       <c r="K99">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="100" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D100" s="6" t="s">
-        <v>95</v>
+      <c r="D100" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>493</v>
+        <v>166</v>
       </c>
       <c r="I100" t="s">
         <v>171</v>
       </c>
       <c r="J100" t="s">
-        <v>484</v>
+        <v>207</v>
       </c>
       <c r="K100">
-        <v>1</v>
-      </c>
-      <c r="L100" t="s">
-        <v>492</v>
+        <v>43</v>
       </c>
     </row>
     <row r="101" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D101" s="6" t="s">
-        <v>95</v>
+      <c r="D101" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>494</v>
+        <v>167</v>
       </c>
       <c r="I101" t="s">
         <v>171</v>
       </c>
       <c r="J101" t="s">
-        <v>485</v>
+        <v>260</v>
       </c>
       <c r="K101">
-        <v>1</v>
-      </c>
-      <c r="L101" t="s">
-        <v>492</v>
+        <v>42</v>
       </c>
     </row>
     <row r="102" spans="2:12" x14ac:dyDescent="0.25">
@@ -5292,13 +5310,13 @@
         <v>95</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I102" t="s">
         <v>171</v>
       </c>
       <c r="J102" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="K102">
         <v>1</v>
@@ -5312,13 +5330,13 @@
         <v>95</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="I103" t="s">
         <v>171</v>
       </c>
       <c r="J103" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="K103">
         <v>1</v>
@@ -5332,13 +5350,13 @@
         <v>95</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I104" t="s">
         <v>171</v>
       </c>
       <c r="J104" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="K104">
         <v>1</v>
@@ -5352,13 +5370,13 @@
         <v>95</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="I105" t="s">
         <v>171</v>
       </c>
       <c r="J105" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="K105">
         <v>1</v>
@@ -5372,13 +5390,13 @@
         <v>95</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="I106" t="s">
         <v>171</v>
       </c>
       <c r="J106" t="s">
-        <v>510</v>
+        <v>488</v>
       </c>
       <c r="K106">
         <v>1</v>
@@ -5392,13 +5410,13 @@
         <v>95</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I107" t="s">
         <v>171</v>
       </c>
       <c r="J107" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K107">
         <v>1</v>
@@ -5412,13 +5430,13 @@
         <v>95</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="I108" t="s">
         <v>171</v>
       </c>
       <c r="J108" t="s">
-        <v>491</v>
+        <v>510</v>
       </c>
       <c r="K108">
         <v>1</v>
@@ -5428,23 +5446,23 @@
       </c>
     </row>
     <row r="109" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>460</v>
-      </c>
       <c r="D109" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>423</v>
+        <v>499</v>
       </c>
       <c r="I109" t="s">
-        <v>455</v>
+        <v>171</v>
       </c>
       <c r="J109" t="s">
-        <v>425</v>
-      </c>
-      <c r="K109" s="10">
-        <v>1</v>
+        <v>490</v>
+      </c>
+      <c r="K109">
+        <v>1</v>
+      </c>
+      <c r="L109" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="110" spans="2:12" x14ac:dyDescent="0.25">
@@ -5452,36 +5470,39 @@
         <v>95</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>519</v>
+        <v>500</v>
       </c>
       <c r="I110" t="s">
-        <v>455</v>
+        <v>171</v>
       </c>
       <c r="J110" t="s">
-        <v>419</v>
-      </c>
-      <c r="K110" s="10">
-        <v>1</v>
+        <v>491</v>
+      </c>
+      <c r="K110">
+        <v>1</v>
+      </c>
+      <c r="L110" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="111" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>460</v>
+      </c>
       <c r="D111" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="I111" t="s">
         <v>455</v>
       </c>
       <c r="J111" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="K111" s="10">
         <v>1</v>
-      </c>
-      <c r="L111" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="112" spans="2:12" x14ac:dyDescent="0.25">
@@ -5489,53 +5510,56 @@
         <v>95</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>461</v>
+        <v>519</v>
       </c>
       <c r="I112" t="s">
         <v>455</v>
       </c>
       <c r="J112" t="s">
-        <v>462</v>
+        <v>419</v>
       </c>
       <c r="K112" s="10">
         <v>1</v>
       </c>
-      <c r="L112" t="s">
-        <v>387</v>
-      </c>
     </row>
     <row r="113" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D113" s="5" t="s">
-        <v>96</v>
+      <c r="D113" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="I113" t="s">
         <v>455</v>
       </c>
       <c r="J113" t="s">
-        <v>426</v>
-      </c>
-      <c r="K113">
-        <v>44</v>
+        <v>418</v>
+      </c>
+      <c r="K113" s="10">
+        <v>1</v>
+      </c>
+      <c r="L113" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="114" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D114" s="5" t="s">
-        <v>96</v>
+      <c r="D114" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>417</v>
+        <v>461</v>
       </c>
       <c r="I114" t="s">
         <v>455</v>
       </c>
       <c r="J114" t="s">
-        <v>196</v>
-      </c>
-      <c r="K114">
-        <v>36</v>
+        <v>462</v>
+      </c>
+      <c r="K114" s="10">
+        <v>1</v>
+      </c>
+      <c r="L114" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="115" spans="2:12" x14ac:dyDescent="0.25">
@@ -5543,19 +5567,16 @@
         <v>96</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="I115" t="s">
         <v>455</v>
       </c>
       <c r="J115" t="s">
-        <v>416</v>
+        <v>426</v>
       </c>
       <c r="K115">
-        <v>33</v>
-      </c>
-      <c r="L115" t="s">
-        <v>387</v>
+        <v>44</v>
       </c>
     </row>
     <row r="116" spans="2:12" x14ac:dyDescent="0.25">
@@ -5563,119 +5584,113 @@
         <v>96</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>453</v>
+        <v>417</v>
       </c>
       <c r="I116" t="s">
         <v>455</v>
       </c>
       <c r="J116" t="s">
+        <v>196</v>
+      </c>
+      <c r="K116">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="117" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D117" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="I117" t="s">
+        <v>455</v>
+      </c>
+      <c r="J117" t="s">
+        <v>416</v>
+      </c>
+      <c r="K117">
+        <v>33</v>
+      </c>
+      <c r="L117" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="118" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D118" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="I118" t="s">
+        <v>455</v>
+      </c>
+      <c r="J118" t="s">
         <v>454</v>
       </c>
-      <c r="K116">
+      <c r="K118">
         <v>31</v>
       </c>
-      <c r="L116" t="s">
+      <c r="L118" t="s">
         <v>387</v>
-      </c>
-    </row>
-    <row r="117" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B117" t="s">
-        <v>175</v>
-      </c>
-      <c r="D117" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F117" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="I117" t="s">
-        <v>456</v>
-      </c>
-      <c r="J117" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="K117" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B118" t="s">
-        <v>245</v>
-      </c>
-      <c r="D118" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="F118" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="I118" t="s">
-        <v>456</v>
-      </c>
-      <c r="J118" s="10" t="s">
-        <v>331</v>
-      </c>
-      <c r="K118" s="10">
-        <v>1</v>
       </c>
     </row>
     <row r="119" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>247</v>
+        <v>175</v>
       </c>
       <c r="D119" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F119" s="9" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="I119" t="s">
         <v>456</v>
       </c>
       <c r="J119" s="10" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="K119" s="10">
         <v>1</v>
-      </c>
-      <c r="L119" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="120" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D120" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>212</v>
+        <v>177</v>
       </c>
       <c r="I120" t="s">
         <v>456</v>
       </c>
       <c r="J120" s="10" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="K120" s="10">
         <v>1</v>
       </c>
-      <c r="L120" t="s">
-        <v>387</v>
-      </c>
     </row>
     <row r="121" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>247</v>
+      </c>
       <c r="D121" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F121" s="9" t="s">
-        <v>328</v>
+        <v>186</v>
       </c>
       <c r="I121" t="s">
         <v>456</v>
       </c>
       <c r="J121" s="10" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="K121" s="10">
         <v>1</v>
@@ -5686,19 +5701,19 @@
     </row>
     <row r="122" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F122" s="9" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="I122" t="s">
         <v>456</v>
       </c>
       <c r="J122" s="10" t="s">
-        <v>241</v>
+        <v>333</v>
       </c>
       <c r="K122" s="10">
         <v>1</v>
@@ -5708,37 +5723,46 @@
       </c>
     </row>
     <row r="123" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D123" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>178</v>
+      <c r="D123" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F123" s="9" t="s">
+        <v>328</v>
       </c>
       <c r="I123" t="s">
         <v>456</v>
       </c>
-      <c r="J123" t="s">
-        <v>208</v>
-      </c>
-      <c r="K123">
-        <v>64</v>
+      <c r="J123" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="K123" s="10">
+        <v>1</v>
+      </c>
+      <c r="L123" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="124" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D124" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>179</v>
+      <c r="B124" t="s">
+        <v>244</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F124" s="9" t="s">
+        <v>240</v>
       </c>
       <c r="I124" t="s">
         <v>456</v>
       </c>
-      <c r="J124" t="s">
-        <v>209</v>
-      </c>
-      <c r="K124">
-        <v>65</v>
+      <c r="J124" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="K124" s="10">
+        <v>1</v>
+      </c>
+      <c r="L124" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="125" spans="2:12" x14ac:dyDescent="0.25">
@@ -5746,16 +5770,16 @@
         <v>96</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>466</v>
+        <v>178</v>
       </c>
       <c r="I125" t="s">
         <v>456</v>
       </c>
       <c r="J125" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="K125">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="126" spans="2:12" x14ac:dyDescent="0.25">
@@ -5763,16 +5787,16 @@
         <v>96</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="I126" t="s">
         <v>456</v>
       </c>
       <c r="J126" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K126">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="127" spans="2:12" x14ac:dyDescent="0.25">
@@ -5780,16 +5804,16 @@
         <v>96</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>227</v>
+        <v>466</v>
       </c>
       <c r="I127" t="s">
         <v>456</v>
       </c>
       <c r="J127" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="K127">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="128" spans="2:12" x14ac:dyDescent="0.25">
@@ -5797,19 +5821,16 @@
         <v>96</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>543</v>
+        <v>187</v>
       </c>
       <c r="I128" t="s">
         <v>456</v>
       </c>
       <c r="J128" t="s">
-        <v>537</v>
+        <v>210</v>
       </c>
       <c r="K128">
-        <v>69</v>
-      </c>
-      <c r="L128" t="s">
-        <v>387</v>
+        <v>68</v>
       </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
@@ -5817,19 +5838,16 @@
         <v>96</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>188</v>
+        <v>227</v>
       </c>
       <c r="I129" t="s">
         <v>456</v>
       </c>
       <c r="J129" t="s">
-        <v>335</v>
+        <v>228</v>
       </c>
       <c r="K129">
-        <v>63</v>
-      </c>
-      <c r="L129" t="s">
-        <v>387</v>
+        <v>67</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
@@ -5837,16 +5855,16 @@
         <v>96</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>334</v>
+        <v>543</v>
       </c>
       <c r="I130" t="s">
         <v>456</v>
       </c>
       <c r="J130" t="s">
-        <v>336</v>
+        <v>537</v>
       </c>
       <c r="K130">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="L130" t="s">
         <v>387</v>
@@ -5857,36 +5875,39 @@
         <v>96</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>242</v>
+        <v>188</v>
       </c>
       <c r="I131" t="s">
         <v>456</v>
       </c>
       <c r="J131" t="s">
-        <v>243</v>
+        <v>335</v>
       </c>
       <c r="K131">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L131" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D132" s="6" t="s">
-        <v>95</v>
+      <c r="D132" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>370</v>
+        <v>334</v>
       </c>
       <c r="I132" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J132" t="s">
-        <v>371</v>
-      </c>
-      <c r="K132" s="10">
-        <v>1</v>
+        <v>336</v>
+      </c>
+      <c r="K132">
+        <v>62</v>
+      </c>
+      <c r="L132" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.25">
@@ -5894,50 +5915,53 @@
         <v>96</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>369</v>
+        <v>242</v>
       </c>
       <c r="I133" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J133" t="s">
-        <v>372</v>
+        <v>243</v>
       </c>
       <c r="K133">
-        <v>71</v>
+        <v>61</v>
+      </c>
+      <c r="L133" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D134" s="5" t="s">
-        <v>96</v>
+      <c r="D134" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>467</v>
+        <v>370</v>
       </c>
       <c r="I134" t="s">
         <v>457</v>
       </c>
       <c r="J134" t="s">
-        <v>373</v>
-      </c>
-      <c r="K134">
-        <v>72</v>
+        <v>371</v>
+      </c>
+      <c r="K134" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D135" s="6" t="s">
-        <v>95</v>
+      <c r="D135" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>220</v>
+        <v>369</v>
       </c>
       <c r="I135" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J135" t="s">
-        <v>294</v>
-      </c>
-      <c r="K135" s="10">
-        <v>1</v>
+        <v>372</v>
+      </c>
+      <c r="K135">
+        <v>71</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
@@ -5945,42 +5969,33 @@
         <v>96</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>221</v>
+        <v>467</v>
       </c>
       <c r="I136" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J136" t="s">
-        <v>222</v>
+        <v>373</v>
       </c>
       <c r="K136">
-        <v>45</v>
+        <v>72</v>
       </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A137">
-        <v>17</v>
-      </c>
-      <c r="B137" t="s">
-        <v>136</v>
-      </c>
       <c r="D137" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F137" s="9" t="s">
-        <v>515</v>
+      <c r="F137" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="I137" t="s">
-        <v>482</v>
-      </c>
-      <c r="J137" s="10" t="s">
-        <v>483</v>
+        <v>458</v>
+      </c>
+      <c r="J137" t="s">
+        <v>294</v>
       </c>
       <c r="K137" s="10">
         <v>1</v>
-      </c>
-      <c r="L137" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.25">
@@ -5988,81 +6003,121 @@
         <v>96</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>481</v>
+        <v>221</v>
       </c>
       <c r="I138" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
       <c r="J138" t="s">
-        <v>345</v>
+        <v>222</v>
       </c>
       <c r="K138">
-        <v>51</v>
-      </c>
-      <c r="L138" t="s">
-        <v>387</v>
+        <v>45</v>
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>17</v>
+      </c>
       <c r="B139" t="s">
-        <v>287</v>
+        <v>136</v>
       </c>
       <c r="D139" s="6" t="s">
         <v>95</v>
       </c>
       <c r="F139" s="9" t="s">
-        <v>288</v>
+        <v>515</v>
       </c>
       <c r="I139" t="s">
-        <v>459</v>
-      </c>
-      <c r="J139" t="s">
-        <v>291</v>
+        <v>482</v>
+      </c>
+      <c r="J139" s="10" t="s">
+        <v>483</v>
       </c>
       <c r="K139" s="10">
         <v>1</v>
       </c>
+      <c r="L139" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D140" s="6" t="s">
-        <v>95</v>
+      <c r="D140" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>296</v>
+        <v>481</v>
       </c>
       <c r="I140" t="s">
-        <v>459</v>
+        <v>482</v>
       </c>
       <c r="J140" t="s">
-        <v>292</v>
-      </c>
-      <c r="K140" s="10">
-        <v>1</v>
+        <v>345</v>
+      </c>
+      <c r="K140">
+        <v>51</v>
       </c>
       <c r="L140" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D141" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F141" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="G141">
-        <v>1</v>
+      <c r="B141" t="s">
+        <v>287</v>
+      </c>
+      <c r="D141" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F141" s="9" t="s">
+        <v>288</v>
       </c>
       <c r="I141" t="s">
         <v>459</v>
       </c>
       <c r="J141" t="s">
+        <v>291</v>
+      </c>
+      <c r="K141" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D142" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="I142" t="s">
+        <v>459</v>
+      </c>
+      <c r="J142" t="s">
+        <v>292</v>
+      </c>
+      <c r="K142" s="10">
+        <v>1</v>
+      </c>
+      <c r="L142" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D143" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="I143" t="s">
+        <v>459</v>
+      </c>
+      <c r="J143" t="s">
         <v>290</v>
       </c>
-      <c r="K141">
+      <c r="K143">
         <v>46</v>
       </c>
-      <c r="L141" t="s">
+      <c r="L143" t="s">
         <v>387</v>
       </c>
     </row>

</xml_diff>

<commit_message>
xd fd cobbection statistics update
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -3086,8 +3086,8 @@
   <dimension ref="A1:L143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5187,9 +5187,6 @@
       <c r="F95" s="9" t="s">
         <v>555</v>
       </c>
-      <c r="H95">
-        <v>1</v>
-      </c>
       <c r="I95" t="s">
         <v>558</v>
       </c>
@@ -5622,6 +5619,9 @@
       </c>
       <c r="F118" s="2" t="s">
         <v>453</v>
+      </c>
+      <c r="G118">
+        <v>1</v>
       </c>
       <c r="I118" t="s">
         <v>455</v>

</xml_diff>

<commit_message>
single connection asymmetry verification added
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="583">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1760,6 +1760,15 @@
   </si>
   <si>
     <t>DATA ANALYSIS X. TRANSLATE DOMAIN (XD) PROXY DEVICES</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\01.CUSTOMERS\Novatek\SAN Assessment\FEB2022</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\Novatek\FEB22\ssave</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\Novatek\FEB22\blade</t>
   </si>
 </sst>
 </file>
@@ -2182,160 +2191,160 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BA15"/>
+  <dimension ref="A1:BB15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="3" width="70" customWidth="1"/>
-    <col min="4" max="4" width="109.42578125" customWidth="1"/>
-    <col min="5" max="5" width="116.7109375" customWidth="1"/>
-    <col min="6" max="6" width="128.5703125" customWidth="1"/>
-    <col min="7" max="7" width="99.85546875" customWidth="1"/>
-    <col min="8" max="8" width="126.5703125" customWidth="1"/>
-    <col min="9" max="9" width="151.28515625" customWidth="1"/>
-    <col min="10" max="10" width="120.42578125" customWidth="1"/>
-    <col min="11" max="11" width="112.42578125" customWidth="1"/>
-    <col min="12" max="12" width="158.5703125" customWidth="1"/>
-    <col min="13" max="13" width="103.7109375" customWidth="1"/>
-    <col min="14" max="14" width="91.85546875" customWidth="1"/>
-    <col min="15" max="15" width="70" customWidth="1"/>
-    <col min="16" max="16" width="124.42578125" customWidth="1"/>
-    <col min="17" max="17" width="103.85546875" customWidth="1"/>
-    <col min="18" max="18" width="48.85546875" customWidth="1"/>
-    <col min="19" max="19" width="29.7109375" customWidth="1"/>
-    <col min="20" max="20" width="80.140625" customWidth="1"/>
-    <col min="21" max="21" width="35.7109375" customWidth="1"/>
-    <col min="22" max="23" width="122.7109375" customWidth="1"/>
-    <col min="24" max="24" width="48.42578125" customWidth="1"/>
-    <col min="25" max="25" width="29.7109375" customWidth="1"/>
-    <col min="26" max="26" width="80.140625" customWidth="1"/>
-    <col min="27" max="27" width="68.5703125" customWidth="1"/>
-    <col min="28" max="28" width="48.7109375" customWidth="1"/>
-    <col min="29" max="29" width="62" customWidth="1"/>
-    <col min="30" max="32" width="89.5703125" customWidth="1"/>
-    <col min="33" max="33" width="69.85546875" customWidth="1"/>
-    <col min="34" max="34" width="52.140625" customWidth="1"/>
-    <col min="35" max="35" width="73.140625" customWidth="1"/>
-    <col min="36" max="36" width="29.7109375" customWidth="1"/>
-    <col min="37" max="38" width="76" customWidth="1"/>
-    <col min="39" max="39" width="72.28515625" customWidth="1"/>
-    <col min="40" max="40" width="61.7109375" customWidth="1"/>
-    <col min="41" max="41" width="60" customWidth="1"/>
-    <col min="42" max="42" width="38.140625" customWidth="1"/>
-    <col min="43" max="43" width="69" customWidth="1"/>
-    <col min="44" max="44" width="72.42578125" customWidth="1"/>
-    <col min="45" max="45" width="111.5703125" customWidth="1"/>
-    <col min="46" max="46" width="72.5703125" customWidth="1"/>
-    <col min="47" max="47" width="86.85546875" customWidth="1"/>
-    <col min="48" max="49" width="64.7109375" customWidth="1"/>
-    <col min="50" max="50" width="54.5703125" customWidth="1"/>
-    <col min="51" max="51" width="75.42578125" customWidth="1"/>
-    <col min="52" max="52" width="58.140625" customWidth="1"/>
+    <col min="2" max="4" width="70" customWidth="1"/>
+    <col min="5" max="5" width="109.42578125" customWidth="1"/>
+    <col min="6" max="6" width="116.7109375" customWidth="1"/>
+    <col min="7" max="7" width="128.5703125" customWidth="1"/>
+    <col min="8" max="8" width="99.85546875" customWidth="1"/>
+    <col min="9" max="9" width="126.5703125" customWidth="1"/>
+    <col min="10" max="10" width="151.28515625" customWidth="1"/>
+    <col min="11" max="11" width="120.42578125" customWidth="1"/>
+    <col min="12" max="12" width="112.42578125" customWidth="1"/>
+    <col min="13" max="13" width="158.5703125" customWidth="1"/>
+    <col min="14" max="14" width="103.7109375" customWidth="1"/>
+    <col min="15" max="15" width="91.85546875" customWidth="1"/>
+    <col min="16" max="16" width="70" customWidth="1"/>
+    <col min="17" max="17" width="124.42578125" customWidth="1"/>
+    <col min="18" max="18" width="103.85546875" customWidth="1"/>
+    <col min="19" max="19" width="48.85546875" customWidth="1"/>
+    <col min="20" max="20" width="29.7109375" customWidth="1"/>
+    <col min="21" max="21" width="80.140625" customWidth="1"/>
+    <col min="22" max="22" width="35.7109375" customWidth="1"/>
+    <col min="23" max="24" width="122.7109375" customWidth="1"/>
+    <col min="25" max="25" width="48.42578125" customWidth="1"/>
+    <col min="26" max="26" width="29.7109375" customWidth="1"/>
+    <col min="27" max="27" width="80.140625" customWidth="1"/>
+    <col min="28" max="28" width="68.5703125" customWidth="1"/>
+    <col min="29" max="29" width="48.7109375" customWidth="1"/>
+    <col min="30" max="30" width="62" customWidth="1"/>
+    <col min="31" max="33" width="89.5703125" customWidth="1"/>
+    <col min="34" max="34" width="69.85546875" customWidth="1"/>
+    <col min="35" max="35" width="52.140625" customWidth="1"/>
+    <col min="36" max="36" width="73.140625" customWidth="1"/>
+    <col min="37" max="37" width="29.7109375" customWidth="1"/>
+    <col min="38" max="39" width="76" customWidth="1"/>
+    <col min="40" max="40" width="72.28515625" customWidth="1"/>
+    <col min="41" max="41" width="61.7109375" customWidth="1"/>
+    <col min="42" max="42" width="60" customWidth="1"/>
+    <col min="43" max="43" width="38.140625" customWidth="1"/>
+    <col min="44" max="44" width="69" customWidth="1"/>
+    <col min="45" max="45" width="72.42578125" customWidth="1"/>
+    <col min="46" max="46" width="111.5703125" customWidth="1"/>
+    <col min="47" max="47" width="72.5703125" customWidth="1"/>
+    <col min="48" max="48" width="86.85546875" customWidth="1"/>
+    <col min="49" max="50" width="64.7109375" customWidth="1"/>
+    <col min="51" max="51" width="54.5703125" customWidth="1"/>
+    <col min="52" max="52" width="75.42578125" customWidth="1"/>
+    <col min="53" max="53" width="58.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
       <c r="C2" t="s">
+        <v>444</v>
+      </c>
+      <c r="D2" t="s">
         <v>230</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>551</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>531</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>539</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>534</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>532</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>531</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>524</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>520</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>382</v>
-      </c>
-      <c r="M2" t="s">
-        <v>502</v>
       </c>
       <c r="N2" t="s">
         <v>502</v>
       </c>
       <c r="O2" t="s">
-        <v>410</v>
+        <v>502</v>
       </c>
       <c r="P2" t="s">
         <v>410</v>
       </c>
       <c r="Q2" t="s">
+        <v>410</v>
+      </c>
+      <c r="R2" t="s">
         <v>444</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>431</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>410</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>230</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>388</v>
-      </c>
-      <c r="V2" t="s">
-        <v>382</v>
       </c>
       <c r="W2" t="s">
         <v>382</v>
       </c>
       <c r="X2" t="s">
+        <v>382</v>
+      </c>
+      <c r="Y2" t="s">
         <v>374</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>354</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>322</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>312</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>305</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>302</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>298</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>306</v>
       </c>
       <c r="AF2" t="s">
         <v>306</v>
@@ -2344,172 +2353,178 @@
         <v>306</v>
       </c>
       <c r="AH2" t="s">
+        <v>306</v>
+      </c>
+      <c r="AI2" t="s">
         <v>269</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>265</v>
       </c>
       <c r="AJ2" t="s">
         <v>265</v>
       </c>
       <c r="AK2" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="AL2" t="s">
         <v>248</v>
       </c>
       <c r="AM2" t="s">
+        <v>248</v>
+      </c>
+      <c r="AN2" t="s">
         <v>230</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>226</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>185</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>184</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>154</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>110</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>97</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AU2" t="s">
         <v>83</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BA2" s="1" t="s">
+      <c r="BB2" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>273</v>
       </c>
       <c r="C3" s="12">
+        <v>44620</v>
+      </c>
+      <c r="D3" s="12">
         <v>44608</v>
       </c>
-      <c r="D3" s="12">
+      <c r="E3" s="12">
         <v>44592</v>
       </c>
-      <c r="E3" s="12">
+      <c r="F3" s="12">
         <v>44575</v>
       </c>
-      <c r="F3" s="12">
+      <c r="G3" s="12">
         <v>44537</v>
       </c>
-      <c r="G3" s="12">
+      <c r="H3" s="12">
         <v>44531</v>
       </c>
-      <c r="H3" s="12">
+      <c r="I3" s="12">
         <v>44530</v>
       </c>
-      <c r="I3" s="12">
+      <c r="J3" s="12">
         <v>44529</v>
       </c>
-      <c r="J3" s="12">
+      <c r="K3" s="12">
         <v>44524</v>
       </c>
-      <c r="K3" s="12">
+      <c r="L3" s="12">
         <v>44503</v>
       </c>
-      <c r="L3" s="12">
+      <c r="M3" s="12">
         <v>44343</v>
-      </c>
-      <c r="M3" s="12">
-        <v>44484</v>
       </c>
       <c r="N3" s="12">
         <v>44484</v>
       </c>
       <c r="O3" s="12">
+        <v>44484</v>
+      </c>
+      <c r="P3" s="12">
         <v>44473</v>
       </c>
-      <c r="P3" s="12">
+      <c r="Q3" s="12">
         <v>44469</v>
       </c>
-      <c r="Q3" s="12">
+      <c r="R3" s="12">
         <v>44453</v>
       </c>
-      <c r="R3" s="12">
+      <c r="S3" s="12">
         <v>44426</v>
       </c>
-      <c r="S3" s="12">
+      <c r="T3" s="12">
         <v>44330</v>
       </c>
-      <c r="T3" s="12">
+      <c r="U3" s="12">
         <v>44307</v>
       </c>
-      <c r="U3" s="12">
+      <c r="V3" s="12">
         <v>44294</v>
       </c>
-      <c r="V3" s="12">
+      <c r="W3" s="12">
         <v>44343</v>
       </c>
-      <c r="W3" s="12">
+      <c r="X3" s="12">
         <v>44292</v>
       </c>
-      <c r="X3" s="12">
+      <c r="Y3" s="12">
         <v>29681</v>
       </c>
-      <c r="Y3" s="12">
+      <c r="Z3" s="12">
         <v>44286</v>
       </c>
-      <c r="Z3" s="12">
+      <c r="AA3" s="12">
         <v>44260</v>
       </c>
-      <c r="AA3" s="12">
+      <c r="AB3" s="12">
         <v>44244</v>
       </c>
-      <c r="AB3" s="12">
+      <c r="AC3" s="12">
         <v>44245</v>
       </c>
-      <c r="AC3" s="12">
+      <c r="AD3" s="12">
         <v>44223</v>
       </c>
-      <c r="AD3" s="12">
+      <c r="AE3" s="12">
         <v>44209</v>
       </c>
-      <c r="AE3" s="12">
+      <c r="AF3" s="12">
         <v>44253</v>
       </c>
-      <c r="AF3" s="12">
+      <c r="AG3" s="12">
         <v>44237</v>
       </c>
-      <c r="AI3" s="12">
+      <c r="AJ3" s="12">
         <v>44181</v>
       </c>
-      <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
       <c r="AX3" s="1"/>
       <c r="AY3" s="1"/>
       <c r="AZ3" s="1"/>
       <c r="BA3" s="1"/>
-    </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BB3" s="1"/>
+    </row>
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>474</v>
       </c>
@@ -2520,7 +2535,7 @@
         <v>552</v>
       </c>
       <c r="E4" t="s">
-        <v>315</v>
+        <v>552</v>
       </c>
       <c r="F4" t="s">
         <v>315</v>
@@ -2541,22 +2556,22 @@
         <v>315</v>
       </c>
       <c r="L4" t="s">
+        <v>315</v>
+      </c>
+      <c r="M4" t="s">
         <v>517</v>
-      </c>
-      <c r="M4" t="s">
-        <v>503</v>
       </c>
       <c r="N4" t="s">
         <v>503</v>
       </c>
       <c r="O4" t="s">
-        <v>468</v>
+        <v>503</v>
       </c>
       <c r="P4" t="s">
         <v>468</v>
       </c>
       <c r="Q4" t="s">
-        <v>315</v>
+        <v>468</v>
       </c>
       <c r="R4" t="s">
         <v>315</v>
@@ -2565,13 +2580,13 @@
         <v>315</v>
       </c>
       <c r="T4" t="s">
+        <v>315</v>
+      </c>
+      <c r="U4" t="s">
         <v>401</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>389</v>
-      </c>
-      <c r="V4" t="s">
-        <v>315</v>
       </c>
       <c r="W4" t="s">
         <v>315</v>
@@ -2580,496 +2595,508 @@
         <v>315</v>
       </c>
       <c r="Y4" t="s">
+        <v>315</v>
+      </c>
+      <c r="Z4" t="s">
         <v>355</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>315</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>311</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>315</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>315</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>319</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>311</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>272</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>271</v>
       </c>
-      <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
       <c r="AY4" s="1"/>
       <c r="AZ4" s="1"/>
       <c r="BA4" s="1"/>
-    </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="BB4" s="1"/>
+    </row>
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C5" t="s">
+        <v>580</v>
+      </c>
+      <c r="D5" t="s">
         <v>573</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>554</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>549</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>540</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>535</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>533</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>530</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>525</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>521</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>516</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>511</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>506</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>479</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>469</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>445</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>432</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>411</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>402</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>390</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>544</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>384</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>375</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="Z5" t="s">
         <v>356</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>323</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>313</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>317</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>303</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>297</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>320</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AG5" t="s">
         <v>309</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AH5" t="s">
         <v>307</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>270</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AJ5" t="s">
         <v>274</v>
       </c>
-      <c r="AJ5" t="s">
+      <c r="AK5" t="s">
         <v>267</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>249</v>
       </c>
       <c r="AL5" t="s">
         <v>249</v>
       </c>
       <c r="AM5" t="s">
+        <v>249</v>
+      </c>
+      <c r="AN5" t="s">
         <v>232</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AO5" t="s">
         <v>225</v>
       </c>
-      <c r="AO5" t="s">
+      <c r="AP5" t="s">
         <v>216</v>
       </c>
-      <c r="AP5" t="s">
+      <c r="AQ5" t="s">
         <v>183</v>
       </c>
-      <c r="AQ5" t="s">
+      <c r="AR5" t="s">
         <v>156</v>
       </c>
-      <c r="AR5" t="s">
+      <c r="AS5" t="s">
         <v>112</v>
       </c>
-      <c r="AS5" t="s">
+      <c r="AT5" t="s">
         <v>98</v>
       </c>
-      <c r="AT5" t="s">
+      <c r="AU5" t="s">
         <v>85</v>
       </c>
-      <c r="AU5" t="s">
-        <v>1</v>
-      </c>
       <c r="AV5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW5" t="s">
         <v>74</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AX5" t="s">
         <v>72</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="AY5" t="s">
         <v>4</v>
       </c>
-      <c r="AY5" t="s">
+      <c r="AZ5" t="s">
         <v>25</v>
       </c>
-      <c r="AZ5" t="s">
+      <c r="BA5" t="s">
         <v>60</v>
       </c>
-      <c r="BA5" t="s">
+      <c r="BB5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="C6" t="s">
+        <v>581</v>
+      </c>
+      <c r="D6" t="s">
         <v>574</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>553</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>569</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>542</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>536</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>550</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>569</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>526</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>523</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>518</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>512</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>504</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>480</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>470</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>446</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>433</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>412</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>403</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>391</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>545</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>383</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>376</v>
       </c>
-      <c r="Y6" t="s">
+      <c r="Z6" t="s">
         <v>357</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>344</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>314</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>316</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>304</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>299</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>321</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AG6" t="s">
         <v>310</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
         <v>308</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>268</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AJ6" t="s">
         <v>275</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AK6" t="s">
         <v>266</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AL6" t="s">
         <v>261</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="AM6" t="s">
         <v>250</v>
       </c>
-      <c r="AM6" t="s">
+      <c r="AN6" t="s">
         <v>231</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AO6" t="s">
         <v>223</v>
       </c>
-      <c r="AO6" t="s">
+      <c r="AP6" t="s">
         <v>215</v>
       </c>
-      <c r="AP6" t="s">
+      <c r="AQ6" t="s">
         <v>182</v>
       </c>
-      <c r="AQ6" t="s">
+      <c r="AR6" t="s">
         <v>155</v>
       </c>
-      <c r="AR6" t="s">
+      <c r="AS6" t="s">
         <v>111</v>
       </c>
-      <c r="AS6" t="s">
+      <c r="AT6" t="s">
         <v>107</v>
       </c>
-      <c r="AT6" t="s">
+      <c r="AU6" t="s">
         <v>84</v>
       </c>
-      <c r="AU6" t="s">
+      <c r="AV6" t="s">
         <v>0</v>
       </c>
-      <c r="AV6" t="s">
+      <c r="AW6" t="s">
         <v>73</v>
       </c>
-      <c r="AW6" t="s">
+      <c r="AX6" t="s">
         <v>71</v>
       </c>
-      <c r="AX6" t="s">
+      <c r="AY6" t="s">
         <v>3</v>
       </c>
-      <c r="AY6" t="s">
+      <c r="AZ6" t="s">
         <v>24</v>
       </c>
-      <c r="AZ6" t="s">
+      <c r="BA6" t="s">
         <v>59</v>
       </c>
-      <c r="BA6" t="s">
+      <c r="BB6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="E7" t="s">
+      <c r="C7" t="s">
+        <v>582</v>
+      </c>
+      <c r="F7" t="s">
         <v>570</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>541</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>538</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>548</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>570</v>
-      </c>
-      <c r="J7" t="s">
-        <v>522</v>
       </c>
       <c r="K7" t="s">
         <v>522</v>
       </c>
-      <c r="M7" t="s">
+      <c r="L7" t="s">
+        <v>522</v>
+      </c>
+      <c r="N7" t="s">
         <v>513</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>505</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>471</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>434</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>413</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>546</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>377</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>324</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>300</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>251</v>
       </c>
       <c r="AL7" t="s">
         <v>251</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AM7" t="s">
+        <v>251</v>
+      </c>
+      <c r="AO7" t="s">
         <v>224</v>
       </c>
-      <c r="AQ7" t="s">
+      <c r="AR7" t="s">
         <v>157</v>
       </c>
-      <c r="AS7" t="s">
+      <c r="AT7" t="s">
         <v>108</v>
       </c>
-      <c r="AT7" t="s">
+      <c r="AU7" t="s">
         <v>87</v>
       </c>
-      <c r="AW7" t="s">
+      <c r="AX7" t="s">
         <v>99</v>
       </c>
-      <c r="AZ7" t="s">
+      <c r="BA7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>252</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>463</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>404</v>
       </c>
-      <c r="Z8" t="s">
+      <c r="AA8" t="s">
         <v>325</v>
-      </c>
-      <c r="AK8" t="s">
-        <v>253</v>
       </c>
       <c r="AL8" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
+      <c r="AM8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>547</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Y9" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>508</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>514</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>478</v>
       </c>
@@ -3086,8 +3113,8 @@
   <dimension ref="A1:L143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G80" sqref="G80"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4808,6 +4835,9 @@
       <c r="F75" s="2" t="s">
         <v>280</v>
       </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
       <c r="I75" t="s">
         <v>169</v>
       </c>
@@ -5619,9 +5649,6 @@
       </c>
       <c r="F118" s="2" t="s">
         <v>453</v>
-      </c>
-      <c r="G118">
-        <v>1</v>
       </c>
       <c r="I118" t="s">
         <v>455</v>

</xml_diff>

<commit_message>
portcmd collection regex patterns and collection algorythm changed
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -2194,7 +2194,7 @@
   <dimension ref="A1:BB15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3113,8 +3113,8 @@
   <dimension ref="A1:L143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G79" sqref="G79"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4835,9 +4835,6 @@
       <c r="F75" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="G75">
-        <v>1</v>
-      </c>
       <c r="I75" t="s">
         <v>169</v>
       </c>
@@ -4864,6 +4861,9 @@
       <c r="F76" s="9" t="s">
         <v>90</v>
       </c>
+      <c r="H76">
+        <v>1</v>
+      </c>
       <c r="I76" t="s">
         <v>170</v>
       </c>
@@ -6054,6 +6054,9 @@
       </c>
       <c r="F139" s="9" t="s">
         <v>515</v>
+      </c>
+      <c r="H139">
+        <v>1</v>
       </c>
       <c r="I139" t="s">
         <v>482</v>

</xml_diff>

<commit_message>
data_names imported from file
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="report_requisites" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="632">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1324,9 +1324,6 @@
     <t>s3mft</t>
   </si>
   <si>
-    <t>C:\Users\vlasenko\Documents\02.DOCUMENTATION\Procedures\SAN Assessment\3par_stats\V5.0087\WINDOWS</t>
-  </si>
-  <si>
     <t>s3mft.exe</t>
   </si>
   <si>
@@ -1768,15 +1765,12 @@
     <t>C:\Program Files\SAN Toolbox - Reloaded</t>
   </si>
   <si>
-    <t>switch_config_preprocessing_output</t>
+    <t>switch_config_preprocessing</t>
   </si>
   <si>
     <t>force_run</t>
   </si>
   <si>
-    <t>zoning_collection_out</t>
-  </si>
-  <si>
     <t>zoning_analysis_out</t>
   </si>
   <si>
@@ -1787,13 +1781,148 @@
   </si>
   <si>
     <t>portcmd_analysis_in</t>
+  </si>
+  <si>
+    <t>errorlog_analysis_in</t>
+  </si>
+  <si>
+    <t>errorlog_analysis_out</t>
+  </si>
+  <si>
+    <t>switch_params_analysis_out</t>
+  </si>
+  <si>
+    <t>switch_params_analysis_in</t>
+  </si>
+  <si>
+    <t>switch_params_sw_pair_analysis_out</t>
+  </si>
+  <si>
+    <t>switch_params_sw_pair_analysis_in</t>
+  </si>
+  <si>
+    <t>isl_analysis_out</t>
+  </si>
+  <si>
+    <t>isl_analysis_in</t>
+  </si>
+  <si>
+    <t>isl_sw_pair_analysis_out</t>
+  </si>
+  <si>
+    <t>isl_sw_pair_analysis_in</t>
+  </si>
+  <si>
+    <t>switch_pair_analysis_out</t>
+  </si>
+  <si>
+    <t>switch_pair_analysis_in</t>
+  </si>
+  <si>
+    <t>maps_npiv_ports_analysis_out</t>
+  </si>
+  <si>
+    <t>maps_npiv_ports_analysis_in</t>
+  </si>
+  <si>
+    <t>fabric_label_analysis_out</t>
+  </si>
+  <si>
+    <t>fabric_label_analysis_in</t>
+  </si>
+  <si>
+    <t>port_err_sfp_cfg_analysis_out</t>
+  </si>
+  <si>
+    <t>port_err_sfp_cfg_analysis_in</t>
+  </si>
+  <si>
+    <t>snesor_analysis_out</t>
+  </si>
+  <si>
+    <t>sensor_analysis_in</t>
+  </si>
+  <si>
+    <t>storage_host_analysis_out</t>
+  </si>
+  <si>
+    <t>storage_host_analysis_in</t>
+  </si>
+  <si>
+    <t>fcr_xd_device_analysis_out</t>
+  </si>
+  <si>
+    <t>fcr_xd_device_analysis_in</t>
+  </si>
+  <si>
+    <t>blade_system_analysis_out</t>
+  </si>
+  <si>
+    <t>blade_system_analysis_in</t>
+  </si>
+  <si>
+    <t>chassis_params_collection</t>
+  </si>
+  <si>
+    <t>switch_params_collection</t>
+  </si>
+  <si>
+    <t>maps_params_collection</t>
+  </si>
+  <si>
+    <t>fabric_membership_collection</t>
+  </si>
+  <si>
+    <t>fcr_membership_collection</t>
+  </si>
+  <si>
+    <t>portcmd_collection</t>
+  </si>
+  <si>
+    <t>port_sfp_cfg_collection</t>
+  </si>
+  <si>
+    <t>nameserver_collection</t>
+  </si>
+  <si>
+    <t>isl_collection</t>
+  </si>
+  <si>
+    <t>zoning_collection</t>
+  </si>
+  <si>
+    <t>sensor_collection</t>
+  </si>
+  <si>
+    <t>errorlog_collection</t>
+  </si>
+  <si>
+    <t>blade_collection</t>
+  </si>
+  <si>
+    <t>synergy_collection</t>
+  </si>
+  <si>
+    <t>storage_3par_collection</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\02.DOCUMENTATION\Procedures\SAN Assessment\3par_stats\V5.0120\WINDOWS</t>
+  </si>
+  <si>
+    <t>port_statistics_analysis_in</t>
+  </si>
+  <si>
+    <t>port_statistics_analysis_out</t>
+  </si>
+  <si>
+    <t>devicename_correction_analysis_in</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1812,6 +1941,18 @@
     <font>
       <sz val="11"/>
       <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFDCDCAA"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -1884,7 +2025,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1904,7 +2045,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2212,8 +2360,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BC15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2272,7 +2420,7 @@
       <c r="A1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2281,46 +2429,46 @@
         <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E2" t="s">
         <v>227</v>
       </c>
       <c r="F2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G2" t="s">
+        <v>524</v>
+      </c>
+      <c r="H2" t="s">
+        <v>532</v>
+      </c>
+      <c r="I2" t="s">
+        <v>527</v>
+      </c>
+      <c r="J2" t="s">
         <v>525</v>
       </c>
-      <c r="H2" t="s">
-        <v>533</v>
-      </c>
-      <c r="I2" t="s">
-        <v>528</v>
-      </c>
-      <c r="J2" t="s">
-        <v>526</v>
-      </c>
       <c r="K2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="L2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="M2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="N2" t="s">
         <v>379</v>
       </c>
       <c r="O2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="P2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Q2" t="s">
         <v>407</v>
@@ -2329,7 +2477,7 @@
         <v>407</v>
       </c>
       <c r="S2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="T2" t="s">
         <v>428</v>
@@ -2553,19 +2701,19 @@
     </row>
     <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="G4" t="s">
         <v>312</v>
@@ -2589,19 +2737,19 @@
         <v>312</v>
       </c>
       <c r="N4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="O4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="P4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Q4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="R4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="S4" t="s">
         <v>312</v>
@@ -2667,55 +2815,55 @@
         <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F5" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G5" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="J5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="K5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="L5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="M5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="N5" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="O5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="P5" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="R5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="S5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="T5" t="s">
         <v>429</v>
@@ -2730,7 +2878,7 @@
         <v>387</v>
       </c>
       <c r="X5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="Y5" t="s">
         <v>381</v>
@@ -2831,55 +2979,55 @@
         <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D6" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E6" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F6" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G6" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I6" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="J6" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="K6" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="L6" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="M6" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="N6" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="O6" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="P6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="Q6" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="R6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="S6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="T6" t="s">
         <v>430</v>
@@ -2894,7 +3042,7 @@
         <v>388</v>
       </c>
       <c r="X6" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="Y6" t="s">
         <v>380</v>
@@ -2995,40 +3143,40 @@
         <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G7" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="H7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="J7" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="K7" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="L7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="M7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="O7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="P7" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="R7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="T7" t="s">
         <v>431</v>
@@ -3037,7 +3185,7 @@
         <v>410</v>
       </c>
       <c r="X7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="Z7" t="s">
         <v>374</v>
@@ -3078,7 +3226,7 @@
         <v>249</v>
       </c>
       <c r="S8" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="V8" t="s">
         <v>401</v>
@@ -3098,7 +3246,7 @@
         <v>343</v>
       </c>
       <c r="X9" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="Z9" t="s">
         <v>375</v>
@@ -3106,13 +3254,13 @@
     </row>
     <row r="10" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="O10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="P10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="11" spans="1:55" x14ac:dyDescent="0.25">
@@ -3122,22 +3270,22 @@
     </row>
     <row r="12" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="13" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="14" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="15" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -3151,9 +3299,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L143"/>
   <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J152" sqref="J152"/>
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3193,7 +3341,7 @@
         <v>22</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>148</v>
@@ -3202,7 +3350,7 @@
         <v>186</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="L1" t="s">
         <v>384</v>
@@ -3264,7 +3412,7 @@
         <v>93</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>208</v>
@@ -3690,13 +3838,13 @@
         <v>93</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I20" t="s">
         <v>142</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K20" s="10">
         <v>1</v>
@@ -3716,13 +3864,13 @@
         <v>93</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I21" t="s">
         <v>142</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="K21" s="10">
         <v>1</v>
@@ -3829,16 +3977,16 @@
         <v>93</v>
       </c>
       <c r="E25" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I25" t="s">
         <v>143</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K25" s="10">
         <v>1</v>
@@ -3863,6 +4011,9 @@
       <c r="F26" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
       <c r="I26" t="s">
         <v>141</v>
       </c>
@@ -3893,7 +4044,7 @@
         <v>141</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="K27" s="10">
         <v>1</v>
@@ -3919,7 +4070,7 @@
         <v>141</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="K28" s="10">
         <v>1</v>
@@ -3945,7 +4096,7 @@
         <v>141</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K29" s="10">
         <v>1</v>
@@ -3968,7 +4119,7 @@
         <v>141</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="K30" s="10">
         <v>1</v>
@@ -4008,13 +4159,13 @@
         <v>93</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I32" t="s">
         <v>141</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="K32" s="10">
         <v>1</v>
@@ -4247,7 +4398,7 @@
         <v>87</v>
       </c>
       <c r="I42" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J42" s="10" t="s">
         <v>378</v>
@@ -4270,7 +4421,7 @@
         <v>88</v>
       </c>
       <c r="I43" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J43" s="10" t="s">
         <v>377</v>
@@ -4293,7 +4444,7 @@
         <v>152</v>
       </c>
       <c r="I44" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J44" s="10" t="s">
         <v>376</v>
@@ -4314,7 +4465,7 @@
         <v>252</v>
       </c>
       <c r="I45" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J45" s="10" t="s">
         <v>254</v>
@@ -4335,7 +4486,7 @@
         <v>253</v>
       </c>
       <c r="I46" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J46" s="10" t="s">
         <v>255</v>
@@ -4356,7 +4507,7 @@
         <v>349</v>
       </c>
       <c r="I47" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J47" s="10" t="s">
         <v>350</v>
@@ -4377,7 +4528,7 @@
         <v>344</v>
       </c>
       <c r="I48" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J48" s="10" t="s">
         <v>347</v>
@@ -4398,7 +4549,7 @@
         <v>345</v>
       </c>
       <c r="I49" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J49" s="10" t="s">
         <v>348</v>
@@ -4419,7 +4570,7 @@
         <v>383</v>
       </c>
       <c r="I50" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J50" s="10" t="s">
         <v>382</v>
@@ -4567,13 +4718,13 @@
         <v>94</v>
       </c>
       <c r="F58" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="I58" t="s">
+        <v>558</v>
+      </c>
+      <c r="J58" s="10" t="s">
         <v>557</v>
-      </c>
-      <c r="I58" t="s">
-        <v>559</v>
-      </c>
-      <c r="J58" s="10" t="s">
-        <v>558</v>
       </c>
       <c r="K58" s="10">
         <v>1</v>
@@ -4767,7 +4918,7 @@
         <v>94</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="I69" s="10" t="s">
         <v>208</v>
@@ -4784,13 +4935,13 @@
         <v>94</v>
       </c>
       <c r="F70" s="9" t="s">
+        <v>559</v>
+      </c>
+      <c r="I70" t="s">
         <v>560</v>
       </c>
-      <c r="I70" t="s">
+      <c r="J70" t="s">
         <v>561</v>
-      </c>
-      <c r="J70" t="s">
-        <v>562</v>
       </c>
       <c r="K70" s="10">
         <v>1</v>
@@ -4801,7 +4952,7 @@
         <v>94</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I71" s="10" t="s">
         <v>208</v>
@@ -5231,13 +5382,13 @@
         <v>94</v>
       </c>
       <c r="F94" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="I94" t="s">
+        <v>572</v>
+      </c>
+      <c r="J94" t="s">
         <v>571</v>
-      </c>
-      <c r="I94" t="s">
-        <v>573</v>
-      </c>
-      <c r="J94" t="s">
-        <v>572</v>
       </c>
       <c r="K94">
         <v>1</v>
@@ -5245,19 +5396,19 @@
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D95" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F95" s="9" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I95" t="s">
+        <v>551</v>
+      </c>
+      <c r="J95" t="s">
         <v>552</v>
-      </c>
-      <c r="J95" t="s">
-        <v>553</v>
       </c>
       <c r="K95">
         <v>1</v>
@@ -5268,13 +5419,13 @@
         <v>94</v>
       </c>
       <c r="F96" s="9" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I96" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="J96" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="K96">
         <v>1</v>
@@ -5285,13 +5436,13 @@
         <v>235</v>
       </c>
       <c r="F97" s="11" t="s">
+        <v>554</v>
+      </c>
+      <c r="I97" t="s">
+        <v>551</v>
+      </c>
+      <c r="J97" t="s">
         <v>555</v>
-      </c>
-      <c r="I97" t="s">
-        <v>552</v>
-      </c>
-      <c r="J97" t="s">
-        <v>556</v>
       </c>
       <c r="K97">
         <v>1</v>
@@ -5373,19 +5524,19 @@
         <v>94</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I102" t="s">
         <v>170</v>
       </c>
       <c r="J102" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K102">
         <v>1</v>
       </c>
       <c r="L102" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="103" spans="2:12" x14ac:dyDescent="0.25">
@@ -5393,19 +5544,19 @@
         <v>94</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I103" t="s">
         <v>170</v>
       </c>
       <c r="J103" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="K103">
         <v>1</v>
       </c>
       <c r="L103" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="104" spans="2:12" x14ac:dyDescent="0.25">
@@ -5413,19 +5564,19 @@
         <v>94</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I104" t="s">
         <v>170</v>
       </c>
       <c r="J104" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K104">
         <v>1</v>
       </c>
       <c r="L104" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="105" spans="2:12" x14ac:dyDescent="0.25">
@@ -5433,19 +5584,19 @@
         <v>94</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I105" t="s">
         <v>170</v>
       </c>
       <c r="J105" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K105">
         <v>1</v>
       </c>
       <c r="L105" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="106" spans="2:12" x14ac:dyDescent="0.25">
@@ -5453,19 +5604,19 @@
         <v>94</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I106" t="s">
         <v>170</v>
       </c>
       <c r="J106" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="K106">
         <v>1</v>
       </c>
       <c r="L106" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="107" spans="2:12" x14ac:dyDescent="0.25">
@@ -5473,19 +5624,19 @@
         <v>94</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I107" t="s">
         <v>170</v>
       </c>
       <c r="J107" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="K107">
         <v>1</v>
       </c>
       <c r="L107" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="108" spans="2:12" x14ac:dyDescent="0.25">
@@ -5493,19 +5644,19 @@
         <v>94</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I108" t="s">
         <v>170</v>
       </c>
       <c r="J108" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="K108">
         <v>1</v>
       </c>
       <c r="L108" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="109" spans="2:12" x14ac:dyDescent="0.25">
@@ -5513,19 +5664,19 @@
         <v>94</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I109" t="s">
         <v>170</v>
       </c>
       <c r="J109" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="K109">
         <v>1</v>
       </c>
       <c r="L109" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="110" spans="2:12" x14ac:dyDescent="0.25">
@@ -5533,24 +5684,24 @@
         <v>94</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I110" t="s">
         <v>170</v>
       </c>
       <c r="J110" t="s">
+        <v>484</v>
+      </c>
+      <c r="K110">
+        <v>1</v>
+      </c>
+      <c r="L110" t="s">
         <v>485</v>
-      </c>
-      <c r="K110">
-        <v>1</v>
-      </c>
-      <c r="L110" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="111" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>94</v>
@@ -5559,7 +5710,7 @@
         <v>420</v>
       </c>
       <c r="I111" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J111" t="s">
         <v>422</v>
@@ -5573,10 +5724,10 @@
         <v>94</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I112" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J112" t="s">
         <v>416</v>
@@ -5593,7 +5744,7 @@
         <v>411</v>
       </c>
       <c r="I113" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J113" t="s">
         <v>415</v>
@@ -5610,13 +5761,13 @@
         <v>94</v>
       </c>
       <c r="F114" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="I114" t="s">
+        <v>449</v>
+      </c>
+      <c r="J114" t="s">
         <v>456</v>
-      </c>
-      <c r="I114" t="s">
-        <v>450</v>
-      </c>
-      <c r="J114" t="s">
-        <v>457</v>
       </c>
       <c r="K114" s="10">
         <v>1</v>
@@ -5633,7 +5784,7 @@
         <v>421</v>
       </c>
       <c r="I115" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J115" t="s">
         <v>423</v>
@@ -5650,7 +5801,7 @@
         <v>414</v>
       </c>
       <c r="I116" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J116" t="s">
         <v>193</v>
@@ -5667,7 +5818,7 @@
         <v>412</v>
       </c>
       <c r="I117" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="J117" t="s">
         <v>413</v>
@@ -5684,13 +5835,13 @@
         <v>95</v>
       </c>
       <c r="F118" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="I118" t="s">
+        <v>449</v>
+      </c>
+      <c r="J118" t="s">
         <v>448</v>
-      </c>
-      <c r="I118" t="s">
-        <v>450</v>
-      </c>
-      <c r="J118" t="s">
-        <v>449</v>
       </c>
       <c r="K118">
         <v>31</v>
@@ -5710,7 +5861,7 @@
         <v>175</v>
       </c>
       <c r="I119" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J119" s="10" t="s">
         <v>327</v>
@@ -5730,7 +5881,7 @@
         <v>176</v>
       </c>
       <c r="I120" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J120" s="10" t="s">
         <v>328</v>
@@ -5750,7 +5901,7 @@
         <v>183</v>
       </c>
       <c r="I121" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J121" s="10" t="s">
         <v>329</v>
@@ -5773,7 +5924,7 @@
         <v>209</v>
       </c>
       <c r="I122" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J122" s="10" t="s">
         <v>330</v>
@@ -5793,7 +5944,7 @@
         <v>325</v>
       </c>
       <c r="I123" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J123" s="10" t="s">
         <v>326</v>
@@ -5816,7 +5967,7 @@
         <v>237</v>
       </c>
       <c r="I124" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J124" s="10" t="s">
         <v>238</v>
@@ -5836,7 +5987,7 @@
         <v>177</v>
       </c>
       <c r="I125" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J125" t="s">
         <v>205</v>
@@ -5853,7 +6004,7 @@
         <v>178</v>
       </c>
       <c r="I126" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J126" t="s">
         <v>206</v>
@@ -5867,10 +6018,10 @@
         <v>95</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I127" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J127" t="s">
         <v>211</v>
@@ -5887,7 +6038,7 @@
         <v>184</v>
       </c>
       <c r="I128" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J128" t="s">
         <v>207</v>
@@ -5904,7 +6055,7 @@
         <v>224</v>
       </c>
       <c r="I129" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J129" t="s">
         <v>225</v>
@@ -5918,13 +6069,13 @@
         <v>95</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I130" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J130" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="K130">
         <v>69</v>
@@ -5941,7 +6092,7 @@
         <v>185</v>
       </c>
       <c r="I131" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J131" t="s">
         <v>332</v>
@@ -5961,7 +6112,7 @@
         <v>331</v>
       </c>
       <c r="I132" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J132" t="s">
         <v>333</v>
@@ -5981,7 +6132,7 @@
         <v>239</v>
       </c>
       <c r="I133" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J133" t="s">
         <v>240</v>
@@ -6001,7 +6152,7 @@
         <v>367</v>
       </c>
       <c r="I134" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J134" t="s">
         <v>368</v>
@@ -6018,7 +6169,7 @@
         <v>366</v>
       </c>
       <c r="I135" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J135" t="s">
         <v>369</v>
@@ -6032,10 +6183,10 @@
         <v>95</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I136" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="J136" t="s">
         <v>370</v>
@@ -6052,7 +6203,7 @@
         <v>217</v>
       </c>
       <c r="I137" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J137" t="s">
         <v>291</v>
@@ -6069,7 +6220,7 @@
         <v>218</v>
       </c>
       <c r="I138" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J138" t="s">
         <v>219</v>
@@ -6089,13 +6240,13 @@
         <v>94</v>
       </c>
       <c r="F139" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I139" t="s">
+        <v>475</v>
+      </c>
+      <c r="J139" s="10" t="s">
         <v>476</v>
-      </c>
-      <c r="J139" s="10" t="s">
-        <v>477</v>
       </c>
       <c r="K139" s="10">
         <v>1</v>
@@ -6109,10 +6260,10 @@
         <v>95</v>
       </c>
       <c r="F140" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="I140" t="s">
         <v>475</v>
-      </c>
-      <c r="I140" t="s">
-        <v>476</v>
       </c>
       <c r="J140" t="s">
         <v>342</v>
@@ -6135,7 +6286,7 @@
         <v>285</v>
       </c>
       <c r="I141" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J141" t="s">
         <v>288</v>
@@ -6152,7 +6303,7 @@
         <v>293</v>
       </c>
       <c r="I142" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J142" t="s">
         <v>289</v>
@@ -6172,7 +6323,7 @@
         <v>286</v>
       </c>
       <c r="I143" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J143" t="s">
         <v>287</v>
@@ -6193,292 +6344,1151 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:AX22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.5703125" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" customWidth="1"/>
-    <col min="5" max="5" width="41.85546875" customWidth="1"/>
-    <col min="6" max="6" width="39.42578125" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" customWidth="1"/>
-    <col min="13" max="13" width="33.5703125" customWidth="1"/>
+    <col min="1" max="2" width="49.5703125" customWidth="1"/>
+    <col min="3" max="4" width="29.5703125" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" customWidth="1"/>
+    <col min="6" max="10" width="29.5703125" customWidth="1"/>
+    <col min="11" max="11" width="28.140625" customWidth="1"/>
+    <col min="12" max="12" width="29.5703125" customWidth="1"/>
+    <col min="13" max="13" width="25" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" customWidth="1"/>
+    <col min="16" max="16" width="32.7109375" customWidth="1"/>
+    <col min="18" max="18" width="29.5703125" customWidth="1"/>
+    <col min="19" max="19" width="30.140625" customWidth="1"/>
+    <col min="20" max="20" width="29.42578125" customWidth="1"/>
+    <col min="21" max="21" width="29" customWidth="1"/>
+    <col min="22" max="22" width="38.42578125" customWidth="1"/>
+    <col min="23" max="23" width="22.42578125" customWidth="1"/>
+    <col min="24" max="24" width="22.28515625" customWidth="1"/>
+    <col min="25" max="25" width="29.140625" customWidth="1"/>
+    <col min="26" max="26" width="29.85546875" customWidth="1"/>
+    <col min="27" max="28" width="37.42578125" customWidth="1"/>
+    <col min="29" max="29" width="25" customWidth="1"/>
+    <col min="30" max="30" width="22.140625" customWidth="1"/>
+    <col min="31" max="31" width="35.140625" customWidth="1"/>
+    <col min="32" max="32" width="24.42578125" customWidth="1"/>
+    <col min="33" max="33" width="29" customWidth="1"/>
+    <col min="34" max="34" width="28.140625" customWidth="1"/>
+    <col min="35" max="35" width="29.42578125" customWidth="1"/>
+    <col min="36" max="36" width="28.28515625" customWidth="1"/>
+    <col min="37" max="37" width="31.42578125" customWidth="1"/>
+    <col min="38" max="39" width="28.28515625" customWidth="1"/>
+    <col min="40" max="40" width="24" customWidth="1"/>
+    <col min="41" max="41" width="31.7109375" customWidth="1"/>
+    <col min="42" max="42" width="31.140625" customWidth="1"/>
+    <col min="43" max="43" width="22.5703125" customWidth="1"/>
+    <col min="44" max="44" width="26.140625" customWidth="1"/>
+    <col min="45" max="45" width="26" customWidth="1"/>
+    <col min="46" max="46" width="22.28515625" customWidth="1"/>
+    <col min="47" max="47" width="26" customWidth="1"/>
+    <col min="48" max="48" width="23.42578125" customWidth="1"/>
+    <col min="49" max="49" width="35.42578125" customWidth="1"/>
+    <col min="50" max="50" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>582</v>
+    <row r="1" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>581</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>585</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>586</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="V1" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="X1" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="Y1" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="Z1" s="15" t="s">
+        <v>590</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="AB1" s="15" t="s">
+        <v>592</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="AD1" s="15" t="s">
+        <v>594</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="AF1" s="15" t="s">
+        <v>596</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="AH1" s="15" t="s">
+        <v>598</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="AJ1" s="15" t="s">
+        <v>629</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="AL1" s="15" t="s">
+        <v>600</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="AN1" s="15" t="s">
+        <v>602</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="AP1" s="15" t="s">
+        <v>604</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="AR1" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="AS1" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="AT1" s="15" t="s">
+        <v>608</v>
+      </c>
+      <c r="AU1" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="AV1" s="15" t="s">
+        <v>610</v>
+      </c>
+      <c r="AW1" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="AX1" s="15" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="L2" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D2" t="s">
+      <c r="S2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="F2" t="s">
+      <c r="U2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="V2" t="s">
+        <v>233</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y2" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO2" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="17"/>
+      <c r="E3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="L3" s="17"/>
+      <c r="N3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="R3" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="S3" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="F3" t="s">
+      <c r="U3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="V3" t="s">
+        <v>236</v>
+      </c>
+      <c r="W3" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="X3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y3" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC3" s="18" t="s">
+        <v>564</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE3" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="AF3" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG3" s="18" t="s">
+        <v>549</v>
+      </c>
+      <c r="AH3" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK3" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="AL3" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AQ3" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="AR3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS3" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AV3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="N4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="R4" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="S4" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="F4" t="s">
+      <c r="U4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="V4" t="s">
+        <v>89</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="X4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE4" s="18" t="s">
+        <v>565</v>
+      </c>
+      <c r="AF4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK4" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="AL4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AO4" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AR4" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="AS4" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>349</v>
+      </c>
+      <c r="AV4" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="R5" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="S5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="T5" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F5" t="s">
+      <c r="U5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+      <c r="V5" t="s">
+        <v>30</v>
+      </c>
+      <c r="X5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD5" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="AE5" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF5" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="AI5" s="20"/>
+      <c r="AJ5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AK5" s="18" t="s">
+        <v>455</v>
+      </c>
+      <c r="AL5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AO5" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>344</v>
+      </c>
+      <c r="AV5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AX5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="R6" s="18" t="s">
         <v>325</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="S6" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="T6" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="F6" t="s">
+      <c r="U6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="V6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X6" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE6" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK6" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="AL6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO6" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="AP6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AT6" t="s">
+        <v>345</v>
+      </c>
+      <c r="AV6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="R7" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="S7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="T7" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="F7" t="s">
+      <c r="U7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="V7" t="s">
+        <v>65</v>
+      </c>
+      <c r="X7" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE7" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="AF7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK7" s="18" t="s">
+        <v>421</v>
+      </c>
+      <c r="AL7" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO7" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AV7" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="R8" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="S8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="T8" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F8" t="s">
+      <c r="U8" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="17" t="s">
+      <c r="V8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK8" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="AL8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AO8" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="AP8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AV8" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="R9" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="S9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="T9" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F9" t="s">
+      <c r="U9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="17" t="s">
-        <v>461</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="V9" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK9" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="AL9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO9" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="AP9" t="s">
+        <v>233</v>
+      </c>
+      <c r="AV9" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="R10" s="18" t="s">
+        <v>460</v>
+      </c>
+      <c r="S10" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="T10" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F10" t="s">
+      <c r="U10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="17" t="s">
+      <c r="V10" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>548</v>
+      </c>
+      <c r="AD10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK10" s="18" t="s">
+        <v>447</v>
+      </c>
+      <c r="AL10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO10" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="AP10" t="s">
+        <v>232</v>
+      </c>
+      <c r="AV10" s="10" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="R11" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="S11" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="T11" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F11" t="s">
+      <c r="U11" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="17" t="s">
+      <c r="V11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK11" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="AL11" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="AO11" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="AP11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="R12" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="S12" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="T12" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F12" t="s">
+      <c r="U12" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="17" t="s">
-        <v>537</v>
-      </c>
-      <c r="D13" s="10" t="s">
+      <c r="V12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD12" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF12" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ12" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL12" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="AO12" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="AP12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="R13" s="18" t="s">
+        <v>536</v>
+      </c>
+      <c r="S13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="T13" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F13" t="s">
+      <c r="U13" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="17" t="s">
+      <c r="V13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ13" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO13" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="AP13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="R14" s="18" t="s">
         <v>185</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="S14" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="T14" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="F14" t="s">
+      <c r="U14" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="17" t="s">
+      <c r="V14" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF14" s="10" t="s">
+        <v>548</v>
+      </c>
+      <c r="AL14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="AP14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="R15" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="S15" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="T15" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="F15" t="s">
+      <c r="U15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="17" t="s">
+      <c r="V15" t="s">
+        <v>253</v>
+      </c>
+      <c r="AL15" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="R16" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="S16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F16" t="s">
+      <c r="U16" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="10" t="s">
+      <c r="V16" t="s">
+        <v>349</v>
+      </c>
+      <c r="AL16" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F17" t="s">
+    </row>
+    <row r="17" spans="19:38" x14ac:dyDescent="0.25">
+      <c r="S17" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="U17" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="10" t="s">
+      <c r="V17" t="s">
         <v>54</v>
       </c>
-      <c r="F18" t="s">
+      <c r="AL17" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="19:38" x14ac:dyDescent="0.25">
+      <c r="S18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="U18" t="s">
         <v>210</v>
+      </c>
+      <c r="AL18" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="19:38" x14ac:dyDescent="0.25">
+      <c r="AC19" s="19"/>
+      <c r="AD19" s="10"/>
+      <c r="AL19" s="10" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="20" spans="19:38" x14ac:dyDescent="0.25">
+      <c r="AL20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="19:38" x14ac:dyDescent="0.25">
+      <c r="AL21" s="10" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="22" spans="19:38" x14ac:dyDescent="0.25">
+      <c r="AL22" s="10" t="s">
+        <v>548</v>
       </c>
     </row>
   </sheetData>
@@ -6493,13 +7503,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B21"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="111" customWidth="1"/>
+    <col min="2" max="2" width="142" customWidth="1"/>
     <col min="3" max="3" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6508,10 +7518,10 @@
         <v>78</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>577</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6519,10 +7529,10 @@
         <v>432</v>
       </c>
       <c r="B2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -6530,10 +7540,10 @@
         <v>433</v>
       </c>
       <c r="B3" t="s">
+        <v>628</v>
+      </c>
+      <c r="C3" t="s">
         <v>434</v>
-      </c>
-      <c r="C3" t="s">
-        <v>435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chassis, maps, switch collection refactoring
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -14,15 +14,14 @@
     <sheet name="software" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">project_steps!$A$3:$L$145</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">project_steps!$A$3:$L$146</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="646">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -1954,6 +1953,12 @@
   </si>
   <si>
     <t>3par</t>
+  </si>
+  <si>
+    <t>chassis_slots</t>
+  </si>
+  <si>
+    <t>Chassis slots collection</t>
   </si>
 </sst>
 </file>
@@ -2482,8 +2487,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BC17"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3432,11 +3437,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:L145"/>
+  <dimension ref="A1:L146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H65" sqref="H65"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3636,29 +3641,19 @@
       <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>171</v>
-      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
       <c r="F11" s="2" t="s">
-        <v>26</v>
+        <v>644</v>
       </c>
       <c r="I11" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>336</v>
+        <v>645</v>
       </c>
       <c r="K11" s="10"/>
     </row>
@@ -3676,70 +3671,73 @@
         <v>93</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
       </c>
       <c r="I12" t="s">
         <v>149</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>93</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K13" s="10"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>13</v>
+        <v>173</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>93</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="I14" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="K14" s="10"/>
     </row>
@@ -3757,70 +3755,70 @@
         <v>93</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="I15" t="s">
         <v>146</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>93</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="I16" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="K16" s="10"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>127</v>
+        <v>30</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="I17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K17" s="10"/>
     </row>
@@ -3838,43 +3836,43 @@
         <v>93</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I18" t="s">
         <v>145</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K18" s="10"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>93</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="I19" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>315</v>
+        <v>392</v>
       </c>
       <c r="K19" s="10"/>
     </row>
@@ -3892,16 +3890,16 @@
         <v>93</v>
       </c>
       <c r="E20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I20" t="s">
         <v>142</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>363</v>
+        <v>315</v>
       </c>
       <c r="K20" s="10"/>
     </row>
@@ -3919,16 +3917,16 @@
         <v>93</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I21" t="s">
         <v>142</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K21" s="10"/>
     </row>
@@ -3945,14 +3943,17 @@
       <c r="D22" s="4" t="s">
         <v>93</v>
       </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
       <c r="F22" s="2" t="s">
-        <v>501</v>
+        <v>34</v>
       </c>
       <c r="I22" t="s">
         <v>142</v>
       </c>
       <c r="J22" s="10" t="s">
-        <v>520</v>
+        <v>364</v>
       </c>
       <c r="K22" s="10"/>
     </row>
@@ -3970,40 +3971,37 @@
         <v>93</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>519</v>
+        <v>501</v>
       </c>
       <c r="I23" t="s">
         <v>142</v>
       </c>
       <c r="J23" s="10" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="K23" s="10"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E24" t="s">
-        <v>35</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>40</v>
+        <v>519</v>
       </c>
       <c r="I24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>393</v>
+        <v>521</v>
       </c>
       <c r="K24" s="10"/>
     </row>
@@ -4021,16 +4019,16 @@
         <v>93</v>
       </c>
       <c r="E25" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I25" t="s">
         <v>143</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K25" s="10"/>
     </row>
@@ -4048,16 +4046,16 @@
         <v>93</v>
       </c>
       <c r="E26" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="I26" t="s">
         <v>143</v>
       </c>
       <c r="J26" s="10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K26" s="10"/>
     </row>
@@ -4075,43 +4073,43 @@
         <v>93</v>
       </c>
       <c r="E27" t="s">
-        <v>435</v>
+        <v>31</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>435</v>
+        <v>31</v>
       </c>
       <c r="I27" t="s">
         <v>143</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>436</v>
+        <v>395</v>
       </c>
       <c r="K27" s="10"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>121</v>
+        <v>40</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>93</v>
       </c>
       <c r="E28" t="s">
-        <v>17</v>
+        <v>435</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>43</v>
+        <v>435</v>
       </c>
       <c r="I28" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="J28" s="10" t="s">
-        <v>396</v>
+        <v>436</v>
       </c>
       <c r="K28" s="10"/>
     </row>
@@ -4128,14 +4126,17 @@
       <c r="D29" s="4" t="s">
         <v>93</v>
       </c>
+      <c r="E29" t="s">
+        <v>17</v>
+      </c>
       <c r="F29" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I29" t="s">
         <v>141</v>
       </c>
       <c r="J29" s="10" t="s">
-        <v>441</v>
+        <v>396</v>
       </c>
       <c r="K29" s="10"/>
     </row>
@@ -4153,13 +4154,13 @@
         <v>93</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I30" t="s">
         <v>141</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="K30" s="10"/>
     </row>
@@ -4177,17 +4178,20 @@
         <v>93</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I31" t="s">
         <v>141</v>
       </c>
       <c r="J31" s="10" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="K31" s="10"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>12</v>
+      </c>
       <c r="B32" s="4" t="s">
         <v>122</v>
       </c>
@@ -4198,13 +4202,13 @@
         <v>93</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I32" t="s">
         <v>141</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="K32" s="10"/>
     </row>
@@ -4219,13 +4223,13 @@
         <v>93</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I33" t="s">
         <v>141</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>208</v>
+        <v>443</v>
       </c>
       <c r="K33" s="10"/>
     </row>
@@ -4240,41 +4244,41 @@
         <v>93</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>567</v>
+        <v>48</v>
       </c>
       <c r="I34" t="s">
         <v>141</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>568</v>
+        <v>208</v>
       </c>
       <c r="K34" s="10"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>13</v>
-      </c>
       <c r="B35" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>93</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>49</v>
+        <v>567</v>
       </c>
       <c r="I35" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>356</v>
+        <v>568</v>
       </c>
       <c r="K35" s="10"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>13</v>
+      </c>
       <c r="B36" s="4" t="s">
         <v>125</v>
       </c>
@@ -4285,13 +4289,13 @@
         <v>93</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I36" t="s">
         <v>147</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K36" s="10"/>
     </row>
@@ -4306,13 +4310,13 @@
         <v>93</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I37" t="s">
         <v>147</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K37" s="10"/>
     </row>
@@ -4327,13 +4331,13 @@
         <v>93</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I38" t="s">
         <v>147</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K38" s="10"/>
     </row>
@@ -4348,13 +4352,13 @@
         <v>93</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I39" t="s">
         <v>147</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K39" s="10"/>
     </row>
@@ -4369,13 +4373,13 @@
         <v>93</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>230</v>
+        <v>52</v>
       </c>
       <c r="I40" t="s">
         <v>147</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K40" s="10"/>
     </row>
@@ -4390,83 +4394,83 @@
         <v>93</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="I41" t="s">
         <v>147</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K41" s="10"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>214</v>
+        <v>125</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>215</v>
+        <v>124</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>93</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="I42" t="s">
-        <v>216</v>
+        <v>147</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="K42" s="10"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
-        <v>282</v>
+        <v>214</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>283</v>
+        <v>215</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>93</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>279</v>
+        <v>215</v>
       </c>
       <c r="I43" t="s">
-        <v>280</v>
+        <v>216</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>281</v>
+        <v>355</v>
       </c>
       <c r="K43" s="10"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>19</v>
-      </c>
       <c r="B44" s="4" t="s">
-        <v>113</v>
+        <v>282</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>129</v>
+        <v>283</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>93</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>87</v>
+        <v>279</v>
       </c>
       <c r="I44" t="s">
-        <v>444</v>
+        <v>280</v>
       </c>
       <c r="J44" s="10" t="s">
-        <v>378</v>
+        <v>281</v>
       </c>
       <c r="K44" s="10"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>19</v>
+      </c>
       <c r="B45" s="4" t="s">
         <v>113</v>
       </c>
@@ -4477,13 +4481,13 @@
         <v>93</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I45" t="s">
         <v>444</v>
       </c>
       <c r="J45" s="10" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="K45" s="10"/>
     </row>
@@ -4498,34 +4502,34 @@
         <v>93</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>152</v>
+        <v>88</v>
       </c>
       <c r="I46" t="s">
         <v>444</v>
       </c>
       <c r="J46" s="10" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="K46" s="10"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
-        <v>251</v>
+        <v>113</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>642</v>
+        <v>129</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>93</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>252</v>
+        <v>152</v>
       </c>
       <c r="I47" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J47" s="10" t="s">
-        <v>254</v>
+        <v>376</v>
       </c>
       <c r="K47" s="10"/>
     </row>
@@ -4540,34 +4544,34 @@
         <v>93</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I48" t="s">
         <v>445</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K48" s="10"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
-        <v>346</v>
+        <v>251</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>93</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>349</v>
+        <v>253</v>
       </c>
       <c r="I49" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J49" s="10" t="s">
-        <v>350</v>
+        <v>255</v>
       </c>
       <c r="K49" s="10"/>
     </row>
@@ -4582,13 +4586,13 @@
         <v>93</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="I50" t="s">
         <v>446</v>
       </c>
       <c r="J50" s="10" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="K50" s="10"/>
     </row>
@@ -4603,13 +4607,13 @@
         <v>93</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I51" t="s">
         <v>446</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K51" s="10"/>
     </row>
@@ -4624,43 +4628,49 @@
         <v>93</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>383</v>
+        <v>345</v>
       </c>
       <c r="I52" t="s">
         <v>446</v>
       </c>
       <c r="J52" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="K52" s="10"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="I53" t="s">
+        <v>446</v>
+      </c>
+      <c r="J53" s="10" t="s">
         <v>382</v>
       </c>
-      <c r="K52" s="10"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="K53" s="10"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54">
         <v>15</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>136</v>
       </c>
-      <c r="D53" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="I53" t="s">
-        <v>157</v>
-      </c>
-      <c r="J53" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="K53" s="10"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D54" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>419</v>
+        <v>54</v>
       </c>
       <c r="I54" t="s">
         <v>157</v>
@@ -4674,14 +4684,14 @@
       <c r="D55" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F55" s="8" t="s">
-        <v>55</v>
+      <c r="F55" s="9" t="s">
+        <v>419</v>
       </c>
       <c r="I55" t="s">
         <v>157</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>292</v>
+        <v>208</v>
       </c>
       <c r="K55" s="10"/>
     </row>
@@ -4690,84 +4700,84 @@
         <v>94</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I56" t="s">
         <v>157</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>208</v>
+        <v>292</v>
       </c>
       <c r="K56" s="10"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>160</v>
-      </c>
       <c r="D57" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F57" s="9" t="s">
+      <c r="F57" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I57" t="s">
+        <v>157</v>
+      </c>
+      <c r="J57" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="K57" s="10"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>160</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F58" s="9" t="s">
         <v>158</v>
-      </c>
-      <c r="I57" t="s">
-        <v>161</v>
-      </c>
-      <c r="J57" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="K57" s="10"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D58" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>159</v>
       </c>
       <c r="I58" t="s">
         <v>161</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J58" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="K58" s="10"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D59" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I59" t="s">
+        <v>161</v>
+      </c>
+      <c r="J59" t="s">
         <v>195</v>
       </c>
-      <c r="K58">
+      <c r="K59">
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60">
         <v>16</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>138</v>
       </c>
-      <c r="D59" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="I59" t="s">
-        <v>167</v>
-      </c>
-      <c r="J59" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="K59" s="10"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D60" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>555</v>
+        <v>65</v>
       </c>
       <c r="I60" t="s">
-        <v>557</v>
+        <v>167</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>556</v>
+        <v>276</v>
       </c>
       <c r="K60" s="10"/>
     </row>
@@ -4775,68 +4785,66 @@
       <c r="D61" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E61" s="16"/>
-      <c r="F61" s="2" t="s">
-        <v>424</v>
+      <c r="F61" s="9" t="s">
+        <v>555</v>
       </c>
       <c r="I61" t="s">
-        <v>167</v>
+        <v>557</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>425</v>
+        <v>556</v>
       </c>
       <c r="K61" s="10"/>
-      <c r="L61" t="s">
-        <v>384</v>
-      </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D62" s="6" t="s">
         <v>94</v>
       </c>
+      <c r="E62" s="16"/>
       <c r="F62" s="2" t="s">
-        <v>162</v>
+        <v>424</v>
       </c>
       <c r="I62" t="s">
         <v>167</v>
       </c>
       <c r="J62" s="10" t="s">
-        <v>208</v>
+        <v>425</v>
       </c>
       <c r="K62" s="10"/>
+      <c r="L62" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D63" s="5" t="s">
-        <v>95</v>
+      <c r="D63" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>60</v>
+        <v>162</v>
       </c>
       <c r="I63" t="s">
         <v>167</v>
       </c>
-      <c r="J63" t="s">
-        <v>187</v>
-      </c>
-      <c r="K63">
-        <v>12</v>
-      </c>
+      <c r="J63" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="K63" s="10"/>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D64" s="5" t="s">
         <v>95</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I64" t="s">
         <v>167</v>
       </c>
       <c r="J64" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K64">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -4844,16 +4852,16 @@
         <v>95</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I65" t="s">
         <v>167</v>
       </c>
       <c r="J65" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="K65">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -4861,16 +4869,16 @@
         <v>95</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I66" t="s">
         <v>167</v>
       </c>
       <c r="J66" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K66">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -4878,16 +4886,16 @@
         <v>95</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I67" t="s">
         <v>167</v>
       </c>
       <c r="J67" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="K67">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -4895,16 +4903,16 @@
         <v>95</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>417</v>
+        <v>63</v>
       </c>
       <c r="I68" t="s">
         <v>167</v>
       </c>
       <c r="J68" t="s">
-        <v>418</v>
+        <v>189</v>
       </c>
       <c r="K68">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -4912,54 +4920,56 @@
         <v>95</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="I69" t="s">
         <v>167</v>
       </c>
       <c r="J69" t="s">
+        <v>418</v>
+      </c>
+      <c r="K69">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D70" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="I70" t="s">
+        <v>167</v>
+      </c>
+      <c r="J70" t="s">
         <v>426</v>
       </c>
-      <c r="K69">
+      <c r="K70">
         <v>11</v>
       </c>
-      <c r="L69" t="s">
+      <c r="L70" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71">
         <v>18</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>137</v>
       </c>
-      <c r="D70" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F70" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="I70" t="s">
-        <v>168</v>
-      </c>
-      <c r="J70" t="s">
-        <v>275</v>
-      </c>
-      <c r="K70" s="10"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D71" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>563</v>
-      </c>
-      <c r="I71" s="10" t="s">
-        <v>208</v>
+        <v>68</v>
+      </c>
+      <c r="I71" t="s">
+        <v>168</v>
       </c>
       <c r="J71" t="s">
-        <v>47</v>
+        <v>275</v>
       </c>
       <c r="K71" s="10"/>
     </row>
@@ -4968,13 +4978,13 @@
         <v>94</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>558</v>
-      </c>
-      <c r="I72" t="s">
-        <v>559</v>
+        <v>563</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>208</v>
       </c>
       <c r="J72" t="s">
-        <v>560</v>
+        <v>47</v>
       </c>
       <c r="K72" s="10"/>
     </row>
@@ -4983,13 +4993,13 @@
         <v>94</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>564</v>
-      </c>
-      <c r="I73" s="10" t="s">
-        <v>208</v>
+        <v>558</v>
+      </c>
+      <c r="I73" t="s">
+        <v>559</v>
       </c>
       <c r="J73" t="s">
-        <v>47</v>
+        <v>560</v>
       </c>
       <c r="K73" s="10"/>
     </row>
@@ -4998,34 +5008,32 @@
         <v>94</v>
       </c>
       <c r="F74" s="9" t="s">
+        <v>564</v>
+      </c>
+      <c r="I74" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="J74" t="s">
+        <v>47</v>
+      </c>
+      <c r="K74" s="10"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D75" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F75" s="9" t="s">
         <v>273</v>
-      </c>
-      <c r="I74" t="s">
-        <v>168</v>
-      </c>
-      <c r="J74" t="s">
-        <v>274</v>
-      </c>
-      <c r="K74" s="10"/>
-      <c r="L74" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D75" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="I75" t="s">
         <v>168</v>
       </c>
       <c r="J75" t="s">
-        <v>198</v>
-      </c>
-      <c r="K75">
-        <v>35</v>
+        <v>274</v>
+      </c>
+      <c r="K75" s="10"/>
+      <c r="L75" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
@@ -5033,16 +5041,16 @@
         <v>95</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I76" t="s">
         <v>168</v>
       </c>
       <c r="J76" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K76">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -5050,75 +5058,71 @@
         <v>95</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>277</v>
+        <v>67</v>
       </c>
       <c r="I77" t="s">
         <v>168</v>
       </c>
       <c r="J77" t="s">
+        <v>199</v>
+      </c>
+      <c r="K77">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D78" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="I78" t="s">
+        <v>168</v>
+      </c>
+      <c r="J78" t="s">
         <v>278</v>
       </c>
-      <c r="K77">
+      <c r="K78">
         <v>32</v>
       </c>
-      <c r="L77" t="s">
+      <c r="L78" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79">
         <v>20</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>130</v>
       </c>
-      <c r="D78" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F78" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="H78">
-        <v>1</v>
-      </c>
-      <c r="I78" t="s">
-        <v>169</v>
-      </c>
-      <c r="J78" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="K78" s="10"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D79" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>406</v>
+        <v>89</v>
       </c>
       <c r="I79" t="s">
         <v>169</v>
       </c>
       <c r="J79" s="10" t="s">
-        <v>403</v>
+        <v>256</v>
       </c>
       <c r="K79" s="10"/>
-      <c r="L79" t="s">
-        <v>384</v>
-      </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D80" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>259</v>
+        <v>406</v>
       </c>
       <c r="I80" t="s">
         <v>169</v>
       </c>
       <c r="J80" s="10" t="s">
-        <v>260</v>
+        <v>403</v>
       </c>
       <c r="K80" s="10"/>
       <c r="L80" t="s">
@@ -5129,38 +5133,41 @@
       <c r="D81" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F81" s="2" t="s">
-        <v>232</v>
+      <c r="F81" s="9" t="s">
+        <v>259</v>
       </c>
       <c r="I81" t="s">
         <v>169</v>
       </c>
       <c r="J81" s="10" t="s">
-        <v>324</v>
+        <v>260</v>
       </c>
       <c r="K81" s="10"/>
+      <c r="L81" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D82" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I82" t="s">
         <v>169</v>
       </c>
       <c r="J82" s="10" t="s">
-        <v>234</v>
+        <v>324</v>
       </c>
       <c r="K82" s="10"/>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D83" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="F83" s="11" t="s">
-        <v>236</v>
+      <c r="D83" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="I83" t="s">
         <v>169</v>
@@ -5171,114 +5178,112 @@
       <c r="K83" s="10"/>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
-        <v>132</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F84" s="8" t="s">
-        <v>108</v>
+      <c r="D84" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="F84" s="11" t="s">
+        <v>236</v>
       </c>
       <c r="I84" t="s">
         <v>169</v>
       </c>
       <c r="J84" s="10" t="s">
-        <v>365</v>
+        <v>234</v>
       </c>
       <c r="K84" s="10"/>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>118</v>
-      </c>
-      <c r="C85" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F85" s="7" t="s">
-        <v>92</v>
+      <c r="F85" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="I85" t="s">
         <v>169</v>
       </c>
       <c r="J85" s="10" t="s">
-        <v>323</v>
+        <v>365</v>
       </c>
       <c r="K85" s="10"/>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>118</v>
+      </c>
+      <c r="C86" t="s">
+        <v>131</v>
+      </c>
       <c r="D86" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>298</v>
+        <v>92</v>
       </c>
       <c r="I86" t="s">
         <v>169</v>
       </c>
       <c r="J86" s="10" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="K86" s="10"/>
     </row>
     <row r="87" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>133</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>402</v>
+      <c r="D87" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>298</v>
       </c>
       <c r="I87" t="s">
         <v>169</v>
       </c>
-      <c r="J87" t="s">
-        <v>190</v>
-      </c>
-      <c r="K87">
-        <v>17</v>
-      </c>
+      <c r="J87" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="K87" s="10"/>
     </row>
     <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>95</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>100</v>
+        <v>402</v>
       </c>
       <c r="I88" t="s">
         <v>169</v>
       </c>
       <c r="J88" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K88">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>134</v>
+      </c>
       <c r="D89" s="5" t="s">
         <v>95</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I89" t="s">
         <v>169</v>
       </c>
       <c r="J89" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K89">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="2:12" x14ac:dyDescent="0.25">
@@ -5286,16 +5291,16 @@
         <v>95</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I90" t="s">
         <v>169</v>
       </c>
       <c r="J90" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="K90">
-        <v>57</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="2:12" x14ac:dyDescent="0.25">
@@ -5303,16 +5308,16 @@
         <v>95</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I91" t="s">
         <v>169</v>
       </c>
       <c r="J91" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K91">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="92" spans="2:12" x14ac:dyDescent="0.25">
@@ -5320,16 +5325,16 @@
         <v>95</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I92" t="s">
         <v>169</v>
       </c>
       <c r="J92" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K92">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="93" spans="2:12" x14ac:dyDescent="0.25">
@@ -5337,16 +5342,16 @@
         <v>95</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I93" t="s">
         <v>169</v>
       </c>
       <c r="J93" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K93">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="94" spans="2:12" x14ac:dyDescent="0.25">
@@ -5354,19 +5359,16 @@
         <v>95</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>405</v>
+        <v>105</v>
       </c>
       <c r="I94" t="s">
         <v>169</v>
       </c>
       <c r="J94" t="s">
-        <v>404</v>
+        <v>203</v>
       </c>
       <c r="K94">
-        <v>53</v>
-      </c>
-      <c r="L94" t="s">
-        <v>384</v>
+        <v>56</v>
       </c>
     </row>
     <row r="95" spans="2:12" x14ac:dyDescent="0.25">
@@ -5374,130 +5376,133 @@
         <v>95</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>261</v>
+        <v>405</v>
       </c>
       <c r="I95" t="s">
         <v>169</v>
       </c>
       <c r="J95" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="K95">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L95" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="96" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D96" s="6" t="s">
-        <v>94</v>
+      <c r="D96" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>569</v>
+        <v>261</v>
       </c>
       <c r="I96" t="s">
-        <v>571</v>
+        <v>169</v>
       </c>
       <c r="J96" t="s">
-        <v>570</v>
+        <v>397</v>
+      </c>
+      <c r="K96">
+        <v>52</v>
+      </c>
+      <c r="L96" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="97" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>549</v>
-      </c>
       <c r="D97" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F97" s="9" t="s">
-        <v>547</v>
+      <c r="F97" s="2" t="s">
+        <v>569</v>
       </c>
       <c r="I97" t="s">
-        <v>550</v>
+        <v>571</v>
       </c>
       <c r="J97" t="s">
-        <v>551</v>
+        <v>570</v>
       </c>
     </row>
     <row r="98" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>549</v>
+      </c>
       <c r="D98" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F98" s="9" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I98" t="s">
         <v>550</v>
       </c>
       <c r="J98" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="99" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D99" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="F99" s="11" t="s">
-        <v>553</v>
+      <c r="D99" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F99" s="9" t="s">
+        <v>548</v>
       </c>
       <c r="I99" t="s">
         <v>550</v>
       </c>
       <c r="J99" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D100" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="F100" s="11" t="s">
+        <v>553</v>
+      </c>
+      <c r="I100" t="s">
+        <v>550</v>
+      </c>
+      <c r="J100" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
+    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
         <v>163</v>
       </c>
-      <c r="D100" s="6" t="s">
+      <c r="D101" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F100" s="9" t="s">
+      <c r="F101" s="9" t="s">
         <v>210</v>
-      </c>
-      <c r="I100" t="s">
-        <v>170</v>
-      </c>
-      <c r="J100" t="s">
-        <v>290</v>
-      </c>
-      <c r="K100" s="10"/>
-    </row>
-    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D101" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="I101" t="s">
         <v>170</v>
       </c>
       <c r="J101" t="s">
-        <v>194</v>
-      </c>
-      <c r="K101">
-        <v>41</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="K101" s="10"/>
     </row>
     <row r="102" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D102" s="5" t="s">
         <v>95</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I102" t="s">
         <v>170</v>
       </c>
       <c r="J102" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="K102">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="103" spans="2:12" x14ac:dyDescent="0.25">
@@ -5505,33 +5510,33 @@
         <v>95</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I103" t="s">
         <v>170</v>
       </c>
       <c r="J103" t="s">
-        <v>257</v>
+        <v>204</v>
       </c>
       <c r="K103">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="104" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D104" s="6" t="s">
-        <v>94</v>
+      <c r="D104" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>485</v>
+        <v>166</v>
       </c>
       <c r="I104" t="s">
         <v>170</v>
       </c>
       <c r="J104" t="s">
-        <v>476</v>
-      </c>
-      <c r="L104" t="s">
-        <v>484</v>
+        <v>257</v>
+      </c>
+      <c r="K104">
+        <v>42</v>
       </c>
     </row>
     <row r="105" spans="2:12" x14ac:dyDescent="0.25">
@@ -5539,13 +5544,13 @@
         <v>94</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I105" t="s">
         <v>170</v>
       </c>
       <c r="J105" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="L105" t="s">
         <v>484</v>
@@ -5556,13 +5561,13 @@
         <v>94</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I106" t="s">
         <v>170</v>
       </c>
       <c r="J106" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="L106" t="s">
         <v>484</v>
@@ -5573,13 +5578,13 @@
         <v>94</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I107" t="s">
         <v>170</v>
       </c>
       <c r="J107" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="L107" t="s">
         <v>484</v>
@@ -5590,13 +5595,13 @@
         <v>94</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I108" t="s">
         <v>170</v>
       </c>
       <c r="J108" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="L108" t="s">
         <v>484</v>
@@ -5607,13 +5612,13 @@
         <v>94</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I109" t="s">
         <v>170</v>
       </c>
       <c r="J109" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L109" t="s">
         <v>484</v>
@@ -5624,13 +5629,13 @@
         <v>94</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="I110" t="s">
         <v>170</v>
       </c>
       <c r="J110" t="s">
-        <v>502</v>
+        <v>481</v>
       </c>
       <c r="L110" t="s">
         <v>484</v>
@@ -5641,13 +5646,13 @@
         <v>94</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="I111" t="s">
         <v>170</v>
       </c>
       <c r="J111" t="s">
-        <v>482</v>
+        <v>502</v>
       </c>
       <c r="L111" t="s">
         <v>484</v>
@@ -5658,48 +5663,50 @@
         <v>94</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I112" t="s">
         <v>170</v>
       </c>
       <c r="J112" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L112" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="113" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B113" t="s">
-        <v>454</v>
-      </c>
       <c r="D113" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>420</v>
+        <v>492</v>
       </c>
       <c r="I113" t="s">
-        <v>449</v>
+        <v>170</v>
       </c>
       <c r="J113" t="s">
-        <v>422</v>
-      </c>
-      <c r="K113" s="10"/>
+        <v>483</v>
+      </c>
+      <c r="L113" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="114" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>454</v>
+      </c>
       <c r="D114" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>511</v>
+        <v>420</v>
       </c>
       <c r="I114" t="s">
         <v>449</v>
       </c>
       <c r="J114" t="s">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="K114" s="10"/>
     </row>
@@ -5708,31 +5715,28 @@
         <v>94</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>411</v>
+        <v>511</v>
       </c>
       <c r="I115" t="s">
         <v>449</v>
       </c>
       <c r="J115" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="K115" s="10"/>
-      <c r="L115" t="s">
-        <v>384</v>
-      </c>
     </row>
     <row r="116" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D116" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>455</v>
+        <v>411</v>
       </c>
       <c r="I116" t="s">
         <v>449</v>
       </c>
       <c r="J116" t="s">
-        <v>456</v>
+        <v>415</v>
       </c>
       <c r="K116" s="10"/>
       <c r="L116" t="s">
@@ -5740,20 +5744,21 @@
       </c>
     </row>
     <row r="117" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D117" s="5" t="s">
-        <v>95</v>
+      <c r="D117" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>421</v>
+        <v>455</v>
       </c>
       <c r="I117" t="s">
         <v>449</v>
       </c>
       <c r="J117" t="s">
-        <v>423</v>
-      </c>
-      <c r="K117">
-        <v>44</v>
+        <v>456</v>
+      </c>
+      <c r="K117" s="10"/>
+      <c r="L117" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="118" spans="2:12" x14ac:dyDescent="0.25">
@@ -5761,16 +5766,16 @@
         <v>95</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="I118" t="s">
         <v>449</v>
       </c>
       <c r="J118" t="s">
-        <v>193</v>
+        <v>423</v>
       </c>
       <c r="K118">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="119" spans="2:12" x14ac:dyDescent="0.25">
@@ -5778,19 +5783,16 @@
         <v>95</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="I119" t="s">
         <v>449</v>
       </c>
       <c r="J119" t="s">
-        <v>413</v>
+        <v>193</v>
       </c>
       <c r="K119">
-        <v>33</v>
-      </c>
-      <c r="L119" t="s">
-        <v>384</v>
+        <v>36</v>
       </c>
     </row>
     <row r="120" spans="2:12" x14ac:dyDescent="0.25">
@@ -5798,93 +5800,92 @@
         <v>95</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>447</v>
+        <v>412</v>
       </c>
       <c r="I120" t="s">
         <v>449</v>
       </c>
       <c r="J120" t="s">
-        <v>448</v>
+        <v>413</v>
       </c>
       <c r="K120">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L120" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="121" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B121" t="s">
-        <v>174</v>
-      </c>
-      <c r="D121" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F121" s="9" t="s">
-        <v>175</v>
+      <c r="D121" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>447</v>
       </c>
       <c r="I121" t="s">
-        <v>450</v>
-      </c>
-      <c r="J121" s="10" t="s">
-        <v>327</v>
-      </c>
-      <c r="K121" s="10"/>
+        <v>449</v>
+      </c>
+      <c r="J121" t="s">
+        <v>448</v>
+      </c>
+      <c r="K121">
+        <v>31</v>
+      </c>
+      <c r="L121" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="122" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>242</v>
+        <v>174</v>
       </c>
       <c r="D122" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F122" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I122" t="s">
         <v>450</v>
       </c>
       <c r="J122" s="10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K122" s="10"/>
     </row>
     <row r="123" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D123" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F123" s="9" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="I123" t="s">
         <v>450</v>
       </c>
       <c r="J123" s="10" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K123" s="10"/>
-      <c r="L123" t="s">
-        <v>384</v>
-      </c>
     </row>
     <row r="124" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F124" s="9" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
       <c r="I124" t="s">
         <v>450</v>
       </c>
       <c r="J124" s="10" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K124" s="10"/>
       <c r="L124" t="s">
@@ -5892,17 +5893,20 @@
       </c>
     </row>
     <row r="125" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>243</v>
+      </c>
       <c r="D125" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F125" s="9" t="s">
-        <v>325</v>
+        <v>209</v>
       </c>
       <c r="I125" t="s">
         <v>450</v>
       </c>
       <c r="J125" s="10" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="K125" s="10"/>
       <c r="L125" t="s">
@@ -5910,20 +5914,17 @@
       </c>
     </row>
     <row r="126" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B126" t="s">
-        <v>241</v>
-      </c>
       <c r="D126" s="6" t="s">
         <v>94</v>
       </c>
       <c r="F126" s="9" t="s">
-        <v>237</v>
+        <v>325</v>
       </c>
       <c r="I126" t="s">
         <v>450</v>
       </c>
       <c r="J126" s="10" t="s">
-        <v>238</v>
+        <v>326</v>
       </c>
       <c r="K126" s="10"/>
       <c r="L126" t="s">
@@ -5931,20 +5932,24 @@
       </c>
     </row>
     <row r="127" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D127" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F127" s="2" t="s">
-        <v>177</v>
+      <c r="B127" t="s">
+        <v>241</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F127" s="9" t="s">
+        <v>237</v>
       </c>
       <c r="I127" t="s">
         <v>450</v>
       </c>
-      <c r="J127" t="s">
-        <v>205</v>
-      </c>
-      <c r="K127">
-        <v>64</v>
+      <c r="J127" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="K127" s="10"/>
+      <c r="L127" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="128" spans="2:12" x14ac:dyDescent="0.25">
@@ -5952,16 +5957,16 @@
         <v>95</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I128" t="s">
         <v>450</v>
       </c>
       <c r="J128" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K128">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
@@ -5969,16 +5974,16 @@
         <v>95</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>460</v>
+        <v>178</v>
       </c>
       <c r="I129" t="s">
         <v>450</v>
       </c>
       <c r="J129" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="K129">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
@@ -5986,16 +5991,16 @@
         <v>95</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>184</v>
+        <v>460</v>
       </c>
       <c r="I130" t="s">
         <v>450</v>
       </c>
       <c r="J130" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="K130">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.25">
@@ -6003,16 +6008,16 @@
         <v>95</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>224</v>
+        <v>184</v>
       </c>
       <c r="I131" t="s">
         <v>450</v>
       </c>
       <c r="J131" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="K131">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
@@ -6020,19 +6025,16 @@
         <v>95</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>535</v>
+        <v>224</v>
       </c>
       <c r="I132" t="s">
         <v>450</v>
       </c>
       <c r="J132" t="s">
-        <v>529</v>
+        <v>225</v>
       </c>
       <c r="K132">
-        <v>69</v>
-      </c>
-      <c r="L132" t="s">
-        <v>384</v>
+        <v>67</v>
       </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.25">
@@ -6040,16 +6042,16 @@
         <v>95</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>185</v>
+        <v>535</v>
       </c>
       <c r="I133" t="s">
         <v>450</v>
       </c>
       <c r="J133" t="s">
-        <v>332</v>
+        <v>529</v>
       </c>
       <c r="K133">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="L133" t="s">
         <v>384</v>
@@ -6060,16 +6062,16 @@
         <v>95</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>331</v>
+        <v>185</v>
       </c>
       <c r="I134" t="s">
         <v>450</v>
       </c>
       <c r="J134" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K134">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L134" t="s">
         <v>384</v>
@@ -6080,199 +6082,219 @@
         <v>95</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>239</v>
+        <v>331</v>
       </c>
       <c r="I135" t="s">
         <v>450</v>
       </c>
       <c r="J135" t="s">
-        <v>240</v>
+        <v>333</v>
       </c>
       <c r="K135">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L135" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D136" s="6" t="s">
+      <c r="D136" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="I136" t="s">
+        <v>450</v>
+      </c>
+      <c r="J136" t="s">
+        <v>240</v>
+      </c>
+      <c r="K136">
+        <v>61</v>
+      </c>
+      <c r="L136" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D137" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F136" s="2" t="s">
+      <c r="F137" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="I136" t="s">
-        <v>451</v>
-      </c>
-      <c r="J136" t="s">
-        <v>368</v>
-      </c>
-      <c r="K136" s="10"/>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D137" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F137" s="2" t="s">
-        <v>366</v>
       </c>
       <c r="I137" t="s">
         <v>451</v>
       </c>
       <c r="J137" t="s">
-        <v>369</v>
-      </c>
-      <c r="K137">
-        <v>71</v>
-      </c>
+        <v>368</v>
+      </c>
+      <c r="K137" s="10"/>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D138" s="5" t="s">
         <v>95</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>461</v>
+        <v>366</v>
       </c>
       <c r="I138" t="s">
         <v>451</v>
       </c>
       <c r="J138" t="s">
+        <v>369</v>
+      </c>
+      <c r="K138">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D139" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="I139" t="s">
+        <v>451</v>
+      </c>
+      <c r="J139" t="s">
         <v>370</v>
       </c>
-      <c r="K138">
+      <c r="K139">
         <v>72</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D139" s="6" t="s">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D140" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F139" s="2" t="s">
+      <c r="F140" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="I139" t="s">
-        <v>452</v>
-      </c>
-      <c r="J139" t="s">
-        <v>291</v>
-      </c>
-      <c r="K139" s="10"/>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D140" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F140" s="2" t="s">
-        <v>218</v>
       </c>
       <c r="I140" t="s">
         <v>452</v>
       </c>
       <c r="J140" t="s">
+        <v>291</v>
+      </c>
+      <c r="K140" s="10"/>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D141" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I141" t="s">
+        <v>452</v>
+      </c>
+      <c r="J141" t="s">
         <v>219</v>
       </c>
-      <c r="K140">
+      <c r="K141">
         <v>45</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A141">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A142">
         <v>17</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B142" t="s">
         <v>135</v>
       </c>
-      <c r="D141" s="6" t="s">
+      <c r="D142" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F141" s="9" t="s">
+      <c r="F142" s="9" t="s">
         <v>507</v>
-      </c>
-      <c r="I141" t="s">
-        <v>474</v>
-      </c>
-      <c r="J141" s="10" t="s">
-        <v>475</v>
-      </c>
-      <c r="K141" s="10"/>
-      <c r="L141" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D142" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="F142" s="2" t="s">
-        <v>473</v>
       </c>
       <c r="I142" t="s">
         <v>474</v>
       </c>
-      <c r="J142" t="s">
-        <v>342</v>
-      </c>
-      <c r="K142">
-        <v>51</v>
-      </c>
+      <c r="J142" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="K142" s="10"/>
       <c r="L142" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B143" t="s">
+      <c r="D143" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="I143" t="s">
+        <v>474</v>
+      </c>
+      <c r="J143" t="s">
+        <v>342</v>
+      </c>
+      <c r="K143">
+        <v>51</v>
+      </c>
+      <c r="L143" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
         <v>284</v>
       </c>
-      <c r="D143" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F143" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="I143" t="s">
-        <v>453</v>
-      </c>
-      <c r="J143" t="s">
-        <v>288</v>
-      </c>
-      <c r="K143" s="10"/>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D144" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F144" s="2" t="s">
-        <v>293</v>
+      <c r="F144" s="9" t="s">
+        <v>285</v>
       </c>
       <c r="I144" t="s">
         <v>453</v>
       </c>
       <c r="J144" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K144" s="10"/>
-      <c r="L144" t="s">
-        <v>384</v>
-      </c>
     </row>
     <row r="145" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D145" s="5" t="s">
-        <v>95</v>
+      <c r="D145" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="I145" t="s">
         <v>453</v>
       </c>
       <c r="J145" t="s">
+        <v>289</v>
+      </c>
+      <c r="K145" s="10"/>
+      <c r="L145" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="146" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D146" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F146" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="I146" t="s">
+        <v>453</v>
+      </c>
+      <c r="J146" t="s">
         <v>287</v>
       </c>
-      <c r="K145">
+      <c r="K146">
         <v>46</v>
       </c>
-      <c r="L145" t="s">
+      <c r="L146" t="s">
         <v>384</v>
       </c>
     </row>
@@ -6291,7 +6313,7 @@
   <dimension ref="A1:AX24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6648,6 +6670,9 @@
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B5" s="2" t="s">
+        <v>644</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
isl collection  current_config_extract separated into sections
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="5" r:id="rId1"/>
@@ -2513,8 +2513,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BC17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3467,7 +3467,7 @@
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4047,6 +4047,9 @@
       <c r="F25" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
       <c r="I25" t="s">
         <v>143</v>
       </c>
@@ -4397,9 +4400,6 @@
       </c>
       <c r="F40" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="H40">
-        <v>1</v>
       </c>
       <c r="I40" t="s">
         <v>147</v>
@@ -6338,7 +6338,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7475,8 +7475,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AW24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fcr collection  current_config_extract separated into sections
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="651">
   <si>
     <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Megafon\All SANs\STF\SSV_coreSTF_20190419</t>
   </si>
@@ -2439,7 +2439,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2513,8 +2513,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BC17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2573,6 +2573,168 @@
       <c r="A1" s="22" t="s">
         <v>630</v>
       </c>
+      <c r="B1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="M1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="O1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="P1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="Q1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="R1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="S1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="T1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="U1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="V1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="W1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="X1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="Y1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="Z1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AA1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AB1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AC1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AD1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AE1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AF1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AG1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AH1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AI1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AJ1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AK1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AL1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AM1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AN1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AO1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AP1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AQ1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AR1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AS1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AT1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AU1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AV1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AW1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AX1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AY1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="AZ1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="BA1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="BB1" s="22" t="s">
+        <v>630</v>
+      </c>
+      <c r="BC1" s="22" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2583,7 +2745,7 @@
       <c r="A3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>79</v>
       </c>
     </row>
@@ -3454,6 +3616,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="contents!A1" display="Contents"/>
+    <hyperlink ref="B1:BC1" location="contents!A1" display="Contents"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3465,9 +3628,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L146"/>
   <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
+      <selection pane="bottomLeft" activeCell="F43" sqref="F43:H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4047,9 +4210,6 @@
       <c r="F25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
       <c r="I25" t="s">
         <v>143</v>
       </c>
@@ -4463,6 +4623,9 @@
       </c>
       <c r="F43" s="2" t="s">
         <v>215</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
       </c>
       <c r="I43" t="s">
         <v>216</v>
@@ -6338,7 +6501,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7476,7 +7639,7 @@
   <dimension ref="A1:AW24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
storage collection current_config_extract separated into sections
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="5" r:id="rId1"/>
@@ -2514,7 +2514,7 @@
   <dimension ref="A1:BC17"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2522,7 +2522,7 @@
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="70" customWidth="1"/>
     <col min="3" max="4" width="116.28515625" customWidth="1"/>
-    <col min="5" max="5" width="70" customWidth="1"/>
+    <col min="5" max="5" width="120.85546875" customWidth="1"/>
     <col min="6" max="6" width="109.42578125" customWidth="1"/>
     <col min="7" max="7" width="116.7109375" customWidth="1"/>
     <col min="8" max="8" width="128.5703125" customWidth="1"/>
@@ -3628,9 +3628,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F43" sqref="F43:H43"/>
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3919,6 +3919,9 @@
       <c r="F14" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
       <c r="I14" t="s">
         <v>150</v>
       </c>
@@ -4623,9 +4626,6 @@
       </c>
       <c r="F43" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="H43">
-        <v>1</v>
       </c>
       <c r="I43" t="s">
         <v>216</v>
@@ -6501,7 +6501,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7638,8 +7638,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AW24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
chassis params collection current_config_extract refactored with defined functions
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="5" r:id="rId1"/>
@@ -2513,8 +2513,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BC17"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2745,7 +2745,7 @@
       <c r="A3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2987,7 +2987,7 @@
         <v>44292</v>
       </c>
       <c r="Z5" s="12">
-        <v>29681</v>
+        <v>44291</v>
       </c>
       <c r="AA5" s="12">
         <v>44286</v>
@@ -3629,8 +3629,8 @@
   <dimension ref="A1:L146"/>
   <sheetViews>
     <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3821,6 +3821,9 @@
       <c r="F10" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
       <c r="I10" t="s">
         <v>140</v>
       </c>
@@ -3918,9 +3921,6 @@
       </c>
       <c r="F14" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
       </c>
       <c r="I14" t="s">
         <v>150</v>
@@ -7638,8 +7638,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AW24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
zonining collection status display
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="contents" sheetId="5" r:id="rId1"/>
@@ -2513,8 +2513,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BC17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3628,9 +3628,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L146"/>
   <sheetViews>
-    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10:H10"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3821,9 +3821,6 @@
       <c r="F10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
       <c r="I10" t="s">
         <v>140</v>
       </c>
@@ -3949,6 +3946,7 @@
       <c r="F15" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="G15" s="4"/>
       <c r="I15" t="s">
         <v>146</v>
       </c>
@@ -3976,6 +3974,7 @@
       <c r="F16" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="G16" s="4"/>
       <c r="I16" t="s">
         <v>146</v>
       </c>
@@ -4003,6 +4002,7 @@
       <c r="F17" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="G17" s="4"/>
       <c r="I17" t="s">
         <v>144</v>
       </c>
@@ -4030,6 +4030,7 @@
       <c r="F18" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="G18" s="4"/>
       <c r="I18" t="s">
         <v>145</v>
       </c>
@@ -4057,6 +4058,7 @@
       <c r="F19" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="G19" s="4"/>
       <c r="I19" t="s">
         <v>145</v>
       </c>
@@ -4084,6 +4086,10 @@
       <c r="F20" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="G20" s="4"/>
+      <c r="H20">
+        <v>1</v>
+      </c>
       <c r="I20" t="s">
         <v>142</v>
       </c>
@@ -4111,6 +4117,7 @@
       <c r="F21" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="G21" s="4"/>
       <c r="I21" t="s">
         <v>142</v>
       </c>
@@ -4138,6 +4145,7 @@
       <c r="F22" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="G22" s="4"/>
       <c r="I22" t="s">
         <v>142</v>
       </c>
@@ -4162,6 +4170,7 @@
       <c r="F23" s="2" t="s">
         <v>500</v>
       </c>
+      <c r="G23" s="4"/>
       <c r="I23" t="s">
         <v>142</v>
       </c>
@@ -4186,6 +4195,7 @@
       <c r="F24" s="2" t="s">
         <v>518</v>
       </c>
+      <c r="G24" s="4"/>
       <c r="I24" t="s">
         <v>142</v>
       </c>
@@ -4213,6 +4223,7 @@
       <c r="F25" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="G25" s="4"/>
       <c r="I25" t="s">
         <v>143</v>
       </c>
@@ -4240,6 +4251,7 @@
       <c r="F26" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="G26" s="4"/>
       <c r="I26" t="s">
         <v>143</v>
       </c>
@@ -4267,6 +4279,7 @@
       <c r="F27" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="G27" s="4"/>
       <c r="I27" t="s">
         <v>143</v>
       </c>
@@ -4294,6 +4307,7 @@
       <c r="F28" s="2" t="s">
         <v>435</v>
       </c>
+      <c r="G28" s="4"/>
       <c r="I28" t="s">
         <v>143</v>
       </c>
@@ -4321,6 +4335,7 @@
       <c r="F29" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="G29" s="4"/>
       <c r="I29" t="s">
         <v>141</v>
       </c>
@@ -4345,6 +4360,7 @@
       <c r="F30" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="G30" s="4"/>
       <c r="I30" t="s">
         <v>141</v>
       </c>
@@ -4369,6 +4385,7 @@
       <c r="F31" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="G31" s="4"/>
       <c r="I31" t="s">
         <v>141</v>
       </c>
@@ -4393,6 +4410,7 @@
       <c r="F32" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="G32" s="4"/>
       <c r="I32" t="s">
         <v>141</v>
       </c>
@@ -4414,6 +4432,7 @@
       <c r="F33" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="G33" s="4"/>
       <c r="I33" t="s">
         <v>141</v>
       </c>
@@ -4435,6 +4454,7 @@
       <c r="F34" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="G34" s="4"/>
       <c r="I34" t="s">
         <v>141</v>
       </c>
@@ -4456,6 +4476,7 @@
       <c r="F35" s="2" t="s">
         <v>566</v>
       </c>
+      <c r="G35" s="4"/>
       <c r="I35" t="s">
         <v>141</v>
       </c>
@@ -4480,6 +4501,7 @@
       <c r="F36" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="G36" s="4"/>
       <c r="I36" t="s">
         <v>147</v>
       </c>
@@ -4501,6 +4523,7 @@
       <c r="F37" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="G37" s="4"/>
       <c r="I37" t="s">
         <v>147</v>
       </c>
@@ -4522,6 +4545,7 @@
       <c r="F38" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="G38" s="4"/>
       <c r="I38" t="s">
         <v>147</v>
       </c>
@@ -4543,6 +4567,7 @@
       <c r="F39" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="G39" s="4"/>
       <c r="I39" t="s">
         <v>147</v>
       </c>
@@ -4564,6 +4589,7 @@
       <c r="F40" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="G40" s="4"/>
       <c r="I40" t="s">
         <v>147</v>
       </c>
@@ -4585,6 +4611,7 @@
       <c r="F41" s="2" t="s">
         <v>230</v>
       </c>
+      <c r="G41" s="4"/>
       <c r="I41" t="s">
         <v>147</v>
       </c>
@@ -4606,6 +4633,7 @@
       <c r="F42" s="2" t="s">
         <v>231</v>
       </c>
+      <c r="G42" s="4"/>
       <c r="I42" t="s">
         <v>147</v>
       </c>
@@ -4627,6 +4655,7 @@
       <c r="F43" s="2" t="s">
         <v>215</v>
       </c>
+      <c r="G43" s="4"/>
       <c r="I43" t="s">
         <v>216</v>
       </c>
@@ -4648,6 +4677,7 @@
       <c r="F44" s="2" t="s">
         <v>279</v>
       </c>
+      <c r="G44" s="4"/>
       <c r="I44" t="s">
         <v>280</v>
       </c>
@@ -6501,7 +6531,7 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7638,8 +7668,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AW24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
switch pair module. excluding vc module from switch_params_aggregated
</commit_message>
<xml_diff>
--- a/report_info.xlsx
+++ b/report_info.xlsx
@@ -954,15 +954,6 @@
     <t>Fabric-Device Management Interface (FDMI) information</t>
   </si>
   <si>
-    <t>SAN Implementation. Checking</t>
-  </si>
-  <si>
-    <t>C:\Users\vlasenko\Documents\01.CUSTOMERS\Lenenergo\FEB2021_verification</t>
-  </si>
-  <si>
-    <t>C:\Users\vlasenko\Documents\06.CONFIGS\Lenenergo\FEB2021\ssave_25022021</t>
-  </si>
-  <si>
     <t>Unicredit</t>
   </si>
   <si>
@@ -1993,6 +1984,15 @@
   </si>
   <si>
     <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\Mechel\29012021</t>
+  </si>
+  <si>
+    <t>SAN implementation check</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\01.CUSTOMERS\Lenenergo\FEB2021_verification</t>
+  </si>
+  <si>
+    <t>C:\Users\vlasenko\OneDrive - Hewlett Packard Enterprise\Documents\06.CONFIGS\Lenenergo\FEB2021\ssave_25022021</t>
   </si>
 </sst>
 </file>
@@ -2525,50 +2525,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="B2" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="B3" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="B4" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="B5" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="B6" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
   </sheetData>
@@ -2588,8 +2588,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BC17"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AC41" sqref="AC41"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AG7" sqref="AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2646,181 +2646,181 @@
   <sheetData>
     <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="Q1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="V1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="X1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="Y1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="Z1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AA1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AB1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AC1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AD1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AE1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AF1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AG1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AH1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AI1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AJ1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AK1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AL1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AM1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AN1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AO1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AP1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AQ1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AR1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AS1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AT1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AU1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AV1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AW1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AX1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AY1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="AZ1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="BA1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="BB1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="BC1" s="21" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="3" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AG3" s="3" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2829,82 +2829,82 @@
         <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="E4" t="s">
         <v>226</v>
       </c>
       <c r="F4" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="G4" t="s">
+        <v>501</v>
+      </c>
+      <c r="H4" t="s">
+        <v>509</v>
+      </c>
+      <c r="I4" t="s">
         <v>504</v>
       </c>
-      <c r="H4" t="s">
-        <v>512</v>
-      </c>
-      <c r="I4" t="s">
-        <v>507</v>
-      </c>
       <c r="J4" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="K4" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="L4" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="M4" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="N4" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="O4" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="P4" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="Q4" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="R4" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="S4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="T4" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="U4" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="V4" t="s">
         <v>226</v>
       </c>
       <c r="W4" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="X4" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="Y4" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="Z4" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="AA4" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="AB4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="AC4" t="s">
         <v>305</v>
@@ -3101,19 +3101,19 @@
     </row>
     <row r="6" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C6" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D6" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="E6" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="F6" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="G6" t="s">
         <v>308</v>
@@ -3137,19 +3137,19 @@
         <v>308</v>
       </c>
       <c r="N6" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="O6" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="P6" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="Q6" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="R6" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="S6" t="s">
         <v>308</v>
@@ -3161,10 +3161,10 @@
         <v>308</v>
       </c>
       <c r="V6" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="W6" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="X6" t="s">
         <v>308</v>
@@ -3176,7 +3176,7 @@
         <v>308</v>
       </c>
       <c r="AA6" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="AB6" t="s">
         <v>308</v>
@@ -3191,7 +3191,7 @@
         <v>308</v>
       </c>
       <c r="AG6" t="s">
-        <v>310</v>
+        <v>654</v>
       </c>
       <c r="AH6" t="s">
         <v>304</v>
@@ -3215,97 +3215,97 @@
         <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D7" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E7" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="F7" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="G7" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="H7" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="I7" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="J7" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="K7" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="L7" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="M7" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="N7" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="O7" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="P7" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="Q7" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="R7" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="S7" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="T7" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="U7" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="V7" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="W7" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="X7" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="Y7" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="Z7" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="AA7" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="AB7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="AC7" t="s">
         <v>306</v>
       </c>
       <c r="AD7" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="AE7" t="s">
         <v>296</v>
       </c>
       <c r="AF7" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="AG7" t="s">
-        <v>311</v>
+        <v>655</v>
       </c>
       <c r="AH7" t="s">
         <v>302</v>
@@ -3379,97 +3379,97 @@
         <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D8" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="E8" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="F8" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="G8" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="H8" t="s">
+        <v>512</v>
+      </c>
+      <c r="I8" t="s">
+        <v>506</v>
+      </c>
+      <c r="J8" t="s">
+        <v>520</v>
+      </c>
+      <c r="K8" t="s">
+        <v>536</v>
+      </c>
+      <c r="L8" t="s">
+        <v>496</v>
+      </c>
+      <c r="M8" t="s">
+        <v>493</v>
+      </c>
+      <c r="N8" t="s">
+        <v>488</v>
+      </c>
+      <c r="O8" t="s">
+        <v>482</v>
+      </c>
+      <c r="P8" t="s">
+        <v>475</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>452</v>
+      </c>
+      <c r="R8" t="s">
+        <v>444</v>
+      </c>
+      <c r="S8" t="s">
+        <v>627</v>
+      </c>
+      <c r="T8" t="s">
+        <v>418</v>
+      </c>
+      <c r="U8" t="s">
+        <v>397</v>
+      </c>
+      <c r="V8" t="s">
+        <v>630</v>
+      </c>
+      <c r="W8" t="s">
+        <v>379</v>
+      </c>
+      <c r="X8" t="s">
         <v>515</v>
       </c>
-      <c r="I8" t="s">
-        <v>509</v>
-      </c>
-      <c r="J8" t="s">
-        <v>523</v>
-      </c>
-      <c r="K8" t="s">
-        <v>539</v>
-      </c>
-      <c r="L8" t="s">
-        <v>499</v>
-      </c>
-      <c r="M8" t="s">
-        <v>496</v>
-      </c>
-      <c r="N8" t="s">
-        <v>491</v>
-      </c>
-      <c r="O8" t="s">
-        <v>485</v>
- 